<commit_message>
Changes to plot functions and updated evp params in evpwdb
</commit_message>
<xml_diff>
--- a/scripts/__other__/__sem__.xlsx
+++ b/scripts/__other__/__sem__.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Janzen\Desktop\code\moga_neml\scripts\__other__\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1ACB1329-CF65-403B-8E7E-CB18CE46B16E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65A614A7-2EC7-4922-97F6-01EE06E16E89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="evpcd" sheetId="8" r:id="rId1"/>
-    <sheet name="evpcd_plots" sheetId="10" r:id="rId2"/>
+    <sheet name="evpcd_" sheetId="10" r:id="rId2"/>
     <sheet name="evpwd" sheetId="9" r:id="rId3"/>
+    <sheet name="evpwd_" sheetId="11" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="22">
   <si>
     <t>temp</t>
   </si>
@@ -220,12 +221,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -252,16 +253,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -814,6 +812,363 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>39460</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>61231</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1457733</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>1479504</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="15" name="Picture 14">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AFC860C8-61CD-3B35-D0F7-27BD12004235}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1258660" y="5833381"/>
+          <a:ext cx="1418273" cy="1418273"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>58510</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>1323975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1485899</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>2749835</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="16" name="Picture 15">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DB50E913-82F3-8EA3-5F8F-6F884E2702C1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1277710" y="7096125"/>
+          <a:ext cx="1427389" cy="1425860"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>49461</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>44823</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1453599</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>1456051</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="19" name="Picture 18">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8FAC191A-1FCC-E3E0-35B8-9F01216511D0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1259696" y="235323"/>
+          <a:ext cx="1404138" cy="1411228"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>56030</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>1344560</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1468118</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>2756648</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="20" name="Picture 19">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1523131E-3966-872C-9B12-05C3A7D3E5CB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1266265" y="1535060"/>
+          <a:ext cx="1412088" cy="1412088"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>123265</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>78438</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1479178</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>1434351</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="21" name="Picture 20">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9C75ECE1-8654-C602-502B-06FAA3FF2D50}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1333500" y="3059203"/>
+          <a:ext cx="1355913" cy="1355913"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>96371</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>1429868</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1452284</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>2785781</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="22" name="Picture 21">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{708B6789-7A67-3F90-E897-9AA317B93F31}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1306606" y="4410633"/>
+          <a:ext cx="1355913" cy="1355913"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>104309</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>50111</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1490870</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>1432351</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D03509EB-CD07-EC75-76C7-C6C58C0B1D89}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1330135" y="8614328"/>
+          <a:ext cx="1386561" cy="1382240"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>101164</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>1348288</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1499151</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>2746685</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BDC029CF-A87E-DEE8-593C-0CAA2B8519E4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1326990" y="9912505"/>
+          <a:ext cx="1397987" cy="1398397"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -1480,18 +1835,18 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59578D89-F974-462A-A8BE-33C4579641C9}">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="14"/>
+    <col min="1" max="1" width="9.140625" style="11"/>
     <col min="2" max="2" width="9.140625" style="12"/>
     <col min="3" max="5" width="22.7109375" style="13" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="14"/>
+    <col min="6" max="16384" width="9.140625" style="11"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -1576,9 +1931,6 @@
       <c r="C7" s="10"/>
       <c r="D7" s="10"/>
       <c r="E7" s="10"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1590,8 +1942,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8265FA44-8E85-43C1-8A54-AE4FC552DE01}">
   <dimension ref="A1:N13"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="N7" sqref="N7"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1657,6 +2009,21 @@
       <c r="C2" s="1" t="s">
         <v>13</v>
       </c>
+      <c r="D2" s="2">
+        <v>11.695</v>
+      </c>
+      <c r="E2" s="2">
+        <v>101.28</v>
+      </c>
+      <c r="F2" s="2">
+        <v>1.1411</v>
+      </c>
+      <c r="G2" s="2">
+        <v>4.6826999999999996</v>
+      </c>
+      <c r="H2" s="2">
+        <v>1595.5</v>
+      </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C3" s="1" t="s">
@@ -1691,6 +2058,21 @@
       <c r="C5" s="1" t="s">
         <v>13</v>
       </c>
+      <c r="D5" s="2">
+        <v>31.327000000000002</v>
+      </c>
+      <c r="E5" s="2">
+        <v>104.92</v>
+      </c>
+      <c r="F5" s="2">
+        <v>0.8548</v>
+      </c>
+      <c r="G5" s="2">
+        <v>3.7507999999999999</v>
+      </c>
+      <c r="H5" s="2">
+        <v>2575.8000000000002</v>
+      </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C6" s="1" t="s">
@@ -1725,6 +2107,21 @@
       <c r="C8" s="1" t="s">
         <v>13</v>
       </c>
+      <c r="D8" s="2">
+        <v>4.8710000000000004</v>
+      </c>
+      <c r="E8" s="2">
+        <v>11.518000000000001</v>
+      </c>
+      <c r="F8" s="2">
+        <v>7.0281000000000002</v>
+      </c>
+      <c r="G8" s="2">
+        <v>4.2420999999999998</v>
+      </c>
+      <c r="H8" s="2">
+        <v>1138.3</v>
+      </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C9" s="1" t="s">
@@ -1759,6 +2156,21 @@
       <c r="C11" s="1" t="s">
         <v>13</v>
       </c>
+      <c r="D11" s="2">
+        <v>4.8238000000000003</v>
+      </c>
+      <c r="E11" s="2">
+        <v>378.86</v>
+      </c>
+      <c r="F11" s="2">
+        <v>0.14230000000000001</v>
+      </c>
+      <c r="G11" s="2">
+        <v>4.4020999999999999</v>
+      </c>
+      <c r="H11" s="2">
+        <v>1006.9</v>
+      </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C12" s="1" t="s">
@@ -1786,4 +2198,109 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F993A154-4E62-4351-9866-5A09D9C5DBD5}">
+  <dimension ref="A1:E7"/>
+  <sheetViews>
+    <sheetView topLeftCell="A3" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="M4" sqref="M4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="11"/>
+    <col min="2" max="2" width="9.140625" style="12"/>
+    <col min="3" max="5" width="22.7109375" style="13" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="11"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" s="8" customFormat="1" ht="219.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="8">
+        <v>800</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
+    </row>
+    <row r="3" spans="1:5" s="8" customFormat="1" ht="219.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="8">
+        <v>800</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="10"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="10"/>
+    </row>
+    <row r="4" spans="1:5" s="8" customFormat="1" ht="219.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="8">
+        <v>900</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="10"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10"/>
+    </row>
+    <row r="5" spans="1:5" s="8" customFormat="1" ht="219.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="8">
+        <v>900</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="10"/>
+      <c r="D5" s="10"/>
+      <c r="E5" s="10"/>
+    </row>
+    <row r="6" spans="1:5" s="8" customFormat="1" ht="219.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="8">
+        <v>1000</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="10"/>
+      <c r="D6" s="10"/>
+      <c r="E6" s="10"/>
+    </row>
+    <row r="7" spans="1:5" s="8" customFormat="1" ht="219.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="8">
+        <v>1000</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="10"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="10"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
minor changes to scripts
</commit_message>
<xml_diff>
--- a/scripts/__other__/__sem__.xlsx
+++ b/scripts/__other__/__sem__.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Janzen\Desktop\code\moga_neml\scripts\__other__\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A509DB90-75DE-4AD8-9261-3C4657F7489D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DD67D5B-7A3F-4331-99BA-7B12DD3D8434}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="15600" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="evpcd" sheetId="8" r:id="rId1"/>
-    <sheet name="evpcd_" sheetId="10" r:id="rId2"/>
-    <sheet name="evpwd" sheetId="9" r:id="rId3"/>
+    <sheet name="evp-cd" sheetId="8" r:id="rId1"/>
+    <sheet name="evp-wd" sheetId="12" r:id="rId2"/>
+    <sheet name="evpcd_" sheetId="10" r:id="rId3"/>
     <sheet name="evpwd_" sheetId="11" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="16">
   <si>
     <t>temp</t>
   </si>
@@ -77,24 +77,6 @@
   <si>
     <t>init</t>
   </si>
-  <si>
-    <t>c_n</t>
-  </si>
-  <si>
-    <t>c_0</t>
-  </si>
-  <si>
-    <t>c_1</t>
-  </si>
-  <si>
-    <t>t_n</t>
-  </si>
-  <si>
-    <t>t_0</t>
-  </si>
-  <si>
-    <t>t_1</t>
-  </si>
 </sst>
 </file>
 
@@ -117,7 +99,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -217,11 +199,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -261,6 +254,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1432,10 +1431,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C8957C7-6C75-407A-91FD-39EC012C6800}">
-  <dimension ref="A1:K19"/>
+  <dimension ref="A1:K91"/>
   <sheetViews>
     <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="C91" sqref="C2:C91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1483,39 +1482,48 @@
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="2">
+      <c r="A2" s="14">
         <v>800</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="14" t="s">
         <v>7</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="2">
+      <c r="D2" s="14">
         <v>4.7069999999999999</v>
       </c>
-      <c r="E2" s="2">
+      <c r="E2" s="14">
         <v>29.9</v>
       </c>
-      <c r="F2" s="2">
+      <c r="F2" s="14">
         <v>47.707000000000001</v>
       </c>
-      <c r="G2" s="2">
+      <c r="G2" s="14">
         <v>3.6625999999999999</v>
       </c>
-      <c r="H2" s="2">
+      <c r="H2" s="14">
         <v>3159.4</v>
       </c>
+      <c r="I2" s="14"/>
+      <c r="J2" s="14"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="14"/>
+      <c r="B3" s="14"/>
       <c r="C3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="I3" s="2">
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="14"/>
+      <c r="G3" s="14"/>
+      <c r="H3" s="14"/>
+      <c r="I3" s="14">
         <v>2169</v>
       </c>
-      <c r="J3" s="2">
+      <c r="J3" s="14">
         <v>5.6902999999999997</v>
       </c>
       <c r="K3" s="1">
@@ -1523,12 +1531,12 @@
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="3"/>
-      <c r="B4" s="3"/>
-      <c r="C4" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D4" s="3">
+      <c r="A4" s="14"/>
+      <c r="B4" s="14"/>
+      <c r="C4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="15">
         <v>6.4737</v>
       </c>
       <c r="E4" s="3">
@@ -1554,225 +1562,135 @@
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="2">
-        <v>800</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>8</v>
-      </c>
+      <c r="A5" s="14"/>
+      <c r="B5" s="14"/>
       <c r="C5" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="2">
-        <v>14.535</v>
-      </c>
-      <c r="E5" s="2">
-        <v>347.93</v>
-      </c>
-      <c r="F5" s="2">
-        <v>0.33581</v>
-      </c>
-      <c r="G5" s="2">
-        <v>3.8755000000000002</v>
-      </c>
-      <c r="H5" s="2">
-        <v>3156.8</v>
-      </c>
+      <c r="D5" s="14"/>
+      <c r="E5" s="14"/>
+      <c r="F5" s="14"/>
+      <c r="G5" s="14"/>
+      <c r="H5" s="14"/>
+      <c r="I5" s="14"/>
+      <c r="J5" s="14"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="14"/>
+      <c r="B6" s="14"/>
       <c r="C6" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="I6" s="2">
-        <v>2603.4</v>
-      </c>
-      <c r="J6" s="2">
-        <v>4.9169</v>
-      </c>
-      <c r="K6" s="1">
-        <v>4.2122999999999999</v>
-      </c>
+      <c r="D6" s="14"/>
+      <c r="E6" s="14"/>
+      <c r="F6" s="14"/>
+      <c r="G6" s="14"/>
+      <c r="H6" s="14"/>
+      <c r="I6" s="14"/>
+      <c r="J6" s="14"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="3"/>
-      <c r="B7" s="3"/>
-      <c r="C7" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D7" s="3">
-        <v>37.386000000000003</v>
-      </c>
-      <c r="E7" s="3">
-        <v>123.76</v>
-      </c>
-      <c r="F7" s="3">
-        <v>4.7188999999999998E-3</v>
-      </c>
-      <c r="G7" s="3">
-        <v>3.7867999999999999</v>
-      </c>
-      <c r="H7" s="3">
-        <v>2557</v>
-      </c>
-      <c r="I7" s="3">
-        <v>2806.6</v>
-      </c>
-      <c r="J7" s="3">
-        <v>5.1410999999999998</v>
-      </c>
-      <c r="K7" s="4">
-        <v>15.73</v>
-      </c>
+      <c r="A7" s="14"/>
+      <c r="B7" s="14"/>
+      <c r="C7" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" s="15"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
+      <c r="K7" s="4"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="2">
-        <v>900</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>7</v>
-      </c>
+      <c r="A8" s="14"/>
+      <c r="B8" s="14"/>
       <c r="C8" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D8" s="2">
-        <v>17.420000000000002</v>
-      </c>
-      <c r="E8" s="2">
-        <v>217.36</v>
-      </c>
-      <c r="F8" s="2">
-        <v>0.33130999999999999</v>
-      </c>
-      <c r="G8" s="2">
-        <v>2.0339999999999998</v>
-      </c>
-      <c r="H8" s="2">
-        <v>42591</v>
-      </c>
+      <c r="D8" s="14"/>
+      <c r="E8" s="14"/>
+      <c r="F8" s="14"/>
+      <c r="G8" s="14"/>
+      <c r="H8" s="14"/>
+      <c r="I8" s="14"/>
+      <c r="J8" s="14"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="14"/>
+      <c r="B9" s="14"/>
       <c r="C9" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="I9" s="2">
-        <v>2632.8</v>
-      </c>
-      <c r="J9" s="2">
-        <v>4.0648</v>
-      </c>
-      <c r="K9" s="1">
-        <v>5.8117000000000001</v>
-      </c>
+      <c r="D9" s="14"/>
+      <c r="E9" s="14"/>
+      <c r="F9" s="14"/>
+      <c r="G9" s="14"/>
+      <c r="H9" s="14"/>
+      <c r="I9" s="14"/>
+      <c r="J9" s="14"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="3"/>
-      <c r="B10" s="3"/>
-      <c r="C10" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D10" s="3">
-        <v>17.484000000000002</v>
-      </c>
-      <c r="E10" s="3">
-        <v>219.83</v>
-      </c>
-      <c r="F10" s="3">
-        <v>0.33289999999999997</v>
-      </c>
-      <c r="G10" s="3">
-        <v>2.0348999999999999</v>
-      </c>
-      <c r="H10" s="3">
-        <v>44594</v>
-      </c>
-      <c r="I10" s="3">
-        <v>2558.9</v>
-      </c>
-      <c r="J10" s="3">
-        <v>4.0648</v>
-      </c>
-      <c r="K10" s="4">
-        <v>5.2969999999999997</v>
-      </c>
+      <c r="A10" s="14"/>
+      <c r="B10" s="14"/>
+      <c r="C10" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D10" s="15"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="3"/>
+      <c r="J10" s="3"/>
+      <c r="K10" s="4"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="2">
-        <v>900</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>8</v>
-      </c>
+      <c r="A11" s="14"/>
+      <c r="B11" s="14"/>
       <c r="C11" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D11" s="2">
-        <v>17.937000000000001</v>
-      </c>
-      <c r="E11" s="2">
-        <v>7.4195000000000002</v>
-      </c>
-      <c r="F11" s="2">
-        <v>15.250999999999999</v>
-      </c>
-      <c r="G11" s="2">
-        <v>2.4441999999999999</v>
-      </c>
-      <c r="H11" s="2">
-        <v>9880.2000000000007</v>
-      </c>
+      <c r="D11" s="14"/>
+      <c r="E11" s="14"/>
+      <c r="F11" s="14"/>
+      <c r="G11" s="14"/>
+      <c r="H11" s="14"/>
+      <c r="I11" s="14"/>
+      <c r="J11" s="14"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="14"/>
+      <c r="B12" s="14"/>
       <c r="C12" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="I12" s="2">
-        <v>1271.0999999999999</v>
-      </c>
-      <c r="J12" s="2">
-        <v>5.1067</v>
-      </c>
-      <c r="K12" s="1">
-        <v>13.686999999999999</v>
-      </c>
+      <c r="D12" s="14"/>
+      <c r="E12" s="14"/>
+      <c r="F12" s="14"/>
+      <c r="G12" s="14"/>
+      <c r="H12" s="14"/>
+      <c r="I12" s="14"/>
+      <c r="J12" s="14"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="3"/>
-      <c r="B13" s="3"/>
-      <c r="C13" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D13" s="3">
-        <v>17.937000000000001</v>
-      </c>
-      <c r="E13" s="3">
-        <v>7.3311999999999999</v>
-      </c>
-      <c r="F13" s="3">
-        <v>14.571999999999999</v>
-      </c>
-      <c r="G13" s="3">
-        <v>2.4605000000000001</v>
-      </c>
-      <c r="H13" s="3">
-        <v>10468</v>
-      </c>
-      <c r="I13" s="3">
-        <v>1426.3</v>
-      </c>
-      <c r="J13" s="3">
-        <v>4.8376000000000001</v>
-      </c>
-      <c r="K13" s="4">
-        <v>9.0043000000000006</v>
-      </c>
+      <c r="A13" s="14"/>
+      <c r="B13" s="14"/>
+      <c r="C13" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D13" s="15"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
+      <c r="H13" s="3"/>
+      <c r="I13" s="3"/>
+      <c r="J13" s="3"/>
+      <c r="K13" s="4"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="2">
-        <v>1000</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>7</v>
-      </c>
       <c r="C14" s="1" t="s">
         <v>13</v>
       </c>
@@ -1798,28 +1716,1436 @@
       <c r="K16" s="4"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="2">
+      <c r="A17" s="14">
+        <v>800</v>
+      </c>
+      <c r="B17" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D17" s="14">
+        <v>14.535</v>
+      </c>
+      <c r="E17" s="14">
+        <v>347.93</v>
+      </c>
+      <c r="F17" s="14">
+        <v>0.33581</v>
+      </c>
+      <c r="G17" s="14">
+        <v>3.8755000000000002</v>
+      </c>
+      <c r="H17" s="14">
+        <v>3156.8</v>
+      </c>
+      <c r="I17" s="14"/>
+      <c r="J17" s="14"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" s="14"/>
+      <c r="B18" s="14"/>
+      <c r="C18" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D18" s="14"/>
+      <c r="E18" s="14"/>
+      <c r="F18" s="14"/>
+      <c r="G18" s="14"/>
+      <c r="H18" s="14"/>
+      <c r="I18" s="14">
+        <v>2603.4</v>
+      </c>
+      <c r="J18" s="14">
+        <v>4.9169</v>
+      </c>
+      <c r="K18" s="1">
+        <v>4.2122999999999999</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" s="14"/>
+      <c r="B19" s="14"/>
+      <c r="C19" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D19" s="15">
+        <v>37.386000000000003</v>
+      </c>
+      <c r="E19" s="3">
+        <v>123.76</v>
+      </c>
+      <c r="F19" s="3">
+        <v>4.7188999999999998E-3</v>
+      </c>
+      <c r="G19" s="3">
+        <v>3.7867999999999999</v>
+      </c>
+      <c r="H19" s="3">
+        <v>2557</v>
+      </c>
+      <c r="I19" s="3">
+        <v>2806.6</v>
+      </c>
+      <c r="J19" s="3">
+        <v>5.1410999999999998</v>
+      </c>
+      <c r="K19" s="4">
+        <v>15.73</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" s="14"/>
+      <c r="B20" s="14"/>
+      <c r="C20" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D20" s="14"/>
+      <c r="E20" s="14"/>
+      <c r="F20" s="14"/>
+      <c r="G20" s="14"/>
+      <c r="H20" s="14"/>
+      <c r="I20" s="14"/>
+      <c r="J20" s="14"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" s="14"/>
+      <c r="B21" s="14"/>
+      <c r="C21" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D21" s="14"/>
+      <c r="E21" s="14"/>
+      <c r="F21" s="14"/>
+      <c r="G21" s="14"/>
+      <c r="H21" s="14"/>
+      <c r="I21" s="14"/>
+      <c r="J21" s="14"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" s="14"/>
+      <c r="B22" s="14"/>
+      <c r="C22" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D22" s="15"/>
+      <c r="E22" s="3"/>
+      <c r="F22" s="3"/>
+      <c r="G22" s="3"/>
+      <c r="H22" s="3"/>
+      <c r="I22" s="3"/>
+      <c r="J22" s="3"/>
+      <c r="K22" s="4"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23" s="14"/>
+      <c r="B23" s="14"/>
+      <c r="C23" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D23" s="14"/>
+      <c r="E23" s="14"/>
+      <c r="F23" s="14"/>
+      <c r="G23" s="14"/>
+      <c r="H23" s="14"/>
+      <c r="I23" s="14"/>
+      <c r="J23" s="14"/>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24" s="14"/>
+      <c r="B24" s="14"/>
+      <c r="C24" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D24" s="14"/>
+      <c r="E24" s="14"/>
+      <c r="F24" s="14"/>
+      <c r="G24" s="14"/>
+      <c r="H24" s="14"/>
+      <c r="I24" s="14"/>
+      <c r="J24" s="14"/>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A25" s="14"/>
+      <c r="B25" s="14"/>
+      <c r="C25" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D25" s="15"/>
+      <c r="E25" s="3"/>
+      <c r="F25" s="3"/>
+      <c r="G25" s="3"/>
+      <c r="H25" s="3"/>
+      <c r="I25" s="3"/>
+      <c r="J25" s="3"/>
+      <c r="K25" s="4"/>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A26" s="14"/>
+      <c r="B26" s="14"/>
+      <c r="C26" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D26" s="14"/>
+      <c r="E26" s="14"/>
+      <c r="F26" s="14"/>
+      <c r="G26" s="14"/>
+      <c r="H26" s="14"/>
+      <c r="I26" s="14"/>
+      <c r="J26" s="14"/>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A27" s="14"/>
+      <c r="B27" s="14"/>
+      <c r="C27" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D27" s="14"/>
+      <c r="E27" s="14"/>
+      <c r="F27" s="14"/>
+      <c r="G27" s="14"/>
+      <c r="H27" s="14"/>
+      <c r="I27" s="14"/>
+      <c r="J27" s="14"/>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A28" s="14"/>
+      <c r="B28" s="14"/>
+      <c r="C28" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D28" s="15"/>
+      <c r="E28" s="3"/>
+      <c r="F28" s="3"/>
+      <c r="G28" s="3"/>
+      <c r="H28" s="3"/>
+      <c r="I28" s="3"/>
+      <c r="J28" s="3"/>
+      <c r="K28" s="4"/>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C29" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C30" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A31" s="3"/>
+      <c r="B31" s="3"/>
+      <c r="C31" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D31" s="3"/>
+      <c r="E31" s="3"/>
+      <c r="F31" s="3"/>
+      <c r="G31" s="3"/>
+      <c r="H31" s="3"/>
+      <c r="I31" s="3"/>
+      <c r="J31" s="3"/>
+      <c r="K31" s="4"/>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A32" s="14">
+        <v>900</v>
+      </c>
+      <c r="B32" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D32" s="14">
+        <v>17.420000000000002</v>
+      </c>
+      <c r="E32" s="14">
+        <v>217.36</v>
+      </c>
+      <c r="F32" s="14">
+        <v>0.33130999999999999</v>
+      </c>
+      <c r="G32" s="14">
+        <v>2.0339999999999998</v>
+      </c>
+      <c r="H32" s="14">
+        <v>42591</v>
+      </c>
+      <c r="I32" s="14"/>
+      <c r="J32" s="14"/>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A33" s="14"/>
+      <c r="B33" s="14"/>
+      <c r="C33" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D33" s="14"/>
+      <c r="E33" s="14"/>
+      <c r="F33" s="14"/>
+      <c r="G33" s="14"/>
+      <c r="H33" s="14"/>
+      <c r="I33" s="14">
+        <v>2632.8</v>
+      </c>
+      <c r="J33" s="14">
+        <v>4.0648</v>
+      </c>
+      <c r="K33" s="1">
+        <v>5.8117000000000001</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A34" s="14"/>
+      <c r="B34" s="14"/>
+      <c r="C34" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D34" s="15">
+        <v>17.484000000000002</v>
+      </c>
+      <c r="E34" s="3">
+        <v>219.83</v>
+      </c>
+      <c r="F34" s="3">
+        <v>0.33289999999999997</v>
+      </c>
+      <c r="G34" s="3">
+        <v>2.0348999999999999</v>
+      </c>
+      <c r="H34" s="3">
+        <v>44594</v>
+      </c>
+      <c r="I34" s="3">
+        <v>2558.9</v>
+      </c>
+      <c r="J34" s="3">
+        <v>4.0648</v>
+      </c>
+      <c r="K34" s="4">
+        <v>5.2969999999999997</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A35" s="14"/>
+      <c r="B35" s="14"/>
+      <c r="C35" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D35" s="14"/>
+      <c r="E35" s="14"/>
+      <c r="F35" s="14"/>
+      <c r="G35" s="14"/>
+      <c r="H35" s="14"/>
+      <c r="I35" s="14"/>
+      <c r="J35" s="14"/>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A36" s="14"/>
+      <c r="B36" s="14"/>
+      <c r="C36" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D36" s="14"/>
+      <c r="E36" s="14"/>
+      <c r="F36" s="14"/>
+      <c r="G36" s="14"/>
+      <c r="H36" s="14"/>
+      <c r="I36" s="14"/>
+      <c r="J36" s="14"/>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A37" s="14"/>
+      <c r="B37" s="14"/>
+      <c r="C37" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D37" s="15"/>
+      <c r="E37" s="3"/>
+      <c r="F37" s="3"/>
+      <c r="G37" s="3"/>
+      <c r="H37" s="3"/>
+      <c r="I37" s="3"/>
+      <c r="J37" s="3"/>
+      <c r="K37" s="4"/>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A38" s="14"/>
+      <c r="B38" s="14"/>
+      <c r="C38" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D38" s="14"/>
+      <c r="E38" s="14"/>
+      <c r="F38" s="14"/>
+      <c r="G38" s="14"/>
+      <c r="H38" s="14"/>
+      <c r="I38" s="14"/>
+      <c r="J38" s="14"/>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A39" s="14"/>
+      <c r="B39" s="14"/>
+      <c r="C39" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D39" s="14"/>
+      <c r="E39" s="14"/>
+      <c r="F39" s="14"/>
+      <c r="G39" s="14"/>
+      <c r="H39" s="14"/>
+      <c r="I39" s="14"/>
+      <c r="J39" s="14"/>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A40" s="14"/>
+      <c r="B40" s="14"/>
+      <c r="C40" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D40" s="15"/>
+      <c r="E40" s="3"/>
+      <c r="F40" s="3"/>
+      <c r="G40" s="3"/>
+      <c r="H40" s="3"/>
+      <c r="I40" s="3"/>
+      <c r="J40" s="3"/>
+      <c r="K40" s="4"/>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A41" s="14"/>
+      <c r="B41" s="14"/>
+      <c r="C41" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D41" s="14"/>
+      <c r="E41" s="14"/>
+      <c r="F41" s="14"/>
+      <c r="G41" s="14"/>
+      <c r="H41" s="14"/>
+      <c r="I41" s="14"/>
+      <c r="J41" s="14"/>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A42" s="14"/>
+      <c r="B42" s="14"/>
+      <c r="C42" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D42" s="14"/>
+      <c r="E42" s="14"/>
+      <c r="F42" s="14"/>
+      <c r="G42" s="14"/>
+      <c r="H42" s="14"/>
+      <c r="I42" s="14"/>
+      <c r="J42" s="14"/>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A43" s="14"/>
+      <c r="B43" s="14"/>
+      <c r="C43" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D43" s="15"/>
+      <c r="E43" s="3"/>
+      <c r="F43" s="3"/>
+      <c r="G43" s="3"/>
+      <c r="H43" s="3"/>
+      <c r="I43" s="3"/>
+      <c r="J43" s="3"/>
+      <c r="K43" s="4"/>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C44" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C45" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A46" s="3"/>
+      <c r="B46" s="3"/>
+      <c r="C46" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D46" s="3"/>
+      <c r="E46" s="3"/>
+      <c r="F46" s="3"/>
+      <c r="G46" s="3"/>
+      <c r="H46" s="3"/>
+      <c r="I46" s="3"/>
+      <c r="J46" s="3"/>
+      <c r="K46" s="4"/>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A47" s="14">
+        <v>900</v>
+      </c>
+      <c r="B47" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D47" s="14">
+        <v>17.937000000000001</v>
+      </c>
+      <c r="E47" s="14">
+        <v>7.4195000000000002</v>
+      </c>
+      <c r="F47" s="14">
+        <v>15.250999999999999</v>
+      </c>
+      <c r="G47" s="14">
+        <v>2.4441999999999999</v>
+      </c>
+      <c r="H47" s="14">
+        <v>9880.2000000000007</v>
+      </c>
+      <c r="I47" s="14"/>
+      <c r="J47" s="14"/>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A48" s="14"/>
+      <c r="B48" s="14"/>
+      <c r="C48" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D48" s="14"/>
+      <c r="E48" s="14"/>
+      <c r="F48" s="14"/>
+      <c r="G48" s="14"/>
+      <c r="H48" s="14"/>
+      <c r="I48" s="14">
+        <v>1271.0999999999999</v>
+      </c>
+      <c r="J48" s="14">
+        <v>5.1067</v>
+      </c>
+      <c r="K48" s="1">
+        <v>13.686999999999999</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A49" s="14"/>
+      <c r="B49" s="14"/>
+      <c r="C49" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D49" s="15">
+        <v>17.937000000000001</v>
+      </c>
+      <c r="E49" s="3">
+        <v>7.3311999999999999</v>
+      </c>
+      <c r="F49" s="3">
+        <v>14.571999999999999</v>
+      </c>
+      <c r="G49" s="3">
+        <v>2.4605000000000001</v>
+      </c>
+      <c r="H49" s="3">
+        <v>10468</v>
+      </c>
+      <c r="I49" s="3">
+        <v>1426.3</v>
+      </c>
+      <c r="J49" s="3">
+        <v>4.8376000000000001</v>
+      </c>
+      <c r="K49" s="4">
+        <v>9.0043000000000006</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A50" s="14"/>
+      <c r="B50" s="14"/>
+      <c r="C50" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D50" s="14"/>
+      <c r="E50" s="14"/>
+      <c r="F50" s="14"/>
+      <c r="G50" s="14"/>
+      <c r="H50" s="14"/>
+      <c r="I50" s="14"/>
+      <c r="J50" s="14"/>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A51" s="14"/>
+      <c r="B51" s="14"/>
+      <c r="C51" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D51" s="14"/>
+      <c r="E51" s="14"/>
+      <c r="F51" s="14"/>
+      <c r="G51" s="14"/>
+      <c r="H51" s="14"/>
+      <c r="I51" s="14"/>
+      <c r="J51" s="14"/>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A52" s="14"/>
+      <c r="B52" s="14"/>
+      <c r="C52" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D52" s="15"/>
+      <c r="E52" s="3"/>
+      <c r="F52" s="3"/>
+      <c r="G52" s="3"/>
+      <c r="H52" s="3"/>
+      <c r="I52" s="3"/>
+      <c r="J52" s="3"/>
+      <c r="K52" s="4"/>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A53" s="14"/>
+      <c r="B53" s="14"/>
+      <c r="C53" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D53" s="14"/>
+      <c r="E53" s="14"/>
+      <c r="F53" s="14"/>
+      <c r="G53" s="14"/>
+      <c r="H53" s="14"/>
+      <c r="I53" s="14"/>
+      <c r="J53" s="14"/>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A54" s="14"/>
+      <c r="B54" s="14"/>
+      <c r="C54" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D54" s="14"/>
+      <c r="E54" s="14"/>
+      <c r="F54" s="14"/>
+      <c r="G54" s="14"/>
+      <c r="H54" s="14"/>
+      <c r="I54" s="14"/>
+      <c r="J54" s="14"/>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A55" s="14"/>
+      <c r="B55" s="14"/>
+      <c r="C55" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D55" s="15"/>
+      <c r="E55" s="3"/>
+      <c r="F55" s="3"/>
+      <c r="G55" s="3"/>
+      <c r="H55" s="3"/>
+      <c r="I55" s="3"/>
+      <c r="J55" s="3"/>
+      <c r="K55" s="4"/>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A56" s="14"/>
+      <c r="B56" s="14"/>
+      <c r="C56" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D56" s="14"/>
+      <c r="E56" s="14"/>
+      <c r="F56" s="14"/>
+      <c r="G56" s="14"/>
+      <c r="H56" s="14"/>
+      <c r="I56" s="14"/>
+      <c r="J56" s="14"/>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A57" s="14"/>
+      <c r="B57" s="14"/>
+      <c r="C57" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D57" s="14"/>
+      <c r="E57" s="14"/>
+      <c r="F57" s="14"/>
+      <c r="G57" s="14"/>
+      <c r="H57" s="14"/>
+      <c r="I57" s="14"/>
+      <c r="J57" s="14"/>
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A58" s="14"/>
+      <c r="B58" s="14"/>
+      <c r="C58" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D58" s="15"/>
+      <c r="E58" s="3"/>
+      <c r="F58" s="3"/>
+      <c r="G58" s="3"/>
+      <c r="H58" s="3"/>
+      <c r="I58" s="3"/>
+      <c r="J58" s="3"/>
+      <c r="K58" s="4"/>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C59" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C60" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A61" s="3"/>
+      <c r="B61" s="3"/>
+      <c r="C61" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D61" s="3"/>
+      <c r="E61" s="3"/>
+      <c r="F61" s="3"/>
+      <c r="G61" s="3"/>
+      <c r="H61" s="3"/>
+      <c r="I61" s="3"/>
+      <c r="J61" s="3"/>
+      <c r="K61" s="4"/>
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A62" s="14">
         <v>1000</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="B62" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D62" s="14"/>
+      <c r="E62" s="14"/>
+      <c r="F62" s="14"/>
+      <c r="G62" s="14"/>
+      <c r="H62" s="14"/>
+      <c r="I62" s="14"/>
+      <c r="J62" s="14"/>
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A63" s="14"/>
+      <c r="B63" s="14"/>
+      <c r="C63" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D63" s="14"/>
+      <c r="E63" s="14"/>
+      <c r="F63" s="14"/>
+      <c r="G63" s="14"/>
+      <c r="H63" s="14"/>
+      <c r="I63" s="14"/>
+      <c r="J63" s="14"/>
+    </row>
+    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A64" s="14"/>
+      <c r="B64" s="14"/>
+      <c r="C64" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D64" s="15"/>
+      <c r="E64" s="3"/>
+      <c r="F64" s="3"/>
+      <c r="G64" s="3"/>
+      <c r="H64" s="3"/>
+      <c r="I64" s="3"/>
+      <c r="J64" s="3"/>
+      <c r="K64" s="4"/>
+    </row>
+    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A65" s="14"/>
+      <c r="B65" s="14"/>
+      <c r="C65" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D65" s="14"/>
+      <c r="E65" s="14"/>
+      <c r="F65" s="14"/>
+      <c r="G65" s="14"/>
+      <c r="H65" s="14"/>
+      <c r="I65" s="14"/>
+      <c r="J65" s="14"/>
+    </row>
+    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A66" s="14"/>
+      <c r="B66" s="14"/>
+      <c r="C66" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D66" s="14"/>
+      <c r="E66" s="14"/>
+      <c r="F66" s="14"/>
+      <c r="G66" s="14"/>
+      <c r="H66" s="14"/>
+      <c r="I66" s="14"/>
+      <c r="J66" s="14"/>
+    </row>
+    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A67" s="14"/>
+      <c r="B67" s="14"/>
+      <c r="C67" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D67" s="15"/>
+      <c r="E67" s="3"/>
+      <c r="F67" s="3"/>
+      <c r="G67" s="3"/>
+      <c r="H67" s="3"/>
+      <c r="I67" s="3"/>
+      <c r="J67" s="3"/>
+      <c r="K67" s="4"/>
+    </row>
+    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A68" s="14"/>
+      <c r="B68" s="14"/>
+      <c r="C68" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D68" s="14"/>
+      <c r="E68" s="14"/>
+      <c r="F68" s="14"/>
+      <c r="G68" s="14"/>
+      <c r="H68" s="14"/>
+      <c r="I68" s="14"/>
+      <c r="J68" s="14"/>
+    </row>
+    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A69" s="14"/>
+      <c r="B69" s="14"/>
+      <c r="C69" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D69" s="14"/>
+      <c r="E69" s="14"/>
+      <c r="F69" s="14"/>
+      <c r="G69" s="14"/>
+      <c r="H69" s="14"/>
+      <c r="I69" s="14"/>
+      <c r="J69" s="14"/>
+    </row>
+    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A70" s="14"/>
+      <c r="B70" s="14"/>
+      <c r="C70" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D70" s="15"/>
+      <c r="E70" s="3"/>
+      <c r="F70" s="3"/>
+      <c r="G70" s="3"/>
+      <c r="H70" s="3"/>
+      <c r="I70" s="3"/>
+      <c r="J70" s="3"/>
+      <c r="K70" s="4"/>
+    </row>
+    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A71" s="14"/>
+      <c r="B71" s="14"/>
+      <c r="C71" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D71" s="14"/>
+      <c r="E71" s="14"/>
+      <c r="F71" s="14"/>
+      <c r="G71" s="14"/>
+      <c r="H71" s="14"/>
+      <c r="I71" s="14"/>
+      <c r="J71" s="14"/>
+    </row>
+    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A72" s="14"/>
+      <c r="B72" s="14"/>
+      <c r="C72" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D72" s="14"/>
+      <c r="E72" s="14"/>
+      <c r="F72" s="14"/>
+      <c r="G72" s="14"/>
+      <c r="H72" s="14"/>
+      <c r="I72" s="14"/>
+      <c r="J72" s="14"/>
+    </row>
+    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A73" s="14"/>
+      <c r="B73" s="14"/>
+      <c r="C73" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D73" s="15"/>
+      <c r="E73" s="3"/>
+      <c r="F73" s="3"/>
+      <c r="G73" s="3"/>
+      <c r="H73" s="3"/>
+      <c r="I73" s="3"/>
+      <c r="J73" s="3"/>
+      <c r="K73" s="4"/>
+    </row>
+    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C74" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C75" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A76" s="3"/>
+      <c r="B76" s="3"/>
+      <c r="C76" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D76" s="3"/>
+      <c r="E76" s="3"/>
+      <c r="F76" s="3"/>
+      <c r="G76" s="3"/>
+      <c r="H76" s="3"/>
+      <c r="I76" s="3"/>
+      <c r="J76" s="3"/>
+      <c r="K76" s="4"/>
+    </row>
+    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A77" s="14">
+        <v>1000</v>
+      </c>
+      <c r="B77" s="14" t="s">
         <v>8</v>
       </c>
+      <c r="C77" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D77" s="14"/>
+      <c r="E77" s="14"/>
+      <c r="F77" s="14"/>
+      <c r="G77" s="14"/>
+      <c r="H77" s="14"/>
+      <c r="I77" s="14"/>
+      <c r="J77" s="14"/>
+    </row>
+    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A78" s="14"/>
+      <c r="B78" s="14"/>
+      <c r="C78" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D78" s="14"/>
+      <c r="E78" s="14"/>
+      <c r="F78" s="14"/>
+      <c r="G78" s="14"/>
+      <c r="H78" s="14"/>
+      <c r="I78" s="14"/>
+      <c r="J78" s="14"/>
+    </row>
+    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A79" s="14"/>
+      <c r="B79" s="14"/>
+      <c r="C79" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D79" s="15"/>
+      <c r="E79" s="3"/>
+      <c r="F79" s="3"/>
+      <c r="G79" s="3"/>
+      <c r="H79" s="3"/>
+      <c r="I79" s="3"/>
+      <c r="J79" s="3"/>
+      <c r="K79" s="4"/>
+    </row>
+    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A80" s="14"/>
+      <c r="B80" s="14"/>
+      <c r="C80" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D80" s="14"/>
+      <c r="E80" s="14"/>
+      <c r="F80" s="14"/>
+      <c r="G80" s="14"/>
+      <c r="H80" s="14"/>
+      <c r="I80" s="14"/>
+      <c r="J80" s="14"/>
+    </row>
+    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A81" s="14"/>
+      <c r="B81" s="14"/>
+      <c r="C81" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D81" s="14"/>
+      <c r="E81" s="14"/>
+      <c r="F81" s="14"/>
+      <c r="G81" s="14"/>
+      <c r="H81" s="14"/>
+      <c r="I81" s="14"/>
+      <c r="J81" s="14"/>
+    </row>
+    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A82" s="14"/>
+      <c r="B82" s="14"/>
+      <c r="C82" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D82" s="15"/>
+      <c r="E82" s="3"/>
+      <c r="F82" s="3"/>
+      <c r="G82" s="3"/>
+      <c r="H82" s="3"/>
+      <c r="I82" s="3"/>
+      <c r="J82" s="3"/>
+      <c r="K82" s="4"/>
+    </row>
+    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A83" s="14"/>
+      <c r="B83" s="14"/>
+      <c r="C83" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D83" s="14"/>
+      <c r="E83" s="14"/>
+      <c r="F83" s="14"/>
+      <c r="G83" s="14"/>
+      <c r="H83" s="14"/>
+      <c r="I83" s="14"/>
+      <c r="J83" s="14"/>
+    </row>
+    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A84" s="14"/>
+      <c r="B84" s="14"/>
+      <c r="C84" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D84" s="14"/>
+      <c r="E84" s="14"/>
+      <c r="F84" s="14"/>
+      <c r="G84" s="14"/>
+      <c r="H84" s="14"/>
+      <c r="I84" s="14"/>
+      <c r="J84" s="14"/>
+    </row>
+    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A85" s="14"/>
+      <c r="B85" s="14"/>
+      <c r="C85" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D85" s="15"/>
+      <c r="E85" s="3"/>
+      <c r="F85" s="3"/>
+      <c r="G85" s="3"/>
+      <c r="H85" s="3"/>
+      <c r="I85" s="3"/>
+      <c r="J85" s="3"/>
+      <c r="K85" s="4"/>
+    </row>
+    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A86" s="14"/>
+      <c r="B86" s="14"/>
+      <c r="C86" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D86" s="14"/>
+      <c r="E86" s="14"/>
+      <c r="F86" s="14"/>
+      <c r="G86" s="14"/>
+      <c r="H86" s="14"/>
+      <c r="I86" s="14"/>
+      <c r="J86" s="14"/>
+    </row>
+    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A87" s="14"/>
+      <c r="B87" s="14"/>
+      <c r="C87" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D87" s="14"/>
+      <c r="E87" s="14"/>
+      <c r="F87" s="14"/>
+      <c r="G87" s="14"/>
+      <c r="H87" s="14"/>
+      <c r="I87" s="14"/>
+      <c r="J87" s="14"/>
+    </row>
+    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A88" s="14"/>
+      <c r="B88" s="14"/>
+      <c r="C88" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D88" s="15"/>
+      <c r="E88" s="3"/>
+      <c r="F88" s="3"/>
+      <c r="G88" s="3"/>
+      <c r="H88" s="3"/>
+      <c r="I88" s="3"/>
+      <c r="J88" s="3"/>
+      <c r="K88" s="4"/>
+    </row>
+    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C89" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C90" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A91" s="3"/>
+      <c r="B91" s="3"/>
+      <c r="C91" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D91" s="3"/>
+      <c r="E91" s="3"/>
+      <c r="F91" s="3"/>
+      <c r="G91" s="3"/>
+      <c r="H91" s="3"/>
+      <c r="I91" s="3"/>
+      <c r="J91" s="3"/>
+      <c r="K91" s="4"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBE5B278-CF38-41EF-A268-D7BDDFF8B1FA}">
+  <dimension ref="A1:K91"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10:F11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="9.140625" style="2"/>
+    <col min="3" max="3" width="9.140625" style="1"/>
+    <col min="4" max="10" width="9.140625" style="2"/>
+    <col min="11" max="11" width="9.140625" style="1"/>
+    <col min="12" max="16384" width="9.140625" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="14">
+        <v>800</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="14">
+        <v>11.695</v>
+      </c>
+      <c r="E2" s="14">
+        <v>101.28</v>
+      </c>
+      <c r="F2" s="14">
+        <v>1.1411</v>
+      </c>
+      <c r="G2" s="14">
+        <v>4.6826999999999996</v>
+      </c>
+      <c r="H2" s="14">
+        <v>1595.5</v>
+      </c>
+      <c r="I2" s="14"/>
+      <c r="J2" s="14"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="14"/>
+      <c r="B3" s="14"/>
+      <c r="C3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="14"/>
+      <c r="G3" s="14"/>
+      <c r="H3" s="14"/>
+      <c r="I3" s="14"/>
+      <c r="J3" s="14"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="14"/>
+      <c r="B4" s="14"/>
+      <c r="C4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="15"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="4"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="14"/>
+      <c r="B5" s="14"/>
+      <c r="C5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="14">
+        <v>9.8171999999999997</v>
+      </c>
+      <c r="E5" s="14">
+        <v>101.47</v>
+      </c>
+      <c r="F5" s="14">
+        <v>1.4056999999999999</v>
+      </c>
+      <c r="G5" s="14">
+        <v>4.6856999999999998</v>
+      </c>
+      <c r="H5" s="14">
+        <v>1595.7</v>
+      </c>
+      <c r="I5" s="14"/>
+      <c r="J5" s="14"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="14"/>
+      <c r="B6" s="14"/>
+      <c r="C6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="14"/>
+      <c r="E6" s="14"/>
+      <c r="F6" s="14"/>
+      <c r="G6" s="14"/>
+      <c r="H6" s="14"/>
+      <c r="I6" s="14"/>
+      <c r="J6" s="14"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="14"/>
+      <c r="B7" s="14"/>
+      <c r="C7" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" s="15"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
+      <c r="K7" s="4"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="14"/>
+      <c r="B8" s="14"/>
+      <c r="C8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" s="14"/>
+      <c r="E8" s="14"/>
+      <c r="F8" s="14"/>
+      <c r="G8" s="14"/>
+      <c r="H8" s="14"/>
+      <c r="I8" s="14"/>
+      <c r="J8" s="14"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="14"/>
+      <c r="B9" s="14"/>
+      <c r="C9" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9" s="14"/>
+      <c r="E9" s="14"/>
+      <c r="F9" s="14"/>
+      <c r="G9" s="14"/>
+      <c r="H9" s="14"/>
+      <c r="I9" s="14"/>
+      <c r="J9" s="14"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="14"/>
+      <c r="B10" s="14"/>
+      <c r="C10" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D10" s="15"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="3"/>
+      <c r="J10" s="3"/>
+      <c r="K10" s="4"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="14"/>
+      <c r="B11" s="14"/>
+      <c r="C11" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D11" s="14"/>
+      <c r="E11" s="14"/>
+      <c r="F11" s="14"/>
+      <c r="G11" s="14"/>
+      <c r="H11" s="14"/>
+      <c r="I11" s="14"/>
+      <c r="J11" s="14"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="14"/>
+      <c r="B12" s="14"/>
+      <c r="C12" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D12" s="14"/>
+      <c r="E12" s="14"/>
+      <c r="F12" s="14"/>
+      <c r="G12" s="14"/>
+      <c r="H12" s="14"/>
+      <c r="I12" s="14"/>
+      <c r="J12" s="14"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" s="14"/>
+      <c r="B13" s="14"/>
+      <c r="C13" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D13" s="15"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
+      <c r="H13" s="3"/>
+      <c r="I13" s="3"/>
+      <c r="J13" s="3"/>
+      <c r="K13" s="4"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C14" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C15" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" s="3"/>
+      <c r="B16" s="3"/>
+      <c r="C16" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
+      <c r="H16" s="3"/>
+      <c r="I16" s="3"/>
+      <c r="J16" s="3"/>
+      <c r="K16" s="4"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" s="14">
+        <v>800</v>
+      </c>
+      <c r="B17" s="14" t="s">
+        <v>8</v>
+      </c>
       <c r="C17" s="1" t="s">
         <v>13</v>
       </c>
+      <c r="D17" s="14">
+        <v>31.327000000000002</v>
+      </c>
+      <c r="E17" s="14">
+        <v>104.92</v>
+      </c>
+      <c r="F17" s="14">
+        <v>0.8548</v>
+      </c>
+      <c r="G17" s="14">
+        <v>3.7507999999999999</v>
+      </c>
+      <c r="H17" s="14">
+        <v>2575.8000000000002</v>
+      </c>
+      <c r="I17" s="14"/>
+      <c r="J17" s="14"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" s="14"/>
+      <c r="B18" s="14"/>
       <c r="C18" s="1" t="s">
         <v>14</v>
       </c>
+      <c r="D18" s="14"/>
+      <c r="E18" s="14"/>
+      <c r="F18" s="14"/>
+      <c r="G18" s="14"/>
+      <c r="H18" s="14"/>
+      <c r="I18" s="14"/>
+      <c r="J18" s="14"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="3"/>
-      <c r="B19" s="3"/>
-      <c r="C19" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D19" s="3"/>
+      <c r="A19" s="14"/>
+      <c r="B19" s="14"/>
+      <c r="C19" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D19" s="15"/>
       <c r="E19" s="3"/>
       <c r="F19" s="3"/>
       <c r="G19" s="3"/>
@@ -1828,12 +3154,990 @@
       <c r="J19" s="3"/>
       <c r="K19" s="4"/>
     </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" s="14"/>
+      <c r="B20" s="14"/>
+      <c r="C20" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D20" s="14"/>
+      <c r="E20" s="14"/>
+      <c r="F20" s="14"/>
+      <c r="G20" s="14"/>
+      <c r="H20" s="14"/>
+      <c r="I20" s="14"/>
+      <c r="J20" s="14"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" s="14"/>
+      <c r="B21" s="14"/>
+      <c r="C21" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D21" s="14"/>
+      <c r="E21" s="14"/>
+      <c r="F21" s="14"/>
+      <c r="G21" s="14"/>
+      <c r="H21" s="14"/>
+      <c r="I21" s="14"/>
+      <c r="J21" s="14"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" s="14"/>
+      <c r="B22" s="14"/>
+      <c r="C22" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D22" s="15"/>
+      <c r="E22" s="3"/>
+      <c r="F22" s="3"/>
+      <c r="G22" s="3"/>
+      <c r="H22" s="3"/>
+      <c r="I22" s="3"/>
+      <c r="J22" s="3"/>
+      <c r="K22" s="4"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23" s="14"/>
+      <c r="B23" s="14"/>
+      <c r="C23" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D23" s="14"/>
+      <c r="E23" s="14"/>
+      <c r="F23" s="14"/>
+      <c r="G23" s="14"/>
+      <c r="H23" s="14"/>
+      <c r="I23" s="14"/>
+      <c r="J23" s="14"/>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24" s="14"/>
+      <c r="B24" s="14"/>
+      <c r="C24" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D24" s="14"/>
+      <c r="E24" s="14"/>
+      <c r="F24" s="14"/>
+      <c r="G24" s="14"/>
+      <c r="H24" s="14"/>
+      <c r="I24" s="14"/>
+      <c r="J24" s="14"/>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A25" s="14"/>
+      <c r="B25" s="14"/>
+      <c r="C25" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D25" s="15"/>
+      <c r="E25" s="3"/>
+      <c r="F25" s="3"/>
+      <c r="G25" s="3"/>
+      <c r="H25" s="3"/>
+      <c r="I25" s="3"/>
+      <c r="J25" s="3"/>
+      <c r="K25" s="4"/>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A26" s="14"/>
+      <c r="B26" s="14"/>
+      <c r="C26" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D26" s="14"/>
+      <c r="E26" s="14"/>
+      <c r="F26" s="14"/>
+      <c r="G26" s="14"/>
+      <c r="H26" s="14"/>
+      <c r="I26" s="14"/>
+      <c r="J26" s="14"/>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A27" s="14"/>
+      <c r="B27" s="14"/>
+      <c r="C27" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D27" s="14"/>
+      <c r="E27" s="14"/>
+      <c r="F27" s="14"/>
+      <c r="G27" s="14"/>
+      <c r="H27" s="14"/>
+      <c r="I27" s="14"/>
+      <c r="J27" s="14"/>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A28" s="14"/>
+      <c r="B28" s="14"/>
+      <c r="C28" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D28" s="15"/>
+      <c r="E28" s="3"/>
+      <c r="F28" s="3"/>
+      <c r="G28" s="3"/>
+      <c r="H28" s="3"/>
+      <c r="I28" s="3"/>
+      <c r="J28" s="3"/>
+      <c r="K28" s="4"/>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C29" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C30" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A31" s="3"/>
+      <c r="B31" s="3"/>
+      <c r="C31" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D31" s="3"/>
+      <c r="E31" s="3"/>
+      <c r="F31" s="3"/>
+      <c r="G31" s="3"/>
+      <c r="H31" s="3"/>
+      <c r="I31" s="3"/>
+      <c r="J31" s="3"/>
+      <c r="K31" s="4"/>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A32" s="14">
+        <v>900</v>
+      </c>
+      <c r="B32" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D32" s="14">
+        <v>4.8710000000000004</v>
+      </c>
+      <c r="E32" s="14">
+        <v>11.518000000000001</v>
+      </c>
+      <c r="F32" s="14">
+        <v>7.0281000000000002</v>
+      </c>
+      <c r="G32" s="14">
+        <v>4.2420999999999998</v>
+      </c>
+      <c r="H32" s="14">
+        <v>1138.3</v>
+      </c>
+      <c r="I32" s="14"/>
+      <c r="J32" s="14"/>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A33" s="14"/>
+      <c r="B33" s="14"/>
+      <c r="C33" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D33" s="14"/>
+      <c r="E33" s="14"/>
+      <c r="F33" s="14"/>
+      <c r="G33" s="14"/>
+      <c r="H33" s="14"/>
+      <c r="I33" s="14"/>
+      <c r="J33" s="14"/>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A34" s="14"/>
+      <c r="B34" s="14"/>
+      <c r="C34" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D34" s="15"/>
+      <c r="E34" s="3"/>
+      <c r="F34" s="3"/>
+      <c r="G34" s="3"/>
+      <c r="H34" s="3"/>
+      <c r="I34" s="3"/>
+      <c r="J34" s="3"/>
+      <c r="K34" s="4"/>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A35" s="14"/>
+      <c r="B35" s="14"/>
+      <c r="C35" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D35" s="14"/>
+      <c r="E35" s="14"/>
+      <c r="F35" s="14"/>
+      <c r="G35" s="14"/>
+      <c r="H35" s="14"/>
+      <c r="I35" s="14"/>
+      <c r="J35" s="14"/>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A36" s="14"/>
+      <c r="B36" s="14"/>
+      <c r="C36" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D36" s="14"/>
+      <c r="E36" s="14"/>
+      <c r="F36" s="14"/>
+      <c r="G36" s="14"/>
+      <c r="H36" s="14"/>
+      <c r="I36" s="14"/>
+      <c r="J36" s="14"/>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A37" s="14"/>
+      <c r="B37" s="14"/>
+      <c r="C37" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D37" s="15"/>
+      <c r="E37" s="3"/>
+      <c r="F37" s="3"/>
+      <c r="G37" s="3"/>
+      <c r="H37" s="3"/>
+      <c r="I37" s="3"/>
+      <c r="J37" s="3"/>
+      <c r="K37" s="4"/>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A38" s="14"/>
+      <c r="B38" s="14"/>
+      <c r="C38" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D38" s="14"/>
+      <c r="E38" s="14"/>
+      <c r="F38" s="14"/>
+      <c r="G38" s="14"/>
+      <c r="H38" s="14"/>
+      <c r="I38" s="14"/>
+      <c r="J38" s="14"/>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A39" s="14"/>
+      <c r="B39" s="14"/>
+      <c r="C39" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D39" s="14"/>
+      <c r="E39" s="14"/>
+      <c r="F39" s="14"/>
+      <c r="G39" s="14"/>
+      <c r="H39" s="14"/>
+      <c r="I39" s="14"/>
+      <c r="J39" s="14"/>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A40" s="14"/>
+      <c r="B40" s="14"/>
+      <c r="C40" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D40" s="15"/>
+      <c r="E40" s="3"/>
+      <c r="F40" s="3"/>
+      <c r="G40" s="3"/>
+      <c r="H40" s="3"/>
+      <c r="I40" s="3"/>
+      <c r="J40" s="3"/>
+      <c r="K40" s="4"/>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A41" s="14"/>
+      <c r="B41" s="14"/>
+      <c r="C41" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D41" s="14"/>
+      <c r="E41" s="14"/>
+      <c r="F41" s="14"/>
+      <c r="G41" s="14"/>
+      <c r="H41" s="14"/>
+      <c r="I41" s="14"/>
+      <c r="J41" s="14"/>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A42" s="14"/>
+      <c r="B42" s="14"/>
+      <c r="C42" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D42" s="14"/>
+      <c r="E42" s="14"/>
+      <c r="F42" s="14"/>
+      <c r="G42" s="14"/>
+      <c r="H42" s="14"/>
+      <c r="I42" s="14"/>
+      <c r="J42" s="14"/>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A43" s="14"/>
+      <c r="B43" s="14"/>
+      <c r="C43" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D43" s="15"/>
+      <c r="E43" s="3"/>
+      <c r="F43" s="3"/>
+      <c r="G43" s="3"/>
+      <c r="H43" s="3"/>
+      <c r="I43" s="3"/>
+      <c r="J43" s="3"/>
+      <c r="K43" s="4"/>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C44" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C45" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A46" s="3"/>
+      <c r="B46" s="3"/>
+      <c r="C46" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D46" s="3"/>
+      <c r="E46" s="3"/>
+      <c r="F46" s="3"/>
+      <c r="G46" s="3"/>
+      <c r="H46" s="3"/>
+      <c r="I46" s="3"/>
+      <c r="J46" s="3"/>
+      <c r="K46" s="4"/>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A47" s="14">
+        <v>900</v>
+      </c>
+      <c r="B47" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D47" s="14">
+        <v>4.8238000000000003</v>
+      </c>
+      <c r="E47" s="14">
+        <v>378.86</v>
+      </c>
+      <c r="F47" s="14">
+        <v>0.14230000000000001</v>
+      </c>
+      <c r="G47" s="14">
+        <v>4.4020999999999999</v>
+      </c>
+      <c r="H47" s="14">
+        <v>1006.9</v>
+      </c>
+      <c r="I47" s="14"/>
+      <c r="J47" s="14"/>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A48" s="14"/>
+      <c r="B48" s="14"/>
+      <c r="C48" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D48" s="14"/>
+      <c r="E48" s="14"/>
+      <c r="F48" s="14"/>
+      <c r="G48" s="14"/>
+      <c r="H48" s="14"/>
+      <c r="I48" s="14"/>
+      <c r="J48" s="14"/>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A49" s="14"/>
+      <c r="B49" s="14"/>
+      <c r="C49" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D49" s="15"/>
+      <c r="E49" s="3"/>
+      <c r="F49" s="3"/>
+      <c r="G49" s="3"/>
+      <c r="H49" s="3"/>
+      <c r="I49" s="3"/>
+      <c r="J49" s="3"/>
+      <c r="K49" s="4"/>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A50" s="14"/>
+      <c r="B50" s="14"/>
+      <c r="C50" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D50" s="14"/>
+      <c r="E50" s="14"/>
+      <c r="F50" s="14"/>
+      <c r="G50" s="14"/>
+      <c r="H50" s="14"/>
+      <c r="I50" s="14"/>
+      <c r="J50" s="14"/>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A51" s="14"/>
+      <c r="B51" s="14"/>
+      <c r="C51" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D51" s="14"/>
+      <c r="E51" s="14"/>
+      <c r="F51" s="14"/>
+      <c r="G51" s="14"/>
+      <c r="H51" s="14"/>
+      <c r="I51" s="14"/>
+      <c r="J51" s="14"/>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A52" s="14"/>
+      <c r="B52" s="14"/>
+      <c r="C52" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D52" s="15"/>
+      <c r="E52" s="3"/>
+      <c r="F52" s="3"/>
+      <c r="G52" s="3"/>
+      <c r="H52" s="3"/>
+      <c r="I52" s="3"/>
+      <c r="J52" s="3"/>
+      <c r="K52" s="4"/>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A53" s="14"/>
+      <c r="B53" s="14"/>
+      <c r="C53" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D53" s="14"/>
+      <c r="E53" s="14"/>
+      <c r="F53" s="14"/>
+      <c r="G53" s="14"/>
+      <c r="H53" s="14"/>
+      <c r="I53" s="14"/>
+      <c r="J53" s="14"/>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A54" s="14"/>
+      <c r="B54" s="14"/>
+      <c r="C54" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D54" s="14"/>
+      <c r="E54" s="14"/>
+      <c r="F54" s="14"/>
+      <c r="G54" s="14"/>
+      <c r="H54" s="14"/>
+      <c r="I54" s="14"/>
+      <c r="J54" s="14"/>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A55" s="14"/>
+      <c r="B55" s="14"/>
+      <c r="C55" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D55" s="15"/>
+      <c r="E55" s="3"/>
+      <c r="F55" s="3"/>
+      <c r="G55" s="3"/>
+      <c r="H55" s="3"/>
+      <c r="I55" s="3"/>
+      <c r="J55" s="3"/>
+      <c r="K55" s="4"/>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A56" s="14"/>
+      <c r="B56" s="14"/>
+      <c r="C56" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D56" s="14"/>
+      <c r="E56" s="14"/>
+      <c r="F56" s="14"/>
+      <c r="G56" s="14"/>
+      <c r="H56" s="14"/>
+      <c r="I56" s="14"/>
+      <c r="J56" s="14"/>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A57" s="14"/>
+      <c r="B57" s="14"/>
+      <c r="C57" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D57" s="14"/>
+      <c r="E57" s="14"/>
+      <c r="F57" s="14"/>
+      <c r="G57" s="14"/>
+      <c r="H57" s="14"/>
+      <c r="I57" s="14"/>
+      <c r="J57" s="14"/>
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A58" s="14"/>
+      <c r="B58" s="14"/>
+      <c r="C58" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D58" s="15"/>
+      <c r="E58" s="3"/>
+      <c r="F58" s="3"/>
+      <c r="G58" s="3"/>
+      <c r="H58" s="3"/>
+      <c r="I58" s="3"/>
+      <c r="J58" s="3"/>
+      <c r="K58" s="4"/>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C59" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C60" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A61" s="3"/>
+      <c r="B61" s="3"/>
+      <c r="C61" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D61" s="3"/>
+      <c r="E61" s="3"/>
+      <c r="F61" s="3"/>
+      <c r="G61" s="3"/>
+      <c r="H61" s="3"/>
+      <c r="I61" s="3"/>
+      <c r="J61" s="3"/>
+      <c r="K61" s="4"/>
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A62" s="14">
+        <v>1000</v>
+      </c>
+      <c r="B62" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D62" s="14"/>
+      <c r="E62" s="14"/>
+      <c r="F62" s="14"/>
+      <c r="G62" s="14"/>
+      <c r="H62" s="14"/>
+      <c r="I62" s="14"/>
+      <c r="J62" s="14"/>
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A63" s="14"/>
+      <c r="B63" s="14"/>
+      <c r="C63" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D63" s="14"/>
+      <c r="E63" s="14"/>
+      <c r="F63" s="14"/>
+      <c r="G63" s="14"/>
+      <c r="H63" s="14"/>
+      <c r="I63" s="14"/>
+      <c r="J63" s="14"/>
+    </row>
+    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A64" s="14"/>
+      <c r="B64" s="14"/>
+      <c r="C64" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D64" s="15"/>
+      <c r="E64" s="3"/>
+      <c r="F64" s="3"/>
+      <c r="G64" s="3"/>
+      <c r="H64" s="3"/>
+      <c r="I64" s="3"/>
+      <c r="J64" s="3"/>
+      <c r="K64" s="4"/>
+    </row>
+    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A65" s="14"/>
+      <c r="B65" s="14"/>
+      <c r="C65" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D65" s="14"/>
+      <c r="E65" s="14"/>
+      <c r="F65" s="14"/>
+      <c r="G65" s="14"/>
+      <c r="H65" s="14"/>
+      <c r="I65" s="14"/>
+      <c r="J65" s="14"/>
+    </row>
+    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A66" s="14"/>
+      <c r="B66" s="14"/>
+      <c r="C66" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D66" s="14"/>
+      <c r="E66" s="14"/>
+      <c r="F66" s="14"/>
+      <c r="G66" s="14"/>
+      <c r="H66" s="14"/>
+      <c r="I66" s="14"/>
+      <c r="J66" s="14"/>
+    </row>
+    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A67" s="14"/>
+      <c r="B67" s="14"/>
+      <c r="C67" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D67" s="15"/>
+      <c r="E67" s="3"/>
+      <c r="F67" s="3"/>
+      <c r="G67" s="3"/>
+      <c r="H67" s="3"/>
+      <c r="I67" s="3"/>
+      <c r="J67" s="3"/>
+      <c r="K67" s="4"/>
+    </row>
+    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A68" s="14"/>
+      <c r="B68" s="14"/>
+      <c r="C68" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D68" s="14"/>
+      <c r="E68" s="14"/>
+      <c r="F68" s="14"/>
+      <c r="G68" s="14"/>
+      <c r="H68" s="14"/>
+      <c r="I68" s="14"/>
+      <c r="J68" s="14"/>
+    </row>
+    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A69" s="14"/>
+      <c r="B69" s="14"/>
+      <c r="C69" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D69" s="14"/>
+      <c r="E69" s="14"/>
+      <c r="F69" s="14"/>
+      <c r="G69" s="14"/>
+      <c r="H69" s="14"/>
+      <c r="I69" s="14"/>
+      <c r="J69" s="14"/>
+    </row>
+    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A70" s="14"/>
+      <c r="B70" s="14"/>
+      <c r="C70" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D70" s="15"/>
+      <c r="E70" s="3"/>
+      <c r="F70" s="3"/>
+      <c r="G70" s="3"/>
+      <c r="H70" s="3"/>
+      <c r="I70" s="3"/>
+      <c r="J70" s="3"/>
+      <c r="K70" s="4"/>
+    </row>
+    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A71" s="14"/>
+      <c r="B71" s="14"/>
+      <c r="C71" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D71" s="14"/>
+      <c r="E71" s="14"/>
+      <c r="F71" s="14"/>
+      <c r="G71" s="14"/>
+      <c r="H71" s="14"/>
+      <c r="I71" s="14"/>
+      <c r="J71" s="14"/>
+    </row>
+    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A72" s="14"/>
+      <c r="B72" s="14"/>
+      <c r="C72" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D72" s="14"/>
+      <c r="E72" s="14"/>
+      <c r="F72" s="14"/>
+      <c r="G72" s="14"/>
+      <c r="H72" s="14"/>
+      <c r="I72" s="14"/>
+      <c r="J72" s="14"/>
+    </row>
+    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A73" s="14"/>
+      <c r="B73" s="14"/>
+      <c r="C73" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D73" s="15"/>
+      <c r="E73" s="3"/>
+      <c r="F73" s="3"/>
+      <c r="G73" s="3"/>
+      <c r="H73" s="3"/>
+      <c r="I73" s="3"/>
+      <c r="J73" s="3"/>
+      <c r="K73" s="4"/>
+    </row>
+    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C74" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C75" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A76" s="3"/>
+      <c r="B76" s="3"/>
+      <c r="C76" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D76" s="3"/>
+      <c r="E76" s="3"/>
+      <c r="F76" s="3"/>
+      <c r="G76" s="3"/>
+      <c r="H76" s="3"/>
+      <c r="I76" s="3"/>
+      <c r="J76" s="3"/>
+      <c r="K76" s="4"/>
+    </row>
+    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A77" s="14">
+        <v>1000</v>
+      </c>
+      <c r="B77" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="C77" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D77" s="14"/>
+      <c r="E77" s="14"/>
+      <c r="F77" s="14"/>
+      <c r="G77" s="14"/>
+      <c r="H77" s="14"/>
+      <c r="I77" s="14"/>
+      <c r="J77" s="14"/>
+    </row>
+    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A78" s="14"/>
+      <c r="B78" s="14"/>
+      <c r="C78" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D78" s="14"/>
+      <c r="E78" s="14"/>
+      <c r="F78" s="14"/>
+      <c r="G78" s="14"/>
+      <c r="H78" s="14"/>
+      <c r="I78" s="14"/>
+      <c r="J78" s="14"/>
+    </row>
+    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A79" s="14"/>
+      <c r="B79" s="14"/>
+      <c r="C79" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D79" s="15"/>
+      <c r="E79" s="3"/>
+      <c r="F79" s="3"/>
+      <c r="G79" s="3"/>
+      <c r="H79" s="3"/>
+      <c r="I79" s="3"/>
+      <c r="J79" s="3"/>
+      <c r="K79" s="4"/>
+    </row>
+    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A80" s="14"/>
+      <c r="B80" s="14"/>
+      <c r="C80" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D80" s="14"/>
+      <c r="E80" s="14"/>
+      <c r="F80" s="14"/>
+      <c r="G80" s="14"/>
+      <c r="H80" s="14"/>
+      <c r="I80" s="14"/>
+      <c r="J80" s="14"/>
+    </row>
+    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A81" s="14"/>
+      <c r="B81" s="14"/>
+      <c r="C81" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D81" s="14"/>
+      <c r="E81" s="14"/>
+      <c r="F81" s="14"/>
+      <c r="G81" s="14"/>
+      <c r="H81" s="14"/>
+      <c r="I81" s="14"/>
+      <c r="J81" s="14"/>
+    </row>
+    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A82" s="14"/>
+      <c r="B82" s="14"/>
+      <c r="C82" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D82" s="15"/>
+      <c r="E82" s="3"/>
+      <c r="F82" s="3"/>
+      <c r="G82" s="3"/>
+      <c r="H82" s="3"/>
+      <c r="I82" s="3"/>
+      <c r="J82" s="3"/>
+      <c r="K82" s="4"/>
+    </row>
+    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A83" s="14"/>
+      <c r="B83" s="14"/>
+      <c r="C83" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D83" s="14"/>
+      <c r="E83" s="14"/>
+      <c r="F83" s="14"/>
+      <c r="G83" s="14"/>
+      <c r="H83" s="14"/>
+      <c r="I83" s="14"/>
+      <c r="J83" s="14"/>
+    </row>
+    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A84" s="14"/>
+      <c r="B84" s="14"/>
+      <c r="C84" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D84" s="14"/>
+      <c r="E84" s="14"/>
+      <c r="F84" s="14"/>
+      <c r="G84" s="14"/>
+      <c r="H84" s="14"/>
+      <c r="I84" s="14"/>
+      <c r="J84" s="14"/>
+    </row>
+    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A85" s="14"/>
+      <c r="B85" s="14"/>
+      <c r="C85" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D85" s="15"/>
+      <c r="E85" s="3"/>
+      <c r="F85" s="3"/>
+      <c r="G85" s="3"/>
+      <c r="H85" s="3"/>
+      <c r="I85" s="3"/>
+      <c r="J85" s="3"/>
+      <c r="K85" s="4"/>
+    </row>
+    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A86" s="14"/>
+      <c r="B86" s="14"/>
+      <c r="C86" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D86" s="14"/>
+      <c r="E86" s="14"/>
+      <c r="F86" s="14"/>
+      <c r="G86" s="14"/>
+      <c r="H86" s="14"/>
+      <c r="I86" s="14"/>
+      <c r="J86" s="14"/>
+    </row>
+    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A87" s="14"/>
+      <c r="B87" s="14"/>
+      <c r="C87" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D87" s="14"/>
+      <c r="E87" s="14"/>
+      <c r="F87" s="14"/>
+      <c r="G87" s="14"/>
+      <c r="H87" s="14"/>
+      <c r="I87" s="14"/>
+      <c r="J87" s="14"/>
+    </row>
+    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A88" s="14"/>
+      <c r="B88" s="14"/>
+      <c r="C88" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D88" s="15"/>
+      <c r="E88" s="3"/>
+      <c r="F88" s="3"/>
+      <c r="G88" s="3"/>
+      <c r="H88" s="3"/>
+      <c r="I88" s="3"/>
+      <c r="J88" s="3"/>
+      <c r="K88" s="4"/>
+    </row>
+    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C89" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C90" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A91" s="3"/>
+      <c r="B91" s="3"/>
+      <c r="C91" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D91" s="3"/>
+      <c r="E91" s="3"/>
+      <c r="F91" s="3"/>
+      <c r="G91" s="3"/>
+      <c r="H91" s="3"/>
+      <c r="I91" s="3"/>
+      <c r="J91" s="3"/>
+      <c r="K91" s="4"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59578D89-F974-462A-A8BE-33C4579641C9}">
   <dimension ref="A1:E7"/>
   <sheetViews>
@@ -1935,268 +4239,6 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8265FA44-8E85-43C1-8A54-AE4FC552DE01}">
-  <dimension ref="A1:N13"/>
-  <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="2" width="9.140625" style="2"/>
-    <col min="3" max="3" width="9.140625" style="1"/>
-    <col min="4" max="13" width="9.140625" style="2"/>
-    <col min="14" max="14" width="9.140625" style="1"/>
-    <col min="15" max="16384" width="9.140625" style="2"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="L1" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="M1" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="N1" s="4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" s="2">
-        <v>800</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D2" s="2">
-        <v>11.695</v>
-      </c>
-      <c r="E2" s="2">
-        <v>101.28</v>
-      </c>
-      <c r="F2" s="2">
-        <v>1.1411</v>
-      </c>
-      <c r="G2" s="2">
-        <v>4.6826999999999996</v>
-      </c>
-      <c r="H2" s="2">
-        <v>1595.5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="C3" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A4" s="3"/>
-      <c r="B4" s="3"/>
-      <c r="C4" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
-      <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
-      <c r="K4" s="3"/>
-      <c r="L4" s="3"/>
-      <c r="M4" s="3"/>
-      <c r="N4" s="4"/>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A5" s="2">
-        <v>800</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D5" s="2">
-        <v>31.327000000000002</v>
-      </c>
-      <c r="E5" s="2">
-        <v>104.92</v>
-      </c>
-      <c r="F5" s="2">
-        <v>0.8548</v>
-      </c>
-      <c r="G5" s="2">
-        <v>3.7507999999999999</v>
-      </c>
-      <c r="H5" s="2">
-        <v>2575.8000000000002</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="C6" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A7" s="3"/>
-      <c r="B7" s="3"/>
-      <c r="C7" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
-      <c r="I7" s="3"/>
-      <c r="J7" s="3"/>
-      <c r="K7" s="3"/>
-      <c r="L7" s="3"/>
-      <c r="M7" s="3"/>
-      <c r="N7" s="4"/>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A8" s="2">
-        <v>900</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D8" s="2">
-        <v>4.8710000000000004</v>
-      </c>
-      <c r="E8" s="2">
-        <v>11.518000000000001</v>
-      </c>
-      <c r="F8" s="2">
-        <v>7.0281000000000002</v>
-      </c>
-      <c r="G8" s="2">
-        <v>4.2420999999999998</v>
-      </c>
-      <c r="H8" s="2">
-        <v>1138.3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="C9" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A10" s="3"/>
-      <c r="B10" s="3"/>
-      <c r="C10" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
-      <c r="I10" s="3"/>
-      <c r="J10" s="3"/>
-      <c r="K10" s="3"/>
-      <c r="L10" s="3"/>
-      <c r="M10" s="3"/>
-      <c r="N10" s="4"/>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A11" s="2">
-        <v>900</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D11" s="2">
-        <v>4.8238000000000003</v>
-      </c>
-      <c r="E11" s="2">
-        <v>378.86</v>
-      </c>
-      <c r="F11" s="2">
-        <v>0.14230000000000001</v>
-      </c>
-      <c r="G11" s="2">
-        <v>4.4020999999999999</v>
-      </c>
-      <c r="H11" s="2">
-        <v>1006.9</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="C12" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A13" s="3"/>
-      <c r="B13" s="3"/>
-      <c r="C13" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="3"/>
-      <c r="G13" s="3"/>
-      <c r="H13" s="3"/>
-      <c r="I13" s="3"/>
-      <c r="J13" s="3"/>
-      <c r="K13" s="3"/>
-      <c r="L13" s="3"/>
-      <c r="M13" s="3"/>
-      <c r="N13" s="4"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Minor changes and added yield error to evp_t scripts
</commit_message>
<xml_diff>
--- a/scripts/__other__/__sem__.xlsx
+++ b/scripts/__other__/__sem__.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Janzen\Desktop\code\moga_neml\scripts\__other__\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DD67D5B-7A3F-4331-99BA-7B12DD3D8434}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46E92EC4-05C1-4A8E-9945-61485B4D742A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="22">
   <si>
     <t>temp</t>
   </si>
@@ -76,6 +76,24 @@
   </si>
   <si>
     <t>init</t>
+  </si>
+  <si>
+    <t>c_0</t>
+  </si>
+  <si>
+    <t>c_n</t>
+  </si>
+  <si>
+    <t>c_1</t>
+  </si>
+  <si>
+    <t>t_n</t>
+  </si>
+  <si>
+    <t>t_0</t>
+  </si>
+  <si>
+    <t>t_1</t>
   </si>
 </sst>
 </file>
@@ -214,7 +232,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -254,9 +272,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1433,8 +1448,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C8957C7-6C75-407A-91FD-39EC012C6800}">
   <dimension ref="A1:K91"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="C91" sqref="C2:C91"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1482,48 +1498,39 @@
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="14">
+      <c r="A2" s="2">
         <v>800</v>
       </c>
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="14">
+      <c r="D2" s="2">
         <v>4.7069999999999999</v>
       </c>
-      <c r="E2" s="14">
+      <c r="E2" s="2">
         <v>29.9</v>
       </c>
-      <c r="F2" s="14">
+      <c r="F2" s="2">
         <v>47.707000000000001</v>
       </c>
-      <c r="G2" s="14">
+      <c r="G2" s="2">
         <v>3.6625999999999999</v>
       </c>
-      <c r="H2" s="14">
+      <c r="H2" s="2">
         <v>3159.4</v>
       </c>
-      <c r="I2" s="14"/>
-      <c r="J2" s="14"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="14"/>
-      <c r="B3" s="14"/>
       <c r="C3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="14"/>
-      <c r="E3" s="14"/>
-      <c r="F3" s="14"/>
-      <c r="G3" s="14"/>
-      <c r="H3" s="14"/>
-      <c r="I3" s="14">
+      <c r="I3" s="2">
         <v>2169</v>
       </c>
-      <c r="J3" s="14">
+      <c r="J3" s="2">
         <v>5.6902999999999997</v>
       </c>
       <c r="K3" s="1">
@@ -1531,12 +1538,10 @@
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="14"/>
-      <c r="B4" s="14"/>
       <c r="C4" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="15">
+      <c r="D4" s="14">
         <v>6.4737</v>
       </c>
       <c r="E4" s="3">
@@ -1562,40 +1567,20 @@
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="14"/>
-      <c r="B5" s="14"/>
       <c r="C5" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="14"/>
-      <c r="E5" s="14"/>
-      <c r="F5" s="14"/>
-      <c r="G5" s="14"/>
-      <c r="H5" s="14"/>
-      <c r="I5" s="14"/>
-      <c r="J5" s="14"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="14"/>
-      <c r="B6" s="14"/>
       <c r="C6" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="14"/>
-      <c r="E6" s="14"/>
-      <c r="F6" s="14"/>
-      <c r="G6" s="14"/>
-      <c r="H6" s="14"/>
-      <c r="I6" s="14"/>
-      <c r="J6" s="14"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="14"/>
-      <c r="B7" s="14"/>
       <c r="C7" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D7" s="15"/>
+      <c r="D7" s="14"/>
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
       <c r="G7" s="3"/>
@@ -1605,40 +1590,20 @@
       <c r="K7" s="4"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="14"/>
-      <c r="B8" s="14"/>
       <c r="C8" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D8" s="14"/>
-      <c r="E8" s="14"/>
-      <c r="F8" s="14"/>
-      <c r="G8" s="14"/>
-      <c r="H8" s="14"/>
-      <c r="I8" s="14"/>
-      <c r="J8" s="14"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="14"/>
-      <c r="B9" s="14"/>
       <c r="C9" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D9" s="14"/>
-      <c r="E9" s="14"/>
-      <c r="F9" s="14"/>
-      <c r="G9" s="14"/>
-      <c r="H9" s="14"/>
-      <c r="I9" s="14"/>
-      <c r="J9" s="14"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="14"/>
-      <c r="B10" s="14"/>
       <c r="C10" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D10" s="15"/>
+      <c r="D10" s="14"/>
       <c r="E10" s="3"/>
       <c r="F10" s="3"/>
       <c r="G10" s="3"/>
@@ -1648,40 +1613,20 @@
       <c r="K10" s="4"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="14"/>
-      <c r="B11" s="14"/>
       <c r="C11" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D11" s="14"/>
-      <c r="E11" s="14"/>
-      <c r="F11" s="14"/>
-      <c r="G11" s="14"/>
-      <c r="H11" s="14"/>
-      <c r="I11" s="14"/>
-      <c r="J11" s="14"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="14"/>
-      <c r="B12" s="14"/>
       <c r="C12" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D12" s="14"/>
-      <c r="E12" s="14"/>
-      <c r="F12" s="14"/>
-      <c r="G12" s="14"/>
-      <c r="H12" s="14"/>
-      <c r="I12" s="14"/>
-      <c r="J12" s="14"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="14"/>
-      <c r="B13" s="14"/>
       <c r="C13" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D13" s="15"/>
+      <c r="D13" s="14"/>
       <c r="E13" s="3"/>
       <c r="F13" s="3"/>
       <c r="G13" s="3"/>
@@ -1716,48 +1661,39 @@
       <c r="K16" s="4"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="14">
+      <c r="A17" s="2">
         <v>800</v>
       </c>
-      <c r="B17" s="14" t="s">
+      <c r="B17" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D17" s="14">
+      <c r="D17" s="2">
         <v>14.535</v>
       </c>
-      <c r="E17" s="14">
+      <c r="E17" s="2">
         <v>347.93</v>
       </c>
-      <c r="F17" s="14">
+      <c r="F17" s="2">
         <v>0.33581</v>
       </c>
-      <c r="G17" s="14">
+      <c r="G17" s="2">
         <v>3.8755000000000002</v>
       </c>
-      <c r="H17" s="14">
+      <c r="H17" s="2">
         <v>3156.8</v>
       </c>
-      <c r="I17" s="14"/>
-      <c r="J17" s="14"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="14"/>
-      <c r="B18" s="14"/>
       <c r="C18" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D18" s="14"/>
-      <c r="E18" s="14"/>
-      <c r="F18" s="14"/>
-      <c r="G18" s="14"/>
-      <c r="H18" s="14"/>
-      <c r="I18" s="14">
+      <c r="I18" s="2">
         <v>2603.4</v>
       </c>
-      <c r="J18" s="14">
+      <c r="J18" s="2">
         <v>4.9169</v>
       </c>
       <c r="K18" s="1">
@@ -1765,12 +1701,10 @@
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="14"/>
-      <c r="B19" s="14"/>
       <c r="C19" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D19" s="15">
+      <c r="D19" s="14">
         <v>37.386000000000003</v>
       </c>
       <c r="E19" s="3">
@@ -1796,40 +1730,20 @@
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="14"/>
-      <c r="B20" s="14"/>
       <c r="C20" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D20" s="14"/>
-      <c r="E20" s="14"/>
-      <c r="F20" s="14"/>
-      <c r="G20" s="14"/>
-      <c r="H20" s="14"/>
-      <c r="I20" s="14"/>
-      <c r="J20" s="14"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21" s="14"/>
-      <c r="B21" s="14"/>
       <c r="C21" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D21" s="14"/>
-      <c r="E21" s="14"/>
-      <c r="F21" s="14"/>
-      <c r="G21" s="14"/>
-      <c r="H21" s="14"/>
-      <c r="I21" s="14"/>
-      <c r="J21" s="14"/>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22" s="14"/>
-      <c r="B22" s="14"/>
       <c r="C22" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D22" s="15"/>
+      <c r="D22" s="14"/>
       <c r="E22" s="3"/>
       <c r="F22" s="3"/>
       <c r="G22" s="3"/>
@@ -1839,40 +1753,20 @@
       <c r="K22" s="4"/>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23" s="14"/>
-      <c r="B23" s="14"/>
       <c r="C23" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D23" s="14"/>
-      <c r="E23" s="14"/>
-      <c r="F23" s="14"/>
-      <c r="G23" s="14"/>
-      <c r="H23" s="14"/>
-      <c r="I23" s="14"/>
-      <c r="J23" s="14"/>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A24" s="14"/>
-      <c r="B24" s="14"/>
       <c r="C24" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D24" s="14"/>
-      <c r="E24" s="14"/>
-      <c r="F24" s="14"/>
-      <c r="G24" s="14"/>
-      <c r="H24" s="14"/>
-      <c r="I24" s="14"/>
-      <c r="J24" s="14"/>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A25" s="14"/>
-      <c r="B25" s="14"/>
       <c r="C25" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D25" s="15"/>
+      <c r="D25" s="14"/>
       <c r="E25" s="3"/>
       <c r="F25" s="3"/>
       <c r="G25" s="3"/>
@@ -1882,40 +1776,20 @@
       <c r="K25" s="4"/>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A26" s="14"/>
-      <c r="B26" s="14"/>
       <c r="C26" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D26" s="14"/>
-      <c r="E26" s="14"/>
-      <c r="F26" s="14"/>
-      <c r="G26" s="14"/>
-      <c r="H26" s="14"/>
-      <c r="I26" s="14"/>
-      <c r="J26" s="14"/>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A27" s="14"/>
-      <c r="B27" s="14"/>
       <c r="C27" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D27" s="14"/>
-      <c r="E27" s="14"/>
-      <c r="F27" s="14"/>
-      <c r="G27" s="14"/>
-      <c r="H27" s="14"/>
-      <c r="I27" s="14"/>
-      <c r="J27" s="14"/>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A28" s="14"/>
-      <c r="B28" s="14"/>
       <c r="C28" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D28" s="15"/>
+      <c r="D28" s="14"/>
       <c r="E28" s="3"/>
       <c r="F28" s="3"/>
       <c r="G28" s="3"/>
@@ -1950,48 +1824,39 @@
       <c r="K31" s="4"/>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A32" s="14">
+      <c r="A32" s="2">
         <v>900</v>
       </c>
-      <c r="B32" s="14" t="s">
+      <c r="B32" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D32" s="14">
+      <c r="D32" s="2">
         <v>17.420000000000002</v>
       </c>
-      <c r="E32" s="14">
+      <c r="E32" s="2">
         <v>217.36</v>
       </c>
-      <c r="F32" s="14">
+      <c r="F32" s="2">
         <v>0.33130999999999999</v>
       </c>
-      <c r="G32" s="14">
+      <c r="G32" s="2">
         <v>2.0339999999999998</v>
       </c>
-      <c r="H32" s="14">
+      <c r="H32" s="2">
         <v>42591</v>
       </c>
-      <c r="I32" s="14"/>
-      <c r="J32" s="14"/>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A33" s="14"/>
-      <c r="B33" s="14"/>
       <c r="C33" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D33" s="14"/>
-      <c r="E33" s="14"/>
-      <c r="F33" s="14"/>
-      <c r="G33" s="14"/>
-      <c r="H33" s="14"/>
-      <c r="I33" s="14">
+      <c r="I33" s="2">
         <v>2632.8</v>
       </c>
-      <c r="J33" s="14">
+      <c r="J33" s="2">
         <v>4.0648</v>
       </c>
       <c r="K33" s="1">
@@ -1999,12 +1864,10 @@
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A34" s="14"/>
-      <c r="B34" s="14"/>
       <c r="C34" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D34" s="15">
+      <c r="D34" s="14">
         <v>17.484000000000002</v>
       </c>
       <c r="E34" s="3">
@@ -2030,40 +1893,20 @@
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A35" s="14"/>
-      <c r="B35" s="14"/>
       <c r="C35" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D35" s="14"/>
-      <c r="E35" s="14"/>
-      <c r="F35" s="14"/>
-      <c r="G35" s="14"/>
-      <c r="H35" s="14"/>
-      <c r="I35" s="14"/>
-      <c r="J35" s="14"/>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A36" s="14"/>
-      <c r="B36" s="14"/>
       <c r="C36" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D36" s="14"/>
-      <c r="E36" s="14"/>
-      <c r="F36" s="14"/>
-      <c r="G36" s="14"/>
-      <c r="H36" s="14"/>
-      <c r="I36" s="14"/>
-      <c r="J36" s="14"/>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A37" s="14"/>
-      <c r="B37" s="14"/>
       <c r="C37" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D37" s="15"/>
+      <c r="D37" s="14"/>
       <c r="E37" s="3"/>
       <c r="F37" s="3"/>
       <c r="G37" s="3"/>
@@ -2073,40 +1916,20 @@
       <c r="K37" s="4"/>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A38" s="14"/>
-      <c r="B38" s="14"/>
       <c r="C38" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D38" s="14"/>
-      <c r="E38" s="14"/>
-      <c r="F38" s="14"/>
-      <c r="G38" s="14"/>
-      <c r="H38" s="14"/>
-      <c r="I38" s="14"/>
-      <c r="J38" s="14"/>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A39" s="14"/>
-      <c r="B39" s="14"/>
       <c r="C39" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D39" s="14"/>
-      <c r="E39" s="14"/>
-      <c r="F39" s="14"/>
-      <c r="G39" s="14"/>
-      <c r="H39" s="14"/>
-      <c r="I39" s="14"/>
-      <c r="J39" s="14"/>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A40" s="14"/>
-      <c r="B40" s="14"/>
       <c r="C40" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D40" s="15"/>
+      <c r="D40" s="14"/>
       <c r="E40" s="3"/>
       <c r="F40" s="3"/>
       <c r="G40" s="3"/>
@@ -2116,40 +1939,20 @@
       <c r="K40" s="4"/>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A41" s="14"/>
-      <c r="B41" s="14"/>
       <c r="C41" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D41" s="14"/>
-      <c r="E41" s="14"/>
-      <c r="F41" s="14"/>
-      <c r="G41" s="14"/>
-      <c r="H41" s="14"/>
-      <c r="I41" s="14"/>
-      <c r="J41" s="14"/>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A42" s="14"/>
-      <c r="B42" s="14"/>
       <c r="C42" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D42" s="14"/>
-      <c r="E42" s="14"/>
-      <c r="F42" s="14"/>
-      <c r="G42" s="14"/>
-      <c r="H42" s="14"/>
-      <c r="I42" s="14"/>
-      <c r="J42" s="14"/>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A43" s="14"/>
-      <c r="B43" s="14"/>
       <c r="C43" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D43" s="15"/>
+      <c r="D43" s="14"/>
       <c r="E43" s="3"/>
       <c r="F43" s="3"/>
       <c r="G43" s="3"/>
@@ -2184,48 +1987,39 @@
       <c r="K46" s="4"/>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A47" s="14">
+      <c r="A47" s="2">
         <v>900</v>
       </c>
-      <c r="B47" s="14" t="s">
+      <c r="B47" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C47" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D47" s="14">
+      <c r="D47" s="2">
         <v>17.937000000000001</v>
       </c>
-      <c r="E47" s="14">
+      <c r="E47" s="2">
         <v>7.4195000000000002</v>
       </c>
-      <c r="F47" s="14">
+      <c r="F47" s="2">
         <v>15.250999999999999</v>
       </c>
-      <c r="G47" s="14">
+      <c r="G47" s="2">
         <v>2.4441999999999999</v>
       </c>
-      <c r="H47" s="14">
+      <c r="H47" s="2">
         <v>9880.2000000000007</v>
       </c>
-      <c r="I47" s="14"/>
-      <c r="J47" s="14"/>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A48" s="14"/>
-      <c r="B48" s="14"/>
       <c r="C48" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D48" s="14"/>
-      <c r="E48" s="14"/>
-      <c r="F48" s="14"/>
-      <c r="G48" s="14"/>
-      <c r="H48" s="14"/>
-      <c r="I48" s="14">
+      <c r="I48" s="2">
         <v>1271.0999999999999</v>
       </c>
-      <c r="J48" s="14">
+      <c r="J48" s="2">
         <v>5.1067</v>
       </c>
       <c r="K48" s="1">
@@ -2233,12 +2027,10 @@
       </c>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A49" s="14"/>
-      <c r="B49" s="14"/>
       <c r="C49" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D49" s="15">
+      <c r="D49" s="14">
         <v>17.937000000000001</v>
       </c>
       <c r="E49" s="3">
@@ -2264,40 +2056,20 @@
       </c>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A50" s="14"/>
-      <c r="B50" s="14"/>
       <c r="C50" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D50" s="14"/>
-      <c r="E50" s="14"/>
-      <c r="F50" s="14"/>
-      <c r="G50" s="14"/>
-      <c r="H50" s="14"/>
-      <c r="I50" s="14"/>
-      <c r="J50" s="14"/>
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A51" s="14"/>
-      <c r="B51" s="14"/>
       <c r="C51" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D51" s="14"/>
-      <c r="E51" s="14"/>
-      <c r="F51" s="14"/>
-      <c r="G51" s="14"/>
-      <c r="H51" s="14"/>
-      <c r="I51" s="14"/>
-      <c r="J51" s="14"/>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A52" s="14"/>
-      <c r="B52" s="14"/>
       <c r="C52" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D52" s="15"/>
+      <c r="D52" s="14"/>
       <c r="E52" s="3"/>
       <c r="F52" s="3"/>
       <c r="G52" s="3"/>
@@ -2307,40 +2079,20 @@
       <c r="K52" s="4"/>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A53" s="14"/>
-      <c r="B53" s="14"/>
       <c r="C53" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D53" s="14"/>
-      <c r="E53" s="14"/>
-      <c r="F53" s="14"/>
-      <c r="G53" s="14"/>
-      <c r="H53" s="14"/>
-      <c r="I53" s="14"/>
-      <c r="J53" s="14"/>
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A54" s="14"/>
-      <c r="B54" s="14"/>
       <c r="C54" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D54" s="14"/>
-      <c r="E54" s="14"/>
-      <c r="F54" s="14"/>
-      <c r="G54" s="14"/>
-      <c r="H54" s="14"/>
-      <c r="I54" s="14"/>
-      <c r="J54" s="14"/>
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A55" s="14"/>
-      <c r="B55" s="14"/>
       <c r="C55" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D55" s="15"/>
+      <c r="D55" s="14"/>
       <c r="E55" s="3"/>
       <c r="F55" s="3"/>
       <c r="G55" s="3"/>
@@ -2350,40 +2102,20 @@
       <c r="K55" s="4"/>
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A56" s="14"/>
-      <c r="B56" s="14"/>
       <c r="C56" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D56" s="14"/>
-      <c r="E56" s="14"/>
-      <c r="F56" s="14"/>
-      <c r="G56" s="14"/>
-      <c r="H56" s="14"/>
-      <c r="I56" s="14"/>
-      <c r="J56" s="14"/>
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A57" s="14"/>
-      <c r="B57" s="14"/>
       <c r="C57" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D57" s="14"/>
-      <c r="E57" s="14"/>
-      <c r="F57" s="14"/>
-      <c r="G57" s="14"/>
-      <c r="H57" s="14"/>
-      <c r="I57" s="14"/>
-      <c r="J57" s="14"/>
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A58" s="14"/>
-      <c r="B58" s="14"/>
       <c r="C58" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D58" s="15"/>
+      <c r="D58" s="14"/>
       <c r="E58" s="3"/>
       <c r="F58" s="3"/>
       <c r="G58" s="3"/>
@@ -2418,44 +2150,26 @@
       <c r="K61" s="4"/>
     </row>
     <row r="62" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A62" s="14">
+      <c r="A62" s="2">
         <v>1000</v>
       </c>
-      <c r="B62" s="14" t="s">
+      <c r="B62" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C62" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D62" s="14"/>
-      <c r="E62" s="14"/>
-      <c r="F62" s="14"/>
-      <c r="G62" s="14"/>
-      <c r="H62" s="14"/>
-      <c r="I62" s="14"/>
-      <c r="J62" s="14"/>
     </row>
     <row r="63" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A63" s="14"/>
-      <c r="B63" s="14"/>
       <c r="C63" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D63" s="14"/>
-      <c r="E63" s="14"/>
-      <c r="F63" s="14"/>
-      <c r="G63" s="14"/>
-      <c r="H63" s="14"/>
-      <c r="I63" s="14"/>
-      <c r="J63" s="14"/>
     </row>
     <row r="64" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A64" s="14"/>
-      <c r="B64" s="14"/>
       <c r="C64" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D64" s="15"/>
+      <c r="D64" s="14"/>
       <c r="E64" s="3"/>
       <c r="F64" s="3"/>
       <c r="G64" s="3"/>
@@ -2465,40 +2179,20 @@
       <c r="K64" s="4"/>
     </row>
     <row r="65" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A65" s="14"/>
-      <c r="B65" s="14"/>
       <c r="C65" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D65" s="14"/>
-      <c r="E65" s="14"/>
-      <c r="F65" s="14"/>
-      <c r="G65" s="14"/>
-      <c r="H65" s="14"/>
-      <c r="I65" s="14"/>
-      <c r="J65" s="14"/>
     </row>
     <row r="66" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A66" s="14"/>
-      <c r="B66" s="14"/>
       <c r="C66" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D66" s="14"/>
-      <c r="E66" s="14"/>
-      <c r="F66" s="14"/>
-      <c r="G66" s="14"/>
-      <c r="H66" s="14"/>
-      <c r="I66" s="14"/>
-      <c r="J66" s="14"/>
     </row>
     <row r="67" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A67" s="14"/>
-      <c r="B67" s="14"/>
       <c r="C67" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D67" s="15"/>
+      <c r="D67" s="14"/>
       <c r="E67" s="3"/>
       <c r="F67" s="3"/>
       <c r="G67" s="3"/>
@@ -2508,40 +2202,20 @@
       <c r="K67" s="4"/>
     </row>
     <row r="68" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A68" s="14"/>
-      <c r="B68" s="14"/>
       <c r="C68" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D68" s="14"/>
-      <c r="E68" s="14"/>
-      <c r="F68" s="14"/>
-      <c r="G68" s="14"/>
-      <c r="H68" s="14"/>
-      <c r="I68" s="14"/>
-      <c r="J68" s="14"/>
     </row>
     <row r="69" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A69" s="14"/>
-      <c r="B69" s="14"/>
       <c r="C69" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D69" s="14"/>
-      <c r="E69" s="14"/>
-      <c r="F69" s="14"/>
-      <c r="G69" s="14"/>
-      <c r="H69" s="14"/>
-      <c r="I69" s="14"/>
-      <c r="J69" s="14"/>
     </row>
     <row r="70" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A70" s="14"/>
-      <c r="B70" s="14"/>
       <c r="C70" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D70" s="15"/>
+      <c r="D70" s="14"/>
       <c r="E70" s="3"/>
       <c r="F70" s="3"/>
       <c r="G70" s="3"/>
@@ -2551,40 +2225,20 @@
       <c r="K70" s="4"/>
     </row>
     <row r="71" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A71" s="14"/>
-      <c r="B71" s="14"/>
       <c r="C71" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D71" s="14"/>
-      <c r="E71" s="14"/>
-      <c r="F71" s="14"/>
-      <c r="G71" s="14"/>
-      <c r="H71" s="14"/>
-      <c r="I71" s="14"/>
-      <c r="J71" s="14"/>
     </row>
     <row r="72" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A72" s="14"/>
-      <c r="B72" s="14"/>
       <c r="C72" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D72" s="14"/>
-      <c r="E72" s="14"/>
-      <c r="F72" s="14"/>
-      <c r="G72" s="14"/>
-      <c r="H72" s="14"/>
-      <c r="I72" s="14"/>
-      <c r="J72" s="14"/>
     </row>
     <row r="73" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A73" s="14"/>
-      <c r="B73" s="14"/>
       <c r="C73" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D73" s="15"/>
+      <c r="D73" s="14"/>
       <c r="E73" s="3"/>
       <c r="F73" s="3"/>
       <c r="G73" s="3"/>
@@ -2619,44 +2273,26 @@
       <c r="K76" s="4"/>
     </row>
     <row r="77" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A77" s="14">
+      <c r="A77" s="2">
         <v>1000</v>
       </c>
-      <c r="B77" s="14" t="s">
+      <c r="B77" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C77" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D77" s="14"/>
-      <c r="E77" s="14"/>
-      <c r="F77" s="14"/>
-      <c r="G77" s="14"/>
-      <c r="H77" s="14"/>
-      <c r="I77" s="14"/>
-      <c r="J77" s="14"/>
     </row>
     <row r="78" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A78" s="14"/>
-      <c r="B78" s="14"/>
       <c r="C78" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D78" s="14"/>
-      <c r="E78" s="14"/>
-      <c r="F78" s="14"/>
-      <c r="G78" s="14"/>
-      <c r="H78" s="14"/>
-      <c r="I78" s="14"/>
-      <c r="J78" s="14"/>
     </row>
     <row r="79" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A79" s="14"/>
-      <c r="B79" s="14"/>
       <c r="C79" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D79" s="15"/>
+      <c r="D79" s="14"/>
       <c r="E79" s="3"/>
       <c r="F79" s="3"/>
       <c r="G79" s="3"/>
@@ -2666,40 +2302,20 @@
       <c r="K79" s="4"/>
     </row>
     <row r="80" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A80" s="14"/>
-      <c r="B80" s="14"/>
       <c r="C80" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D80" s="14"/>
-      <c r="E80" s="14"/>
-      <c r="F80" s="14"/>
-      <c r="G80" s="14"/>
-      <c r="H80" s="14"/>
-      <c r="I80" s="14"/>
-      <c r="J80" s="14"/>
     </row>
     <row r="81" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A81" s="14"/>
-      <c r="B81" s="14"/>
       <c r="C81" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D81" s="14"/>
-      <c r="E81" s="14"/>
-      <c r="F81" s="14"/>
-      <c r="G81" s="14"/>
-      <c r="H81" s="14"/>
-      <c r="I81" s="14"/>
-      <c r="J81" s="14"/>
     </row>
     <row r="82" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A82" s="14"/>
-      <c r="B82" s="14"/>
       <c r="C82" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D82" s="15"/>
+      <c r="D82" s="14"/>
       <c r="E82" s="3"/>
       <c r="F82" s="3"/>
       <c r="G82" s="3"/>
@@ -2709,40 +2325,20 @@
       <c r="K82" s="4"/>
     </row>
     <row r="83" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A83" s="14"/>
-      <c r="B83" s="14"/>
       <c r="C83" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D83" s="14"/>
-      <c r="E83" s="14"/>
-      <c r="F83" s="14"/>
-      <c r="G83" s="14"/>
-      <c r="H83" s="14"/>
-      <c r="I83" s="14"/>
-      <c r="J83" s="14"/>
     </row>
     <row r="84" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A84" s="14"/>
-      <c r="B84" s="14"/>
       <c r="C84" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D84" s="14"/>
-      <c r="E84" s="14"/>
-      <c r="F84" s="14"/>
-      <c r="G84" s="14"/>
-      <c r="H84" s="14"/>
-      <c r="I84" s="14"/>
-      <c r="J84" s="14"/>
     </row>
     <row r="85" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A85" s="14"/>
-      <c r="B85" s="14"/>
       <c r="C85" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D85" s="15"/>
+      <c r="D85" s="14"/>
       <c r="E85" s="3"/>
       <c r="F85" s="3"/>
       <c r="G85" s="3"/>
@@ -2752,40 +2348,20 @@
       <c r="K85" s="4"/>
     </row>
     <row r="86" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A86" s="14"/>
-      <c r="B86" s="14"/>
       <c r="C86" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D86" s="14"/>
-      <c r="E86" s="14"/>
-      <c r="F86" s="14"/>
-      <c r="G86" s="14"/>
-      <c r="H86" s="14"/>
-      <c r="I86" s="14"/>
-      <c r="J86" s="14"/>
     </row>
     <row r="87" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A87" s="14"/>
-      <c r="B87" s="14"/>
       <c r="C87" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D87" s="14"/>
-      <c r="E87" s="14"/>
-      <c r="F87" s="14"/>
-      <c r="G87" s="14"/>
-      <c r="H87" s="14"/>
-      <c r="I87" s="14"/>
-      <c r="J87" s="14"/>
     </row>
     <row r="88" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A88" s="14"/>
-      <c r="B88" s="14"/>
       <c r="C88" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D88" s="15"/>
+      <c r="D88" s="14"/>
       <c r="E88" s="3"/>
       <c r="F88" s="3"/>
       <c r="G88" s="3"/>
@@ -2826,22 +2402,23 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBE5B278-CF38-41EF-A268-D7BDDFF8B1FA}">
-  <dimension ref="A1:K91"/>
+  <dimension ref="A1:N91"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10:F11"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="9.140625" style="2"/>
     <col min="3" max="3" width="9.140625" style="1"/>
-    <col min="4" max="10" width="9.140625" style="2"/>
-    <col min="11" max="11" width="9.140625" style="1"/>
-    <col min="12" max="16384" width="9.140625" style="2"/>
+    <col min="4" max="13" width="9.140625" style="2"/>
+    <col min="14" max="14" width="9.140625" style="1"/>
+    <col min="15" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -2867,222 +2444,190 @@
         <v>6</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="K1" s="4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="14">
+        <v>16</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="N1" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
         <v>800</v>
       </c>
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="14">
+      <c r="D2" s="2">
         <v>11.695</v>
       </c>
-      <c r="E2" s="14">
+      <c r="E2" s="2">
         <v>101.28</v>
       </c>
-      <c r="F2" s="14">
+      <c r="F2" s="2">
         <v>1.1411</v>
       </c>
-      <c r="G2" s="14">
+      <c r="G2" s="2">
         <v>4.6826999999999996</v>
       </c>
-      <c r="H2" s="14">
+      <c r="H2" s="2">
         <v>1595.5</v>
       </c>
-      <c r="I2" s="14"/>
-      <c r="J2" s="14"/>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="14"/>
-      <c r="B3" s="14"/>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="14"/>
-      <c r="E3" s="14"/>
-      <c r="F3" s="14"/>
-      <c r="G3" s="14"/>
-      <c r="H3" s="14"/>
-      <c r="I3" s="14"/>
-      <c r="J3" s="14"/>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="14"/>
-      <c r="B4" s="14"/>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C4" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="15"/>
+      <c r="D4" s="14"/>
       <c r="E4" s="3"/>
       <c r="F4" s="3"/>
       <c r="G4" s="3"/>
       <c r="H4" s="3"/>
       <c r="I4" s="3"/>
       <c r="J4" s="3"/>
-      <c r="K4" s="4"/>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="14"/>
-      <c r="B5" s="14"/>
+      <c r="K4" s="3"/>
+      <c r="L4" s="3"/>
+      <c r="M4" s="3"/>
+      <c r="N4" s="4"/>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C5" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="14">
+      <c r="D5" s="2">
         <v>9.8171999999999997</v>
       </c>
-      <c r="E5" s="14">
+      <c r="E5" s="2">
         <v>101.47</v>
       </c>
-      <c r="F5" s="14">
+      <c r="F5" s="2">
         <v>1.4056999999999999</v>
       </c>
-      <c r="G5" s="14">
+      <c r="G5" s="2">
         <v>4.6856999999999998</v>
       </c>
-      <c r="H5" s="14">
+      <c r="H5" s="2">
         <v>1595.7</v>
       </c>
-      <c r="I5" s="14"/>
-      <c r="J5" s="14"/>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="14"/>
-      <c r="B6" s="14"/>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C6" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="14"/>
-      <c r="E6" s="14"/>
-      <c r="F6" s="14"/>
-      <c r="G6" s="14"/>
-      <c r="H6" s="14"/>
-      <c r="I6" s="14"/>
-      <c r="J6" s="14"/>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="14"/>
-      <c r="B7" s="14"/>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C7" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D7" s="15"/>
+      <c r="D7" s="14"/>
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
       <c r="G7" s="3"/>
       <c r="H7" s="3"/>
       <c r="I7" s="3"/>
       <c r="J7" s="3"/>
-      <c r="K7" s="4"/>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="14"/>
-      <c r="B8" s="14"/>
+      <c r="K7" s="3"/>
+      <c r="L7" s="3"/>
+      <c r="M7" s="3"/>
+      <c r="N7" s="4"/>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C8" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D8" s="14"/>
-      <c r="E8" s="14"/>
-      <c r="F8" s="14"/>
-      <c r="G8" s="14"/>
-      <c r="H8" s="14"/>
-      <c r="I8" s="14"/>
-      <c r="J8" s="14"/>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="14"/>
-      <c r="B9" s="14"/>
+      <c r="D8" s="2">
+        <v>4.8710000000000004</v>
+      </c>
+      <c r="E8" s="2">
+        <v>11.518000000000001</v>
+      </c>
+      <c r="F8" s="2">
+        <v>7.0281000000000002</v>
+      </c>
+      <c r="G8" s="2">
+        <v>4.2420999999999998</v>
+      </c>
+      <c r="H8" s="2">
+        <v>1138.3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C9" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D9" s="14"/>
-      <c r="E9" s="14"/>
-      <c r="F9" s="14"/>
-      <c r="G9" s="14"/>
-      <c r="H9" s="14"/>
-      <c r="I9" s="14"/>
-      <c r="J9" s="14"/>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="14"/>
-      <c r="B10" s="14"/>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C10" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D10" s="15"/>
+      <c r="D10" s="14"/>
       <c r="E10" s="3"/>
       <c r="F10" s="3"/>
       <c r="G10" s="3"/>
       <c r="H10" s="3"/>
       <c r="I10" s="3"/>
       <c r="J10" s="3"/>
-      <c r="K10" s="4"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="14"/>
-      <c r="B11" s="14"/>
+      <c r="K10" s="3"/>
+      <c r="L10" s="3"/>
+      <c r="M10" s="3"/>
+      <c r="N10" s="4"/>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C11" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D11" s="14"/>
-      <c r="E11" s="14"/>
-      <c r="F11" s="14"/>
-      <c r="G11" s="14"/>
-      <c r="H11" s="14"/>
-      <c r="I11" s="14"/>
-      <c r="J11" s="14"/>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="14"/>
-      <c r="B12" s="14"/>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C12" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D12" s="14"/>
-      <c r="E12" s="14"/>
-      <c r="F12" s="14"/>
-      <c r="G12" s="14"/>
-      <c r="H12" s="14"/>
-      <c r="I12" s="14"/>
-      <c r="J12" s="14"/>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="14"/>
-      <c r="B13" s="14"/>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C13" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D13" s="15"/>
+      <c r="D13" s="14"/>
       <c r="E13" s="3"/>
       <c r="F13" s="3"/>
       <c r="G13" s="3"/>
       <c r="H13" s="3"/>
       <c r="I13" s="3"/>
       <c r="J13" s="3"/>
-      <c r="K13" s="4"/>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K13" s="3"/>
+      <c r="L13" s="3"/>
+      <c r="M13" s="3"/>
+      <c r="N13" s="4"/>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C14" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C15" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="3"/>
       <c r="B16" s="3"/>
       <c r="C16" s="4" t="s">
@@ -3095,205 +2640,147 @@
       <c r="H16" s="3"/>
       <c r="I16" s="3"/>
       <c r="J16" s="3"/>
-      <c r="K16" s="4"/>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="14">
+      <c r="K16" s="3"/>
+      <c r="L16" s="3"/>
+      <c r="M16" s="3"/>
+      <c r="N16" s="4"/>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A17" s="2">
         <v>800</v>
       </c>
-      <c r="B17" s="14" t="s">
+      <c r="B17" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D17" s="14">
+      <c r="D17" s="2">
         <v>31.327000000000002</v>
       </c>
-      <c r="E17" s="14">
+      <c r="E17" s="2">
         <v>104.92</v>
       </c>
-      <c r="F17" s="14">
+      <c r="F17" s="2">
         <v>0.8548</v>
       </c>
-      <c r="G17" s="14">
+      <c r="G17" s="2">
         <v>3.7507999999999999</v>
       </c>
-      <c r="H17" s="14">
+      <c r="H17" s="2">
         <v>2575.8000000000002</v>
       </c>
-      <c r="I17" s="14"/>
-      <c r="J17" s="14"/>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="14"/>
-      <c r="B18" s="14"/>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C18" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D18" s="14"/>
-      <c r="E18" s="14"/>
-      <c r="F18" s="14"/>
-      <c r="G18" s="14"/>
-      <c r="H18" s="14"/>
-      <c r="I18" s="14"/>
-      <c r="J18" s="14"/>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="14"/>
-      <c r="B19" s="14"/>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C19" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D19" s="15"/>
+      <c r="D19" s="14"/>
       <c r="E19" s="3"/>
       <c r="F19" s="3"/>
       <c r="G19" s="3"/>
       <c r="H19" s="3"/>
       <c r="I19" s="3"/>
       <c r="J19" s="3"/>
-      <c r="K19" s="4"/>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="14"/>
-      <c r="B20" s="14"/>
+      <c r="K19" s="3"/>
+      <c r="L19" s="3"/>
+      <c r="M19" s="3"/>
+      <c r="N19" s="4"/>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C20" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D20" s="14"/>
-      <c r="E20" s="14"/>
-      <c r="F20" s="14"/>
-      <c r="G20" s="14"/>
-      <c r="H20" s="14"/>
-      <c r="I20" s="14"/>
-      <c r="J20" s="14"/>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21" s="14"/>
-      <c r="B21" s="14"/>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C21" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D21" s="14"/>
-      <c r="E21" s="14"/>
-      <c r="F21" s="14"/>
-      <c r="G21" s="14"/>
-      <c r="H21" s="14"/>
-      <c r="I21" s="14"/>
-      <c r="J21" s="14"/>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22" s="14"/>
-      <c r="B22" s="14"/>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C22" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D22" s="15"/>
+      <c r="D22" s="14"/>
       <c r="E22" s="3"/>
       <c r="F22" s="3"/>
       <c r="G22" s="3"/>
       <c r="H22" s="3"/>
       <c r="I22" s="3"/>
       <c r="J22" s="3"/>
-      <c r="K22" s="4"/>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23" s="14"/>
-      <c r="B23" s="14"/>
+      <c r="K22" s="3"/>
+      <c r="L22" s="3"/>
+      <c r="M22" s="3"/>
+      <c r="N22" s="4"/>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C23" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D23" s="14"/>
-      <c r="E23" s="14"/>
-      <c r="F23" s="14"/>
-      <c r="G23" s="14"/>
-      <c r="H23" s="14"/>
-      <c r="I23" s="14"/>
-      <c r="J23" s="14"/>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A24" s="14"/>
-      <c r="B24" s="14"/>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C24" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D24" s="14"/>
-      <c r="E24" s="14"/>
-      <c r="F24" s="14"/>
-      <c r="G24" s="14"/>
-      <c r="H24" s="14"/>
-      <c r="I24" s="14"/>
-      <c r="J24" s="14"/>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A25" s="14"/>
-      <c r="B25" s="14"/>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C25" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D25" s="15"/>
+      <c r="D25" s="14"/>
       <c r="E25" s="3"/>
       <c r="F25" s="3"/>
       <c r="G25" s="3"/>
       <c r="H25" s="3"/>
       <c r="I25" s="3"/>
       <c r="J25" s="3"/>
-      <c r="K25" s="4"/>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A26" s="14"/>
-      <c r="B26" s="14"/>
+      <c r="K25" s="3"/>
+      <c r="L25" s="3"/>
+      <c r="M25" s="3"/>
+      <c r="N25" s="4"/>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C26" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D26" s="14"/>
-      <c r="E26" s="14"/>
-      <c r="F26" s="14"/>
-      <c r="G26" s="14"/>
-      <c r="H26" s="14"/>
-      <c r="I26" s="14"/>
-      <c r="J26" s="14"/>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A27" s="14"/>
-      <c r="B27" s="14"/>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C27" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D27" s="14"/>
-      <c r="E27" s="14"/>
-      <c r="F27" s="14"/>
-      <c r="G27" s="14"/>
-      <c r="H27" s="14"/>
-      <c r="I27" s="14"/>
-      <c r="J27" s="14"/>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A28" s="14"/>
-      <c r="B28" s="14"/>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C28" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D28" s="15"/>
+      <c r="D28" s="14"/>
       <c r="E28" s="3"/>
       <c r="F28" s="3"/>
       <c r="G28" s="3"/>
       <c r="H28" s="3"/>
       <c r="I28" s="3"/>
       <c r="J28" s="3"/>
-      <c r="K28" s="4"/>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K28" s="3"/>
+      <c r="L28" s="3"/>
+      <c r="M28" s="3"/>
+      <c r="N28" s="4"/>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C29" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C30" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31" s="3"/>
       <c r="B31" s="3"/>
       <c r="C31" s="4" t="s">
@@ -3306,205 +2793,165 @@
       <c r="H31" s="3"/>
       <c r="I31" s="3"/>
       <c r="J31" s="3"/>
-      <c r="K31" s="4"/>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A32" s="14">
+      <c r="K31" s="3"/>
+      <c r="L31" s="3"/>
+      <c r="M31" s="3"/>
+      <c r="N31" s="4"/>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A32" s="2">
         <v>900</v>
       </c>
-      <c r="B32" s="14" t="s">
+      <c r="B32" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D32" s="14">
+      <c r="D32" s="2">
         <v>4.8710000000000004</v>
       </c>
-      <c r="E32" s="14">
+      <c r="E32" s="2">
         <v>11.518000000000001</v>
       </c>
-      <c r="F32" s="14">
+      <c r="F32" s="2">
         <v>7.0281000000000002</v>
       </c>
-      <c r="G32" s="14">
+      <c r="G32" s="2">
         <v>4.2420999999999998</v>
       </c>
-      <c r="H32" s="14">
+      <c r="H32" s="2">
         <v>1138.3</v>
       </c>
-      <c r="I32" s="14"/>
-      <c r="J32" s="14"/>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A33" s="14"/>
-      <c r="B33" s="14"/>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C33" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D33" s="14"/>
-      <c r="E33" s="14"/>
-      <c r="F33" s="14"/>
-      <c r="G33" s="14"/>
-      <c r="H33" s="14"/>
-      <c r="I33" s="14"/>
-      <c r="J33" s="14"/>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A34" s="14"/>
-      <c r="B34" s="14"/>
+      <c r="I33" s="2">
+        <v>1.2072000000000001</v>
+      </c>
+      <c r="J33" s="2">
+        <v>0.44550000000000001</v>
+      </c>
+      <c r="K33" s="2">
+        <v>3.8687</v>
+      </c>
+      <c r="L33" s="2">
+        <v>3.6877</v>
+      </c>
+      <c r="M33" s="2">
+        <v>0.25385000000000002</v>
+      </c>
+      <c r="N33" s="1">
+        <v>2.5308000000000002</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C34" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D34" s="15"/>
+      <c r="D34" s="14"/>
       <c r="E34" s="3"/>
       <c r="F34" s="3"/>
       <c r="G34" s="3"/>
       <c r="H34" s="3"/>
       <c r="I34" s="3"/>
       <c r="J34" s="3"/>
-      <c r="K34" s="4"/>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A35" s="14"/>
-      <c r="B35" s="14"/>
+      <c r="K34" s="3"/>
+      <c r="L34" s="3"/>
+      <c r="M34" s="3"/>
+      <c r="N34" s="4"/>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C35" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D35" s="14"/>
-      <c r="E35" s="14"/>
-      <c r="F35" s="14"/>
-      <c r="G35" s="14"/>
-      <c r="H35" s="14"/>
-      <c r="I35" s="14"/>
-      <c r="J35" s="14"/>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A36" s="14"/>
-      <c r="B36" s="14"/>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C36" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D36" s="14"/>
-      <c r="E36" s="14"/>
-      <c r="F36" s="14"/>
-      <c r="G36" s="14"/>
-      <c r="H36" s="14"/>
-      <c r="I36" s="14"/>
-      <c r="J36" s="14"/>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A37" s="14"/>
-      <c r="B37" s="14"/>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C37" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D37" s="15"/>
+      <c r="D37" s="14"/>
       <c r="E37" s="3"/>
       <c r="F37" s="3"/>
       <c r="G37" s="3"/>
       <c r="H37" s="3"/>
       <c r="I37" s="3"/>
       <c r="J37" s="3"/>
-      <c r="K37" s="4"/>
-    </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A38" s="14"/>
-      <c r="B38" s="14"/>
+      <c r="K37" s="3"/>
+      <c r="L37" s="3"/>
+      <c r="M37" s="3"/>
+      <c r="N37" s="4"/>
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C38" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D38" s="14"/>
-      <c r="E38" s="14"/>
-      <c r="F38" s="14"/>
-      <c r="G38" s="14"/>
-      <c r="H38" s="14"/>
-      <c r="I38" s="14"/>
-      <c r="J38" s="14"/>
-    </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A39" s="14"/>
-      <c r="B39" s="14"/>
+    </row>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C39" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D39" s="14"/>
-      <c r="E39" s="14"/>
-      <c r="F39" s="14"/>
-      <c r="G39" s="14"/>
-      <c r="H39" s="14"/>
-      <c r="I39" s="14"/>
-      <c r="J39" s="14"/>
-    </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A40" s="14"/>
-      <c r="B40" s="14"/>
+    </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C40" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D40" s="15"/>
+      <c r="D40" s="14"/>
       <c r="E40" s="3"/>
       <c r="F40" s="3"/>
       <c r="G40" s="3"/>
       <c r="H40" s="3"/>
       <c r="I40" s="3"/>
       <c r="J40" s="3"/>
-      <c r="K40" s="4"/>
-    </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A41" s="14"/>
-      <c r="B41" s="14"/>
+      <c r="K40" s="3"/>
+      <c r="L40" s="3"/>
+      <c r="M40" s="3"/>
+      <c r="N40" s="4"/>
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C41" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D41" s="14"/>
-      <c r="E41" s="14"/>
-      <c r="F41" s="14"/>
-      <c r="G41" s="14"/>
-      <c r="H41" s="14"/>
-      <c r="I41" s="14"/>
-      <c r="J41" s="14"/>
-    </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A42" s="14"/>
-      <c r="B42" s="14"/>
+    </row>
+    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C42" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D42" s="14"/>
-      <c r="E42" s="14"/>
-      <c r="F42" s="14"/>
-      <c r="G42" s="14"/>
-      <c r="H42" s="14"/>
-      <c r="I42" s="14"/>
-      <c r="J42" s="14"/>
-    </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A43" s="14"/>
-      <c r="B43" s="14"/>
+    </row>
+    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C43" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D43" s="15"/>
+      <c r="D43" s="14"/>
       <c r="E43" s="3"/>
       <c r="F43" s="3"/>
       <c r="G43" s="3"/>
       <c r="H43" s="3"/>
       <c r="I43" s="3"/>
       <c r="J43" s="3"/>
-      <c r="K43" s="4"/>
-    </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K43" s="3"/>
+      <c r="L43" s="3"/>
+      <c r="M43" s="3"/>
+      <c r="N43" s="4"/>
+    </row>
+    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C44" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C45" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A46" s="3"/>
       <c r="B46" s="3"/>
       <c r="C46" s="4" t="s">
@@ -3517,205 +2964,165 @@
       <c r="H46" s="3"/>
       <c r="I46" s="3"/>
       <c r="J46" s="3"/>
-      <c r="K46" s="4"/>
-    </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A47" s="14">
+      <c r="K46" s="3"/>
+      <c r="L46" s="3"/>
+      <c r="M46" s="3"/>
+      <c r="N46" s="4"/>
+    </row>
+    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A47" s="2">
         <v>900</v>
       </c>
-      <c r="B47" s="14" t="s">
+      <c r="B47" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C47" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D47" s="14">
+      <c r="D47" s="2">
         <v>4.8238000000000003</v>
       </c>
-      <c r="E47" s="14">
+      <c r="E47" s="2">
         <v>378.86</v>
       </c>
-      <c r="F47" s="14">
+      <c r="F47" s="2">
         <v>0.14230000000000001</v>
       </c>
-      <c r="G47" s="14">
+      <c r="G47" s="2">
         <v>4.4020999999999999</v>
       </c>
-      <c r="H47" s="14">
+      <c r="H47" s="2">
         <v>1006.9</v>
       </c>
-      <c r="I47" s="14"/>
-      <c r="J47" s="14"/>
-    </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A48" s="14"/>
-      <c r="B48" s="14"/>
+    </row>
+    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C48" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D48" s="14"/>
-      <c r="E48" s="14"/>
-      <c r="F48" s="14"/>
-      <c r="G48" s="14"/>
-      <c r="H48" s="14"/>
-      <c r="I48" s="14"/>
-      <c r="J48" s="14"/>
-    </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A49" s="14"/>
-      <c r="B49" s="14"/>
+      <c r="I48" s="2">
+        <v>1.3282</v>
+      </c>
+      <c r="J48" s="2">
+        <v>0.54573000000000005</v>
+      </c>
+      <c r="K48" s="2">
+        <v>4.6946000000000003</v>
+      </c>
+      <c r="L48" s="2">
+        <v>3.1678999999999999</v>
+      </c>
+      <c r="M48" s="2">
+        <v>0.25372</v>
+      </c>
+      <c r="N48" s="1">
+        <v>2.5291999999999999</v>
+      </c>
+    </row>
+    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C49" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D49" s="15"/>
+      <c r="D49" s="14"/>
       <c r="E49" s="3"/>
       <c r="F49" s="3"/>
       <c r="G49" s="3"/>
       <c r="H49" s="3"/>
       <c r="I49" s="3"/>
       <c r="J49" s="3"/>
-      <c r="K49" s="4"/>
-    </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A50" s="14"/>
-      <c r="B50" s="14"/>
+      <c r="K49" s="3"/>
+      <c r="L49" s="3"/>
+      <c r="M49" s="3"/>
+      <c r="N49" s="4"/>
+    </row>
+    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C50" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D50" s="14"/>
-      <c r="E50" s="14"/>
-      <c r="F50" s="14"/>
-      <c r="G50" s="14"/>
-      <c r="H50" s="14"/>
-      <c r="I50" s="14"/>
-      <c r="J50" s="14"/>
-    </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A51" s="14"/>
-      <c r="B51" s="14"/>
+    </row>
+    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C51" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D51" s="14"/>
-      <c r="E51" s="14"/>
-      <c r="F51" s="14"/>
-      <c r="G51" s="14"/>
-      <c r="H51" s="14"/>
-      <c r="I51" s="14"/>
-      <c r="J51" s="14"/>
-    </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A52" s="14"/>
-      <c r="B52" s="14"/>
+    </row>
+    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C52" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D52" s="15"/>
+      <c r="D52" s="14"/>
       <c r="E52" s="3"/>
       <c r="F52" s="3"/>
       <c r="G52" s="3"/>
       <c r="H52" s="3"/>
       <c r="I52" s="3"/>
       <c r="J52" s="3"/>
-      <c r="K52" s="4"/>
-    </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A53" s="14"/>
-      <c r="B53" s="14"/>
+      <c r="K52" s="3"/>
+      <c r="L52" s="3"/>
+      <c r="M52" s="3"/>
+      <c r="N52" s="4"/>
+    </row>
+    <row r="53" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C53" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D53" s="14"/>
-      <c r="E53" s="14"/>
-      <c r="F53" s="14"/>
-      <c r="G53" s="14"/>
-      <c r="H53" s="14"/>
-      <c r="I53" s="14"/>
-      <c r="J53" s="14"/>
-    </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A54" s="14"/>
-      <c r="B54" s="14"/>
+    </row>
+    <row r="54" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C54" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D54" s="14"/>
-      <c r="E54" s="14"/>
-      <c r="F54" s="14"/>
-      <c r="G54" s="14"/>
-      <c r="H54" s="14"/>
-      <c r="I54" s="14"/>
-      <c r="J54" s="14"/>
-    </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A55" s="14"/>
-      <c r="B55" s="14"/>
+    </row>
+    <row r="55" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C55" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D55" s="15"/>
+      <c r="D55" s="14"/>
       <c r="E55" s="3"/>
       <c r="F55" s="3"/>
       <c r="G55" s="3"/>
       <c r="H55" s="3"/>
       <c r="I55" s="3"/>
       <c r="J55" s="3"/>
-      <c r="K55" s="4"/>
-    </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A56" s="14"/>
-      <c r="B56" s="14"/>
+      <c r="K55" s="3"/>
+      <c r="L55" s="3"/>
+      <c r="M55" s="3"/>
+      <c r="N55" s="4"/>
+    </row>
+    <row r="56" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C56" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D56" s="14"/>
-      <c r="E56" s="14"/>
-      <c r="F56" s="14"/>
-      <c r="G56" s="14"/>
-      <c r="H56" s="14"/>
-      <c r="I56" s="14"/>
-      <c r="J56" s="14"/>
-    </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A57" s="14"/>
-      <c r="B57" s="14"/>
+    </row>
+    <row r="57" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C57" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D57" s="14"/>
-      <c r="E57" s="14"/>
-      <c r="F57" s="14"/>
-      <c r="G57" s="14"/>
-      <c r="H57" s="14"/>
-      <c r="I57" s="14"/>
-      <c r="J57" s="14"/>
-    </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A58" s="14"/>
-      <c r="B58" s="14"/>
+    </row>
+    <row r="58" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C58" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D58" s="15"/>
+      <c r="D58" s="14"/>
       <c r="E58" s="3"/>
       <c r="F58" s="3"/>
       <c r="G58" s="3"/>
       <c r="H58" s="3"/>
       <c r="I58" s="3"/>
       <c r="J58" s="3"/>
-      <c r="K58" s="4"/>
-    </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K58" s="3"/>
+      <c r="L58" s="3"/>
+      <c r="M58" s="3"/>
+      <c r="N58" s="4"/>
+    </row>
+    <row r="59" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C59" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C60" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A61" s="3"/>
       <c r="B61" s="3"/>
       <c r="C61" s="4" t="s">
@@ -3728,195 +3135,132 @@
       <c r="H61" s="3"/>
       <c r="I61" s="3"/>
       <c r="J61" s="3"/>
-      <c r="K61" s="4"/>
-    </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A62" s="14">
+      <c r="K61" s="3"/>
+      <c r="L61" s="3"/>
+      <c r="M61" s="3"/>
+      <c r="N61" s="4"/>
+    </row>
+    <row r="62" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A62" s="2">
         <v>1000</v>
       </c>
-      <c r="B62" s="14" t="s">
+      <c r="B62" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C62" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D62" s="14"/>
-      <c r="E62" s="14"/>
-      <c r="F62" s="14"/>
-      <c r="G62" s="14"/>
-      <c r="H62" s="14"/>
-      <c r="I62" s="14"/>
-      <c r="J62" s="14"/>
-    </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A63" s="14"/>
-      <c r="B63" s="14"/>
+    </row>
+    <row r="63" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C63" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D63" s="14"/>
-      <c r="E63" s="14"/>
-      <c r="F63" s="14"/>
-      <c r="G63" s="14"/>
-      <c r="H63" s="14"/>
-      <c r="I63" s="14"/>
-      <c r="J63" s="14"/>
-    </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A64" s="14"/>
-      <c r="B64" s="14"/>
+    </row>
+    <row r="64" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C64" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D64" s="15"/>
+      <c r="D64" s="14"/>
       <c r="E64" s="3"/>
       <c r="F64" s="3"/>
       <c r="G64" s="3"/>
       <c r="H64" s="3"/>
       <c r="I64" s="3"/>
       <c r="J64" s="3"/>
-      <c r="K64" s="4"/>
-    </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A65" s="14"/>
-      <c r="B65" s="14"/>
+      <c r="K64" s="3"/>
+      <c r="L64" s="3"/>
+      <c r="M64" s="3"/>
+      <c r="N64" s="4"/>
+    </row>
+    <row r="65" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C65" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D65" s="14"/>
-      <c r="E65" s="14"/>
-      <c r="F65" s="14"/>
-      <c r="G65" s="14"/>
-      <c r="H65" s="14"/>
-      <c r="I65" s="14"/>
-      <c r="J65" s="14"/>
-    </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A66" s="14"/>
-      <c r="B66" s="14"/>
+    </row>
+    <row r="66" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C66" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D66" s="14"/>
-      <c r="E66" s="14"/>
-      <c r="F66" s="14"/>
-      <c r="G66" s="14"/>
-      <c r="H66" s="14"/>
-      <c r="I66" s="14"/>
-      <c r="J66" s="14"/>
-    </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A67" s="14"/>
-      <c r="B67" s="14"/>
+    </row>
+    <row r="67" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C67" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D67" s="15"/>
+      <c r="D67" s="14"/>
       <c r="E67" s="3"/>
       <c r="F67" s="3"/>
       <c r="G67" s="3"/>
       <c r="H67" s="3"/>
       <c r="I67" s="3"/>
       <c r="J67" s="3"/>
-      <c r="K67" s="4"/>
-    </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A68" s="14"/>
-      <c r="B68" s="14"/>
+      <c r="K67" s="3"/>
+      <c r="L67" s="3"/>
+      <c r="M67" s="3"/>
+      <c r="N67" s="4"/>
+    </row>
+    <row r="68" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C68" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D68" s="14"/>
-      <c r="E68" s="14"/>
-      <c r="F68" s="14"/>
-      <c r="G68" s="14"/>
-      <c r="H68" s="14"/>
-      <c r="I68" s="14"/>
-      <c r="J68" s="14"/>
-    </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A69" s="14"/>
-      <c r="B69" s="14"/>
+    </row>
+    <row r="69" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C69" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D69" s="14"/>
-      <c r="E69" s="14"/>
-      <c r="F69" s="14"/>
-      <c r="G69" s="14"/>
-      <c r="H69" s="14"/>
-      <c r="I69" s="14"/>
-      <c r="J69" s="14"/>
-    </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A70" s="14"/>
-      <c r="B70" s="14"/>
+    </row>
+    <row r="70" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C70" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D70" s="15"/>
+      <c r="D70" s="14"/>
       <c r="E70" s="3"/>
       <c r="F70" s="3"/>
       <c r="G70" s="3"/>
       <c r="H70" s="3"/>
       <c r="I70" s="3"/>
       <c r="J70" s="3"/>
-      <c r="K70" s="4"/>
-    </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A71" s="14"/>
-      <c r="B71" s="14"/>
+      <c r="K70" s="3"/>
+      <c r="L70" s="3"/>
+      <c r="M70" s="3"/>
+      <c r="N70" s="4"/>
+    </row>
+    <row r="71" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C71" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D71" s="14"/>
-      <c r="E71" s="14"/>
-      <c r="F71" s="14"/>
-      <c r="G71" s="14"/>
-      <c r="H71" s="14"/>
-      <c r="I71" s="14"/>
-      <c r="J71" s="14"/>
-    </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A72" s="14"/>
-      <c r="B72" s="14"/>
+    </row>
+    <row r="72" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C72" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D72" s="14"/>
-      <c r="E72" s="14"/>
-      <c r="F72" s="14"/>
-      <c r="G72" s="14"/>
-      <c r="H72" s="14"/>
-      <c r="I72" s="14"/>
-      <c r="J72" s="14"/>
-    </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A73" s="14"/>
-      <c r="B73" s="14"/>
+    </row>
+    <row r="73" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C73" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D73" s="15"/>
+      <c r="D73" s="14"/>
       <c r="E73" s="3"/>
       <c r="F73" s="3"/>
       <c r="G73" s="3"/>
       <c r="H73" s="3"/>
       <c r="I73" s="3"/>
       <c r="J73" s="3"/>
-      <c r="K73" s="4"/>
-    </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K73" s="3"/>
+      <c r="L73" s="3"/>
+      <c r="M73" s="3"/>
+      <c r="N73" s="4"/>
+    </row>
+    <row r="74" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C74" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C75" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A76" s="3"/>
       <c r="B76" s="3"/>
       <c r="C76" s="4" t="s">
@@ -3929,195 +3273,132 @@
       <c r="H76" s="3"/>
       <c r="I76" s="3"/>
       <c r="J76" s="3"/>
-      <c r="K76" s="4"/>
-    </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A77" s="14">
+      <c r="K76" s="3"/>
+      <c r="L76" s="3"/>
+      <c r="M76" s="3"/>
+      <c r="N76" s="4"/>
+    </row>
+    <row r="77" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A77" s="2">
         <v>1000</v>
       </c>
-      <c r="B77" s="14" t="s">
+      <c r="B77" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C77" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D77" s="14"/>
-      <c r="E77" s="14"/>
-      <c r="F77" s="14"/>
-      <c r="G77" s="14"/>
-      <c r="H77" s="14"/>
-      <c r="I77" s="14"/>
-      <c r="J77" s="14"/>
-    </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A78" s="14"/>
-      <c r="B78" s="14"/>
+    </row>
+    <row r="78" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C78" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D78" s="14"/>
-      <c r="E78" s="14"/>
-      <c r="F78" s="14"/>
-      <c r="G78" s="14"/>
-      <c r="H78" s="14"/>
-      <c r="I78" s="14"/>
-      <c r="J78" s="14"/>
-    </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A79" s="14"/>
-      <c r="B79" s="14"/>
+    </row>
+    <row r="79" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C79" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D79" s="15"/>
+      <c r="D79" s="14"/>
       <c r="E79" s="3"/>
       <c r="F79" s="3"/>
       <c r="G79" s="3"/>
       <c r="H79" s="3"/>
       <c r="I79" s="3"/>
       <c r="J79" s="3"/>
-      <c r="K79" s="4"/>
-    </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A80" s="14"/>
-      <c r="B80" s="14"/>
+      <c r="K79" s="3"/>
+      <c r="L79" s="3"/>
+      <c r="M79" s="3"/>
+      <c r="N79" s="4"/>
+    </row>
+    <row r="80" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C80" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D80" s="14"/>
-      <c r="E80" s="14"/>
-      <c r="F80" s="14"/>
-      <c r="G80" s="14"/>
-      <c r="H80" s="14"/>
-      <c r="I80" s="14"/>
-      <c r="J80" s="14"/>
-    </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A81" s="14"/>
-      <c r="B81" s="14"/>
+    </row>
+    <row r="81" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C81" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D81" s="14"/>
-      <c r="E81" s="14"/>
-      <c r="F81" s="14"/>
-      <c r="G81" s="14"/>
-      <c r="H81" s="14"/>
-      <c r="I81" s="14"/>
-      <c r="J81" s="14"/>
-    </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A82" s="14"/>
-      <c r="B82" s="14"/>
+    </row>
+    <row r="82" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C82" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D82" s="15"/>
+      <c r="D82" s="14"/>
       <c r="E82" s="3"/>
       <c r="F82" s="3"/>
       <c r="G82" s="3"/>
       <c r="H82" s="3"/>
       <c r="I82" s="3"/>
       <c r="J82" s="3"/>
-      <c r="K82" s="4"/>
-    </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A83" s="14"/>
-      <c r="B83" s="14"/>
+      <c r="K82" s="3"/>
+      <c r="L82" s="3"/>
+      <c r="M82" s="3"/>
+      <c r="N82" s="4"/>
+    </row>
+    <row r="83" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C83" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D83" s="14"/>
-      <c r="E83" s="14"/>
-      <c r="F83" s="14"/>
-      <c r="G83" s="14"/>
-      <c r="H83" s="14"/>
-      <c r="I83" s="14"/>
-      <c r="J83" s="14"/>
-    </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A84" s="14"/>
-      <c r="B84" s="14"/>
+    </row>
+    <row r="84" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C84" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D84" s="14"/>
-      <c r="E84" s="14"/>
-      <c r="F84" s="14"/>
-      <c r="G84" s="14"/>
-      <c r="H84" s="14"/>
-      <c r="I84" s="14"/>
-      <c r="J84" s="14"/>
-    </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A85" s="14"/>
-      <c r="B85" s="14"/>
+    </row>
+    <row r="85" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C85" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D85" s="15"/>
+      <c r="D85" s="14"/>
       <c r="E85" s="3"/>
       <c r="F85" s="3"/>
       <c r="G85" s="3"/>
       <c r="H85" s="3"/>
       <c r="I85" s="3"/>
       <c r="J85" s="3"/>
-      <c r="K85" s="4"/>
-    </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A86" s="14"/>
-      <c r="B86" s="14"/>
+      <c r="K85" s="3"/>
+      <c r="L85" s="3"/>
+      <c r="M85" s="3"/>
+      <c r="N85" s="4"/>
+    </row>
+    <row r="86" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C86" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D86" s="14"/>
-      <c r="E86" s="14"/>
-      <c r="F86" s="14"/>
-      <c r="G86" s="14"/>
-      <c r="H86" s="14"/>
-      <c r="I86" s="14"/>
-      <c r="J86" s="14"/>
-    </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A87" s="14"/>
-      <c r="B87" s="14"/>
+    </row>
+    <row r="87" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C87" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D87" s="14"/>
-      <c r="E87" s="14"/>
-      <c r="F87" s="14"/>
-      <c r="G87" s="14"/>
-      <c r="H87" s="14"/>
-      <c r="I87" s="14"/>
-      <c r="J87" s="14"/>
-    </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A88" s="14"/>
-      <c r="B88" s="14"/>
+    </row>
+    <row r="88" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C88" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D88" s="15"/>
+      <c r="D88" s="14"/>
       <c r="E88" s="3"/>
       <c r="F88" s="3"/>
       <c r="G88" s="3"/>
       <c r="H88" s="3"/>
       <c r="I88" s="3"/>
       <c r="J88" s="3"/>
-      <c r="K88" s="4"/>
-    </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K88" s="3"/>
+      <c r="L88" s="3"/>
+      <c r="M88" s="3"/>
+      <c r="N88" s="4"/>
+    </row>
+    <row r="89" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C89" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C90" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A91" s="3"/>
       <c r="B91" s="3"/>
       <c r="C91" s="4" t="s">
@@ -4130,7 +3411,10 @@
       <c r="H91" s="3"/>
       <c r="I91" s="3"/>
       <c r="J91" s="3"/>
-      <c r="K91" s="4"/>
+      <c r="K91" s="3"/>
+      <c r="L91" s="3"/>
+      <c r="M91" s="3"/>
+      <c r="N91" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4247,7 +3531,7 @@
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView topLeftCell="A3" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="M4" sqref="M4"/>
+      <selection activeCell="D5" sqref="D4:D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
fixed yield error and set yield stress for evpt scripts
</commit_message>
<xml_diff>
--- a/scripts/__other__/__sem__.xlsx
+++ b/scripts/__other__/__sem__.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Janzen\Desktop\code\moga_neml\scripts\__other__\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46E92EC4-05C1-4A8E-9945-61485B4D742A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5E3BFF6-C13E-48E7-A2AE-A956B931B486}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2406,7 +2406,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F11" sqref="F11"/>
+      <selection pane="bottomLeft" activeCell="I9" sqref="D8:I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2554,21 +2554,6 @@
       <c r="C8" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D8" s="2">
-        <v>4.8710000000000004</v>
-      </c>
-      <c r="E8" s="2">
-        <v>11.518000000000001</v>
-      </c>
-      <c r="F8" s="2">
-        <v>7.0281000000000002</v>
-      </c>
-      <c r="G8" s="2">
-        <v>4.2420999999999998</v>
-      </c>
-      <c r="H8" s="2">
-        <v>1138.3</v>
-      </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C9" s="1" t="s">
@@ -2866,6 +2851,21 @@
     <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C35" s="1" t="s">
         <v>13</v>
+      </c>
+      <c r="D35" s="2">
+        <v>4.8710000000000004</v>
+      </c>
+      <c r="E35" s="2">
+        <v>11.518000000000001</v>
+      </c>
+      <c r="F35" s="2">
+        <v>7.0281000000000002</v>
+      </c>
+      <c r="G35" s="2">
+        <v>4.2420999999999998</v>
+      </c>
+      <c r="H35" s="2">
+        <v>1138.3</v>
       </c>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Altered plotting code and changed bounds of evp
</commit_message>
<xml_diff>
--- a/scripts/__other__/__sem__.xlsx
+++ b/scripts/__other__/__sem__.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Janzen\Desktop\code\moga_neml\scripts\__other__\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B73552A-1BC3-4CB7-8A7E-18C995D12128}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D23BB5F4-946E-4D58-8F36-F6DE14F142DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -167,7 +167,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -182,9 +182,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -471,7 +468,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H80" sqref="H80"/>
+      <selection pane="bottomLeft" activeCell="L7" sqref="D6:L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -592,82 +589,57 @@
         <v>13</v>
       </c>
       <c r="D5" s="2">
-        <v>4.8710000000000004</v>
+        <v>0.67196999999999996</v>
       </c>
       <c r="E5" s="2">
-        <v>11.52</v>
+        <v>25.75</v>
       </c>
       <c r="F5" s="2">
-        <v>7.0279999999999996</v>
+        <v>43.168999999999997</v>
       </c>
       <c r="G5" s="2">
-        <v>4.242</v>
+        <v>4.4878999999999998</v>
       </c>
       <c r="H5" s="2">
-        <v>1138</v>
+        <v>1669.9</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C6" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="I6" s="2">
-        <v>2001.1</v>
-      </c>
-      <c r="J6" s="2">
-        <v>4.3449999999999998</v>
-      </c>
-      <c r="K6" s="1">
-        <v>6.5937000000000001</v>
-      </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C7" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D7" s="5">
-        <v>6.7199</v>
-      </c>
-      <c r="E7" s="3">
-        <v>10.962</v>
-      </c>
-      <c r="F7" s="3">
-        <v>7.1666999999999996</v>
-      </c>
-      <c r="G7" s="3">
-        <v>4.2279999999999998</v>
-      </c>
-      <c r="H7" s="3">
-        <v>1138.0999999999999</v>
-      </c>
-      <c r="I7" s="3">
-        <v>5653.1</v>
-      </c>
-      <c r="J7" s="3">
-        <v>3.4941</v>
-      </c>
-      <c r="K7" s="4">
-        <v>6.4192</v>
-      </c>
+      <c r="D7" s="5"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
+      <c r="K7" s="4"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C8" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D8" s="2">
-        <v>29.48710434625011</v>
+        <v>29.486999999999998</v>
       </c>
       <c r="E8" s="2">
-        <v>16.249786454450639</v>
+        <v>16.2498</v>
       </c>
       <c r="F8" s="2">
-        <v>54.943238516067588</v>
+        <v>54.942999999999998</v>
       </c>
       <c r="G8" s="2">
-        <v>2.338120137251932</v>
+        <v>2.3380999999999998</v>
       </c>
       <c r="H8" s="2">
-        <v>29597.640177599191</v>
+        <v>29598</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
@@ -693,19 +665,19 @@
         <v>13</v>
       </c>
       <c r="D11" s="2">
-        <v>41.512193477437982</v>
+        <v>41.512</v>
       </c>
       <c r="E11" s="2">
-        <v>26.942086185360139</v>
+        <v>26.942</v>
       </c>
       <c r="F11" s="2">
-        <v>0.38245424784143423</v>
+        <v>0.38245000000000001</v>
       </c>
       <c r="G11" s="2">
-        <v>2.542940330293872</v>
+        <v>2.5428999999999999</v>
       </c>
       <c r="H11" s="2">
-        <v>18404.701345106248</v>
+        <v>18405</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
@@ -830,37 +802,30 @@
       <c r="C20" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D20" s="6">
+      <c r="D20" s="2">
         <v>16.04428385491871</v>
       </c>
-      <c r="E20" s="6">
+      <c r="E20" s="2">
         <v>34.763324369786773</v>
       </c>
-      <c r="F20" s="6">
+      <c r="F20" s="2">
         <v>20.428082185584771</v>
       </c>
-      <c r="G20" s="6">
+      <c r="G20" s="2">
         <v>3.4181098245129382</v>
       </c>
-      <c r="H20" s="6">
+      <c r="H20" s="2">
         <v>3359.022419623268</v>
       </c>
-      <c r="I20" s="6"/>
-      <c r="J20" s="6"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C21" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D21" s="6"/>
-      <c r="E21" s="6"/>
-      <c r="F21" s="6"/>
-      <c r="G21" s="6"/>
-      <c r="H21" s="6"/>
-      <c r="I21" s="6">
+      <c r="I21" s="2">
         <v>1810.3618787343121</v>
       </c>
-      <c r="J21" s="6">
+      <c r="J21" s="2">
         <v>5.6613449320954823</v>
       </c>
       <c r="K21" s="1">
@@ -884,37 +849,30 @@
       <c r="C23" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D23" s="6">
+      <c r="D23" s="2">
         <v>12.92875597442686</v>
       </c>
-      <c r="E23" s="6">
+      <c r="E23" s="2">
         <v>37.179916942379421</v>
       </c>
-      <c r="F23" s="6">
+      <c r="F23" s="2">
         <v>29.64304595299074</v>
       </c>
-      <c r="G23" s="6">
+      <c r="G23" s="2">
         <v>2.9071671931862282</v>
       </c>
-      <c r="H23" s="6">
+      <c r="H23" s="2">
         <v>7297.7055051839016</v>
       </c>
-      <c r="I23" s="6"/>
-      <c r="J23" s="6"/>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C24" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D24" s="6"/>
-      <c r="E24" s="6"/>
-      <c r="F24" s="6"/>
-      <c r="G24" s="6"/>
-      <c r="H24" s="6"/>
-      <c r="I24" s="6">
+      <c r="I24" s="2">
         <v>1732.0325860447231</v>
       </c>
-      <c r="J24" s="6">
+      <c r="J24" s="2">
         <v>5.7769616328705169</v>
       </c>
       <c r="K24" s="1">
@@ -938,37 +896,30 @@
       <c r="C26" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D26" s="6">
+      <c r="D26" s="2">
         <v>18.53076465328833</v>
       </c>
-      <c r="E26" s="6">
+      <c r="E26" s="2">
         <v>28.649378900720709</v>
       </c>
-      <c r="F26" s="6">
+      <c r="F26" s="2">
         <v>24.82714264975634</v>
       </c>
-      <c r="G26" s="6">
+      <c r="G26" s="2">
         <v>3.3281591046792629</v>
       </c>
-      <c r="H26" s="6">
+      <c r="H26" s="2">
         <v>3890.91748087838</v>
       </c>
-      <c r="I26" s="6"/>
-      <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C27" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D27" s="6"/>
-      <c r="E27" s="6"/>
-      <c r="F27" s="6"/>
-      <c r="G27" s="6"/>
-      <c r="H27" s="6"/>
-      <c r="I27" s="6">
+      <c r="I27" s="2">
         <v>1866.999975475695</v>
       </c>
-      <c r="J27" s="6">
+      <c r="J27" s="2">
         <v>5.6610176207638876</v>
       </c>
       <c r="K27" s="1">
@@ -1107,19 +1058,19 @@
         <v>13</v>
       </c>
       <c r="D38" s="2">
-        <v>0.6719725137228032</v>
+        <v>0.67196999999999996</v>
       </c>
       <c r="E38" s="2">
-        <v>25.749973486243881</v>
+        <v>25.75</v>
       </c>
       <c r="F38" s="2">
-        <v>43.168813737144347</v>
+        <v>43.168999999999997</v>
       </c>
       <c r="G38" s="2">
-        <v>4.4878846976929143</v>
+        <v>4.4878999999999998</v>
       </c>
       <c r="H38" s="2">
-        <v>1669.8507856032959</v>
+        <v>1669.9</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
@@ -1206,37 +1157,30 @@
       <c r="C44" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D44" s="6">
+      <c r="D44" s="2">
         <v>17.444047229999999</v>
       </c>
-      <c r="E44" s="6">
+      <c r="E44" s="2">
         <v>12.402704849999999</v>
       </c>
-      <c r="F44" s="6">
+      <c r="F44" s="2">
         <v>7.7502457690000002</v>
       </c>
-      <c r="G44" s="6">
+      <c r="G44" s="2">
         <v>1.924995791</v>
       </c>
-      <c r="H44" s="6">
+      <c r="H44" s="2">
         <v>70080.791989999998</v>
       </c>
-      <c r="I44" s="6"/>
-      <c r="J44" s="6"/>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C45" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D45" s="6"/>
-      <c r="E45" s="6"/>
-      <c r="F45" s="6"/>
-      <c r="G45" s="6"/>
-      <c r="H45" s="6"/>
-      <c r="I45" s="6">
+      <c r="I45" s="2">
         <v>2370.035856</v>
       </c>
-      <c r="J45" s="6">
+      <c r="J45" s="2">
         <v>4.2028263880000001</v>
       </c>
       <c r="K45" s="1">
@@ -1771,6 +1715,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
added new parameters to evpcd and evpwd scripts
</commit_message>
<xml_diff>
--- a/scripts/__other__/__sem__.xlsx
+++ b/scripts/__other__/__sem__.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Janzen\Desktop\code\moga_neml\scripts\__other__\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E91B00F-30E1-4A95-8C8E-3ED2ABA02537}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{507D1849-8B6A-45A6-92CB-0CE144A12CFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="evp" sheetId="13" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="33">
   <si>
     <t>temp</t>
   </si>
@@ -113,6 +113,30 @@
   </si>
   <si>
     <t>x</t>
+  </si>
+  <si>
+    <t>ST cr eh</t>
+  </si>
+  <si>
+    <t>cr eh; ts over</t>
+  </si>
+  <si>
+    <t>cr eh</t>
+  </si>
+  <si>
+    <t>evpcd</t>
+  </si>
+  <si>
+    <t>evpwd</t>
+  </si>
+  <si>
+    <t>cr early</t>
+  </si>
+  <si>
+    <t>cr und; ts und</t>
+  </si>
+  <si>
+    <t>cr und</t>
   </si>
 </sst>
 </file>
@@ -230,7 +254,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -279,6 +303,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -562,9 +592,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4D7A15E-4182-42F6-82DA-99E9B04906BA}">
   <dimension ref="A1:O73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I11" sqref="I11"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L30" sqref="L30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -574,10 +604,11 @@
     <col min="3" max="3" width="15.7109375" style="8" customWidth="1"/>
     <col min="4" max="7" width="9.140625" style="4"/>
     <col min="8" max="8" width="9.140625" style="3"/>
-    <col min="9" max="16384" width="9.140625" style="4"/>
+    <col min="9" max="10" width="15.7109375" style="8" customWidth="1"/>
+    <col min="11" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -602,8 +633,14 @@
       <c r="H1" s="6" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I1" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="J1" s="7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="11">
         <v>800</v>
       </c>
@@ -611,7 +648,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="12"/>
       <c r="B3" s="15"/>
       <c r="C3" s="8" t="s">
@@ -632,11 +669,14 @@
       <c r="H3" s="3">
         <v>1783.5</v>
       </c>
-      <c r="I3" s="4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I3" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="J3" s="8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="12"/>
       <c r="B4" s="15"/>
       <c r="C4" s="8" t="s">
@@ -657,8 +697,14 @@
       <c r="H4" s="1">
         <v>1621.6</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I4" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="J4" s="8" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="12"/>
       <c r="B5" s="15"/>
       <c r="C5" s="8" t="s">
@@ -680,7 +726,7 @@
         <v>1775.9</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="12"/>
       <c r="B6" s="15"/>
       <c r="C6" s="8" t="s">
@@ -702,7 +748,7 @@
         <v>1598.4</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="12"/>
       <c r="B7" s="15"/>
       <c r="C7" s="8" t="s">
@@ -724,7 +770,7 @@
         <v>1574.3</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="12"/>
       <c r="B8" s="15"/>
       <c r="C8" s="8" t="s">
@@ -746,7 +792,7 @@
         <v>1944.6</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="12"/>
       <c r="B9" s="15"/>
       <c r="C9" s="8" t="s">
@@ -768,7 +814,7 @@
         <v>2454.8000000000002</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="12"/>
       <c r="B10" s="15"/>
       <c r="C10" s="8" t="s">
@@ -790,7 +836,7 @@
         <v>2390.5</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="12"/>
       <c r="B11" s="15"/>
       <c r="C11" s="8" t="s">
@@ -812,7 +858,7 @@
         <v>1614.6</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="12"/>
       <c r="B12" s="15"/>
       <c r="C12" s="8" t="s">
@@ -834,13 +880,15 @@
         <v>1841</v>
       </c>
     </row>
-    <row r="13" spans="1:9" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="13"/>
       <c r="B13" s="16"/>
       <c r="C13" s="7"/>
       <c r="H13" s="6"/>
-    </row>
-    <row r="14" spans="1:9" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I13" s="7"/>
+      <c r="J13" s="7"/>
+    </row>
+    <row r="14" spans="1:10" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="11">
         <v>800</v>
       </c>
@@ -848,7 +896,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="12"/>
       <c r="B15" s="15"/>
       <c r="C15" s="8" t="s">
@@ -869,11 +917,11 @@
       <c r="H15" s="3">
         <v>2575.8000000000002</v>
       </c>
-      <c r="I15" s="4" t="s">
+      <c r="I15" s="8" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="12"/>
       <c r="B16" s="15"/>
       <c r="C16" s="8" t="s">
@@ -894,8 +942,14 @@
       <c r="H16" s="1">
         <v>1828.1</v>
       </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I16" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="J16" s="8" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="12"/>
       <c r="B17" s="15"/>
       <c r="C17" s="8" t="s">
@@ -917,7 +971,7 @@
         <v>2221.6</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="12"/>
       <c r="B18" s="15"/>
       <c r="C18" s="8" t="s">
@@ -939,7 +993,7 @@
         <v>3172</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="12"/>
       <c r="B19" s="15"/>
       <c r="C19" s="8" t="s">
@@ -961,7 +1015,7 @@
         <v>1677.4</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="12"/>
       <c r="B20" s="15"/>
       <c r="C20" s="8" t="s">
@@ -983,7 +1037,7 @@
         <v>1822.6</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="12"/>
       <c r="B21" s="15"/>
       <c r="C21" s="8" t="s">
@@ -1005,7 +1059,7 @@
         <v>2583</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="12"/>
       <c r="B22" s="15"/>
       <c r="C22" s="8" t="s">
@@ -1027,7 +1081,7 @@
         <v>2101.3000000000002</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="12"/>
       <c r="B23" s="15"/>
       <c r="C23" s="8" t="s">
@@ -1049,7 +1103,7 @@
         <v>1261.4000000000001</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="12"/>
       <c r="B24" s="15"/>
       <c r="C24" s="8" t="s">
@@ -1071,13 +1125,15 @@
         <v>3016.2</v>
       </c>
     </row>
-    <row r="25" spans="1:9" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="13"/>
       <c r="B25" s="16"/>
       <c r="C25" s="7"/>
       <c r="H25" s="6"/>
-    </row>
-    <row r="26" spans="1:9" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I25" s="7"/>
+      <c r="J25" s="7"/>
+    </row>
+    <row r="26" spans="1:10" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="11">
         <v>900</v>
       </c>
@@ -1085,161 +1141,176 @@
         <v>6</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="12"/>
       <c r="B27" s="15"/>
       <c r="C27" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="D27" s="2">
-        <v>10.692</v>
-      </c>
-      <c r="E27" s="2">
-        <v>29.068000000000001</v>
-      </c>
-      <c r="F27" s="2">
-        <v>2.9830999999999999</v>
-      </c>
-      <c r="G27" s="2">
-        <v>3.7277999999999998</v>
-      </c>
-      <c r="H27" s="1">
-        <v>1433.5</v>
-      </c>
-      <c r="I27" s="4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D27" s="4">
+        <v>4.8710000000000004</v>
+      </c>
+      <c r="E27" s="4">
+        <v>11.518000000000001</v>
+      </c>
+      <c r="F27" s="4">
+        <v>7.0281000000000002</v>
+      </c>
+      <c r="G27" s="4">
+        <v>4.2420999999999998</v>
+      </c>
+      <c r="H27" s="3">
+        <v>1138.3</v>
+      </c>
+      <c r="I27" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="J27" s="8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="12"/>
       <c r="B28" s="15"/>
       <c r="C28" s="8" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D28" s="2">
-        <v>11.2</v>
+        <v>10.692</v>
       </c>
       <c r="E28" s="2">
-        <v>24.262</v>
+        <v>29.068000000000001</v>
       </c>
       <c r="F28" s="2">
-        <v>2.2614999999999998</v>
+        <v>2.9830999999999999</v>
       </c>
       <c r="G28" s="2">
-        <v>3.9651000000000001</v>
+        <v>3.7277999999999998</v>
       </c>
       <c r="H28" s="1">
-        <v>1163</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1433.5</v>
+      </c>
+      <c r="I28" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="J28" s="8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="12"/>
       <c r="B29" s="15"/>
       <c r="C29" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="D29" s="4">
-        <v>11.208</v>
-      </c>
-      <c r="E29" s="4">
-        <v>16.738</v>
-      </c>
-      <c r="F29" s="4">
-        <v>5.9587000000000003</v>
-      </c>
-      <c r="G29" s="4">
-        <v>3.6377000000000002</v>
-      </c>
-      <c r="H29" s="3">
-        <v>1530.1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+      <c r="D29" s="2">
+        <v>11.2</v>
+      </c>
+      <c r="E29" s="2">
+        <v>24.262</v>
+      </c>
+      <c r="F29" s="2">
+        <v>2.2614999999999998</v>
+      </c>
+      <c r="G29" s="2">
+        <v>3.9651000000000001</v>
+      </c>
+      <c r="H29" s="1">
+        <v>1163</v>
+      </c>
+      <c r="I29" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="J29" s="8" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="12"/>
       <c r="B30" s="15"/>
       <c r="C30" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="D30" s="2">
-        <v>10.45</v>
-      </c>
-      <c r="E30" s="2">
-        <v>14.769</v>
-      </c>
-      <c r="F30" s="2">
-        <v>7.8792</v>
-      </c>
-      <c r="G30" s="2">
-        <v>3.54</v>
-      </c>
-      <c r="H30" s="1">
-        <v>1787.3</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+      <c r="D30" s="4">
+        <v>11.208</v>
+      </c>
+      <c r="E30" s="4">
+        <v>16.738</v>
+      </c>
+      <c r="F30" s="4">
+        <v>5.9587000000000003</v>
+      </c>
+      <c r="G30" s="4">
+        <v>3.6377000000000002</v>
+      </c>
+      <c r="H30" s="3">
+        <v>1530.1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="12"/>
       <c r="B31" s="15"/>
       <c r="C31" s="8" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D31" s="2">
-        <v>11.010999999999999</v>
+        <v>10.45</v>
       </c>
       <c r="E31" s="2">
-        <v>11.071</v>
+        <v>14.769</v>
       </c>
       <c r="F31" s="2">
-        <v>13.523</v>
+        <v>7.8792</v>
       </c>
       <c r="G31" s="2">
-        <v>3.5672000000000001</v>
+        <v>3.54</v>
       </c>
       <c r="H31" s="1">
-        <v>1593.8</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1787.3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="12"/>
       <c r="B32" s="15"/>
       <c r="C32" s="8" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D32" s="2">
-        <v>5.6656000000000004</v>
+        <v>11.010999999999999</v>
       </c>
       <c r="E32" s="2">
-        <v>8.2222000000000008</v>
+        <v>11.071</v>
       </c>
       <c r="F32" s="2">
-        <v>14.47</v>
+        <v>13.523</v>
       </c>
       <c r="G32" s="2">
-        <v>4.3000999999999996</v>
+        <v>3.5672000000000001</v>
       </c>
       <c r="H32" s="1">
-        <v>1000.8</v>
+        <v>1593.8</v>
       </c>
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A33" s="12"/>
       <c r="B33" s="15"/>
       <c r="C33" s="8" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D33" s="2">
-        <v>15.185</v>
+        <v>5.6656000000000004</v>
       </c>
       <c r="E33" s="2">
-        <v>64.875</v>
+        <v>8.2222000000000008</v>
       </c>
       <c r="F33" s="2">
-        <v>1.4525999999999999</v>
+        <v>14.47</v>
       </c>
       <c r="G33" s="2">
-        <v>3.2002999999999999</v>
+        <v>4.3000999999999996</v>
       </c>
       <c r="H33" s="1">
-        <v>2110.6</v>
+        <v>1000.8</v>
       </c>
     </row>
     <row r="34" spans="1:15" x14ac:dyDescent="0.25">
@@ -1249,19 +1320,19 @@
         <v>19</v>
       </c>
       <c r="D34" s="2">
-        <v>8.0571999999999999</v>
+        <v>15.185</v>
       </c>
       <c r="E34" s="2">
-        <v>29.803999999999998</v>
+        <v>64.875</v>
       </c>
       <c r="F34" s="2">
-        <v>2.5836000000000001</v>
+        <v>1.4525999999999999</v>
       </c>
       <c r="G34" s="2">
-        <v>4.0204000000000004</v>
+        <v>3.2002999999999999</v>
       </c>
       <c r="H34" s="1">
-        <v>1210.4000000000001</v>
+        <v>2110.6</v>
       </c>
     </row>
     <row r="35" spans="1:15" x14ac:dyDescent="0.25">
@@ -1271,19 +1342,19 @@
         <v>19</v>
       </c>
       <c r="D35" s="2">
-        <v>7.5292000000000003</v>
+        <v>8.0571999999999999</v>
       </c>
       <c r="E35" s="2">
-        <v>23.504999999999999</v>
+        <v>29.803999999999998</v>
       </c>
       <c r="F35" s="2">
-        <v>4.9898999999999996</v>
+        <v>2.5836000000000001</v>
       </c>
       <c r="G35" s="2">
-        <v>3.8622999999999998</v>
+        <v>4.0204000000000004</v>
       </c>
       <c r="H35" s="1">
-        <v>1369.1</v>
+        <v>1210.4000000000001</v>
       </c>
     </row>
     <row r="36" spans="1:15" x14ac:dyDescent="0.25">
@@ -1292,20 +1363,20 @@
       <c r="C36" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="D36" s="4">
-        <v>4.8710000000000004</v>
-      </c>
-      <c r="E36" s="4">
-        <v>11.518000000000001</v>
-      </c>
-      <c r="F36" s="4">
-        <v>7.0281000000000002</v>
-      </c>
-      <c r="G36" s="4">
-        <v>4.2420999999999998</v>
-      </c>
-      <c r="H36" s="3">
-        <v>1138.3</v>
+      <c r="D36" s="2">
+        <v>7.5292000000000003</v>
+      </c>
+      <c r="E36" s="2">
+        <v>23.504999999999999</v>
+      </c>
+      <c r="F36" s="2">
+        <v>4.9898999999999996</v>
+      </c>
+      <c r="G36" s="2">
+        <v>3.8622999999999998</v>
+      </c>
+      <c r="H36" s="1">
+        <v>1369.1</v>
       </c>
     </row>
     <row r="37" spans="1:15" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
@@ -1313,6 +1384,8 @@
       <c r="B37" s="16"/>
       <c r="C37" s="7"/>
       <c r="H37" s="6"/>
+      <c r="I37" s="7"/>
+      <c r="J37" s="7"/>
     </row>
     <row r="38" spans="1:15" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="11">
@@ -1326,25 +1399,28 @@
       <c r="A39" s="12"/>
       <c r="B39" s="15"/>
       <c r="C39" s="8" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D39" s="4">
-        <v>7.1036999999999999</v>
+        <v>4.8238000000000003</v>
       </c>
       <c r="E39" s="4">
-        <v>48.234999999999999</v>
+        <v>378.86</v>
       </c>
       <c r="F39" s="4">
-        <v>4.2972000000000001</v>
+        <v>0.14230000000000001</v>
       </c>
       <c r="G39" s="4">
-        <v>3.4083999999999999</v>
+        <v>4.4020999999999999</v>
       </c>
       <c r="H39" s="3">
-        <v>1829.9</v>
-      </c>
-      <c r="I39" s="4" t="s">
-        <v>24</v>
+        <v>1006.9</v>
+      </c>
+      <c r="I39" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="J39" s="8" t="s">
+        <v>22</v>
       </c>
       <c r="K39" s="2"/>
       <c r="L39" s="2"/>
@@ -1356,23 +1432,34 @@
       <c r="A40" s="12"/>
       <c r="B40" s="15"/>
       <c r="C40" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D40" s="4">
-        <v>3.0461</v>
+        <v>7.1036999999999999</v>
       </c>
       <c r="E40" s="4">
-        <v>19.608000000000001</v>
+        <v>48.234999999999999</v>
       </c>
       <c r="F40" s="4">
-        <v>32.420999999999999</v>
+        <v>4.2972000000000001</v>
       </c>
       <c r="G40" s="4">
-        <v>3.2736000000000001</v>
+        <v>3.4083999999999999</v>
       </c>
       <c r="H40" s="3">
-        <v>2022.3</v>
-      </c>
+        <v>1829.9</v>
+      </c>
+      <c r="I40" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="J40" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="K40" s="2"/>
+      <c r="L40" s="2"/>
+      <c r="M40" s="2"/>
+      <c r="N40" s="2"/>
+      <c r="O40" s="2"/>
     </row>
     <row r="41" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A41" s="12"/>
@@ -1380,64 +1467,64 @@
       <c r="C41" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="D41" s="2">
-        <v>4.6340000000000003</v>
-      </c>
-      <c r="E41" s="2">
-        <v>18.606999999999999</v>
-      </c>
-      <c r="F41" s="2">
-        <v>24.896000000000001</v>
-      </c>
-      <c r="G41" s="2">
-        <v>3.3435999999999999</v>
-      </c>
-      <c r="H41" s="1">
-        <v>1999.7</v>
+      <c r="D41" s="4">
+        <v>3.0461</v>
+      </c>
+      <c r="E41" s="4">
+        <v>19.608000000000001</v>
+      </c>
+      <c r="F41" s="4">
+        <v>32.420999999999999</v>
+      </c>
+      <c r="G41" s="4">
+        <v>3.2736000000000001</v>
+      </c>
+      <c r="H41" s="3">
+        <v>2022.3</v>
       </c>
     </row>
     <row r="42" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A42" s="12"/>
       <c r="B42" s="15"/>
       <c r="C42" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D42" s="2">
-        <v>16.286999999999999</v>
+        <v>4.6340000000000003</v>
       </c>
       <c r="E42" s="2">
-        <v>181.45</v>
+        <v>18.606999999999999</v>
       </c>
       <c r="F42" s="2">
-        <v>0.52517000000000003</v>
+        <v>24.896000000000001</v>
       </c>
       <c r="G42" s="2">
-        <v>3.0160999999999998</v>
+        <v>3.3435999999999999</v>
       </c>
       <c r="H42" s="1">
-        <v>2606.1999999999998</v>
+        <v>1999.7</v>
       </c>
     </row>
     <row r="43" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A43" s="12"/>
       <c r="B43" s="15"/>
       <c r="C43" s="8" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="D43" s="2">
-        <v>9.5312999999999999</v>
+        <v>16.286999999999999</v>
       </c>
       <c r="E43" s="2">
-        <v>148.61000000000001</v>
+        <v>181.45</v>
       </c>
       <c r="F43" s="2">
-        <v>0.37484000000000001</v>
+        <v>0.52517000000000003</v>
       </c>
       <c r="G43" s="2">
-        <v>3.9621</v>
+        <v>3.0160999999999998</v>
       </c>
       <c r="H43" s="1">
-        <v>1253.9000000000001</v>
+        <v>2606.1999999999998</v>
       </c>
     </row>
     <row r="44" spans="1:15" x14ac:dyDescent="0.25">
@@ -1447,19 +1534,19 @@
         <v>19</v>
       </c>
       <c r="D44" s="2">
-        <v>6.3647</v>
+        <v>9.5312999999999999</v>
       </c>
       <c r="E44" s="2">
-        <v>149.54</v>
+        <v>148.61000000000001</v>
       </c>
       <c r="F44" s="2">
-        <v>0.43913000000000002</v>
+        <v>0.37484000000000001</v>
       </c>
       <c r="G44" s="2">
-        <v>4.1839000000000004</v>
+        <v>3.9621</v>
       </c>
       <c r="H44" s="1">
-        <v>1127.5999999999999</v>
+        <v>1253.9000000000001</v>
       </c>
     </row>
     <row r="45" spans="1:15" x14ac:dyDescent="0.25">
@@ -1469,19 +1556,19 @@
         <v>19</v>
       </c>
       <c r="D45" s="2">
-        <v>12.622</v>
+        <v>6.3647</v>
       </c>
       <c r="E45" s="2">
-        <v>15.441000000000001</v>
+        <v>149.54</v>
       </c>
       <c r="F45" s="2">
-        <v>4.5385999999999997</v>
+        <v>0.43913000000000002</v>
       </c>
       <c r="G45" s="2">
-        <v>3.7305000000000001</v>
+        <v>4.1839000000000004</v>
       </c>
       <c r="H45" s="1">
-        <v>1371.6</v>
+        <v>1127.5999999999999</v>
       </c>
     </row>
     <row r="46" spans="1:15" x14ac:dyDescent="0.25">
@@ -1490,20 +1577,20 @@
       <c r="C46" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="D46" s="4">
-        <v>12.256</v>
-      </c>
-      <c r="E46" s="4">
-        <v>273.68</v>
-      </c>
-      <c r="F46" s="4">
-        <v>0.20866000000000001</v>
-      </c>
-      <c r="G46" s="4">
-        <v>3.8422000000000001</v>
-      </c>
-      <c r="H46" s="3">
-        <v>1242.3</v>
+      <c r="D46" s="2">
+        <v>12.622</v>
+      </c>
+      <c r="E46" s="2">
+        <v>15.441000000000001</v>
+      </c>
+      <c r="F46" s="2">
+        <v>4.5385999999999997</v>
+      </c>
+      <c r="G46" s="2">
+        <v>3.7305000000000001</v>
+      </c>
+      <c r="H46" s="1">
+        <v>1371.6</v>
       </c>
     </row>
     <row r="47" spans="1:15" x14ac:dyDescent="0.25">
@@ -1513,19 +1600,19 @@
         <v>19</v>
       </c>
       <c r="D47" s="4">
-        <v>4.8238000000000003</v>
+        <v>12.256</v>
       </c>
       <c r="E47" s="4">
-        <v>378.86</v>
+        <v>273.68</v>
       </c>
       <c r="F47" s="4">
-        <v>0.14230000000000001</v>
+        <v>0.20866000000000001</v>
       </c>
       <c r="G47" s="4">
-        <v>4.4020999999999999</v>
+        <v>3.8422000000000001</v>
       </c>
       <c r="H47" s="3">
-        <v>1006.9</v>
+        <v>1242.3</v>
       </c>
     </row>
     <row r="48" spans="1:15" x14ac:dyDescent="0.25">
@@ -1550,13 +1637,15 @@
         <v>1090</v>
       </c>
     </row>
-    <row r="49" spans="1:8" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:10" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="13"/>
       <c r="B49" s="16"/>
       <c r="C49" s="7"/>
       <c r="H49" s="6"/>
-    </row>
-    <row r="50" spans="1:8" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I49" s="7"/>
+      <c r="J49" s="7"/>
+    </row>
+    <row r="50" spans="1:10" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="11">
         <v>1000</v>
       </c>
@@ -1564,53 +1653,55 @@
         <v>6</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" s="12"/>
       <c r="B51" s="15"/>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" s="12"/>
       <c r="B52" s="15"/>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" s="12"/>
       <c r="B53" s="15"/>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" s="12"/>
       <c r="B54" s="15"/>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" s="12"/>
       <c r="B55" s="15"/>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" s="12"/>
       <c r="B56" s="15"/>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" s="12"/>
       <c r="B57" s="15"/>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" s="12"/>
       <c r="B58" s="15"/>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59" s="12"/>
       <c r="B59" s="15"/>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60" s="12"/>
       <c r="B60" s="15"/>
     </row>
-    <row r="61" spans="1:8" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:10" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="13"/>
       <c r="B61" s="16"/>
       <c r="C61" s="7"/>
       <c r="H61" s="6"/>
-    </row>
-    <row r="62" spans="1:8" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I61" s="7"/>
+      <c r="J61" s="7"/>
+    </row>
+    <row r="62" spans="1:10" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="11">
         <v>1000</v>
       </c>
@@ -1618,66 +1709,68 @@
         <v>7</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63" s="12"/>
       <c r="B63" s="15"/>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A64" s="12"/>
       <c r="B64" s="15"/>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A65" s="12"/>
       <c r="B65" s="15"/>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A66" s="12"/>
       <c r="B66" s="15"/>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A67" s="12"/>
       <c r="B67" s="15"/>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A68" s="12"/>
       <c r="B68" s="15"/>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A69" s="12"/>
       <c r="B69" s="15"/>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A70" s="12"/>
       <c r="B70" s="15"/>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A71" s="12"/>
       <c r="B71" s="15"/>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A72" s="12"/>
       <c r="B72" s="15"/>
     </row>
-    <row r="73" spans="1:8" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:10" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="13"/>
       <c r="B73" s="16"/>
       <c r="C73" s="7"/>
       <c r="H73" s="6"/>
+      <c r="I73" s="7"/>
+      <c r="J73" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A38:A49"/>
+    <mergeCell ref="B38:B49"/>
+    <mergeCell ref="A50:A61"/>
+    <mergeCell ref="B50:B61"/>
+    <mergeCell ref="A62:A73"/>
+    <mergeCell ref="B62:B73"/>
     <mergeCell ref="A2:A13"/>
     <mergeCell ref="B2:B13"/>
     <mergeCell ref="A14:A25"/>
     <mergeCell ref="B14:B25"/>
     <mergeCell ref="A26:A37"/>
     <mergeCell ref="B26:B37"/>
-    <mergeCell ref="A38:A49"/>
-    <mergeCell ref="B38:B49"/>
-    <mergeCell ref="A50:A61"/>
-    <mergeCell ref="B50:B61"/>
-    <mergeCell ref="A62:A73"/>
-    <mergeCell ref="B62:B73"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -1686,11 +1779,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE483CC8-AF2C-4D5A-AEE5-EF7DF4EC0883}">
-  <dimension ref="A1:S73"/>
+  <dimension ref="A1:T73"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G11" sqref="G11"/>
+      <selection pane="bottomLeft" activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1700,12 +1793,13 @@
     <col min="3" max="3" width="15.7109375" style="8" customWidth="1"/>
     <col min="4" max="10" width="9.140625" style="4"/>
     <col min="11" max="11" width="9.140625" style="3"/>
-    <col min="12" max="18" width="9.140625" style="4"/>
-    <col min="19" max="19" width="9.140625" style="3"/>
-    <col min="20" max="16384" width="9.140625" style="4"/>
+    <col min="12" max="12" width="15.7109375" style="8" customWidth="1"/>
+    <col min="13" max="19" width="9.140625" style="4"/>
+    <col min="20" max="20" width="9.140625" style="3"/>
+    <col min="21" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -1739,32 +1833,35 @@
       <c r="K1" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="L1" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="M1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="M1" s="5" t="s">
+      <c r="N1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="N1" s="5" t="s">
+      <c r="O1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="O1" s="5" t="s">
+      <c r="P1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="P1" s="5" t="s">
+      <c r="Q1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="Q1" s="5" t="s">
+      <c r="R1" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="R1" s="5" t="s">
+      <c r="S1" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="S1" s="6" t="s">
+      <c r="T1" s="6" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:19" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="11">
         <v>800</v>
       </c>
@@ -1772,129 +1869,86 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" s="12"/>
       <c r="B3" s="15"/>
+      <c r="C3" s="8" t="s">
+        <v>31</v>
+      </c>
       <c r="D3" s="4">
-        <v>10.077</v>
+        <v>17.216999999999999</v>
       </c>
       <c r="E3" s="4">
-        <v>32.911000000000001</v>
+        <v>179.74</v>
       </c>
       <c r="F3" s="4">
-        <v>21.905999999999999</v>
+        <v>0.61753999999999998</v>
       </c>
       <c r="G3" s="4">
-        <v>3.5992000000000002</v>
-      </c>
-      <c r="H3" s="4">
-        <v>3063</v>
-      </c>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+        <v>4.4165999999999999</v>
+      </c>
+      <c r="H3" s="17">
+        <v>1783.5</v>
+      </c>
+      <c r="I3" s="18">
+        <v>1761.4</v>
+      </c>
+      <c r="J3" s="2">
+        <v>5.6002000000000001</v>
+      </c>
+      <c r="K3" s="2">
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" s="12"/>
       <c r="B4" s="15"/>
-      <c r="D4" s="4">
-        <v>11.695</v>
-      </c>
-      <c r="E4" s="4">
-        <v>101.28</v>
-      </c>
-      <c r="F4" s="4">
-        <v>1.1411</v>
-      </c>
-      <c r="G4" s="4">
-        <v>4.6826999999999996</v>
-      </c>
-      <c r="H4" s="4">
-        <v>1595.5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="H4" s="17"/>
+      <c r="I4" s="17"/>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" s="12"/>
       <c r="B5" s="15"/>
-      <c r="D5" s="4">
-        <v>9.8171999999999997</v>
-      </c>
-      <c r="E5" s="4">
-        <v>101.47</v>
-      </c>
-      <c r="F5" s="4">
-        <v>1.4056999999999999</v>
-      </c>
-      <c r="G5" s="4">
-        <v>4.6856999999999998</v>
-      </c>
-      <c r="H5" s="4">
-        <v>1595.7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="H5" s="17"/>
+      <c r="I5" s="17"/>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" s="12"/>
       <c r="B6" s="15"/>
-      <c r="D6" s="4">
-        <v>31.815999999999999</v>
-      </c>
-      <c r="E6" s="4">
-        <v>59.655000000000001</v>
-      </c>
-      <c r="F6" s="4">
-        <v>1.0424</v>
-      </c>
-      <c r="G6" s="4">
-        <v>3.6473</v>
-      </c>
-      <c r="H6" s="4">
-        <v>2944</v>
-      </c>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" s="12"/>
       <c r="B7" s="15"/>
-      <c r="D7" s="4">
-        <v>20.015999999999998</v>
-      </c>
-      <c r="E7" s="4">
-        <v>69.863</v>
-      </c>
-      <c r="F7" s="4">
-        <v>1.1780999999999999</v>
-      </c>
-      <c r="G7" s="4">
-        <v>4.3254999999999999</v>
-      </c>
-      <c r="H7" s="4">
-        <v>1881.4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" s="12"/>
       <c r="B8" s="15"/>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" s="12"/>
       <c r="B9" s="15"/>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10" s="12"/>
       <c r="B10" s="15"/>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11" s="12"/>
       <c r="B11" s="15"/>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12" s="12"/>
       <c r="B12" s="15"/>
     </row>
-    <row r="13" spans="1:19" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:20" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="13"/>
       <c r="B13" s="16"/>
       <c r="C13" s="7"/>
       <c r="K13" s="6"/>
-      <c r="S13" s="6"/>
-    </row>
-    <row r="14" spans="1:19" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L13" s="7"/>
+      <c r="T13" s="6"/>
+    </row>
+    <row r="14" spans="1:20" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="11">
         <v>800</v>
       </c>
@@ -1902,129 +1956,55 @@
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15" s="12"/>
       <c r="B15" s="15"/>
-      <c r="D15" s="4">
-        <v>19.913</v>
-      </c>
-      <c r="E15" s="4">
-        <v>52.043999999999997</v>
-      </c>
-      <c r="F15" s="4">
-        <v>2.2252000000000001</v>
-      </c>
-      <c r="G15" s="4">
-        <v>4.3255999999999997</v>
-      </c>
-      <c r="H15" s="4">
-        <v>1847.9</v>
-      </c>
-    </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16" s="12"/>
       <c r="B16" s="15"/>
-      <c r="D16" s="4">
-        <v>31.327000000000002</v>
-      </c>
-      <c r="E16" s="4">
-        <v>104.92</v>
-      </c>
-      <c r="F16" s="4">
-        <v>0.8548</v>
-      </c>
-      <c r="G16" s="4">
-        <v>3.7507999999999999</v>
-      </c>
-      <c r="H16" s="4">
-        <v>2575.8000000000002</v>
-      </c>
-    </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A17" s="12"/>
       <c r="B17" s="15"/>
-      <c r="D17" s="4">
-        <v>0.85682000000000003</v>
-      </c>
-      <c r="E17" s="4">
-        <v>42.524000000000001</v>
-      </c>
-      <c r="F17" s="4">
-        <v>9.6282999999999994</v>
-      </c>
-      <c r="G17" s="4">
-        <v>4.5033000000000003</v>
-      </c>
-      <c r="H17" s="4">
-        <v>1707</v>
-      </c>
-    </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A18" s="12"/>
       <c r="B18" s="15"/>
-      <c r="D18" s="4">
-        <v>1.2122000000000001E-2</v>
-      </c>
-      <c r="E18" s="4">
-        <v>52.49</v>
-      </c>
-      <c r="F18" s="4">
-        <v>21.795999999999999</v>
-      </c>
-      <c r="G18" s="4">
-        <v>3.2532999999999999</v>
-      </c>
-      <c r="H18" s="4">
-        <v>3778</v>
-      </c>
-    </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A19" s="12"/>
       <c r="B19" s="15"/>
-      <c r="D19" s="4">
-        <v>17.216999999999999</v>
-      </c>
-      <c r="E19" s="4">
-        <v>179.74</v>
-      </c>
-      <c r="F19" s="4">
-        <v>0.61753999999999998</v>
-      </c>
-      <c r="G19" s="4">
-        <v>4.4165999999999999</v>
-      </c>
-      <c r="H19" s="4">
-        <v>1783.5</v>
-      </c>
-    </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A20" s="12"/>
       <c r="B20" s="15"/>
     </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A21" s="12"/>
       <c r="B21" s="15"/>
     </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A22" s="12"/>
       <c r="B22" s="15"/>
     </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A23" s="12"/>
       <c r="B23" s="15"/>
     </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A24" s="12"/>
       <c r="B24" s="15"/>
     </row>
-    <row r="25" spans="1:19" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:20" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="13"/>
       <c r="B25" s="16"/>
       <c r="C25" s="7"/>
       <c r="K25" s="6"/>
-      <c r="S25" s="6"/>
-    </row>
-    <row r="26" spans="1:19" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L25" s="7"/>
+      <c r="T25" s="6"/>
+    </row>
+    <row r="26" spans="1:20" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="11">
         <v>900</v>
       </c>
@@ -2032,9 +2012,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A27" s="12"/>
       <c r="B27" s="15"/>
+      <c r="C27" s="8" t="s">
+        <v>25</v>
+      </c>
       <c r="D27" s="4">
         <v>4.8710000000000004</v>
       </c>
@@ -2060,125 +2043,78 @@
         <v>7.5202</v>
       </c>
     </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A28" s="12"/>
       <c r="B28" s="15"/>
+      <c r="C28" s="8" t="s">
+        <v>19</v>
+      </c>
       <c r="D28" s="4">
-        <v>13.14</v>
+        <v>10.692</v>
       </c>
       <c r="E28" s="4">
-        <v>39.933999999999997</v>
+        <v>29.068000000000001</v>
       </c>
       <c r="F28" s="4">
-        <v>2.5283000000000002</v>
+        <v>2.9830999999999999</v>
       </c>
       <c r="G28" s="4">
-        <v>3.4655</v>
+        <v>3.7277999999999998</v>
       </c>
       <c r="H28" s="4">
-        <v>1648.3</v>
-      </c>
-    </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
+        <v>1433.5</v>
+      </c>
+      <c r="I28" s="4">
+        <v>1588.8</v>
+      </c>
+      <c r="J28" s="4">
+        <v>4.5518000000000001</v>
+      </c>
+      <c r="K28" s="3">
+        <v>5.8509000000000002</v>
+      </c>
+    </row>
+    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A29" s="12"/>
       <c r="B29" s="15"/>
-      <c r="D29" s="4">
-        <v>5.1102999999999996</v>
-      </c>
-      <c r="E29" s="4">
-        <v>11.731</v>
-      </c>
-      <c r="F29" s="4">
-        <v>11.74</v>
-      </c>
-      <c r="G29" s="4">
-        <v>4.1925999999999997</v>
-      </c>
-      <c r="H29" s="4">
-        <v>1109.8</v>
-      </c>
-    </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A30" s="12"/>
       <c r="B30" s="15"/>
-      <c r="D30" s="4">
-        <v>7.3842999999999996</v>
-      </c>
-      <c r="E30" s="4">
-        <v>24.515000000000001</v>
-      </c>
-      <c r="F30" s="4">
-        <v>3.0272000000000001</v>
-      </c>
-      <c r="G30" s="4">
-        <v>3.8938999999999999</v>
-      </c>
-      <c r="H30" s="4">
-        <v>1467</v>
-      </c>
-    </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A31" s="12"/>
       <c r="B31" s="15"/>
-      <c r="D31" s="4">
-        <v>2.9946999999999999</v>
-      </c>
-      <c r="E31" s="4">
-        <v>38.689</v>
-      </c>
-      <c r="F31" s="4">
-        <v>2.0182000000000002</v>
-      </c>
-      <c r="G31" s="4">
-        <v>4.8173000000000004</v>
-      </c>
-      <c r="H31" s="4">
-        <v>747.28</v>
-      </c>
-    </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A32" s="12"/>
       <c r="B32" s="15"/>
-      <c r="D32" s="4">
-        <v>3.4691999999999998</v>
-      </c>
-      <c r="E32" s="4">
-        <v>11.414</v>
-      </c>
-      <c r="F32" s="4">
-        <v>8.2040000000000006</v>
-      </c>
-      <c r="G32" s="4">
-        <v>4.3040000000000003</v>
-      </c>
-      <c r="H32" s="4">
-        <v>1127.5</v>
-      </c>
-    </row>
-    <row r="33" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="33" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A33" s="12"/>
       <c r="B33" s="15"/>
     </row>
-    <row r="34" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A34" s="12"/>
       <c r="B34" s="15"/>
     </row>
-    <row r="35" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A35" s="12"/>
       <c r="B35" s="15"/>
     </row>
-    <row r="36" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A36" s="12"/>
       <c r="B36" s="15"/>
     </row>
-    <row r="37" spans="1:19" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:20" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="13"/>
       <c r="B37" s="16"/>
       <c r="C37" s="7"/>
       <c r="K37" s="6"/>
-      <c r="S37" s="6"/>
-    </row>
-    <row r="38" spans="1:19" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L37" s="7"/>
+      <c r="T37" s="6"/>
+    </row>
+    <row r="38" spans="1:20" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="11">
         <v>900</v>
       </c>
@@ -2186,9 +2122,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="39" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A39" s="12"/>
       <c r="B39" s="15"/>
+      <c r="C39" s="8" t="s">
+        <v>19</v>
+      </c>
       <c r="D39" s="4">
         <v>4.8238000000000003</v>
       </c>
@@ -2204,81 +2143,88 @@
       <c r="H39" s="4">
         <v>1006.9</v>
       </c>
-    </row>
-    <row r="40" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="I39" s="4">
+        <v>1762.8</v>
+      </c>
+      <c r="J39" s="4">
+        <v>4.5347</v>
+      </c>
+      <c r="K39" s="3">
+        <v>7.3331</v>
+      </c>
+    </row>
+    <row r="40" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A40" s="12"/>
       <c r="B40" s="15"/>
+      <c r="C40" s="8" t="s">
+        <v>32</v>
+      </c>
       <c r="D40" s="4">
-        <v>12.256</v>
+        <v>7.1036999999999999</v>
       </c>
       <c r="E40" s="4">
-        <v>273.68</v>
+        <v>48.234999999999999</v>
       </c>
       <c r="F40" s="4">
-        <v>0.20866000000000001</v>
+        <v>4.2972000000000001</v>
       </c>
       <c r="G40" s="4">
-        <v>3.8422000000000001</v>
+        <v>3.4083999999999999</v>
       </c>
       <c r="H40" s="4">
-        <v>1242.3</v>
-      </c>
-    </row>
-    <row r="41" spans="1:19" x14ac:dyDescent="0.25">
+        <v>1829.9</v>
+      </c>
+      <c r="I40" s="4">
+        <v>1702.3</v>
+      </c>
+      <c r="J40" s="4">
+        <v>4.4939999999999998</v>
+      </c>
+      <c r="K40" s="3">
+        <v>5.4440999999999997</v>
+      </c>
+    </row>
+    <row r="41" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A41" s="12"/>
       <c r="B41" s="15"/>
-      <c r="D41" s="4">
-        <v>11.208</v>
-      </c>
-      <c r="E41" s="4">
-        <v>16.738</v>
-      </c>
-      <c r="F41" s="4">
-        <v>5.9587000000000003</v>
-      </c>
-      <c r="G41" s="4">
-        <v>3.6377000000000002</v>
-      </c>
-      <c r="H41" s="4">
-        <v>1530.1</v>
-      </c>
-    </row>
-    <row r="42" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="42" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A42" s="12"/>
       <c r="B42" s="15"/>
     </row>
-    <row r="43" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A43" s="12"/>
       <c r="B43" s="15"/>
     </row>
-    <row r="44" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A44" s="12"/>
       <c r="B44" s="15"/>
     </row>
-    <row r="45" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A45" s="12"/>
       <c r="B45" s="15"/>
     </row>
-    <row r="46" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A46" s="12"/>
       <c r="B46" s="15"/>
     </row>
-    <row r="47" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A47" s="12"/>
       <c r="B47" s="15"/>
     </row>
-    <row r="48" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A48" s="12"/>
       <c r="B48" s="15"/>
     </row>
-    <row r="49" spans="1:19" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:20" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="13"/>
       <c r="B49" s="16"/>
       <c r="C49" s="7"/>
       <c r="K49" s="6"/>
-      <c r="S49" s="6"/>
-    </row>
-    <row r="50" spans="1:19" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L49" s="7"/>
+      <c r="T49" s="6"/>
+    </row>
+    <row r="50" spans="1:20" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="11">
         <v>1000</v>
       </c>
@@ -2286,54 +2232,55 @@
         <v>6</v>
       </c>
     </row>
-    <row r="51" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A51" s="12"/>
       <c r="B51" s="15"/>
     </row>
-    <row r="52" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A52" s="12"/>
       <c r="B52" s="15"/>
     </row>
-    <row r="53" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A53" s="12"/>
       <c r="B53" s="15"/>
     </row>
-    <row r="54" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A54" s="12"/>
       <c r="B54" s="15"/>
     </row>
-    <row r="55" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A55" s="12"/>
       <c r="B55" s="15"/>
     </row>
-    <row r="56" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A56" s="12"/>
       <c r="B56" s="15"/>
     </row>
-    <row r="57" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A57" s="12"/>
       <c r="B57" s="15"/>
     </row>
-    <row r="58" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A58" s="12"/>
       <c r="B58" s="15"/>
     </row>
-    <row r="59" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A59" s="12"/>
       <c r="B59" s="15"/>
     </row>
-    <row r="60" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A60" s="12"/>
       <c r="B60" s="15"/>
     </row>
-    <row r="61" spans="1:19" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:20" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="13"/>
       <c r="B61" s="16"/>
       <c r="C61" s="7"/>
       <c r="K61" s="6"/>
-      <c r="S61" s="6"/>
-    </row>
-    <row r="62" spans="1:19" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L61" s="7"/>
+      <c r="T61" s="6"/>
+    </row>
+    <row r="62" spans="1:20" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="11">
         <v>1000</v>
       </c>
@@ -2341,67 +2288,68 @@
         <v>7</v>
       </c>
     </row>
-    <row r="63" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A63" s="12"/>
       <c r="B63" s="15"/>
     </row>
-    <row r="64" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A64" s="12"/>
       <c r="B64" s="15"/>
     </row>
-    <row r="65" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A65" s="12"/>
       <c r="B65" s="15"/>
     </row>
-    <row r="66" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A66" s="12"/>
       <c r="B66" s="15"/>
     </row>
-    <row r="67" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A67" s="12"/>
       <c r="B67" s="15"/>
     </row>
-    <row r="68" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A68" s="12"/>
       <c r="B68" s="15"/>
     </row>
-    <row r="69" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A69" s="12"/>
       <c r="B69" s="15"/>
     </row>
-    <row r="70" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A70" s="12"/>
       <c r="B70" s="15"/>
     </row>
-    <row r="71" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A71" s="12"/>
       <c r="B71" s="15"/>
     </row>
-    <row r="72" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A72" s="12"/>
       <c r="B72" s="15"/>
     </row>
-    <row r="73" spans="1:19" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:20" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="13"/>
       <c r="B73" s="16"/>
       <c r="C73" s="7"/>
       <c r="K73" s="6"/>
-      <c r="S73" s="6"/>
+      <c r="L73" s="7"/>
+      <c r="T73" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A38:A49"/>
+    <mergeCell ref="B38:B49"/>
+    <mergeCell ref="A50:A61"/>
+    <mergeCell ref="B50:B61"/>
+    <mergeCell ref="A62:A73"/>
+    <mergeCell ref="B62:B73"/>
     <mergeCell ref="A2:A13"/>
     <mergeCell ref="B2:B13"/>
     <mergeCell ref="A14:A25"/>
     <mergeCell ref="B14:B25"/>
     <mergeCell ref="A26:A37"/>
     <mergeCell ref="B26:B37"/>
-    <mergeCell ref="A38:A49"/>
-    <mergeCell ref="B38:B49"/>
-    <mergeCell ref="A50:A61"/>
-    <mergeCell ref="B50:B61"/>
-    <mergeCell ref="A62:A73"/>
-    <mergeCell ref="B62:B73"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -2410,11 +2358,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C18A26E-30CA-4E63-A18A-C9C101DAF33C}">
-  <dimension ref="A1:Y73"/>
+  <dimension ref="A1:Z73"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B14" sqref="B14:B25"/>
+      <selection pane="bottomLeft" activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2424,12 +2372,13 @@
     <col min="3" max="3" width="15.7109375" style="8" customWidth="1"/>
     <col min="4" max="13" width="9.140625" style="4"/>
     <col min="14" max="14" width="9.140625" style="3"/>
-    <col min="15" max="24" width="9.140625" style="4"/>
-    <col min="25" max="25" width="9.140625" style="3"/>
-    <col min="26" max="16384" width="9.140625" style="4"/>
+    <col min="15" max="15" width="15.7109375" style="8" customWidth="1"/>
+    <col min="16" max="25" width="9.140625" style="4"/>
+    <col min="26" max="26" width="9.140625" style="3"/>
+    <col min="27" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -2472,41 +2421,44 @@
       <c r="N1" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="O1" s="5" t="s">
+      <c r="O1" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="P1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="P1" s="5" t="s">
+      <c r="Q1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="Q1" s="5" t="s">
+      <c r="R1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="R1" s="5" t="s">
+      <c r="S1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="S1" s="5" t="s">
+      <c r="T1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="T1" s="5" t="s">
+      <c r="U1" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="U1" s="5" t="s">
+      <c r="V1" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="V1" s="5" t="s">
+      <c r="W1" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="W1" s="5" t="s">
+      <c r="X1" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="X1" s="5" t="s">
+      <c r="Y1" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="Y1" s="6" t="s">
+      <c r="Z1" s="6" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:25" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:26" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="11">
         <v>800</v>
       </c>
@@ -2514,129 +2466,91 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A3" s="12"/>
       <c r="B3" s="15"/>
+      <c r="C3" s="8" t="s">
+        <v>30</v>
+      </c>
       <c r="D3" s="4">
-        <v>10.077</v>
+        <v>17.216999999999999</v>
       </c>
       <c r="E3" s="4">
-        <v>32.911000000000001</v>
+        <v>179.74</v>
       </c>
       <c r="F3" s="4">
-        <v>21.905999999999999</v>
+        <v>0.61753999999999998</v>
       </c>
       <c r="G3" s="4">
-        <v>3.5992000000000002</v>
+        <v>4.4165999999999999</v>
       </c>
       <c r="H3" s="4">
-        <v>3063</v>
-      </c>
-    </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
+        <v>1783.5</v>
+      </c>
+      <c r="I3" s="4">
+        <v>1.3053999999999999</v>
+      </c>
+      <c r="J3" s="4">
+        <v>0.57770999999999995</v>
+      </c>
+      <c r="K3" s="4">
+        <v>4.8882000000000003</v>
+      </c>
+      <c r="L3" s="4">
+        <v>4.7967000000000004</v>
+      </c>
+      <c r="M3" s="4">
+        <v>7.5513999999999998E-2</v>
+      </c>
+      <c r="N3" s="3">
+        <v>2.4582999999999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A4" s="12"/>
       <c r="B4" s="15"/>
-      <c r="D4" s="4">
-        <v>11.695</v>
-      </c>
-      <c r="E4" s="4">
-        <v>101.28</v>
-      </c>
-      <c r="F4" s="4">
-        <v>1.1411</v>
-      </c>
-      <c r="G4" s="4">
-        <v>4.6826999999999996</v>
-      </c>
-      <c r="H4" s="4">
-        <v>1595.5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A5" s="12"/>
       <c r="B5" s="15"/>
-      <c r="D5" s="4">
-        <v>9.8171999999999997</v>
-      </c>
-      <c r="E5" s="4">
-        <v>101.47</v>
-      </c>
-      <c r="F5" s="4">
-        <v>1.4056999999999999</v>
-      </c>
-      <c r="G5" s="4">
-        <v>4.6856999999999998</v>
-      </c>
-      <c r="H5" s="4">
-        <v>1595.7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A6" s="12"/>
       <c r="B6" s="15"/>
-      <c r="D6" s="4">
-        <v>31.815999999999999</v>
-      </c>
-      <c r="E6" s="4">
-        <v>59.655000000000001</v>
-      </c>
-      <c r="F6" s="4">
-        <v>1.0424</v>
-      </c>
-      <c r="G6" s="4">
-        <v>3.6473</v>
-      </c>
-      <c r="H6" s="4">
-        <v>2944</v>
-      </c>
-    </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A7" s="12"/>
       <c r="B7" s="15"/>
-      <c r="D7" s="4">
-        <v>20.015999999999998</v>
-      </c>
-      <c r="E7" s="4">
-        <v>69.863</v>
-      </c>
-      <c r="F7" s="4">
-        <v>1.1780999999999999</v>
-      </c>
-      <c r="G7" s="4">
-        <v>4.3254999999999999</v>
-      </c>
-      <c r="H7" s="4">
-        <v>1881.4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A8" s="12"/>
       <c r="B8" s="15"/>
     </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A9" s="12"/>
       <c r="B9" s="15"/>
     </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A10" s="12"/>
       <c r="B10" s="15"/>
     </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A11" s="12"/>
       <c r="B11" s="15"/>
     </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A12" s="12"/>
       <c r="B12" s="15"/>
     </row>
-    <row r="13" spans="1:25" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:26" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="13"/>
       <c r="B13" s="16"/>
       <c r="C13" s="7"/>
       <c r="N13" s="6"/>
-      <c r="Y13" s="6"/>
-    </row>
-    <row r="14" spans="1:25" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O13" s="7"/>
+      <c r="Z13" s="6"/>
+    </row>
+    <row r="14" spans="1:26" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="11">
         <v>800</v>
       </c>
@@ -2644,129 +2558,55 @@
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A15" s="12"/>
       <c r="B15" s="15"/>
-      <c r="D15" s="4">
-        <v>19.913</v>
-      </c>
-      <c r="E15" s="4">
-        <v>52.043999999999997</v>
-      </c>
-      <c r="F15" s="4">
-        <v>2.2252000000000001</v>
-      </c>
-      <c r="G15" s="4">
-        <v>4.3255999999999997</v>
-      </c>
-      <c r="H15" s="4">
-        <v>1847.9</v>
-      </c>
-    </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A16" s="12"/>
       <c r="B16" s="15"/>
-      <c r="D16" s="4">
-        <v>31.327000000000002</v>
-      </c>
-      <c r="E16" s="4">
-        <v>104.92</v>
-      </c>
-      <c r="F16" s="4">
-        <v>0.8548</v>
-      </c>
-      <c r="G16" s="4">
-        <v>3.7507999999999999</v>
-      </c>
-      <c r="H16" s="4">
-        <v>2575.8000000000002</v>
-      </c>
-    </row>
-    <row r="17" spans="1:25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A17" s="12"/>
       <c r="B17" s="15"/>
-      <c r="D17" s="4">
-        <v>0.85682000000000003</v>
-      </c>
-      <c r="E17" s="4">
-        <v>42.524000000000001</v>
-      </c>
-      <c r="F17" s="4">
-        <v>9.6282999999999994</v>
-      </c>
-      <c r="G17" s="4">
-        <v>4.5033000000000003</v>
-      </c>
-      <c r="H17" s="4">
-        <v>1707</v>
-      </c>
-    </row>
-    <row r="18" spans="1:25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A18" s="12"/>
       <c r="B18" s="15"/>
-      <c r="D18" s="4">
-        <v>1.2122000000000001E-2</v>
-      </c>
-      <c r="E18" s="4">
-        <v>52.49</v>
-      </c>
-      <c r="F18" s="4">
-        <v>21.795999999999999</v>
-      </c>
-      <c r="G18" s="4">
-        <v>3.2532999999999999</v>
-      </c>
-      <c r="H18" s="4">
-        <v>3778</v>
-      </c>
-    </row>
-    <row r="19" spans="1:25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A19" s="12"/>
       <c r="B19" s="15"/>
-      <c r="D19" s="4">
-        <v>17.216999999999999</v>
-      </c>
-      <c r="E19" s="4">
-        <v>179.74</v>
-      </c>
-      <c r="F19" s="4">
-        <v>0.61753999999999998</v>
-      </c>
-      <c r="G19" s="4">
-        <v>4.4165999999999999</v>
-      </c>
-      <c r="H19" s="4">
-        <v>1783.5</v>
-      </c>
-    </row>
-    <row r="20" spans="1:25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A20" s="12"/>
       <c r="B20" s="15"/>
     </row>
-    <row r="21" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A21" s="12"/>
       <c r="B21" s="15"/>
     </row>
-    <row r="22" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A22" s="12"/>
       <c r="B22" s="15"/>
     </row>
-    <row r="23" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A23" s="12"/>
       <c r="B23" s="15"/>
     </row>
-    <row r="24" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A24" s="12"/>
       <c r="B24" s="15"/>
     </row>
-    <row r="25" spans="1:25" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:26" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="13"/>
       <c r="B25" s="16"/>
       <c r="C25" s="7"/>
       <c r="N25" s="6"/>
-      <c r="Y25" s="6"/>
-    </row>
-    <row r="26" spans="1:25" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O25" s="7"/>
+      <c r="Z25" s="6"/>
+    </row>
+    <row r="26" spans="1:26" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="11">
         <v>900</v>
       </c>
@@ -2774,9 +2614,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="27" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A27" s="12"/>
       <c r="B27" s="15"/>
+      <c r="C27" s="8" t="s">
+        <v>19</v>
+      </c>
       <c r="D27" s="4">
         <v>4.8710000000000004</v>
       </c>
@@ -2811,125 +2654,87 @@
         <v>2.5308000000000002</v>
       </c>
     </row>
-    <row r="28" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A28" s="12"/>
       <c r="B28" s="15"/>
+      <c r="C28" s="8" t="s">
+        <v>27</v>
+      </c>
       <c r="D28" s="4">
-        <v>13.14</v>
+        <v>10.692</v>
       </c>
       <c r="E28" s="4">
-        <v>39.933999999999997</v>
+        <v>29.068000000000001</v>
       </c>
       <c r="F28" s="4">
-        <v>2.5283000000000002</v>
+        <v>2.9830999999999999</v>
       </c>
       <c r="G28" s="4">
-        <v>3.4655</v>
+        <v>3.7277999999999998</v>
       </c>
       <c r="H28" s="4">
-        <v>1648.3</v>
-      </c>
-    </row>
-    <row r="29" spans="1:25" x14ac:dyDescent="0.25">
+        <v>1433.5</v>
+      </c>
+      <c r="I28" s="4">
+        <v>2.7648999999999999</v>
+      </c>
+      <c r="J28" s="4">
+        <v>0.68981999999999999</v>
+      </c>
+      <c r="K28" s="4">
+        <v>5.0537999999999998</v>
+      </c>
+      <c r="L28" s="4">
+        <v>6.1146000000000003</v>
+      </c>
+      <c r="M28" s="4">
+        <v>0.19602</v>
+      </c>
+      <c r="N28" s="3">
+        <v>2.4864000000000002</v>
+      </c>
+    </row>
+    <row r="29" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A29" s="12"/>
       <c r="B29" s="15"/>
-      <c r="D29" s="4">
-        <v>5.1102999999999996</v>
-      </c>
-      <c r="E29" s="4">
-        <v>11.731</v>
-      </c>
-      <c r="F29" s="4">
-        <v>11.74</v>
-      </c>
-      <c r="G29" s="4">
-        <v>4.1925999999999997</v>
-      </c>
-      <c r="H29" s="4">
-        <v>1109.8</v>
-      </c>
-    </row>
-    <row r="30" spans="1:25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="30" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A30" s="12"/>
       <c r="B30" s="15"/>
-      <c r="D30" s="4">
-        <v>7.3842999999999996</v>
-      </c>
-      <c r="E30" s="4">
-        <v>24.515000000000001</v>
-      </c>
-      <c r="F30" s="4">
-        <v>3.0272000000000001</v>
-      </c>
-      <c r="G30" s="4">
-        <v>3.8938999999999999</v>
-      </c>
-      <c r="H30" s="4">
-        <v>1467</v>
-      </c>
-    </row>
-    <row r="31" spans="1:25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="31" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A31" s="12"/>
       <c r="B31" s="15"/>
-      <c r="D31" s="4">
-        <v>2.9946999999999999</v>
-      </c>
-      <c r="E31" s="4">
-        <v>38.689</v>
-      </c>
-      <c r="F31" s="4">
-        <v>2.0182000000000002</v>
-      </c>
-      <c r="G31" s="4">
-        <v>4.8173000000000004</v>
-      </c>
-      <c r="H31" s="4">
-        <v>747.28</v>
-      </c>
-    </row>
-    <row r="32" spans="1:25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="32" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A32" s="12"/>
       <c r="B32" s="15"/>
-      <c r="D32" s="4">
-        <v>3.4691999999999998</v>
-      </c>
-      <c r="E32" s="4">
-        <v>11.414</v>
-      </c>
-      <c r="F32" s="4">
-        <v>8.2040000000000006</v>
-      </c>
-      <c r="G32" s="4">
-        <v>4.3040000000000003</v>
-      </c>
-      <c r="H32" s="4">
-        <v>1127.5</v>
-      </c>
-    </row>
-    <row r="33" spans="1:25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="33" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A33" s="12"/>
       <c r="B33" s="15"/>
     </row>
-    <row r="34" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A34" s="12"/>
       <c r="B34" s="15"/>
     </row>
-    <row r="35" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A35" s="12"/>
       <c r="B35" s="15"/>
     </row>
-    <row r="36" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A36" s="12"/>
       <c r="B36" s="15"/>
     </row>
-    <row r="37" spans="1:25" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:26" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="13"/>
       <c r="B37" s="16"/>
       <c r="C37" s="7"/>
       <c r="N37" s="6"/>
-      <c r="Y37" s="6"/>
-    </row>
-    <row r="38" spans="1:25" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O37" s="7"/>
+      <c r="Z37" s="6"/>
+    </row>
+    <row r="38" spans="1:26" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="11">
         <v>900</v>
       </c>
@@ -2937,9 +2742,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="39" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A39" s="12"/>
       <c r="B39" s="15"/>
+      <c r="C39" s="8" t="s">
+        <v>22</v>
+      </c>
       <c r="D39" s="4">
         <v>4.8238000000000003</v>
       </c>
@@ -2974,80 +2782,87 @@
         <v>2.5291999999999999</v>
       </c>
     </row>
-    <row r="40" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A40" s="12"/>
       <c r="B40" s="15"/>
+      <c r="C40" s="8" t="s">
+        <v>26</v>
+      </c>
       <c r="D40" s="4">
-        <v>12.256</v>
+        <v>7.1036999999999999</v>
       </c>
       <c r="E40" s="4">
-        <v>273.68</v>
+        <v>48.234999999999999</v>
       </c>
       <c r="F40" s="4">
-        <v>0.20866000000000001</v>
+        <v>4.2972000000000001</v>
       </c>
       <c r="G40" s="4">
-        <v>3.8422000000000001</v>
+        <v>3.4083999999999999</v>
       </c>
       <c r="H40" s="4">
-        <v>1242.3</v>
-      </c>
-    </row>
-    <row r="41" spans="1:25" x14ac:dyDescent="0.25">
+        <v>1829.9</v>
+      </c>
+      <c r="I40" s="4">
+        <v>1.4641</v>
+      </c>
+      <c r="J40" s="4">
+        <v>0.47352</v>
+      </c>
+      <c r="K40" s="4">
+        <v>3.8866999999999998</v>
+      </c>
+      <c r="L40" s="4">
+        <v>7.1471</v>
+      </c>
+      <c r="M40" s="4">
+        <v>5.6285000000000002E-2</v>
+      </c>
+      <c r="N40" s="3">
+        <v>2.2601</v>
+      </c>
+    </row>
+    <row r="41" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A41" s="12"/>
       <c r="B41" s="15"/>
-      <c r="D41" s="4">
-        <v>11.208</v>
-      </c>
-      <c r="E41" s="4">
-        <v>16.738</v>
-      </c>
-      <c r="F41" s="4">
-        <v>5.9587000000000003</v>
-      </c>
-      <c r="G41" s="4">
-        <v>3.6377000000000002</v>
-      </c>
-      <c r="H41" s="4">
-        <v>1530.1</v>
-      </c>
-    </row>
-    <row r="42" spans="1:25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="42" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A42" s="12"/>
       <c r="B42" s="15"/>
     </row>
-    <row r="43" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A43" s="12"/>
       <c r="B43" s="15"/>
     </row>
-    <row r="44" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A44" s="12"/>
       <c r="B44" s="15"/>
     </row>
-    <row r="45" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A45" s="12"/>
       <c r="B45" s="15"/>
     </row>
-    <row r="46" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A46" s="12"/>
       <c r="B46" s="15"/>
     </row>
-    <row r="47" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A47" s="12"/>
       <c r="B47" s="15"/>
     </row>
-    <row r="48" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A48" s="12"/>
       <c r="B48" s="15"/>
     </row>
-    <row r="49" spans="1:25" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:26" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="13"/>
       <c r="B49" s="16"/>
       <c r="C49" s="7"/>
       <c r="N49" s="6"/>
-      <c r="Y49" s="6"/>
-    </row>
-    <row r="50" spans="1:25" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O49" s="7"/>
+      <c r="Z49" s="6"/>
+    </row>
+    <row r="50" spans="1:26" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="11">
         <v>1000</v>
       </c>
@@ -3055,54 +2870,55 @@
         <v>6</v>
       </c>
     </row>
-    <row r="51" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A51" s="12"/>
       <c r="B51" s="15"/>
     </row>
-    <row r="52" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A52" s="12"/>
       <c r="B52" s="15"/>
     </row>
-    <row r="53" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A53" s="12"/>
       <c r="B53" s="15"/>
     </row>
-    <row r="54" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A54" s="12"/>
       <c r="B54" s="15"/>
     </row>
-    <row r="55" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A55" s="12"/>
       <c r="B55" s="15"/>
     </row>
-    <row r="56" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A56" s="12"/>
       <c r="B56" s="15"/>
     </row>
-    <row r="57" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A57" s="12"/>
       <c r="B57" s="15"/>
     </row>
-    <row r="58" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A58" s="12"/>
       <c r="B58" s="15"/>
     </row>
-    <row r="59" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A59" s="12"/>
       <c r="B59" s="15"/>
     </row>
-    <row r="60" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A60" s="12"/>
       <c r="B60" s="15"/>
     </row>
-    <row r="61" spans="1:25" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:26" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="13"/>
       <c r="B61" s="16"/>
       <c r="C61" s="7"/>
       <c r="N61" s="6"/>
-      <c r="Y61" s="6"/>
-    </row>
-    <row r="62" spans="1:25" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O61" s="7"/>
+      <c r="Z61" s="6"/>
+    </row>
+    <row r="62" spans="1:26" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="11">
         <v>1000</v>
       </c>
@@ -3110,67 +2926,68 @@
         <v>7</v>
       </c>
     </row>
-    <row r="63" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A63" s="12"/>
       <c r="B63" s="15"/>
     </row>
-    <row r="64" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A64" s="12"/>
       <c r="B64" s="15"/>
     </row>
-    <row r="65" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A65" s="12"/>
       <c r="B65" s="15"/>
     </row>
-    <row r="66" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A66" s="12"/>
       <c r="B66" s="15"/>
     </row>
-    <row r="67" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A67" s="12"/>
       <c r="B67" s="15"/>
     </row>
-    <row r="68" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A68" s="12"/>
       <c r="B68" s="15"/>
     </row>
-    <row r="69" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A69" s="12"/>
       <c r="B69" s="15"/>
     </row>
-    <row r="70" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A70" s="12"/>
       <c r="B70" s="15"/>
     </row>
-    <row r="71" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A71" s="12"/>
       <c r="B71" s="15"/>
     </row>
-    <row r="72" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A72" s="12"/>
       <c r="B72" s="15"/>
     </row>
-    <row r="73" spans="1:25" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:26" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="13"/>
       <c r="B73" s="16"/>
       <c r="C73" s="7"/>
       <c r="N73" s="6"/>
-      <c r="Y73" s="6"/>
+      <c r="O73" s="7"/>
+      <c r="Z73" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A38:A49"/>
+    <mergeCell ref="B38:B49"/>
+    <mergeCell ref="A50:A61"/>
+    <mergeCell ref="B50:B61"/>
+    <mergeCell ref="A62:A73"/>
+    <mergeCell ref="B62:B73"/>
     <mergeCell ref="A2:A13"/>
     <mergeCell ref="B2:B13"/>
     <mergeCell ref="A14:A25"/>
     <mergeCell ref="B14:B25"/>
     <mergeCell ref="A26:A37"/>
     <mergeCell ref="B26:B37"/>
-    <mergeCell ref="A38:A49"/>
-    <mergeCell ref="B38:B49"/>
-    <mergeCell ref="A50:A61"/>
-    <mergeCell ref="B50:B61"/>
-    <mergeCell ref="A62:A73"/>
-    <mergeCell ref="B62:B73"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
added loss history writer
</commit_message>
<xml_diff>
--- a/scripts/__other__/__sem__.xlsx
+++ b/scripts/__other__/__sem__.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Janzen\Desktop\code\moga_neml\scripts\__other__\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{507D1849-8B6A-45A6-92CB-0CE144A12CFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B161D93-0884-4157-9E15-738927958F1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="34">
   <si>
     <t>temp</t>
   </si>
@@ -137,6 +137,9 @@
   </si>
   <si>
     <t>cr und</t>
+  </si>
+  <si>
+    <t>bad</t>
   </si>
 </sst>
 </file>
@@ -254,7 +257,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -303,12 +306,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -593,8 +590,8 @@
   <dimension ref="A1:O73"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L30" sqref="L30"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M16" sqref="M16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -920,6 +917,9 @@
       <c r="I15" s="8" t="s">
         <v>24</v>
       </c>
+      <c r="J15" s="8" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="12"/>
@@ -1481,6 +1481,12 @@
       </c>
       <c r="H41" s="3">
         <v>2022.3</v>
+      </c>
+      <c r="I41" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="J41" s="8" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="42" spans="1:15" x14ac:dyDescent="0.25">
@@ -1783,7 +1789,7 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C3" sqref="C3"/>
+      <selection pane="bottomLeft" activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1887,10 +1893,10 @@
       <c r="G3" s="4">
         <v>4.4165999999999999</v>
       </c>
-      <c r="H3" s="17">
+      <c r="H3" s="4">
         <v>1783.5</v>
       </c>
-      <c r="I3" s="18">
+      <c r="I3" s="2">
         <v>1761.4</v>
       </c>
       <c r="J3" s="2">
@@ -1903,14 +1909,10 @@
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" s="12"/>
       <c r="B4" s="15"/>
-      <c r="H4" s="17"/>
-      <c r="I4" s="17"/>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" s="12"/>
       <c r="B5" s="15"/>
-      <c r="H5" s="17"/>
-      <c r="I5" s="17"/>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" s="12"/>
@@ -1959,6 +1961,33 @@
     <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15" s="12"/>
       <c r="B15" s="15"/>
+      <c r="C15" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="D15" s="4">
+        <v>31.327000000000002</v>
+      </c>
+      <c r="E15" s="4">
+        <v>104.92</v>
+      </c>
+      <c r="F15" s="4">
+        <v>0.8548</v>
+      </c>
+      <c r="G15" s="4">
+        <v>3.7507999999999999</v>
+      </c>
+      <c r="H15" s="4">
+        <v>2575.8000000000002</v>
+      </c>
+      <c r="I15" s="4">
+        <v>1200.7</v>
+      </c>
+      <c r="J15" s="4">
+        <v>6.6093999999999999</v>
+      </c>
+      <c r="K15" s="3">
+        <v>7.3170000000000002</v>
+      </c>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16" s="12"/>

</xml_diff>

<commit_message>
removed stress obj function
</commit_message>
<xml_diff>
--- a/scripts/__other__/__sem__.xlsx
+++ b/scripts/__other__/__sem__.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Janzen\Desktop\code\moga_neml\scripts\__other__\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B161D93-0884-4157-9E15-738927958F1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D9F2FBA-ABCA-429A-935C-C3CCA8748A58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="33">
   <si>
     <t>temp</t>
   </si>
@@ -137,9 +137,6 @@
   </si>
   <si>
     <t>cr und</t>
-  </si>
-  <si>
-    <t>bad</t>
   </si>
 </sst>
 </file>
@@ -591,7 +588,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M16" sqref="M16"/>
+      <selection pane="bottomLeft" activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -915,7 +912,7 @@
         <v>2575.8000000000002</v>
       </c>
       <c r="I15" s="8" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="J15" s="8" t="s">
         <v>24</v>
@@ -1765,18 +1762,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A2:A13"/>
+    <mergeCell ref="B2:B13"/>
+    <mergeCell ref="A14:A25"/>
+    <mergeCell ref="B14:B25"/>
+    <mergeCell ref="A26:A37"/>
+    <mergeCell ref="B26:B37"/>
     <mergeCell ref="A38:A49"/>
     <mergeCell ref="B38:B49"/>
     <mergeCell ref="A50:A61"/>
     <mergeCell ref="B50:B61"/>
     <mergeCell ref="A62:A73"/>
     <mergeCell ref="B62:B73"/>
-    <mergeCell ref="A2:A13"/>
-    <mergeCell ref="B2:B13"/>
-    <mergeCell ref="A14:A25"/>
-    <mergeCell ref="B14:B25"/>
-    <mergeCell ref="A26:A37"/>
-    <mergeCell ref="B26:B37"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -1789,7 +1786,7 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J20" sqref="J20"/>
+      <selection pane="bottomLeft" activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1962,7 +1959,7 @@
       <c r="A15" s="12"/>
       <c r="B15" s="15"/>
       <c r="C15" s="8" t="s">
-        <v>33</v>
+        <v>19</v>
       </c>
       <c r="D15" s="4">
         <v>31.327000000000002</v>
@@ -1980,13 +1977,13 @@
         <v>2575.8000000000002</v>
       </c>
       <c r="I15" s="4">
-        <v>1200.7</v>
+        <v>1787.7</v>
       </c>
       <c r="J15" s="4">
-        <v>6.6093999999999999</v>
+        <v>5.6729000000000003</v>
       </c>
       <c r="K15" s="3">
-        <v>7.3170000000000002</v>
+        <v>6.7279</v>
       </c>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.25">
@@ -2367,18 +2364,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A2:A13"/>
+    <mergeCell ref="B2:B13"/>
+    <mergeCell ref="A14:A25"/>
+    <mergeCell ref="B14:B25"/>
+    <mergeCell ref="A26:A37"/>
+    <mergeCell ref="B26:B37"/>
     <mergeCell ref="A38:A49"/>
     <mergeCell ref="B38:B49"/>
     <mergeCell ref="A50:A61"/>
     <mergeCell ref="B50:B61"/>
     <mergeCell ref="A62:A73"/>
     <mergeCell ref="B62:B73"/>
-    <mergeCell ref="A2:A13"/>
-    <mergeCell ref="B2:B13"/>
-    <mergeCell ref="A14:A25"/>
-    <mergeCell ref="B14:B25"/>
-    <mergeCell ref="A26:A37"/>
-    <mergeCell ref="B26:B37"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -3005,18 +3002,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A2:A13"/>
+    <mergeCell ref="B2:B13"/>
+    <mergeCell ref="A14:A25"/>
+    <mergeCell ref="B14:B25"/>
+    <mergeCell ref="A26:A37"/>
+    <mergeCell ref="B26:B37"/>
     <mergeCell ref="A38:A49"/>
     <mergeCell ref="B38:B49"/>
     <mergeCell ref="A50:A61"/>
     <mergeCell ref="B50:B61"/>
     <mergeCell ref="A62:A73"/>
     <mergeCell ref="B62:B73"/>
-    <mergeCell ref="A2:A13"/>
-    <mergeCell ref="B2:B13"/>
-    <mergeCell ref="A14:A25"/>
-    <mergeCell ref="B14:B25"/>
-    <mergeCell ref="A26:A37"/>
-    <mergeCell ref="B26:B37"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
added strain obj for evpcd
</commit_message>
<xml_diff>
--- a/scripts/__other__/__sem__.xlsx
+++ b/scripts/__other__/__sem__.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Janzen\Desktop\code\moga_neml\scripts\__other__\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D9F2FBA-ABCA-429A-935C-C3CCA8748A58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F4D5F26-B5FE-4678-8F96-615F646F9507}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15600" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="evp" sheetId="13" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="32">
   <si>
     <t>temp</t>
   </si>
@@ -130,13 +130,10 @@
     <t>evpwd</t>
   </si>
   <si>
-    <t>cr early</t>
-  </si>
-  <si>
-    <t>cr und; ts und</t>
-  </si>
-  <si>
     <t>cr und</t>
+  </si>
+  <si>
+    <t>cr early; bad</t>
   </si>
 </sst>
 </file>
@@ -586,9 +583,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4D7A15E-4182-42F6-82DA-99E9B04906BA}">
   <dimension ref="A1:O73"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView topLeftCell="D1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I15" sqref="I15"/>
+      <selection pane="bottomLeft" activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -664,10 +661,10 @@
         <v>1783.5</v>
       </c>
       <c r="I3" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="J3" s="8" t="s">
         <v>31</v>
-      </c>
-      <c r="J3" s="8" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -1447,7 +1444,7 @@
         <v>1829.9</v>
       </c>
       <c r="I40" s="8" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="J40" s="8" t="s">
         <v>26</v>
@@ -1762,18 +1759,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A38:A49"/>
+    <mergeCell ref="B38:B49"/>
+    <mergeCell ref="A50:A61"/>
+    <mergeCell ref="B50:B61"/>
+    <mergeCell ref="A62:A73"/>
+    <mergeCell ref="B62:B73"/>
     <mergeCell ref="A2:A13"/>
     <mergeCell ref="B2:B13"/>
     <mergeCell ref="A14:A25"/>
     <mergeCell ref="B14:B25"/>
     <mergeCell ref="A26:A37"/>
     <mergeCell ref="B26:B37"/>
-    <mergeCell ref="A38:A49"/>
-    <mergeCell ref="B38:B49"/>
-    <mergeCell ref="A50:A61"/>
-    <mergeCell ref="B50:B61"/>
-    <mergeCell ref="A62:A73"/>
-    <mergeCell ref="B62:B73"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -1786,7 +1783,7 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C15" sqref="C15"/>
+      <selection pane="bottomLeft" activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1876,7 +1873,7 @@
       <c r="A3" s="12"/>
       <c r="B3" s="15"/>
       <c r="C3" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D3" s="4">
         <v>17.216999999999999</v>
@@ -1894,13 +1891,13 @@
         <v>1783.5</v>
       </c>
       <c r="I3" s="2">
-        <v>1761.4</v>
+        <v>1905.8</v>
       </c>
       <c r="J3" s="2">
-        <v>5.6002000000000001</v>
+        <v>5.5621</v>
       </c>
       <c r="K3" s="2">
-        <v>6.5</v>
+        <v>6.6371000000000002</v>
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
@@ -1977,13 +1974,13 @@
         <v>2575.8000000000002</v>
       </c>
       <c r="I15" s="4">
-        <v>1787.7</v>
+        <v>2126.4</v>
       </c>
       <c r="J15" s="4">
-        <v>5.6729000000000003</v>
+        <v>5.3209</v>
       </c>
       <c r="K15" s="3">
-        <v>6.7279</v>
+        <v>6.5503999999999998</v>
       </c>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.25">
@@ -2183,7 +2180,7 @@
       <c r="A40" s="12"/>
       <c r="B40" s="15"/>
       <c r="C40" s="8" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D40" s="4">
         <v>7.1036999999999999</v>
@@ -2364,18 +2361,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A38:A49"/>
+    <mergeCell ref="B38:B49"/>
+    <mergeCell ref="A50:A61"/>
+    <mergeCell ref="B50:B61"/>
+    <mergeCell ref="A62:A73"/>
+    <mergeCell ref="B62:B73"/>
     <mergeCell ref="A2:A13"/>
     <mergeCell ref="B2:B13"/>
     <mergeCell ref="A14:A25"/>
     <mergeCell ref="B14:B25"/>
     <mergeCell ref="A26:A37"/>
     <mergeCell ref="B26:B37"/>
-    <mergeCell ref="A38:A49"/>
-    <mergeCell ref="B38:B49"/>
-    <mergeCell ref="A50:A61"/>
-    <mergeCell ref="B50:B61"/>
-    <mergeCell ref="A62:A73"/>
-    <mergeCell ref="B62:B73"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -2386,9 +2383,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C18A26E-30CA-4E63-A18A-C9C101DAF33C}">
   <dimension ref="A1:Z73"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E29" sqref="E29"/>
+      <selection pane="bottomLeft" activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2496,7 +2493,7 @@
       <c r="A3" s="12"/>
       <c r="B3" s="15"/>
       <c r="C3" s="8" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D3" s="4">
         <v>17.216999999999999</v>
@@ -3002,18 +2999,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A38:A49"/>
+    <mergeCell ref="B38:B49"/>
+    <mergeCell ref="A50:A61"/>
+    <mergeCell ref="B50:B61"/>
+    <mergeCell ref="A62:A73"/>
+    <mergeCell ref="B62:B73"/>
     <mergeCell ref="A2:A13"/>
     <mergeCell ref="B2:B13"/>
     <mergeCell ref="A14:A25"/>
     <mergeCell ref="B14:B25"/>
     <mergeCell ref="A26:A37"/>
     <mergeCell ref="B26:B37"/>
-    <mergeCell ref="A38:A49"/>
-    <mergeCell ref="B38:B49"/>
-    <mergeCell ref="A50:A61"/>
-    <mergeCell ref="B50:B61"/>
-    <mergeCell ref="A62:A73"/>
-    <mergeCell ref="B62:B73"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
Changed results to rating system; param changes to plot function
</commit_message>
<xml_diff>
--- a/scripts/__other__/__sem__.xlsx
+++ b/scripts/__other__/__sem__.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unsw-my.sharepoint.com/personal/z5208868_ad_unsw_edu_au/Documents/Desktop/code/moga_neml/scripts/__other__/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Janzen\Desktop\code\moga_neml\scripts\__other__\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="12" documentId="13_ncr:1_{5F4D5F26-B5FE-4678-8F96-615F646F9507}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B45C60F1-82B8-48FA-8F62-66AD6EFACA73}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70CB2808-E177-4FB6-B5A8-ECB4755D81A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9510" yWindow="0" windowWidth="9780" windowHeight="10170" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="evp" sheetId="13" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="43">
   <si>
     <t>temp</t>
   </si>
@@ -94,46 +94,79 @@
     <t>t_1</t>
   </si>
   <si>
-    <t>notes</t>
-  </si>
-  <si>
-    <t>good</t>
-  </si>
-  <si>
-    <t>ts over</t>
-  </si>
-  <si>
-    <t>ts under</t>
-  </si>
-  <si>
-    <t>LT cr eh</t>
-  </si>
-  <si>
-    <t>LT cr eh; ts over</t>
-  </si>
-  <si>
-    <t>x</t>
-  </si>
-  <si>
-    <t>ST cr eh</t>
-  </si>
-  <si>
-    <t>cr eh; ts over</t>
-  </si>
-  <si>
-    <t>cr eh</t>
-  </si>
-  <si>
-    <t>evpcd</t>
-  </si>
-  <si>
-    <t>evpwd</t>
-  </si>
-  <si>
-    <t>cr und</t>
-  </si>
-  <si>
-    <t>cr eh; ts late</t>
+    <t>10; 10</t>
+  </si>
+  <si>
+    <t>10; 8</t>
+  </si>
+  <si>
+    <t>10; 7</t>
+  </si>
+  <si>
+    <t>rating</t>
+  </si>
+  <si>
+    <t>10; 9</t>
+  </si>
+  <si>
+    <t>8; 9</t>
+  </si>
+  <si>
+    <t>evp-cd rating</t>
+  </si>
+  <si>
+    <t>evp-wd rating</t>
+  </si>
+  <si>
+    <t>8; 10</t>
+  </si>
+  <si>
+    <t>7; 10</t>
+  </si>
+  <si>
+    <t>9; 10</t>
+  </si>
+  <si>
+    <t>10; 6</t>
+  </si>
+  <si>
+    <t>9; 8</t>
+  </si>
+  <si>
+    <t>9; 6</t>
+  </si>
+  <si>
+    <t>10; 5</t>
+  </si>
+  <si>
+    <t>8; 7</t>
+  </si>
+  <si>
+    <t>8; 6</t>
+  </si>
+  <si>
+    <t>6; 7</t>
+  </si>
+  <si>
+    <t>7; 6</t>
+  </si>
+  <si>
+    <t>7; 5</t>
+  </si>
+  <si>
+    <t>7; 9</t>
+  </si>
+  <si>
+    <t>7; 8</t>
+  </si>
+  <si>
+    <t>6; 8</t>
+  </si>
+  <si>
+    <t>5; 10</t>
+  </si>
+  <si>
+    <t>5; 8</t>
   </si>
 </sst>
 </file>
@@ -583,23 +616,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4D7A15E-4182-42F6-82DA-99E9B04906BA}">
   <dimension ref="A1:O73"/>
   <sheetViews>
-    <sheetView zoomScale="78" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F25" sqref="F25"/>
+      <selection pane="bottomLeft" activeCell="M9" sqref="M9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.1796875" style="4"/>
-    <col min="2" max="2" width="9.1796875" style="3"/>
-    <col min="3" max="3" width="15.7265625" style="8" customWidth="1"/>
-    <col min="4" max="7" width="9.1796875" style="4"/>
-    <col min="8" max="8" width="9.1796875" style="3"/>
-    <col min="9" max="10" width="15.7265625" style="8" customWidth="1"/>
-    <col min="11" max="16384" width="9.1796875" style="4"/>
+    <col min="1" max="1" width="9.140625" style="4"/>
+    <col min="2" max="2" width="9.140625" style="3"/>
+    <col min="3" max="3" width="15.7109375" style="8" customWidth="1"/>
+    <col min="4" max="7" width="9.140625" style="4"/>
+    <col min="8" max="8" width="9.140625" style="3"/>
+    <col min="9" max="10" width="15.7109375" style="8" customWidth="1"/>
+    <col min="11" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -607,7 +640,7 @@
         <v>11</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="D1" s="5" t="s">
         <v>1</v>
@@ -625,13 +658,13 @@
         <v>5</v>
       </c>
       <c r="I1" s="7" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="J1" s="7" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" ht="5.15" customHeight="1" x14ac:dyDescent="0.35">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="11">
         <v>800</v>
       </c>
@@ -639,11 +672,11 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="12"/>
       <c r="B3" s="15"/>
       <c r="C3" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D3" s="4">
         <v>17.216999999999999</v>
@@ -661,17 +694,17 @@
         <v>1783.5</v>
       </c>
       <c r="I3" s="8" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="J3" s="8" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="12"/>
       <c r="B4" s="15"/>
       <c r="C4" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D4" s="10">
         <v>5.6908000000000003</v>
@@ -689,17 +722,17 @@
         <v>1621.6</v>
       </c>
       <c r="I4" s="8" t="s">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="J4" s="8" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="12"/>
       <c r="B5" s="15"/>
       <c r="C5" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D5" s="10">
         <v>9.3076000000000008</v>
@@ -717,11 +750,11 @@
         <v>1775.9</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="12"/>
       <c r="B6" s="15"/>
       <c r="C6" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D6" s="10">
         <v>5.8951000000000002</v>
@@ -739,11 +772,11 @@
         <v>1598.4</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="12"/>
       <c r="B7" s="15"/>
       <c r="C7" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D7" s="10">
         <v>4.1862000000000004</v>
@@ -761,7 +794,7 @@
         <v>1574.3</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="12"/>
       <c r="B8" s="15"/>
       <c r="C8" s="8" t="s">
@@ -783,11 +816,11 @@
         <v>1944.6</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="12"/>
       <c r="B9" s="15"/>
       <c r="C9" s="8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D9" s="2">
         <v>27.547000000000001</v>
@@ -805,11 +838,11 @@
         <v>2454.8000000000002</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="12"/>
       <c r="B10" s="15"/>
       <c r="C10" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D10" s="2">
         <v>27.885000000000002</v>
@@ -827,11 +860,11 @@
         <v>2390.5</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="12"/>
       <c r="B11" s="15"/>
       <c r="C11" s="8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D11" s="2">
         <v>19.2</v>
@@ -849,11 +882,11 @@
         <v>1614.6</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="12"/>
       <c r="B12" s="15"/>
       <c r="C12" s="8" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="D12" s="9">
         <v>8.5922999999999998</v>
@@ -871,7 +904,7 @@
         <v>1841</v>
       </c>
     </row>
-    <row r="13" spans="1:10" s="5" customFormat="1" ht="5.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:10" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="13"/>
       <c r="B13" s="16"/>
       <c r="C13" s="7"/>
@@ -879,7 +912,7 @@
       <c r="I13" s="7"/>
       <c r="J13" s="7"/>
     </row>
-    <row r="14" spans="1:10" ht="5.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:10" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="11">
         <v>800</v>
       </c>
@@ -887,7 +920,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="12"/>
       <c r="B15" s="15"/>
       <c r="C15" s="8" t="s">
@@ -909,17 +942,17 @@
         <v>2575.8000000000002</v>
       </c>
       <c r="I15" s="8" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="J15" s="8" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="12"/>
       <c r="B16" s="15"/>
       <c r="C16" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D16" s="2">
         <v>22.393000000000001</v>
@@ -937,17 +970,17 @@
         <v>1828.1</v>
       </c>
       <c r="I16" s="8" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="J16" s="8" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="12"/>
       <c r="B17" s="15"/>
       <c r="C17" s="8" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="D17" s="4">
         <v>11.45</v>
@@ -965,11 +998,11 @@
         <v>2221.6</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="12"/>
       <c r="B18" s="15"/>
       <c r="C18" s="8" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="D18" s="4">
         <v>37.741999999999997</v>
@@ -987,11 +1020,11 @@
         <v>3172</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="12"/>
       <c r="B19" s="15"/>
       <c r="C19" s="8" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D19" s="2">
         <v>18.768000000000001</v>
@@ -1009,11 +1042,11 @@
         <v>1677.4</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="12"/>
       <c r="B20" s="15"/>
       <c r="C20" s="8" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D20" s="2">
         <v>23.303999999999998</v>
@@ -1031,11 +1064,11 @@
         <v>1822.6</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="12"/>
       <c r="B21" s="15"/>
       <c r="C21" s="8" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="D21" s="2">
         <v>31.137</v>
@@ -1053,11 +1086,11 @@
         <v>2583</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="12"/>
       <c r="B22" s="15"/>
       <c r="C22" s="8" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="D22" s="2">
         <v>29.725999999999999</v>
@@ -1075,11 +1108,11 @@
         <v>2101.3000000000002</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="12"/>
       <c r="B23" s="15"/>
       <c r="C23" s="8" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="D23" s="2">
         <v>4.2226999999999997</v>
@@ -1097,7 +1130,7 @@
         <v>1261.4000000000001</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="12"/>
       <c r="B24" s="15"/>
       <c r="C24" s="8" t="s">
@@ -1119,7 +1152,7 @@
         <v>3016.2</v>
       </c>
     </row>
-    <row r="25" spans="1:10" s="5" customFormat="1" ht="5.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:10" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="13"/>
       <c r="B25" s="16"/>
       <c r="C25" s="7"/>
@@ -1127,7 +1160,7 @@
       <c r="I25" s="7"/>
       <c r="J25" s="7"/>
     </row>
-    <row r="26" spans="1:10" ht="5.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:10" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="11">
         <v>900</v>
       </c>
@@ -1135,11 +1168,11 @@
         <v>6</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="12"/>
       <c r="B27" s="15"/>
       <c r="C27" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D27" s="4">
         <v>4.8710000000000004</v>
@@ -1157,17 +1190,17 @@
         <v>1138.3</v>
       </c>
       <c r="I27" s="8" t="s">
-        <v>19</v>
+        <v>34</v>
       </c>
       <c r="J27" s="8" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.35">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="12"/>
       <c r="B28" s="15"/>
       <c r="C28" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D28" s="2">
         <v>10.692</v>
@@ -1185,17 +1218,17 @@
         <v>1433.5</v>
       </c>
       <c r="I28" s="8" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="J28" s="8" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.35">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="12"/>
       <c r="B29" s="15"/>
       <c r="C29" s="8" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="D29" s="2">
         <v>11.2</v>
@@ -1213,17 +1246,17 @@
         <v>1163</v>
       </c>
       <c r="I29" s="8" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="J29" s="8" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.35">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="12"/>
       <c r="B30" s="15"/>
       <c r="C30" s="8" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="D30" s="4">
         <v>11.208</v>
@@ -1241,7 +1274,7 @@
         <v>1530.1</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="12"/>
       <c r="B31" s="15"/>
       <c r="C31" s="8" t="s">
@@ -1263,11 +1296,11 @@
         <v>1787.3</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="12"/>
       <c r="B32" s="15"/>
       <c r="C32" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D32" s="2">
         <v>11.010999999999999</v>
@@ -1285,11 +1318,11 @@
         <v>1593.8</v>
       </c>
     </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A33" s="12"/>
       <c r="B33" s="15"/>
       <c r="C33" s="8" t="s">
-        <v>21</v>
+        <v>32</v>
       </c>
       <c r="D33" s="2">
         <v>5.6656000000000004</v>
@@ -1307,7 +1340,7 @@
         <v>1000.8</v>
       </c>
     </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A34" s="12"/>
       <c r="B34" s="15"/>
       <c r="C34" s="8" t="s">
@@ -1329,11 +1362,11 @@
         <v>2110.6</v>
       </c>
     </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A35" s="12"/>
       <c r="B35" s="15"/>
       <c r="C35" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D35" s="2">
         <v>8.0571999999999999</v>
@@ -1351,11 +1384,11 @@
         <v>1210.4000000000001</v>
       </c>
     </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A36" s="12"/>
       <c r="B36" s="15"/>
       <c r="C36" s="8" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="D36" s="2">
         <v>7.5292000000000003</v>
@@ -1373,7 +1406,7 @@
         <v>1369.1</v>
       </c>
     </row>
-    <row r="37" spans="1:15" s="5" customFormat="1" ht="5.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:15" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="13"/>
       <c r="B37" s="16"/>
       <c r="C37" s="7"/>
@@ -1381,7 +1414,7 @@
       <c r="I37" s="7"/>
       <c r="J37" s="7"/>
     </row>
-    <row r="38" spans="1:15" ht="5.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:15" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="11">
         <v>900</v>
       </c>
@@ -1389,11 +1422,11 @@
         <v>7</v>
       </c>
     </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A39" s="12"/>
       <c r="B39" s="15"/>
       <c r="C39" s="8" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="D39" s="4">
         <v>4.8238000000000003</v>
@@ -1411,10 +1444,10 @@
         <v>1006.9</v>
       </c>
       <c r="I39" s="8" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="J39" s="8" t="s">
-        <v>22</v>
+        <v>38</v>
       </c>
       <c r="K39" s="2"/>
       <c r="L39" s="2"/>
@@ -1422,11 +1455,11 @@
       <c r="N39" s="2"/>
       <c r="O39" s="2"/>
     </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A40" s="12"/>
       <c r="B40" s="15"/>
       <c r="C40" s="8" t="s">
-        <v>21</v>
+        <v>33</v>
       </c>
       <c r="D40" s="4">
         <v>7.1036999999999999</v>
@@ -1444,10 +1477,10 @@
         <v>1829.9</v>
       </c>
       <c r="I40" s="8" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="J40" s="8" t="s">
-        <v>26</v>
+        <v>42</v>
       </c>
       <c r="K40" s="2"/>
       <c r="L40" s="2"/>
@@ -1455,11 +1488,11 @@
       <c r="N40" s="2"/>
       <c r="O40" s="2"/>
     </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A41" s="12"/>
       <c r="B41" s="15"/>
       <c r="C41" s="8" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="D41" s="4">
         <v>3.0461</v>
@@ -1477,17 +1510,17 @@
         <v>2022.3</v>
       </c>
       <c r="I41" s="8" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="J41" s="8" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.35">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A42" s="12"/>
       <c r="B42" s="15"/>
       <c r="C42" s="8" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="D42" s="2">
         <v>4.6340000000000003</v>
@@ -1505,11 +1538,11 @@
         <v>1999.7</v>
       </c>
     </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A43" s="12"/>
       <c r="B43" s="15"/>
       <c r="C43" s="8" t="s">
-        <v>23</v>
+        <v>34</v>
       </c>
       <c r="D43" s="2">
         <v>16.286999999999999</v>
@@ -1527,11 +1560,11 @@
         <v>2606.1999999999998</v>
       </c>
     </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A44" s="12"/>
       <c r="B44" s="15"/>
       <c r="C44" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D44" s="2">
         <v>9.5312999999999999</v>
@@ -1549,11 +1582,11 @@
         <v>1253.9000000000001</v>
       </c>
     </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A45" s="12"/>
       <c r="B45" s="15"/>
       <c r="C45" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D45" s="2">
         <v>6.3647</v>
@@ -1571,11 +1604,11 @@
         <v>1127.5999999999999</v>
       </c>
     </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A46" s="12"/>
       <c r="B46" s="15"/>
       <c r="C46" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D46" s="2">
         <v>12.622</v>
@@ -1593,11 +1626,11 @@
         <v>1371.6</v>
       </c>
     </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A47" s="12"/>
       <c r="B47" s="15"/>
       <c r="C47" s="8" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="D47" s="4">
         <v>12.256</v>
@@ -1615,11 +1648,11 @@
         <v>1242.3</v>
       </c>
     </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A48" s="12"/>
       <c r="B48" s="15"/>
       <c r="C48" s="8" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D48" s="2">
         <v>7.0439999999999996</v>
@@ -1637,7 +1670,7 @@
         <v>1090</v>
       </c>
     </row>
-    <row r="49" spans="1:10" s="5" customFormat="1" ht="5.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:10" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="13"/>
       <c r="B49" s="16"/>
       <c r="C49" s="7"/>
@@ -1645,7 +1678,7 @@
       <c r="I49" s="7"/>
       <c r="J49" s="7"/>
     </row>
-    <row r="50" spans="1:10" ht="5.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:10" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="11">
         <v>1000</v>
       </c>
@@ -1653,47 +1686,47 @@
         <v>6</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" s="12"/>
       <c r="B51" s="15"/>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" s="12"/>
       <c r="B52" s="15"/>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" s="12"/>
       <c r="B53" s="15"/>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" s="12"/>
       <c r="B54" s="15"/>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" s="12"/>
       <c r="B55" s="15"/>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" s="12"/>
       <c r="B56" s="15"/>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" s="12"/>
       <c r="B57" s="15"/>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" s="12"/>
       <c r="B58" s="15"/>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59" s="12"/>
       <c r="B59" s="15"/>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60" s="12"/>
       <c r="B60" s="15"/>
     </row>
-    <row r="61" spans="1:10" s="5" customFormat="1" ht="5.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:10" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="13"/>
       <c r="B61" s="16"/>
       <c r="C61" s="7"/>
@@ -1701,7 +1734,7 @@
       <c r="I61" s="7"/>
       <c r="J61" s="7"/>
     </row>
-    <row r="62" spans="1:10" ht="5.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:10" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="11">
         <v>1000</v>
       </c>
@@ -1709,47 +1742,47 @@
         <v>7</v>
       </c>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63" s="12"/>
       <c r="B63" s="15"/>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A64" s="12"/>
       <c r="B64" s="15"/>
     </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A65" s="12"/>
       <c r="B65" s="15"/>
     </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A66" s="12"/>
       <c r="B66" s="15"/>
     </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A67" s="12"/>
       <c r="B67" s="15"/>
     </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A68" s="12"/>
       <c r="B68" s="15"/>
     </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A69" s="12"/>
       <c r="B69" s="15"/>
     </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A70" s="12"/>
       <c r="B70" s="15"/>
     </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A71" s="12"/>
       <c r="B71" s="15"/>
     </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A72" s="12"/>
       <c r="B72" s="15"/>
     </row>
-    <row r="73" spans="1:10" s="5" customFormat="1" ht="5.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:10" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="13"/>
       <c r="B73" s="16"/>
       <c r="C73" s="7"/>
@@ -1759,18 +1792,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A38:A49"/>
+    <mergeCell ref="B38:B49"/>
+    <mergeCell ref="A50:A61"/>
+    <mergeCell ref="B50:B61"/>
+    <mergeCell ref="A62:A73"/>
+    <mergeCell ref="B62:B73"/>
     <mergeCell ref="A2:A13"/>
     <mergeCell ref="B2:B13"/>
     <mergeCell ref="A14:A25"/>
     <mergeCell ref="B14:B25"/>
     <mergeCell ref="A26:A37"/>
     <mergeCell ref="B26:B37"/>
-    <mergeCell ref="A38:A49"/>
-    <mergeCell ref="B38:B49"/>
-    <mergeCell ref="A50:A61"/>
-    <mergeCell ref="B50:B61"/>
-    <mergeCell ref="A62:A73"/>
-    <mergeCell ref="B62:B73"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -1781,25 +1814,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE483CC8-AF2C-4D5A-AEE5-EF7DF4EC0883}">
   <dimension ref="A1:T73"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D15" sqref="D15:H15"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C3" sqref="C3:C41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.1796875" style="4"/>
-    <col min="2" max="2" width="9.1796875" style="3"/>
-    <col min="3" max="3" width="15.7265625" style="8" customWidth="1"/>
-    <col min="4" max="10" width="9.1796875" style="4"/>
-    <col min="11" max="11" width="9.1796875" style="3"/>
-    <col min="12" max="12" width="15.7265625" style="8" customWidth="1"/>
-    <col min="13" max="19" width="9.1796875" style="4"/>
-    <col min="20" max="20" width="9.1796875" style="3"/>
-    <col min="21" max="16384" width="9.1796875" style="4"/>
+    <col min="1" max="1" width="9.140625" style="4"/>
+    <col min="2" max="2" width="9.140625" style="3"/>
+    <col min="3" max="3" width="15.7109375" style="8" customWidth="1"/>
+    <col min="4" max="10" width="9.140625" style="4"/>
+    <col min="11" max="11" width="9.140625" style="3"/>
+    <col min="12" max="12" width="15.7109375" style="8" customWidth="1"/>
+    <col min="13" max="19" width="9.140625" style="4"/>
+    <col min="20" max="20" width="9.140625" style="3"/>
+    <col min="21" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -1807,7 +1840,7 @@
         <v>11</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="D1" s="5" t="s">
         <v>1</v>
@@ -1834,7 +1867,7 @@
         <v>10</v>
       </c>
       <c r="L1" s="7" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="M1" s="5" t="s">
         <v>1</v>
@@ -1861,7 +1894,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:20" ht="5.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:20" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="11">
         <v>800</v>
       </c>
@@ -1869,11 +1902,11 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" s="12"/>
       <c r="B3" s="15"/>
       <c r="C3" s="8" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="D3" s="4">
         <v>17.216999999999999</v>
@@ -1891,52 +1924,79 @@
         <v>1783.5</v>
       </c>
       <c r="I3" s="2">
-        <v>1894.9</v>
+        <v>1889.7</v>
       </c>
       <c r="J3" s="2">
-        <v>5.5266999999999999</v>
+        <v>5.5457000000000001</v>
       </c>
       <c r="K3" s="2">
-        <v>6.4467999999999996</v>
-      </c>
-    </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.35">
+        <v>6.5846</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" s="12"/>
       <c r="B4" s="15"/>
-    </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="C4" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="D4" s="4">
+        <v>5.6908000000000003</v>
+      </c>
+      <c r="E4" s="4">
+        <v>66.626999999999995</v>
+      </c>
+      <c r="F4" s="4">
+        <v>1.9851000000000001</v>
+      </c>
+      <c r="G4" s="4">
+        <v>4.7723000000000004</v>
+      </c>
+      <c r="H4" s="4">
+        <v>1621.6</v>
+      </c>
+      <c r="I4" s="2">
+        <v>1793.4</v>
+      </c>
+      <c r="J4" s="2">
+        <v>5.6519000000000004</v>
+      </c>
+      <c r="K4" s="2">
+        <v>6.8314000000000004</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" s="12"/>
       <c r="B5" s="15"/>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" s="12"/>
       <c r="B6" s="15"/>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" s="12"/>
       <c r="B7" s="15"/>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" s="12"/>
       <c r="B8" s="15"/>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" s="12"/>
       <c r="B9" s="15"/>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10" s="12"/>
       <c r="B10" s="15"/>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11" s="12"/>
       <c r="B11" s="15"/>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12" s="12"/>
       <c r="B12" s="15"/>
     </row>
-    <row r="13" spans="1:20" s="5" customFormat="1" ht="5.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:20" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="13"/>
       <c r="B13" s="16"/>
       <c r="C13" s="7"/>
@@ -1944,7 +2004,7 @@
       <c r="L13" s="7"/>
       <c r="T13" s="6"/>
     </row>
-    <row r="14" spans="1:20" ht="5.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:20" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="11">
         <v>800</v>
       </c>
@@ -1952,11 +2012,11 @@
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15" s="12"/>
       <c r="B15" s="15"/>
       <c r="C15" s="8" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D15" s="4">
         <v>31.327000000000002</v>
@@ -1983,43 +2043,70 @@
         <v>6.5503999999999998</v>
       </c>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16" s="12"/>
       <c r="B16" s="15"/>
-    </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="C16" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D16" s="2">
+        <v>22.393000000000001</v>
+      </c>
+      <c r="E16" s="2">
+        <v>462.57</v>
+      </c>
+      <c r="F16" s="2">
+        <v>0.13572999999999999</v>
+      </c>
+      <c r="G16" s="2">
+        <v>4.3140000000000001</v>
+      </c>
+      <c r="H16" s="2">
+        <v>1828.1</v>
+      </c>
+      <c r="I16" s="2">
+        <v>1912.9</v>
+      </c>
+      <c r="J16" s="2">
+        <v>5.5168999999999997</v>
+      </c>
+      <c r="K16" s="2">
+        <v>6.9638999999999998</v>
+      </c>
+    </row>
+    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A17" s="12"/>
       <c r="B17" s="15"/>
     </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A18" s="12"/>
       <c r="B18" s="15"/>
     </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A19" s="12"/>
       <c r="B19" s="15"/>
     </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A20" s="12"/>
       <c r="B20" s="15"/>
     </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A21" s="12"/>
       <c r="B21" s="15"/>
     </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A22" s="12"/>
       <c r="B22" s="15"/>
     </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A23" s="12"/>
       <c r="B23" s="15"/>
     </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A24" s="12"/>
       <c r="B24" s="15"/>
     </row>
-    <row r="25" spans="1:20" s="5" customFormat="1" ht="5.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:20" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="13"/>
       <c r="B25" s="16"/>
       <c r="C25" s="7"/>
@@ -2027,7 +2114,7 @@
       <c r="L25" s="7"/>
       <c r="T25" s="6"/>
     </row>
-    <row r="26" spans="1:20" ht="5.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:20" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="11">
         <v>900</v>
       </c>
@@ -2035,11 +2122,11 @@
         <v>6</v>
       </c>
     </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A27" s="12"/>
       <c r="B27" s="15"/>
       <c r="C27" s="8" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="D27" s="4">
         <v>4.8710000000000004</v>
@@ -2066,11 +2153,11 @@
         <v>7.5202</v>
       </c>
     </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A28" s="12"/>
       <c r="B28" s="15"/>
       <c r="C28" s="8" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D28" s="4">
         <v>10.692</v>
@@ -2097,39 +2184,66 @@
         <v>5.8509000000000002</v>
       </c>
     </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A29" s="12"/>
       <c r="B29" s="15"/>
-    </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="C29" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D29" s="4">
+        <v>11.2</v>
+      </c>
+      <c r="E29" s="4">
+        <v>24.262</v>
+      </c>
+      <c r="F29" s="4">
+        <v>2.2614999999999998</v>
+      </c>
+      <c r="G29" s="4">
+        <v>3.9651000000000001</v>
+      </c>
+      <c r="H29" s="4">
+        <v>1163</v>
+      </c>
+      <c r="I29" s="2">
+        <v>1730.2</v>
+      </c>
+      <c r="J29" s="2">
+        <v>4.5327000000000002</v>
+      </c>
+      <c r="K29" s="2">
+        <v>7.9908000000000001</v>
+      </c>
+    </row>
+    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A30" s="12"/>
       <c r="B30" s="15"/>
     </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A31" s="12"/>
       <c r="B31" s="15"/>
     </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A32" s="12"/>
       <c r="B32" s="15"/>
     </row>
-    <row r="33" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A33" s="12"/>
       <c r="B33" s="15"/>
     </row>
-    <row r="34" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A34" s="12"/>
       <c r="B34" s="15"/>
     </row>
-    <row r="35" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A35" s="12"/>
       <c r="B35" s="15"/>
     </row>
-    <row r="36" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A36" s="12"/>
       <c r="B36" s="15"/>
     </row>
-    <row r="37" spans="1:20" s="5" customFormat="1" ht="5.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:20" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="13"/>
       <c r="B37" s="16"/>
       <c r="C37" s="7"/>
@@ -2137,7 +2251,7 @@
       <c r="L37" s="7"/>
       <c r="T37" s="6"/>
     </row>
-    <row r="38" spans="1:20" ht="5.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:20" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="11">
         <v>900</v>
       </c>
@@ -2145,11 +2259,11 @@
         <v>7</v>
       </c>
     </row>
-    <row r="39" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A39" s="12"/>
       <c r="B39" s="15"/>
       <c r="C39" s="8" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="D39" s="4">
         <v>4.8238000000000003</v>
@@ -2176,11 +2290,11 @@
         <v>7.3331</v>
       </c>
     </row>
-    <row r="40" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A40" s="12"/>
       <c r="B40" s="15"/>
       <c r="C40" s="8" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D40" s="4">
         <v>7.1036999999999999</v>
@@ -2197,49 +2311,76 @@
       <c r="H40" s="4">
         <v>1829.9</v>
       </c>
-      <c r="I40" s="4">
-        <v>1702.3</v>
-      </c>
-      <c r="J40" s="4">
-        <v>4.4939999999999998</v>
-      </c>
-      <c r="K40" s="3">
-        <v>5.4440999999999997</v>
-      </c>
-    </row>
-    <row r="41" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="I40" s="2">
+        <v>1433</v>
+      </c>
+      <c r="J40" s="2">
+        <v>4.6205999999999996</v>
+      </c>
+      <c r="K40" s="2">
+        <v>4.3208000000000002</v>
+      </c>
+    </row>
+    <row r="41" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A41" s="12"/>
       <c r="B41" s="15"/>
-    </row>
-    <row r="42" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="C41" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="D41" s="4">
+        <v>3.0461</v>
+      </c>
+      <c r="E41" s="4">
+        <v>19.608000000000001</v>
+      </c>
+      <c r="F41" s="4">
+        <v>32.420999999999999</v>
+      </c>
+      <c r="G41" s="4">
+        <v>3.2736000000000001</v>
+      </c>
+      <c r="H41" s="4">
+        <v>2022.3</v>
+      </c>
+      <c r="I41" s="2">
+        <v>2563.4</v>
+      </c>
+      <c r="J41" s="2">
+        <v>4.2545000000000002</v>
+      </c>
+      <c r="K41" s="2">
+        <v>13.452999999999999</v>
+      </c>
+    </row>
+    <row r="42" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A42" s="12"/>
       <c r="B42" s="15"/>
     </row>
-    <row r="43" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A43" s="12"/>
       <c r="B43" s="15"/>
     </row>
-    <row r="44" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A44" s="12"/>
       <c r="B44" s="15"/>
     </row>
-    <row r="45" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A45" s="12"/>
       <c r="B45" s="15"/>
     </row>
-    <row r="46" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A46" s="12"/>
       <c r="B46" s="15"/>
     </row>
-    <row r="47" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A47" s="12"/>
       <c r="B47" s="15"/>
     </row>
-    <row r="48" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A48" s="12"/>
       <c r="B48" s="15"/>
     </row>
-    <row r="49" spans="1:20" s="5" customFormat="1" ht="5.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:20" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="13"/>
       <c r="B49" s="16"/>
       <c r="C49" s="7"/>
@@ -2247,7 +2388,7 @@
       <c r="L49" s="7"/>
       <c r="T49" s="6"/>
     </row>
-    <row r="50" spans="1:20" ht="5.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:20" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="11">
         <v>1000</v>
       </c>
@@ -2255,47 +2396,47 @@
         <v>6</v>
       </c>
     </row>
-    <row r="51" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A51" s="12"/>
       <c r="B51" s="15"/>
     </row>
-    <row r="52" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A52" s="12"/>
       <c r="B52" s="15"/>
     </row>
-    <row r="53" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A53" s="12"/>
       <c r="B53" s="15"/>
     </row>
-    <row r="54" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A54" s="12"/>
       <c r="B54" s="15"/>
     </row>
-    <row r="55" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A55" s="12"/>
       <c r="B55" s="15"/>
     </row>
-    <row r="56" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A56" s="12"/>
       <c r="B56" s="15"/>
     </row>
-    <row r="57" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A57" s="12"/>
       <c r="B57" s="15"/>
     </row>
-    <row r="58" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A58" s="12"/>
       <c r="B58" s="15"/>
     </row>
-    <row r="59" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A59" s="12"/>
       <c r="B59" s="15"/>
     </row>
-    <row r="60" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A60" s="12"/>
       <c r="B60" s="15"/>
     </row>
-    <row r="61" spans="1:20" s="5" customFormat="1" ht="5.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:20" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="13"/>
       <c r="B61" s="16"/>
       <c r="C61" s="7"/>
@@ -2303,7 +2444,7 @@
       <c r="L61" s="7"/>
       <c r="T61" s="6"/>
     </row>
-    <row r="62" spans="1:20" ht="5.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:20" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="11">
         <v>1000</v>
       </c>
@@ -2311,47 +2452,47 @@
         <v>7</v>
       </c>
     </row>
-    <row r="63" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A63" s="12"/>
       <c r="B63" s="15"/>
     </row>
-    <row r="64" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A64" s="12"/>
       <c r="B64" s="15"/>
     </row>
-    <row r="65" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A65" s="12"/>
       <c r="B65" s="15"/>
     </row>
-    <row r="66" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A66" s="12"/>
       <c r="B66" s="15"/>
     </row>
-    <row r="67" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A67" s="12"/>
       <c r="B67" s="15"/>
     </row>
-    <row r="68" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A68" s="12"/>
       <c r="B68" s="15"/>
     </row>
-    <row r="69" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A69" s="12"/>
       <c r="B69" s="15"/>
     </row>
-    <row r="70" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A70" s="12"/>
       <c r="B70" s="15"/>
     </row>
-    <row r="71" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A71" s="12"/>
       <c r="B71" s="15"/>
     </row>
-    <row r="72" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A72" s="12"/>
       <c r="B72" s="15"/>
     </row>
-    <row r="73" spans="1:20" s="5" customFormat="1" ht="5.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:20" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="13"/>
       <c r="B73" s="16"/>
       <c r="C73" s="7"/>
@@ -2361,18 +2502,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A38:A49"/>
+    <mergeCell ref="B38:B49"/>
+    <mergeCell ref="A50:A61"/>
+    <mergeCell ref="B50:B61"/>
+    <mergeCell ref="A62:A73"/>
+    <mergeCell ref="B62:B73"/>
     <mergeCell ref="A2:A13"/>
     <mergeCell ref="B2:B13"/>
     <mergeCell ref="A14:A25"/>
     <mergeCell ref="B14:B25"/>
     <mergeCell ref="A26:A37"/>
     <mergeCell ref="B26:B37"/>
-    <mergeCell ref="A38:A49"/>
-    <mergeCell ref="B38:B49"/>
-    <mergeCell ref="A50:A61"/>
-    <mergeCell ref="B50:B61"/>
-    <mergeCell ref="A62:A73"/>
-    <mergeCell ref="B62:B73"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -2383,25 +2524,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C18A26E-30CA-4E63-A18A-C9C101DAF33C}">
   <dimension ref="A1:Z73"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E10" sqref="E10"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C3" sqref="C3:C41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.1796875" style="4"/>
-    <col min="2" max="2" width="9.1796875" style="3"/>
-    <col min="3" max="3" width="15.7265625" style="8" customWidth="1"/>
-    <col min="4" max="13" width="9.1796875" style="4"/>
-    <col min="14" max="14" width="9.1796875" style="3"/>
-    <col min="15" max="15" width="15.7265625" style="8" customWidth="1"/>
-    <col min="16" max="25" width="9.1796875" style="4"/>
-    <col min="26" max="26" width="9.1796875" style="3"/>
-    <col min="27" max="16384" width="9.1796875" style="4"/>
+    <col min="1" max="1" width="9.140625" style="4"/>
+    <col min="2" max="2" width="9.140625" style="3"/>
+    <col min="3" max="3" width="15.7109375" style="8" customWidth="1"/>
+    <col min="4" max="13" width="9.140625" style="4"/>
+    <col min="14" max="14" width="9.140625" style="3"/>
+    <col min="15" max="15" width="15.7109375" style="8" customWidth="1"/>
+    <col min="16" max="25" width="9.140625" style="4"/>
+    <col min="26" max="26" width="9.140625" style="3"/>
+    <col min="27" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:26" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -2409,7 +2550,7 @@
         <v>11</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="D1" s="5" t="s">
         <v>1</v>
@@ -2445,7 +2586,7 @@
         <v>17</v>
       </c>
       <c r="O1" s="7" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="P1" s="5" t="s">
         <v>1</v>
@@ -2481,7 +2622,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:26" ht="5.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:26" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="11">
         <v>800</v>
       </c>
@@ -2489,11 +2630,11 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A3" s="12"/>
       <c r="B3" s="15"/>
       <c r="C3" s="8" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="D3" s="4">
         <v>17.216999999999999</v>
@@ -2510,62 +2651,98 @@
       <c r="H3" s="4">
         <v>1783.5</v>
       </c>
-      <c r="I3" s="4">
-        <v>2.1827999999999999</v>
-      </c>
-      <c r="J3" s="4">
-        <v>0.47720000000000001</v>
-      </c>
-      <c r="K3" s="4">
-        <v>4.1695000000000002</v>
-      </c>
-      <c r="L3" s="4">
-        <v>3.6650999999999998</v>
-      </c>
-      <c r="M3" s="4">
-        <v>0.13758999999999999</v>
-      </c>
-      <c r="N3" s="3">
-        <v>2.6194999999999999</v>
-      </c>
-    </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="I3" s="2">
+        <v>2.2067000000000001</v>
+      </c>
+      <c r="J3" s="2">
+        <v>0.48282999999999998</v>
+      </c>
+      <c r="K3" s="2">
+        <v>4.1563999999999997</v>
+      </c>
+      <c r="L3" s="2">
+        <v>4.4695</v>
+      </c>
+      <c r="M3" s="2">
+        <v>8.2167000000000004E-3</v>
+      </c>
+      <c r="N3" s="2">
+        <v>2.5705</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A4" s="12"/>
       <c r="B4" s="15"/>
-    </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="C4" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="D4" s="4">
+        <v>5.6908000000000003</v>
+      </c>
+      <c r="E4" s="4">
+        <v>66.626999999999995</v>
+      </c>
+      <c r="F4" s="4">
+        <v>1.9851000000000001</v>
+      </c>
+      <c r="G4" s="4">
+        <v>4.7723000000000004</v>
+      </c>
+      <c r="H4" s="4">
+        <v>1621.6</v>
+      </c>
+      <c r="I4" s="4">
+        <v>2.5101</v>
+      </c>
+      <c r="J4" s="4">
+        <v>0.51356000000000002</v>
+      </c>
+      <c r="K4" s="4">
+        <v>4.2454000000000001</v>
+      </c>
+      <c r="L4" s="4">
+        <v>1.9213</v>
+      </c>
+      <c r="M4" s="4">
+        <v>1.5276E-2</v>
+      </c>
+      <c r="N4" s="3">
+        <v>2.6046</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A5" s="12"/>
       <c r="B5" s="15"/>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A6" s="12"/>
       <c r="B6" s="15"/>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A7" s="12"/>
       <c r="B7" s="15"/>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A8" s="12"/>
       <c r="B8" s="15"/>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A9" s="12"/>
       <c r="B9" s="15"/>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A10" s="12"/>
       <c r="B10" s="15"/>
     </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A11" s="12"/>
       <c r="B11" s="15"/>
     </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A12" s="12"/>
       <c r="B12" s="15"/>
     </row>
-    <row r="13" spans="1:26" s="5" customFormat="1" ht="5.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:26" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="13"/>
       <c r="B13" s="16"/>
       <c r="C13" s="7"/>
@@ -2573,7 +2750,7 @@
       <c r="O13" s="7"/>
       <c r="Z13" s="6"/>
     </row>
-    <row r="14" spans="1:26" ht="5.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:26" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="11">
         <v>800</v>
       </c>
@@ -2581,7 +2758,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A15" s="12"/>
       <c r="B15" s="15"/>
       <c r="C15" s="8" t="s">
@@ -2621,43 +2798,79 @@
         <v>0.28255999999999998</v>
       </c>
     </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A16" s="12"/>
       <c r="B16" s="15"/>
-    </row>
-    <row r="17" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="C16" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="D16" s="4">
+        <v>22.393000000000001</v>
+      </c>
+      <c r="E16" s="4">
+        <v>462.57</v>
+      </c>
+      <c r="F16" s="4">
+        <v>0.13572999999999999</v>
+      </c>
+      <c r="G16" s="4">
+        <v>4.3140000000000001</v>
+      </c>
+      <c r="H16" s="4">
+        <v>1828.1</v>
+      </c>
+      <c r="I16" s="4">
+        <v>2.0305</v>
+      </c>
+      <c r="J16" s="4">
+        <v>0.26046999999999998</v>
+      </c>
+      <c r="K16" s="4">
+        <v>3.0701000000000001</v>
+      </c>
+      <c r="L16" s="4">
+        <v>4.7169999999999996</v>
+      </c>
+      <c r="M16" s="4">
+        <v>0.15376000000000001</v>
+      </c>
+      <c r="N16" s="3">
+        <v>2.6135999999999999</v>
+      </c>
+    </row>
+    <row r="17" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A17" s="12"/>
       <c r="B17" s="15"/>
     </row>
-    <row r="18" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A18" s="12"/>
       <c r="B18" s="15"/>
     </row>
-    <row r="19" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A19" s="12"/>
       <c r="B19" s="15"/>
     </row>
-    <row r="20" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A20" s="12"/>
       <c r="B20" s="15"/>
     </row>
-    <row r="21" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A21" s="12"/>
       <c r="B21" s="15"/>
     </row>
-    <row r="22" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A22" s="12"/>
       <c r="B22" s="15"/>
     </row>
-    <row r="23" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A23" s="12"/>
       <c r="B23" s="15"/>
     </row>
-    <row r="24" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A24" s="12"/>
       <c r="B24" s="15"/>
     </row>
-    <row r="25" spans="1:26" s="5" customFormat="1" ht="5.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:26" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="13"/>
       <c r="B25" s="16"/>
       <c r="C25" s="7"/>
@@ -2665,7 +2878,7 @@
       <c r="O25" s="7"/>
       <c r="Z25" s="6"/>
     </row>
-    <row r="26" spans="1:26" ht="5.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:26" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="11">
         <v>900</v>
       </c>
@@ -2673,11 +2886,11 @@
         <v>6</v>
       </c>
     </row>
-    <row r="27" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A27" s="12"/>
       <c r="B27" s="15"/>
       <c r="C27" s="8" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="D27" s="4">
         <v>4.8710000000000004</v>
@@ -2713,11 +2926,11 @@
         <v>2.5308000000000002</v>
       </c>
     </row>
-    <row r="28" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A28" s="12"/>
       <c r="B28" s="15"/>
       <c r="C28" s="8" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="D28" s="4">
         <v>10.692</v>
@@ -2753,39 +2966,75 @@
         <v>2.4864000000000002</v>
       </c>
     </row>
-    <row r="29" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A29" s="12"/>
       <c r="B29" s="15"/>
-    </row>
-    <row r="30" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="C29" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="D29" s="4">
+        <v>11.2</v>
+      </c>
+      <c r="E29" s="4">
+        <v>24.262</v>
+      </c>
+      <c r="F29" s="4">
+        <v>2.2614999999999998</v>
+      </c>
+      <c r="G29" s="4">
+        <v>3.9651000000000001</v>
+      </c>
+      <c r="H29" s="4">
+        <v>1163</v>
+      </c>
+      <c r="I29" s="4">
+        <v>1.7908999999999999</v>
+      </c>
+      <c r="J29" s="4">
+        <v>0.45981</v>
+      </c>
+      <c r="K29" s="4">
+        <v>3.9491000000000001</v>
+      </c>
+      <c r="L29" s="4">
+        <v>3.3142</v>
+      </c>
+      <c r="M29" s="4">
+        <v>0.20016999999999999</v>
+      </c>
+      <c r="N29" s="3">
+        <v>2.4437000000000002</v>
+      </c>
+    </row>
+    <row r="30" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A30" s="12"/>
       <c r="B30" s="15"/>
     </row>
-    <row r="31" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A31" s="12"/>
       <c r="B31" s="15"/>
     </row>
-    <row r="32" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A32" s="12"/>
       <c r="B32" s="15"/>
     </row>
-    <row r="33" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A33" s="12"/>
       <c r="B33" s="15"/>
     </row>
-    <row r="34" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A34" s="12"/>
       <c r="B34" s="15"/>
     </row>
-    <row r="35" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A35" s="12"/>
       <c r="B35" s="15"/>
     </row>
-    <row r="36" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A36" s="12"/>
       <c r="B36" s="15"/>
     </row>
-    <row r="37" spans="1:26" s="5" customFormat="1" ht="5.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:26" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="13"/>
       <c r="B37" s="16"/>
       <c r="C37" s="7"/>
@@ -2793,7 +3042,7 @@
       <c r="O37" s="7"/>
       <c r="Z37" s="6"/>
     </row>
-    <row r="38" spans="1:26" ht="5.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:26" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="11">
         <v>900</v>
       </c>
@@ -2801,11 +3050,11 @@
         <v>7</v>
       </c>
     </row>
-    <row r="39" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A39" s="12"/>
       <c r="B39" s="15"/>
       <c r="C39" s="8" t="s">
-        <v>22</v>
+        <v>38</v>
       </c>
       <c r="D39" s="4">
         <v>4.8238000000000003</v>
@@ -2841,11 +3090,11 @@
         <v>2.5291999999999999</v>
       </c>
     </row>
-    <row r="40" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A40" s="12"/>
       <c r="B40" s="15"/>
       <c r="C40" s="8" t="s">
-        <v>26</v>
+        <v>42</v>
       </c>
       <c r="D40" s="4">
         <v>7.1036999999999999</v>
@@ -2881,39 +3130,75 @@
         <v>2.2601</v>
       </c>
     </row>
-    <row r="41" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A41" s="12"/>
       <c r="B41" s="15"/>
-    </row>
-    <row r="42" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="C41" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="D41" s="4">
+        <v>3.0461</v>
+      </c>
+      <c r="E41" s="4">
+        <v>19.608000000000001</v>
+      </c>
+      <c r="F41" s="4">
+        <v>32.420999999999999</v>
+      </c>
+      <c r="G41" s="4">
+        <v>3.2736000000000001</v>
+      </c>
+      <c r="H41" s="4">
+        <v>2022.3</v>
+      </c>
+      <c r="I41" s="2">
+        <v>2.8746999999999998</v>
+      </c>
+      <c r="J41" s="2">
+        <v>0.35838999999999999</v>
+      </c>
+      <c r="K41" s="2">
+        <v>3.0428999999999999</v>
+      </c>
+      <c r="L41" s="2">
+        <v>9.1083999999999996</v>
+      </c>
+      <c r="M41" s="2">
+        <v>7.6354000000000005E-2</v>
+      </c>
+      <c r="N41" s="2">
+        <v>2.1876000000000002</v>
+      </c>
+    </row>
+    <row r="42" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A42" s="12"/>
       <c r="B42" s="15"/>
     </row>
-    <row r="43" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A43" s="12"/>
       <c r="B43" s="15"/>
     </row>
-    <row r="44" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A44" s="12"/>
       <c r="B44" s="15"/>
     </row>
-    <row r="45" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A45" s="12"/>
       <c r="B45" s="15"/>
     </row>
-    <row r="46" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A46" s="12"/>
       <c r="B46" s="15"/>
     </row>
-    <row r="47" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A47" s="12"/>
       <c r="B47" s="15"/>
     </row>
-    <row r="48" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A48" s="12"/>
       <c r="B48" s="15"/>
     </row>
-    <row r="49" spans="1:26" s="5" customFormat="1" ht="5.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:26" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="13"/>
       <c r="B49" s="16"/>
       <c r="C49" s="7"/>
@@ -2921,7 +3206,7 @@
       <c r="O49" s="7"/>
       <c r="Z49" s="6"/>
     </row>
-    <row r="50" spans="1:26" ht="5.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:26" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="11">
         <v>1000</v>
       </c>
@@ -2929,47 +3214,47 @@
         <v>6</v>
       </c>
     </row>
-    <row r="51" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A51" s="12"/>
       <c r="B51" s="15"/>
     </row>
-    <row r="52" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A52" s="12"/>
       <c r="B52" s="15"/>
     </row>
-    <row r="53" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A53" s="12"/>
       <c r="B53" s="15"/>
     </row>
-    <row r="54" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A54" s="12"/>
       <c r="B54" s="15"/>
     </row>
-    <row r="55" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A55" s="12"/>
       <c r="B55" s="15"/>
     </row>
-    <row r="56" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A56" s="12"/>
       <c r="B56" s="15"/>
     </row>
-    <row r="57" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A57" s="12"/>
       <c r="B57" s="15"/>
     </row>
-    <row r="58" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A58" s="12"/>
       <c r="B58" s="15"/>
     </row>
-    <row r="59" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A59" s="12"/>
       <c r="B59" s="15"/>
     </row>
-    <row r="60" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A60" s="12"/>
       <c r="B60" s="15"/>
     </row>
-    <row r="61" spans="1:26" s="5" customFormat="1" ht="5.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:26" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="13"/>
       <c r="B61" s="16"/>
       <c r="C61" s="7"/>
@@ -2977,7 +3262,7 @@
       <c r="O61" s="7"/>
       <c r="Z61" s="6"/>
     </row>
-    <row r="62" spans="1:26" ht="5.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:26" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="11">
         <v>1000</v>
       </c>
@@ -2985,47 +3270,47 @@
         <v>7</v>
       </c>
     </row>
-    <row r="63" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A63" s="12"/>
       <c r="B63" s="15"/>
     </row>
-    <row r="64" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A64" s="12"/>
       <c r="B64" s="15"/>
     </row>
-    <row r="65" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A65" s="12"/>
       <c r="B65" s="15"/>
     </row>
-    <row r="66" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A66" s="12"/>
       <c r="B66" s="15"/>
     </row>
-    <row r="67" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A67" s="12"/>
       <c r="B67" s="15"/>
     </row>
-    <row r="68" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A68" s="12"/>
       <c r="B68" s="15"/>
     </row>
-    <row r="69" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A69" s="12"/>
       <c r="B69" s="15"/>
     </row>
-    <row r="70" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A70" s="12"/>
       <c r="B70" s="15"/>
     </row>
-    <row r="71" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A71" s="12"/>
       <c r="B71" s="15"/>
     </row>
-    <row r="72" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A72" s="12"/>
       <c r="B72" s="15"/>
     </row>
-    <row r="73" spans="1:26" s="5" customFormat="1" ht="5.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:26" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="13"/>
       <c r="B73" s="16"/>
       <c r="C73" s="7"/>
@@ -3035,18 +3320,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A38:A49"/>
+    <mergeCell ref="B38:B49"/>
+    <mergeCell ref="A50:A61"/>
+    <mergeCell ref="B50:B61"/>
+    <mergeCell ref="A62:A73"/>
+    <mergeCell ref="B62:B73"/>
     <mergeCell ref="A2:A13"/>
     <mergeCell ref="B2:B13"/>
     <mergeCell ref="A14:A25"/>
     <mergeCell ref="B14:B25"/>
     <mergeCell ref="A26:A37"/>
     <mergeCell ref="B26:B37"/>
-    <mergeCell ref="A38:A49"/>
-    <mergeCell ref="B38:B49"/>
-    <mergeCell ref="A50:A61"/>
-    <mergeCell ref="B50:B61"/>
-    <mergeCell ref="A62:A73"/>
-    <mergeCell ref="B62:B73"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
Added new obj functions to scripts
</commit_message>
<xml_diff>
--- a/scripts/__other__/__sem__.xlsx
+++ b/scripts/__other__/__sem__.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Janzen\Desktop\code\moga_neml\scripts\__other__\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70CB2808-E177-4FB6-B5A8-ECB4755D81A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8CE690E-75C1-40F0-BC54-29532D442EAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="15600" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="evp" sheetId="13" r:id="rId1"/>
@@ -127,9 +127,6 @@
     <t>9; 10</t>
   </si>
   <si>
-    <t>10; 6</t>
-  </si>
-  <si>
     <t>9; 8</t>
   </si>
   <si>
@@ -167,6 +164,9 @@
   </si>
   <si>
     <t>5; 8</t>
+  </si>
+  <si>
+    <t>8; 8</t>
   </si>
 </sst>
 </file>
@@ -616,9 +616,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4D7A15E-4182-42F6-82DA-99E9B04906BA}">
   <dimension ref="A1:O73"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M9" sqref="M9"/>
+      <selection pane="bottomLeft" activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -694,10 +694,10 @@
         <v>1783.5</v>
       </c>
       <c r="I3" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="J3" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -722,10 +722,10 @@
         <v>1621.6</v>
       </c>
       <c r="I4" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="J4" s="8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -945,7 +945,7 @@
         <v>20</v>
       </c>
       <c r="J15" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
@@ -973,7 +973,7 @@
         <v>20</v>
       </c>
       <c r="J16" s="8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
@@ -1112,22 +1112,22 @@
       <c r="A23" s="12"/>
       <c r="B23" s="15"/>
       <c r="C23" s="8" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="D23" s="2">
-        <v>4.2226999999999997</v>
+        <v>0.85682000000000003</v>
       </c>
       <c r="E23" s="2">
-        <v>26.503</v>
+        <v>42.524000000000001</v>
       </c>
       <c r="F23" s="2">
-        <v>4.0461</v>
+        <v>9.6282999999999994</v>
       </c>
       <c r="G23" s="2">
-        <v>5.25</v>
+        <v>4.5033000000000003</v>
       </c>
       <c r="H23" s="1">
-        <v>1261.4000000000001</v>
+        <v>1707</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
@@ -1190,7 +1190,7 @@
         <v>1138.3</v>
       </c>
       <c r="I27" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="J27" s="8" t="s">
         <v>23</v>
@@ -1221,14 +1221,14 @@
         <v>20</v>
       </c>
       <c r="J28" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="12"/>
       <c r="B29" s="15"/>
       <c r="C29" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D29" s="2">
         <v>11.2</v>
@@ -1249,7 +1249,7 @@
         <v>19</v>
       </c>
       <c r="J29" s="8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
@@ -1322,7 +1322,7 @@
       <c r="A33" s="12"/>
       <c r="B33" s="15"/>
       <c r="C33" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D33" s="2">
         <v>5.6656000000000004</v>
@@ -1447,7 +1447,7 @@
         <v>26</v>
       </c>
       <c r="J39" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K39" s="2"/>
       <c r="L39" s="2"/>
@@ -1459,7 +1459,7 @@
       <c r="A40" s="12"/>
       <c r="B40" s="15"/>
       <c r="C40" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D40" s="4">
         <v>7.1036999999999999</v>
@@ -1477,10 +1477,10 @@
         <v>1829.9</v>
       </c>
       <c r="I40" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J40" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K40" s="2"/>
       <c r="L40" s="2"/>
@@ -1510,17 +1510,17 @@
         <v>2022.3</v>
       </c>
       <c r="I41" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J41" s="8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="42" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A42" s="12"/>
       <c r="B42" s="15"/>
       <c r="C42" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D42" s="2">
         <v>4.6340000000000003</v>
@@ -1542,7 +1542,7 @@
       <c r="A43" s="12"/>
       <c r="B43" s="15"/>
       <c r="C43" s="8" t="s">
-        <v>34</v>
+        <v>42</v>
       </c>
       <c r="D43" s="2">
         <v>16.286999999999999</v>
@@ -1814,9 +1814,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE483CC8-AF2C-4D5A-AEE5-EF7DF4EC0883}">
   <dimension ref="A1:T73"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C3" sqref="C3:C41"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1906,7 +1906,7 @@
       <c r="A3" s="12"/>
       <c r="B3" s="15"/>
       <c r="C3" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D3" s="4">
         <v>17.216999999999999</v>
@@ -1937,7 +1937,7 @@
       <c r="A4" s="12"/>
       <c r="B4" s="15"/>
       <c r="C4" s="8" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="D4" s="4">
         <v>5.6908000000000003</v>
@@ -1955,13 +1955,13 @@
         <v>1621.6</v>
       </c>
       <c r="I4" s="2">
-        <v>1793.4</v>
+        <v>1846.1</v>
       </c>
       <c r="J4" s="2">
-        <v>5.6519000000000004</v>
+        <v>5.5984999999999996</v>
       </c>
       <c r="K4" s="2">
-        <v>6.8314000000000004</v>
+        <v>6.6852999999999998</v>
       </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
@@ -2047,7 +2047,7 @@
       <c r="A16" s="12"/>
       <c r="B16" s="15"/>
       <c r="C16" s="8" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D16" s="2">
         <v>22.393000000000001</v>
@@ -2126,7 +2126,7 @@
       <c r="A27" s="12"/>
       <c r="B27" s="15"/>
       <c r="C27" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D27" s="4">
         <v>4.8710000000000004</v>
@@ -2294,7 +2294,7 @@
       <c r="A40" s="12"/>
       <c r="B40" s="15"/>
       <c r="C40" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D40" s="4">
         <v>7.1036999999999999</v>
@@ -2325,7 +2325,7 @@
       <c r="A41" s="12"/>
       <c r="B41" s="15"/>
       <c r="C41" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D41" s="4">
         <v>3.0461</v>
@@ -2634,7 +2634,7 @@
       <c r="A3" s="12"/>
       <c r="B3" s="15"/>
       <c r="C3" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D3" s="4">
         <v>17.216999999999999</v>
@@ -2674,7 +2674,7 @@
       <c r="A4" s="12"/>
       <c r="B4" s="15"/>
       <c r="C4" s="8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D4" s="4">
         <v>5.6908000000000003</v>
@@ -2762,7 +2762,7 @@
       <c r="A15" s="12"/>
       <c r="B15" s="15"/>
       <c r="C15" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D15" s="4">
         <v>31.327000000000002</v>
@@ -2802,7 +2802,7 @@
       <c r="A16" s="12"/>
       <c r="B16" s="15"/>
       <c r="C16" s="8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D16" s="4">
         <v>22.393000000000001</v>
@@ -2930,7 +2930,7 @@
       <c r="A28" s="12"/>
       <c r="B28" s="15"/>
       <c r="C28" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D28" s="4">
         <v>10.692</v>
@@ -2970,7 +2970,7 @@
       <c r="A29" s="12"/>
       <c r="B29" s="15"/>
       <c r="C29" s="8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D29" s="4">
         <v>11.2</v>
@@ -3054,7 +3054,7 @@
       <c r="A39" s="12"/>
       <c r="B39" s="15"/>
       <c r="C39" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D39" s="4">
         <v>4.8238000000000003</v>
@@ -3094,7 +3094,7 @@
       <c r="A40" s="12"/>
       <c r="B40" s="15"/>
       <c r="C40" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D40" s="4">
         <v>7.1036999999999999</v>
@@ -3134,7 +3134,7 @@
       <c r="A41" s="12"/>
       <c r="B41" s="15"/>
       <c r="C41" s="8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D41" s="4">
         <v>3.0461</v>

</xml_diff>

<commit_message>
Changed parameters to evpwd model
</commit_message>
<xml_diff>
--- a/scripts/__other__/__sem__.xlsx
+++ b/scripts/__other__/__sem__.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Janzen\Desktop\code\moga_neml\scripts\__other__\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8CE690E-75C1-40F0-BC54-29532D442EAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6201E7D5-D366-48F1-88C1-88F97E9CADDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="15600" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="evp" sheetId="13" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="45">
   <si>
     <t>temp</t>
   </si>
@@ -167,6 +167,12 @@
   </si>
   <si>
     <t>8; 8</t>
+  </si>
+  <si>
+    <t>9; 9</t>
+  </si>
+  <si>
+    <t>7; 7</t>
   </si>
 </sst>
 </file>
@@ -1814,9 +1820,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE483CC8-AF2C-4D5A-AEE5-EF7DF4EC0883}">
   <dimension ref="A1:T73"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J20" sqref="J20"/>
+      <selection pane="bottomLeft" activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1906,7 +1912,7 @@
       <c r="A3" s="12"/>
       <c r="B3" s="15"/>
       <c r="C3" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D3" s="4">
         <v>17.216999999999999</v>
@@ -1924,13 +1930,13 @@
         <v>1783.5</v>
       </c>
       <c r="I3" s="2">
-        <v>1889.7</v>
+        <v>2778.6</v>
       </c>
       <c r="J3" s="2">
-        <v>5.5457000000000001</v>
+        <v>4.9512</v>
       </c>
       <c r="K3" s="2">
-        <v>6.5846</v>
+        <v>6.3958000000000004</v>
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
@@ -2126,7 +2132,7 @@
       <c r="A27" s="12"/>
       <c r="B27" s="15"/>
       <c r="C27" s="8" t="s">
-        <v>33</v>
+        <v>43</v>
       </c>
       <c r="D27" s="4">
         <v>4.8710000000000004</v>
@@ -2143,14 +2149,14 @@
       <c r="H27" s="4">
         <v>1138.3</v>
       </c>
-      <c r="I27" s="4">
-        <v>5825.6</v>
-      </c>
-      <c r="J27" s="4">
-        <v>3.4992000000000001</v>
-      </c>
-      <c r="K27" s="3">
-        <v>7.5202</v>
+      <c r="I27" s="2">
+        <v>1899.3</v>
+      </c>
+      <c r="J27" s="2">
+        <v>4.4973999999999998</v>
+      </c>
+      <c r="K27" s="2">
+        <v>9.6201000000000008</v>
       </c>
     </row>
     <row r="28" spans="1:20" x14ac:dyDescent="0.25">
@@ -2188,7 +2194,7 @@
       <c r="A29" s="12"/>
       <c r="B29" s="15"/>
       <c r="C29" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D29" s="4">
         <v>11.2</v>
@@ -2206,13 +2212,13 @@
         <v>1163</v>
       </c>
       <c r="I29" s="2">
-        <v>1730.2</v>
+        <v>1703.2</v>
       </c>
       <c r="J29" s="2">
-        <v>4.5327000000000002</v>
+        <v>4.5818000000000003</v>
       </c>
       <c r="K29" s="2">
-        <v>7.9908000000000001</v>
+        <v>9.0646000000000004</v>
       </c>
     </row>
     <row r="30" spans="1:20" x14ac:dyDescent="0.25">
@@ -2281,13 +2287,13 @@
         <v>1006.9</v>
       </c>
       <c r="I39" s="4">
-        <v>1762.8</v>
+        <v>1532</v>
       </c>
       <c r="J39" s="4">
-        <v>4.5347</v>
+        <v>4.6818</v>
       </c>
       <c r="K39" s="3">
-        <v>7.3331</v>
+        <v>6.5256999999999996</v>
       </c>
     </row>
     <row r="40" spans="1:20" x14ac:dyDescent="0.25">
@@ -2524,9 +2530,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C18A26E-30CA-4E63-A18A-C9C101DAF33C}">
   <dimension ref="A1:Z73"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C3" sqref="C3:C41"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2634,7 +2640,7 @@
       <c r="A3" s="12"/>
       <c r="B3" s="15"/>
       <c r="C3" s="8" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="D3" s="4">
         <v>17.216999999999999</v>
@@ -2652,22 +2658,22 @@
         <v>1783.5</v>
       </c>
       <c r="I3" s="2">
-        <v>2.2067000000000001</v>
+        <v>1.4998</v>
       </c>
       <c r="J3" s="2">
-        <v>0.48282999999999998</v>
+        <v>0.64100999999999997</v>
       </c>
       <c r="K3" s="2">
-        <v>4.1563999999999997</v>
+        <v>5.4347000000000003</v>
       </c>
       <c r="L3" s="2">
-        <v>4.4695</v>
+        <v>1.7194</v>
       </c>
       <c r="M3" s="2">
-        <v>8.2167000000000004E-3</v>
+        <v>0.30907000000000001</v>
       </c>
       <c r="N3" s="2">
-        <v>2.5705</v>
+        <v>3.3214999999999999</v>
       </c>
     </row>
     <row r="4" spans="1:26" x14ac:dyDescent="0.25">
@@ -2762,7 +2768,7 @@
       <c r="A15" s="12"/>
       <c r="B15" s="15"/>
       <c r="C15" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D15" s="4">
         <v>31.327000000000002</v>
@@ -2783,26 +2789,26 @@
         <v>1.6236999999999999</v>
       </c>
       <c r="J15" s="4">
-        <v>0.26358999999999999</v>
+        <v>0.39095000000000002</v>
       </c>
       <c r="K15" s="4">
-        <v>3.1652</v>
+        <v>3.8603999999999998</v>
       </c>
       <c r="L15" s="4">
-        <v>1.7229000000000001</v>
+        <v>3.4752999999999998</v>
       </c>
       <c r="M15" s="4">
-        <v>0.52891999999999995</v>
+        <v>0.11533</v>
       </c>
       <c r="N15" s="3">
-        <v>0.28255999999999998</v>
+        <v>2.5640000000000001</v>
       </c>
     </row>
     <row r="16" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A16" s="12"/>
       <c r="B16" s="15"/>
       <c r="C16" s="8" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="D16" s="4">
         <v>22.393000000000001</v>
@@ -2820,22 +2826,22 @@
         <v>1828.1</v>
       </c>
       <c r="I16" s="4">
-        <v>2.0305</v>
+        <v>2.0705</v>
       </c>
       <c r="J16" s="4">
-        <v>0.26046999999999998</v>
+        <v>0.52429999999999999</v>
       </c>
       <c r="K16" s="4">
-        <v>3.0701000000000001</v>
+        <v>4.4337</v>
       </c>
       <c r="L16" s="4">
-        <v>4.7169999999999996</v>
+        <v>5.2408999999999999</v>
       </c>
       <c r="M16" s="4">
-        <v>0.15376000000000001</v>
+        <v>3.4408000000000001E-2</v>
       </c>
       <c r="N16" s="3">
-        <v>2.6135999999999999</v>
+        <v>2.3807999999999998</v>
       </c>
     </row>
     <row r="17" spans="1:26" x14ac:dyDescent="0.25">
@@ -2970,7 +2976,7 @@
       <c r="A29" s="12"/>
       <c r="B29" s="15"/>
       <c r="C29" s="8" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="D29" s="4">
         <v>11.2</v>
@@ -3134,7 +3140,7 @@
       <c r="A41" s="12"/>
       <c r="B41" s="15"/>
       <c r="C41" s="8" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="D41" s="4">
         <v>3.0461</v>
@@ -3152,22 +3158,22 @@
         <v>2022.3</v>
       </c>
       <c r="I41" s="2">
-        <v>2.8746999999999998</v>
+        <v>1.9328000000000001</v>
       </c>
       <c r="J41" s="2">
-        <v>0.35838999999999999</v>
+        <v>0.59299999999999997</v>
       </c>
       <c r="K41" s="2">
-        <v>3.0428999999999999</v>
+        <v>4.7255000000000003</v>
       </c>
       <c r="L41" s="2">
-        <v>9.1083999999999996</v>
+        <v>2.6515</v>
       </c>
       <c r="M41" s="2">
-        <v>7.6354000000000005E-2</v>
+        <v>0.25479000000000002</v>
       </c>
       <c r="N41" s="2">
-        <v>2.1876000000000002</v>
+        <v>2.5724</v>
       </c>
     </row>
     <row r="42" spans="1:26" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Changed parameters to evpcd model
</commit_message>
<xml_diff>
--- a/scripts/__other__/__sem__.xlsx
+++ b/scripts/__other__/__sem__.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Janzen\Desktop\code\moga_neml\scripts\__other__\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6201E7D5-D366-48F1-88C1-88F97E9CADDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0061927F-723F-4092-9BD2-D6870FA64542}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="15600" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="evp" sheetId="13" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="41">
   <si>
     <t>temp</t>
   </si>
@@ -139,28 +139,16 @@
     <t>8; 7</t>
   </si>
   <si>
-    <t>8; 6</t>
-  </si>
-  <si>
     <t>6; 7</t>
   </si>
   <si>
     <t>7; 6</t>
   </si>
   <si>
-    <t>7; 5</t>
-  </si>
-  <si>
     <t>7; 9</t>
   </si>
   <si>
     <t>7; 8</t>
-  </si>
-  <si>
-    <t>6; 8</t>
-  </si>
-  <si>
-    <t>5; 10</t>
   </si>
   <si>
     <t>5; 8</t>
@@ -355,6 +343,539 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>91110</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>52224</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>157370</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>184745</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F0F901CE-1434-B384-7F73-CFA7D97B9B3D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7537175" y="242724"/>
+          <a:ext cx="1904999" cy="1904999"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>140806</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>55084</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>196802</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>177341</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{04ED5CA5-5DE3-9849-0C0A-E308227FE011}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9425610" y="245584"/>
+          <a:ext cx="1894735" cy="1894735"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>49697</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>38684</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>115958</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>171206</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{48B2C33C-EE1B-BE9F-8E6D-A431558E4B96}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7495762" y="2250141"/>
+          <a:ext cx="1905000" cy="1905000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>115959</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>50347</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>182222</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>182871</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5B1D8717-2C25-526A-5E72-1C31CF079EF3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9400763" y="2261804"/>
+          <a:ext cx="1905002" cy="1905002"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>56793</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>49159</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>149088</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>17215</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8C257DB0-555A-73C5-3B81-7069D962C0A2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7502858" y="4281572"/>
+          <a:ext cx="1931034" cy="1931034"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>157372</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>47782</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>258461</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>24632</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Picture 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{56307D0B-D72F-5816-98E6-F87F6C0734A7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9442176" y="4280195"/>
+          <a:ext cx="1939828" cy="1939828"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>69809</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>50057</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>152170</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>8179</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Picture 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BA886998-B57F-CD0F-41AB-D9F969D1F9E9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7515874" y="6303427"/>
+          <a:ext cx="1921100" cy="1921100"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>149087</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>56062</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>240196</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>22932</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Picture 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8D1F3CBC-D163-4B80-A0A6-CAD68A079AC2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9433891" y="6309432"/>
+          <a:ext cx="1929848" cy="1929848"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>182217</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>49698</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>323021</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>186362</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="10" name="Picture 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{60E02592-69E5-5340-EA44-6900EE49FFD7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11305760" y="240198"/>
+          <a:ext cx="3818283" cy="1909142"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>198784</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>41415</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>331301</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>173935</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="11" name="Picture 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6E13AFE2-FE68-0998-7EDB-B7915E90A03E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11322327" y="2252872"/>
+          <a:ext cx="3809996" cy="1904998"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>231914</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>41412</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>401248</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>190499</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="12" name="Picture 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FC7F3F7B-E7BE-D52A-4508-858F51AD5EED}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11355457" y="4273825"/>
+          <a:ext cx="3846813" cy="1921565"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>238125</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>409575</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="13" name="Picture 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8327A454-9110-1BC4-6A15-6937729DA59A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId12"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11306175" y="6305550"/>
+          <a:ext cx="3829050" cy="1914525"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -624,7 +1145,7 @@
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G19" sqref="G19"/>
+      <selection pane="bottomLeft" activeCell="D1" sqref="D1:H1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -700,10 +1221,10 @@
         <v>1783.5</v>
       </c>
       <c r="I3" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J3" s="8" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -728,10 +1249,10 @@
         <v>1621.6</v>
       </c>
       <c r="I4" s="8" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
       <c r="J4" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -951,7 +1472,7 @@
         <v>20</v>
       </c>
       <c r="J15" s="8" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
@@ -976,10 +1497,10 @@
         <v>1828.1</v>
       </c>
       <c r="I16" s="8" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="J16" s="8" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
@@ -1196,7 +1717,7 @@
         <v>1138.3</v>
       </c>
       <c r="I27" s="8" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="J27" s="8" t="s">
         <v>23</v>
@@ -1227,7 +1748,7 @@
         <v>20</v>
       </c>
       <c r="J28" s="8" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
@@ -1252,7 +1773,7 @@
         <v>1163</v>
       </c>
       <c r="I29" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J29" s="8" t="s">
         <v>39</v>
@@ -1453,7 +1974,7 @@
         <v>26</v>
       </c>
       <c r="J39" s="8" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="K39" s="2"/>
       <c r="L39" s="2"/>
@@ -1486,7 +2007,7 @@
         <v>30</v>
       </c>
       <c r="J40" s="8" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="K40" s="2"/>
       <c r="L40" s="2"/>
@@ -1516,10 +2037,10 @@
         <v>2022.3</v>
       </c>
       <c r="I41" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="J41" s="8" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="42" spans="1:15" x14ac:dyDescent="0.25">
@@ -1548,7 +2069,7 @@
       <c r="A43" s="12"/>
       <c r="B43" s="15"/>
       <c r="C43" s="8" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="D43" s="2">
         <v>16.286999999999999</v>
@@ -1798,21 +2319,22 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A2:A13"/>
+    <mergeCell ref="B2:B13"/>
+    <mergeCell ref="A14:A25"/>
+    <mergeCell ref="B14:B25"/>
+    <mergeCell ref="A26:A37"/>
+    <mergeCell ref="B26:B37"/>
     <mergeCell ref="A38:A49"/>
     <mergeCell ref="B38:B49"/>
     <mergeCell ref="A50:A61"/>
     <mergeCell ref="B50:B61"/>
     <mergeCell ref="A62:A73"/>
     <mergeCell ref="B62:B73"/>
-    <mergeCell ref="A2:A13"/>
-    <mergeCell ref="B2:B13"/>
-    <mergeCell ref="A14:A25"/>
-    <mergeCell ref="B14:B25"/>
-    <mergeCell ref="A26:A37"/>
-    <mergeCell ref="B26:B37"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -1820,9 +2342,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE483CC8-AF2C-4D5A-AEE5-EF7DF4EC0883}">
   <dimension ref="A1:T73"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J18" sqref="J18"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C42" sqref="C42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1973,34 +2495,166 @@
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" s="12"/>
       <c r="B5" s="15"/>
+      <c r="C5" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" s="4">
+        <v>9.3076000000000008</v>
+      </c>
+      <c r="E5" s="4">
+        <v>32.595999999999997</v>
+      </c>
+      <c r="F5" s="4">
+        <v>5.8113999999999999</v>
+      </c>
+      <c r="G5" s="4">
+        <v>4.5263</v>
+      </c>
+      <c r="H5" s="4">
+        <v>1775.9</v>
+      </c>
+      <c r="I5" s="4">
+        <v>3171.9</v>
+      </c>
+      <c r="J5" s="4">
+        <v>4.7907999999999999</v>
+      </c>
+      <c r="K5" s="3">
+        <v>6.8902999999999999</v>
+      </c>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" s="12"/>
       <c r="B6" s="15"/>
+      <c r="D6" s="4">
+        <v>5.8951000000000002</v>
+      </c>
+      <c r="E6" s="4">
+        <v>36.244999999999997</v>
+      </c>
+      <c r="F6" s="4">
+        <v>5.3757000000000001</v>
+      </c>
+      <c r="G6" s="4">
+        <v>4.7310999999999996</v>
+      </c>
+      <c r="H6" s="4">
+        <v>1598.4</v>
+      </c>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" s="12"/>
       <c r="B7" s="15"/>
+      <c r="D7" s="4">
+        <v>4.1862000000000004</v>
+      </c>
+      <c r="E7" s="4">
+        <v>84.548000000000002</v>
+      </c>
+      <c r="F7" s="4">
+        <v>2.1122999999999998</v>
+      </c>
+      <c r="G7" s="4">
+        <v>4.7751999999999999</v>
+      </c>
+      <c r="H7" s="4">
+        <v>1574.3</v>
+      </c>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" s="12"/>
       <c r="B8" s="15"/>
+      <c r="D8" s="4">
+        <v>25.038</v>
+      </c>
+      <c r="E8" s="4">
+        <v>90.692999999999998</v>
+      </c>
+      <c r="F8" s="4">
+        <v>0.61002000000000001</v>
+      </c>
+      <c r="G8" s="4">
+        <v>4.1981999999999999</v>
+      </c>
+      <c r="H8" s="4">
+        <v>1944.6</v>
+      </c>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" s="12"/>
       <c r="B9" s="15"/>
+      <c r="D9" s="4">
+        <v>27.547000000000001</v>
+      </c>
+      <c r="E9" s="4">
+        <v>78.081000000000003</v>
+      </c>
+      <c r="F9" s="4">
+        <v>0.84272999999999998</v>
+      </c>
+      <c r="G9" s="4">
+        <v>3.8992</v>
+      </c>
+      <c r="H9" s="4">
+        <v>2454.8000000000002</v>
+      </c>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10" s="12"/>
       <c r="B10" s="15"/>
+      <c r="D10" s="4">
+        <v>27.885000000000002</v>
+      </c>
+      <c r="E10" s="4">
+        <v>124.89</v>
+      </c>
+      <c r="F10" s="4">
+        <v>0.65636000000000005</v>
+      </c>
+      <c r="G10" s="4">
+        <v>3.8874</v>
+      </c>
+      <c r="H10" s="4">
+        <v>2390.5</v>
+      </c>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11" s="12"/>
       <c r="B11" s="15"/>
+      <c r="D11" s="4">
+        <v>19.2</v>
+      </c>
+      <c r="E11" s="4">
+        <v>52.204000000000001</v>
+      </c>
+      <c r="F11" s="4">
+        <v>1.7579</v>
+      </c>
+      <c r="G11" s="4">
+        <v>4.5105000000000004</v>
+      </c>
+      <c r="H11" s="4">
+        <v>1614.6</v>
+      </c>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12" s="12"/>
       <c r="B12" s="15"/>
+      <c r="D12" s="4">
+        <v>8.5922999999999998</v>
+      </c>
+      <c r="E12" s="4">
+        <v>38.904000000000003</v>
+      </c>
+      <c r="F12" s="4">
+        <v>5.4828999999999999</v>
+      </c>
+      <c r="G12" s="4">
+        <v>4.4794999999999998</v>
+      </c>
+      <c r="H12" s="4">
+        <v>1841</v>
+      </c>
     </row>
     <row r="13" spans="1:20" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="13"/>
@@ -2083,34 +2737,166 @@
     <row r="17" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A17" s="12"/>
       <c r="B17" s="15"/>
+      <c r="C17" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="D17" s="4">
+        <v>11.45</v>
+      </c>
+      <c r="E17" s="4">
+        <v>53.151000000000003</v>
+      </c>
+      <c r="F17" s="4">
+        <v>7.1665999999999999</v>
+      </c>
+      <c r="G17" s="4">
+        <v>3.9502000000000002</v>
+      </c>
+      <c r="H17" s="4">
+        <v>2221.6</v>
+      </c>
+      <c r="I17" s="4">
+        <v>4328.7</v>
+      </c>
+      <c r="J17" s="4">
+        <v>4.3678999999999997</v>
+      </c>
+      <c r="K17" s="3">
+        <v>5.3108000000000004</v>
+      </c>
     </row>
     <row r="18" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A18" s="12"/>
       <c r="B18" s="15"/>
+      <c r="D18" s="4">
+        <v>37.741999999999997</v>
+      </c>
+      <c r="E18" s="4">
+        <v>49.122999999999998</v>
+      </c>
+      <c r="F18" s="4">
+        <v>2.4996</v>
+      </c>
+      <c r="G18" s="4">
+        <v>3.4102000000000001</v>
+      </c>
+      <c r="H18" s="4">
+        <v>3172</v>
+      </c>
     </row>
     <row r="19" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A19" s="12"/>
       <c r="B19" s="15"/>
+      <c r="D19" s="4">
+        <v>18.768000000000001</v>
+      </c>
+      <c r="E19" s="4">
+        <v>89.18</v>
+      </c>
+      <c r="F19" s="4">
+        <v>0.88068999999999997</v>
+      </c>
+      <c r="G19" s="4">
+        <v>4.5054999999999996</v>
+      </c>
+      <c r="H19" s="4">
+        <v>1677.4</v>
+      </c>
     </row>
     <row r="20" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A20" s="12"/>
       <c r="B20" s="15"/>
+      <c r="D20" s="4">
+        <v>23.303999999999998</v>
+      </c>
+      <c r="E20" s="4">
+        <v>306.58</v>
+      </c>
+      <c r="F20" s="4">
+        <v>0.32123000000000002</v>
+      </c>
+      <c r="G20" s="4">
+        <v>4.2591999999999999</v>
+      </c>
+      <c r="H20" s="4">
+        <v>1822.6</v>
+      </c>
     </row>
     <row r="21" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A21" s="12"/>
       <c r="B21" s="15"/>
+      <c r="D21" s="4">
+        <v>31.137</v>
+      </c>
+      <c r="E21" s="4">
+        <v>31.413</v>
+      </c>
+      <c r="F21" s="4">
+        <v>4.6002999999999998</v>
+      </c>
+      <c r="G21" s="4">
+        <v>3.6958000000000002</v>
+      </c>
+      <c r="H21" s="4">
+        <v>2583</v>
+      </c>
     </row>
     <row r="22" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A22" s="12"/>
       <c r="B22" s="15"/>
+      <c r="D22" s="4">
+        <v>29.725999999999999</v>
+      </c>
+      <c r="E22" s="4">
+        <v>45.991</v>
+      </c>
+      <c r="F22" s="4">
+        <v>2.3174000000000001</v>
+      </c>
+      <c r="G22" s="4">
+        <v>3.9613</v>
+      </c>
+      <c r="H22" s="4">
+        <v>2101.3000000000002</v>
+      </c>
     </row>
     <row r="23" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A23" s="12"/>
       <c r="B23" s="15"/>
+      <c r="D23" s="4">
+        <v>0.85682000000000003</v>
+      </c>
+      <c r="E23" s="4">
+        <v>42.524000000000001</v>
+      </c>
+      <c r="F23" s="4">
+        <v>9.6282999999999994</v>
+      </c>
+      <c r="G23" s="4">
+        <v>4.5033000000000003</v>
+      </c>
+      <c r="H23" s="4">
+        <v>1707</v>
+      </c>
     </row>
     <row r="24" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A24" s="12"/>
       <c r="B24" s="15"/>
+      <c r="D24" s="4">
+        <v>4.4611000000000001</v>
+      </c>
+      <c r="E24" s="4">
+        <v>35.628</v>
+      </c>
+      <c r="F24" s="4">
+        <v>31.021000000000001</v>
+      </c>
+      <c r="G24" s="4">
+        <v>3.6185999999999998</v>
+      </c>
+      <c r="H24" s="4">
+        <v>3016.2</v>
+      </c>
     </row>
     <row r="25" spans="1:20" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="13"/>
@@ -2132,7 +2918,7 @@
       <c r="A27" s="12"/>
       <c r="B27" s="15"/>
       <c r="C27" s="8" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="D27" s="4">
         <v>4.8710000000000004</v>
@@ -2224,30 +3010,147 @@
     <row r="30" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A30" s="12"/>
       <c r="B30" s="15"/>
+      <c r="C30" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D30" s="4">
+        <v>11.208</v>
+      </c>
+      <c r="E30" s="4">
+        <v>16.738</v>
+      </c>
+      <c r="F30" s="4">
+        <v>5.9587000000000003</v>
+      </c>
+      <c r="G30" s="4">
+        <v>3.6377000000000002</v>
+      </c>
+      <c r="H30" s="4">
+        <v>1530.1</v>
+      </c>
+      <c r="I30" s="4">
+        <v>2070.1999999999998</v>
+      </c>
+      <c r="J30" s="4">
+        <v>4.3163999999999998</v>
+      </c>
+      <c r="K30" s="3">
+        <v>7.4964000000000004</v>
+      </c>
     </row>
     <row r="31" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A31" s="12"/>
       <c r="B31" s="15"/>
+      <c r="D31" s="4">
+        <v>10.45</v>
+      </c>
+      <c r="E31" s="4">
+        <v>14.769</v>
+      </c>
+      <c r="F31" s="4">
+        <v>7.8792</v>
+      </c>
+      <c r="G31" s="4">
+        <v>3.54</v>
+      </c>
+      <c r="H31" s="4">
+        <v>1787.3</v>
+      </c>
     </row>
     <row r="32" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A32" s="12"/>
       <c r="B32" s="15"/>
+      <c r="D32" s="4">
+        <v>11.010999999999999</v>
+      </c>
+      <c r="E32" s="4">
+        <v>11.071</v>
+      </c>
+      <c r="F32" s="4">
+        <v>13.523</v>
+      </c>
+      <c r="G32" s="4">
+        <v>3.5672000000000001</v>
+      </c>
+      <c r="H32" s="4">
+        <v>1593.8</v>
+      </c>
     </row>
     <row r="33" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A33" s="12"/>
       <c r="B33" s="15"/>
+      <c r="D33" s="4">
+        <v>5.6656000000000004</v>
+      </c>
+      <c r="E33" s="4">
+        <v>8.2222000000000008</v>
+      </c>
+      <c r="F33" s="4">
+        <v>14.47</v>
+      </c>
+      <c r="G33" s="4">
+        <v>4.3000999999999996</v>
+      </c>
+      <c r="H33" s="4">
+        <v>1000.8</v>
+      </c>
     </row>
     <row r="34" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A34" s="12"/>
       <c r="B34" s="15"/>
+      <c r="D34" s="4">
+        <v>15.185</v>
+      </c>
+      <c r="E34" s="4">
+        <v>64.875</v>
+      </c>
+      <c r="F34" s="4">
+        <v>1.4525999999999999</v>
+      </c>
+      <c r="G34" s="4">
+        <v>3.2002999999999999</v>
+      </c>
+      <c r="H34" s="4">
+        <v>2110.6</v>
+      </c>
     </row>
     <row r="35" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A35" s="12"/>
       <c r="B35" s="15"/>
+      <c r="D35" s="4">
+        <v>8.0571999999999999</v>
+      </c>
+      <c r="E35" s="4">
+        <v>29.803999999999998</v>
+      </c>
+      <c r="F35" s="4">
+        <v>2.5836000000000001</v>
+      </c>
+      <c r="G35" s="4">
+        <v>4.0204000000000004</v>
+      </c>
+      <c r="H35" s="4">
+        <v>1210.4000000000001</v>
+      </c>
     </row>
     <row r="36" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A36" s="12"/>
       <c r="B36" s="15"/>
+      <c r="D36" s="4">
+        <v>7.5292000000000003</v>
+      </c>
+      <c r="E36" s="4">
+        <v>23.504999999999999</v>
+      </c>
+      <c r="F36" s="4">
+        <v>4.9898999999999996</v>
+      </c>
+      <c r="G36" s="4">
+        <v>3.8622999999999998</v>
+      </c>
+      <c r="H36" s="4">
+        <v>1369.1</v>
+      </c>
     </row>
     <row r="37" spans="1:20" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="13"/>
@@ -2331,7 +3234,7 @@
       <c r="A41" s="12"/>
       <c r="B41" s="15"/>
       <c r="C41" s="8" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D41" s="4">
         <v>3.0461</v>
@@ -2349,42 +3252,147 @@
         <v>2022.3</v>
       </c>
       <c r="I41" s="2">
-        <v>2563.4</v>
+        <v>2114.8000000000002</v>
       </c>
       <c r="J41" s="2">
-        <v>4.2545000000000002</v>
+        <v>4.4790000000000001</v>
       </c>
       <c r="K41" s="2">
-        <v>13.452999999999999</v>
+        <v>13.782999999999999</v>
       </c>
     </row>
     <row r="42" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A42" s="12"/>
       <c r="B42" s="15"/>
+      <c r="D42" s="4">
+        <v>4.6340000000000003</v>
+      </c>
+      <c r="E42" s="4">
+        <v>18.606999999999999</v>
+      </c>
+      <c r="F42" s="4">
+        <v>24.896000000000001</v>
+      </c>
+      <c r="G42" s="4">
+        <v>3.3435999999999999</v>
+      </c>
+      <c r="H42" s="4">
+        <v>1999.7</v>
+      </c>
     </row>
     <row r="43" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A43" s="12"/>
       <c r="B43" s="15"/>
+      <c r="D43" s="4">
+        <v>16.286999999999999</v>
+      </c>
+      <c r="E43" s="4">
+        <v>181.45</v>
+      </c>
+      <c r="F43" s="4">
+        <v>0.52517000000000003</v>
+      </c>
+      <c r="G43" s="4">
+        <v>3.0160999999999998</v>
+      </c>
+      <c r="H43" s="4">
+        <v>2606.1999999999998</v>
+      </c>
     </row>
     <row r="44" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A44" s="12"/>
       <c r="B44" s="15"/>
+      <c r="D44" s="4">
+        <v>9.5312999999999999</v>
+      </c>
+      <c r="E44" s="4">
+        <v>148.61000000000001</v>
+      </c>
+      <c r="F44" s="4">
+        <v>0.37484000000000001</v>
+      </c>
+      <c r="G44" s="4">
+        <v>3.9621</v>
+      </c>
+      <c r="H44" s="4">
+        <v>1253.9000000000001</v>
+      </c>
     </row>
     <row r="45" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A45" s="12"/>
       <c r="B45" s="15"/>
+      <c r="D45" s="4">
+        <v>6.3647</v>
+      </c>
+      <c r="E45" s="4">
+        <v>149.54</v>
+      </c>
+      <c r="F45" s="4">
+        <v>0.43913000000000002</v>
+      </c>
+      <c r="G45" s="4">
+        <v>4.1839000000000004</v>
+      </c>
+      <c r="H45" s="4">
+        <v>1127.5999999999999</v>
+      </c>
     </row>
     <row r="46" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A46" s="12"/>
       <c r="B46" s="15"/>
+      <c r="D46" s="4">
+        <v>12.622</v>
+      </c>
+      <c r="E46" s="4">
+        <v>15.441000000000001</v>
+      </c>
+      <c r="F46" s="4">
+        <v>4.5385999999999997</v>
+      </c>
+      <c r="G46" s="4">
+        <v>3.7305000000000001</v>
+      </c>
+      <c r="H46" s="4">
+        <v>1371.6</v>
+      </c>
     </row>
     <row r="47" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A47" s="12"/>
       <c r="B47" s="15"/>
+      <c r="D47" s="4">
+        <v>12.256</v>
+      </c>
+      <c r="E47" s="4">
+        <v>273.68</v>
+      </c>
+      <c r="F47" s="4">
+        <v>0.20866000000000001</v>
+      </c>
+      <c r="G47" s="4">
+        <v>3.8422000000000001</v>
+      </c>
+      <c r="H47" s="4">
+        <v>1242.3</v>
+      </c>
     </row>
     <row r="48" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A48" s="12"/>
       <c r="B48" s="15"/>
+      <c r="D48" s="4">
+        <v>7.0439999999999996</v>
+      </c>
+      <c r="E48" s="4">
+        <v>16.175000000000001</v>
+      </c>
+      <c r="F48" s="4">
+        <v>6.7949000000000002</v>
+      </c>
+      <c r="G48" s="4">
+        <v>4.1207000000000003</v>
+      </c>
+      <c r="H48" s="4">
+        <v>1090</v>
+      </c>
     </row>
     <row r="49" spans="1:20" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="13"/>
@@ -2508,18 +3516,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A2:A13"/>
+    <mergeCell ref="B2:B13"/>
+    <mergeCell ref="A14:A25"/>
+    <mergeCell ref="B14:B25"/>
+    <mergeCell ref="A26:A37"/>
+    <mergeCell ref="B26:B37"/>
     <mergeCell ref="A38:A49"/>
     <mergeCell ref="B38:B49"/>
     <mergeCell ref="A50:A61"/>
     <mergeCell ref="B50:B61"/>
     <mergeCell ref="A62:A73"/>
     <mergeCell ref="B62:B73"/>
-    <mergeCell ref="A2:A13"/>
-    <mergeCell ref="B2:B13"/>
-    <mergeCell ref="A14:A25"/>
-    <mergeCell ref="B14:B25"/>
-    <mergeCell ref="A26:A37"/>
-    <mergeCell ref="B26:B37"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -2530,9 +3538,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C18A26E-30CA-4E63-A18A-C9C101DAF33C}">
   <dimension ref="A1:Z73"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C4" sqref="C4"/>
+      <selection pane="bottomLeft" activeCell="I43" sqref="I43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2640,7 +3648,7 @@
       <c r="A3" s="12"/>
       <c r="B3" s="15"/>
       <c r="C3" s="8" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="D3" s="4">
         <v>17.216999999999999</v>
@@ -2680,7 +3688,7 @@
       <c r="A4" s="12"/>
       <c r="B4" s="15"/>
       <c r="C4" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D4" s="4">
         <v>5.6908000000000003</v>
@@ -2719,34 +3727,154 @@
     <row r="5" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A5" s="12"/>
       <c r="B5" s="15"/>
+      <c r="D5" s="4">
+        <v>9.3076000000000008</v>
+      </c>
+      <c r="E5" s="4">
+        <v>32.595999999999997</v>
+      </c>
+      <c r="F5" s="4">
+        <v>5.8113999999999999</v>
+      </c>
+      <c r="G5" s="4">
+        <v>4.5263</v>
+      </c>
+      <c r="H5" s="4">
+        <v>1775.9</v>
+      </c>
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A6" s="12"/>
       <c r="B6" s="15"/>
+      <c r="D6" s="4">
+        <v>5.8951000000000002</v>
+      </c>
+      <c r="E6" s="4">
+        <v>36.244999999999997</v>
+      </c>
+      <c r="F6" s="4">
+        <v>5.3757000000000001</v>
+      </c>
+      <c r="G6" s="4">
+        <v>4.7310999999999996</v>
+      </c>
+      <c r="H6" s="4">
+        <v>1598.4</v>
+      </c>
     </row>
     <row r="7" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A7" s="12"/>
       <c r="B7" s="15"/>
+      <c r="D7" s="4">
+        <v>4.1862000000000004</v>
+      </c>
+      <c r="E7" s="4">
+        <v>84.548000000000002</v>
+      </c>
+      <c r="F7" s="4">
+        <v>2.1122999999999998</v>
+      </c>
+      <c r="G7" s="4">
+        <v>4.7751999999999999</v>
+      </c>
+      <c r="H7" s="4">
+        <v>1574.3</v>
+      </c>
     </row>
     <row r="8" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A8" s="12"/>
       <c r="B8" s="15"/>
+      <c r="D8" s="4">
+        <v>25.038</v>
+      </c>
+      <c r="E8" s="4">
+        <v>90.692999999999998</v>
+      </c>
+      <c r="F8" s="4">
+        <v>0.61002000000000001</v>
+      </c>
+      <c r="G8" s="4">
+        <v>4.1981999999999999</v>
+      </c>
+      <c r="H8" s="4">
+        <v>1944.6</v>
+      </c>
     </row>
     <row r="9" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A9" s="12"/>
       <c r="B9" s="15"/>
+      <c r="D9" s="4">
+        <v>27.547000000000001</v>
+      </c>
+      <c r="E9" s="4">
+        <v>78.081000000000003</v>
+      </c>
+      <c r="F9" s="4">
+        <v>0.84272999999999998</v>
+      </c>
+      <c r="G9" s="4">
+        <v>3.8992</v>
+      </c>
+      <c r="H9" s="4">
+        <v>2454.8000000000002</v>
+      </c>
     </row>
     <row r="10" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A10" s="12"/>
       <c r="B10" s="15"/>
+      <c r="D10" s="4">
+        <v>27.885000000000002</v>
+      </c>
+      <c r="E10" s="4">
+        <v>124.89</v>
+      </c>
+      <c r="F10" s="4">
+        <v>0.65636000000000005</v>
+      </c>
+      <c r="G10" s="4">
+        <v>3.8874</v>
+      </c>
+      <c r="H10" s="4">
+        <v>2390.5</v>
+      </c>
     </row>
     <row r="11" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A11" s="12"/>
       <c r="B11" s="15"/>
+      <c r="D11" s="4">
+        <v>19.2</v>
+      </c>
+      <c r="E11" s="4">
+        <v>52.204000000000001</v>
+      </c>
+      <c r="F11" s="4">
+        <v>1.7579</v>
+      </c>
+      <c r="G11" s="4">
+        <v>4.5105000000000004</v>
+      </c>
+      <c r="H11" s="4">
+        <v>1614.6</v>
+      </c>
     </row>
     <row r="12" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A12" s="12"/>
       <c r="B12" s="15"/>
+      <c r="D12" s="4">
+        <v>8.5922999999999998</v>
+      </c>
+      <c r="E12" s="4">
+        <v>38.904000000000003</v>
+      </c>
+      <c r="F12" s="4">
+        <v>5.4828999999999999</v>
+      </c>
+      <c r="G12" s="4">
+        <v>4.4794999999999998</v>
+      </c>
+      <c r="H12" s="4">
+        <v>1841</v>
+      </c>
     </row>
     <row r="13" spans="1:26" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="13"/>
@@ -2768,7 +3896,7 @@
       <c r="A15" s="12"/>
       <c r="B15" s="15"/>
       <c r="C15" s="8" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="D15" s="4">
         <v>31.327000000000002</v>
@@ -2808,7 +3936,7 @@
       <c r="A16" s="12"/>
       <c r="B16" s="15"/>
       <c r="C16" s="8" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D16" s="4">
         <v>22.393000000000001</v>
@@ -2847,34 +3975,154 @@
     <row r="17" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A17" s="12"/>
       <c r="B17" s="15"/>
+      <c r="D17" s="4">
+        <v>11.45</v>
+      </c>
+      <c r="E17" s="4">
+        <v>53.151000000000003</v>
+      </c>
+      <c r="F17" s="4">
+        <v>7.1665999999999999</v>
+      </c>
+      <c r="G17" s="4">
+        <v>3.9502000000000002</v>
+      </c>
+      <c r="H17" s="4">
+        <v>2221.6</v>
+      </c>
     </row>
     <row r="18" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A18" s="12"/>
       <c r="B18" s="15"/>
+      <c r="D18" s="4">
+        <v>37.741999999999997</v>
+      </c>
+      <c r="E18" s="4">
+        <v>49.122999999999998</v>
+      </c>
+      <c r="F18" s="4">
+        <v>2.4996</v>
+      </c>
+      <c r="G18" s="4">
+        <v>3.4102000000000001</v>
+      </c>
+      <c r="H18" s="4">
+        <v>3172</v>
+      </c>
     </row>
     <row r="19" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A19" s="12"/>
       <c r="B19" s="15"/>
+      <c r="D19" s="4">
+        <v>18.768000000000001</v>
+      </c>
+      <c r="E19" s="4">
+        <v>89.18</v>
+      </c>
+      <c r="F19" s="4">
+        <v>0.88068999999999997</v>
+      </c>
+      <c r="G19" s="4">
+        <v>4.5054999999999996</v>
+      </c>
+      <c r="H19" s="4">
+        <v>1677.4</v>
+      </c>
     </row>
     <row r="20" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A20" s="12"/>
       <c r="B20" s="15"/>
+      <c r="D20" s="4">
+        <v>23.303999999999998</v>
+      </c>
+      <c r="E20" s="4">
+        <v>306.58</v>
+      </c>
+      <c r="F20" s="4">
+        <v>0.32123000000000002</v>
+      </c>
+      <c r="G20" s="4">
+        <v>4.2591999999999999</v>
+      </c>
+      <c r="H20" s="4">
+        <v>1822.6</v>
+      </c>
     </row>
     <row r="21" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A21" s="12"/>
       <c r="B21" s="15"/>
+      <c r="D21" s="4">
+        <v>31.137</v>
+      </c>
+      <c r="E21" s="4">
+        <v>31.413</v>
+      </c>
+      <c r="F21" s="4">
+        <v>4.6002999999999998</v>
+      </c>
+      <c r="G21" s="4">
+        <v>3.6958000000000002</v>
+      </c>
+      <c r="H21" s="4">
+        <v>2583</v>
+      </c>
     </row>
     <row r="22" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A22" s="12"/>
       <c r="B22" s="15"/>
+      <c r="D22" s="4">
+        <v>29.725999999999999</v>
+      </c>
+      <c r="E22" s="4">
+        <v>45.991</v>
+      </c>
+      <c r="F22" s="4">
+        <v>2.3174000000000001</v>
+      </c>
+      <c r="G22" s="4">
+        <v>3.9613</v>
+      </c>
+      <c r="H22" s="4">
+        <v>2101.3000000000002</v>
+      </c>
     </row>
     <row r="23" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A23" s="12"/>
       <c r="B23" s="15"/>
+      <c r="D23" s="4">
+        <v>0.85682000000000003</v>
+      </c>
+      <c r="E23" s="4">
+        <v>42.524000000000001</v>
+      </c>
+      <c r="F23" s="4">
+        <v>9.6282999999999994</v>
+      </c>
+      <c r="G23" s="4">
+        <v>4.5033000000000003</v>
+      </c>
+      <c r="H23" s="4">
+        <v>1707</v>
+      </c>
     </row>
     <row r="24" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A24" s="12"/>
       <c r="B24" s="15"/>
+      <c r="D24" s="4">
+        <v>4.4611000000000001</v>
+      </c>
+      <c r="E24" s="4">
+        <v>35.628</v>
+      </c>
+      <c r="F24" s="4">
+        <v>31.021000000000001</v>
+      </c>
+      <c r="G24" s="4">
+        <v>3.6185999999999998</v>
+      </c>
+      <c r="H24" s="4">
+        <v>3016.2</v>
+      </c>
     </row>
     <row r="25" spans="1:26" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="13"/>
@@ -2896,7 +4144,7 @@
       <c r="A27" s="12"/>
       <c r="B27" s="15"/>
       <c r="C27" s="8" t="s">
-        <v>23</v>
+        <v>39</v>
       </c>
       <c r="D27" s="4">
         <v>4.8710000000000004</v>
@@ -2936,7 +4184,7 @@
       <c r="A28" s="12"/>
       <c r="B28" s="15"/>
       <c r="C28" s="8" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D28" s="4">
         <v>10.692</v>
@@ -2976,7 +4224,7 @@
       <c r="A29" s="12"/>
       <c r="B29" s="15"/>
       <c r="C29" s="8" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="D29" s="4">
         <v>11.2</v>
@@ -3015,30 +4263,135 @@
     <row r="30" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A30" s="12"/>
       <c r="B30" s="15"/>
+      <c r="D30" s="4">
+        <v>11.208</v>
+      </c>
+      <c r="E30" s="4">
+        <v>16.738</v>
+      </c>
+      <c r="F30" s="4">
+        <v>5.9587000000000003</v>
+      </c>
+      <c r="G30" s="4">
+        <v>3.6377000000000002</v>
+      </c>
+      <c r="H30" s="4">
+        <v>1530.1</v>
+      </c>
     </row>
     <row r="31" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A31" s="12"/>
       <c r="B31" s="15"/>
+      <c r="D31" s="4">
+        <v>10.45</v>
+      </c>
+      <c r="E31" s="4">
+        <v>14.769</v>
+      </c>
+      <c r="F31" s="4">
+        <v>7.8792</v>
+      </c>
+      <c r="G31" s="4">
+        <v>3.54</v>
+      </c>
+      <c r="H31" s="4">
+        <v>1787.3</v>
+      </c>
     </row>
     <row r="32" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A32" s="12"/>
       <c r="B32" s="15"/>
+      <c r="D32" s="4">
+        <v>11.010999999999999</v>
+      </c>
+      <c r="E32" s="4">
+        <v>11.071</v>
+      </c>
+      <c r="F32" s="4">
+        <v>13.523</v>
+      </c>
+      <c r="G32" s="4">
+        <v>3.5672000000000001</v>
+      </c>
+      <c r="H32" s="4">
+        <v>1593.8</v>
+      </c>
     </row>
     <row r="33" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A33" s="12"/>
       <c r="B33" s="15"/>
+      <c r="D33" s="4">
+        <v>5.6656000000000004</v>
+      </c>
+      <c r="E33" s="4">
+        <v>8.2222000000000008</v>
+      </c>
+      <c r="F33" s="4">
+        <v>14.47</v>
+      </c>
+      <c r="G33" s="4">
+        <v>4.3000999999999996</v>
+      </c>
+      <c r="H33" s="4">
+        <v>1000.8</v>
+      </c>
     </row>
     <row r="34" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A34" s="12"/>
       <c r="B34" s="15"/>
+      <c r="D34" s="4">
+        <v>15.185</v>
+      </c>
+      <c r="E34" s="4">
+        <v>64.875</v>
+      </c>
+      <c r="F34" s="4">
+        <v>1.4525999999999999</v>
+      </c>
+      <c r="G34" s="4">
+        <v>3.2002999999999999</v>
+      </c>
+      <c r="H34" s="4">
+        <v>2110.6</v>
+      </c>
     </row>
     <row r="35" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A35" s="12"/>
       <c r="B35" s="15"/>
+      <c r="D35" s="4">
+        <v>8.0571999999999999</v>
+      </c>
+      <c r="E35" s="4">
+        <v>29.803999999999998</v>
+      </c>
+      <c r="F35" s="4">
+        <v>2.5836000000000001</v>
+      </c>
+      <c r="G35" s="4">
+        <v>4.0204000000000004</v>
+      </c>
+      <c r="H35" s="4">
+        <v>1210.4000000000001</v>
+      </c>
     </row>
     <row r="36" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A36" s="12"/>
       <c r="B36" s="15"/>
+      <c r="D36" s="4">
+        <v>7.5292000000000003</v>
+      </c>
+      <c r="E36" s="4">
+        <v>23.504999999999999</v>
+      </c>
+      <c r="F36" s="4">
+        <v>4.9898999999999996</v>
+      </c>
+      <c r="G36" s="4">
+        <v>3.8622999999999998</v>
+      </c>
+      <c r="H36" s="4">
+        <v>1369.1</v>
+      </c>
     </row>
     <row r="37" spans="1:26" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="13"/>
@@ -3060,7 +4413,7 @@
       <c r="A39" s="12"/>
       <c r="B39" s="15"/>
       <c r="C39" s="8" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D39" s="4">
         <v>4.8238000000000003</v>
@@ -3100,7 +4453,7 @@
       <c r="A40" s="12"/>
       <c r="B40" s="15"/>
       <c r="C40" s="8" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="D40" s="4">
         <v>7.1036999999999999</v>
@@ -3140,7 +4493,7 @@
       <c r="A41" s="12"/>
       <c r="B41" s="15"/>
       <c r="C41" s="8" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="D41" s="4">
         <v>3.0461</v>
@@ -3179,30 +4532,135 @@
     <row r="42" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A42" s="12"/>
       <c r="B42" s="15"/>
+      <c r="D42" s="4">
+        <v>4.6340000000000003</v>
+      </c>
+      <c r="E42" s="4">
+        <v>18.606999999999999</v>
+      </c>
+      <c r="F42" s="4">
+        <v>24.896000000000001</v>
+      </c>
+      <c r="G42" s="4">
+        <v>3.3435999999999999</v>
+      </c>
+      <c r="H42" s="4">
+        <v>1999.7</v>
+      </c>
     </row>
     <row r="43" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A43" s="12"/>
       <c r="B43" s="15"/>
+      <c r="D43" s="4">
+        <v>16.286999999999999</v>
+      </c>
+      <c r="E43" s="4">
+        <v>181.45</v>
+      </c>
+      <c r="F43" s="4">
+        <v>0.52517000000000003</v>
+      </c>
+      <c r="G43" s="4">
+        <v>3.0160999999999998</v>
+      </c>
+      <c r="H43" s="4">
+        <v>2606.1999999999998</v>
+      </c>
     </row>
     <row r="44" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A44" s="12"/>
       <c r="B44" s="15"/>
+      <c r="D44" s="4">
+        <v>9.5312999999999999</v>
+      </c>
+      <c r="E44" s="4">
+        <v>148.61000000000001</v>
+      </c>
+      <c r="F44" s="4">
+        <v>0.37484000000000001</v>
+      </c>
+      <c r="G44" s="4">
+        <v>3.9621</v>
+      </c>
+      <c r="H44" s="4">
+        <v>1253.9000000000001</v>
+      </c>
     </row>
     <row r="45" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A45" s="12"/>
       <c r="B45" s="15"/>
+      <c r="D45" s="4">
+        <v>6.3647</v>
+      </c>
+      <c r="E45" s="4">
+        <v>149.54</v>
+      </c>
+      <c r="F45" s="4">
+        <v>0.43913000000000002</v>
+      </c>
+      <c r="G45" s="4">
+        <v>4.1839000000000004</v>
+      </c>
+      <c r="H45" s="4">
+        <v>1127.5999999999999</v>
+      </c>
     </row>
     <row r="46" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A46" s="12"/>
       <c r="B46" s="15"/>
+      <c r="D46" s="4">
+        <v>12.622</v>
+      </c>
+      <c r="E46" s="4">
+        <v>15.441000000000001</v>
+      </c>
+      <c r="F46" s="4">
+        <v>4.5385999999999997</v>
+      </c>
+      <c r="G46" s="4">
+        <v>3.7305000000000001</v>
+      </c>
+      <c r="H46" s="4">
+        <v>1371.6</v>
+      </c>
     </row>
     <row r="47" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A47" s="12"/>
       <c r="B47" s="15"/>
+      <c r="D47" s="4">
+        <v>12.256</v>
+      </c>
+      <c r="E47" s="4">
+        <v>273.68</v>
+      </c>
+      <c r="F47" s="4">
+        <v>0.20866000000000001</v>
+      </c>
+      <c r="G47" s="4">
+        <v>3.8422000000000001</v>
+      </c>
+      <c r="H47" s="4">
+        <v>1242.3</v>
+      </c>
     </row>
     <row r="48" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A48" s="12"/>
       <c r="B48" s="15"/>
+      <c r="D48" s="4">
+        <v>7.0439999999999996</v>
+      </c>
+      <c r="E48" s="4">
+        <v>16.175000000000001</v>
+      </c>
+      <c r="F48" s="4">
+        <v>6.7949000000000002</v>
+      </c>
+      <c r="G48" s="4">
+        <v>4.1207000000000003</v>
+      </c>
+      <c r="H48" s="4">
+        <v>1090</v>
+      </c>
     </row>
     <row r="49" spans="1:26" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="13"/>
@@ -3326,18 +4784,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A2:A13"/>
+    <mergeCell ref="B2:B13"/>
+    <mergeCell ref="A14:A25"/>
+    <mergeCell ref="B14:B25"/>
+    <mergeCell ref="A26:A37"/>
+    <mergeCell ref="B26:B37"/>
     <mergeCell ref="A38:A49"/>
     <mergeCell ref="B38:B49"/>
     <mergeCell ref="A50:A61"/>
     <mergeCell ref="B50:B61"/>
     <mergeCell ref="A62:A73"/>
     <mergeCell ref="B62:B73"/>
-    <mergeCell ref="A2:A13"/>
-    <mergeCell ref="B2:B13"/>
-    <mergeCell ref="A14:A25"/>
-    <mergeCell ref="B14:B25"/>
-    <mergeCell ref="A26:A37"/>
-    <mergeCell ref="B26:B37"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
Added arg_max obj func and changed scripts to incorporate arg_max
</commit_message>
<xml_diff>
--- a/scripts/__other__/__sem__.xlsx
+++ b/scripts/__other__/__sem__.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Janzen\Desktop\code\moga_neml\scripts\__other__\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0061927F-723F-4092-9BD2-D6870FA64542}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A46D5D86-5AD9-4582-88B7-75266FFA5488}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="15600" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15600" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="evp" sheetId="13" r:id="rId1"/>
@@ -2319,18 +2319,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A38:A49"/>
+    <mergeCell ref="B38:B49"/>
+    <mergeCell ref="A50:A61"/>
+    <mergeCell ref="B50:B61"/>
+    <mergeCell ref="A62:A73"/>
+    <mergeCell ref="B62:B73"/>
     <mergeCell ref="A2:A13"/>
     <mergeCell ref="B2:B13"/>
     <mergeCell ref="A14:A25"/>
     <mergeCell ref="B14:B25"/>
     <mergeCell ref="A26:A37"/>
     <mergeCell ref="B26:B37"/>
-    <mergeCell ref="A38:A49"/>
-    <mergeCell ref="B38:B49"/>
-    <mergeCell ref="A50:A61"/>
-    <mergeCell ref="B50:B61"/>
-    <mergeCell ref="A62:A73"/>
-    <mergeCell ref="B62:B73"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -2343,8 +2343,8 @@
   <dimension ref="A1:T73"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C42" sqref="C42"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2465,7 +2465,7 @@
       <c r="A4" s="12"/>
       <c r="B4" s="15"/>
       <c r="C4" s="8" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="D4" s="4">
         <v>5.6908000000000003</v>
@@ -3516,18 +3516,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A38:A49"/>
+    <mergeCell ref="B38:B49"/>
+    <mergeCell ref="A50:A61"/>
+    <mergeCell ref="B50:B61"/>
+    <mergeCell ref="A62:A73"/>
+    <mergeCell ref="B62:B73"/>
     <mergeCell ref="A2:A13"/>
     <mergeCell ref="B2:B13"/>
     <mergeCell ref="A14:A25"/>
     <mergeCell ref="B14:B25"/>
     <mergeCell ref="A26:A37"/>
     <mergeCell ref="B26:B37"/>
-    <mergeCell ref="A38:A49"/>
-    <mergeCell ref="B38:B49"/>
-    <mergeCell ref="A50:A61"/>
-    <mergeCell ref="B50:B61"/>
-    <mergeCell ref="A62:A73"/>
-    <mergeCell ref="B62:B73"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -4784,18 +4784,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A38:A49"/>
+    <mergeCell ref="B38:B49"/>
+    <mergeCell ref="A50:A61"/>
+    <mergeCell ref="B50:B61"/>
+    <mergeCell ref="A62:A73"/>
+    <mergeCell ref="B62:B73"/>
     <mergeCell ref="A2:A13"/>
     <mergeCell ref="B2:B13"/>
     <mergeCell ref="A14:A25"/>
     <mergeCell ref="B14:B25"/>
     <mergeCell ref="A26:A37"/>
     <mergeCell ref="B26:B37"/>
-    <mergeCell ref="A38:A49"/>
-    <mergeCell ref="B38:B49"/>
-    <mergeCell ref="A50:A61"/>
-    <mergeCell ref="B50:B61"/>
-    <mergeCell ref="A62:A73"/>
-    <mergeCell ref="B62:B73"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
Added new params for evpcd
</commit_message>
<xml_diff>
--- a/scripts/__other__/__sem__.xlsx
+++ b/scripts/__other__/__sem__.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Janzen\Desktop\code\moga_neml\scripts\__other__\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03009706-4478-4249-AECE-6099A0354AAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA77BB9A-8129-4494-9398-04E8AA4B0EAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="15600" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15600" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="evp" sheetId="13" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="43">
   <si>
     <t>temp</t>
   </si>
@@ -164,6 +164,9 @@
   </si>
   <si>
     <t>6; 10</t>
+  </si>
+  <si>
+    <t>9; 7</t>
   </si>
 </sst>
 </file>
@@ -2322,18 +2325,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A2:A13"/>
+    <mergeCell ref="B2:B13"/>
+    <mergeCell ref="A14:A25"/>
+    <mergeCell ref="B14:B25"/>
+    <mergeCell ref="A26:A37"/>
+    <mergeCell ref="B26:B37"/>
     <mergeCell ref="A38:A49"/>
     <mergeCell ref="B38:B49"/>
     <mergeCell ref="A50:A61"/>
     <mergeCell ref="B50:B61"/>
     <mergeCell ref="A62:A73"/>
     <mergeCell ref="B62:B73"/>
-    <mergeCell ref="A2:A13"/>
-    <mergeCell ref="B2:B13"/>
-    <mergeCell ref="A14:A25"/>
-    <mergeCell ref="B14:B25"/>
-    <mergeCell ref="A26:A37"/>
-    <mergeCell ref="B26:B37"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -2346,8 +2349,8 @@
   <dimension ref="A1:T73"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C43" sqref="C43"/>
+      <pane ySplit="1" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I36" sqref="I36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2560,6 +2563,9 @@
     <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" s="12"/>
       <c r="B7" s="15"/>
+      <c r="C7" s="8" t="s">
+        <v>19</v>
+      </c>
       <c r="D7" s="4">
         <v>4.1862000000000004</v>
       </c>
@@ -2574,11 +2580,23 @@
       </c>
       <c r="H7" s="4">
         <v>1574.3</v>
+      </c>
+      <c r="I7" s="4">
+        <v>2883.2</v>
+      </c>
+      <c r="J7" s="4">
+        <v>4.8533999999999997</v>
+      </c>
+      <c r="K7" s="3">
+        <v>4.6837</v>
       </c>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" s="12"/>
       <c r="B8" s="15"/>
+      <c r="C8" s="8" t="s">
+        <v>19</v>
+      </c>
       <c r="D8" s="4">
         <v>25.038</v>
       </c>
@@ -2593,6 +2611,15 @@
       </c>
       <c r="H8" s="4">
         <v>1944.6</v>
+      </c>
+      <c r="I8" s="2">
+        <v>2654.9</v>
+      </c>
+      <c r="J8" s="2">
+        <v>5.1295999999999999</v>
+      </c>
+      <c r="K8" s="2">
+        <v>10.247999999999999</v>
       </c>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.25">
@@ -2814,6 +2841,9 @@
     <row r="19" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A19" s="12"/>
       <c r="B19" s="15"/>
+      <c r="C19" s="8" t="s">
+        <v>32</v>
+      </c>
       <c r="D19" s="4">
         <v>18.768000000000001</v>
       </c>
@@ -2828,11 +2858,23 @@
       </c>
       <c r="H19" s="4">
         <v>1677.4</v>
+      </c>
+      <c r="I19" s="4">
+        <v>2589.6999999999998</v>
+      </c>
+      <c r="J19" s="4">
+        <v>5.1066000000000003</v>
+      </c>
+      <c r="K19" s="3">
+        <v>8.5634999999999994</v>
       </c>
     </row>
     <row r="20" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A20" s="12"/>
       <c r="B20" s="15"/>
+      <c r="C20" s="8" t="s">
+        <v>39</v>
+      </c>
       <c r="D20" s="4">
         <v>23.303999999999998</v>
       </c>
@@ -2847,11 +2889,23 @@
       </c>
       <c r="H20" s="4">
         <v>1822.6</v>
+      </c>
+      <c r="I20" s="4">
+        <v>2676.8</v>
+      </c>
+      <c r="J20" s="4">
+        <v>5.1559999999999997</v>
+      </c>
+      <c r="K20" s="3">
+        <v>11.901999999999999</v>
       </c>
     </row>
     <row r="21" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A21" s="12"/>
       <c r="B21" s="15"/>
+      <c r="C21" s="8" t="s">
+        <v>42</v>
+      </c>
       <c r="D21" s="4">
         <v>31.137</v>
       </c>
@@ -2866,6 +2920,15 @@
       </c>
       <c r="H21" s="4">
         <v>2583</v>
+      </c>
+      <c r="I21" s="4">
+        <v>2169.1</v>
+      </c>
+      <c r="J21" s="4">
+        <v>5.3201999999999998</v>
+      </c>
+      <c r="K21" s="3">
+        <v>6.8597999999999999</v>
       </c>
     </row>
     <row r="22" spans="1:20" x14ac:dyDescent="0.25">
@@ -3099,6 +3162,9 @@
     <row r="32" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A32" s="12"/>
       <c r="B32" s="15"/>
+      <c r="C32" s="8" t="s">
+        <v>19</v>
+      </c>
       <c r="D32" s="4">
         <v>11.010999999999999</v>
       </c>
@@ -3113,11 +3179,23 @@
       </c>
       <c r="H32" s="4">
         <v>1593.8</v>
+      </c>
+      <c r="I32" s="4">
+        <v>1955.7</v>
+      </c>
+      <c r="J32" s="4">
+        <v>4.4015000000000004</v>
+      </c>
+      <c r="K32" s="3">
+        <v>8.5838000000000001</v>
       </c>
     </row>
     <row r="33" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A33" s="12"/>
       <c r="B33" s="15"/>
+      <c r="C33" s="8" t="s">
+        <v>20</v>
+      </c>
       <c r="D33" s="4">
         <v>5.6656000000000004</v>
       </c>
@@ -3132,6 +3210,15 @@
       </c>
       <c r="H33" s="4">
         <v>1000.8</v>
+      </c>
+      <c r="I33" s="4">
+        <v>3494.5</v>
+      </c>
+      <c r="J33" s="4">
+        <v>3.9569000000000001</v>
+      </c>
+      <c r="K33" s="3">
+        <v>11.773</v>
       </c>
     </row>
     <row r="34" spans="1:20" x14ac:dyDescent="0.25">
@@ -3334,6 +3421,9 @@
     <row r="43" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A43" s="12"/>
       <c r="B43" s="15"/>
+      <c r="C43" s="8" t="s">
+        <v>39</v>
+      </c>
       <c r="D43" s="4">
         <v>16.286999999999999</v>
       </c>
@@ -3348,11 +3438,23 @@
       </c>
       <c r="H43" s="4">
         <v>2606.1999999999998</v>
+      </c>
+      <c r="I43" s="4">
+        <v>2445.1999999999998</v>
+      </c>
+      <c r="J43" s="4">
+        <v>4.13</v>
+      </c>
+      <c r="K43" s="3">
+        <v>5.8582999999999998</v>
       </c>
     </row>
     <row r="44" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A44" s="12"/>
       <c r="B44" s="15"/>
+      <c r="C44" s="8" t="s">
+        <v>28</v>
+      </c>
       <c r="D44" s="4">
         <v>9.5312999999999999</v>
       </c>
@@ -3367,6 +3469,15 @@
       </c>
       <c r="H44" s="4">
         <v>1253.9000000000001</v>
+      </c>
+      <c r="I44" s="2">
+        <v>2014.6</v>
+      </c>
+      <c r="J44" s="2">
+        <v>4.3747999999999996</v>
+      </c>
+      <c r="K44" s="2">
+        <v>8.0503999999999998</v>
       </c>
     </row>
     <row r="45" spans="1:20" x14ac:dyDescent="0.25">
@@ -3567,18 +3678,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A2:A13"/>
+    <mergeCell ref="B2:B13"/>
+    <mergeCell ref="A14:A25"/>
+    <mergeCell ref="B14:B25"/>
+    <mergeCell ref="A26:A37"/>
+    <mergeCell ref="B26:B37"/>
     <mergeCell ref="A38:A49"/>
     <mergeCell ref="B38:B49"/>
     <mergeCell ref="A50:A61"/>
     <mergeCell ref="B50:B61"/>
     <mergeCell ref="A62:A73"/>
     <mergeCell ref="B62:B73"/>
-    <mergeCell ref="A2:A13"/>
-    <mergeCell ref="B2:B13"/>
-    <mergeCell ref="A14:A25"/>
-    <mergeCell ref="B14:B25"/>
-    <mergeCell ref="A26:A37"/>
-    <mergeCell ref="B26:B37"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -4835,18 +4946,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A2:A13"/>
+    <mergeCell ref="B2:B13"/>
+    <mergeCell ref="A14:A25"/>
+    <mergeCell ref="B14:B25"/>
+    <mergeCell ref="A26:A37"/>
+    <mergeCell ref="B26:B37"/>
     <mergeCell ref="A38:A49"/>
     <mergeCell ref="B38:B49"/>
     <mergeCell ref="A50:A61"/>
     <mergeCell ref="B50:B61"/>
     <mergeCell ref="A62:A73"/>
     <mergeCell ref="B62:B73"/>
-    <mergeCell ref="A2:A13"/>
-    <mergeCell ref="B2:B13"/>
-    <mergeCell ref="A14:A25"/>
-    <mergeCell ref="B14:B25"/>
-    <mergeCell ref="A26:A37"/>
-    <mergeCell ref="B26:B37"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
Updated params in results file
</commit_message>
<xml_diff>
--- a/scripts/__other__/__sem__.xlsx
+++ b/scripts/__other__/__sem__.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Janzen\Desktop\code\moga_neml\scripts\__other__\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA77BB9A-8129-4494-9398-04E8AA4B0EAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59C5DB62-8BD2-454D-A35C-2E9A572B7207}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15600" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="evp" sheetId="13" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="44">
   <si>
     <t>temp</t>
   </si>
@@ -167,6 +167,9 @@
   </si>
   <si>
     <t>9; 7</t>
+  </si>
+  <si>
+    <t>8; 6</t>
   </si>
 </sst>
 </file>
@@ -2325,18 +2328,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A38:A49"/>
+    <mergeCell ref="B38:B49"/>
+    <mergeCell ref="A50:A61"/>
+    <mergeCell ref="B50:B61"/>
+    <mergeCell ref="A62:A73"/>
+    <mergeCell ref="B62:B73"/>
     <mergeCell ref="A2:A13"/>
     <mergeCell ref="B2:B13"/>
     <mergeCell ref="A14:A25"/>
     <mergeCell ref="B14:B25"/>
     <mergeCell ref="A26:A37"/>
     <mergeCell ref="B26:B37"/>
-    <mergeCell ref="A38:A49"/>
-    <mergeCell ref="B38:B49"/>
-    <mergeCell ref="A50:A61"/>
-    <mergeCell ref="B50:B61"/>
-    <mergeCell ref="A62:A73"/>
-    <mergeCell ref="B62:B73"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -2349,8 +2352,8 @@
   <dimension ref="A1:T73"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I36" sqref="I36"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I6" sqref="I6:K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2471,7 +2474,7 @@
       <c r="A4" s="12"/>
       <c r="B4" s="15"/>
       <c r="C4" s="8" t="s">
-        <v>23</v>
+        <v>43</v>
       </c>
       <c r="D4" s="4">
         <v>5.6908000000000003</v>
@@ -2533,7 +2536,7 @@
       <c r="A6" s="12"/>
       <c r="B6" s="15"/>
       <c r="C6" s="8" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="D6" s="4">
         <v>5.8951000000000002</v>
@@ -2550,21 +2553,21 @@
       <c r="H6" s="4">
         <v>1598.4</v>
       </c>
-      <c r="I6" s="4">
-        <v>2397.5</v>
-      </c>
-      <c r="J6" s="4">
-        <v>5.3810000000000002</v>
-      </c>
-      <c r="K6" s="3">
-        <v>14.128</v>
+      <c r="I6" s="2">
+        <v>2223.9</v>
+      </c>
+      <c r="J6" s="2">
+        <v>5.2808999999999999</v>
+      </c>
+      <c r="K6" s="2">
+        <v>6.7355</v>
       </c>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" s="12"/>
       <c r="B7" s="15"/>
       <c r="C7" s="8" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="D7" s="4">
         <v>4.1862000000000004</v>
@@ -2873,7 +2876,7 @@
       <c r="A20" s="12"/>
       <c r="B20" s="15"/>
       <c r="C20" s="8" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="D20" s="4">
         <v>23.303999999999998</v>
@@ -2891,21 +2894,18 @@
         <v>1822.6</v>
       </c>
       <c r="I20" s="4">
-        <v>2676.8</v>
+        <v>2169.1</v>
       </c>
       <c r="J20" s="4">
-        <v>5.1559999999999997</v>
+        <v>5.3201999999999998</v>
       </c>
       <c r="K20" s="3">
-        <v>11.901999999999999</v>
+        <v>6.8597999999999999</v>
       </c>
     </row>
     <row r="21" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A21" s="12"/>
       <c r="B21" s="15"/>
-      <c r="C21" s="8" t="s">
-        <v>42</v>
-      </c>
       <c r="D21" s="4">
         <v>31.137</v>
       </c>
@@ -2920,15 +2920,6 @@
       </c>
       <c r="H21" s="4">
         <v>2583</v>
-      </c>
-      <c r="I21" s="4">
-        <v>2169.1</v>
-      </c>
-      <c r="J21" s="4">
-        <v>5.3201999999999998</v>
-      </c>
-      <c r="K21" s="3">
-        <v>6.8597999999999999</v>
       </c>
     </row>
     <row r="22" spans="1:20" x14ac:dyDescent="0.25">
@@ -3678,18 +3669,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A38:A49"/>
+    <mergeCell ref="B38:B49"/>
+    <mergeCell ref="A50:A61"/>
+    <mergeCell ref="B50:B61"/>
+    <mergeCell ref="A62:A73"/>
+    <mergeCell ref="B62:B73"/>
     <mergeCell ref="A2:A13"/>
     <mergeCell ref="B2:B13"/>
     <mergeCell ref="A14:A25"/>
     <mergeCell ref="B14:B25"/>
     <mergeCell ref="A26:A37"/>
     <mergeCell ref="B26:B37"/>
-    <mergeCell ref="A38:A49"/>
-    <mergeCell ref="B38:B49"/>
-    <mergeCell ref="A50:A61"/>
-    <mergeCell ref="B50:B61"/>
-    <mergeCell ref="A62:A73"/>
-    <mergeCell ref="B62:B73"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -3702,7 +3693,7 @@
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I43" sqref="I43"/>
+      <selection pane="bottomLeft" activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4946,18 +4937,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A38:A49"/>
+    <mergeCell ref="B38:B49"/>
+    <mergeCell ref="A50:A61"/>
+    <mergeCell ref="B50:B61"/>
+    <mergeCell ref="A62:A73"/>
+    <mergeCell ref="B62:B73"/>
     <mergeCell ref="A2:A13"/>
     <mergeCell ref="B2:B13"/>
     <mergeCell ref="A14:A25"/>
     <mergeCell ref="B14:B25"/>
     <mergeCell ref="A26:A37"/>
     <mergeCell ref="B26:B37"/>
-    <mergeCell ref="A38:A49"/>
-    <mergeCell ref="B38:B49"/>
-    <mergeCell ref="A50:A61"/>
-    <mergeCell ref="B50:B61"/>
-    <mergeCell ref="A62:A73"/>
-    <mergeCell ref="B62:B73"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
Added new params for evpcd and updated sem
</commit_message>
<xml_diff>
--- a/scripts/__other__/__sem__.xlsx
+++ b/scripts/__other__/__sem__.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Janzen\Desktop\code\moga_neml\scripts\__other__\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59C5DB62-8BD2-454D-A35C-2E9A572B7207}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4CD954C-D859-406D-9D32-26281735C984}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15600" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="evp" sheetId="13" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="44">
   <si>
     <t>temp</t>
   </si>
@@ -2328,18 +2328,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A2:A13"/>
+    <mergeCell ref="B2:B13"/>
+    <mergeCell ref="A14:A25"/>
+    <mergeCell ref="B14:B25"/>
+    <mergeCell ref="A26:A37"/>
+    <mergeCell ref="B26:B37"/>
     <mergeCell ref="A38:A49"/>
     <mergeCell ref="B38:B49"/>
     <mergeCell ref="A50:A61"/>
     <mergeCell ref="B50:B61"/>
     <mergeCell ref="A62:A73"/>
     <mergeCell ref="B62:B73"/>
-    <mergeCell ref="A2:A13"/>
-    <mergeCell ref="B2:B13"/>
-    <mergeCell ref="A14:A25"/>
-    <mergeCell ref="B14:B25"/>
-    <mergeCell ref="A26:A37"/>
-    <mergeCell ref="B26:B37"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -2352,8 +2352,8 @@
   <dimension ref="A1:T73"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I6" sqref="I6:K6"/>
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C47" sqref="C47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2628,6 +2628,9 @@
     <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" s="12"/>
       <c r="B9" s="15"/>
+      <c r="C9" s="8" t="s">
+        <v>28</v>
+      </c>
       <c r="D9" s="4">
         <v>27.547000000000001</v>
       </c>
@@ -2642,11 +2645,23 @@
       </c>
       <c r="H9" s="4">
         <v>2454.8000000000002</v>
+      </c>
+      <c r="I9" s="4">
+        <v>2960.7</v>
+      </c>
+      <c r="J9" s="4">
+        <v>4.9866999999999999</v>
+      </c>
+      <c r="K9" s="3">
+        <v>10.836</v>
       </c>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10" s="12"/>
       <c r="B10" s="15"/>
+      <c r="C10" s="8" t="s">
+        <v>19</v>
+      </c>
       <c r="D10" s="4">
         <v>27.885000000000002</v>
       </c>
@@ -2661,6 +2676,15 @@
       </c>
       <c r="H10" s="4">
         <v>2390.5</v>
+      </c>
+      <c r="I10" s="2">
+        <v>2711.4</v>
+      </c>
+      <c r="J10" s="2">
+        <v>5.0381999999999998</v>
+      </c>
+      <c r="K10" s="2">
+        <v>7.7606999999999999</v>
       </c>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.25">
@@ -2906,6 +2930,9 @@
     <row r="21" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A21" s="12"/>
       <c r="B21" s="15"/>
+      <c r="C21" s="8" t="s">
+        <v>39</v>
+      </c>
       <c r="D21" s="4">
         <v>31.137</v>
       </c>
@@ -2920,11 +2947,23 @@
       </c>
       <c r="H21" s="4">
         <v>2583</v>
+      </c>
+      <c r="I21" s="2">
+        <v>2511.6999999999998</v>
+      </c>
+      <c r="J21" s="2">
+        <v>5.1558999999999999</v>
+      </c>
+      <c r="K21" s="2">
+        <v>8.7353000000000005</v>
       </c>
     </row>
     <row r="22" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A22" s="12"/>
       <c r="B22" s="15"/>
+      <c r="C22" s="8" t="s">
+        <v>29</v>
+      </c>
       <c r="D22" s="4">
         <v>29.725999999999999</v>
       </c>
@@ -2939,6 +2978,15 @@
       </c>
       <c r="H22" s="4">
         <v>2101.3000000000002</v>
+      </c>
+      <c r="I22" s="2">
+        <v>2259.1999999999998</v>
+      </c>
+      <c r="J22" s="2">
+        <v>5.3186999999999998</v>
+      </c>
+      <c r="K22" s="2">
+        <v>8.5096000000000007</v>
       </c>
     </row>
     <row r="23" spans="1:20" x14ac:dyDescent="0.25">
@@ -3215,6 +3263,9 @@
     <row r="34" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A34" s="12"/>
       <c r="B34" s="15"/>
+      <c r="C34" s="8" t="s">
+        <v>39</v>
+      </c>
       <c r="D34" s="4">
         <v>15.185</v>
       </c>
@@ -3229,11 +3280,23 @@
       </c>
       <c r="H34" s="4">
         <v>2110.6</v>
+      </c>
+      <c r="I34" s="2">
+        <v>2312.8000000000002</v>
+      </c>
+      <c r="J34" s="2">
+        <v>4.1947999999999999</v>
+      </c>
+      <c r="K34" s="2">
+        <v>6.7274000000000003</v>
       </c>
     </row>
     <row r="35" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A35" s="12"/>
       <c r="B35" s="15"/>
+      <c r="C35" s="8" t="s">
+        <v>19</v>
+      </c>
       <c r="D35" s="4">
         <v>8.0571999999999999</v>
       </c>
@@ -3248,6 +3311,15 @@
       </c>
       <c r="H35" s="4">
         <v>1210.4000000000001</v>
+      </c>
+      <c r="I35" s="2">
+        <v>1624.1</v>
+      </c>
+      <c r="J35" s="2">
+        <v>4.5871000000000004</v>
+      </c>
+      <c r="K35" s="2">
+        <v>7.1367000000000003</v>
       </c>
     </row>
     <row r="36" spans="1:20" x14ac:dyDescent="0.25">
@@ -3474,6 +3546,9 @@
     <row r="45" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A45" s="12"/>
       <c r="B45" s="15"/>
+      <c r="C45" s="8" t="s">
+        <v>26</v>
+      </c>
       <c r="D45" s="4">
         <v>6.3647</v>
       </c>
@@ -3488,11 +3563,23 @@
       </c>
       <c r="H45" s="4">
         <v>1127.5999999999999</v>
+      </c>
+      <c r="I45" s="2">
+        <v>1881.2</v>
+      </c>
+      <c r="J45" s="2">
+        <v>4.4539</v>
+      </c>
+      <c r="K45" s="2">
+        <v>6.9904999999999999</v>
       </c>
     </row>
     <row r="46" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A46" s="12"/>
       <c r="B46" s="15"/>
+      <c r="C46" s="8" t="s">
+        <v>23</v>
+      </c>
       <c r="D46" s="4">
         <v>12.622</v>
       </c>
@@ -3507,6 +3594,15 @@
       </c>
       <c r="H46" s="4">
         <v>1371.6</v>
+      </c>
+      <c r="I46" s="2">
+        <v>1850.2</v>
+      </c>
+      <c r="J46" s="2">
+        <v>4.5259999999999998</v>
+      </c>
+      <c r="K46" s="2">
+        <v>9.6370000000000005</v>
       </c>
     </row>
     <row r="47" spans="1:20" x14ac:dyDescent="0.25">
@@ -3669,18 +3765,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A2:A13"/>
+    <mergeCell ref="B2:B13"/>
+    <mergeCell ref="A14:A25"/>
+    <mergeCell ref="B14:B25"/>
+    <mergeCell ref="A26:A37"/>
+    <mergeCell ref="B26:B37"/>
     <mergeCell ref="A38:A49"/>
     <mergeCell ref="B38:B49"/>
     <mergeCell ref="A50:A61"/>
     <mergeCell ref="B50:B61"/>
     <mergeCell ref="A62:A73"/>
     <mergeCell ref="B62:B73"/>
-    <mergeCell ref="A2:A13"/>
-    <mergeCell ref="B2:B13"/>
-    <mergeCell ref="A14:A25"/>
-    <mergeCell ref="B14:B25"/>
-    <mergeCell ref="A26:A37"/>
-    <mergeCell ref="B26:B37"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -4937,18 +5033,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A2:A13"/>
+    <mergeCell ref="B2:B13"/>
+    <mergeCell ref="A14:A25"/>
+    <mergeCell ref="B14:B25"/>
+    <mergeCell ref="A26:A37"/>
+    <mergeCell ref="B26:B37"/>
     <mergeCell ref="A38:A49"/>
     <mergeCell ref="B38:B49"/>
     <mergeCell ref="A50:A61"/>
     <mergeCell ref="B50:B61"/>
     <mergeCell ref="A62:A73"/>
     <mergeCell ref="B62:B73"/>
-    <mergeCell ref="A2:A13"/>
-    <mergeCell ref="B2:B13"/>
-    <mergeCell ref="A14:A25"/>
-    <mergeCell ref="B14:B25"/>
-    <mergeCell ref="A26:A37"/>
-    <mergeCell ref="B26:B37"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
Added evpcd_i and changed some code in fixed scripts
</commit_message>
<xml_diff>
--- a/scripts/__other__/__sem__.xlsx
+++ b/scripts/__other__/__sem__.xlsx
@@ -1,21 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Janzen\Desktop\code\moga_neml\scripts\__other__\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{410AEF24-F7B3-4331-839A-69120BFEC5F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78F71341-3985-4116-810B-071D967FF693}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15600" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="evp" sheetId="13" r:id="rId1"/>
-    <sheet name="evp-cd" sheetId="14" r:id="rId2"/>
-    <sheet name="evp-wd" sheetId="15" r:id="rId3"/>
+    <sheet name="evp-cd_f" sheetId="14" r:id="rId2"/>
+    <sheet name="evp-cd_i" sheetId="17" r:id="rId3"/>
+    <sheet name="evp-wd_f" sheetId="15" r:id="rId4"/>
+    <sheet name="evp-wd_i" sheetId="18" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="45">
   <si>
     <t>temp</t>
   </si>
@@ -103,19 +105,10 @@
     <t>10; 7</t>
   </si>
   <si>
-    <t>rating</t>
-  </si>
-  <si>
     <t>10; 9</t>
   </si>
   <si>
     <t>8; 9</t>
-  </si>
-  <si>
-    <t>evp-cd rating</t>
-  </si>
-  <si>
-    <t>evp-wd rating</t>
   </si>
   <si>
     <t>8; 10</t>
@@ -137,9 +130,6 @@
   </si>
   <si>
     <t>8; 7</t>
-  </si>
-  <si>
-    <t>6; 7</t>
   </si>
   <si>
     <t>7; 6</t>
@@ -170,6 +160,21 @@
   </si>
   <si>
     <t>8; 6</t>
+  </si>
+  <si>
+    <t>evp-cd_f</t>
+  </si>
+  <si>
+    <t>evp-wd_f</t>
+  </si>
+  <si>
+    <t>evp-wd_i</t>
+  </si>
+  <si>
+    <t>evp-cd_i</t>
+  </si>
+  <si>
+    <t>evp</t>
   </si>
 </sst>
 </file>
@@ -358,13 +363,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>10</xdr:col>
+      <xdr:col>12</xdr:col>
       <xdr:colOff>91110</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>52224</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
+      <xdr:col>15</xdr:col>
       <xdr:colOff>157370</xdr:colOff>
       <xdr:row>11</xdr:row>
       <xdr:rowOff>184745</xdr:rowOff>
@@ -402,13 +407,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>13</xdr:col>
+      <xdr:col>15</xdr:col>
       <xdr:colOff>140806</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>55084</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
+      <xdr:col>18</xdr:col>
       <xdr:colOff>196802</xdr:colOff>
       <xdr:row>11</xdr:row>
       <xdr:rowOff>177341</xdr:rowOff>
@@ -446,13 +451,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>10</xdr:col>
+      <xdr:col>12</xdr:col>
       <xdr:colOff>49697</xdr:colOff>
       <xdr:row>13</xdr:row>
       <xdr:rowOff>38684</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
+      <xdr:col>15</xdr:col>
       <xdr:colOff>115958</xdr:colOff>
       <xdr:row>23</xdr:row>
       <xdr:rowOff>171206</xdr:rowOff>
@@ -490,13 +495,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>13</xdr:col>
+      <xdr:col>15</xdr:col>
       <xdr:colOff>115959</xdr:colOff>
       <xdr:row>13</xdr:row>
       <xdr:rowOff>50347</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
+      <xdr:col>18</xdr:col>
       <xdr:colOff>182222</xdr:colOff>
       <xdr:row>23</xdr:row>
       <xdr:rowOff>182871</xdr:rowOff>
@@ -534,13 +539,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>10</xdr:col>
+      <xdr:col>12</xdr:col>
       <xdr:colOff>56793</xdr:colOff>
       <xdr:row>25</xdr:row>
       <xdr:rowOff>49159</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
+      <xdr:col>15</xdr:col>
       <xdr:colOff>149088</xdr:colOff>
       <xdr:row>36</xdr:row>
       <xdr:rowOff>17215</xdr:rowOff>
@@ -578,13 +583,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>13</xdr:col>
+      <xdr:col>15</xdr:col>
       <xdr:colOff>157372</xdr:colOff>
       <xdr:row>25</xdr:row>
       <xdr:rowOff>47782</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
+      <xdr:col>18</xdr:col>
       <xdr:colOff>258461</xdr:colOff>
       <xdr:row>36</xdr:row>
       <xdr:rowOff>24632</xdr:rowOff>
@@ -622,13 +627,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>10</xdr:col>
+      <xdr:col>12</xdr:col>
       <xdr:colOff>69809</xdr:colOff>
       <xdr:row>37</xdr:row>
       <xdr:rowOff>50057</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
+      <xdr:col>15</xdr:col>
       <xdr:colOff>152170</xdr:colOff>
       <xdr:row>48</xdr:row>
       <xdr:rowOff>8179</xdr:rowOff>
@@ -666,13 +671,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>13</xdr:col>
+      <xdr:col>15</xdr:col>
       <xdr:colOff>149087</xdr:colOff>
       <xdr:row>37</xdr:row>
       <xdr:rowOff>56062</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
+      <xdr:col>18</xdr:col>
       <xdr:colOff>240196</xdr:colOff>
       <xdr:row>48</xdr:row>
       <xdr:rowOff>22932</xdr:rowOff>
@@ -710,13 +715,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>16</xdr:col>
+      <xdr:col>18</xdr:col>
       <xdr:colOff>182217</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>49698</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>22</xdr:col>
+      <xdr:col>24</xdr:col>
       <xdr:colOff>323021</xdr:colOff>
       <xdr:row>11</xdr:row>
       <xdr:rowOff>186362</xdr:rowOff>
@@ -754,13 +759,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>16</xdr:col>
+      <xdr:col>18</xdr:col>
       <xdr:colOff>198784</xdr:colOff>
       <xdr:row>13</xdr:row>
       <xdr:rowOff>41415</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>22</xdr:col>
+      <xdr:col>24</xdr:col>
       <xdr:colOff>331301</xdr:colOff>
       <xdr:row>23</xdr:row>
       <xdr:rowOff>173935</xdr:rowOff>
@@ -798,13 +803,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>16</xdr:col>
+      <xdr:col>18</xdr:col>
       <xdr:colOff>231914</xdr:colOff>
       <xdr:row>25</xdr:row>
       <xdr:rowOff>41412</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>22</xdr:col>
+      <xdr:col>24</xdr:col>
       <xdr:colOff>401248</xdr:colOff>
       <xdr:row>35</xdr:row>
       <xdr:rowOff>190499</xdr:rowOff>
@@ -842,13 +847,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>16</xdr:col>
+      <xdr:col>18</xdr:col>
       <xdr:colOff>238125</xdr:colOff>
       <xdr:row>38</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>22</xdr:col>
+      <xdr:col>24</xdr:col>
       <xdr:colOff>409575</xdr:colOff>
       <xdr:row>48</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
@@ -1150,11 +1155,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4D7A15E-4182-42F6-82DA-99E9B04906BA}">
-  <dimension ref="A1:O73"/>
+  <dimension ref="A1:Q73"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D1" sqref="D1:H1048576"/>
+      <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1164,11 +1169,11 @@
     <col min="3" max="3" width="15.7109375" style="8" customWidth="1"/>
     <col min="4" max="7" width="9.140625" style="4"/>
     <col min="8" max="8" width="9.140625" style="3"/>
-    <col min="9" max="10" width="15.7109375" style="8" customWidth="1"/>
-    <col min="11" max="16384" width="9.140625" style="4"/>
+    <col min="9" max="12" width="15.7109375" style="8" customWidth="1"/>
+    <col min="13" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -1176,7 +1181,7 @@
         <v>11</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>21</v>
+        <v>44</v>
       </c>
       <c r="D1" s="5" t="s">
         <v>1</v>
@@ -1194,13 +1199,19 @@
         <v>5</v>
       </c>
       <c r="I1" s="7" t="s">
-        <v>24</v>
+        <v>40</v>
       </c>
       <c r="J1" s="7" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+      <c r="K1" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="L1" s="7" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="11">
         <v>800</v>
       </c>
@@ -1208,7 +1219,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="12"/>
       <c r="B3" s="15"/>
       <c r="C3" s="8" t="s">
@@ -1230,13 +1241,13 @@
         <v>1783.5</v>
       </c>
       <c r="I3" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="J3" s="8" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+      <c r="K3" s="8" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="12"/>
       <c r="B4" s="15"/>
       <c r="C4" s="8" t="s">
@@ -1258,13 +1269,13 @@
         <v>1621.6</v>
       </c>
       <c r="I4" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="J4" s="8" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+      <c r="K4" s="8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="12"/>
       <c r="B5" s="15"/>
       <c r="C5" s="8" t="s">
@@ -1285,8 +1296,11 @@
       <c r="H5" s="1">
         <v>1775.9</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I5" s="8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="12"/>
       <c r="B6" s="15"/>
       <c r="C6" s="8" t="s">
@@ -1307,8 +1321,11 @@
       <c r="H6" s="1">
         <v>1598.4</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I6" s="8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="12"/>
       <c r="B7" s="15"/>
       <c r="C7" s="8" t="s">
@@ -1329,8 +1346,11 @@
       <c r="H7" s="1">
         <v>1574.3</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I7" s="8" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="12"/>
       <c r="B8" s="15"/>
       <c r="C8" s="8" t="s">
@@ -1351,8 +1371,11 @@
       <c r="H8" s="1">
         <v>1944.6</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I8" s="8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="12"/>
       <c r="B9" s="15"/>
       <c r="C9" s="8" t="s">
@@ -1373,8 +1396,11 @@
       <c r="H9" s="1">
         <v>2454.8000000000002</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I9" s="8" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="12"/>
       <c r="B10" s="15"/>
       <c r="C10" s="8" t="s">
@@ -1395,8 +1421,11 @@
       <c r="H10" s="1">
         <v>2390.5</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I10" s="8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="12"/>
       <c r="B11" s="15"/>
       <c r="C11" s="8" t="s">
@@ -1417,12 +1446,15 @@
       <c r="H11" s="1">
         <v>1614.6</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I11" s="8" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="12"/>
       <c r="B12" s="15"/>
       <c r="C12" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D12" s="9">
         <v>8.5922999999999998</v>
@@ -1439,16 +1471,21 @@
       <c r="H12" s="3">
         <v>1841</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I12" s="8" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="13"/>
       <c r="B13" s="16"/>
       <c r="C13" s="7"/>
       <c r="H13" s="6"/>
       <c r="I13" s="7"/>
       <c r="J13" s="7"/>
-    </row>
-    <row r="14" spans="1:10" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K13" s="7"/>
+      <c r="L13" s="7"/>
+    </row>
+    <row r="14" spans="1:12" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="11">
         <v>800</v>
       </c>
@@ -1456,11 +1493,11 @@
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="12"/>
       <c r="B15" s="15"/>
       <c r="C15" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D15" s="4">
         <v>31.327000000000002</v>
@@ -1480,11 +1517,11 @@
       <c r="I15" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="J15" s="8" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K15" s="8" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="12"/>
       <c r="B16" s="15"/>
       <c r="C16" s="8" t="s">
@@ -1506,17 +1543,17 @@
         <v>1828.1</v>
       </c>
       <c r="I16" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="J16" s="8" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+      <c r="K16" s="8" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="12"/>
       <c r="B17" s="15"/>
       <c r="C17" s="8" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D17" s="4">
         <v>11.45</v>
@@ -1533,12 +1570,15 @@
       <c r="H17" s="3">
         <v>2221.6</v>
       </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I17" s="8" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="12"/>
       <c r="B18" s="15"/>
       <c r="C18" s="8" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D18" s="4">
         <v>37.741999999999997</v>
@@ -1555,8 +1595,11 @@
       <c r="H18" s="3">
         <v>3172</v>
       </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I18" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="12"/>
       <c r="B19" s="15"/>
       <c r="C19" s="8" t="s">
@@ -1577,8 +1620,11 @@
       <c r="H19" s="1">
         <v>1677.4</v>
       </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I19" s="8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="12"/>
       <c r="B20" s="15"/>
       <c r="C20" s="8" t="s">
@@ -1599,12 +1645,15 @@
       <c r="H20" s="1">
         <v>1822.6</v>
       </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I20" s="8" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="12"/>
       <c r="B21" s="15"/>
       <c r="C21" s="8" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D21" s="2">
         <v>31.137</v>
@@ -1621,12 +1670,15 @@
       <c r="H21" s="1">
         <v>2583</v>
       </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I21" s="8" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="12"/>
       <c r="B22" s="15"/>
       <c r="C22" s="8" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D22" s="2">
         <v>29.725999999999999</v>
@@ -1643,8 +1695,11 @@
       <c r="H22" s="1">
         <v>2101.3000000000002</v>
       </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I22" s="8" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="12"/>
       <c r="B23" s="15"/>
       <c r="C23" s="8" t="s">
@@ -1665,8 +1720,11 @@
       <c r="H23" s="1">
         <v>1707</v>
       </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I23" s="8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="12"/>
       <c r="B24" s="15"/>
       <c r="C24" s="8" t="s">
@@ -1687,16 +1745,21 @@
       <c r="H24" s="3">
         <v>3016.2</v>
       </c>
-    </row>
-    <row r="25" spans="1:10" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I24" s="8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="13"/>
       <c r="B25" s="16"/>
       <c r="C25" s="7"/>
       <c r="H25" s="6"/>
       <c r="I25" s="7"/>
       <c r="J25" s="7"/>
-    </row>
-    <row r="26" spans="1:10" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K25" s="7"/>
+      <c r="L25" s="7"/>
+    </row>
+    <row r="26" spans="1:12" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="11">
         <v>900</v>
       </c>
@@ -1704,7 +1767,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="12"/>
       <c r="B27" s="15"/>
       <c r="C27" s="8" t="s">
@@ -1726,13 +1789,13 @@
         <v>1138.3</v>
       </c>
       <c r="I27" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="J27" s="8" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+      <c r="K27" s="8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="12"/>
       <c r="B28" s="15"/>
       <c r="C28" s="8" t="s">
@@ -1756,15 +1819,15 @@
       <c r="I28" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="J28" s="8" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K28" s="8" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" s="12"/>
       <c r="B29" s="15"/>
       <c r="C29" s="8" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D29" s="2">
         <v>11.2</v>
@@ -1784,11 +1847,11 @@
       <c r="I29" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="J29" s="8" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K29" s="8" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" s="12"/>
       <c r="B30" s="15"/>
       <c r="C30" s="8" t="s">
@@ -1809,8 +1872,11 @@
       <c r="H30" s="3">
         <v>1530.1</v>
       </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I30" s="8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" s="12"/>
       <c r="B31" s="15"/>
       <c r="C31" s="8" t="s">
@@ -1831,8 +1897,11 @@
       <c r="H31" s="1">
         <v>1787.3</v>
       </c>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I31" s="8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" s="12"/>
       <c r="B32" s="15"/>
       <c r="C32" s="8" t="s">
@@ -1853,12 +1922,15 @@
       <c r="H32" s="1">
         <v>1593.8</v>
       </c>
-    </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="I32" s="8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A33" s="12"/>
       <c r="B33" s="15"/>
       <c r="C33" s="8" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D33" s="2">
         <v>5.6656000000000004</v>
@@ -1875,8 +1947,11 @@
       <c r="H33" s="1">
         <v>1000.8</v>
       </c>
-    </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="I33" s="8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A34" s="12"/>
       <c r="B34" s="15"/>
       <c r="C34" s="8" t="s">
@@ -1897,8 +1972,11 @@
       <c r="H34" s="1">
         <v>2110.6</v>
       </c>
-    </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="I34" s="8" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A35" s="12"/>
       <c r="B35" s="15"/>
       <c r="C35" s="8" t="s">
@@ -1919,12 +1997,15 @@
       <c r="H35" s="1">
         <v>1210.4000000000001</v>
       </c>
-    </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="I35" s="8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A36" s="12"/>
       <c r="B36" s="15"/>
       <c r="C36" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D36" s="2">
         <v>7.5292000000000003</v>
@@ -1941,16 +2022,21 @@
       <c r="H36" s="1">
         <v>1369.1</v>
       </c>
-    </row>
-    <row r="37" spans="1:15" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I36" s="8" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="37" spans="1:17" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="13"/>
       <c r="B37" s="16"/>
       <c r="C37" s="7"/>
       <c r="H37" s="6"/>
       <c r="I37" s="7"/>
       <c r="J37" s="7"/>
-    </row>
-    <row r="38" spans="1:15" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K37" s="7"/>
+      <c r="L37" s="7"/>
+    </row>
+    <row r="38" spans="1:17" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="11">
         <v>900</v>
       </c>
@@ -1958,11 +2044,11 @@
         <v>7</v>
       </c>
     </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A39" s="12"/>
       <c r="B39" s="15"/>
       <c r="C39" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D39" s="4">
         <v>4.8238000000000003</v>
@@ -1980,22 +2066,22 @@
         <v>1006.9</v>
       </c>
       <c r="I39" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="J39" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="K39" s="2"/>
-      <c r="L39" s="2"/>
+        <v>23</v>
+      </c>
+      <c r="K39" s="8" t="s">
+        <v>31</v>
+      </c>
       <c r="M39" s="2"/>
       <c r="N39" s="2"/>
       <c r="O39" s="2"/>
-    </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P39" s="2"/>
+      <c r="Q39" s="2"/>
+    </row>
+    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A40" s="12"/>
       <c r="B40" s="15"/>
       <c r="C40" s="8" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D40" s="4">
         <v>7.1036999999999999</v>
@@ -2013,22 +2099,22 @@
         <v>1829.9</v>
       </c>
       <c r="I40" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="J40" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="K40" s="2"/>
-      <c r="L40" s="2"/>
+        <v>38</v>
+      </c>
+      <c r="K40" s="8" t="s">
+        <v>33</v>
+      </c>
       <c r="M40" s="2"/>
       <c r="N40" s="2"/>
       <c r="O40" s="2"/>
-    </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P40" s="2"/>
+      <c r="Q40" s="2"/>
+    </row>
+    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A41" s="12"/>
       <c r="B41" s="15"/>
       <c r="C41" s="8" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D41" s="4">
         <v>3.0461</v>
@@ -2046,17 +2132,17 @@
         <v>2022.3</v>
       </c>
       <c r="I41" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="J41" s="8" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+      <c r="K41" s="8" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A42" s="12"/>
       <c r="B42" s="15"/>
       <c r="C42" s="8" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D42" s="2">
         <v>4.6340000000000003</v>
@@ -2073,12 +2159,15 @@
       <c r="H42" s="1">
         <v>1999.7</v>
       </c>
-    </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="I42" s="8" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A43" s="12"/>
       <c r="B43" s="15"/>
       <c r="C43" s="8" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="D43" s="2">
         <v>16.286999999999999</v>
@@ -2095,8 +2184,11 @@
       <c r="H43" s="1">
         <v>2606.1999999999998</v>
       </c>
-    </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="I43" s="8" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A44" s="12"/>
       <c r="B44" s="15"/>
       <c r="C44" s="8" t="s">
@@ -2117,8 +2209,11 @@
       <c r="H44" s="1">
         <v>1253.9000000000001</v>
       </c>
-    </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="I44" s="8" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A45" s="12"/>
       <c r="B45" s="15"/>
       <c r="C45" s="8" t="s">
@@ -2139,8 +2234,11 @@
       <c r="H45" s="1">
         <v>1127.5999999999999</v>
       </c>
-    </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="I45" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="46" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A46" s="12"/>
       <c r="B46" s="15"/>
       <c r="C46" s="8" t="s">
@@ -2161,12 +2259,15 @@
       <c r="H46" s="1">
         <v>1371.6</v>
       </c>
-    </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="I46" s="8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="47" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A47" s="12"/>
       <c r="B47" s="15"/>
       <c r="C47" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D47" s="4">
         <v>12.256</v>
@@ -2183,8 +2284,11 @@
       <c r="H47" s="3">
         <v>1242.3</v>
       </c>
-    </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="I47" s="8" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="48" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A48" s="12"/>
       <c r="B48" s="15"/>
       <c r="C48" s="8" t="s">
@@ -2205,16 +2309,21 @@
       <c r="H48" s="1">
         <v>1090</v>
       </c>
-    </row>
-    <row r="49" spans="1:10" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I48" s="8" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="13"/>
       <c r="B49" s="16"/>
       <c r="C49" s="7"/>
       <c r="H49" s="6"/>
       <c r="I49" s="7"/>
       <c r="J49" s="7"/>
-    </row>
-    <row r="50" spans="1:10" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K49" s="7"/>
+      <c r="L49" s="7"/>
+    </row>
+    <row r="50" spans="1:12" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="11">
         <v>1000</v>
       </c>
@@ -2222,55 +2331,57 @@
         <v>6</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A51" s="12"/>
       <c r="B51" s="15"/>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A52" s="12"/>
       <c r="B52" s="15"/>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A53" s="12"/>
       <c r="B53" s="15"/>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A54" s="12"/>
       <c r="B54" s="15"/>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A55" s="12"/>
       <c r="B55" s="15"/>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A56" s="12"/>
       <c r="B56" s="15"/>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A57" s="12"/>
       <c r="B57" s="15"/>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A58" s="12"/>
       <c r="B58" s="15"/>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A59" s="12"/>
       <c r="B59" s="15"/>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A60" s="12"/>
       <c r="B60" s="15"/>
     </row>
-    <row r="61" spans="1:10" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:12" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="13"/>
       <c r="B61" s="16"/>
       <c r="C61" s="7"/>
       <c r="H61" s="6"/>
       <c r="I61" s="7"/>
       <c r="J61" s="7"/>
-    </row>
-    <row r="62" spans="1:10" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K61" s="7"/>
+      <c r="L61" s="7"/>
+    </row>
+    <row r="62" spans="1:12" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="11">
         <v>1000</v>
       </c>
@@ -2278,53 +2389,55 @@
         <v>7</v>
       </c>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A63" s="12"/>
       <c r="B63" s="15"/>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A64" s="12"/>
       <c r="B64" s="15"/>
     </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A65" s="12"/>
       <c r="B65" s="15"/>
     </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A66" s="12"/>
       <c r="B66" s="15"/>
     </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A67" s="12"/>
       <c r="B67" s="15"/>
     </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A68" s="12"/>
       <c r="B68" s="15"/>
     </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A69" s="12"/>
       <c r="B69" s="15"/>
     </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A70" s="12"/>
       <c r="B70" s="15"/>
     </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A71" s="12"/>
       <c r="B71" s="15"/>
     </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A72" s="12"/>
       <c r="B72" s="15"/>
     </row>
-    <row r="73" spans="1:10" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:12" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="13"/>
       <c r="B73" s="16"/>
       <c r="C73" s="7"/>
       <c r="H73" s="6"/>
       <c r="I73" s="7"/>
       <c r="J73" s="7"/>
+      <c r="K73" s="7"/>
+      <c r="L73" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="12">
@@ -2349,11 +2462,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE483CC8-AF2C-4D5A-AEE5-EF7DF4EC0883}">
-  <dimension ref="A1:T73"/>
+  <dimension ref="A1:K73"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E43" sqref="E43"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2363,13 +2476,10 @@
     <col min="3" max="3" width="15.7109375" style="8" customWidth="1"/>
     <col min="4" max="10" width="9.140625" style="4"/>
     <col min="11" max="11" width="9.140625" style="3"/>
-    <col min="12" max="12" width="15.7109375" style="8" customWidth="1"/>
-    <col min="13" max="19" width="9.140625" style="4"/>
-    <col min="20" max="20" width="9.140625" style="3"/>
-    <col min="21" max="16384" width="9.140625" style="4"/>
+    <col min="12" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -2377,7 +2487,7 @@
         <v>11</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>21</v>
+        <v>40</v>
       </c>
       <c r="D1" s="5" t="s">
         <v>1</v>
@@ -2403,35 +2513,8 @@
       <c r="K1" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="M1" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="N1" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="O1" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="P1" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q1" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="R1" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="S1" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="T1" s="6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:20" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:11" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="11">
         <v>800</v>
       </c>
@@ -2439,11 +2522,11 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="12"/>
       <c r="B3" s="15"/>
       <c r="C3" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D3" s="4">
         <v>17.216999999999999</v>
@@ -2466,15 +2549,15 @@
       <c r="J3" s="2">
         <v>4.8244999999999996</v>
       </c>
-      <c r="K3" s="2">
+      <c r="K3" s="1">
         <v>6.6364000000000001</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="12"/>
       <c r="B4" s="15"/>
       <c r="C4" s="8" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="D4" s="4">
         <v>5.6908000000000003</v>
@@ -2492,16 +2575,16 @@
         <v>1621.6</v>
       </c>
       <c r="I4" s="2">
-        <v>1846.1</v>
+        <v>1960.8</v>
       </c>
       <c r="J4" s="2">
-        <v>5.5984999999999996</v>
-      </c>
-      <c r="K4" s="2">
-        <v>6.6852999999999998</v>
-      </c>
-    </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+        <v>5.4898999999999996</v>
+      </c>
+      <c r="K4" s="1">
+        <v>7.0751999999999997</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="12"/>
       <c r="B5" s="15"/>
       <c r="C5" s="8" t="s">
@@ -2528,11 +2611,11 @@
       <c r="J5" s="2">
         <v>5.0411999999999999</v>
       </c>
-      <c r="K5" s="2">
+      <c r="K5" s="1">
         <v>9.5797000000000008</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="12"/>
       <c r="B6" s="15"/>
       <c r="C6" s="8" t="s">
@@ -2559,15 +2642,15 @@
       <c r="J6" s="2">
         <v>5.2808999999999999</v>
       </c>
-      <c r="K6" s="2">
+      <c r="K6" s="1">
         <v>6.7355</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="12"/>
       <c r="B7" s="15"/>
       <c r="C7" s="8" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D7" s="4">
         <v>4.1862000000000004</v>
@@ -2594,7 +2677,7 @@
         <v>4.6837</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="12"/>
       <c r="B8" s="15"/>
       <c r="C8" s="8" t="s">
@@ -2621,15 +2704,15 @@
       <c r="J8" s="2">
         <v>5.1295999999999999</v>
       </c>
-      <c r="K8" s="2">
+      <c r="K8" s="1">
         <v>10.247999999999999</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="12"/>
       <c r="B9" s="15"/>
       <c r="C9" s="8" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D9" s="4">
         <v>27.547000000000001</v>
@@ -2656,7 +2739,7 @@
         <v>10.836</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="12"/>
       <c r="B10" s="15"/>
       <c r="C10" s="8" t="s">
@@ -2683,13 +2766,16 @@
       <c r="J10" s="2">
         <v>5.0381999999999998</v>
       </c>
-      <c r="K10" s="2">
+      <c r="K10" s="1">
         <v>7.7606999999999999</v>
       </c>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="12"/>
       <c r="B11" s="15"/>
+      <c r="C11" s="8" t="s">
+        <v>38</v>
+      </c>
       <c r="D11" s="4">
         <v>19.2</v>
       </c>
@@ -2705,10 +2791,22 @@
       <c r="H11" s="4">
         <v>1614.6</v>
       </c>
-    </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="I11" s="4">
+        <v>1951.3</v>
+      </c>
+      <c r="J11" s="4">
+        <v>5.5552000000000001</v>
+      </c>
+      <c r="K11" s="3">
+        <v>8.4002999999999997</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="12"/>
       <c r="B12" s="15"/>
+      <c r="C12" s="8" t="s">
+        <v>26</v>
+      </c>
       <c r="D12" s="4">
         <v>8.5922999999999998</v>
       </c>
@@ -2724,16 +2822,23 @@
       <c r="H12" s="4">
         <v>1841</v>
       </c>
-    </row>
-    <row r="13" spans="1:20" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I12" s="2">
+        <v>2195.8000000000002</v>
+      </c>
+      <c r="J12" s="2">
+        <v>5.3108000000000004</v>
+      </c>
+      <c r="K12" s="1">
+        <v>6.9560000000000004</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="13"/>
       <c r="B13" s="16"/>
       <c r="C13" s="7"/>
       <c r="K13" s="6"/>
-      <c r="L13" s="7"/>
-      <c r="T13" s="6"/>
-    </row>
-    <row r="14" spans="1:20" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:11" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="11">
         <v>800</v>
       </c>
@@ -2741,7 +2846,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="12"/>
       <c r="B15" s="15"/>
       <c r="C15" s="8" t="s">
@@ -2772,11 +2877,11 @@
         <v>6.5503999999999998</v>
       </c>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="12"/>
       <c r="B16" s="15"/>
       <c r="C16" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D16" s="2">
         <v>22.393000000000001</v>
@@ -2799,15 +2904,15 @@
       <c r="J16" s="2">
         <v>5.5168999999999997</v>
       </c>
-      <c r="K16" s="2">
+      <c r="K16" s="1">
         <v>6.9638999999999998</v>
       </c>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="12"/>
       <c r="B17" s="15"/>
       <c r="C17" s="8" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="D17" s="4">
         <v>11.45</v>
@@ -2834,11 +2939,11 @@
         <v>5.3108000000000004</v>
       </c>
     </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="12"/>
       <c r="B18" s="15"/>
       <c r="C18" s="8" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D18" s="4">
         <v>37.741999999999997</v>
@@ -2865,11 +2970,11 @@
         <v>9.9024000000000001</v>
       </c>
     </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="12"/>
       <c r="B19" s="15"/>
       <c r="C19" s="8" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D19" s="4">
         <v>18.768000000000001</v>
@@ -2896,11 +3001,11 @@
         <v>8.5634999999999994</v>
       </c>
     </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="12"/>
       <c r="B20" s="15"/>
       <c r="C20" s="8" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="D20" s="4">
         <v>23.303999999999998</v>
@@ -2927,11 +3032,11 @@
         <v>6.8597999999999999</v>
       </c>
     </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="12"/>
       <c r="B21" s="15"/>
       <c r="C21" s="8" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="D21" s="4">
         <v>31.137</v>
@@ -2954,15 +3059,15 @@
       <c r="J21" s="2">
         <v>5.1558999999999999</v>
       </c>
-      <c r="K21" s="2">
+      <c r="K21" s="1">
         <v>8.7353000000000005</v>
       </c>
     </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="12"/>
       <c r="B22" s="15"/>
       <c r="C22" s="8" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D22" s="4">
         <v>29.725999999999999</v>
@@ -2985,13 +3090,16 @@
       <c r="J22" s="2">
         <v>5.3186999999999998</v>
       </c>
-      <c r="K22" s="2">
+      <c r="K22" s="1">
         <v>8.5096000000000007</v>
       </c>
     </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="12"/>
       <c r="B23" s="15"/>
+      <c r="C23" s="8" t="s">
+        <v>29</v>
+      </c>
       <c r="D23" s="4">
         <v>0.85682000000000003</v>
       </c>
@@ -3007,10 +3115,22 @@
       <c r="H23" s="4">
         <v>1707</v>
       </c>
-    </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="I23" s="4">
+        <v>1896.9</v>
+      </c>
+      <c r="J23" s="4">
+        <v>5.5469999999999997</v>
+      </c>
+      <c r="K23" s="3">
+        <v>6.8471000000000002</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="12"/>
       <c r="B24" s="15"/>
+      <c r="C24" s="8" t="s">
+        <v>21</v>
+      </c>
       <c r="D24" s="4">
         <v>4.4611000000000001</v>
       </c>
@@ -3026,16 +3146,23 @@
       <c r="H24" s="4">
         <v>3016.2</v>
       </c>
-    </row>
-    <row r="25" spans="1:20" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I24" s="2">
+        <v>3411.1</v>
+      </c>
+      <c r="J24" s="2">
+        <v>4.8323</v>
+      </c>
+      <c r="K24" s="1">
+        <v>12.863</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="13"/>
       <c r="B25" s="16"/>
       <c r="C25" s="7"/>
       <c r="K25" s="6"/>
-      <c r="L25" s="7"/>
-      <c r="T25" s="6"/>
-    </row>
-    <row r="26" spans="1:20" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="1:11" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="11">
         <v>900</v>
       </c>
@@ -3043,11 +3170,11 @@
         <v>6</v>
       </c>
     </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="12"/>
       <c r="B27" s="15"/>
       <c r="C27" s="8" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="D27" s="4">
         <v>4.8710000000000004</v>
@@ -3070,11 +3197,11 @@
       <c r="J27" s="2">
         <v>4.4973999999999998</v>
       </c>
-      <c r="K27" s="2">
+      <c r="K27" s="1">
         <v>9.6201000000000008</v>
       </c>
     </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="12"/>
       <c r="B28" s="15"/>
       <c r="C28" s="8" t="s">
@@ -3105,7 +3232,7 @@
         <v>5.8509000000000002</v>
       </c>
     </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="12"/>
       <c r="B29" s="15"/>
       <c r="C29" s="8" t="s">
@@ -3132,11 +3259,11 @@
       <c r="J29" s="2">
         <v>4.5818000000000003</v>
       </c>
-      <c r="K29" s="2">
+      <c r="K29" s="1">
         <v>9.0646000000000004</v>
       </c>
     </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="12"/>
       <c r="B30" s="15"/>
       <c r="C30" s="8" t="s">
@@ -3167,7 +3294,7 @@
         <v>7.4964000000000004</v>
       </c>
     </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="12"/>
       <c r="B31" s="15"/>
       <c r="C31" s="8" t="s">
@@ -3198,7 +3325,7 @@
         <v>8.3942999999999994</v>
       </c>
     </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="12"/>
       <c r="B32" s="15"/>
       <c r="C32" s="8" t="s">
@@ -3229,7 +3356,7 @@
         <v>8.5838000000000001</v>
       </c>
     </row>
-    <row r="33" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" s="12"/>
       <c r="B33" s="15"/>
       <c r="C33" s="8" t="s">
@@ -3260,11 +3387,11 @@
         <v>11.773</v>
       </c>
     </row>
-    <row r="34" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" s="12"/>
       <c r="B34" s="15"/>
       <c r="C34" s="8" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="D34" s="4">
         <v>15.185</v>
@@ -3287,11 +3414,11 @@
       <c r="J34" s="2">
         <v>4.1947999999999999</v>
       </c>
-      <c r="K34" s="2">
+      <c r="K34" s="1">
         <v>6.7274000000000003</v>
       </c>
     </row>
-    <row r="35" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" s="12"/>
       <c r="B35" s="15"/>
       <c r="C35" s="8" t="s">
@@ -3318,13 +3445,16 @@
       <c r="J35" s="2">
         <v>4.5871000000000004</v>
       </c>
-      <c r="K35" s="2">
+      <c r="K35" s="1">
         <v>7.1367000000000003</v>
       </c>
     </row>
-    <row r="36" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" s="12"/>
       <c r="B36" s="15"/>
+      <c r="C36" s="8" t="s">
+        <v>35</v>
+      </c>
       <c r="D36" s="4">
         <v>7.5292000000000003</v>
       </c>
@@ -3340,16 +3470,23 @@
       <c r="H36" s="4">
         <v>1369.1</v>
       </c>
-    </row>
-    <row r="37" spans="1:20" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I36" s="4">
+        <v>2070.6999999999998</v>
+      </c>
+      <c r="J36" s="4">
+        <v>4.3048999999999999</v>
+      </c>
+      <c r="K36" s="3">
+        <v>6.8212000000000002</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="13"/>
       <c r="B37" s="16"/>
       <c r="C37" s="7"/>
       <c r="K37" s="6"/>
-      <c r="L37" s="7"/>
-      <c r="T37" s="6"/>
-    </row>
-    <row r="38" spans="1:20" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="38" spans="1:11" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="11">
         <v>900</v>
       </c>
@@ -3357,11 +3494,11 @@
         <v>7</v>
       </c>
     </row>
-    <row r="39" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" s="12"/>
       <c r="B39" s="15"/>
       <c r="C39" s="8" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D39" s="4">
         <v>4.8238000000000003</v>
@@ -3388,11 +3525,11 @@
         <v>6.5256999999999996</v>
       </c>
     </row>
-    <row r="40" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" s="12"/>
       <c r="B40" s="15"/>
       <c r="C40" s="8" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="D40" s="4">
         <v>7.1036999999999999</v>
@@ -3410,20 +3547,20 @@
         <v>1829.9</v>
       </c>
       <c r="I40" s="2">
-        <v>1433</v>
+        <v>2105.1</v>
       </c>
       <c r="J40" s="2">
-        <v>4.6205999999999996</v>
-      </c>
-      <c r="K40" s="2">
-        <v>4.3208000000000002</v>
-      </c>
-    </row>
-    <row r="41" spans="1:20" x14ac:dyDescent="0.25">
+        <v>4.1879999999999997</v>
+      </c>
+      <c r="K40" s="1">
+        <v>3.5083000000000002</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" s="12"/>
       <c r="B41" s="15"/>
       <c r="C41" s="8" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="D41" s="4">
         <v>3.0461</v>
@@ -3441,20 +3578,20 @@
         <v>2022.3</v>
       </c>
       <c r="I41" s="2">
-        <v>2114.8000000000002</v>
+        <v>2242.6</v>
       </c>
       <c r="J41" s="2">
-        <v>4.4790000000000001</v>
-      </c>
-      <c r="K41" s="2">
-        <v>13.782999999999999</v>
-      </c>
-    </row>
-    <row r="42" spans="1:20" x14ac:dyDescent="0.25">
+        <v>4.4061000000000003</v>
+      </c>
+      <c r="K41" s="1">
+        <v>13.364000000000001</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" s="12"/>
       <c r="B42" s="15"/>
       <c r="C42" s="8" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="D42" s="4">
         <v>4.6340000000000003</v>
@@ -3477,15 +3614,15 @@
       <c r="J42" s="2">
         <v>4.3769999999999998</v>
       </c>
-      <c r="K42" s="2">
+      <c r="K42" s="1">
         <v>21.834</v>
       </c>
     </row>
-    <row r="43" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" s="12"/>
       <c r="B43" s="15"/>
       <c r="C43" s="8" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="D43" s="4">
         <v>16.286999999999999</v>
@@ -3512,11 +3649,11 @@
         <v>5.8582999999999998</v>
       </c>
     </row>
-    <row r="44" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" s="12"/>
       <c r="B44" s="15"/>
       <c r="C44" s="8" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D44" s="4">
         <v>9.5312999999999999</v>
@@ -3539,15 +3676,15 @@
       <c r="J44" s="2">
         <v>4.3747999999999996</v>
       </c>
-      <c r="K44" s="2">
+      <c r="K44" s="1">
         <v>8.0503999999999998</v>
       </c>
     </row>
-    <row r="45" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" s="12"/>
       <c r="B45" s="15"/>
       <c r="C45" s="8" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D45" s="4">
         <v>6.3647</v>
@@ -3570,15 +3707,15 @@
       <c r="J45" s="2">
         <v>4.4539</v>
       </c>
-      <c r="K45" s="2">
+      <c r="K45" s="1">
         <v>6.9904999999999999</v>
       </c>
     </row>
-    <row r="46" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" s="12"/>
       <c r="B46" s="15"/>
       <c r="C46" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D46" s="4">
         <v>12.622</v>
@@ -3601,13 +3738,16 @@
       <c r="J46" s="2">
         <v>4.5259999999999998</v>
       </c>
-      <c r="K46" s="2">
+      <c r="K46" s="1">
         <v>9.6370000000000005</v>
       </c>
     </row>
-    <row r="47" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" s="12"/>
       <c r="B47" s="15"/>
+      <c r="C47" s="8" t="s">
+        <v>34</v>
+      </c>
       <c r="D47" s="4">
         <v>12.256</v>
       </c>
@@ -3623,10 +3763,22 @@
       <c r="H47" s="4">
         <v>1242.3</v>
       </c>
-    </row>
-    <row r="48" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="I47" s="4">
+        <v>1723.9</v>
+      </c>
+      <c r="J47" s="4">
+        <v>4.5678000000000001</v>
+      </c>
+      <c r="K47" s="3">
+        <v>7.4751000000000003</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" s="12"/>
       <c r="B48" s="15"/>
+      <c r="C48" s="8" t="s">
+        <v>26</v>
+      </c>
       <c r="D48" s="4">
         <v>7.0439999999999996</v>
       </c>
@@ -3642,16 +3794,23 @@
       <c r="H48" s="4">
         <v>1090</v>
       </c>
-    </row>
-    <row r="49" spans="1:20" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I48" s="2">
+        <v>1699.1</v>
+      </c>
+      <c r="J48" s="2">
+        <v>4.5578000000000003</v>
+      </c>
+      <c r="K48" s="1">
+        <v>8.0541</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="13"/>
       <c r="B49" s="16"/>
       <c r="C49" s="7"/>
       <c r="K49" s="6"/>
-      <c r="L49" s="7"/>
-      <c r="T49" s="6"/>
-    </row>
-    <row r="50" spans="1:20" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="50" spans="1:11" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="11">
         <v>1000</v>
       </c>
@@ -3659,55 +3818,53 @@
         <v>6</v>
       </c>
     </row>
-    <row r="51" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51" s="12"/>
       <c r="B51" s="15"/>
     </row>
-    <row r="52" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52" s="12"/>
       <c r="B52" s="15"/>
     </row>
-    <row r="53" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53" s="12"/>
       <c r="B53" s="15"/>
     </row>
-    <row r="54" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54" s="12"/>
       <c r="B54" s="15"/>
     </row>
-    <row r="55" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55" s="12"/>
       <c r="B55" s="15"/>
     </row>
-    <row r="56" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A56" s="12"/>
       <c r="B56" s="15"/>
     </row>
-    <row r="57" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A57" s="12"/>
       <c r="B57" s="15"/>
     </row>
-    <row r="58" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A58" s="12"/>
       <c r="B58" s="15"/>
     </row>
-    <row r="59" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A59" s="12"/>
       <c r="B59" s="15"/>
     </row>
-    <row r="60" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A60" s="12"/>
       <c r="B60" s="15"/>
     </row>
-    <row r="61" spans="1:20" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:11" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="13"/>
       <c r="B61" s="16"/>
       <c r="C61" s="7"/>
       <c r="K61" s="6"/>
-      <c r="L61" s="7"/>
-      <c r="T61" s="6"/>
-    </row>
-    <row r="62" spans="1:20" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="62" spans="1:11" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="11">
         <v>1000</v>
       </c>
@@ -3715,53 +3872,51 @@
         <v>7</v>
       </c>
     </row>
-    <row r="63" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A63" s="12"/>
       <c r="B63" s="15"/>
     </row>
-    <row r="64" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A64" s="12"/>
       <c r="B64" s="15"/>
     </row>
-    <row r="65" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A65" s="12"/>
       <c r="B65" s="15"/>
     </row>
-    <row r="66" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A66" s="12"/>
       <c r="B66" s="15"/>
     </row>
-    <row r="67" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A67" s="12"/>
       <c r="B67" s="15"/>
     </row>
-    <row r="68" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A68" s="12"/>
       <c r="B68" s="15"/>
     </row>
-    <row r="69" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A69" s="12"/>
       <c r="B69" s="15"/>
     </row>
-    <row r="70" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A70" s="12"/>
       <c r="B70" s="15"/>
     </row>
-    <row r="71" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A71" s="12"/>
       <c r="B71" s="15"/>
     </row>
-    <row r="72" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A72" s="12"/>
       <c r="B72" s="15"/>
     </row>
-    <row r="73" spans="1:20" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:11" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="13"/>
       <c r="B73" s="16"/>
       <c r="C73" s="7"/>
       <c r="K73" s="6"/>
-      <c r="L73" s="7"/>
-      <c r="T73" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="12">
@@ -3784,12 +3939,481 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF6E341A-51E3-4AF7-809B-A8594B1323BC}">
+  <dimension ref="A1:K73"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F27" sqref="F27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="4"/>
+    <col min="2" max="2" width="9.140625" style="3"/>
+    <col min="3" max="3" width="15.7109375" style="8" customWidth="1"/>
+    <col min="4" max="10" width="9.140625" style="4"/>
+    <col min="11" max="11" width="9.140625" style="3"/>
+    <col min="12" max="16384" width="9.140625" style="4"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="11">
+        <v>800</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="12"/>
+      <c r="B3" s="15"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="1"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="12"/>
+      <c r="B4" s="15"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="1"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="12"/>
+      <c r="B5" s="15"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
+      <c r="K5" s="1"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="12"/>
+      <c r="B6" s="15"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
+      <c r="K6" s="1"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="12"/>
+      <c r="B7" s="15"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="12"/>
+      <c r="B8" s="15"/>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
+      <c r="K8" s="1"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="12"/>
+      <c r="B9" s="15"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="12"/>
+      <c r="B10" s="15"/>
+      <c r="I10" s="2"/>
+      <c r="J10" s="2"/>
+      <c r="K10" s="1"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="12"/>
+      <c r="B11" s="15"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="12"/>
+      <c r="B12" s="15"/>
+      <c r="I12" s="2"/>
+      <c r="J12" s="2"/>
+      <c r="K12" s="1"/>
+    </row>
+    <row r="13" spans="1:11" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="13"/>
+      <c r="B13" s="16"/>
+      <c r="C13" s="7"/>
+      <c r="K13" s="6"/>
+    </row>
+    <row r="14" spans="1:11" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="11">
+        <v>800</v>
+      </c>
+      <c r="B14" s="14" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" s="12"/>
+      <c r="B15" s="15"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" s="12"/>
+      <c r="B16" s="15"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="2"/>
+      <c r="H16" s="2"/>
+      <c r="I16" s="2"/>
+      <c r="J16" s="2"/>
+      <c r="K16" s="1"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" s="12"/>
+      <c r="B17" s="15"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" s="12"/>
+      <c r="B18" s="15"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" s="12"/>
+      <c r="B19" s="15"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" s="12"/>
+      <c r="B20" s="15"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" s="12"/>
+      <c r="B21" s="15"/>
+      <c r="I21" s="2"/>
+      <c r="J21" s="2"/>
+      <c r="K21" s="1"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" s="12"/>
+      <c r="B22" s="15"/>
+      <c r="I22" s="2"/>
+      <c r="J22" s="2"/>
+      <c r="K22" s="1"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23" s="12"/>
+      <c r="B23" s="15"/>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24" s="12"/>
+      <c r="B24" s="15"/>
+      <c r="I24" s="2"/>
+      <c r="J24" s="2"/>
+      <c r="K24" s="1"/>
+    </row>
+    <row r="25" spans="1:11" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="13"/>
+      <c r="B25" s="16"/>
+      <c r="C25" s="7"/>
+      <c r="K25" s="6"/>
+    </row>
+    <row r="26" spans="1:11" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="11">
+        <v>900</v>
+      </c>
+      <c r="B26" s="14" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A27" s="12"/>
+      <c r="B27" s="15"/>
+      <c r="I27" s="2"/>
+      <c r="J27" s="2"/>
+      <c r="K27" s="1"/>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A28" s="12"/>
+      <c r="B28" s="15"/>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A29" s="12"/>
+      <c r="B29" s="15"/>
+      <c r="I29" s="2"/>
+      <c r="J29" s="2"/>
+      <c r="K29" s="1"/>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A30" s="12"/>
+      <c r="B30" s="15"/>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A31" s="12"/>
+      <c r="B31" s="15"/>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A32" s="12"/>
+      <c r="B32" s="15"/>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A33" s="12"/>
+      <c r="B33" s="15"/>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A34" s="12"/>
+      <c r="B34" s="15"/>
+      <c r="I34" s="2"/>
+      <c r="J34" s="2"/>
+      <c r="K34" s="1"/>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A35" s="12"/>
+      <c r="B35" s="15"/>
+      <c r="I35" s="2"/>
+      <c r="J35" s="2"/>
+      <c r="K35" s="1"/>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A36" s="12"/>
+      <c r="B36" s="15"/>
+    </row>
+    <row r="37" spans="1:11" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="13"/>
+      <c r="B37" s="16"/>
+      <c r="C37" s="7"/>
+      <c r="K37" s="6"/>
+    </row>
+    <row r="38" spans="1:11" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="11">
+        <v>900</v>
+      </c>
+      <c r="B38" s="14" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A39" s="12"/>
+      <c r="B39" s="15"/>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A40" s="12"/>
+      <c r="B40" s="15"/>
+      <c r="I40" s="2"/>
+      <c r="J40" s="2"/>
+      <c r="K40" s="1"/>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A41" s="12"/>
+      <c r="B41" s="15"/>
+      <c r="I41" s="2"/>
+      <c r="J41" s="2"/>
+      <c r="K41" s="1"/>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A42" s="12"/>
+      <c r="B42" s="15"/>
+      <c r="I42" s="2"/>
+      <c r="J42" s="2"/>
+      <c r="K42" s="1"/>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A43" s="12"/>
+      <c r="B43" s="15"/>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A44" s="12"/>
+      <c r="B44" s="15"/>
+      <c r="I44" s="2"/>
+      <c r="J44" s="2"/>
+      <c r="K44" s="1"/>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A45" s="12"/>
+      <c r="B45" s="15"/>
+      <c r="I45" s="2"/>
+      <c r="J45" s="2"/>
+      <c r="K45" s="1"/>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A46" s="12"/>
+      <c r="B46" s="15"/>
+      <c r="I46" s="2"/>
+      <c r="J46" s="2"/>
+      <c r="K46" s="1"/>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A47" s="12"/>
+      <c r="B47" s="15"/>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A48" s="12"/>
+      <c r="B48" s="15"/>
+      <c r="I48" s="2"/>
+      <c r="J48" s="2"/>
+      <c r="K48" s="1"/>
+    </row>
+    <row r="49" spans="1:11" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="13"/>
+      <c r="B49" s="16"/>
+      <c r="C49" s="7"/>
+      <c r="K49" s="6"/>
+    </row>
+    <row r="50" spans="1:11" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="11">
+        <v>1000</v>
+      </c>
+      <c r="B50" s="14" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A51" s="12"/>
+      <c r="B51" s="15"/>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A52" s="12"/>
+      <c r="B52" s="15"/>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A53" s="12"/>
+      <c r="B53" s="15"/>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A54" s="12"/>
+      <c r="B54" s="15"/>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A55" s="12"/>
+      <c r="B55" s="15"/>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A56" s="12"/>
+      <c r="B56" s="15"/>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A57" s="12"/>
+      <c r="B57" s="15"/>
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A58" s="12"/>
+      <c r="B58" s="15"/>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A59" s="12"/>
+      <c r="B59" s="15"/>
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A60" s="12"/>
+      <c r="B60" s="15"/>
+    </row>
+    <row r="61" spans="1:11" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="13"/>
+      <c r="B61" s="16"/>
+      <c r="C61" s="7"/>
+      <c r="K61" s="6"/>
+    </row>
+    <row r="62" spans="1:11" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="11">
+        <v>1000</v>
+      </c>
+      <c r="B62" s="14" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A63" s="12"/>
+      <c r="B63" s="15"/>
+    </row>
+    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A64" s="12"/>
+      <c r="B64" s="15"/>
+    </row>
+    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A65" s="12"/>
+      <c r="B65" s="15"/>
+    </row>
+    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A66" s="12"/>
+      <c r="B66" s="15"/>
+    </row>
+    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A67" s="12"/>
+      <c r="B67" s="15"/>
+    </row>
+    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A68" s="12"/>
+      <c r="B68" s="15"/>
+    </row>
+    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A69" s="12"/>
+      <c r="B69" s="15"/>
+    </row>
+    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A70" s="12"/>
+      <c r="B70" s="15"/>
+    </row>
+    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A71" s="12"/>
+      <c r="B71" s="15"/>
+    </row>
+    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A72" s="12"/>
+      <c r="B72" s="15"/>
+    </row>
+    <row r="73" spans="1:11" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A73" s="13"/>
+      <c r="B73" s="16"/>
+      <c r="C73" s="7"/>
+      <c r="K73" s="6"/>
+    </row>
+  </sheetData>
+  <mergeCells count="12">
+    <mergeCell ref="A38:A49"/>
+    <mergeCell ref="B38:B49"/>
+    <mergeCell ref="A50:A61"/>
+    <mergeCell ref="B50:B61"/>
+    <mergeCell ref="A62:A73"/>
+    <mergeCell ref="B62:B73"/>
+    <mergeCell ref="A2:A13"/>
+    <mergeCell ref="B2:B13"/>
+    <mergeCell ref="A14:A25"/>
+    <mergeCell ref="B14:B25"/>
+    <mergeCell ref="A26:A37"/>
+    <mergeCell ref="B26:B37"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C18A26E-30CA-4E63-A18A-C9C101DAF33C}">
-  <dimension ref="A1:Z73"/>
+  <dimension ref="A1:N73"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D41" sqref="D41"/>
+      <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3799,13 +4423,10 @@
     <col min="3" max="3" width="15.7109375" style="8" customWidth="1"/>
     <col min="4" max="13" width="9.140625" style="4"/>
     <col min="14" max="14" width="9.140625" style="3"/>
-    <col min="15" max="15" width="15.7109375" style="8" customWidth="1"/>
-    <col min="16" max="25" width="9.140625" style="4"/>
-    <col min="26" max="26" width="9.140625" style="3"/>
-    <col min="27" max="16384" width="9.140625" style="4"/>
+    <col min="15" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -3813,7 +4434,7 @@
         <v>11</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>21</v>
+        <v>41</v>
       </c>
       <c r="D1" s="5" t="s">
         <v>1</v>
@@ -3848,44 +4469,8 @@
       <c r="N1" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="O1" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="P1" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="Q1" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="R1" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="S1" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="T1" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="U1" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="V1" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="W1" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="X1" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="Y1" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="Z1" s="6" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:26" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:14" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="11">
         <v>800</v>
       </c>
@@ -3893,11 +4478,11 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="12"/>
       <c r="B3" s="15"/>
       <c r="C3" s="8" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="D3" s="4">
         <v>17.216999999999999</v>
@@ -3929,15 +4514,15 @@
       <c r="M3" s="2">
         <v>0.30907000000000001</v>
       </c>
-      <c r="N3" s="2">
+      <c r="N3" s="1">
         <v>3.3214999999999999</v>
       </c>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="12"/>
       <c r="B4" s="15"/>
       <c r="C4" s="8" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="D4" s="4">
         <v>5.6908000000000003</v>
@@ -3973,7 +4558,7 @@
         <v>2.6046</v>
       </c>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="12"/>
       <c r="B5" s="15"/>
       <c r="D5" s="4">
@@ -3992,7 +4577,7 @@
         <v>1775.9</v>
       </c>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="12"/>
       <c r="B6" s="15"/>
       <c r="D6" s="4">
@@ -4011,7 +4596,7 @@
         <v>1598.4</v>
       </c>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="12"/>
       <c r="B7" s="15"/>
       <c r="D7" s="4">
@@ -4030,7 +4615,7 @@
         <v>1574.3</v>
       </c>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="12"/>
       <c r="B8" s="15"/>
       <c r="D8" s="4">
@@ -4049,7 +4634,7 @@
         <v>1944.6</v>
       </c>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="12"/>
       <c r="B9" s="15"/>
       <c r="D9" s="4">
@@ -4068,7 +4653,7 @@
         <v>2454.8000000000002</v>
       </c>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="12"/>
       <c r="B10" s="15"/>
       <c r="D10" s="4">
@@ -4087,7 +4672,7 @@
         <v>2390.5</v>
       </c>
     </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="12"/>
       <c r="B11" s="15"/>
       <c r="D11" s="4">
@@ -4106,7 +4691,7 @@
         <v>1614.6</v>
       </c>
     </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="12"/>
       <c r="B12" s="15"/>
       <c r="D12" s="4">
@@ -4125,15 +4710,13 @@
         <v>1841</v>
       </c>
     </row>
-    <row r="13" spans="1:26" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="13"/>
       <c r="B13" s="16"/>
       <c r="C13" s="7"/>
       <c r="N13" s="6"/>
-      <c r="O13" s="7"/>
-      <c r="Z13" s="6"/>
-    </row>
-    <row r="14" spans="1:26" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:14" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="11">
         <v>800</v>
       </c>
@@ -4141,11 +4724,11 @@
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="12"/>
       <c r="B15" s="15"/>
       <c r="C15" s="8" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="D15" s="4">
         <v>31.327000000000002</v>
@@ -4181,11 +4764,11 @@
         <v>2.5640000000000001</v>
       </c>
     </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="12"/>
       <c r="B16" s="15"/>
       <c r="C16" s="8" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="D16" s="4">
         <v>22.393000000000001</v>
@@ -4221,7 +4804,7 @@
         <v>2.3807999999999998</v>
       </c>
     </row>
-    <row r="17" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" s="12"/>
       <c r="B17" s="15"/>
       <c r="D17" s="4">
@@ -4240,7 +4823,7 @@
         <v>2221.6</v>
       </c>
     </row>
-    <row r="18" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" s="12"/>
       <c r="B18" s="15"/>
       <c r="D18" s="4">
@@ -4259,7 +4842,7 @@
         <v>3172</v>
       </c>
     </row>
-    <row r="19" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" s="12"/>
       <c r="B19" s="15"/>
       <c r="D19" s="4">
@@ -4278,7 +4861,7 @@
         <v>1677.4</v>
       </c>
     </row>
-    <row r="20" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" s="12"/>
       <c r="B20" s="15"/>
       <c r="D20" s="4">
@@ -4297,7 +4880,7 @@
         <v>1822.6</v>
       </c>
     </row>
-    <row r="21" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" s="12"/>
       <c r="B21" s="15"/>
       <c r="D21" s="4">
@@ -4316,7 +4899,7 @@
         <v>2583</v>
       </c>
     </row>
-    <row r="22" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" s="12"/>
       <c r="B22" s="15"/>
       <c r="D22" s="4">
@@ -4335,7 +4918,7 @@
         <v>2101.3000000000002</v>
       </c>
     </row>
-    <row r="23" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" s="12"/>
       <c r="B23" s="15"/>
       <c r="D23" s="4">
@@ -4354,7 +4937,7 @@
         <v>1707</v>
       </c>
     </row>
-    <row r="24" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" s="12"/>
       <c r="B24" s="15"/>
       <c r="D24" s="4">
@@ -4373,15 +4956,13 @@
         <v>3016.2</v>
       </c>
     </row>
-    <row r="25" spans="1:26" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:14" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="13"/>
       <c r="B25" s="16"/>
       <c r="C25" s="7"/>
       <c r="N25" s="6"/>
-      <c r="O25" s="7"/>
-      <c r="Z25" s="6"/>
-    </row>
-    <row r="26" spans="1:26" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="1:14" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="11">
         <v>900</v>
       </c>
@@ -4389,11 +4970,11 @@
         <v>6</v>
       </c>
     </row>
-    <row r="27" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" s="12"/>
       <c r="B27" s="15"/>
       <c r="C27" s="8" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="D27" s="4">
         <v>4.8710000000000004</v>
@@ -4429,11 +5010,11 @@
         <v>2.5308000000000002</v>
       </c>
     </row>
-    <row r="28" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" s="12"/>
       <c r="B28" s="15"/>
       <c r="C28" s="8" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="D28" s="4">
         <v>10.692</v>
@@ -4469,11 +5050,11 @@
         <v>2.4864000000000002</v>
       </c>
     </row>
-    <row r="29" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29" s="12"/>
       <c r="B29" s="15"/>
       <c r="C29" s="8" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="D29" s="4">
         <v>11.2</v>
@@ -4509,7 +5090,7 @@
         <v>2.4437000000000002</v>
       </c>
     </row>
-    <row r="30" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30" s="12"/>
       <c r="B30" s="15"/>
       <c r="D30" s="4">
@@ -4528,7 +5109,7 @@
         <v>1530.1</v>
       </c>
     </row>
-    <row r="31" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31" s="12"/>
       <c r="B31" s="15"/>
       <c r="D31" s="4">
@@ -4547,7 +5128,7 @@
         <v>1787.3</v>
       </c>
     </row>
-    <row r="32" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32" s="12"/>
       <c r="B32" s="15"/>
       <c r="D32" s="4">
@@ -4566,7 +5147,7 @@
         <v>1593.8</v>
       </c>
     </row>
-    <row r="33" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A33" s="12"/>
       <c r="B33" s="15"/>
       <c r="D33" s="4">
@@ -4585,7 +5166,7 @@
         <v>1000.8</v>
       </c>
     </row>
-    <row r="34" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A34" s="12"/>
       <c r="B34" s="15"/>
       <c r="D34" s="4">
@@ -4604,7 +5185,7 @@
         <v>2110.6</v>
       </c>
     </row>
-    <row r="35" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A35" s="12"/>
       <c r="B35" s="15"/>
       <c r="D35" s="4">
@@ -4623,7 +5204,7 @@
         <v>1210.4000000000001</v>
       </c>
     </row>
-    <row r="36" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A36" s="12"/>
       <c r="B36" s="15"/>
       <c r="D36" s="4">
@@ -4642,15 +5223,13 @@
         <v>1369.1</v>
       </c>
     </row>
-    <row r="37" spans="1:26" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:14" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="13"/>
       <c r="B37" s="16"/>
       <c r="C37" s="7"/>
       <c r="N37" s="6"/>
-      <c r="O37" s="7"/>
-      <c r="Z37" s="6"/>
-    </row>
-    <row r="38" spans="1:26" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="38" spans="1:14" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="11">
         <v>900</v>
       </c>
@@ -4658,11 +5237,11 @@
         <v>7</v>
       </c>
     </row>
-    <row r="39" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A39" s="12"/>
       <c r="B39" s="15"/>
       <c r="C39" s="8" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="D39" s="4">
         <v>4.8238000000000003</v>
@@ -4698,11 +5277,11 @@
         <v>2.5291999999999999</v>
       </c>
     </row>
-    <row r="40" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A40" s="12"/>
       <c r="B40" s="15"/>
       <c r="C40" s="8" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="D40" s="4">
         <v>7.1036999999999999</v>
@@ -4738,11 +5317,11 @@
         <v>2.2601</v>
       </c>
     </row>
-    <row r="41" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A41" s="12"/>
       <c r="B41" s="15"/>
       <c r="C41" s="8" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="D41" s="4">
         <v>3.0461</v>
@@ -4774,11 +5353,11 @@
       <c r="M41" s="2">
         <v>0.25479000000000002</v>
       </c>
-      <c r="N41" s="2">
+      <c r="N41" s="1">
         <v>2.5724</v>
       </c>
     </row>
-    <row r="42" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A42" s="12"/>
       <c r="B42" s="15"/>
       <c r="D42" s="4">
@@ -4797,7 +5376,7 @@
         <v>1999.7</v>
       </c>
     </row>
-    <row r="43" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A43" s="12"/>
       <c r="B43" s="15"/>
       <c r="D43" s="4">
@@ -4816,7 +5395,7 @@
         <v>2606.1999999999998</v>
       </c>
     </row>
-    <row r="44" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A44" s="12"/>
       <c r="B44" s="15"/>
       <c r="D44" s="4">
@@ -4835,7 +5414,7 @@
         <v>1253.9000000000001</v>
       </c>
     </row>
-    <row r="45" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A45" s="12"/>
       <c r="B45" s="15"/>
       <c r="D45" s="4">
@@ -4854,7 +5433,7 @@
         <v>1127.5999999999999</v>
       </c>
     </row>
-    <row r="46" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A46" s="12"/>
       <c r="B46" s="15"/>
       <c r="D46" s="4">
@@ -4873,7 +5452,7 @@
         <v>1371.6</v>
       </c>
     </row>
-    <row r="47" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A47" s="12"/>
       <c r="B47" s="15"/>
       <c r="D47" s="4">
@@ -4892,7 +5471,7 @@
         <v>1242.3</v>
       </c>
     </row>
-    <row r="48" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A48" s="12"/>
       <c r="B48" s="15"/>
       <c r="D48" s="4">
@@ -4911,15 +5490,13 @@
         <v>1090</v>
       </c>
     </row>
-    <row r="49" spans="1:26" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:14" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="13"/>
       <c r="B49" s="16"/>
       <c r="C49" s="7"/>
       <c r="N49" s="6"/>
-      <c r="O49" s="7"/>
-      <c r="Z49" s="6"/>
-    </row>
-    <row r="50" spans="1:26" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="50" spans="1:14" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="11">
         <v>1000</v>
       </c>
@@ -4927,55 +5504,53 @@
         <v>6</v>
       </c>
     </row>
-    <row r="51" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A51" s="12"/>
       <c r="B51" s="15"/>
     </row>
-    <row r="52" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A52" s="12"/>
       <c r="B52" s="15"/>
     </row>
-    <row r="53" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A53" s="12"/>
       <c r="B53" s="15"/>
     </row>
-    <row r="54" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A54" s="12"/>
       <c r="B54" s="15"/>
     </row>
-    <row r="55" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A55" s="12"/>
       <c r="B55" s="15"/>
     </row>
-    <row r="56" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A56" s="12"/>
       <c r="B56" s="15"/>
     </row>
-    <row r="57" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A57" s="12"/>
       <c r="B57" s="15"/>
     </row>
-    <row r="58" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A58" s="12"/>
       <c r="B58" s="15"/>
     </row>
-    <row r="59" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A59" s="12"/>
       <c r="B59" s="15"/>
     </row>
-    <row r="60" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A60" s="12"/>
       <c r="B60" s="15"/>
     </row>
-    <row r="61" spans="1:26" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:14" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="13"/>
       <c r="B61" s="16"/>
       <c r="C61" s="7"/>
       <c r="N61" s="6"/>
-      <c r="O61" s="7"/>
-      <c r="Z61" s="6"/>
-    </row>
-    <row r="62" spans="1:26" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="62" spans="1:14" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="11">
         <v>1000</v>
       </c>
@@ -4983,53 +5558,51 @@
         <v>7</v>
       </c>
     </row>
-    <row r="63" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A63" s="12"/>
       <c r="B63" s="15"/>
     </row>
-    <row r="64" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A64" s="12"/>
       <c r="B64" s="15"/>
     </row>
-    <row r="65" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A65" s="12"/>
       <c r="B65" s="15"/>
     </row>
-    <row r="66" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A66" s="12"/>
       <c r="B66" s="15"/>
     </row>
-    <row r="67" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A67" s="12"/>
       <c r="B67" s="15"/>
     </row>
-    <row r="68" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A68" s="12"/>
       <c r="B68" s="15"/>
     </row>
-    <row r="69" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A69" s="12"/>
       <c r="B69" s="15"/>
     </row>
-    <row r="70" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A70" s="12"/>
       <c r="B70" s="15"/>
     </row>
-    <row r="71" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A71" s="12"/>
       <c r="B71" s="15"/>
     </row>
-    <row r="72" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A72" s="12"/>
       <c r="B72" s="15"/>
     </row>
-    <row r="73" spans="1:26" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:14" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="13"/>
       <c r="B73" s="16"/>
       <c r="C73" s="7"/>
       <c r="N73" s="6"/>
-      <c r="O73" s="7"/>
-      <c r="Z73" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="12">
@@ -5049,4 +5622,423 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F200E048-5FAF-4136-82F6-92204CC50E12}">
+  <dimension ref="A1:N73"/>
+  <sheetViews>
+    <sheetView topLeftCell="B1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="N55" sqref="C3:N55"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="4"/>
+    <col min="2" max="2" width="9.140625" style="3"/>
+    <col min="3" max="3" width="15.7109375" style="8" customWidth="1"/>
+    <col min="4" max="13" width="9.140625" style="4"/>
+    <col min="14" max="14" width="9.140625" style="3"/>
+    <col min="15" max="16384" width="9.140625" style="4"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="L1" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="M1" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="N1" s="6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="11">
+        <v>800</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3" s="12"/>
+      <c r="B3" s="15"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2"/>
+      <c r="N3" s="1"/>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4" s="12"/>
+      <c r="B4" s="15"/>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5" s="12"/>
+      <c r="B5" s="15"/>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6" s="12"/>
+      <c r="B6" s="15"/>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A7" s="12"/>
+      <c r="B7" s="15"/>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A8" s="12"/>
+      <c r="B8" s="15"/>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A9" s="12"/>
+      <c r="B9" s="15"/>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A10" s="12"/>
+      <c r="B10" s="15"/>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A11" s="12"/>
+      <c r="B11" s="15"/>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A12" s="12"/>
+      <c r="B12" s="15"/>
+    </row>
+    <row r="13" spans="1:14" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="13"/>
+      <c r="B13" s="16"/>
+      <c r="C13" s="7"/>
+      <c r="N13" s="6"/>
+    </row>
+    <row r="14" spans="1:14" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="11">
+        <v>800</v>
+      </c>
+      <c r="B14" s="14" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A15" s="12"/>
+      <c r="B15" s="15"/>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A16" s="12"/>
+      <c r="B16" s="15"/>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A17" s="12"/>
+      <c r="B17" s="15"/>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A18" s="12"/>
+      <c r="B18" s="15"/>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A19" s="12"/>
+      <c r="B19" s="15"/>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A20" s="12"/>
+      <c r="B20" s="15"/>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A21" s="12"/>
+      <c r="B21" s="15"/>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A22" s="12"/>
+      <c r="B22" s="15"/>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A23" s="12"/>
+      <c r="B23" s="15"/>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A24" s="12"/>
+      <c r="B24" s="15"/>
+    </row>
+    <row r="25" spans="1:14" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="13"/>
+      <c r="B25" s="16"/>
+      <c r="C25" s="7"/>
+      <c r="N25" s="6"/>
+    </row>
+    <row r="26" spans="1:14" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="11">
+        <v>900</v>
+      </c>
+      <c r="B26" s="14" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A27" s="12"/>
+      <c r="B27" s="15"/>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A28" s="12"/>
+      <c r="B28" s="15"/>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A29" s="12"/>
+      <c r="B29" s="15"/>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A30" s="12"/>
+      <c r="B30" s="15"/>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A31" s="12"/>
+      <c r="B31" s="15"/>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A32" s="12"/>
+      <c r="B32" s="15"/>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A33" s="12"/>
+      <c r="B33" s="15"/>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A34" s="12"/>
+      <c r="B34" s="15"/>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A35" s="12"/>
+      <c r="B35" s="15"/>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A36" s="12"/>
+      <c r="B36" s="15"/>
+    </row>
+    <row r="37" spans="1:14" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="13"/>
+      <c r="B37" s="16"/>
+      <c r="C37" s="7"/>
+      <c r="N37" s="6"/>
+    </row>
+    <row r="38" spans="1:14" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="11">
+        <v>900</v>
+      </c>
+      <c r="B38" s="14" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A39" s="12"/>
+      <c r="B39" s="15"/>
+    </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A40" s="12"/>
+      <c r="B40" s="15"/>
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A41" s="12"/>
+      <c r="B41" s="15"/>
+      <c r="I41" s="2"/>
+      <c r="J41" s="2"/>
+      <c r="K41" s="2"/>
+      <c r="L41" s="2"/>
+      <c r="M41" s="2"/>
+      <c r="N41" s="1"/>
+    </row>
+    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A42" s="12"/>
+      <c r="B42" s="15"/>
+    </row>
+    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A43" s="12"/>
+      <c r="B43" s="15"/>
+    </row>
+    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A44" s="12"/>
+      <c r="B44" s="15"/>
+    </row>
+    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A45" s="12"/>
+      <c r="B45" s="15"/>
+    </row>
+    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A46" s="12"/>
+      <c r="B46" s="15"/>
+    </row>
+    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A47" s="12"/>
+      <c r="B47" s="15"/>
+    </row>
+    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A48" s="12"/>
+      <c r="B48" s="15"/>
+    </row>
+    <row r="49" spans="1:14" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="13"/>
+      <c r="B49" s="16"/>
+      <c r="C49" s="7"/>
+      <c r="N49" s="6"/>
+    </row>
+    <row r="50" spans="1:14" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="11">
+        <v>1000</v>
+      </c>
+      <c r="B50" s="14" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A51" s="12"/>
+      <c r="B51" s="15"/>
+    </row>
+    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A52" s="12"/>
+      <c r="B52" s="15"/>
+    </row>
+    <row r="53" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A53" s="12"/>
+      <c r="B53" s="15"/>
+    </row>
+    <row r="54" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A54" s="12"/>
+      <c r="B54" s="15"/>
+    </row>
+    <row r="55" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A55" s="12"/>
+      <c r="B55" s="15"/>
+    </row>
+    <row r="56" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A56" s="12"/>
+      <c r="B56" s="15"/>
+    </row>
+    <row r="57" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A57" s="12"/>
+      <c r="B57" s="15"/>
+    </row>
+    <row r="58" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A58" s="12"/>
+      <c r="B58" s="15"/>
+    </row>
+    <row r="59" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A59" s="12"/>
+      <c r="B59" s="15"/>
+    </row>
+    <row r="60" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A60" s="12"/>
+      <c r="B60" s="15"/>
+    </row>
+    <row r="61" spans="1:14" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="13"/>
+      <c r="B61" s="16"/>
+      <c r="C61" s="7"/>
+      <c r="N61" s="6"/>
+    </row>
+    <row r="62" spans="1:14" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="11">
+        <v>1000</v>
+      </c>
+      <c r="B62" s="14" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="63" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A63" s="12"/>
+      <c r="B63" s="15"/>
+    </row>
+    <row r="64" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A64" s="12"/>
+      <c r="B64" s="15"/>
+    </row>
+    <row r="65" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A65" s="12"/>
+      <c r="B65" s="15"/>
+    </row>
+    <row r="66" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A66" s="12"/>
+      <c r="B66" s="15"/>
+    </row>
+    <row r="67" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A67" s="12"/>
+      <c r="B67" s="15"/>
+    </row>
+    <row r="68" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A68" s="12"/>
+      <c r="B68" s="15"/>
+    </row>
+    <row r="69" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A69" s="12"/>
+      <c r="B69" s="15"/>
+    </row>
+    <row r="70" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A70" s="12"/>
+      <c r="B70" s="15"/>
+    </row>
+    <row r="71" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A71" s="12"/>
+      <c r="B71" s="15"/>
+    </row>
+    <row r="72" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A72" s="12"/>
+      <c r="B72" s="15"/>
+    </row>
+    <row r="73" spans="1:14" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A73" s="13"/>
+      <c r="B73" s="16"/>
+      <c r="C73" s="7"/>
+      <c r="N73" s="6"/>
+    </row>
+  </sheetData>
+  <mergeCells count="12">
+    <mergeCell ref="A38:A49"/>
+    <mergeCell ref="B38:B49"/>
+    <mergeCell ref="A50:A61"/>
+    <mergeCell ref="B50:B61"/>
+    <mergeCell ref="A62:A73"/>
+    <mergeCell ref="B62:B73"/>
+    <mergeCell ref="A2:A13"/>
+    <mergeCell ref="B2:B13"/>
+    <mergeCell ref="A14:A25"/>
+    <mergeCell ref="B14:B25"/>
+    <mergeCell ref="A26:A37"/>
+    <mergeCell ref="B26:B37"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added plots to sem results file
</commit_message>
<xml_diff>
--- a/scripts/__other__/__sem__.xlsx
+++ b/scripts/__other__/__sem__.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Janzen\Desktop\code\moga_neml\scripts\__other__\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78F71341-3985-4116-810B-071D967FF693}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B06DF333-E249-400A-9303-E1900F0A075E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="evp" sheetId="13" r:id="rId1"/>
@@ -892,6 +892,539 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>104775</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{69DA5A1B-9569-10C7-25ED-AEFDF30D9B72}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7172325" y="247650"/>
+          <a:ext cx="1905000" cy="1905000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>85725</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{056B1923-F0F7-F1B1-2A73-0F28E2460C60}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9058275" y="219075"/>
+          <a:ext cx="1933575" cy="1933575"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>262559</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>22777</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>431288</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>161855</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{964D8901-33E2-3935-18FE-CC641ECC7028}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11121059" y="213277"/>
+          <a:ext cx="3846207" cy="1911556"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>41412</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>24849</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>157369</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>16567</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{401E5F7B-6B7F-D60D-61D0-2F1E8C2EF3BD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7222434" y="2236306"/>
+          <a:ext cx="1954696" cy="1954696"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>140805</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>24847</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>256761</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>16564</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CB670FC0-93B5-7858-2032-A705893DEFDA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9160566" y="2236304"/>
+          <a:ext cx="1954695" cy="1954695"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>231913</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>33131</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>437030</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>11379</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Picture 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{85D7DDE1-3557-9427-671D-BA5F0BD620E4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10967148" y="2240690"/>
+          <a:ext cx="3835823" cy="1939277"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>51290</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>21981</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>183174</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>14654</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Picture 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CF01C1FA-1538-022B-312D-27EA77492DDC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7180386" y="4256943"/>
+          <a:ext cx="1956288" cy="1956288"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>314740</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>49696</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>439312</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>177363</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="10" name="Picture 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8F59AE14-82C2-67E5-4773-BDE18467080D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11140395" y="4286679"/>
+          <a:ext cx="3790055" cy="1901287"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>39412</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>39413</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>137947</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>6569</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="12" name="Picture 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CD96A227-EBA0-8DE0-C6F6-8E9DF1DD2499}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7199584" y="6299637"/>
+          <a:ext cx="1931277" cy="1931277"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>151087</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>32845</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>271097</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>21726</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="13" name="Picture 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D6127B03-D0C1-9321-6F47-4FCD42443831}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9104587" y="6290037"/>
+          <a:ext cx="1944414" cy="1952497"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>285292</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>30682</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>476249</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>176551</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="14" name="Picture 13">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{391005F3-D050-42A5-B95F-F0584C9591C8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11048542" y="6293370"/>
+          <a:ext cx="3834270" cy="1919900"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>172639</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>53578</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>291702</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>29766</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="15" name="Picture 14">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9DC7C34D-24B9-5EB5-99C1-EAA5E9BDE018}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId12"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9114233" y="4292203"/>
+          <a:ext cx="1940719" cy="1940719"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -2464,9 +2997,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE483CC8-AF2C-4D5A-AEE5-EF7DF4EC0883}">
   <dimension ref="A1:K73"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D35" sqref="D35"/>
+      <selection pane="bottomLeft" activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3935,6 +4468,7 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -3942,7 +4476,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF6E341A-51E3-4AF7-809B-A8594B1323BC}">
   <dimension ref="A1:K73"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="F27" sqref="F27"/>
     </sheetView>

</xml_diff>

<commit_message>
Added new plots to sem results file
</commit_message>
<xml_diff>
--- a/scripts/__other__/__sem__.xlsx
+++ b/scripts/__other__/__sem__.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Janzen\Desktop\code\moga_neml\scripts\__other__\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B06DF333-E249-400A-9303-E1900F0A075E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8379F356-40C3-4408-8E0F-5F5EA10845C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -363,366 +363,14 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>91110</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>52224</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>157370</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>184745</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F0F901CE-1434-B384-7F73-CFA7D97B9B3D}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="7537175" y="242724"/>
-          <a:ext cx="1904999" cy="1904999"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>140806</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>55084</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>196802</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>177341</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{04ED5CA5-5DE3-9849-0C0A-E308227FE011}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="9425610" y="245584"/>
-          <a:ext cx="1894735" cy="1894735"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>49697</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>38684</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>115958</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>171206</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Picture 3">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{48B2C33C-EE1B-BE9F-8E6D-A431558E4B96}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="7495762" y="2250141"/>
-          <a:ext cx="1905000" cy="1905000"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>115959</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>50347</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>182222</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>182871</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="5" name="Picture 4">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5B1D8717-2C25-526A-5E72-1C31CF079EF3}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="9400763" y="2261804"/>
-          <a:ext cx="1905002" cy="1905002"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>56793</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>49159</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>149088</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>17215</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="6" name="Picture 5">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8C257DB0-555A-73C5-3B81-7069D962C0A2}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="7502858" y="4281572"/>
-          <a:ext cx="1931034" cy="1931034"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>157372</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>47782</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>258461</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>24632</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="7" name="Picture 6">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{56307D0B-D72F-5816-98E6-F87F6C0734A7}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="9442176" y="4280195"/>
-          <a:ext cx="1939828" cy="1939828"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>69809</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>50057</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>152170</xdr:colOff>
-      <xdr:row>48</xdr:row>
-      <xdr:rowOff>8179</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="8" name="Picture 7">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BA886998-B57F-CD0F-41AB-D9F969D1F9E9}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="7515874" y="6303427"/>
-          <a:ext cx="1921100" cy="1921100"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>149087</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>56062</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>240196</xdr:colOff>
-      <xdr:row>48</xdr:row>
-      <xdr:rowOff>22932</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="9" name="Picture 8">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8D1F3CBC-D163-4B80-A0A6-CAD68A079AC2}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="9433891" y="6309432"/>
-          <a:ext cx="1929848" cy="1929848"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>182217</xdr:colOff>
+      <xdr:colOff>204198</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>49698</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>24</xdr:col>
-      <xdr:colOff>323021</xdr:colOff>
+      <xdr:colOff>345002</xdr:colOff>
       <xdr:row>11</xdr:row>
       <xdr:rowOff>186362</xdr:rowOff>
     </xdr:to>
@@ -740,15 +388,15 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="11305760" y="240198"/>
-          <a:ext cx="3818283" cy="1909142"/>
+          <a:off x="13348698" y="240198"/>
+          <a:ext cx="3789612" cy="1909779"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -784,7 +432,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -828,7 +476,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -872,7 +520,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId12"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -881,6 +529,358 @@
         <a:xfrm>
           <a:off x="11306175" y="6305550"/>
           <a:ext cx="3829050" cy="1914525"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>65943</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>161192</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>14653</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="14" name="Picture 13">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3C07A6C5-78ED-25E8-5E02-FD43AB5A2D69}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9561635" y="249115"/>
+          <a:ext cx="1919653" cy="1919653"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>87925</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>36634</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>212481</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>21979</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="15" name="Picture 14">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1119B891-843A-59E6-A84D-EF4025013A32}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11408021" y="227134"/>
+          <a:ext cx="1948960" cy="1948960"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>45902</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>33618</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>171450</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>16333</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="16" name="Picture 15">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4B1D1A6F-68FF-39A6-0FD4-F47C0D14BDCD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9551852" y="2243418"/>
+          <a:ext cx="1954348" cy="1944865"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>131885</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>31506</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>178868</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="17" name="Picture 16">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4FF3334C-8450-409E-C836-7337AD330FDD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11466635" y="2241306"/>
+          <a:ext cx="1925515" cy="1919012"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>49091</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>46894</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>1423</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="18" name="Picture 17">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{92A243BE-C9FD-9A1F-16BF-4DF0AA2AF7E2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9555041" y="4275994"/>
+          <a:ext cx="1922584" cy="1916679"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>116498</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>25646</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>238125</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>10324</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="19" name="Picture 18">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E0102139-6119-B4CF-C6F7-EC31C7714E33}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11451248" y="4254746"/>
+          <a:ext cx="1950427" cy="1946828"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>38099</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>19049</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>133350</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="20" name="Picture 19">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{43F263AF-9D67-305A-04A9-D26BB2EA9F71}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9544049" y="6267449"/>
+          <a:ext cx="1924051" cy="1924051"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="21" name="Picture 20">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{71E7E10A-A351-D44A-2886-D8BC97424D5E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId12"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11410950" y="6286500"/>
+          <a:ext cx="1943100" cy="1943100"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1690,9 +1690,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4D7A15E-4182-42F6-82DA-99E9B04906BA}">
   <dimension ref="A1:Q73"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
+      <selection pane="bottomLeft" activeCell="K35" sqref="K35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2997,8 +2997,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE483CC8-AF2C-4D5A-AEE5-EF7DF4EC0883}">
   <dimension ref="A1:K73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Added opt_err output and new params for evpcd_i
</commit_message>
<xml_diff>
--- a/scripts/__other__/__sem__.xlsx
+++ b/scripts/__other__/__sem__.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Janzen\Desktop\code\moga_neml\scripts\__other__\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8379F356-40C3-4408-8E0F-5F5EA10845C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F65C60E-29C5-429C-8D64-B672A93A17B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="45">
   <si>
     <t>temp</t>
   </si>
@@ -198,7 +198,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -288,11 +288,22 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -323,6 +334,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1745,16 +1759,16 @@
       </c>
     </row>
     <row r="2" spans="1:12" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="11">
+      <c r="A2" s="12">
         <v>800</v>
       </c>
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="15" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="12"/>
-      <c r="B3" s="15"/>
+      <c r="A3" s="13"/>
+      <c r="B3" s="16"/>
       <c r="C3" s="8" t="s">
         <v>18</v>
       </c>
@@ -1781,8 +1795,8 @@
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="12"/>
-      <c r="B4" s="15"/>
+      <c r="A4" s="13"/>
+      <c r="B4" s="16"/>
       <c r="C4" s="8" t="s">
         <v>18</v>
       </c>
@@ -1809,8 +1823,8 @@
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" s="12"/>
-      <c r="B5" s="15"/>
+      <c r="A5" s="13"/>
+      <c r="B5" s="16"/>
       <c r="C5" s="8" t="s">
         <v>18</v>
       </c>
@@ -1834,8 +1848,8 @@
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="12"/>
-      <c r="B6" s="15"/>
+      <c r="A6" s="13"/>
+      <c r="B6" s="16"/>
       <c r="C6" s="8" t="s">
         <v>18</v>
       </c>
@@ -1859,8 +1873,8 @@
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="12"/>
-      <c r="B7" s="15"/>
+      <c r="A7" s="13"/>
+      <c r="B7" s="16"/>
       <c r="C7" s="8" t="s">
         <v>18</v>
       </c>
@@ -1884,8 +1898,8 @@
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" s="12"/>
-      <c r="B8" s="15"/>
+      <c r="A8" s="13"/>
+      <c r="B8" s="16"/>
       <c r="C8" s="8" t="s">
         <v>19</v>
       </c>
@@ -1909,8 +1923,8 @@
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" s="12"/>
-      <c r="B9" s="15"/>
+      <c r="A9" s="13"/>
+      <c r="B9" s="16"/>
       <c r="C9" s="8" t="s">
         <v>19</v>
       </c>
@@ -1934,8 +1948,8 @@
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" s="12"/>
-      <c r="B10" s="15"/>
+      <c r="A10" s="13"/>
+      <c r="B10" s="16"/>
       <c r="C10" s="8" t="s">
         <v>18</v>
       </c>
@@ -1959,8 +1973,8 @@
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" s="12"/>
-      <c r="B11" s="15"/>
+      <c r="A11" s="13"/>
+      <c r="B11" s="16"/>
       <c r="C11" s="8" t="s">
         <v>20</v>
       </c>
@@ -1984,8 +1998,8 @@
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" s="12"/>
-      <c r="B12" s="15"/>
+      <c r="A12" s="13"/>
+      <c r="B12" s="16"/>
       <c r="C12" s="8" t="s">
         <v>21</v>
       </c>
@@ -2009,8 +2023,8 @@
       </c>
     </row>
     <row r="13" spans="1:12" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="13"/>
-      <c r="B13" s="16"/>
+      <c r="A13" s="14"/>
+      <c r="B13" s="17"/>
       <c r="C13" s="7"/>
       <c r="H13" s="6"/>
       <c r="I13" s="7"/>
@@ -2019,16 +2033,16 @@
       <c r="L13" s="7"/>
     </row>
     <row r="14" spans="1:12" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="11">
+      <c r="A14" s="12">
         <v>800</v>
       </c>
-      <c r="B14" s="14" t="s">
+      <c r="B14" s="15" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A15" s="12"/>
-      <c r="B15" s="15"/>
+      <c r="A15" s="13"/>
+      <c r="B15" s="16"/>
       <c r="C15" s="8" t="s">
         <v>22</v>
       </c>
@@ -2055,8 +2069,8 @@
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A16" s="12"/>
-      <c r="B16" s="15"/>
+      <c r="A16" s="13"/>
+      <c r="B16" s="16"/>
       <c r="C16" s="8" t="s">
         <v>18</v>
       </c>
@@ -2083,8 +2097,8 @@
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A17" s="12"/>
-      <c r="B17" s="15"/>
+      <c r="A17" s="13"/>
+      <c r="B17" s="16"/>
       <c r="C17" s="8" t="s">
         <v>23</v>
       </c>
@@ -2108,8 +2122,8 @@
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A18" s="12"/>
-      <c r="B18" s="15"/>
+      <c r="A18" s="13"/>
+      <c r="B18" s="16"/>
       <c r="C18" s="8" t="s">
         <v>24</v>
       </c>
@@ -2133,8 +2147,8 @@
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A19" s="12"/>
-      <c r="B19" s="15"/>
+      <c r="A19" s="13"/>
+      <c r="B19" s="16"/>
       <c r="C19" s="8" t="s">
         <v>19</v>
       </c>
@@ -2158,8 +2172,8 @@
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A20" s="12"/>
-      <c r="B20" s="15"/>
+      <c r="A20" s="13"/>
+      <c r="B20" s="16"/>
       <c r="C20" s="8" t="s">
         <v>19</v>
       </c>
@@ -2183,8 +2197,8 @@
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A21" s="12"/>
-      <c r="B21" s="15"/>
+      <c r="A21" s="13"/>
+      <c r="B21" s="16"/>
       <c r="C21" s="8" t="s">
         <v>25</v>
       </c>
@@ -2208,8 +2222,8 @@
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A22" s="12"/>
-      <c r="B22" s="15"/>
+      <c r="A22" s="13"/>
+      <c r="B22" s="16"/>
       <c r="C22" s="8" t="s">
         <v>25</v>
       </c>
@@ -2233,8 +2247,8 @@
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A23" s="12"/>
-      <c r="B23" s="15"/>
+      <c r="A23" s="13"/>
+      <c r="B23" s="16"/>
       <c r="C23" s="8" t="s">
         <v>18</v>
       </c>
@@ -2258,8 +2272,8 @@
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A24" s="12"/>
-      <c r="B24" s="15"/>
+      <c r="A24" s="13"/>
+      <c r="B24" s="16"/>
       <c r="C24" s="8" t="s">
         <v>20</v>
       </c>
@@ -2283,8 +2297,8 @@
       </c>
     </row>
     <row r="25" spans="1:12" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="13"/>
-      <c r="B25" s="16"/>
+      <c r="A25" s="14"/>
+      <c r="B25" s="17"/>
       <c r="C25" s="7"/>
       <c r="H25" s="6"/>
       <c r="I25" s="7"/>
@@ -2293,16 +2307,16 @@
       <c r="L25" s="7"/>
     </row>
     <row r="26" spans="1:12" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="11">
+      <c r="A26" s="12">
         <v>900</v>
       </c>
-      <c r="B26" s="14" t="s">
+      <c r="B26" s="15" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A27" s="12"/>
-      <c r="B27" s="15"/>
+      <c r="A27" s="13"/>
+      <c r="B27" s="16"/>
       <c r="C27" s="8" t="s">
         <v>18</v>
       </c>
@@ -2329,8 +2343,8 @@
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A28" s="12"/>
-      <c r="B28" s="15"/>
+      <c r="A28" s="13"/>
+      <c r="B28" s="16"/>
       <c r="C28" s="8" t="s">
         <v>18</v>
       </c>
@@ -2357,8 +2371,8 @@
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A29" s="12"/>
-      <c r="B29" s="15"/>
+      <c r="A29" s="13"/>
+      <c r="B29" s="16"/>
       <c r="C29" s="8" t="s">
         <v>27</v>
       </c>
@@ -2385,8 +2399,8 @@
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A30" s="12"/>
-      <c r="B30" s="15"/>
+      <c r="A30" s="13"/>
+      <c r="B30" s="16"/>
       <c r="C30" s="8" t="s">
         <v>18</v>
       </c>
@@ -2410,8 +2424,8 @@
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A31" s="12"/>
-      <c r="B31" s="15"/>
+      <c r="A31" s="13"/>
+      <c r="B31" s="16"/>
       <c r="C31" s="8" t="s">
         <v>20</v>
       </c>
@@ -2435,8 +2449,8 @@
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A32" s="12"/>
-      <c r="B32" s="15"/>
+      <c r="A32" s="13"/>
+      <c r="B32" s="16"/>
       <c r="C32" s="8" t="s">
         <v>18</v>
       </c>
@@ -2460,8 +2474,8 @@
       </c>
     </row>
     <row r="33" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A33" s="12"/>
-      <c r="B33" s="15"/>
+      <c r="A33" s="13"/>
+      <c r="B33" s="16"/>
       <c r="C33" s="8" t="s">
         <v>28</v>
       </c>
@@ -2485,8 +2499,8 @@
       </c>
     </row>
     <row r="34" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A34" s="12"/>
-      <c r="B34" s="15"/>
+      <c r="A34" s="13"/>
+      <c r="B34" s="16"/>
       <c r="C34" s="8" t="s">
         <v>19</v>
       </c>
@@ -2510,8 +2524,8 @@
       </c>
     </row>
     <row r="35" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A35" s="12"/>
-      <c r="B35" s="15"/>
+      <c r="A35" s="13"/>
+      <c r="B35" s="16"/>
       <c r="C35" s="8" t="s">
         <v>18</v>
       </c>
@@ -2535,8 +2549,8 @@
       </c>
     </row>
     <row r="36" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A36" s="12"/>
-      <c r="B36" s="15"/>
+      <c r="A36" s="13"/>
+      <c r="B36" s="16"/>
       <c r="C36" s="8" t="s">
         <v>21</v>
       </c>
@@ -2560,8 +2574,8 @@
       </c>
     </row>
     <row r="37" spans="1:17" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="13"/>
-      <c r="B37" s="16"/>
+      <c r="A37" s="14"/>
+      <c r="B37" s="17"/>
       <c r="C37" s="7"/>
       <c r="H37" s="6"/>
       <c r="I37" s="7"/>
@@ -2570,16 +2584,16 @@
       <c r="L37" s="7"/>
     </row>
     <row r="38" spans="1:17" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="11">
+      <c r="A38" s="12">
         <v>900</v>
       </c>
-      <c r="B38" s="14" t="s">
+      <c r="B38" s="15" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="39" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A39" s="12"/>
-      <c r="B39" s="15"/>
+      <c r="A39" s="13"/>
+      <c r="B39" s="16"/>
       <c r="C39" s="8" t="s">
         <v>21</v>
       </c>
@@ -2611,8 +2625,8 @@
       <c r="Q39" s="2"/>
     </row>
     <row r="40" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A40" s="12"/>
-      <c r="B40" s="15"/>
+      <c r="A40" s="13"/>
+      <c r="B40" s="16"/>
       <c r="C40" s="8" t="s">
         <v>29</v>
       </c>
@@ -2644,8 +2658,8 @@
       <c r="Q40" s="2"/>
     </row>
     <row r="41" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A41" s="12"/>
-      <c r="B41" s="15"/>
+      <c r="A41" s="13"/>
+      <c r="B41" s="16"/>
       <c r="C41" s="8" t="s">
         <v>25</v>
       </c>
@@ -2672,8 +2686,8 @@
       </c>
     </row>
     <row r="42" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A42" s="12"/>
-      <c r="B42" s="15"/>
+      <c r="A42" s="13"/>
+      <c r="B42" s="16"/>
       <c r="C42" s="8" t="s">
         <v>26</v>
       </c>
@@ -2697,8 +2711,8 @@
       </c>
     </row>
     <row r="43" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A43" s="12"/>
-      <c r="B43" s="15"/>
+      <c r="A43" s="13"/>
+      <c r="B43" s="16"/>
       <c r="C43" s="8" t="s">
         <v>34</v>
       </c>
@@ -2722,8 +2736,8 @@
       </c>
     </row>
     <row r="44" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A44" s="12"/>
-      <c r="B44" s="15"/>
+      <c r="A44" s="13"/>
+      <c r="B44" s="16"/>
       <c r="C44" s="8" t="s">
         <v>18</v>
       </c>
@@ -2747,8 +2761,8 @@
       </c>
     </row>
     <row r="45" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A45" s="12"/>
-      <c r="B45" s="15"/>
+      <c r="A45" s="13"/>
+      <c r="B45" s="16"/>
       <c r="C45" s="8" t="s">
         <v>18</v>
       </c>
@@ -2772,8 +2786,8 @@
       </c>
     </row>
     <row r="46" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A46" s="12"/>
-      <c r="B46" s="15"/>
+      <c r="A46" s="13"/>
+      <c r="B46" s="16"/>
       <c r="C46" s="8" t="s">
         <v>18</v>
       </c>
@@ -2797,8 +2811,8 @@
       </c>
     </row>
     <row r="47" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A47" s="12"/>
-      <c r="B47" s="15"/>
+      <c r="A47" s="13"/>
+      <c r="B47" s="16"/>
       <c r="C47" s="8" t="s">
         <v>21</v>
       </c>
@@ -2822,8 +2836,8 @@
       </c>
     </row>
     <row r="48" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A48" s="12"/>
-      <c r="B48" s="15"/>
+      <c r="A48" s="13"/>
+      <c r="B48" s="16"/>
       <c r="C48" s="8" t="s">
         <v>19</v>
       </c>
@@ -2847,8 +2861,8 @@
       </c>
     </row>
     <row r="49" spans="1:12" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="13"/>
-      <c r="B49" s="16"/>
+      <c r="A49" s="14"/>
+      <c r="B49" s="17"/>
       <c r="C49" s="7"/>
       <c r="H49" s="6"/>
       <c r="I49" s="7"/>
@@ -2857,56 +2871,56 @@
       <c r="L49" s="7"/>
     </row>
     <row r="50" spans="1:12" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="11">
+      <c r="A50" s="12">
         <v>1000</v>
       </c>
-      <c r="B50" s="14" t="s">
+      <c r="B50" s="15" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="51" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A51" s="12"/>
-      <c r="B51" s="15"/>
+      <c r="A51" s="13"/>
+      <c r="B51" s="16"/>
     </row>
     <row r="52" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A52" s="12"/>
-      <c r="B52" s="15"/>
+      <c r="A52" s="13"/>
+      <c r="B52" s="16"/>
     </row>
     <row r="53" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A53" s="12"/>
-      <c r="B53" s="15"/>
+      <c r="A53" s="13"/>
+      <c r="B53" s="16"/>
     </row>
     <row r="54" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A54" s="12"/>
-      <c r="B54" s="15"/>
+      <c r="A54" s="13"/>
+      <c r="B54" s="16"/>
     </row>
     <row r="55" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A55" s="12"/>
-      <c r="B55" s="15"/>
+      <c r="A55" s="13"/>
+      <c r="B55" s="16"/>
     </row>
     <row r="56" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A56" s="12"/>
-      <c r="B56" s="15"/>
+      <c r="A56" s="13"/>
+      <c r="B56" s="16"/>
     </row>
     <row r="57" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A57" s="12"/>
-      <c r="B57" s="15"/>
+      <c r="A57" s="13"/>
+      <c r="B57" s="16"/>
     </row>
     <row r="58" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A58" s="12"/>
-      <c r="B58" s="15"/>
+      <c r="A58" s="13"/>
+      <c r="B58" s="16"/>
     </row>
     <row r="59" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A59" s="12"/>
-      <c r="B59" s="15"/>
+      <c r="A59" s="13"/>
+      <c r="B59" s="16"/>
     </row>
     <row r="60" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A60" s="12"/>
-      <c r="B60" s="15"/>
+      <c r="A60" s="13"/>
+      <c r="B60" s="16"/>
     </row>
     <row r="61" spans="1:12" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="13"/>
-      <c r="B61" s="16"/>
+      <c r="A61" s="14"/>
+      <c r="B61" s="17"/>
       <c r="C61" s="7"/>
       <c r="H61" s="6"/>
       <c r="I61" s="7"/>
@@ -2915,56 +2929,56 @@
       <c r="L61" s="7"/>
     </row>
     <row r="62" spans="1:12" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="11">
+      <c r="A62" s="12">
         <v>1000</v>
       </c>
-      <c r="B62" s="14" t="s">
+      <c r="B62" s="15" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="63" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A63" s="12"/>
-      <c r="B63" s="15"/>
+      <c r="A63" s="13"/>
+      <c r="B63" s="16"/>
     </row>
     <row r="64" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A64" s="12"/>
-      <c r="B64" s="15"/>
+      <c r="A64" s="13"/>
+      <c r="B64" s="16"/>
     </row>
     <row r="65" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A65" s="12"/>
-      <c r="B65" s="15"/>
+      <c r="A65" s="13"/>
+      <c r="B65" s="16"/>
     </row>
     <row r="66" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A66" s="12"/>
-      <c r="B66" s="15"/>
+      <c r="A66" s="13"/>
+      <c r="B66" s="16"/>
     </row>
     <row r="67" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A67" s="12"/>
-      <c r="B67" s="15"/>
+      <c r="A67" s="13"/>
+      <c r="B67" s="16"/>
     </row>
     <row r="68" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A68" s="12"/>
-      <c r="B68" s="15"/>
+      <c r="A68" s="13"/>
+      <c r="B68" s="16"/>
     </row>
     <row r="69" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A69" s="12"/>
-      <c r="B69" s="15"/>
+      <c r="A69" s="13"/>
+      <c r="B69" s="16"/>
     </row>
     <row r="70" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A70" s="12"/>
-      <c r="B70" s="15"/>
+      <c r="A70" s="13"/>
+      <c r="B70" s="16"/>
     </row>
     <row r="71" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A71" s="12"/>
-      <c r="B71" s="15"/>
+      <c r="A71" s="13"/>
+      <c r="B71" s="16"/>
     </row>
     <row r="72" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A72" s="12"/>
-      <c r="B72" s="15"/>
+      <c r="A72" s="13"/>
+      <c r="B72" s="16"/>
     </row>
     <row r="73" spans="1:12" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="13"/>
-      <c r="B73" s="16"/>
+      <c r="A73" s="14"/>
+      <c r="B73" s="17"/>
       <c r="C73" s="7"/>
       <c r="H73" s="6"/>
       <c r="I73" s="7"/>
@@ -2995,11 +3009,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE483CC8-AF2C-4D5A-AEE5-EF7DF4EC0883}">
-  <dimension ref="A1:K73"/>
+  <dimension ref="A1:L73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D31" sqref="D31"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G59" sqref="G59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3007,12 +3021,12 @@
     <col min="1" max="1" width="9.140625" style="4"/>
     <col min="2" max="2" width="9.140625" style="3"/>
     <col min="3" max="3" width="15.7109375" style="8" customWidth="1"/>
-    <col min="4" max="10" width="9.140625" style="4"/>
-    <col min="11" max="11" width="9.140625" style="3"/>
-    <col min="12" max="16384" width="9.140625" style="4"/>
+    <col min="4" max="11" width="9.140625" style="4"/>
+    <col min="12" max="12" width="9.140625" style="9"/>
+    <col min="13" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -3043,23 +3057,24 @@
       <c r="J1" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="6" t="s">
+      <c r="K1" s="5" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="11">
+      <c r="L1" s="11"/>
+    </row>
+    <row r="2" spans="1:12" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="12">
         <v>800</v>
       </c>
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="15" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="12"/>
-      <c r="B3" s="15"/>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" s="13"/>
+      <c r="B3" s="16"/>
       <c r="C3" s="8" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="D3" s="4">
         <v>17.216999999999999</v>
@@ -3082,15 +3097,15 @@
       <c r="J3" s="2">
         <v>4.8244999999999996</v>
       </c>
-      <c r="K3" s="1">
+      <c r="K3" s="2">
         <v>6.6364000000000001</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="12"/>
-      <c r="B4" s="15"/>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" s="13"/>
+      <c r="B4" s="16"/>
       <c r="C4" s="8" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="D4" s="4">
         <v>5.6908000000000003</v>
@@ -3108,18 +3123,18 @@
         <v>1621.6</v>
       </c>
       <c r="I4" s="2">
-        <v>1960.8</v>
+        <v>1995</v>
       </c>
       <c r="J4" s="2">
-        <v>5.4898999999999996</v>
-      </c>
-      <c r="K4" s="1">
-        <v>7.0751999999999997</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="12"/>
-      <c r="B5" s="15"/>
+        <v>5.4751000000000003</v>
+      </c>
+      <c r="K4" s="2">
+        <v>6.6859999999999999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" s="13"/>
+      <c r="B5" s="16"/>
       <c r="C5" s="8" t="s">
         <v>20</v>
       </c>
@@ -3144,13 +3159,13 @@
       <c r="J5" s="2">
         <v>5.0411999999999999</v>
       </c>
-      <c r="K5" s="1">
+      <c r="K5" s="2">
         <v>9.5797000000000008</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="12"/>
-      <c r="B6" s="15"/>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" s="13"/>
+      <c r="B6" s="16"/>
       <c r="C6" s="8" t="s">
         <v>20</v>
       </c>
@@ -3175,13 +3190,13 @@
       <c r="J6" s="2">
         <v>5.2808999999999999</v>
       </c>
-      <c r="K6" s="1">
+      <c r="K6" s="2">
         <v>6.7355</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="12"/>
-      <c r="B7" s="15"/>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" s="13"/>
+      <c r="B7" s="16"/>
       <c r="C7" s="8" t="s">
         <v>26</v>
       </c>
@@ -3206,13 +3221,13 @@
       <c r="J7" s="4">
         <v>4.8533999999999997</v>
       </c>
-      <c r="K7" s="3">
+      <c r="K7" s="4">
         <v>4.6837</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="12"/>
-      <c r="B8" s="15"/>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" s="13"/>
+      <c r="B8" s="16"/>
       <c r="C8" s="8" t="s">
         <v>19</v>
       </c>
@@ -3237,13 +3252,13 @@
       <c r="J8" s="2">
         <v>5.1295999999999999</v>
       </c>
-      <c r="K8" s="1">
+      <c r="K8" s="2">
         <v>10.247999999999999</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="12"/>
-      <c r="B9" s="15"/>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" s="13"/>
+      <c r="B9" s="16"/>
       <c r="C9" s="8" t="s">
         <v>25</v>
       </c>
@@ -3268,13 +3283,13 @@
       <c r="J9" s="4">
         <v>4.9866999999999999</v>
       </c>
-      <c r="K9" s="3">
+      <c r="K9" s="4">
         <v>10.836</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="12"/>
-      <c r="B10" s="15"/>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" s="13"/>
+      <c r="B10" s="16"/>
       <c r="C10" s="8" t="s">
         <v>19</v>
       </c>
@@ -3299,13 +3314,13 @@
       <c r="J10" s="2">
         <v>5.0381999999999998</v>
       </c>
-      <c r="K10" s="1">
+      <c r="K10" s="2">
         <v>7.7606999999999999</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="12"/>
-      <c r="B11" s="15"/>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" s="13"/>
+      <c r="B11" s="16"/>
       <c r="C11" s="8" t="s">
         <v>38</v>
       </c>
@@ -3330,13 +3345,13 @@
       <c r="J11" s="4">
         <v>5.5552000000000001</v>
       </c>
-      <c r="K11" s="3">
+      <c r="K11" s="4">
         <v>8.4002999999999997</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="12"/>
-      <c r="B12" s="15"/>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" s="13"/>
+      <c r="B12" s="16"/>
       <c r="C12" s="8" t="s">
         <v>26</v>
       </c>
@@ -3361,27 +3376,27 @@
       <c r="J12" s="2">
         <v>5.3108000000000004</v>
       </c>
-      <c r="K12" s="1">
+      <c r="K12" s="2">
         <v>6.9560000000000004</v>
       </c>
     </row>
-    <row r="13" spans="1:11" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="13"/>
-      <c r="B13" s="16"/>
+    <row r="13" spans="1:12" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="14"/>
+      <c r="B13" s="17"/>
       <c r="C13" s="7"/>
-      <c r="K13" s="6"/>
-    </row>
-    <row r="14" spans="1:11" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="11">
+      <c r="L13" s="11"/>
+    </row>
+    <row r="14" spans="1:12" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="12">
         <v>800</v>
       </c>
-      <c r="B14" s="14" t="s">
+      <c r="B14" s="15" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="12"/>
-      <c r="B15" s="15"/>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15" s="13"/>
+      <c r="B15" s="16"/>
       <c r="C15" s="8" t="s">
         <v>20</v>
       </c>
@@ -3406,15 +3421,15 @@
       <c r="J15" s="4">
         <v>5.3209</v>
       </c>
-      <c r="K15" s="3">
+      <c r="K15" s="4">
         <v>6.5503999999999998</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="12"/>
-      <c r="B16" s="15"/>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A16" s="13"/>
+      <c r="B16" s="16"/>
       <c r="C16" s="8" t="s">
-        <v>21</v>
+        <v>34</v>
       </c>
       <c r="D16" s="2">
         <v>22.393000000000001</v>
@@ -3437,13 +3452,13 @@
       <c r="J16" s="2">
         <v>5.5168999999999997</v>
       </c>
-      <c r="K16" s="1">
+      <c r="K16" s="2">
         <v>6.9638999999999998</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="12"/>
-      <c r="B17" s="15"/>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A17" s="13"/>
+      <c r="B17" s="16"/>
       <c r="C17" s="8" t="s">
         <v>34</v>
       </c>
@@ -3468,13 +3483,13 @@
       <c r="J17" s="4">
         <v>4.3678999999999997</v>
       </c>
-      <c r="K17" s="3">
+      <c r="K17" s="4">
         <v>5.3108000000000004</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="12"/>
-      <c r="B18" s="15"/>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A18" s="13"/>
+      <c r="B18" s="16"/>
       <c r="C18" s="8" t="s">
         <v>23</v>
       </c>
@@ -3499,13 +3514,13 @@
       <c r="J18" s="4">
         <v>5.1186999999999996</v>
       </c>
-      <c r="K18" s="3">
+      <c r="K18" s="4">
         <v>9.9024000000000001</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="12"/>
-      <c r="B19" s="15"/>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A19" s="13"/>
+      <c r="B19" s="16"/>
       <c r="C19" s="8" t="s">
         <v>29</v>
       </c>
@@ -3530,13 +3545,13 @@
       <c r="J19" s="4">
         <v>5.1066000000000003</v>
       </c>
-      <c r="K19" s="3">
+      <c r="K19" s="4">
         <v>8.5634999999999994</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="12"/>
-      <c r="B20" s="15"/>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A20" s="13"/>
+      <c r="B20" s="16"/>
       <c r="C20" s="8" t="s">
         <v>38</v>
       </c>
@@ -3561,13 +3576,13 @@
       <c r="J20" s="4">
         <v>5.3201999999999998</v>
       </c>
-      <c r="K20" s="3">
+      <c r="K20" s="4">
         <v>6.8597999999999999</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21" s="12"/>
-      <c r="B21" s="15"/>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A21" s="13"/>
+      <c r="B21" s="16"/>
       <c r="C21" s="8" t="s">
         <v>35</v>
       </c>
@@ -3592,13 +3607,13 @@
       <c r="J21" s="2">
         <v>5.1558999999999999</v>
       </c>
-      <c r="K21" s="1">
+      <c r="K21" s="2">
         <v>8.7353000000000005</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22" s="12"/>
-      <c r="B22" s="15"/>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A22" s="13"/>
+      <c r="B22" s="16"/>
       <c r="C22" s="8" t="s">
         <v>26</v>
       </c>
@@ -3623,13 +3638,13 @@
       <c r="J22" s="2">
         <v>5.3186999999999998</v>
       </c>
-      <c r="K22" s="1">
+      <c r="K22" s="2">
         <v>8.5096000000000007</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23" s="12"/>
-      <c r="B23" s="15"/>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A23" s="13"/>
+      <c r="B23" s="16"/>
       <c r="C23" s="8" t="s">
         <v>29</v>
       </c>
@@ -3654,13 +3669,13 @@
       <c r="J23" s="4">
         <v>5.5469999999999997</v>
       </c>
-      <c r="K23" s="3">
+      <c r="K23" s="4">
         <v>6.8471000000000002</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A24" s="12"/>
-      <c r="B24" s="15"/>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A24" s="13"/>
+      <c r="B24" s="16"/>
       <c r="C24" s="8" t="s">
         <v>21</v>
       </c>
@@ -3685,29 +3700,29 @@
       <c r="J24" s="2">
         <v>4.8323</v>
       </c>
-      <c r="K24" s="1">
+      <c r="K24" s="2">
         <v>12.863</v>
       </c>
     </row>
-    <row r="25" spans="1:11" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="13"/>
-      <c r="B25" s="16"/>
+    <row r="25" spans="1:12" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="14"/>
+      <c r="B25" s="17"/>
       <c r="C25" s="7"/>
-      <c r="K25" s="6"/>
-    </row>
-    <row r="26" spans="1:11" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="11">
+      <c r="L25" s="11"/>
+    </row>
+    <row r="26" spans="1:12" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="12">
         <v>900</v>
       </c>
-      <c r="B26" s="14" t="s">
+      <c r="B26" s="15" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A27" s="12"/>
-      <c r="B27" s="15"/>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A27" s="13"/>
+      <c r="B27" s="16"/>
       <c r="C27" s="8" t="s">
-        <v>35</v>
+        <v>22</v>
       </c>
       <c r="D27" s="4">
         <v>4.8710000000000004</v>
@@ -3730,15 +3745,15 @@
       <c r="J27" s="2">
         <v>4.4973999999999998</v>
       </c>
-      <c r="K27" s="1">
+      <c r="K27" s="2">
         <v>9.6201000000000008</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A28" s="12"/>
-      <c r="B28" s="15"/>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A28" s="13"/>
+      <c r="B28" s="16"/>
       <c r="C28" s="8" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="D28" s="4">
         <v>10.692</v>
@@ -3761,13 +3776,13 @@
       <c r="J28" s="4">
         <v>4.5518000000000001</v>
       </c>
-      <c r="K28" s="3">
+      <c r="K28" s="4">
         <v>5.8509000000000002</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A29" s="12"/>
-      <c r="B29" s="15"/>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A29" s="13"/>
+      <c r="B29" s="16"/>
       <c r="C29" s="8" t="s">
         <v>18</v>
       </c>
@@ -3792,13 +3807,13 @@
       <c r="J29" s="2">
         <v>4.5818000000000003</v>
       </c>
-      <c r="K29" s="1">
+      <c r="K29" s="2">
         <v>9.0646000000000004</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A30" s="12"/>
-      <c r="B30" s="15"/>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A30" s="13"/>
+      <c r="B30" s="16"/>
       <c r="C30" s="8" t="s">
         <v>20</v>
       </c>
@@ -3823,13 +3838,13 @@
       <c r="J30" s="4">
         <v>4.3163999999999998</v>
       </c>
-      <c r="K30" s="3">
+      <c r="K30" s="4">
         <v>7.4964000000000004</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A31" s="12"/>
-      <c r="B31" s="15"/>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A31" s="13"/>
+      <c r="B31" s="16"/>
       <c r="C31" s="8" t="s">
         <v>20</v>
       </c>
@@ -3854,13 +3869,13 @@
       <c r="J31" s="4">
         <v>3.6387</v>
       </c>
-      <c r="K31" s="3">
+      <c r="K31" s="4">
         <v>8.3942999999999994</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A32" s="12"/>
-      <c r="B32" s="15"/>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A32" s="13"/>
+      <c r="B32" s="16"/>
       <c r="C32" s="8" t="s">
         <v>19</v>
       </c>
@@ -3885,13 +3900,13 @@
       <c r="J32" s="4">
         <v>4.4015000000000004</v>
       </c>
-      <c r="K32" s="3">
+      <c r="K32" s="4">
         <v>8.5838000000000001</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A33" s="12"/>
-      <c r="B33" s="15"/>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A33" s="13"/>
+      <c r="B33" s="16"/>
       <c r="C33" s="8" t="s">
         <v>20</v>
       </c>
@@ -3916,13 +3931,13 @@
       <c r="J33" s="4">
         <v>3.9569000000000001</v>
       </c>
-      <c r="K33" s="3">
+      <c r="K33" s="4">
         <v>11.773</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A34" s="12"/>
-      <c r="B34" s="15"/>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A34" s="13"/>
+      <c r="B34" s="16"/>
       <c r="C34" s="8" t="s">
         <v>35</v>
       </c>
@@ -3947,13 +3962,13 @@
       <c r="J34" s="2">
         <v>4.1947999999999999</v>
       </c>
-      <c r="K34" s="1">
+      <c r="K34" s="2">
         <v>6.7274000000000003</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A35" s="12"/>
-      <c r="B35" s="15"/>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A35" s="13"/>
+      <c r="B35" s="16"/>
       <c r="C35" s="8" t="s">
         <v>19</v>
       </c>
@@ -3978,13 +3993,13 @@
       <c r="J35" s="2">
         <v>4.5871000000000004</v>
       </c>
-      <c r="K35" s="1">
+      <c r="K35" s="2">
         <v>7.1367000000000003</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A36" s="12"/>
-      <c r="B36" s="15"/>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A36" s="13"/>
+      <c r="B36" s="16"/>
       <c r="C36" s="8" t="s">
         <v>35</v>
       </c>
@@ -4009,29 +4024,29 @@
       <c r="J36" s="4">
         <v>4.3048999999999999</v>
       </c>
-      <c r="K36" s="3">
+      <c r="K36" s="4">
         <v>6.8212000000000002</v>
       </c>
     </row>
-    <row r="37" spans="1:11" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="13"/>
-      <c r="B37" s="16"/>
+    <row r="37" spans="1:12" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="14"/>
+      <c r="B37" s="17"/>
       <c r="C37" s="7"/>
-      <c r="K37" s="6"/>
-    </row>
-    <row r="38" spans="1:11" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="11">
+      <c r="L37" s="11"/>
+    </row>
+    <row r="38" spans="1:12" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="12">
         <v>900</v>
       </c>
-      <c r="B38" s="14" t="s">
+      <c r="B38" s="15" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A39" s="12"/>
-      <c r="B39" s="15"/>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A39" s="13"/>
+      <c r="B39" s="16"/>
       <c r="C39" s="8" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="D39" s="4">
         <v>4.8238000000000003</v>
@@ -4054,15 +4069,15 @@
       <c r="J39" s="4">
         <v>4.6818</v>
       </c>
-      <c r="K39" s="3">
+      <c r="K39" s="4">
         <v>6.5256999999999996</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A40" s="12"/>
-      <c r="B40" s="15"/>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A40" s="13"/>
+      <c r="B40" s="16"/>
       <c r="C40" s="8" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D40" s="4">
         <v>7.1036999999999999</v>
@@ -4085,13 +4100,13 @@
       <c r="J40" s="2">
         <v>4.1879999999999997</v>
       </c>
-      <c r="K40" s="1">
+      <c r="K40" s="2">
         <v>3.5083000000000002</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A41" s="12"/>
-      <c r="B41" s="15"/>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A41" s="13"/>
+      <c r="B41" s="16"/>
       <c r="C41" s="8" t="s">
         <v>24</v>
       </c>
@@ -4116,13 +4131,13 @@
       <c r="J41" s="2">
         <v>4.4061000000000003</v>
       </c>
-      <c r="K41" s="1">
+      <c r="K41" s="2">
         <v>13.364000000000001</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A42" s="12"/>
-      <c r="B42" s="15"/>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A42" s="13"/>
+      <c r="B42" s="16"/>
       <c r="C42" s="8" t="s">
         <v>37</v>
       </c>
@@ -4147,13 +4162,13 @@
       <c r="J42" s="2">
         <v>4.3769999999999998</v>
       </c>
-      <c r="K42" s="1">
+      <c r="K42" s="2">
         <v>21.834</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A43" s="12"/>
-      <c r="B43" s="15"/>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A43" s="13"/>
+      <c r="B43" s="16"/>
       <c r="C43" s="8" t="s">
         <v>35</v>
       </c>
@@ -4178,13 +4193,13 @@
       <c r="J43" s="4">
         <v>4.13</v>
       </c>
-      <c r="K43" s="3">
+      <c r="K43" s="4">
         <v>5.8582999999999998</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A44" s="12"/>
-      <c r="B44" s="15"/>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A44" s="13"/>
+      <c r="B44" s="16"/>
       <c r="C44" s="8" t="s">
         <v>25</v>
       </c>
@@ -4209,13 +4224,13 @@
       <c r="J44" s="2">
         <v>4.3747999999999996</v>
       </c>
-      <c r="K44" s="1">
+      <c r="K44" s="2">
         <v>8.0503999999999998</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A45" s="12"/>
-      <c r="B45" s="15"/>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A45" s="13"/>
+      <c r="B45" s="16"/>
       <c r="C45" s="8" t="s">
         <v>23</v>
       </c>
@@ -4240,13 +4255,13 @@
       <c r="J45" s="2">
         <v>4.4539</v>
       </c>
-      <c r="K45" s="1">
+      <c r="K45" s="2">
         <v>6.9904999999999999</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A46" s="12"/>
-      <c r="B46" s="15"/>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A46" s="13"/>
+      <c r="B46" s="16"/>
       <c r="C46" s="8" t="s">
         <v>22</v>
       </c>
@@ -4271,13 +4286,13 @@
       <c r="J46" s="2">
         <v>4.5259999999999998</v>
       </c>
-      <c r="K46" s="1">
+      <c r="K46" s="2">
         <v>9.6370000000000005</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A47" s="12"/>
-      <c r="B47" s="15"/>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A47" s="13"/>
+      <c r="B47" s="16"/>
       <c r="C47" s="8" t="s">
         <v>34</v>
       </c>
@@ -4302,13 +4317,13 @@
       <c r="J47" s="4">
         <v>4.5678000000000001</v>
       </c>
-      <c r="K47" s="3">
+      <c r="K47" s="4">
         <v>7.4751000000000003</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A48" s="12"/>
-      <c r="B48" s="15"/>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A48" s="13"/>
+      <c r="B48" s="16"/>
       <c r="C48" s="8" t="s">
         <v>26</v>
       </c>
@@ -4333,123 +4348,123 @@
       <c r="J48" s="2">
         <v>4.5578000000000003</v>
       </c>
-      <c r="K48" s="1">
+      <c r="K48" s="2">
         <v>8.0541</v>
       </c>
     </row>
-    <row r="49" spans="1:11" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="13"/>
-      <c r="B49" s="16"/>
+    <row r="49" spans="1:12" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="14"/>
+      <c r="B49" s="17"/>
       <c r="C49" s="7"/>
-      <c r="K49" s="6"/>
-    </row>
-    <row r="50" spans="1:11" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="11">
+      <c r="L49" s="11"/>
+    </row>
+    <row r="50" spans="1:12" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="12">
         <v>1000</v>
       </c>
-      <c r="B50" s="14" t="s">
+      <c r="B50" s="15" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A51" s="12"/>
-      <c r="B51" s="15"/>
-    </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A52" s="12"/>
-      <c r="B52" s="15"/>
-    </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A53" s="12"/>
-      <c r="B53" s="15"/>
-    </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A54" s="12"/>
-      <c r="B54" s="15"/>
-    </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A55" s="12"/>
-      <c r="B55" s="15"/>
-    </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A56" s="12"/>
-      <c r="B56" s="15"/>
-    </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A57" s="12"/>
-      <c r="B57" s="15"/>
-    </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A58" s="12"/>
-      <c r="B58" s="15"/>
-    </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A59" s="12"/>
-      <c r="B59" s="15"/>
-    </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A60" s="12"/>
-      <c r="B60" s="15"/>
-    </row>
-    <row r="61" spans="1:11" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="13"/>
-      <c r="B61" s="16"/>
+    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A51" s="13"/>
+      <c r="B51" s="16"/>
+    </row>
+    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A52" s="13"/>
+      <c r="B52" s="16"/>
+    </row>
+    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A53" s="13"/>
+      <c r="B53" s="16"/>
+    </row>
+    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A54" s="13"/>
+      <c r="B54" s="16"/>
+    </row>
+    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A55" s="13"/>
+      <c r="B55" s="16"/>
+    </row>
+    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A56" s="13"/>
+      <c r="B56" s="16"/>
+    </row>
+    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A57" s="13"/>
+      <c r="B57" s="16"/>
+    </row>
+    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A58" s="13"/>
+      <c r="B58" s="16"/>
+    </row>
+    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A59" s="13"/>
+      <c r="B59" s="16"/>
+    </row>
+    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A60" s="13"/>
+      <c r="B60" s="16"/>
+    </row>
+    <row r="61" spans="1:12" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="14"/>
+      <c r="B61" s="17"/>
       <c r="C61" s="7"/>
-      <c r="K61" s="6"/>
-    </row>
-    <row r="62" spans="1:11" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="11">
+      <c r="L61" s="11"/>
+    </row>
+    <row r="62" spans="1:12" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="12">
         <v>1000</v>
       </c>
-      <c r="B62" s="14" t="s">
+      <c r="B62" s="15" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A63" s="12"/>
-      <c r="B63" s="15"/>
-    </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A64" s="12"/>
-      <c r="B64" s="15"/>
-    </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A65" s="12"/>
-      <c r="B65" s="15"/>
-    </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A66" s="12"/>
-      <c r="B66" s="15"/>
-    </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A67" s="12"/>
-      <c r="B67" s="15"/>
-    </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A68" s="12"/>
-      <c r="B68" s="15"/>
-    </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A69" s="12"/>
-      <c r="B69" s="15"/>
-    </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A70" s="12"/>
-      <c r="B70" s="15"/>
-    </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A71" s="12"/>
-      <c r="B71" s="15"/>
-    </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A72" s="12"/>
-      <c r="B72" s="15"/>
-    </row>
-    <row r="73" spans="1:11" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="13"/>
-      <c r="B73" s="16"/>
+    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A63" s="13"/>
+      <c r="B63" s="16"/>
+    </row>
+    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A64" s="13"/>
+      <c r="B64" s="16"/>
+    </row>
+    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A65" s="13"/>
+      <c r="B65" s="16"/>
+    </row>
+    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A66" s="13"/>
+      <c r="B66" s="16"/>
+    </row>
+    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A67" s="13"/>
+      <c r="B67" s="16"/>
+    </row>
+    <row r="68" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A68" s="13"/>
+      <c r="B68" s="16"/>
+    </row>
+    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A69" s="13"/>
+      <c r="B69" s="16"/>
+    </row>
+    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A70" s="13"/>
+      <c r="B70" s="16"/>
+    </row>
+    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A71" s="13"/>
+      <c r="B71" s="16"/>
+    </row>
+    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A72" s="13"/>
+      <c r="B72" s="16"/>
+    </row>
+    <row r="73" spans="1:12" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A73" s="14"/>
+      <c r="B73" s="17"/>
       <c r="C73" s="7"/>
-      <c r="K73" s="6"/>
+      <c r="L73" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="12">
@@ -4474,11 +4489,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF6E341A-51E3-4AF7-809B-A8594B1323BC}">
-  <dimension ref="A1:K73"/>
+  <dimension ref="A1:L73"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F27" sqref="F27"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4486,12 +4501,12 @@
     <col min="1" max="1" width="9.140625" style="4"/>
     <col min="2" max="2" width="9.140625" style="3"/>
     <col min="3" max="3" width="15.7109375" style="8" customWidth="1"/>
-    <col min="4" max="10" width="9.140625" style="4"/>
-    <col min="11" max="11" width="9.140625" style="3"/>
-    <col min="12" max="16384" width="9.140625" style="4"/>
+    <col min="4" max="11" width="9.140625" style="4"/>
+    <col min="12" max="12" width="9.140625" style="9"/>
+    <col min="13" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -4522,404 +4537,609 @@
       <c r="J1" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="6" t="s">
+      <c r="K1" s="5" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="11">
+      <c r="L1" s="11"/>
+    </row>
+    <row r="2" spans="1:12" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="12">
         <v>800</v>
       </c>
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="15" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="12"/>
-      <c r="B3" s="15"/>
-      <c r="I3" s="2"/>
-      <c r="J3" s="2"/>
-      <c r="K3" s="1"/>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="12"/>
-      <c r="B4" s="15"/>
-      <c r="I4" s="2"/>
-      <c r="J4" s="2"/>
-      <c r="K4" s="1"/>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="12"/>
-      <c r="B5" s="15"/>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" s="13"/>
+      <c r="B3" s="16"/>
+      <c r="C3" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" s="4">
+        <v>16.994</v>
+      </c>
+      <c r="E3" s="4">
+        <v>187.83</v>
+      </c>
+      <c r="F3" s="4">
+        <v>0.26103999999999999</v>
+      </c>
+      <c r="G3" s="4">
+        <v>4.5019999999999998</v>
+      </c>
+      <c r="H3" s="4">
+        <v>1784.8</v>
+      </c>
+      <c r="I3" s="2">
+        <v>3263.5</v>
+      </c>
+      <c r="J3" s="2">
+        <v>4.9230999999999998</v>
+      </c>
+      <c r="K3" s="2">
+        <v>13.172000000000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" s="13"/>
+      <c r="B4" s="16"/>
+      <c r="C4" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D4" s="4">
+        <v>22.454000000000001</v>
+      </c>
+      <c r="E4" s="4">
+        <v>66.77</v>
+      </c>
+      <c r="F4" s="4">
+        <v>0.92681000000000002</v>
+      </c>
+      <c r="G4" s="4">
+        <v>4.4191000000000003</v>
+      </c>
+      <c r="H4" s="4">
+        <v>1610.1</v>
+      </c>
+      <c r="I4" s="2">
+        <v>2142</v>
+      </c>
+      <c r="J4" s="2">
+        <v>5.4843999999999999</v>
+      </c>
+      <c r="K4" s="2">
+        <v>11.449</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" s="13"/>
+      <c r="B5" s="16"/>
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
-      <c r="K5" s="1"/>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="12"/>
-      <c r="B6" s="15"/>
+      <c r="K5" s="2"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" s="13"/>
+      <c r="B6" s="16"/>
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
-      <c r="K6" s="1"/>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="12"/>
-      <c r="B7" s="15"/>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="12"/>
-      <c r="B8" s="15"/>
+      <c r="K6" s="2"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" s="13"/>
+      <c r="B7" s="16"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" s="13"/>
+      <c r="B8" s="16"/>
       <c r="I8" s="2"/>
       <c r="J8" s="2"/>
-      <c r="K8" s="1"/>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="12"/>
-      <c r="B9" s="15"/>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="12"/>
-      <c r="B10" s="15"/>
+      <c r="K8" s="2"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" s="13"/>
+      <c r="B9" s="16"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" s="13"/>
+      <c r="B10" s="16"/>
       <c r="I10" s="2"/>
       <c r="J10" s="2"/>
-      <c r="K10" s="1"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="12"/>
-      <c r="B11" s="15"/>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="12"/>
-      <c r="B12" s="15"/>
+      <c r="K10" s="2"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" s="13"/>
+      <c r="B11" s="16"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" s="13"/>
+      <c r="B12" s="16"/>
       <c r="I12" s="2"/>
       <c r="J12" s="2"/>
-      <c r="K12" s="1"/>
-    </row>
-    <row r="13" spans="1:11" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="13"/>
-      <c r="B13" s="16"/>
+      <c r="K12" s="2"/>
+    </row>
+    <row r="13" spans="1:12" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="14"/>
+      <c r="B13" s="17"/>
       <c r="C13" s="7"/>
-      <c r="K13" s="6"/>
-    </row>
-    <row r="14" spans="1:11" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="11">
+      <c r="L13" s="11"/>
+    </row>
+    <row r="14" spans="1:12" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="12">
         <v>800</v>
       </c>
-      <c r="B14" s="14" t="s">
+      <c r="B14" s="15" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="12"/>
-      <c r="B15" s="15"/>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="12"/>
-      <c r="B16" s="15"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
-      <c r="G16" s="2"/>
-      <c r="H16" s="2"/>
-      <c r="I16" s="2"/>
-      <c r="J16" s="2"/>
-      <c r="K16" s="1"/>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="12"/>
-      <c r="B17" s="15"/>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="12"/>
-      <c r="B18" s="15"/>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="12"/>
-      <c r="B19" s="15"/>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="12"/>
-      <c r="B20" s="15"/>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21" s="12"/>
-      <c r="B21" s="15"/>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15" s="13"/>
+      <c r="B15" s="16"/>
+      <c r="C15" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D15" s="4">
+        <v>31.646999999999998</v>
+      </c>
+      <c r="E15" s="4">
+        <v>120.62</v>
+      </c>
+      <c r="F15" s="4">
+        <v>0.85485</v>
+      </c>
+      <c r="G15" s="4">
+        <v>3.7265999999999999</v>
+      </c>
+      <c r="H15" s="4">
+        <v>2297.8000000000002</v>
+      </c>
+      <c r="I15" s="4">
+        <v>2165.6999999999998</v>
+      </c>
+      <c r="J15" s="4">
+        <v>5.3247</v>
+      </c>
+      <c r="K15" s="4">
+        <v>7.7724000000000002</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A16" s="13"/>
+      <c r="B16" s="16"/>
+      <c r="C16" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D16" s="2">
+        <v>33.296999999999997</v>
+      </c>
+      <c r="E16" s="2">
+        <v>522.85</v>
+      </c>
+      <c r="F16" s="2">
+        <v>0.11871</v>
+      </c>
+      <c r="G16" s="2">
+        <v>3.9767000000000001</v>
+      </c>
+      <c r="H16" s="2">
+        <v>1762.4</v>
+      </c>
+      <c r="I16" s="2">
+        <v>1913.8</v>
+      </c>
+      <c r="J16" s="2">
+        <v>5.6638000000000002</v>
+      </c>
+      <c r="K16" s="2">
+        <v>11.287000000000001</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A17" s="13"/>
+      <c r="B17" s="16"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="2"/>
+      <c r="H17" s="2"/>
+      <c r="I17" s="2"/>
+      <c r="J17" s="2"/>
+      <c r="K17" s="2"/>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A18" s="13"/>
+      <c r="B18" s="16"/>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A19" s="13"/>
+      <c r="B19" s="16"/>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A20" s="13"/>
+      <c r="B20" s="16"/>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A21" s="13"/>
+      <c r="B21" s="16"/>
       <c r="I21" s="2"/>
       <c r="J21" s="2"/>
-      <c r="K21" s="1"/>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22" s="12"/>
-      <c r="B22" s="15"/>
+      <c r="K21" s="2"/>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A22" s="13"/>
+      <c r="B22" s="16"/>
       <c r="I22" s="2"/>
       <c r="J22" s="2"/>
-      <c r="K22" s="1"/>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23" s="12"/>
-      <c r="B23" s="15"/>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A24" s="12"/>
-      <c r="B24" s="15"/>
+      <c r="K22" s="2"/>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A23" s="13"/>
+      <c r="B23" s="16"/>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A24" s="13"/>
+      <c r="B24" s="16"/>
       <c r="I24" s="2"/>
       <c r="J24" s="2"/>
-      <c r="K24" s="1"/>
-    </row>
-    <row r="25" spans="1:11" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="13"/>
-      <c r="B25" s="16"/>
+      <c r="K24" s="2"/>
+    </row>
+    <row r="25" spans="1:12" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="14"/>
+      <c r="B25" s="17"/>
       <c r="C25" s="7"/>
-      <c r="K25" s="6"/>
-    </row>
-    <row r="26" spans="1:11" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="11">
+      <c r="L25" s="11"/>
+    </row>
+    <row r="26" spans="1:12" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="12">
         <v>900</v>
       </c>
-      <c r="B26" s="14" t="s">
+      <c r="B26" s="15" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A27" s="12"/>
-      <c r="B27" s="15"/>
-      <c r="I27" s="2"/>
-      <c r="J27" s="2"/>
-      <c r="K27" s="1"/>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A28" s="12"/>
-      <c r="B28" s="15"/>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A29" s="12"/>
-      <c r="B29" s="15"/>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A27" s="13"/>
+      <c r="B27" s="16"/>
+      <c r="C27" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D27" s="2">
+        <v>3.6261999999999999</v>
+      </c>
+      <c r="E27" s="2">
+        <v>13.804</v>
+      </c>
+      <c r="F27" s="2">
+        <v>6.9824999999999999</v>
+      </c>
+      <c r="G27" s="2">
+        <v>4.2416</v>
+      </c>
+      <c r="H27" s="2">
+        <v>1138.2</v>
+      </c>
+      <c r="I27" s="2">
+        <v>1986</v>
+      </c>
+      <c r="J27" s="2">
+        <v>4.4408000000000003</v>
+      </c>
+      <c r="K27" s="2">
+        <v>9.1929999999999996</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A28" s="13"/>
+      <c r="B28" s="16"/>
+      <c r="C28" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="D28" s="2">
+        <v>10.683</v>
+      </c>
+      <c r="E28" s="2">
+        <v>31.381</v>
+      </c>
+      <c r="F28" s="2">
+        <v>2.9727000000000001</v>
+      </c>
+      <c r="G28" s="2">
+        <v>3.7155</v>
+      </c>
+      <c r="H28" s="2">
+        <v>1422</v>
+      </c>
+      <c r="I28" s="2">
+        <v>1626.7</v>
+      </c>
+      <c r="J28" s="2">
+        <v>4.5519999999999996</v>
+      </c>
+      <c r="K28" s="2">
+        <v>6.2319000000000004</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A29" s="13"/>
+      <c r="B29" s="16"/>
       <c r="I29" s="2"/>
       <c r="J29" s="2"/>
-      <c r="K29" s="1"/>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A30" s="12"/>
-      <c r="B30" s="15"/>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A31" s="12"/>
-      <c r="B31" s="15"/>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A32" s="12"/>
-      <c r="B32" s="15"/>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A33" s="12"/>
-      <c r="B33" s="15"/>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A34" s="12"/>
-      <c r="B34" s="15"/>
+      <c r="K29" s="2"/>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A30" s="13"/>
+      <c r="B30" s="16"/>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A31" s="13"/>
+      <c r="B31" s="16"/>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A32" s="13"/>
+      <c r="B32" s="16"/>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A33" s="13"/>
+      <c r="B33" s="16"/>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A34" s="13"/>
+      <c r="B34" s="16"/>
       <c r="I34" s="2"/>
       <c r="J34" s="2"/>
-      <c r="K34" s="1"/>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A35" s="12"/>
-      <c r="B35" s="15"/>
+      <c r="K34" s="2"/>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A35" s="13"/>
+      <c r="B35" s="16"/>
       <c r="I35" s="2"/>
       <c r="J35" s="2"/>
-      <c r="K35" s="1"/>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A36" s="12"/>
-      <c r="B36" s="15"/>
-    </row>
-    <row r="37" spans="1:11" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="13"/>
-      <c r="B37" s="16"/>
+      <c r="K35" s="2"/>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A36" s="13"/>
+      <c r="B36" s="16"/>
+    </row>
+    <row r="37" spans="1:12" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="14"/>
+      <c r="B37" s="17"/>
       <c r="C37" s="7"/>
-      <c r="K37" s="6"/>
-    </row>
-    <row r="38" spans="1:11" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="11">
+      <c r="L37" s="11"/>
+    </row>
+    <row r="38" spans="1:12" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="12">
         <v>900</v>
       </c>
-      <c r="B38" s="14" t="s">
+      <c r="B38" s="15" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A39" s="12"/>
-      <c r="B39" s="15"/>
-    </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A40" s="12"/>
-      <c r="B40" s="15"/>
-      <c r="I40" s="2"/>
-      <c r="J40" s="2"/>
-      <c r="K40" s="1"/>
-    </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A41" s="12"/>
-      <c r="B41" s="15"/>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A39" s="13"/>
+      <c r="B39" s="16"/>
+      <c r="C39" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D39" s="4">
+        <v>8.7007999999999992</v>
+      </c>
+      <c r="E39" s="4">
+        <v>379.67</v>
+      </c>
+      <c r="F39" s="4">
+        <v>0.15739</v>
+      </c>
+      <c r="G39" s="4">
+        <v>4.2165999999999997</v>
+      </c>
+      <c r="H39" s="4">
+        <v>994.53</v>
+      </c>
+      <c r="I39" s="4">
+        <v>1533.4</v>
+      </c>
+      <c r="J39" s="4">
+        <v>4.6802000000000001</v>
+      </c>
+      <c r="K39" s="4">
+        <v>7.0461</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A40" s="13"/>
+      <c r="B40" s="16"/>
+      <c r="C40" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D40" s="2">
+        <v>9.3439999999999994</v>
+      </c>
+      <c r="E40" s="2">
+        <v>45.972000000000001</v>
+      </c>
+      <c r="F40" s="2">
+        <v>2.5375000000000001</v>
+      </c>
+      <c r="G40" s="2">
+        <v>3.4094000000000002</v>
+      </c>
+      <c r="H40" s="2">
+        <v>1902</v>
+      </c>
+      <c r="I40" s="2">
+        <v>2101.5</v>
+      </c>
+      <c r="J40" s="2">
+        <v>4.3022</v>
+      </c>
+      <c r="K40" s="2">
+        <v>6.1081000000000003</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A41" s="13"/>
+      <c r="B41" s="16"/>
       <c r="I41" s="2"/>
       <c r="J41" s="2"/>
-      <c r="K41" s="1"/>
-    </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A42" s="12"/>
-      <c r="B42" s="15"/>
+      <c r="K41" s="2"/>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A42" s="13"/>
+      <c r="B42" s="16"/>
       <c r="I42" s="2"/>
       <c r="J42" s="2"/>
-      <c r="K42" s="1"/>
-    </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A43" s="12"/>
-      <c r="B43" s="15"/>
-    </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A44" s="12"/>
-      <c r="B44" s="15"/>
+      <c r="K42" s="2"/>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A43" s="13"/>
+      <c r="B43" s="16"/>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A44" s="13"/>
+      <c r="B44" s="16"/>
       <c r="I44" s="2"/>
       <c r="J44" s="2"/>
-      <c r="K44" s="1"/>
-    </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A45" s="12"/>
-      <c r="B45" s="15"/>
+      <c r="K44" s="2"/>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A45" s="13"/>
+      <c r="B45" s="16"/>
       <c r="I45" s="2"/>
       <c r="J45" s="2"/>
-      <c r="K45" s="1"/>
-    </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A46" s="12"/>
-      <c r="B46" s="15"/>
+      <c r="K45" s="2"/>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A46" s="13"/>
+      <c r="B46" s="16"/>
       <c r="I46" s="2"/>
       <c r="J46" s="2"/>
-      <c r="K46" s="1"/>
-    </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A47" s="12"/>
-      <c r="B47" s="15"/>
-    </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A48" s="12"/>
-      <c r="B48" s="15"/>
+      <c r="K46" s="2"/>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A47" s="13"/>
+      <c r="B47" s="16"/>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A48" s="13"/>
+      <c r="B48" s="16"/>
       <c r="I48" s="2"/>
       <c r="J48" s="2"/>
-      <c r="K48" s="1"/>
-    </row>
-    <row r="49" spans="1:11" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="13"/>
-      <c r="B49" s="16"/>
+      <c r="K48" s="2"/>
+    </row>
+    <row r="49" spans="1:12" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="14"/>
+      <c r="B49" s="17"/>
       <c r="C49" s="7"/>
-      <c r="K49" s="6"/>
-    </row>
-    <row r="50" spans="1:11" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="11">
+      <c r="L49" s="11"/>
+    </row>
+    <row r="50" spans="1:12" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="12">
         <v>1000</v>
       </c>
-      <c r="B50" s="14" t="s">
+      <c r="B50" s="15" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A51" s="12"/>
-      <c r="B51" s="15"/>
-    </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A52" s="12"/>
-      <c r="B52" s="15"/>
-    </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A53" s="12"/>
-      <c r="B53" s="15"/>
-    </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A54" s="12"/>
-      <c r="B54" s="15"/>
-    </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A55" s="12"/>
-      <c r="B55" s="15"/>
-    </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A56" s="12"/>
-      <c r="B56" s="15"/>
-    </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A57" s="12"/>
-      <c r="B57" s="15"/>
-    </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A58" s="12"/>
-      <c r="B58" s="15"/>
-    </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A59" s="12"/>
-      <c r="B59" s="15"/>
-    </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A60" s="12"/>
-      <c r="B60" s="15"/>
-    </row>
-    <row r="61" spans="1:11" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="13"/>
-      <c r="B61" s="16"/>
+    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A51" s="13"/>
+      <c r="B51" s="16"/>
+    </row>
+    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A52" s="13"/>
+      <c r="B52" s="16"/>
+    </row>
+    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A53" s="13"/>
+      <c r="B53" s="16"/>
+    </row>
+    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A54" s="13"/>
+      <c r="B54" s="16"/>
+    </row>
+    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A55" s="13"/>
+      <c r="B55" s="16"/>
+    </row>
+    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A56" s="13"/>
+      <c r="B56" s="16"/>
+    </row>
+    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A57" s="13"/>
+      <c r="B57" s="16"/>
+    </row>
+    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A58" s="13"/>
+      <c r="B58" s="16"/>
+    </row>
+    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A59" s="13"/>
+      <c r="B59" s="16"/>
+    </row>
+    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A60" s="13"/>
+      <c r="B60" s="16"/>
+    </row>
+    <row r="61" spans="1:12" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="14"/>
+      <c r="B61" s="17"/>
       <c r="C61" s="7"/>
-      <c r="K61" s="6"/>
-    </row>
-    <row r="62" spans="1:11" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="11">
+      <c r="L61" s="11"/>
+    </row>
+    <row r="62" spans="1:12" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="12">
         <v>1000</v>
       </c>
-      <c r="B62" s="14" t="s">
+      <c r="B62" s="15" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A63" s="12"/>
-      <c r="B63" s="15"/>
-    </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A64" s="12"/>
-      <c r="B64" s="15"/>
-    </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A65" s="12"/>
-      <c r="B65" s="15"/>
-    </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A66" s="12"/>
-      <c r="B66" s="15"/>
-    </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A67" s="12"/>
-      <c r="B67" s="15"/>
-    </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A68" s="12"/>
-      <c r="B68" s="15"/>
-    </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A69" s="12"/>
-      <c r="B69" s="15"/>
-    </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A70" s="12"/>
-      <c r="B70" s="15"/>
-    </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A71" s="12"/>
-      <c r="B71" s="15"/>
-    </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A72" s="12"/>
-      <c r="B72" s="15"/>
-    </row>
-    <row r="73" spans="1:11" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="13"/>
-      <c r="B73" s="16"/>
+    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A63" s="13"/>
+      <c r="B63" s="16"/>
+    </row>
+    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A64" s="13"/>
+      <c r="B64" s="16"/>
+    </row>
+    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A65" s="13"/>
+      <c r="B65" s="16"/>
+    </row>
+    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A66" s="13"/>
+      <c r="B66" s="16"/>
+    </row>
+    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A67" s="13"/>
+      <c r="B67" s="16"/>
+    </row>
+    <row r="68" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A68" s="13"/>
+      <c r="B68" s="16"/>
+    </row>
+    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A69" s="13"/>
+      <c r="B69" s="16"/>
+    </row>
+    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A70" s="13"/>
+      <c r="B70" s="16"/>
+    </row>
+    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A71" s="13"/>
+      <c r="B71" s="16"/>
+    </row>
+    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A72" s="13"/>
+      <c r="B72" s="16"/>
+    </row>
+    <row r="73" spans="1:12" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A73" s="14"/>
+      <c r="B73" s="17"/>
       <c r="C73" s="7"/>
-      <c r="K73" s="6"/>
+      <c r="L73" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="12">
@@ -4943,11 +5163,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C18A26E-30CA-4E63-A18A-C9C101DAF33C}">
-  <dimension ref="A1:N73"/>
+  <dimension ref="A1:O73"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
+      <selection pane="bottomLeft" activeCell="M12" sqref="M12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4957,10 +5177,11 @@
     <col min="3" max="3" width="15.7109375" style="8" customWidth="1"/>
     <col min="4" max="13" width="9.140625" style="4"/>
     <col min="14" max="14" width="9.140625" style="3"/>
-    <col min="15" max="16384" width="9.140625" style="4"/>
+    <col min="15" max="15" width="9.140625" style="9"/>
+    <col min="16" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -5003,18 +5224,19 @@
       <c r="N1" s="6" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="2" spans="1:14" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="11">
+      <c r="O1" s="11"/>
+    </row>
+    <row r="2" spans="1:15" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="12">
         <v>800</v>
       </c>
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="15" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A3" s="12"/>
-      <c r="B3" s="15"/>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3" s="13"/>
+      <c r="B3" s="16"/>
       <c r="C3" s="8" t="s">
         <v>36</v>
       </c>
@@ -5052,9 +5274,9 @@
         <v>3.3214999999999999</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A4" s="12"/>
-      <c r="B4" s="15"/>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4" s="13"/>
+      <c r="B4" s="16"/>
       <c r="C4" s="8" t="s">
         <v>30</v>
       </c>
@@ -5092,9 +5314,9 @@
         <v>2.6046</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A5" s="12"/>
-      <c r="B5" s="15"/>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5" s="13"/>
+      <c r="B5" s="16"/>
       <c r="D5" s="4">
         <v>9.3076000000000008</v>
       </c>
@@ -5111,9 +5333,9 @@
         <v>1775.9</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6" s="12"/>
-      <c r="B6" s="15"/>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6" s="13"/>
+      <c r="B6" s="16"/>
       <c r="D6" s="4">
         <v>5.8951000000000002</v>
       </c>
@@ -5130,9 +5352,9 @@
         <v>1598.4</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A7" s="12"/>
-      <c r="B7" s="15"/>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A7" s="13"/>
+      <c r="B7" s="16"/>
       <c r="D7" s="4">
         <v>4.1862000000000004</v>
       </c>
@@ -5149,9 +5371,9 @@
         <v>1574.3</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A8" s="12"/>
-      <c r="B8" s="15"/>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A8" s="13"/>
+      <c r="B8" s="16"/>
       <c r="D8" s="4">
         <v>25.038</v>
       </c>
@@ -5168,9 +5390,9 @@
         <v>1944.6</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A9" s="12"/>
-      <c r="B9" s="15"/>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A9" s="13"/>
+      <c r="B9" s="16"/>
       <c r="D9" s="4">
         <v>27.547000000000001</v>
       </c>
@@ -5187,9 +5409,9 @@
         <v>2454.8000000000002</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A10" s="12"/>
-      <c r="B10" s="15"/>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A10" s="13"/>
+      <c r="B10" s="16"/>
       <c r="D10" s="4">
         <v>27.885000000000002</v>
       </c>
@@ -5206,9 +5428,9 @@
         <v>2390.5</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A11" s="12"/>
-      <c r="B11" s="15"/>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A11" s="13"/>
+      <c r="B11" s="16"/>
       <c r="D11" s="4">
         <v>19.2</v>
       </c>
@@ -5225,9 +5447,9 @@
         <v>1614.6</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A12" s="12"/>
-      <c r="B12" s="15"/>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A12" s="13"/>
+      <c r="B12" s="16"/>
       <c r="D12" s="4">
         <v>8.5922999999999998</v>
       </c>
@@ -5244,23 +5466,24 @@
         <v>1841</v>
       </c>
     </row>
-    <row r="13" spans="1:14" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="13"/>
-      <c r="B13" s="16"/>
+    <row r="13" spans="1:15" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="14"/>
+      <c r="B13" s="17"/>
       <c r="C13" s="7"/>
       <c r="N13" s="6"/>
-    </row>
-    <row r="14" spans="1:14" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="11">
+      <c r="O13" s="11"/>
+    </row>
+    <row r="14" spans="1:15" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="12">
         <v>800</v>
       </c>
-      <c r="B14" s="14" t="s">
+      <c r="B14" s="15" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A15" s="12"/>
-      <c r="B15" s="15"/>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A15" s="13"/>
+      <c r="B15" s="16"/>
       <c r="C15" s="8" t="s">
         <v>34</v>
       </c>
@@ -5298,9 +5521,9 @@
         <v>2.5640000000000001</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A16" s="12"/>
-      <c r="B16" s="15"/>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A16" s="13"/>
+      <c r="B16" s="16"/>
       <c r="C16" s="8" t="s">
         <v>32</v>
       </c>
@@ -5338,9 +5561,9 @@
         <v>2.3807999999999998</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A17" s="12"/>
-      <c r="B17" s="15"/>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A17" s="13"/>
+      <c r="B17" s="16"/>
       <c r="D17" s="4">
         <v>11.45</v>
       </c>
@@ -5357,9 +5580,9 @@
         <v>2221.6</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A18" s="12"/>
-      <c r="B18" s="15"/>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A18" s="13"/>
+      <c r="B18" s="16"/>
       <c r="D18" s="4">
         <v>37.741999999999997</v>
       </c>
@@ -5376,9 +5599,9 @@
         <v>3172</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A19" s="12"/>
-      <c r="B19" s="15"/>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A19" s="13"/>
+      <c r="B19" s="16"/>
       <c r="D19" s="4">
         <v>18.768000000000001</v>
       </c>
@@ -5395,9 +5618,9 @@
         <v>1677.4</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A20" s="12"/>
-      <c r="B20" s="15"/>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A20" s="13"/>
+      <c r="B20" s="16"/>
       <c r="D20" s="4">
         <v>23.303999999999998</v>
       </c>
@@ -5414,9 +5637,9 @@
         <v>1822.6</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A21" s="12"/>
-      <c r="B21" s="15"/>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A21" s="13"/>
+      <c r="B21" s="16"/>
       <c r="D21" s="4">
         <v>31.137</v>
       </c>
@@ -5433,9 +5656,9 @@
         <v>2583</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A22" s="12"/>
-      <c r="B22" s="15"/>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A22" s="13"/>
+      <c r="B22" s="16"/>
       <c r="D22" s="4">
         <v>29.725999999999999</v>
       </c>
@@ -5452,9 +5675,9 @@
         <v>2101.3000000000002</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A23" s="12"/>
-      <c r="B23" s="15"/>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A23" s="13"/>
+      <c r="B23" s="16"/>
       <c r="D23" s="4">
         <v>0.85682000000000003</v>
       </c>
@@ -5471,9 +5694,9 @@
         <v>1707</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A24" s="12"/>
-      <c r="B24" s="15"/>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A24" s="13"/>
+      <c r="B24" s="16"/>
       <c r="D24" s="4">
         <v>4.4611000000000001</v>
       </c>
@@ -5490,23 +5713,24 @@
         <v>3016.2</v>
       </c>
     </row>
-    <row r="25" spans="1:14" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="13"/>
-      <c r="B25" s="16"/>
+    <row r="25" spans="1:15" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="14"/>
+      <c r="B25" s="17"/>
       <c r="C25" s="7"/>
       <c r="N25" s="6"/>
-    </row>
-    <row r="26" spans="1:14" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="11">
+      <c r="O25" s="11"/>
+    </row>
+    <row r="26" spans="1:15" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="12">
         <v>900</v>
       </c>
-      <c r="B26" s="14" t="s">
+      <c r="B26" s="15" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A27" s="12"/>
-      <c r="B27" s="15"/>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A27" s="13"/>
+      <c r="B27" s="16"/>
       <c r="C27" s="8" t="s">
         <v>35</v>
       </c>
@@ -5544,9 +5768,9 @@
         <v>2.5308000000000002</v>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A28" s="12"/>
-      <c r="B28" s="15"/>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A28" s="13"/>
+      <c r="B28" s="16"/>
       <c r="C28" s="8" t="s">
         <v>32</v>
       </c>
@@ -5584,9 +5808,9 @@
         <v>2.4864000000000002</v>
       </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A29" s="12"/>
-      <c r="B29" s="15"/>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A29" s="13"/>
+      <c r="B29" s="16"/>
       <c r="C29" s="8" t="s">
         <v>35</v>
       </c>
@@ -5624,9 +5848,9 @@
         <v>2.4437000000000002</v>
       </c>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A30" s="12"/>
-      <c r="B30" s="15"/>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A30" s="13"/>
+      <c r="B30" s="16"/>
       <c r="D30" s="4">
         <v>11.208</v>
       </c>
@@ -5643,9 +5867,9 @@
         <v>1530.1</v>
       </c>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A31" s="12"/>
-      <c r="B31" s="15"/>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A31" s="13"/>
+      <c r="B31" s="16"/>
       <c r="D31" s="4">
         <v>10.45</v>
       </c>
@@ -5662,9 +5886,9 @@
         <v>1787.3</v>
       </c>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A32" s="12"/>
-      <c r="B32" s="15"/>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A32" s="13"/>
+      <c r="B32" s="16"/>
       <c r="D32" s="4">
         <v>11.010999999999999</v>
       </c>
@@ -5681,9 +5905,9 @@
         <v>1593.8</v>
       </c>
     </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A33" s="12"/>
-      <c r="B33" s="15"/>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A33" s="13"/>
+      <c r="B33" s="16"/>
       <c r="D33" s="4">
         <v>5.6656000000000004</v>
       </c>
@@ -5700,9 +5924,9 @@
         <v>1000.8</v>
       </c>
     </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A34" s="12"/>
-      <c r="B34" s="15"/>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A34" s="13"/>
+      <c r="B34" s="16"/>
       <c r="D34" s="4">
         <v>15.185</v>
       </c>
@@ -5719,9 +5943,9 @@
         <v>2110.6</v>
       </c>
     </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A35" s="12"/>
-      <c r="B35" s="15"/>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A35" s="13"/>
+      <c r="B35" s="16"/>
       <c r="D35" s="4">
         <v>8.0571999999999999</v>
       </c>
@@ -5738,9 +5962,9 @@
         <v>1210.4000000000001</v>
       </c>
     </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A36" s="12"/>
-      <c r="B36" s="15"/>
+    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A36" s="13"/>
+      <c r="B36" s="16"/>
       <c r="D36" s="4">
         <v>7.5292000000000003</v>
       </c>
@@ -5757,23 +5981,24 @@
         <v>1369.1</v>
       </c>
     </row>
-    <row r="37" spans="1:14" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="13"/>
-      <c r="B37" s="16"/>
+    <row r="37" spans="1:15" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="14"/>
+      <c r="B37" s="17"/>
       <c r="C37" s="7"/>
       <c r="N37" s="6"/>
-    </row>
-    <row r="38" spans="1:14" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="11">
+      <c r="O37" s="11"/>
+    </row>
+    <row r="38" spans="1:15" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="12">
         <v>900</v>
       </c>
-      <c r="B38" s="14" t="s">
+      <c r="B38" s="15" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A39" s="12"/>
-      <c r="B39" s="15"/>
+    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A39" s="13"/>
+      <c r="B39" s="16"/>
       <c r="C39" s="8" t="s">
         <v>31</v>
       </c>
@@ -5811,9 +6036,9 @@
         <v>2.5291999999999999</v>
       </c>
     </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A40" s="12"/>
-      <c r="B40" s="15"/>
+    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A40" s="13"/>
+      <c r="B40" s="16"/>
       <c r="C40" s="8" t="s">
         <v>33</v>
       </c>
@@ -5851,9 +6076,9 @@
         <v>2.2601</v>
       </c>
     </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A41" s="12"/>
-      <c r="B41" s="15"/>
+    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A41" s="13"/>
+      <c r="B41" s="16"/>
       <c r="C41" s="8" t="s">
         <v>34</v>
       </c>
@@ -5891,9 +6116,9 @@
         <v>2.5724</v>
       </c>
     </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A42" s="12"/>
-      <c r="B42" s="15"/>
+    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A42" s="13"/>
+      <c r="B42" s="16"/>
       <c r="D42" s="4">
         <v>4.6340000000000003</v>
       </c>
@@ -5910,9 +6135,9 @@
         <v>1999.7</v>
       </c>
     </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A43" s="12"/>
-      <c r="B43" s="15"/>
+    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A43" s="13"/>
+      <c r="B43" s="16"/>
       <c r="D43" s="4">
         <v>16.286999999999999</v>
       </c>
@@ -5929,9 +6154,9 @@
         <v>2606.1999999999998</v>
       </c>
     </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A44" s="12"/>
-      <c r="B44" s="15"/>
+    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A44" s="13"/>
+      <c r="B44" s="16"/>
       <c r="D44" s="4">
         <v>9.5312999999999999</v>
       </c>
@@ -5948,9 +6173,9 @@
         <v>1253.9000000000001</v>
       </c>
     </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A45" s="12"/>
-      <c r="B45" s="15"/>
+    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A45" s="13"/>
+      <c r="B45" s="16"/>
       <c r="D45" s="4">
         <v>6.3647</v>
       </c>
@@ -5967,9 +6192,9 @@
         <v>1127.5999999999999</v>
       </c>
     </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A46" s="12"/>
-      <c r="B46" s="15"/>
+    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A46" s="13"/>
+      <c r="B46" s="16"/>
       <c r="D46" s="4">
         <v>12.622</v>
       </c>
@@ -5986,9 +6211,9 @@
         <v>1371.6</v>
       </c>
     </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A47" s="12"/>
-      <c r="B47" s="15"/>
+    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A47" s="13"/>
+      <c r="B47" s="16"/>
       <c r="D47" s="4">
         <v>12.256</v>
       </c>
@@ -6005,9 +6230,9 @@
         <v>1242.3</v>
       </c>
     </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A48" s="12"/>
-      <c r="B48" s="15"/>
+    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A48" s="13"/>
+      <c r="B48" s="16"/>
       <c r="D48" s="4">
         <v>7.0439999999999996</v>
       </c>
@@ -6024,119 +6249,122 @@
         <v>1090</v>
       </c>
     </row>
-    <row r="49" spans="1:14" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="13"/>
-      <c r="B49" s="16"/>
+    <row r="49" spans="1:15" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="14"/>
+      <c r="B49" s="17"/>
       <c r="C49" s="7"/>
       <c r="N49" s="6"/>
-    </row>
-    <row r="50" spans="1:14" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="11">
+      <c r="O49" s="11"/>
+    </row>
+    <row r="50" spans="1:15" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="12">
         <v>1000</v>
       </c>
-      <c r="B50" s="14" t="s">
+      <c r="B50" s="15" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A51" s="12"/>
-      <c r="B51" s="15"/>
-    </row>
-    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A52" s="12"/>
-      <c r="B52" s="15"/>
-    </row>
-    <row r="53" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A53" s="12"/>
-      <c r="B53" s="15"/>
-    </row>
-    <row r="54" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A54" s="12"/>
-      <c r="B54" s="15"/>
-    </row>
-    <row r="55" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A55" s="12"/>
-      <c r="B55" s="15"/>
-    </row>
-    <row r="56" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A56" s="12"/>
-      <c r="B56" s="15"/>
-    </row>
-    <row r="57" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A57" s="12"/>
-      <c r="B57" s="15"/>
-    </row>
-    <row r="58" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A58" s="12"/>
-      <c r="B58" s="15"/>
-    </row>
-    <row r="59" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A59" s="12"/>
-      <c r="B59" s="15"/>
-    </row>
-    <row r="60" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A60" s="12"/>
-      <c r="B60" s="15"/>
-    </row>
-    <row r="61" spans="1:14" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="13"/>
-      <c r="B61" s="16"/>
+    <row r="51" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A51" s="13"/>
+      <c r="B51" s="16"/>
+    </row>
+    <row r="52" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A52" s="13"/>
+      <c r="B52" s="16"/>
+    </row>
+    <row r="53" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A53" s="13"/>
+      <c r="B53" s="16"/>
+    </row>
+    <row r="54" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A54" s="13"/>
+      <c r="B54" s="16"/>
+    </row>
+    <row r="55" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A55" s="13"/>
+      <c r="B55" s="16"/>
+    </row>
+    <row r="56" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A56" s="13"/>
+      <c r="B56" s="16"/>
+    </row>
+    <row r="57" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A57" s="13"/>
+      <c r="B57" s="16"/>
+    </row>
+    <row r="58" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A58" s="13"/>
+      <c r="B58" s="16"/>
+    </row>
+    <row r="59" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A59" s="13"/>
+      <c r="B59" s="16"/>
+    </row>
+    <row r="60" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A60" s="13"/>
+      <c r="B60" s="16"/>
+    </row>
+    <row r="61" spans="1:15" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="14"/>
+      <c r="B61" s="17"/>
       <c r="C61" s="7"/>
       <c r="N61" s="6"/>
-    </row>
-    <row r="62" spans="1:14" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="11">
+      <c r="O61" s="11"/>
+    </row>
+    <row r="62" spans="1:15" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="12">
         <v>1000</v>
       </c>
-      <c r="B62" s="14" t="s">
+      <c r="B62" s="15" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="63" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A63" s="12"/>
-      <c r="B63" s="15"/>
-    </row>
-    <row r="64" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A64" s="12"/>
-      <c r="B64" s="15"/>
-    </row>
-    <row r="65" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A65" s="12"/>
-      <c r="B65" s="15"/>
-    </row>
-    <row r="66" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A66" s="12"/>
-      <c r="B66" s="15"/>
-    </row>
-    <row r="67" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A67" s="12"/>
-      <c r="B67" s="15"/>
-    </row>
-    <row r="68" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A68" s="12"/>
-      <c r="B68" s="15"/>
-    </row>
-    <row r="69" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A69" s="12"/>
-      <c r="B69" s="15"/>
-    </row>
-    <row r="70" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A70" s="12"/>
-      <c r="B70" s="15"/>
-    </row>
-    <row r="71" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A71" s="12"/>
-      <c r="B71" s="15"/>
-    </row>
-    <row r="72" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A72" s="12"/>
-      <c r="B72" s="15"/>
-    </row>
-    <row r="73" spans="1:14" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="13"/>
-      <c r="B73" s="16"/>
+    <row r="63" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A63" s="13"/>
+      <c r="B63" s="16"/>
+    </row>
+    <row r="64" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A64" s="13"/>
+      <c r="B64" s="16"/>
+    </row>
+    <row r="65" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A65" s="13"/>
+      <c r="B65" s="16"/>
+    </row>
+    <row r="66" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A66" s="13"/>
+      <c r="B66" s="16"/>
+    </row>
+    <row r="67" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A67" s="13"/>
+      <c r="B67" s="16"/>
+    </row>
+    <row r="68" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A68" s="13"/>
+      <c r="B68" s="16"/>
+    </row>
+    <row r="69" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A69" s="13"/>
+      <c r="B69" s="16"/>
+    </row>
+    <row r="70" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A70" s="13"/>
+      <c r="B70" s="16"/>
+    </row>
+    <row r="71" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A71" s="13"/>
+      <c r="B71" s="16"/>
+    </row>
+    <row r="72" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A72" s="13"/>
+      <c r="B72" s="16"/>
+    </row>
+    <row r="73" spans="1:15" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A73" s="14"/>
+      <c r="B73" s="17"/>
       <c r="C73" s="7"/>
       <c r="N73" s="6"/>
+      <c r="O73" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="12">
@@ -6160,11 +6388,11 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F200E048-5FAF-4136-82F6-92204CC50E12}">
-  <dimension ref="A1:N73"/>
+  <dimension ref="A1:O73"/>
   <sheetViews>
     <sheetView topLeftCell="B1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N55" sqref="C3:N55"/>
+      <selection pane="bottomLeft" activeCell="O1" sqref="O1:O1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6174,10 +6402,11 @@
     <col min="3" max="3" width="15.7109375" style="8" customWidth="1"/>
     <col min="4" max="13" width="9.140625" style="4"/>
     <col min="14" max="14" width="9.140625" style="3"/>
-    <col min="15" max="16384" width="9.140625" style="4"/>
+    <col min="15" max="15" width="9.140625" style="9"/>
+    <col min="16" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -6220,18 +6449,19 @@
       <c r="N1" s="6" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="2" spans="1:14" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="11">
+      <c r="O1" s="11"/>
+    </row>
+    <row r="2" spans="1:15" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="12">
         <v>800</v>
       </c>
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="15" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A3" s="12"/>
-      <c r="B3" s="15"/>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3" s="13"/>
+      <c r="B3" s="16"/>
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
       <c r="K3" s="2"/>
@@ -6239,175 +6469,178 @@
       <c r="M3" s="2"/>
       <c r="N3" s="1"/>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A4" s="12"/>
-      <c r="B4" s="15"/>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A5" s="12"/>
-      <c r="B5" s="15"/>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6" s="12"/>
-      <c r="B6" s="15"/>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A7" s="12"/>
-      <c r="B7" s="15"/>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A8" s="12"/>
-      <c r="B8" s="15"/>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A9" s="12"/>
-      <c r="B9" s="15"/>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A10" s="12"/>
-      <c r="B10" s="15"/>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A11" s="12"/>
-      <c r="B11" s="15"/>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A12" s="12"/>
-      <c r="B12" s="15"/>
-    </row>
-    <row r="13" spans="1:14" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="13"/>
-      <c r="B13" s="16"/>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4" s="13"/>
+      <c r="B4" s="16"/>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5" s="13"/>
+      <c r="B5" s="16"/>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6" s="13"/>
+      <c r="B6" s="16"/>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A7" s="13"/>
+      <c r="B7" s="16"/>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A8" s="13"/>
+      <c r="B8" s="16"/>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A9" s="13"/>
+      <c r="B9" s="16"/>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A10" s="13"/>
+      <c r="B10" s="16"/>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A11" s="13"/>
+      <c r="B11" s="16"/>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A12" s="13"/>
+      <c r="B12" s="16"/>
+    </row>
+    <row r="13" spans="1:15" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="14"/>
+      <c r="B13" s="17"/>
       <c r="C13" s="7"/>
       <c r="N13" s="6"/>
-    </row>
-    <row r="14" spans="1:14" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="11">
+      <c r="O13" s="11"/>
+    </row>
+    <row r="14" spans="1:15" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="12">
         <v>800</v>
       </c>
-      <c r="B14" s="14" t="s">
+      <c r="B14" s="15" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A15" s="12"/>
-      <c r="B15" s="15"/>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A16" s="12"/>
-      <c r="B16" s="15"/>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A17" s="12"/>
-      <c r="B17" s="15"/>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A18" s="12"/>
-      <c r="B18" s="15"/>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A19" s="12"/>
-      <c r="B19" s="15"/>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A20" s="12"/>
-      <c r="B20" s="15"/>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A21" s="12"/>
-      <c r="B21" s="15"/>
-    </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A22" s="12"/>
-      <c r="B22" s="15"/>
-    </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A23" s="12"/>
-      <c r="B23" s="15"/>
-    </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A24" s="12"/>
-      <c r="B24" s="15"/>
-    </row>
-    <row r="25" spans="1:14" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="13"/>
-      <c r="B25" s="16"/>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A15" s="13"/>
+      <c r="B15" s="16"/>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A16" s="13"/>
+      <c r="B16" s="16"/>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A17" s="13"/>
+      <c r="B17" s="16"/>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A18" s="13"/>
+      <c r="B18" s="16"/>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A19" s="13"/>
+      <c r="B19" s="16"/>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A20" s="13"/>
+      <c r="B20" s="16"/>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A21" s="13"/>
+      <c r="B21" s="16"/>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A22" s="13"/>
+      <c r="B22" s="16"/>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A23" s="13"/>
+      <c r="B23" s="16"/>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A24" s="13"/>
+      <c r="B24" s="16"/>
+    </row>
+    <row r="25" spans="1:15" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="14"/>
+      <c r="B25" s="17"/>
       <c r="C25" s="7"/>
       <c r="N25" s="6"/>
-    </row>
-    <row r="26" spans="1:14" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="11">
+      <c r="O25" s="11"/>
+    </row>
+    <row r="26" spans="1:15" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="12">
         <v>900</v>
       </c>
-      <c r="B26" s="14" t="s">
+      <c r="B26" s="15" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A27" s="12"/>
-      <c r="B27" s="15"/>
-    </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A28" s="12"/>
-      <c r="B28" s="15"/>
-    </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A29" s="12"/>
-      <c r="B29" s="15"/>
-    </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A30" s="12"/>
-      <c r="B30" s="15"/>
-    </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A31" s="12"/>
-      <c r="B31" s="15"/>
-    </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A32" s="12"/>
-      <c r="B32" s="15"/>
-    </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A33" s="12"/>
-      <c r="B33" s="15"/>
-    </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A34" s="12"/>
-      <c r="B34" s="15"/>
-    </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A35" s="12"/>
-      <c r="B35" s="15"/>
-    </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A36" s="12"/>
-      <c r="B36" s="15"/>
-    </row>
-    <row r="37" spans="1:14" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="13"/>
-      <c r="B37" s="16"/>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A27" s="13"/>
+      <c r="B27" s="16"/>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A28" s="13"/>
+      <c r="B28" s="16"/>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A29" s="13"/>
+      <c r="B29" s="16"/>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A30" s="13"/>
+      <c r="B30" s="16"/>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A31" s="13"/>
+      <c r="B31" s="16"/>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A32" s="13"/>
+      <c r="B32" s="16"/>
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A33" s="13"/>
+      <c r="B33" s="16"/>
+    </row>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A34" s="13"/>
+      <c r="B34" s="16"/>
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A35" s="13"/>
+      <c r="B35" s="16"/>
+    </row>
+    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A36" s="13"/>
+      <c r="B36" s="16"/>
+    </row>
+    <row r="37" spans="1:15" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="14"/>
+      <c r="B37" s="17"/>
       <c r="C37" s="7"/>
       <c r="N37" s="6"/>
-    </row>
-    <row r="38" spans="1:14" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="11">
+      <c r="O37" s="11"/>
+    </row>
+    <row r="38" spans="1:15" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="12">
         <v>900</v>
       </c>
-      <c r="B38" s="14" t="s">
+      <c r="B38" s="15" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A39" s="12"/>
-      <c r="B39" s="15"/>
-    </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A40" s="12"/>
-      <c r="B40" s="15"/>
-    </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A41" s="12"/>
-      <c r="B41" s="15"/>
+    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A39" s="13"/>
+      <c r="B39" s="16"/>
+    </row>
+    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A40" s="13"/>
+      <c r="B40" s="16"/>
+    </row>
+    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A41" s="13"/>
+      <c r="B41" s="16"/>
       <c r="I41" s="2"/>
       <c r="J41" s="2"/>
       <c r="K41" s="2"/>
@@ -6415,147 +6648,150 @@
       <c r="M41" s="2"/>
       <c r="N41" s="1"/>
     </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A42" s="12"/>
-      <c r="B42" s="15"/>
-    </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A43" s="12"/>
-      <c r="B43" s="15"/>
-    </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A44" s="12"/>
-      <c r="B44" s="15"/>
-    </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A45" s="12"/>
-      <c r="B45" s="15"/>
-    </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A46" s="12"/>
-      <c r="B46" s="15"/>
-    </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A47" s="12"/>
-      <c r="B47" s="15"/>
-    </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A48" s="12"/>
-      <c r="B48" s="15"/>
-    </row>
-    <row r="49" spans="1:14" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="13"/>
-      <c r="B49" s="16"/>
+    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A42" s="13"/>
+      <c r="B42" s="16"/>
+    </row>
+    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A43" s="13"/>
+      <c r="B43" s="16"/>
+    </row>
+    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A44" s="13"/>
+      <c r="B44" s="16"/>
+    </row>
+    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A45" s="13"/>
+      <c r="B45" s="16"/>
+    </row>
+    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A46" s="13"/>
+      <c r="B46" s="16"/>
+    </row>
+    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A47" s="13"/>
+      <c r="B47" s="16"/>
+    </row>
+    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A48" s="13"/>
+      <c r="B48" s="16"/>
+    </row>
+    <row r="49" spans="1:15" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="14"/>
+      <c r="B49" s="17"/>
       <c r="C49" s="7"/>
       <c r="N49" s="6"/>
-    </row>
-    <row r="50" spans="1:14" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="11">
+      <c r="O49" s="11"/>
+    </row>
+    <row r="50" spans="1:15" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="12">
         <v>1000</v>
       </c>
-      <c r="B50" s="14" t="s">
+      <c r="B50" s="15" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A51" s="12"/>
-      <c r="B51" s="15"/>
-    </row>
-    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A52" s="12"/>
-      <c r="B52" s="15"/>
-    </row>
-    <row r="53" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A53" s="12"/>
-      <c r="B53" s="15"/>
-    </row>
-    <row r="54" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A54" s="12"/>
-      <c r="B54" s="15"/>
-    </row>
-    <row r="55" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A55" s="12"/>
-      <c r="B55" s="15"/>
-    </row>
-    <row r="56" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A56" s="12"/>
-      <c r="B56" s="15"/>
-    </row>
-    <row r="57" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A57" s="12"/>
-      <c r="B57" s="15"/>
-    </row>
-    <row r="58" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A58" s="12"/>
-      <c r="B58" s="15"/>
-    </row>
-    <row r="59" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A59" s="12"/>
-      <c r="B59" s="15"/>
-    </row>
-    <row r="60" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A60" s="12"/>
-      <c r="B60" s="15"/>
-    </row>
-    <row r="61" spans="1:14" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="13"/>
-      <c r="B61" s="16"/>
+    <row r="51" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A51" s="13"/>
+      <c r="B51" s="16"/>
+    </row>
+    <row r="52" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A52" s="13"/>
+      <c r="B52" s="16"/>
+    </row>
+    <row r="53" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A53" s="13"/>
+      <c r="B53" s="16"/>
+    </row>
+    <row r="54" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A54" s="13"/>
+      <c r="B54" s="16"/>
+    </row>
+    <row r="55" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A55" s="13"/>
+      <c r="B55" s="16"/>
+    </row>
+    <row r="56" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A56" s="13"/>
+      <c r="B56" s="16"/>
+    </row>
+    <row r="57" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A57" s="13"/>
+      <c r="B57" s="16"/>
+    </row>
+    <row r="58" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A58" s="13"/>
+      <c r="B58" s="16"/>
+    </row>
+    <row r="59" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A59" s="13"/>
+      <c r="B59" s="16"/>
+    </row>
+    <row r="60" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A60" s="13"/>
+      <c r="B60" s="16"/>
+    </row>
+    <row r="61" spans="1:15" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="14"/>
+      <c r="B61" s="17"/>
       <c r="C61" s="7"/>
       <c r="N61" s="6"/>
-    </row>
-    <row r="62" spans="1:14" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="11">
+      <c r="O61" s="11"/>
+    </row>
+    <row r="62" spans="1:15" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="12">
         <v>1000</v>
       </c>
-      <c r="B62" s="14" t="s">
+      <c r="B62" s="15" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="63" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A63" s="12"/>
-      <c r="B63" s="15"/>
-    </row>
-    <row r="64" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A64" s="12"/>
-      <c r="B64" s="15"/>
-    </row>
-    <row r="65" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A65" s="12"/>
-      <c r="B65" s="15"/>
-    </row>
-    <row r="66" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A66" s="12"/>
-      <c r="B66" s="15"/>
-    </row>
-    <row r="67" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A67" s="12"/>
-      <c r="B67" s="15"/>
-    </row>
-    <row r="68" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A68" s="12"/>
-      <c r="B68" s="15"/>
-    </row>
-    <row r="69" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A69" s="12"/>
-      <c r="B69" s="15"/>
-    </row>
-    <row r="70" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A70" s="12"/>
-      <c r="B70" s="15"/>
-    </row>
-    <row r="71" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A71" s="12"/>
-      <c r="B71" s="15"/>
-    </row>
-    <row r="72" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A72" s="12"/>
-      <c r="B72" s="15"/>
-    </row>
-    <row r="73" spans="1:14" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="13"/>
-      <c r="B73" s="16"/>
+    <row r="63" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A63" s="13"/>
+      <c r="B63" s="16"/>
+    </row>
+    <row r="64" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A64" s="13"/>
+      <c r="B64" s="16"/>
+    </row>
+    <row r="65" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A65" s="13"/>
+      <c r="B65" s="16"/>
+    </row>
+    <row r="66" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A66" s="13"/>
+      <c r="B66" s="16"/>
+    </row>
+    <row r="67" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A67" s="13"/>
+      <c r="B67" s="16"/>
+    </row>
+    <row r="68" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A68" s="13"/>
+      <c r="B68" s="16"/>
+    </row>
+    <row r="69" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A69" s="13"/>
+      <c r="B69" s="16"/>
+    </row>
+    <row r="70" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A70" s="13"/>
+      <c r="B70" s="16"/>
+    </row>
+    <row r="71" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A71" s="13"/>
+      <c r="B71" s="16"/>
+    </row>
+    <row r="72" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A72" s="13"/>
+      <c r="B72" s="16"/>
+    </row>
+    <row r="73" spans="1:15" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A73" s="14"/>
+      <c r="B73" s="17"/>
       <c r="C73" s="7"/>
       <c r="N73" s="6"/>
+      <c r="O73" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="12">

</xml_diff>

<commit_message>
Added new params to sem results file
</commit_message>
<xml_diff>
--- a/scripts/__other__/__sem__.xlsx
+++ b/scripts/__other__/__sem__.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Janzen\Desktop\code\moga_neml\scripts\__other__\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F65C60E-29C5-429C-8D64-B672A93A17B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{750900A2-5BB0-4E24-890C-2A687FFC121E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="15600" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="evp" sheetId="13" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="46">
   <si>
     <t>temp</t>
   </si>
@@ -175,6 +175,9 @@
   </si>
   <si>
     <t>evp</t>
+  </si>
+  <si>
+    <t>5; 10</t>
   </si>
 </sst>
 </file>
@@ -2988,18 +2991,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A38:A49"/>
+    <mergeCell ref="B38:B49"/>
+    <mergeCell ref="A50:A61"/>
+    <mergeCell ref="B50:B61"/>
+    <mergeCell ref="A62:A73"/>
+    <mergeCell ref="B62:B73"/>
     <mergeCell ref="A2:A13"/>
     <mergeCell ref="B2:B13"/>
     <mergeCell ref="A14:A25"/>
     <mergeCell ref="B14:B25"/>
     <mergeCell ref="A26:A37"/>
     <mergeCell ref="B26:B37"/>
-    <mergeCell ref="A38:A49"/>
-    <mergeCell ref="B38:B49"/>
-    <mergeCell ref="A50:A61"/>
-    <mergeCell ref="B50:B61"/>
-    <mergeCell ref="A62:A73"/>
-    <mergeCell ref="B62:B73"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -3011,9 +3014,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE483CC8-AF2C-4D5A-AEE5-EF7DF4EC0883}">
   <dimension ref="A1:L73"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G59" sqref="G59"/>
+    <sheetView topLeftCell="B1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3136,7 +3139,7 @@
       <c r="A5" s="13"/>
       <c r="B5" s="16"/>
       <c r="C5" s="8" t="s">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="D5" s="4">
         <v>9.3076000000000008</v>
@@ -3167,7 +3170,7 @@
       <c r="A6" s="13"/>
       <c r="B6" s="16"/>
       <c r="C6" s="8" t="s">
-        <v>20</v>
+        <v>38</v>
       </c>
       <c r="D6" s="4">
         <v>5.8951000000000002</v>
@@ -3491,7 +3494,7 @@
       <c r="A18" s="13"/>
       <c r="B18" s="16"/>
       <c r="C18" s="8" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D18" s="4">
         <v>37.741999999999997</v>
@@ -3784,7 +3787,7 @@
       <c r="A29" s="13"/>
       <c r="B29" s="16"/>
       <c r="C29" s="8" t="s">
-        <v>18</v>
+        <v>35</v>
       </c>
       <c r="D29" s="4">
         <v>11.2</v>
@@ -4139,7 +4142,7 @@
       <c r="A42" s="13"/>
       <c r="B42" s="16"/>
       <c r="C42" s="8" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="D42" s="4">
         <v>4.6340000000000003</v>
@@ -4468,18 +4471,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A38:A49"/>
+    <mergeCell ref="B38:B49"/>
+    <mergeCell ref="A50:A61"/>
+    <mergeCell ref="B50:B61"/>
+    <mergeCell ref="A62:A73"/>
+    <mergeCell ref="B62:B73"/>
     <mergeCell ref="A2:A13"/>
     <mergeCell ref="B2:B13"/>
     <mergeCell ref="A14:A25"/>
     <mergeCell ref="B14:B25"/>
     <mergeCell ref="A26:A37"/>
     <mergeCell ref="B26:B37"/>
-    <mergeCell ref="A38:A49"/>
-    <mergeCell ref="B38:B49"/>
-    <mergeCell ref="A50:A61"/>
-    <mergeCell ref="B50:B61"/>
-    <mergeCell ref="A62:A73"/>
-    <mergeCell ref="B62:B73"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -4491,9 +4494,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF6E341A-51E3-4AF7-809B-A8594B1323BC}">
   <dimension ref="A1:L73"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C40" sqref="C40"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C43" sqref="C43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4615,16 +4618,64 @@
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="13"/>
       <c r="B5" s="16"/>
-      <c r="I5" s="2"/>
-      <c r="J5" s="2"/>
-      <c r="K5" s="2"/>
+      <c r="C5" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" s="4">
+        <v>9.1647999999999996</v>
+      </c>
+      <c r="E5" s="4">
+        <v>36.326000000000001</v>
+      </c>
+      <c r="F5" s="4">
+        <v>12.337</v>
+      </c>
+      <c r="G5" s="4">
+        <v>4.2247000000000003</v>
+      </c>
+      <c r="H5" s="4">
+        <v>1776.1</v>
+      </c>
+      <c r="I5" s="2">
+        <v>2731</v>
+      </c>
+      <c r="J5" s="2">
+        <v>5.0411000000000001</v>
+      </c>
+      <c r="K5" s="2">
+        <v>8.3102999999999998</v>
+      </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="13"/>
       <c r="B6" s="16"/>
-      <c r="I6" s="2"/>
-      <c r="J6" s="2"/>
-      <c r="K6" s="2"/>
+      <c r="C6" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" s="4">
+        <v>5.8951000000000002</v>
+      </c>
+      <c r="E6" s="4">
+        <v>36.906999999999996</v>
+      </c>
+      <c r="F6" s="4">
+        <v>5.3551000000000002</v>
+      </c>
+      <c r="G6" s="4">
+        <v>4.7310999999999996</v>
+      </c>
+      <c r="H6" s="4">
+        <v>1557.8</v>
+      </c>
+      <c r="I6" s="2">
+        <v>2224.1</v>
+      </c>
+      <c r="J6" s="2">
+        <v>5.2808999999999999</v>
+      </c>
+      <c r="K6" s="2">
+        <v>6.5113000000000003</v>
+      </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="13"/>
@@ -4738,18 +4789,64 @@
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="13"/>
       <c r="B17" s="16"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
-      <c r="G17" s="2"/>
-      <c r="H17" s="2"/>
-      <c r="I17" s="2"/>
-      <c r="J17" s="2"/>
-      <c r="K17" s="2"/>
+      <c r="C17" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="D17" s="2">
+        <v>13.247</v>
+      </c>
+      <c r="E17" s="2">
+        <v>47.88</v>
+      </c>
+      <c r="F17" s="2">
+        <v>7.2160000000000002</v>
+      </c>
+      <c r="G17" s="2">
+        <v>3.9582999999999999</v>
+      </c>
+      <c r="H17" s="2">
+        <v>2115.6</v>
+      </c>
+      <c r="I17" s="2">
+        <v>3764.3</v>
+      </c>
+      <c r="J17" s="2">
+        <v>4.4740000000000002</v>
+      </c>
+      <c r="K17" s="2">
+        <v>5.1694000000000004</v>
+      </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="13"/>
       <c r="B18" s="16"/>
+      <c r="C18" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D18" s="2">
+        <v>38.180999999999997</v>
+      </c>
+      <c r="E18" s="2">
+        <v>51.055</v>
+      </c>
+      <c r="F18" s="2">
+        <v>2.4819</v>
+      </c>
+      <c r="G18" s="2">
+        <v>3.2572000000000001</v>
+      </c>
+      <c r="H18" s="2">
+        <v>3154.4</v>
+      </c>
+      <c r="I18" s="2">
+        <v>2725.2</v>
+      </c>
+      <c r="J18" s="2">
+        <v>5.0167000000000002</v>
+      </c>
+      <c r="K18" s="2">
+        <v>8.33</v>
+      </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="13"/>
@@ -4863,13 +4960,64 @@
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" s="13"/>
       <c r="B29" s="16"/>
-      <c r="I29" s="2"/>
-      <c r="J29" s="2"/>
-      <c r="K29" s="2"/>
+      <c r="C29" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="D29" s="2">
+        <v>10.340999999999999</v>
+      </c>
+      <c r="E29" s="2">
+        <v>24.475999999999999</v>
+      </c>
+      <c r="F29" s="2">
+        <v>2.3226</v>
+      </c>
+      <c r="G29" s="2">
+        <v>3.9651000000000001</v>
+      </c>
+      <c r="H29" s="2">
+        <v>1176.4000000000001</v>
+      </c>
+      <c r="I29" s="2">
+        <v>1743</v>
+      </c>
+      <c r="J29" s="2">
+        <v>4.5865</v>
+      </c>
+      <c r="K29" s="2">
+        <v>9.1586999999999996</v>
+      </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" s="13"/>
       <c r="B30" s="16"/>
+      <c r="C30" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D30" s="2">
+        <v>11.112</v>
+      </c>
+      <c r="E30" s="2">
+        <v>18.959</v>
+      </c>
+      <c r="F30" s="2">
+        <v>5.9504999999999999</v>
+      </c>
+      <c r="G30" s="2">
+        <v>3.6368</v>
+      </c>
+      <c r="H30" s="2">
+        <v>1471.6</v>
+      </c>
+      <c r="I30" s="2">
+        <v>2064.3000000000002</v>
+      </c>
+      <c r="J30" s="2">
+        <v>4.3163999999999998</v>
+      </c>
+      <c r="K30" s="2">
+        <v>7.2249999999999996</v>
+      </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" s="13"/>
@@ -4980,16 +5128,64 @@
     <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41" s="13"/>
       <c r="B41" s="16"/>
-      <c r="I41" s="2"/>
-      <c r="J41" s="2"/>
-      <c r="K41" s="2"/>
+      <c r="C41" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D41" s="2">
+        <v>3.0011000000000001</v>
+      </c>
+      <c r="E41" s="2">
+        <v>18.974</v>
+      </c>
+      <c r="F41" s="2">
+        <v>32.389000000000003</v>
+      </c>
+      <c r="G41" s="2">
+        <v>3.2721</v>
+      </c>
+      <c r="H41" s="2">
+        <v>2021.2</v>
+      </c>
+      <c r="I41" s="2">
+        <v>2356.1999999999998</v>
+      </c>
+      <c r="J41" s="2">
+        <v>4.4100999999999999</v>
+      </c>
+      <c r="K41" s="2">
+        <v>17.539000000000001</v>
+      </c>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42" s="13"/>
       <c r="B42" s="16"/>
-      <c r="I42" s="2"/>
-      <c r="J42" s="2"/>
-      <c r="K42" s="2"/>
+      <c r="C42" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="D42" s="2">
+        <v>2.1263000000000001</v>
+      </c>
+      <c r="E42" s="2">
+        <v>19.571000000000002</v>
+      </c>
+      <c r="F42" s="2">
+        <v>18.852</v>
+      </c>
+      <c r="G42" s="2">
+        <v>3.3525</v>
+      </c>
+      <c r="H42" s="2">
+        <v>1999.6</v>
+      </c>
+      <c r="I42" s="2">
+        <v>2639.8</v>
+      </c>
+      <c r="J42" s="2">
+        <v>4.3577000000000004</v>
+      </c>
+      <c r="K42" s="2">
+        <v>21.824999999999999</v>
+      </c>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43" s="13"/>
@@ -5143,18 +5339,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A2:A13"/>
+    <mergeCell ref="B2:B13"/>
+    <mergeCell ref="A14:A25"/>
+    <mergeCell ref="B14:B25"/>
+    <mergeCell ref="A26:A37"/>
+    <mergeCell ref="B26:B37"/>
     <mergeCell ref="A38:A49"/>
     <mergeCell ref="B38:B49"/>
     <mergeCell ref="A50:A61"/>
     <mergeCell ref="B50:B61"/>
     <mergeCell ref="A62:A73"/>
     <mergeCell ref="B62:B73"/>
-    <mergeCell ref="A2:A13"/>
-    <mergeCell ref="B2:B13"/>
-    <mergeCell ref="A14:A25"/>
-    <mergeCell ref="B14:B25"/>
-    <mergeCell ref="A26:A37"/>
-    <mergeCell ref="B26:B37"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -6368,18 +6564,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A38:A49"/>
+    <mergeCell ref="B38:B49"/>
+    <mergeCell ref="A50:A61"/>
+    <mergeCell ref="B50:B61"/>
+    <mergeCell ref="A62:A73"/>
+    <mergeCell ref="B62:B73"/>
     <mergeCell ref="A2:A13"/>
     <mergeCell ref="B2:B13"/>
     <mergeCell ref="A14:A25"/>
     <mergeCell ref="B14:B25"/>
     <mergeCell ref="A26:A37"/>
     <mergeCell ref="B26:B37"/>
-    <mergeCell ref="A38:A49"/>
-    <mergeCell ref="B38:B49"/>
-    <mergeCell ref="A50:A61"/>
-    <mergeCell ref="B50:B61"/>
-    <mergeCell ref="A62:A73"/>
-    <mergeCell ref="B62:B73"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -6795,18 +6991,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A2:A13"/>
+    <mergeCell ref="B2:B13"/>
+    <mergeCell ref="A14:A25"/>
+    <mergeCell ref="B14:B25"/>
+    <mergeCell ref="A26:A37"/>
+    <mergeCell ref="B26:B37"/>
     <mergeCell ref="A38:A49"/>
     <mergeCell ref="B38:B49"/>
     <mergeCell ref="A50:A61"/>
     <mergeCell ref="B50:B61"/>
     <mergeCell ref="A62:A73"/>
     <mergeCell ref="B62:B73"/>
-    <mergeCell ref="A2:A13"/>
-    <mergeCell ref="B2:B13"/>
-    <mergeCell ref="A14:A25"/>
-    <mergeCell ref="B14:B25"/>
-    <mergeCell ref="A26:A37"/>
-    <mergeCell ref="B26:B37"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
Cleaned up code for writing to file while file is open
</commit_message>
<xml_diff>
--- a/scripts/__other__/__sem__.xlsx
+++ b/scripts/__other__/__sem__.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Janzen\Desktop\code\moga_neml\scripts\__other__\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{750900A2-5BB0-4E24-890C-2A687FFC121E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC2A5EBF-F893-4206-AF79-158886D3AF8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="15600" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="46">
   <si>
     <t>temp</t>
   </si>
@@ -3014,9 +3014,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE483CC8-AF2C-4D5A-AEE5-EF7DF4EC0883}">
   <dimension ref="A1:L73"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D36" sqref="D36"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C44" sqref="C44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3201,7 +3201,7 @@
       <c r="A7" s="13"/>
       <c r="B7" s="16"/>
       <c r="C7" s="8" t="s">
-        <v>26</v>
+        <v>38</v>
       </c>
       <c r="D7" s="4">
         <v>4.1862000000000004</v>
@@ -3849,7 +3849,7 @@
       <c r="A31" s="13"/>
       <c r="B31" s="16"/>
       <c r="C31" s="8" t="s">
-        <v>20</v>
+        <v>38</v>
       </c>
       <c r="D31" s="4">
         <v>10.45</v>
@@ -3880,7 +3880,7 @@
       <c r="A32" s="13"/>
       <c r="B32" s="16"/>
       <c r="C32" s="8" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="D32" s="4">
         <v>11.010999999999999</v>
@@ -4173,7 +4173,7 @@
       <c r="A43" s="13"/>
       <c r="B43" s="16"/>
       <c r="C43" s="8" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="D43" s="4">
         <v>16.286999999999999</v>
@@ -4495,8 +4495,8 @@
   <dimension ref="A1:L73"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C43" sqref="C43"/>
+      <pane ySplit="1" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C44" sqref="C44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4680,13 +4680,64 @@
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="13"/>
       <c r="B7" s="16"/>
+      <c r="C7" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D7" s="4">
+        <v>4.1860999999999997</v>
+      </c>
+      <c r="E7" s="4">
+        <v>84.548000000000002</v>
+      </c>
+      <c r="F7" s="4">
+        <v>2.1124999999999998</v>
+      </c>
+      <c r="G7" s="4">
+        <v>4.7670000000000003</v>
+      </c>
+      <c r="H7" s="4">
+        <v>1574.1</v>
+      </c>
+      <c r="I7" s="4">
+        <v>2883.2</v>
+      </c>
+      <c r="J7" s="4">
+        <v>4.8395000000000001</v>
+      </c>
+      <c r="K7" s="4">
+        <v>4.5430999999999999</v>
+      </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="13"/>
       <c r="B8" s="16"/>
-      <c r="I8" s="2"/>
-      <c r="J8" s="2"/>
-      <c r="K8" s="2"/>
+      <c r="C8" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" s="2">
+        <v>27.867999999999999</v>
+      </c>
+      <c r="E8" s="2">
+        <v>89.338999999999999</v>
+      </c>
+      <c r="F8" s="2">
+        <v>0.59711999999999998</v>
+      </c>
+      <c r="G8" s="2">
+        <v>4.1981999999999999</v>
+      </c>
+      <c r="H8" s="2">
+        <v>1818</v>
+      </c>
+      <c r="I8" s="2">
+        <v>2645.2</v>
+      </c>
+      <c r="J8" s="2">
+        <v>5.1192000000000002</v>
+      </c>
+      <c r="K8" s="2">
+        <v>10.125</v>
+      </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="13"/>
@@ -4851,10 +4902,64 @@
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="13"/>
       <c r="B19" s="16"/>
+      <c r="C19" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="D19" s="4">
+        <v>24.888999999999999</v>
+      </c>
+      <c r="E19" s="4">
+        <v>44.932000000000002</v>
+      </c>
+      <c r="F19" s="4">
+        <v>1.2076</v>
+      </c>
+      <c r="G19" s="4">
+        <v>4.5054999999999996</v>
+      </c>
+      <c r="H19" s="4">
+        <v>1527.9</v>
+      </c>
+      <c r="I19" s="4">
+        <v>2589.6999999999998</v>
+      </c>
+      <c r="J19" s="4">
+        <v>5.1066000000000003</v>
+      </c>
+      <c r="K19" s="4">
+        <v>8.6950000000000003</v>
+      </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="13"/>
       <c r="B20" s="16"/>
+      <c r="C20" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D20" s="2">
+        <v>23.303999999999998</v>
+      </c>
+      <c r="E20" s="2">
+        <v>276.66000000000003</v>
+      </c>
+      <c r="F20" s="2">
+        <v>0.32123000000000002</v>
+      </c>
+      <c r="G20" s="2">
+        <v>4.2591999999999999</v>
+      </c>
+      <c r="H20" s="2">
+        <v>1767.2</v>
+      </c>
+      <c r="I20" s="2">
+        <v>2168.5</v>
+      </c>
+      <c r="J20" s="2">
+        <v>5.3181000000000003</v>
+      </c>
+      <c r="K20" s="2">
+        <v>6.7618999999999998</v>
+      </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="13"/>
@@ -5022,10 +5127,64 @@
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" s="13"/>
       <c r="B31" s="16"/>
+      <c r="C31" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D31" s="2">
+        <v>8.0817999999999994</v>
+      </c>
+      <c r="E31" s="2">
+        <v>9.2744</v>
+      </c>
+      <c r="F31" s="2">
+        <v>7.9561999999999999</v>
+      </c>
+      <c r="G31" s="2">
+        <v>3.9839000000000002</v>
+      </c>
+      <c r="H31" s="2">
+        <v>1310.7</v>
+      </c>
+      <c r="I31" s="2">
+        <v>4972.3999999999996</v>
+      </c>
+      <c r="J31" s="2">
+        <v>3.6442999999999999</v>
+      </c>
+      <c r="K31" s="2">
+        <v>9.6707000000000001</v>
+      </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" s="13"/>
       <c r="B32" s="16"/>
+      <c r="C32" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D32" s="2">
+        <v>11.394</v>
+      </c>
+      <c r="E32" s="2">
+        <v>13.887</v>
+      </c>
+      <c r="F32" s="2">
+        <v>7.532</v>
+      </c>
+      <c r="G32" s="2">
+        <v>3.5691000000000002</v>
+      </c>
+      <c r="H32" s="2">
+        <v>1581.2</v>
+      </c>
+      <c r="I32" s="2">
+        <v>1959.8</v>
+      </c>
+      <c r="J32" s="2">
+        <v>4.4120999999999997</v>
+      </c>
+      <c r="K32" s="2">
+        <v>8.5846999999999998</v>
+      </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" s="13"/>
@@ -5190,13 +5349,64 @@
     <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43" s="13"/>
       <c r="B43" s="16"/>
+      <c r="C43" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D43" s="2">
+        <v>16.257000000000001</v>
+      </c>
+      <c r="E43" s="2">
+        <v>181.45</v>
+      </c>
+      <c r="F43" s="2">
+        <v>0.50260000000000005</v>
+      </c>
+      <c r="G43" s="2">
+        <v>3.0154000000000001</v>
+      </c>
+      <c r="H43" s="2">
+        <v>2606.1999999999998</v>
+      </c>
+      <c r="I43" s="2">
+        <v>2445.1</v>
+      </c>
+      <c r="J43" s="2">
+        <v>4.1307</v>
+      </c>
+      <c r="K43" s="2">
+        <v>5.6963999999999997</v>
+      </c>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44" s="13"/>
       <c r="B44" s="16"/>
-      <c r="I44" s="2"/>
-      <c r="J44" s="2"/>
-      <c r="K44" s="2"/>
+      <c r="C44" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="D44" s="2">
+        <v>9.5314999999999994</v>
+      </c>
+      <c r="E44" s="2">
+        <v>149.26</v>
+      </c>
+      <c r="F44" s="2">
+        <v>0.37325999999999998</v>
+      </c>
+      <c r="G44" s="2">
+        <v>3.9582000000000002</v>
+      </c>
+      <c r="H44" s="2">
+        <v>1254.5999999999999</v>
+      </c>
+      <c r="I44" s="2">
+        <v>2014.8</v>
+      </c>
+      <c r="J44" s="2">
+        <v>4.3853999999999997</v>
+      </c>
+      <c r="K44" s="2">
+        <v>8.0510999999999999</v>
+      </c>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A45" s="13"/>

</xml_diff>

<commit_message>
added new params for evpcd_i
</commit_message>
<xml_diff>
--- a/scripts/__other__/__sem__.xlsx
+++ b/scripts/__other__/__sem__.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Janzen\Desktop\code\moga_neml\scripts\__other__\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC2A5EBF-F893-4206-AF79-158886D3AF8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D198638C-591B-46A3-9347-CB91288CD462}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="15600" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="46">
   <si>
     <t>temp</t>
   </si>
@@ -2991,18 +2991,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A2:A13"/>
+    <mergeCell ref="B2:B13"/>
+    <mergeCell ref="A14:A25"/>
+    <mergeCell ref="B14:B25"/>
+    <mergeCell ref="A26:A37"/>
+    <mergeCell ref="B26:B37"/>
     <mergeCell ref="A38:A49"/>
     <mergeCell ref="B38:B49"/>
     <mergeCell ref="A50:A61"/>
     <mergeCell ref="B50:B61"/>
     <mergeCell ref="A62:A73"/>
     <mergeCell ref="B62:B73"/>
-    <mergeCell ref="A2:A13"/>
-    <mergeCell ref="B2:B13"/>
-    <mergeCell ref="A14:A25"/>
-    <mergeCell ref="B14:B25"/>
-    <mergeCell ref="A26:A37"/>
-    <mergeCell ref="B26:B37"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -3015,8 +3015,8 @@
   <dimension ref="A1:L73"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C44" sqref="C44"/>
+      <pane ySplit="1" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C48" sqref="C48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3680,7 +3680,7 @@
       <c r="A24" s="13"/>
       <c r="B24" s="16"/>
       <c r="C24" s="8" t="s">
-        <v>21</v>
+        <v>35</v>
       </c>
       <c r="D24" s="4">
         <v>4.4611000000000001</v>
@@ -3973,7 +3973,7 @@
       <c r="A35" s="13"/>
       <c r="B35" s="16"/>
       <c r="C35" s="8" t="s">
-        <v>19</v>
+        <v>34</v>
       </c>
       <c r="D35" s="4">
         <v>8.0571999999999999</v>
@@ -4004,7 +4004,7 @@
       <c r="A36" s="13"/>
       <c r="B36" s="16"/>
       <c r="C36" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D36" s="4">
         <v>7.5292000000000003</v>
@@ -4328,7 +4328,7 @@
       <c r="A48" s="13"/>
       <c r="B48" s="16"/>
       <c r="C48" s="8" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="D48" s="4">
         <v>7.0439999999999996</v>
@@ -4471,18 +4471,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A2:A13"/>
+    <mergeCell ref="B2:B13"/>
+    <mergeCell ref="A14:A25"/>
+    <mergeCell ref="B14:B25"/>
+    <mergeCell ref="A26:A37"/>
+    <mergeCell ref="B26:B37"/>
     <mergeCell ref="A38:A49"/>
     <mergeCell ref="B38:B49"/>
     <mergeCell ref="A50:A61"/>
     <mergeCell ref="B50:B61"/>
     <mergeCell ref="A62:A73"/>
     <mergeCell ref="B62:B73"/>
-    <mergeCell ref="A2:A13"/>
-    <mergeCell ref="B2:B13"/>
-    <mergeCell ref="A14:A25"/>
-    <mergeCell ref="B14:B25"/>
-    <mergeCell ref="A26:A37"/>
-    <mergeCell ref="B26:B37"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -4495,8 +4495,8 @@
   <dimension ref="A1:L73"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C44" sqref="C44"/>
+      <pane ySplit="1" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4753,13 +4753,64 @@
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="13"/>
       <c r="B11" s="16"/>
+      <c r="C11" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="D11" s="4">
+        <v>19.125</v>
+      </c>
+      <c r="E11" s="4">
+        <v>43.640999999999998</v>
+      </c>
+      <c r="F11" s="4">
+        <v>5.6147999999999998</v>
+      </c>
+      <c r="G11" s="4">
+        <v>4.1688000000000001</v>
+      </c>
+      <c r="H11" s="4">
+        <v>1616</v>
+      </c>
+      <c r="I11" s="4">
+        <v>1876.8</v>
+      </c>
+      <c r="J11" s="4">
+        <v>5.5594000000000001</v>
+      </c>
+      <c r="K11" s="4">
+        <v>6.8653000000000004</v>
+      </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="13"/>
       <c r="B12" s="16"/>
-      <c r="I12" s="2"/>
-      <c r="J12" s="2"/>
-      <c r="K12" s="2"/>
+      <c r="C12" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D12" s="4">
+        <v>22.012</v>
+      </c>
+      <c r="E12" s="4">
+        <v>38.872999999999998</v>
+      </c>
+      <c r="F12" s="4">
+        <v>2.2033</v>
+      </c>
+      <c r="G12" s="4">
+        <v>4.2450000000000001</v>
+      </c>
+      <c r="H12" s="4">
+        <v>1841.2</v>
+      </c>
+      <c r="I12" s="2">
+        <v>2377</v>
+      </c>
+      <c r="J12" s="2">
+        <v>5.2897999999999996</v>
+      </c>
+      <c r="K12" s="2">
+        <v>9.7712000000000003</v>
+      </c>
     </row>
     <row r="13" spans="1:12" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="14"/>
@@ -4978,13 +5029,64 @@
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="13"/>
       <c r="B23" s="16"/>
+      <c r="C23" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="D23" s="4">
+        <v>5.0568999999999997</v>
+      </c>
+      <c r="E23" s="4">
+        <v>40.475999999999999</v>
+      </c>
+      <c r="F23" s="4">
+        <v>10.016999999999999</v>
+      </c>
+      <c r="G23" s="4">
+        <v>4.1585000000000001</v>
+      </c>
+      <c r="H23" s="4">
+        <v>1730.1</v>
+      </c>
+      <c r="I23" s="4">
+        <v>1998.1</v>
+      </c>
+      <c r="J23" s="4">
+        <v>5.5564</v>
+      </c>
+      <c r="K23" s="4">
+        <v>10.337</v>
+      </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="13"/>
       <c r="B24" s="16"/>
-      <c r="I24" s="2"/>
-      <c r="J24" s="2"/>
-      <c r="K24" s="2"/>
+      <c r="C24" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="D24" s="4">
+        <v>0.36498999999999998</v>
+      </c>
+      <c r="E24" s="4">
+        <v>45.374000000000002</v>
+      </c>
+      <c r="F24" s="4">
+        <v>15.686999999999999</v>
+      </c>
+      <c r="G24" s="4">
+        <v>3.6105</v>
+      </c>
+      <c r="H24" s="4">
+        <v>2878.3</v>
+      </c>
+      <c r="I24" s="2">
+        <v>3325.8</v>
+      </c>
+      <c r="J24" s="2">
+        <v>4.8470000000000004</v>
+      </c>
+      <c r="K24" s="2">
+        <v>12.327999999999999</v>
+      </c>
     </row>
     <row r="25" spans="1:12" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="14"/>
@@ -5200,13 +5302,64 @@
     <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" s="13"/>
       <c r="B35" s="16"/>
-      <c r="I35" s="2"/>
-      <c r="J35" s="2"/>
-      <c r="K35" s="2"/>
+      <c r="C35" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="D35" s="4">
+        <v>8.0267999999999997</v>
+      </c>
+      <c r="E35" s="4">
+        <v>28.899000000000001</v>
+      </c>
+      <c r="F35" s="4">
+        <v>2.5811000000000002</v>
+      </c>
+      <c r="G35" s="4">
+        <v>4.0179999999999998</v>
+      </c>
+      <c r="H35" s="4">
+        <v>1213.4000000000001</v>
+      </c>
+      <c r="I35" s="2">
+        <v>1698.5</v>
+      </c>
+      <c r="J35" s="2">
+        <v>4.5711000000000004</v>
+      </c>
+      <c r="K35" s="2">
+        <v>7.3220999999999998</v>
+      </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" s="13"/>
       <c r="B36" s="16"/>
+      <c r="C36" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D36" s="4">
+        <v>8.0846</v>
+      </c>
+      <c r="E36" s="4">
+        <v>21.623000000000001</v>
+      </c>
+      <c r="F36" s="4">
+        <v>4.9984999999999999</v>
+      </c>
+      <c r="G36" s="4">
+        <v>3.8734000000000002</v>
+      </c>
+      <c r="H36" s="4">
+        <v>1330.8</v>
+      </c>
+      <c r="I36" s="4">
+        <v>2586.3000000000002</v>
+      </c>
+      <c r="J36" s="4">
+        <v>4.0925000000000002</v>
+      </c>
+      <c r="K36" s="4">
+        <v>6.8217999999999996</v>
+      </c>
     </row>
     <row r="37" spans="1:12" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="14"/>
@@ -5425,13 +5578,64 @@
     <row r="47" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A47" s="13"/>
       <c r="B47" s="16"/>
+      <c r="C47" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="D47" s="4">
+        <v>11.849</v>
+      </c>
+      <c r="E47" s="4">
+        <v>272.72000000000003</v>
+      </c>
+      <c r="F47" s="4">
+        <v>0.21346999999999999</v>
+      </c>
+      <c r="G47" s="4">
+        <v>3.8447</v>
+      </c>
+      <c r="H47" s="4">
+        <v>1238.3</v>
+      </c>
+      <c r="I47" s="4">
+        <v>1731</v>
+      </c>
+      <c r="J47" s="4">
+        <v>4.5635000000000003</v>
+      </c>
+      <c r="K47" s="4">
+        <v>7.4757999999999996</v>
+      </c>
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A48" s="13"/>
       <c r="B48" s="16"/>
-      <c r="I48" s="2"/>
-      <c r="J48" s="2"/>
-      <c r="K48" s="2"/>
+      <c r="C48" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D48" s="4">
+        <v>7.9996999999999998</v>
+      </c>
+      <c r="E48" s="4">
+        <v>25.007999999999999</v>
+      </c>
+      <c r="F48" s="4">
+        <v>2.2597</v>
+      </c>
+      <c r="G48" s="4">
+        <v>4.1269999999999998</v>
+      </c>
+      <c r="H48" s="4">
+        <v>1102.2</v>
+      </c>
+      <c r="I48" s="2">
+        <v>1841.7</v>
+      </c>
+      <c r="J48" s="2">
+        <v>4.5534999999999997</v>
+      </c>
+      <c r="K48" s="2">
+        <v>10.206</v>
+      </c>
     </row>
     <row r="49" spans="1:12" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="14"/>
@@ -5549,18 +5753,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A38:A49"/>
+    <mergeCell ref="B38:B49"/>
+    <mergeCell ref="A50:A61"/>
+    <mergeCell ref="B50:B61"/>
+    <mergeCell ref="A62:A73"/>
+    <mergeCell ref="B62:B73"/>
     <mergeCell ref="A2:A13"/>
     <mergeCell ref="B2:B13"/>
     <mergeCell ref="A14:A25"/>
     <mergeCell ref="B14:B25"/>
     <mergeCell ref="A26:A37"/>
     <mergeCell ref="B26:B37"/>
-    <mergeCell ref="A38:A49"/>
-    <mergeCell ref="B38:B49"/>
-    <mergeCell ref="A50:A61"/>
-    <mergeCell ref="B50:B61"/>
-    <mergeCell ref="A62:A73"/>
-    <mergeCell ref="B62:B73"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -6774,18 +6978,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A2:A13"/>
+    <mergeCell ref="B2:B13"/>
+    <mergeCell ref="A14:A25"/>
+    <mergeCell ref="B14:B25"/>
+    <mergeCell ref="A26:A37"/>
+    <mergeCell ref="B26:B37"/>
     <mergeCell ref="A38:A49"/>
     <mergeCell ref="B38:B49"/>
     <mergeCell ref="A50:A61"/>
     <mergeCell ref="B50:B61"/>
     <mergeCell ref="A62:A73"/>
     <mergeCell ref="B62:B73"/>
-    <mergeCell ref="A2:A13"/>
-    <mergeCell ref="B2:B13"/>
-    <mergeCell ref="A14:A25"/>
-    <mergeCell ref="B14:B25"/>
-    <mergeCell ref="A26:A37"/>
-    <mergeCell ref="B26:B37"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -7201,18 +7405,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A38:A49"/>
+    <mergeCell ref="B38:B49"/>
+    <mergeCell ref="A50:A61"/>
+    <mergeCell ref="B50:B61"/>
+    <mergeCell ref="A62:A73"/>
+    <mergeCell ref="B62:B73"/>
     <mergeCell ref="A2:A13"/>
     <mergeCell ref="B2:B13"/>
     <mergeCell ref="A14:A25"/>
     <mergeCell ref="B14:B25"/>
     <mergeCell ref="A26:A37"/>
     <mergeCell ref="B26:B37"/>
-    <mergeCell ref="A38:A49"/>
-    <mergeCell ref="B38:B49"/>
-    <mergeCell ref="A50:A61"/>
-    <mergeCell ref="B50:B61"/>
-    <mergeCell ref="A62:A73"/>
-    <mergeCell ref="B62:B73"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
added all sem results for evpcd
</commit_message>
<xml_diff>
--- a/scripts/__other__/__sem__.xlsx
+++ b/scripts/__other__/__sem__.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Janzen\Desktop\code\moga_neml\scripts\__other__\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D198638C-591B-46A3-9347-CB91288CD462}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4281FF1-1F1B-4A74-9E7C-8C33147D4FBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="15600" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="evp" sheetId="13" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="45">
   <si>
     <t>temp</t>
   </si>
@@ -157,9 +157,6 @@
   </si>
   <si>
     <t>9; 7</t>
-  </si>
-  <si>
-    <t>8; 6</t>
   </si>
   <si>
     <t>evp-cd_f</t>
@@ -374,1072 +371,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>204198</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>49698</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>24</xdr:col>
-      <xdr:colOff>345002</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>186362</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="10" name="Picture 9">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{60E02592-69E5-5340-EA44-6900EE49FFD7}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="13348698" y="240198"/>
-          <a:ext cx="3789612" cy="1909779"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>198784</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>41415</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>24</xdr:col>
-      <xdr:colOff>331301</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>173935</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="11" name="Picture 10">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6E13AFE2-FE68-0998-7EDB-B7915E90A03E}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="11322327" y="2252872"/>
-          <a:ext cx="3809996" cy="1904998"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>231914</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>41412</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>24</xdr:col>
-      <xdr:colOff>401248</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>190499</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="12" name="Picture 11">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FC7F3F7B-E7BE-D52A-4508-858F51AD5EED}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="11355457" y="4273825"/>
-          <a:ext cx="3846813" cy="1921565"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>238125</xdr:colOff>
-      <xdr:row>38</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>24</xdr:col>
-      <xdr:colOff>409575</xdr:colOff>
-      <xdr:row>48</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="13" name="Picture 12">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8327A454-9110-1BC4-6A15-6937729DA59A}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="11306175" y="6305550"/>
-          <a:ext cx="3829050" cy="1914525"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>65943</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>161192</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>14653</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="14" name="Picture 13">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3C07A6C5-78ED-25E8-5E02-FD43AB5A2D69}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="9561635" y="249115"/>
-          <a:ext cx="1919653" cy="1919653"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>87925</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>36634</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>212481</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>21979</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="15" name="Picture 14">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1119B891-843A-59E6-A84D-EF4025013A32}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="11408021" y="227134"/>
-          <a:ext cx="1948960" cy="1948960"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>45902</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>33618</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>171450</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>16333</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="16" name="Picture 15">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4B1D1A6F-68FF-39A6-0FD4-F47C0D14BDCD}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="9551852" y="2243418"/>
-          <a:ext cx="1954348" cy="1944865"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>131885</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>31506</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>228600</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>178868</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="17" name="Picture 16">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4FF3334C-8450-409E-C836-7337AD330FDD}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="11466635" y="2241306"/>
-          <a:ext cx="1925515" cy="1919012"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>49091</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>46894</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>142875</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>1423</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="18" name="Picture 17">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{92A243BE-C9FD-9A1F-16BF-4DF0AA2AF7E2}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="9555041" y="4275994"/>
-          <a:ext cx="1922584" cy="1916679"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>116498</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>25646</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>238125</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>10324</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="19" name="Picture 18">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E0102139-6119-B4CF-C6F7-EC31C7714E33}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="11451248" y="4254746"/>
-          <a:ext cx="1950427" cy="1946828"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>38099</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>19049</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>133350</xdr:colOff>
-      <xdr:row>47</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="20" name="Picture 19">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{43F263AF-9D67-305A-04A9-D26BB2EA9F71}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="9544049" y="6267449"/>
-          <a:ext cx="1924051" cy="1924051"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>76200</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>190500</xdr:colOff>
-      <xdr:row>48</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="21" name="Picture 20">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{71E7E10A-A351-D44A-2886-D8BC97424D5E}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId12"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="11410950" y="6286500"/>
-          <a:ext cx="1943100" cy="1943100"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>28575</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>104775</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{69DA5A1B-9569-10C7-25ED-AEFDF30D9B72}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="7172325" y="247650"/>
-          <a:ext cx="1905000" cy="1905000"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>85725</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>190500</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{056B1923-F0F7-F1B1-2A73-0F28E2460C60}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="9058275" y="219075"/>
-          <a:ext cx="1933575" cy="1933575"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>262559</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>22777</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>23</xdr:col>
-      <xdr:colOff>431288</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>161855</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Picture 3">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{964D8901-33E2-3935-18FE-CC641ECC7028}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="11121059" y="213277"/>
-          <a:ext cx="3846207" cy="1911556"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>41412</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>24849</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>157369</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>16567</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="5" name="Picture 4">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{401E5F7B-6B7F-D60D-61D0-2F1E8C2EF3BD}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="7222434" y="2236306"/>
-          <a:ext cx="1954696" cy="1954696"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>140805</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>24847</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>256761</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>16564</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="6" name="Picture 5">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CB670FC0-93B5-7858-2032-A705893DEFDA}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="9160566" y="2236304"/>
-          <a:ext cx="1954695" cy="1954695"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>231913</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>33131</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>23</xdr:col>
-      <xdr:colOff>437030</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>11379</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="7" name="Picture 6">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{85D7DDE1-3557-9427-671D-BA5F0BD620E4}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="10967148" y="2240690"/>
-          <a:ext cx="3835823" cy="1939277"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>51290</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>21981</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>183174</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>14654</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="8" name="Picture 7">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CF01C1FA-1538-022B-312D-27EA77492DDC}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="7180386" y="4256943"/>
-          <a:ext cx="1956288" cy="1956288"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>314740</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>49696</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>23</xdr:col>
-      <xdr:colOff>439312</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>177363</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="10" name="Picture 9">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8F59AE14-82C2-67E5-4773-BDE18467080D}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="11140395" y="4286679"/>
-          <a:ext cx="3790055" cy="1901287"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>39412</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>39413</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>137947</xdr:colOff>
-      <xdr:row>48</xdr:row>
-      <xdr:rowOff>6569</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="12" name="Picture 11">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CD96A227-EBA0-8DE0-C6F6-8E9DF1DD2499}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="7199584" y="6299637"/>
-          <a:ext cx="1931277" cy="1931277"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>151087</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>32845</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>271097</xdr:colOff>
-      <xdr:row>48</xdr:row>
-      <xdr:rowOff>21726</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="13" name="Picture 12">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D6127B03-D0C1-9321-6F47-4FCD42443831}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="9104587" y="6290037"/>
-          <a:ext cx="1944414" cy="1952497"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>285292</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>30682</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>23</xdr:col>
-      <xdr:colOff>476249</xdr:colOff>
-      <xdr:row>47</xdr:row>
-      <xdr:rowOff>176551</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="14" name="Picture 13">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{391005F3-D050-42A5-B95F-F0584C9591C8}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="11048542" y="6293370"/>
-          <a:ext cx="3834270" cy="1919900"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>172639</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>53578</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>291702</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>29766</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="15" name="Picture 14">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9DC7C34D-24B9-5EB5-99C1-EAA5E9BDE018}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId12"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="9114233" y="4292203"/>
-          <a:ext cx="1940719" cy="1940719"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1709,7 +640,7 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K35" sqref="K35"/>
+      <selection pane="bottomLeft" activeCell="T41" sqref="T41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1731,7 +662,7 @@
         <v>11</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D1" s="5" t="s">
         <v>1</v>
@@ -1749,16 +680,16 @@
         <v>5</v>
       </c>
       <c r="I1" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="J1" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="K1" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="J1" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="K1" s="7" t="s">
+      <c r="L1" s="7" t="s">
         <v>41</v>
-      </c>
-      <c r="L1" s="7" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
@@ -1791,6 +722,9 @@
         <v>1783.5</v>
       </c>
       <c r="I3" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="J3" s="8" t="s">
         <v>22</v>
       </c>
       <c r="K3" s="8" t="s">
@@ -1819,7 +753,10 @@
         <v>1621.6</v>
       </c>
       <c r="I4" s="8" t="s">
-        <v>39</v>
+        <v>29</v>
+      </c>
+      <c r="J4" s="8" t="s">
+        <v>26</v>
       </c>
       <c r="K4" s="8" t="s">
         <v>30</v>
@@ -1847,7 +784,10 @@
         <v>1775.9</v>
       </c>
       <c r="I5" s="8" t="s">
-        <v>20</v>
+        <v>31</v>
+      </c>
+      <c r="J5" s="8" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
@@ -1872,6 +812,9 @@
         <v>1598.4</v>
       </c>
       <c r="I6" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="J6" s="8" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1897,6 +840,9 @@
         <v>1574.3</v>
       </c>
       <c r="I7" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="J7" s="8" t="s">
         <v>26</v>
       </c>
     </row>
@@ -1924,6 +870,9 @@
       <c r="I8" s="8" t="s">
         <v>19</v>
       </c>
+      <c r="J8" s="8" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="13"/>
@@ -1947,7 +896,10 @@
         <v>2454.8000000000002</v>
       </c>
       <c r="I9" s="8" t="s">
-        <v>25</v>
+        <v>23</v>
+      </c>
+      <c r="J9" s="8" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
@@ -1972,7 +924,10 @@
         <v>2390.5</v>
       </c>
       <c r="I10" s="8" t="s">
-        <v>19</v>
+        <v>29</v>
+      </c>
+      <c r="J10" s="8" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
@@ -1999,6 +954,9 @@
       <c r="I11" s="8" t="s">
         <v>38</v>
       </c>
+      <c r="J11" s="8" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="13"/>
@@ -2022,6 +980,9 @@
         <v>1841</v>
       </c>
       <c r="I12" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="J12" s="8" t="s">
         <v>26</v>
       </c>
     </row>
@@ -2067,6 +1028,9 @@
       <c r="I15" s="8" t="s">
         <v>20</v>
       </c>
+      <c r="J15" s="8" t="s">
+        <v>26</v>
+      </c>
       <c r="K15" s="8" t="s">
         <v>34</v>
       </c>
@@ -2093,7 +1057,10 @@
         <v>1828.1</v>
       </c>
       <c r="I16" s="8" t="s">
-        <v>21</v>
+        <v>34</v>
+      </c>
+      <c r="J16" s="8" t="s">
+        <v>26</v>
       </c>
       <c r="K16" s="8" t="s">
         <v>32</v>
@@ -2123,6 +1090,9 @@
       <c r="I17" s="8" t="s">
         <v>34</v>
       </c>
+      <c r="J17" s="8" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="13"/>
@@ -2146,7 +1116,10 @@
         <v>3172</v>
       </c>
       <c r="I18" s="8" t="s">
-        <v>23</v>
+        <v>24</v>
+      </c>
+      <c r="J18" s="8" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
@@ -2173,6 +1146,9 @@
       <c r="I19" s="8" t="s">
         <v>29</v>
       </c>
+      <c r="J19" s="8" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="13"/>
@@ -2198,6 +1174,9 @@
       <c r="I20" s="8" t="s">
         <v>38</v>
       </c>
+      <c r="J20" s="8" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="13"/>
@@ -2221,7 +1200,10 @@
         <v>2583</v>
       </c>
       <c r="I21" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
+      </c>
+      <c r="J21" s="8" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
@@ -2246,7 +1228,10 @@
         <v>2101.3000000000002</v>
       </c>
       <c r="I22" s="8" t="s">
-        <v>26</v>
+        <v>32</v>
+      </c>
+      <c r="J22" s="8" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
@@ -2273,6 +1258,9 @@
       <c r="I23" s="8" t="s">
         <v>29</v>
       </c>
+      <c r="J23" s="8" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="13"/>
@@ -2296,7 +1284,10 @@
         <v>3016.2</v>
       </c>
       <c r="I24" s="8" t="s">
-        <v>21</v>
+        <v>35</v>
+      </c>
+      <c r="J24" s="8" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="25" spans="1:12" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
@@ -2339,7 +1330,10 @@
         <v>1138.3</v>
       </c>
       <c r="I27" s="8" t="s">
-        <v>35</v>
+        <v>22</v>
+      </c>
+      <c r="J27" s="8" t="s">
+        <v>23</v>
       </c>
       <c r="K27" s="8" t="s">
         <v>22</v>
@@ -2367,7 +1361,10 @@
         <v>1433.5</v>
       </c>
       <c r="I28" s="8" t="s">
-        <v>20</v>
+        <v>26</v>
+      </c>
+      <c r="J28" s="8" t="s">
+        <v>35</v>
       </c>
       <c r="K28" s="8" t="s">
         <v>32</v>
@@ -2395,7 +1392,10 @@
         <v>1163</v>
       </c>
       <c r="I29" s="8" t="s">
-        <v>18</v>
+        <v>35</v>
+      </c>
+      <c r="J29" s="8" t="s">
+        <v>35</v>
       </c>
       <c r="K29" s="8" t="s">
         <v>35</v>
@@ -2425,6 +1425,9 @@
       <c r="I30" s="8" t="s">
         <v>20</v>
       </c>
+      <c r="J30" s="8" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" s="13"/>
@@ -2448,7 +1451,10 @@
         <v>1787.3</v>
       </c>
       <c r="I31" s="8" t="s">
-        <v>20</v>
+        <v>38</v>
+      </c>
+      <c r="J31" s="8" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
@@ -2473,7 +1479,10 @@
         <v>1593.8</v>
       </c>
       <c r="I32" s="8" t="s">
-        <v>19</v>
+        <v>26</v>
+      </c>
+      <c r="J32" s="8" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="33" spans="1:17" x14ac:dyDescent="0.25">
@@ -2500,6 +1509,9 @@
       <c r="I33" s="8" t="s">
         <v>20</v>
       </c>
+      <c r="J33" s="8" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="34" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A34" s="13"/>
@@ -2523,7 +1535,10 @@
         <v>2110.6</v>
       </c>
       <c r="I34" s="8" t="s">
-        <v>35</v>
+        <v>31</v>
+      </c>
+      <c r="J34" s="8" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="35" spans="1:17" x14ac:dyDescent="0.25">
@@ -2548,7 +1563,10 @@
         <v>1210.4000000000001</v>
       </c>
       <c r="I35" s="8" t="s">
-        <v>19</v>
+        <v>34</v>
+      </c>
+      <c r="J35" s="8" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="36" spans="1:17" x14ac:dyDescent="0.25">
@@ -2573,7 +1591,10 @@
         <v>1369.1</v>
       </c>
       <c r="I36" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
+      </c>
+      <c r="J36" s="8" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="37" spans="1:17" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
@@ -2616,7 +1637,10 @@
         <v>1006.9</v>
       </c>
       <c r="I39" s="8" t="s">
-        <v>23</v>
+        <v>31</v>
+      </c>
+      <c r="J39" s="8" t="s">
+        <v>22</v>
       </c>
       <c r="K39" s="8" t="s">
         <v>31</v>
@@ -2649,7 +1673,10 @@
         <v>1829.9</v>
       </c>
       <c r="I40" s="8" t="s">
-        <v>38</v>
+        <v>36</v>
+      </c>
+      <c r="J40" s="8" t="s">
+        <v>22</v>
       </c>
       <c r="K40" s="8" t="s">
         <v>33</v>
@@ -2684,6 +1711,9 @@
       <c r="I41" s="8" t="s">
         <v>24</v>
       </c>
+      <c r="J41" s="8" t="s">
+        <v>23</v>
+      </c>
       <c r="K41" s="8" t="s">
         <v>34</v>
       </c>
@@ -2710,6 +1740,9 @@
         <v>1999.7</v>
       </c>
       <c r="I42" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="J42" s="8" t="s">
         <v>37</v>
       </c>
     </row>
@@ -2735,7 +1768,10 @@
         <v>2606.1999999999998</v>
       </c>
       <c r="I43" s="8" t="s">
-        <v>35</v>
+        <v>31</v>
+      </c>
+      <c r="J43" s="8" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="44" spans="1:17" x14ac:dyDescent="0.25">
@@ -2762,6 +1798,9 @@
       <c r="I44" s="8" t="s">
         <v>25</v>
       </c>
+      <c r="J44" s="8" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="45" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A45" s="13"/>
@@ -2787,6 +1826,9 @@
       <c r="I45" s="8" t="s">
         <v>23</v>
       </c>
+      <c r="J45" s="8" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="46" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A46" s="13"/>
@@ -2810,6 +1852,9 @@
         <v>1371.6</v>
       </c>
       <c r="I46" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="J46" s="8" t="s">
         <v>22</v>
       </c>
     </row>
@@ -2837,6 +1882,9 @@
       <c r="I47" s="8" t="s">
         <v>34</v>
       </c>
+      <c r="J47" s="8" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="48" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A48" s="13"/>
@@ -2860,7 +1908,10 @@
         <v>1090</v>
       </c>
       <c r="I48" s="8" t="s">
-        <v>26</v>
+        <v>34</v>
+      </c>
+      <c r="J48" s="8" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="49" spans="1:12" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
@@ -2991,22 +2042,21 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A38:A49"/>
+    <mergeCell ref="B38:B49"/>
+    <mergeCell ref="A50:A61"/>
+    <mergeCell ref="B50:B61"/>
+    <mergeCell ref="A62:A73"/>
+    <mergeCell ref="B62:B73"/>
     <mergeCell ref="A2:A13"/>
     <mergeCell ref="B2:B13"/>
     <mergeCell ref="A14:A25"/>
     <mergeCell ref="B14:B25"/>
     <mergeCell ref="A26:A37"/>
     <mergeCell ref="B26:B37"/>
-    <mergeCell ref="A38:A49"/>
-    <mergeCell ref="B38:B49"/>
-    <mergeCell ref="A50:A61"/>
-    <mergeCell ref="B50:B61"/>
-    <mergeCell ref="A62:A73"/>
-    <mergeCell ref="B62:B73"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
-  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -3014,9 +2064,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE483CC8-AF2C-4D5A-AEE5-EF7DF4EC0883}">
   <dimension ref="A1:L73"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C48" sqref="C48"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="Q17" sqref="Q17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3037,7 +2087,7 @@
         <v>11</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D1" s="5" t="s">
         <v>1</v>
@@ -3263,7 +2313,7 @@
       <c r="A9" s="13"/>
       <c r="B9" s="16"/>
       <c r="C9" s="8" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D9" s="4">
         <v>27.547000000000001</v>
@@ -3294,7 +2344,7 @@
       <c r="A10" s="13"/>
       <c r="B10" s="16"/>
       <c r="C10" s="8" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="D10" s="4">
         <v>27.885000000000002</v>
@@ -3587,7 +2637,7 @@
       <c r="A21" s="13"/>
       <c r="B21" s="16"/>
       <c r="C21" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D21" s="4">
         <v>31.137</v>
@@ -3618,7 +2668,7 @@
       <c r="A22" s="13"/>
       <c r="B22" s="16"/>
       <c r="C22" s="8" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="D22" s="4">
         <v>29.725999999999999</v>
@@ -3942,7 +2992,7 @@
       <c r="A34" s="13"/>
       <c r="B34" s="16"/>
       <c r="C34" s="8" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="D34" s="4">
         <v>15.185</v>
@@ -4142,7 +3192,7 @@
       <c r="A42" s="13"/>
       <c r="B42" s="16"/>
       <c r="C42" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D42" s="4">
         <v>4.6340000000000003</v>
@@ -4266,7 +3316,7 @@
       <c r="A46" s="13"/>
       <c r="B46" s="16"/>
       <c r="C46" s="8" t="s">
-        <v>22</v>
+        <v>31</v>
       </c>
       <c r="D46" s="4">
         <v>12.622</v>
@@ -4471,22 +3521,21 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A38:A49"/>
+    <mergeCell ref="B38:B49"/>
+    <mergeCell ref="A50:A61"/>
+    <mergeCell ref="B50:B61"/>
+    <mergeCell ref="A62:A73"/>
+    <mergeCell ref="B62:B73"/>
     <mergeCell ref="A2:A13"/>
     <mergeCell ref="B2:B13"/>
     <mergeCell ref="A14:A25"/>
     <mergeCell ref="B14:B25"/>
     <mergeCell ref="A26:A37"/>
     <mergeCell ref="B26:B37"/>
-    <mergeCell ref="A38:A49"/>
-    <mergeCell ref="B38:B49"/>
-    <mergeCell ref="A50:A61"/>
-    <mergeCell ref="B50:B61"/>
-    <mergeCell ref="A62:A73"/>
-    <mergeCell ref="B62:B73"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
-  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -4494,9 +3543,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF6E341A-51E3-4AF7-809B-A8594B1323BC}">
   <dimension ref="A1:L73"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I23" sqref="I23"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F55" sqref="F55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4517,7 +3566,7 @@
         <v>11</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D1" s="5" t="s">
         <v>1</v>
@@ -4742,13 +3791,64 @@
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="13"/>
       <c r="B9" s="16"/>
+      <c r="C9" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="D9" s="2">
+        <v>28.599</v>
+      </c>
+      <c r="E9" s="2">
+        <v>78.057000000000002</v>
+      </c>
+      <c r="F9" s="2">
+        <v>0.84292</v>
+      </c>
+      <c r="G9" s="2">
+        <v>3.8371</v>
+      </c>
+      <c r="H9" s="2">
+        <v>2441.5</v>
+      </c>
+      <c r="I9" s="2">
+        <v>2969.6</v>
+      </c>
+      <c r="J9" s="2">
+        <v>4.9976000000000003</v>
+      </c>
+      <c r="K9" s="2">
+        <v>10.641999999999999</v>
+      </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="13"/>
       <c r="B10" s="16"/>
-      <c r="I10" s="2"/>
-      <c r="J10" s="2"/>
-      <c r="K10" s="2"/>
+      <c r="C10" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="D10" s="2">
+        <v>29.978999999999999</v>
+      </c>
+      <c r="E10" s="2">
+        <v>119.58</v>
+      </c>
+      <c r="F10" s="2">
+        <v>0.55200000000000005</v>
+      </c>
+      <c r="G10" s="2">
+        <v>3.8504999999999998</v>
+      </c>
+      <c r="H10" s="2">
+        <v>2314.4</v>
+      </c>
+      <c r="I10" s="2">
+        <v>2808.8</v>
+      </c>
+      <c r="J10" s="2">
+        <v>5.0354000000000001</v>
+      </c>
+      <c r="K10" s="2">
+        <v>9.5434999999999999</v>
+      </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="13"/>
@@ -5015,46 +4115,94 @@
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="13"/>
       <c r="B21" s="16"/>
-      <c r="I21" s="2"/>
-      <c r="J21" s="2"/>
-      <c r="K21" s="2"/>
+      <c r="C21" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D21" s="2">
+        <v>30.401</v>
+      </c>
+      <c r="E21" s="2">
+        <v>34.817</v>
+      </c>
+      <c r="F21" s="2">
+        <v>4.5983000000000001</v>
+      </c>
+      <c r="G21" s="2">
+        <v>3.5323000000000002</v>
+      </c>
+      <c r="H21" s="2">
+        <v>2583</v>
+      </c>
+      <c r="I21" s="2">
+        <v>2520.9</v>
+      </c>
+      <c r="J21" s="2">
+        <v>5.1558999999999999</v>
+      </c>
+      <c r="K21" s="2">
+        <v>8.5891000000000002</v>
+      </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="13"/>
       <c r="B22" s="16"/>
-      <c r="I22" s="2"/>
-      <c r="J22" s="2"/>
-      <c r="K22" s="2"/>
+      <c r="C22" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="D22" s="4">
+        <v>5.0568999999999997</v>
+      </c>
+      <c r="E22" s="4">
+        <v>40.475999999999999</v>
+      </c>
+      <c r="F22" s="4">
+        <v>10.016999999999999</v>
+      </c>
+      <c r="G22" s="4">
+        <v>4.1585000000000001</v>
+      </c>
+      <c r="H22" s="4">
+        <v>1730.1</v>
+      </c>
+      <c r="I22" s="4">
+        <v>1998.1</v>
+      </c>
+      <c r="J22" s="4">
+        <v>5.5564</v>
+      </c>
+      <c r="K22" s="4">
+        <v>10.337</v>
+      </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="13"/>
       <c r="B23" s="16"/>
       <c r="C23" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="D23" s="4">
-        <v>5.0568999999999997</v>
-      </c>
-      <c r="E23" s="4">
-        <v>40.475999999999999</v>
-      </c>
-      <c r="F23" s="4">
-        <v>10.016999999999999</v>
-      </c>
-      <c r="G23" s="4">
-        <v>4.1585000000000001</v>
-      </c>
-      <c r="H23" s="4">
-        <v>1730.1</v>
-      </c>
-      <c r="I23" s="4">
-        <v>1998.1</v>
-      </c>
-      <c r="J23" s="4">
-        <v>5.5564</v>
-      </c>
-      <c r="K23" s="4">
-        <v>10.337</v>
+        <v>20</v>
+      </c>
+      <c r="D23" s="2">
+        <v>31.809000000000001</v>
+      </c>
+      <c r="E23" s="2">
+        <v>43.194000000000003</v>
+      </c>
+      <c r="F23" s="2">
+        <v>2.2399</v>
+      </c>
+      <c r="G23" s="2">
+        <v>3.9613</v>
+      </c>
+      <c r="H23" s="2">
+        <v>1820.1</v>
+      </c>
+      <c r="I23" s="2">
+        <v>2245.4</v>
+      </c>
+      <c r="J23" s="2">
+        <v>5.3178999999999998</v>
+      </c>
+      <c r="K23" s="2">
+        <v>8.5096000000000007</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
@@ -5291,13 +4439,64 @@
     <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" s="13"/>
       <c r="B33" s="16"/>
+      <c r="C33" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D33" s="4">
+        <v>5.6656000000000004</v>
+      </c>
+      <c r="E33" s="4">
+        <v>7.6356999999999999</v>
+      </c>
+      <c r="F33" s="4">
+        <v>9.1336999999999993</v>
+      </c>
+      <c r="G33" s="4">
+        <v>4.3000999999999996</v>
+      </c>
+      <c r="H33" s="4">
+        <v>1055.4000000000001</v>
+      </c>
+      <c r="I33" s="4">
+        <v>3494.5</v>
+      </c>
+      <c r="J33" s="4">
+        <v>3.9628999999999999</v>
+      </c>
+      <c r="K33" s="4">
+        <v>11.622999999999999</v>
+      </c>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" s="13"/>
       <c r="B34" s="16"/>
-      <c r="I34" s="2"/>
-      <c r="J34" s="2"/>
-      <c r="K34" s="2"/>
+      <c r="C34" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D34" s="2">
+        <v>15.177</v>
+      </c>
+      <c r="E34" s="2">
+        <v>64.875</v>
+      </c>
+      <c r="F34" s="2">
+        <v>1.1737</v>
+      </c>
+      <c r="G34" s="2">
+        <v>3.2002999999999999</v>
+      </c>
+      <c r="H34" s="2">
+        <v>2165.3000000000002</v>
+      </c>
+      <c r="I34" s="2">
+        <v>2320.3000000000002</v>
+      </c>
+      <c r="J34" s="2">
+        <v>4.1947999999999999</v>
+      </c>
+      <c r="K34" s="2">
+        <v>6.7274000000000003</v>
+      </c>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" s="13"/>
@@ -5564,16 +4763,64 @@
     <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A45" s="13"/>
       <c r="B45" s="16"/>
-      <c r="I45" s="2"/>
-      <c r="J45" s="2"/>
-      <c r="K45" s="2"/>
+      <c r="C45" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D45" s="2">
+        <v>6.4694000000000003</v>
+      </c>
+      <c r="E45" s="2">
+        <v>149.62</v>
+      </c>
+      <c r="F45" s="2">
+        <v>0.29610999999999998</v>
+      </c>
+      <c r="G45" s="2">
+        <v>4.1942000000000004</v>
+      </c>
+      <c r="H45" s="2">
+        <v>1123.8</v>
+      </c>
+      <c r="I45" s="2">
+        <v>2045.9</v>
+      </c>
+      <c r="J45" s="2">
+        <v>4.4272</v>
+      </c>
+      <c r="K45" s="2">
+        <v>9.5322999999999993</v>
+      </c>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A46" s="13"/>
       <c r="B46" s="16"/>
-      <c r="I46" s="2"/>
-      <c r="J46" s="2"/>
-      <c r="K46" s="2"/>
+      <c r="C46" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D46" s="2">
+        <v>12.617000000000001</v>
+      </c>
+      <c r="E46" s="2">
+        <v>119.8</v>
+      </c>
+      <c r="F46" s="2">
+        <v>0.37544</v>
+      </c>
+      <c r="G46" s="2">
+        <v>3.7416</v>
+      </c>
+      <c r="H46" s="2">
+        <v>1366.4</v>
+      </c>
+      <c r="I46" s="2">
+        <v>1894.5</v>
+      </c>
+      <c r="J46" s="2">
+        <v>4.5370999999999997</v>
+      </c>
+      <c r="K46" s="2">
+        <v>9.6135999999999999</v>
+      </c>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A47" s="13"/>
@@ -5753,18 +5000,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A2:A13"/>
+    <mergeCell ref="B2:B13"/>
+    <mergeCell ref="A14:A25"/>
+    <mergeCell ref="B14:B25"/>
+    <mergeCell ref="A26:A37"/>
+    <mergeCell ref="B26:B37"/>
     <mergeCell ref="A38:A49"/>
     <mergeCell ref="B38:B49"/>
     <mergeCell ref="A50:A61"/>
     <mergeCell ref="B50:B61"/>
     <mergeCell ref="A62:A73"/>
     <mergeCell ref="B62:B73"/>
-    <mergeCell ref="A2:A13"/>
-    <mergeCell ref="B2:B13"/>
-    <mergeCell ref="A14:A25"/>
-    <mergeCell ref="B14:B25"/>
-    <mergeCell ref="A26:A37"/>
-    <mergeCell ref="B26:B37"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -5799,7 +5046,7 @@
         <v>11</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D1" s="5" t="s">
         <v>1</v>
@@ -6978,18 +6225,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A38:A49"/>
+    <mergeCell ref="B38:B49"/>
+    <mergeCell ref="A50:A61"/>
+    <mergeCell ref="B50:B61"/>
+    <mergeCell ref="A62:A73"/>
+    <mergeCell ref="B62:B73"/>
     <mergeCell ref="A2:A13"/>
     <mergeCell ref="B2:B13"/>
     <mergeCell ref="A14:A25"/>
     <mergeCell ref="B14:B25"/>
     <mergeCell ref="A26:A37"/>
     <mergeCell ref="B26:B37"/>
-    <mergeCell ref="A38:A49"/>
-    <mergeCell ref="B38:B49"/>
-    <mergeCell ref="A50:A61"/>
-    <mergeCell ref="B50:B61"/>
-    <mergeCell ref="A62:A73"/>
-    <mergeCell ref="B62:B73"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -7024,7 +6271,7 @@
         <v>11</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D1" s="5" t="s">
         <v>1</v>
@@ -7405,18 +6652,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A2:A13"/>
+    <mergeCell ref="B2:B13"/>
+    <mergeCell ref="A14:A25"/>
+    <mergeCell ref="B14:B25"/>
+    <mergeCell ref="A26:A37"/>
+    <mergeCell ref="B26:B37"/>
     <mergeCell ref="A38:A49"/>
     <mergeCell ref="B38:B49"/>
     <mergeCell ref="A50:A61"/>
     <mergeCell ref="B50:B61"/>
     <mergeCell ref="A62:A73"/>
     <mergeCell ref="B62:B73"/>
-    <mergeCell ref="A2:A13"/>
-    <mergeCell ref="B2:B13"/>
-    <mergeCell ref="A14:A25"/>
-    <mergeCell ref="B14:B25"/>
-    <mergeCell ref="A26:A37"/>
-    <mergeCell ref="B26:B37"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
added new params to sem results
</commit_message>
<xml_diff>
--- a/scripts/__other__/__sem__.xlsx
+++ b/scripts/__other__/__sem__.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Janzen\Desktop\code\moga_neml\scripts\__other__\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4281FF1-1F1B-4A74-9E7C-8C33147D4FBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77059F96-D831-4F84-8CE5-02BA9B648BE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="evp" sheetId="13" r:id="rId1"/>
@@ -2042,18 +2042,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A2:A13"/>
+    <mergeCell ref="B2:B13"/>
+    <mergeCell ref="A14:A25"/>
+    <mergeCell ref="B14:B25"/>
+    <mergeCell ref="A26:A37"/>
+    <mergeCell ref="B26:B37"/>
     <mergeCell ref="A38:A49"/>
     <mergeCell ref="B38:B49"/>
     <mergeCell ref="A50:A61"/>
     <mergeCell ref="B50:B61"/>
     <mergeCell ref="A62:A73"/>
     <mergeCell ref="B62:B73"/>
-    <mergeCell ref="A2:A13"/>
-    <mergeCell ref="B2:B13"/>
-    <mergeCell ref="A14:A25"/>
-    <mergeCell ref="B14:B25"/>
-    <mergeCell ref="A26:A37"/>
-    <mergeCell ref="B26:B37"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -2064,9 +2064,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE483CC8-AF2C-4D5A-AEE5-EF7DF4EC0883}">
   <dimension ref="A1:L73"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Q17" sqref="Q17"/>
+      <selection pane="bottomLeft" activeCell="N17" sqref="N17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2530,14 +2530,14 @@
       <c r="H17" s="4">
         <v>2221.6</v>
       </c>
-      <c r="I17" s="4">
-        <v>4328.7</v>
-      </c>
-      <c r="J17" s="4">
-        <v>4.3678999999999997</v>
-      </c>
-      <c r="K17" s="4">
-        <v>5.3108000000000004</v>
+      <c r="I17" s="2">
+        <v>3182.9</v>
+      </c>
+      <c r="J17" s="2">
+        <v>4.6406999999999998</v>
+      </c>
+      <c r="K17" s="2">
+        <v>3.7244999999999999</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
@@ -3521,18 +3521,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A2:A13"/>
+    <mergeCell ref="B2:B13"/>
+    <mergeCell ref="A14:A25"/>
+    <mergeCell ref="B14:B25"/>
+    <mergeCell ref="A26:A37"/>
+    <mergeCell ref="B26:B37"/>
     <mergeCell ref="A38:A49"/>
     <mergeCell ref="B38:B49"/>
     <mergeCell ref="A50:A61"/>
     <mergeCell ref="B50:B61"/>
     <mergeCell ref="A62:A73"/>
     <mergeCell ref="B62:B73"/>
-    <mergeCell ref="A2:A13"/>
-    <mergeCell ref="B2:B13"/>
-    <mergeCell ref="A14:A25"/>
-    <mergeCell ref="B14:B25"/>
-    <mergeCell ref="A26:A37"/>
-    <mergeCell ref="B26:B37"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -3543,9 +3543,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF6E341A-51E3-4AF7-809B-A8594B1323BC}">
   <dimension ref="A1:L73"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F55" sqref="F55"/>
+      <selection pane="bottomLeft" activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3995,28 +3995,28 @@
         <v>34</v>
       </c>
       <c r="D17" s="2">
-        <v>13.247</v>
+        <v>10.788</v>
       </c>
       <c r="E17" s="2">
-        <v>47.88</v>
+        <v>53.85</v>
       </c>
       <c r="F17" s="2">
-        <v>7.2160000000000002</v>
+        <v>7.1745999999999999</v>
       </c>
       <c r="G17" s="2">
-        <v>3.9582999999999999</v>
+        <v>3.8603999999999998</v>
       </c>
       <c r="H17" s="2">
-        <v>2115.6</v>
+        <v>2196.3000000000002</v>
       </c>
       <c r="I17" s="2">
-        <v>3764.3</v>
+        <v>3182.9</v>
       </c>
       <c r="J17" s="2">
-        <v>4.4740000000000002</v>
+        <v>4.6458000000000004</v>
       </c>
       <c r="K17" s="2">
-        <v>5.1694000000000004</v>
+        <v>3.7222</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
@@ -5000,18 +5000,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A38:A49"/>
+    <mergeCell ref="B38:B49"/>
+    <mergeCell ref="A50:A61"/>
+    <mergeCell ref="B50:B61"/>
+    <mergeCell ref="A62:A73"/>
+    <mergeCell ref="B62:B73"/>
     <mergeCell ref="A2:A13"/>
     <mergeCell ref="B2:B13"/>
     <mergeCell ref="A14:A25"/>
     <mergeCell ref="B14:B25"/>
     <mergeCell ref="A26:A37"/>
     <mergeCell ref="B26:B37"/>
-    <mergeCell ref="A38:A49"/>
-    <mergeCell ref="B38:B49"/>
-    <mergeCell ref="A50:A61"/>
-    <mergeCell ref="B50:B61"/>
-    <mergeCell ref="A62:A73"/>
-    <mergeCell ref="B62:B73"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -6225,18 +6225,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A2:A13"/>
+    <mergeCell ref="B2:B13"/>
+    <mergeCell ref="A14:A25"/>
+    <mergeCell ref="B14:B25"/>
+    <mergeCell ref="A26:A37"/>
+    <mergeCell ref="B26:B37"/>
     <mergeCell ref="A38:A49"/>
     <mergeCell ref="B38:B49"/>
     <mergeCell ref="A50:A61"/>
     <mergeCell ref="B50:B61"/>
     <mergeCell ref="A62:A73"/>
     <mergeCell ref="B62:B73"/>
-    <mergeCell ref="A2:A13"/>
-    <mergeCell ref="B2:B13"/>
-    <mergeCell ref="A14:A25"/>
-    <mergeCell ref="B14:B25"/>
-    <mergeCell ref="A26:A37"/>
-    <mergeCell ref="B26:B37"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -6652,18 +6652,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A38:A49"/>
+    <mergeCell ref="B38:B49"/>
+    <mergeCell ref="A50:A61"/>
+    <mergeCell ref="B50:B61"/>
+    <mergeCell ref="A62:A73"/>
+    <mergeCell ref="B62:B73"/>
     <mergeCell ref="A2:A13"/>
     <mergeCell ref="B2:B13"/>
     <mergeCell ref="A14:A25"/>
     <mergeCell ref="B14:B25"/>
     <mergeCell ref="A26:A37"/>
     <mergeCell ref="B26:B37"/>
-    <mergeCell ref="A38:A49"/>
-    <mergeCell ref="B38:B49"/>
-    <mergeCell ref="A50:A61"/>
-    <mergeCell ref="B50:B61"/>
-    <mergeCell ref="A62:A73"/>
-    <mergeCell ref="B62:B73"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
Minor changes and changed number of steps in driver
</commit_message>
<xml_diff>
--- a/scripts/__other__/__sem__.xlsx
+++ b/scripts/__other__/__sem__.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Janzen\Desktop\code\moga_neml\scripts\__other__\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77059F96-D831-4F84-8CE5-02BA9B648BE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D045F33-5097-403A-B3C8-92DE9E7EF2E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="15600" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="evp" sheetId="13" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="46">
   <si>
     <t>temp</t>
   </si>
@@ -175,6 +175,9 @@
   </si>
   <si>
     <t>5; 10</t>
+  </si>
+  <si>
+    <t>6; 8</t>
   </si>
 </sst>
 </file>
@@ -2042,18 +2045,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A38:A49"/>
+    <mergeCell ref="B38:B49"/>
+    <mergeCell ref="A50:A61"/>
+    <mergeCell ref="B50:B61"/>
+    <mergeCell ref="A62:A73"/>
+    <mergeCell ref="B62:B73"/>
     <mergeCell ref="A2:A13"/>
     <mergeCell ref="B2:B13"/>
     <mergeCell ref="A14:A25"/>
     <mergeCell ref="B14:B25"/>
     <mergeCell ref="A26:A37"/>
     <mergeCell ref="B26:B37"/>
-    <mergeCell ref="A38:A49"/>
-    <mergeCell ref="B38:B49"/>
-    <mergeCell ref="A50:A61"/>
-    <mergeCell ref="B50:B61"/>
-    <mergeCell ref="A62:A73"/>
-    <mergeCell ref="B62:B73"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -2066,7 +2069,7 @@
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N17" sqref="N17"/>
+      <selection pane="bottomLeft" activeCell="D3" sqref="D3:K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2513,7 +2516,7 @@
       <c r="A17" s="13"/>
       <c r="B17" s="16"/>
       <c r="C17" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D17" s="4">
         <v>11.45</v>
@@ -3403,6 +3406,1485 @@
       </c>
       <c r="K48" s="2">
         <v>8.0541</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="14"/>
+      <c r="B49" s="17"/>
+      <c r="C49" s="7"/>
+      <c r="L49" s="11"/>
+    </row>
+    <row r="50" spans="1:12" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="12">
+        <v>1000</v>
+      </c>
+      <c r="B50" s="15" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A51" s="13"/>
+      <c r="B51" s="16"/>
+    </row>
+    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A52" s="13"/>
+      <c r="B52" s="16"/>
+    </row>
+    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A53" s="13"/>
+      <c r="B53" s="16"/>
+    </row>
+    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A54" s="13"/>
+      <c r="B54" s="16"/>
+    </row>
+    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A55" s="13"/>
+      <c r="B55" s="16"/>
+    </row>
+    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A56" s="13"/>
+      <c r="B56" s="16"/>
+    </row>
+    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A57" s="13"/>
+      <c r="B57" s="16"/>
+    </row>
+    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A58" s="13"/>
+      <c r="B58" s="16"/>
+    </row>
+    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A59" s="13"/>
+      <c r="B59" s="16"/>
+    </row>
+    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A60" s="13"/>
+      <c r="B60" s="16"/>
+    </row>
+    <row r="61" spans="1:12" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="14"/>
+      <c r="B61" s="17"/>
+      <c r="C61" s="7"/>
+      <c r="L61" s="11"/>
+    </row>
+    <row r="62" spans="1:12" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="12">
+        <v>1000</v>
+      </c>
+      <c r="B62" s="15" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A63" s="13"/>
+      <c r="B63" s="16"/>
+    </row>
+    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A64" s="13"/>
+      <c r="B64" s="16"/>
+    </row>
+    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A65" s="13"/>
+      <c r="B65" s="16"/>
+    </row>
+    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A66" s="13"/>
+      <c r="B66" s="16"/>
+    </row>
+    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A67" s="13"/>
+      <c r="B67" s="16"/>
+    </row>
+    <row r="68" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A68" s="13"/>
+      <c r="B68" s="16"/>
+    </row>
+    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A69" s="13"/>
+      <c r="B69" s="16"/>
+    </row>
+    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A70" s="13"/>
+      <c r="B70" s="16"/>
+    </row>
+    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A71" s="13"/>
+      <c r="B71" s="16"/>
+    </row>
+    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A72" s="13"/>
+      <c r="B72" s="16"/>
+    </row>
+    <row r="73" spans="1:12" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A73" s="14"/>
+      <c r="B73" s="17"/>
+      <c r="C73" s="7"/>
+      <c r="L73" s="11"/>
+    </row>
+  </sheetData>
+  <mergeCells count="12">
+    <mergeCell ref="A38:A49"/>
+    <mergeCell ref="B38:B49"/>
+    <mergeCell ref="A50:A61"/>
+    <mergeCell ref="B50:B61"/>
+    <mergeCell ref="A62:A73"/>
+    <mergeCell ref="B62:B73"/>
+    <mergeCell ref="A2:A13"/>
+    <mergeCell ref="B2:B13"/>
+    <mergeCell ref="A14:A25"/>
+    <mergeCell ref="B14:B25"/>
+    <mergeCell ref="A26:A37"/>
+    <mergeCell ref="B26:B37"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF6E341A-51E3-4AF7-809B-A8594B1323BC}">
+  <dimension ref="A1:L73"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G21" sqref="G21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="4"/>
+    <col min="2" max="2" width="9.140625" style="3"/>
+    <col min="3" max="3" width="15.7109375" style="8" customWidth="1"/>
+    <col min="4" max="11" width="9.140625" style="4"/>
+    <col min="12" max="12" width="9.140625" style="9"/>
+    <col min="13" max="16384" width="9.140625" style="4"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="11"/>
+    </row>
+    <row r="2" spans="1:12" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="12">
+        <v>800</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" s="13"/>
+      <c r="B3" s="16"/>
+      <c r="C3" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" s="4">
+        <v>16.994</v>
+      </c>
+      <c r="E3" s="4">
+        <v>187.83</v>
+      </c>
+      <c r="F3" s="4">
+        <v>0.26103999999999999</v>
+      </c>
+      <c r="G3" s="4">
+        <v>4.5019999999999998</v>
+      </c>
+      <c r="H3" s="4">
+        <v>1784.8</v>
+      </c>
+      <c r="I3" s="2">
+        <v>3263.5</v>
+      </c>
+      <c r="J3" s="2">
+        <v>4.9230999999999998</v>
+      </c>
+      <c r="K3" s="2">
+        <v>13.172000000000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" s="13"/>
+      <c r="B4" s="16"/>
+      <c r="C4" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D4" s="4">
+        <v>22.454000000000001</v>
+      </c>
+      <c r="E4" s="4">
+        <v>66.77</v>
+      </c>
+      <c r="F4" s="4">
+        <v>0.92681000000000002</v>
+      </c>
+      <c r="G4" s="4">
+        <v>4.4191000000000003</v>
+      </c>
+      <c r="H4" s="4">
+        <v>1610.1</v>
+      </c>
+      <c r="I4" s="2">
+        <v>2142</v>
+      </c>
+      <c r="J4" s="2">
+        <v>5.4843999999999999</v>
+      </c>
+      <c r="K4" s="2">
+        <v>11.449</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" s="13"/>
+      <c r="B5" s="16"/>
+      <c r="C5" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" s="4">
+        <v>9.1647999999999996</v>
+      </c>
+      <c r="E5" s="4">
+        <v>36.326000000000001</v>
+      </c>
+      <c r="F5" s="4">
+        <v>12.337</v>
+      </c>
+      <c r="G5" s="4">
+        <v>4.2247000000000003</v>
+      </c>
+      <c r="H5" s="4">
+        <v>1776.1</v>
+      </c>
+      <c r="I5" s="2">
+        <v>2731</v>
+      </c>
+      <c r="J5" s="2">
+        <v>5.0411000000000001</v>
+      </c>
+      <c r="K5" s="2">
+        <v>8.3102999999999998</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" s="13"/>
+      <c r="B6" s="16"/>
+      <c r="C6" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" s="4">
+        <v>5.8951000000000002</v>
+      </c>
+      <c r="E6" s="4">
+        <v>36.906999999999996</v>
+      </c>
+      <c r="F6" s="4">
+        <v>5.3551000000000002</v>
+      </c>
+      <c r="G6" s="4">
+        <v>4.7310999999999996</v>
+      </c>
+      <c r="H6" s="4">
+        <v>1557.8</v>
+      </c>
+      <c r="I6" s="2">
+        <v>2224.1</v>
+      </c>
+      <c r="J6" s="2">
+        <v>5.2808999999999999</v>
+      </c>
+      <c r="K6" s="2">
+        <v>6.5113000000000003</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" s="13"/>
+      <c r="B7" s="16"/>
+      <c r="C7" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D7" s="4">
+        <v>4.1860999999999997</v>
+      </c>
+      <c r="E7" s="4">
+        <v>84.548000000000002</v>
+      </c>
+      <c r="F7" s="4">
+        <v>2.1124999999999998</v>
+      </c>
+      <c r="G7" s="4">
+        <v>4.7670000000000003</v>
+      </c>
+      <c r="H7" s="4">
+        <v>1574.1</v>
+      </c>
+      <c r="I7" s="4">
+        <v>2883.2</v>
+      </c>
+      <c r="J7" s="4">
+        <v>4.8395000000000001</v>
+      </c>
+      <c r="K7" s="4">
+        <v>4.5430999999999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" s="13"/>
+      <c r="B8" s="16"/>
+      <c r="C8" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" s="2">
+        <v>27.867999999999999</v>
+      </c>
+      <c r="E8" s="2">
+        <v>89.338999999999999</v>
+      </c>
+      <c r="F8" s="2">
+        <v>0.59711999999999998</v>
+      </c>
+      <c r="G8" s="2">
+        <v>4.1981999999999999</v>
+      </c>
+      <c r="H8" s="2">
+        <v>1818</v>
+      </c>
+      <c r="I8" s="2">
+        <v>2645.2</v>
+      </c>
+      <c r="J8" s="2">
+        <v>5.1192000000000002</v>
+      </c>
+      <c r="K8" s="2">
+        <v>10.125</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" s="13"/>
+      <c r="B9" s="16"/>
+      <c r="C9" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="D9" s="2">
+        <v>28.599</v>
+      </c>
+      <c r="E9" s="2">
+        <v>78.057000000000002</v>
+      </c>
+      <c r="F9" s="2">
+        <v>0.84292</v>
+      </c>
+      <c r="G9" s="2">
+        <v>3.8371</v>
+      </c>
+      <c r="H9" s="2">
+        <v>2441.5</v>
+      </c>
+      <c r="I9" s="2">
+        <v>2969.6</v>
+      </c>
+      <c r="J9" s="2">
+        <v>4.9976000000000003</v>
+      </c>
+      <c r="K9" s="2">
+        <v>10.641999999999999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" s="13"/>
+      <c r="B10" s="16"/>
+      <c r="C10" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="D10" s="2">
+        <v>29.978999999999999</v>
+      </c>
+      <c r="E10" s="2">
+        <v>119.58</v>
+      </c>
+      <c r="F10" s="2">
+        <v>0.55200000000000005</v>
+      </c>
+      <c r="G10" s="2">
+        <v>3.8504999999999998</v>
+      </c>
+      <c r="H10" s="2">
+        <v>2314.4</v>
+      </c>
+      <c r="I10" s="2">
+        <v>2808.8</v>
+      </c>
+      <c r="J10" s="2">
+        <v>5.0354000000000001</v>
+      </c>
+      <c r="K10" s="2">
+        <v>9.5434999999999999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" s="13"/>
+      <c r="B11" s="16"/>
+      <c r="C11" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="D11" s="4">
+        <v>19.125</v>
+      </c>
+      <c r="E11" s="4">
+        <v>43.640999999999998</v>
+      </c>
+      <c r="F11" s="4">
+        <v>5.6147999999999998</v>
+      </c>
+      <c r="G11" s="4">
+        <v>4.1688000000000001</v>
+      </c>
+      <c r="H11" s="4">
+        <v>1616</v>
+      </c>
+      <c r="I11" s="4">
+        <v>1876.8</v>
+      </c>
+      <c r="J11" s="4">
+        <v>5.5594000000000001</v>
+      </c>
+      <c r="K11" s="4">
+        <v>6.8653000000000004</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" s="13"/>
+      <c r="B12" s="16"/>
+      <c r="C12" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D12" s="4">
+        <v>22.012</v>
+      </c>
+      <c r="E12" s="4">
+        <v>38.872999999999998</v>
+      </c>
+      <c r="F12" s="4">
+        <v>2.2033</v>
+      </c>
+      <c r="G12" s="4">
+        <v>4.2450000000000001</v>
+      </c>
+      <c r="H12" s="4">
+        <v>1841.2</v>
+      </c>
+      <c r="I12" s="2">
+        <v>2377</v>
+      </c>
+      <c r="J12" s="2">
+        <v>5.2897999999999996</v>
+      </c>
+      <c r="K12" s="2">
+        <v>9.7712000000000003</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="14"/>
+      <c r="B13" s="17"/>
+      <c r="C13" s="7"/>
+      <c r="L13" s="11"/>
+    </row>
+    <row r="14" spans="1:12" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="12">
+        <v>800</v>
+      </c>
+      <c r="B14" s="15" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15" s="13"/>
+      <c r="B15" s="16"/>
+      <c r="C15" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D15" s="4">
+        <v>31.646999999999998</v>
+      </c>
+      <c r="E15" s="4">
+        <v>120.62</v>
+      </c>
+      <c r="F15" s="4">
+        <v>0.85485</v>
+      </c>
+      <c r="G15" s="4">
+        <v>3.7265999999999999</v>
+      </c>
+      <c r="H15" s="4">
+        <v>2297.8000000000002</v>
+      </c>
+      <c r="I15" s="4">
+        <v>2165.6999999999998</v>
+      </c>
+      <c r="J15" s="4">
+        <v>5.3247</v>
+      </c>
+      <c r="K15" s="4">
+        <v>7.7724000000000002</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A16" s="13"/>
+      <c r="B16" s="16"/>
+      <c r="C16" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D16" s="2">
+        <v>33.296999999999997</v>
+      </c>
+      <c r="E16" s="2">
+        <v>522.85</v>
+      </c>
+      <c r="F16" s="2">
+        <v>0.11871</v>
+      </c>
+      <c r="G16" s="2">
+        <v>3.9767000000000001</v>
+      </c>
+      <c r="H16" s="2">
+        <v>1762.4</v>
+      </c>
+      <c r="I16" s="2">
+        <v>1913.8</v>
+      </c>
+      <c r="J16" s="2">
+        <v>5.6638000000000002</v>
+      </c>
+      <c r="K16" s="2">
+        <v>11.287000000000001</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A17" s="13"/>
+      <c r="B17" s="16"/>
+      <c r="C17" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="D17" s="2">
+        <v>10.788</v>
+      </c>
+      <c r="E17" s="2">
+        <v>53.85</v>
+      </c>
+      <c r="F17" s="2">
+        <v>7.1745999999999999</v>
+      </c>
+      <c r="G17" s="2">
+        <v>3.8603999999999998</v>
+      </c>
+      <c r="H17" s="2">
+        <v>2196.3000000000002</v>
+      </c>
+      <c r="I17" s="2">
+        <v>3182.9</v>
+      </c>
+      <c r="J17" s="2">
+        <v>4.6458000000000004</v>
+      </c>
+      <c r="K17" s="2">
+        <v>3.7222</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A18" s="13"/>
+      <c r="B18" s="16"/>
+      <c r="C18" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D18" s="2">
+        <v>38.180999999999997</v>
+      </c>
+      <c r="E18" s="2">
+        <v>51.055</v>
+      </c>
+      <c r="F18" s="2">
+        <v>2.4819</v>
+      </c>
+      <c r="G18" s="2">
+        <v>3.2572000000000001</v>
+      </c>
+      <c r="H18" s="2">
+        <v>3154.4</v>
+      </c>
+      <c r="I18" s="2">
+        <v>2725.2</v>
+      </c>
+      <c r="J18" s="2">
+        <v>5.0167000000000002</v>
+      </c>
+      <c r="K18" s="2">
+        <v>8.33</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A19" s="13"/>
+      <c r="B19" s="16"/>
+      <c r="C19" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="D19" s="4">
+        <v>24.888999999999999</v>
+      </c>
+      <c r="E19" s="4">
+        <v>44.932000000000002</v>
+      </c>
+      <c r="F19" s="4">
+        <v>1.2076</v>
+      </c>
+      <c r="G19" s="4">
+        <v>4.5054999999999996</v>
+      </c>
+      <c r="H19" s="4">
+        <v>1527.9</v>
+      </c>
+      <c r="I19" s="4">
+        <v>2589.6999999999998</v>
+      </c>
+      <c r="J19" s="4">
+        <v>5.1066000000000003</v>
+      </c>
+      <c r="K19" s="4">
+        <v>8.6950000000000003</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A20" s="13"/>
+      <c r="B20" s="16"/>
+      <c r="C20" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D20" s="2">
+        <v>23.303999999999998</v>
+      </c>
+      <c r="E20" s="2">
+        <v>276.66000000000003</v>
+      </c>
+      <c r="F20" s="2">
+        <v>0.32123000000000002</v>
+      </c>
+      <c r="G20" s="2">
+        <v>4.2591999999999999</v>
+      </c>
+      <c r="H20" s="2">
+        <v>1767.2</v>
+      </c>
+      <c r="I20" s="2">
+        <v>2168.5</v>
+      </c>
+      <c r="J20" s="2">
+        <v>5.3181000000000003</v>
+      </c>
+      <c r="K20" s="2">
+        <v>6.7618999999999998</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A21" s="13"/>
+      <c r="B21" s="16"/>
+      <c r="C21" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D21" s="2">
+        <v>30.401</v>
+      </c>
+      <c r="E21" s="2">
+        <v>34.817</v>
+      </c>
+      <c r="F21" s="2">
+        <v>4.5983000000000001</v>
+      </c>
+      <c r="G21" s="2">
+        <v>3.5323000000000002</v>
+      </c>
+      <c r="H21" s="2">
+        <v>2583</v>
+      </c>
+      <c r="I21" s="2">
+        <v>2520.9</v>
+      </c>
+      <c r="J21" s="2">
+        <v>5.1558999999999999</v>
+      </c>
+      <c r="K21" s="2">
+        <v>8.5891000000000002</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A22" s="13"/>
+      <c r="B22" s="16"/>
+      <c r="C22" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="D22" s="4">
+        <v>5.0568999999999997</v>
+      </c>
+      <c r="E22" s="4">
+        <v>40.475999999999999</v>
+      </c>
+      <c r="F22" s="4">
+        <v>10.016999999999999</v>
+      </c>
+      <c r="G22" s="4">
+        <v>4.1585000000000001</v>
+      </c>
+      <c r="H22" s="4">
+        <v>1730.1</v>
+      </c>
+      <c r="I22" s="4">
+        <v>1998.1</v>
+      </c>
+      <c r="J22" s="4">
+        <v>5.5564</v>
+      </c>
+      <c r="K22" s="4">
+        <v>10.337</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A23" s="13"/>
+      <c r="B23" s="16"/>
+      <c r="C23" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D23" s="2">
+        <v>31.809000000000001</v>
+      </c>
+      <c r="E23" s="2">
+        <v>43.194000000000003</v>
+      </c>
+      <c r="F23" s="2">
+        <v>2.2399</v>
+      </c>
+      <c r="G23" s="2">
+        <v>3.9613</v>
+      </c>
+      <c r="H23" s="2">
+        <v>1820.1</v>
+      </c>
+      <c r="I23" s="2">
+        <v>2245.4</v>
+      </c>
+      <c r="J23" s="2">
+        <v>5.3178999999999998</v>
+      </c>
+      <c r="K23" s="2">
+        <v>8.5096000000000007</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A24" s="13"/>
+      <c r="B24" s="16"/>
+      <c r="C24" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="D24" s="4">
+        <v>0.36498999999999998</v>
+      </c>
+      <c r="E24" s="4">
+        <v>45.374000000000002</v>
+      </c>
+      <c r="F24" s="4">
+        <v>15.686999999999999</v>
+      </c>
+      <c r="G24" s="4">
+        <v>3.6105</v>
+      </c>
+      <c r="H24" s="4">
+        <v>2878.3</v>
+      </c>
+      <c r="I24" s="2">
+        <v>3325.8</v>
+      </c>
+      <c r="J24" s="2">
+        <v>4.8470000000000004</v>
+      </c>
+      <c r="K24" s="2">
+        <v>12.327999999999999</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="14"/>
+      <c r="B25" s="17"/>
+      <c r="C25" s="7"/>
+      <c r="L25" s="11"/>
+    </row>
+    <row r="26" spans="1:12" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="12">
+        <v>900</v>
+      </c>
+      <c r="B26" s="15" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A27" s="13"/>
+      <c r="B27" s="16"/>
+      <c r="C27" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D27" s="2">
+        <v>3.6261999999999999</v>
+      </c>
+      <c r="E27" s="2">
+        <v>13.804</v>
+      </c>
+      <c r="F27" s="2">
+        <v>6.9824999999999999</v>
+      </c>
+      <c r="G27" s="2">
+        <v>4.2416</v>
+      </c>
+      <c r="H27" s="2">
+        <v>1138.2</v>
+      </c>
+      <c r="I27" s="2">
+        <v>1986</v>
+      </c>
+      <c r="J27" s="2">
+        <v>4.4408000000000003</v>
+      </c>
+      <c r="K27" s="2">
+        <v>9.1929999999999996</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A28" s="13"/>
+      <c r="B28" s="16"/>
+      <c r="C28" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="D28" s="2">
+        <v>10.683</v>
+      </c>
+      <c r="E28" s="2">
+        <v>31.381</v>
+      </c>
+      <c r="F28" s="2">
+        <v>2.9727000000000001</v>
+      </c>
+      <c r="G28" s="2">
+        <v>3.7155</v>
+      </c>
+      <c r="H28" s="2">
+        <v>1422</v>
+      </c>
+      <c r="I28" s="2">
+        <v>1626.7</v>
+      </c>
+      <c r="J28" s="2">
+        <v>4.5519999999999996</v>
+      </c>
+      <c r="K28" s="2">
+        <v>6.2319000000000004</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A29" s="13"/>
+      <c r="B29" s="16"/>
+      <c r="C29" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="D29" s="2">
+        <v>10.340999999999999</v>
+      </c>
+      <c r="E29" s="2">
+        <v>24.475999999999999</v>
+      </c>
+      <c r="F29" s="2">
+        <v>2.3226</v>
+      </c>
+      <c r="G29" s="2">
+        <v>3.9651000000000001</v>
+      </c>
+      <c r="H29" s="2">
+        <v>1176.4000000000001</v>
+      </c>
+      <c r="I29" s="2">
+        <v>1743</v>
+      </c>
+      <c r="J29" s="2">
+        <v>4.5865</v>
+      </c>
+      <c r="K29" s="2">
+        <v>9.1586999999999996</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A30" s="13"/>
+      <c r="B30" s="16"/>
+      <c r="C30" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D30" s="2">
+        <v>11.112</v>
+      </c>
+      <c r="E30" s="2">
+        <v>18.959</v>
+      </c>
+      <c r="F30" s="2">
+        <v>5.9504999999999999</v>
+      </c>
+      <c r="G30" s="2">
+        <v>3.6368</v>
+      </c>
+      <c r="H30" s="2">
+        <v>1471.6</v>
+      </c>
+      <c r="I30" s="2">
+        <v>2064.3000000000002</v>
+      </c>
+      <c r="J30" s="2">
+        <v>4.3163999999999998</v>
+      </c>
+      <c r="K30" s="2">
+        <v>7.2249999999999996</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A31" s="13"/>
+      <c r="B31" s="16"/>
+      <c r="C31" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D31" s="2">
+        <v>8.0817999999999994</v>
+      </c>
+      <c r="E31" s="2">
+        <v>9.2744</v>
+      </c>
+      <c r="F31" s="2">
+        <v>7.9561999999999999</v>
+      </c>
+      <c r="G31" s="2">
+        <v>3.9839000000000002</v>
+      </c>
+      <c r="H31" s="2">
+        <v>1310.7</v>
+      </c>
+      <c r="I31" s="2">
+        <v>4972.3999999999996</v>
+      </c>
+      <c r="J31" s="2">
+        <v>3.6442999999999999</v>
+      </c>
+      <c r="K31" s="2">
+        <v>9.6707000000000001</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A32" s="13"/>
+      <c r="B32" s="16"/>
+      <c r="C32" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D32" s="2">
+        <v>11.394</v>
+      </c>
+      <c r="E32" s="2">
+        <v>13.887</v>
+      </c>
+      <c r="F32" s="2">
+        <v>7.532</v>
+      </c>
+      <c r="G32" s="2">
+        <v>3.5691000000000002</v>
+      </c>
+      <c r="H32" s="2">
+        <v>1581.2</v>
+      </c>
+      <c r="I32" s="2">
+        <v>1959.8</v>
+      </c>
+      <c r="J32" s="2">
+        <v>4.4120999999999997</v>
+      </c>
+      <c r="K32" s="2">
+        <v>8.5846999999999998</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A33" s="13"/>
+      <c r="B33" s="16"/>
+      <c r="C33" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D33" s="4">
+        <v>5.6656000000000004</v>
+      </c>
+      <c r="E33" s="4">
+        <v>7.6356999999999999</v>
+      </c>
+      <c r="F33" s="4">
+        <v>9.1336999999999993</v>
+      </c>
+      <c r="G33" s="4">
+        <v>4.3000999999999996</v>
+      </c>
+      <c r="H33" s="4">
+        <v>1055.4000000000001</v>
+      </c>
+      <c r="I33" s="4">
+        <v>3494.5</v>
+      </c>
+      <c r="J33" s="4">
+        <v>3.9628999999999999</v>
+      </c>
+      <c r="K33" s="4">
+        <v>11.622999999999999</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A34" s="13"/>
+      <c r="B34" s="16"/>
+      <c r="C34" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D34" s="2">
+        <v>15.177</v>
+      </c>
+      <c r="E34" s="2">
+        <v>64.875</v>
+      </c>
+      <c r="F34" s="2">
+        <v>1.1737</v>
+      </c>
+      <c r="G34" s="2">
+        <v>3.2002999999999999</v>
+      </c>
+      <c r="H34" s="2">
+        <v>2165.3000000000002</v>
+      </c>
+      <c r="I34" s="2">
+        <v>2320.3000000000002</v>
+      </c>
+      <c r="J34" s="2">
+        <v>4.1947999999999999</v>
+      </c>
+      <c r="K34" s="2">
+        <v>6.7274000000000003</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A35" s="13"/>
+      <c r="B35" s="16"/>
+      <c r="C35" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="D35" s="4">
+        <v>8.0267999999999997</v>
+      </c>
+      <c r="E35" s="4">
+        <v>28.899000000000001</v>
+      </c>
+      <c r="F35" s="4">
+        <v>2.5811000000000002</v>
+      </c>
+      <c r="G35" s="4">
+        <v>4.0179999999999998</v>
+      </c>
+      <c r="H35" s="4">
+        <v>1213.4000000000001</v>
+      </c>
+      <c r="I35" s="2">
+        <v>1698.5</v>
+      </c>
+      <c r="J35" s="2">
+        <v>4.5711000000000004</v>
+      </c>
+      <c r="K35" s="2">
+        <v>7.3220999999999998</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A36" s="13"/>
+      <c r="B36" s="16"/>
+      <c r="C36" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D36" s="4">
+        <v>8.0846</v>
+      </c>
+      <c r="E36" s="4">
+        <v>21.623000000000001</v>
+      </c>
+      <c r="F36" s="4">
+        <v>4.9984999999999999</v>
+      </c>
+      <c r="G36" s="4">
+        <v>3.8734000000000002</v>
+      </c>
+      <c r="H36" s="4">
+        <v>1330.8</v>
+      </c>
+      <c r="I36" s="4">
+        <v>2586.3000000000002</v>
+      </c>
+      <c r="J36" s="4">
+        <v>4.0925000000000002</v>
+      </c>
+      <c r="K36" s="4">
+        <v>6.8217999999999996</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="14"/>
+      <c r="B37" s="17"/>
+      <c r="C37" s="7"/>
+      <c r="L37" s="11"/>
+    </row>
+    <row r="38" spans="1:12" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="12">
+        <v>900</v>
+      </c>
+      <c r="B38" s="15" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A39" s="13"/>
+      <c r="B39" s="16"/>
+      <c r="C39" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D39" s="4">
+        <v>8.7007999999999992</v>
+      </c>
+      <c r="E39" s="4">
+        <v>379.67</v>
+      </c>
+      <c r="F39" s="4">
+        <v>0.15739</v>
+      </c>
+      <c r="G39" s="4">
+        <v>4.2165999999999997</v>
+      </c>
+      <c r="H39" s="4">
+        <v>994.53</v>
+      </c>
+      <c r="I39" s="4">
+        <v>1533.4</v>
+      </c>
+      <c r="J39" s="4">
+        <v>4.6802000000000001</v>
+      </c>
+      <c r="K39" s="4">
+        <v>7.0461</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A40" s="13"/>
+      <c r="B40" s="16"/>
+      <c r="C40" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D40" s="2">
+        <v>9.3439999999999994</v>
+      </c>
+      <c r="E40" s="2">
+        <v>45.972000000000001</v>
+      </c>
+      <c r="F40" s="2">
+        <v>2.5375000000000001</v>
+      </c>
+      <c r="G40" s="2">
+        <v>3.4094000000000002</v>
+      </c>
+      <c r="H40" s="2">
+        <v>1902</v>
+      </c>
+      <c r="I40" s="2">
+        <v>2101.5</v>
+      </c>
+      <c r="J40" s="2">
+        <v>4.3022</v>
+      </c>
+      <c r="K40" s="2">
+        <v>6.1081000000000003</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A41" s="13"/>
+      <c r="B41" s="16"/>
+      <c r="C41" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D41" s="2">
+        <v>3.0011000000000001</v>
+      </c>
+      <c r="E41" s="2">
+        <v>18.974</v>
+      </c>
+      <c r="F41" s="2">
+        <v>32.389000000000003</v>
+      </c>
+      <c r="G41" s="2">
+        <v>3.2721</v>
+      </c>
+      <c r="H41" s="2">
+        <v>2021.2</v>
+      </c>
+      <c r="I41" s="2">
+        <v>2356.1999999999998</v>
+      </c>
+      <c r="J41" s="2">
+        <v>4.4100999999999999</v>
+      </c>
+      <c r="K41" s="2">
+        <v>17.539000000000001</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A42" s="13"/>
+      <c r="B42" s="16"/>
+      <c r="C42" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="D42" s="2">
+        <v>2.1263000000000001</v>
+      </c>
+      <c r="E42" s="2">
+        <v>19.571000000000002</v>
+      </c>
+      <c r="F42" s="2">
+        <v>18.852</v>
+      </c>
+      <c r="G42" s="2">
+        <v>3.3525</v>
+      </c>
+      <c r="H42" s="2">
+        <v>1999.6</v>
+      </c>
+      <c r="I42" s="2">
+        <v>2639.8</v>
+      </c>
+      <c r="J42" s="2">
+        <v>4.3577000000000004</v>
+      </c>
+      <c r="K42" s="2">
+        <v>21.824999999999999</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A43" s="13"/>
+      <c r="B43" s="16"/>
+      <c r="C43" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D43" s="2">
+        <v>16.257000000000001</v>
+      </c>
+      <c r="E43" s="2">
+        <v>181.45</v>
+      </c>
+      <c r="F43" s="2">
+        <v>0.50260000000000005</v>
+      </c>
+      <c r="G43" s="2">
+        <v>3.0154000000000001</v>
+      </c>
+      <c r="H43" s="2">
+        <v>2606.1999999999998</v>
+      </c>
+      <c r="I43" s="2">
+        <v>2445.1</v>
+      </c>
+      <c r="J43" s="2">
+        <v>4.1307</v>
+      </c>
+      <c r="K43" s="2">
+        <v>5.6963999999999997</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A44" s="13"/>
+      <c r="B44" s="16"/>
+      <c r="C44" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="D44" s="2">
+        <v>9.5314999999999994</v>
+      </c>
+      <c r="E44" s="2">
+        <v>149.26</v>
+      </c>
+      <c r="F44" s="2">
+        <v>0.37325999999999998</v>
+      </c>
+      <c r="G44" s="2">
+        <v>3.9582000000000002</v>
+      </c>
+      <c r="H44" s="2">
+        <v>1254.5999999999999</v>
+      </c>
+      <c r="I44" s="2">
+        <v>2014.8</v>
+      </c>
+      <c r="J44" s="2">
+        <v>4.3853999999999997</v>
+      </c>
+      <c r="K44" s="2">
+        <v>8.0510999999999999</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A45" s="13"/>
+      <c r="B45" s="16"/>
+      <c r="C45" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D45" s="2">
+        <v>6.4694000000000003</v>
+      </c>
+      <c r="E45" s="2">
+        <v>149.62</v>
+      </c>
+      <c r="F45" s="2">
+        <v>0.29610999999999998</v>
+      </c>
+      <c r="G45" s="2">
+        <v>4.1942000000000004</v>
+      </c>
+      <c r="H45" s="2">
+        <v>1123.8</v>
+      </c>
+      <c r="I45" s="2">
+        <v>2045.9</v>
+      </c>
+      <c r="J45" s="2">
+        <v>4.4272</v>
+      </c>
+      <c r="K45" s="2">
+        <v>9.5322999999999993</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A46" s="13"/>
+      <c r="B46" s="16"/>
+      <c r="C46" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D46" s="2">
+        <v>12.617000000000001</v>
+      </c>
+      <c r="E46" s="2">
+        <v>119.8</v>
+      </c>
+      <c r="F46" s="2">
+        <v>0.37544</v>
+      </c>
+      <c r="G46" s="2">
+        <v>3.7416</v>
+      </c>
+      <c r="H46" s="2">
+        <v>1366.4</v>
+      </c>
+      <c r="I46" s="2">
+        <v>1894.5</v>
+      </c>
+      <c r="J46" s="2">
+        <v>4.5370999999999997</v>
+      </c>
+      <c r="K46" s="2">
+        <v>9.6135999999999999</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A47" s="13"/>
+      <c r="B47" s="16"/>
+      <c r="C47" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="D47" s="4">
+        <v>11.849</v>
+      </c>
+      <c r="E47" s="4">
+        <v>272.72000000000003</v>
+      </c>
+      <c r="F47" s="4">
+        <v>0.21346999999999999</v>
+      </c>
+      <c r="G47" s="4">
+        <v>3.8447</v>
+      </c>
+      <c r="H47" s="4">
+        <v>1238.3</v>
+      </c>
+      <c r="I47" s="4">
+        <v>1731</v>
+      </c>
+      <c r="J47" s="4">
+        <v>4.5635000000000003</v>
+      </c>
+      <c r="K47" s="4">
+        <v>7.4757999999999996</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A48" s="13"/>
+      <c r="B48" s="16"/>
+      <c r="C48" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D48" s="4">
+        <v>7.9996999999999998</v>
+      </c>
+      <c r="E48" s="4">
+        <v>25.007999999999999</v>
+      </c>
+      <c r="F48" s="4">
+        <v>2.2597</v>
+      </c>
+      <c r="G48" s="4">
+        <v>4.1269999999999998</v>
+      </c>
+      <c r="H48" s="4">
+        <v>1102.2</v>
+      </c>
+      <c r="I48" s="2">
+        <v>1841.7</v>
+      </c>
+      <c r="J48" s="2">
+        <v>4.5534999999999997</v>
+      </c>
+      <c r="K48" s="2">
+        <v>10.206</v>
       </c>
     </row>
     <row r="49" spans="1:12" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
@@ -3539,1492 +5021,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF6E341A-51E3-4AF7-809B-A8594B1323BC}">
-  <dimension ref="A1:L73"/>
-  <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F20" sqref="F20"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="9.140625" style="4"/>
-    <col min="2" max="2" width="9.140625" style="3"/>
-    <col min="3" max="3" width="15.7109375" style="8" customWidth="1"/>
-    <col min="4" max="11" width="9.140625" style="4"/>
-    <col min="12" max="12" width="9.140625" style="9"/>
-    <col min="13" max="16384" width="9.140625" style="4"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C1" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="H1" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="I1" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="11"/>
-    </row>
-    <row r="2" spans="1:12" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="12">
-        <v>800</v>
-      </c>
-      <c r="B2" s="15" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="13"/>
-      <c r="B3" s="16"/>
-      <c r="C3" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="D3" s="4">
-        <v>16.994</v>
-      </c>
-      <c r="E3" s="4">
-        <v>187.83</v>
-      </c>
-      <c r="F3" s="4">
-        <v>0.26103999999999999</v>
-      </c>
-      <c r="G3" s="4">
-        <v>4.5019999999999998</v>
-      </c>
-      <c r="H3" s="4">
-        <v>1784.8</v>
-      </c>
-      <c r="I3" s="2">
-        <v>3263.5</v>
-      </c>
-      <c r="J3" s="2">
-        <v>4.9230999999999998</v>
-      </c>
-      <c r="K3" s="2">
-        <v>13.172000000000001</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="13"/>
-      <c r="B4" s="16"/>
-      <c r="C4" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="D4" s="4">
-        <v>22.454000000000001</v>
-      </c>
-      <c r="E4" s="4">
-        <v>66.77</v>
-      </c>
-      <c r="F4" s="4">
-        <v>0.92681000000000002</v>
-      </c>
-      <c r="G4" s="4">
-        <v>4.4191000000000003</v>
-      </c>
-      <c r="H4" s="4">
-        <v>1610.1</v>
-      </c>
-      <c r="I4" s="2">
-        <v>2142</v>
-      </c>
-      <c r="J4" s="2">
-        <v>5.4843999999999999</v>
-      </c>
-      <c r="K4" s="2">
-        <v>11.449</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" s="13"/>
-      <c r="B5" s="16"/>
-      <c r="C5" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="D5" s="4">
-        <v>9.1647999999999996</v>
-      </c>
-      <c r="E5" s="4">
-        <v>36.326000000000001</v>
-      </c>
-      <c r="F5" s="4">
-        <v>12.337</v>
-      </c>
-      <c r="G5" s="4">
-        <v>4.2247000000000003</v>
-      </c>
-      <c r="H5" s="4">
-        <v>1776.1</v>
-      </c>
-      <c r="I5" s="2">
-        <v>2731</v>
-      </c>
-      <c r="J5" s="2">
-        <v>5.0411000000000001</v>
-      </c>
-      <c r="K5" s="2">
-        <v>8.3102999999999998</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="13"/>
-      <c r="B6" s="16"/>
-      <c r="C6" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="D6" s="4">
-        <v>5.8951000000000002</v>
-      </c>
-      <c r="E6" s="4">
-        <v>36.906999999999996</v>
-      </c>
-      <c r="F6" s="4">
-        <v>5.3551000000000002</v>
-      </c>
-      <c r="G6" s="4">
-        <v>4.7310999999999996</v>
-      </c>
-      <c r="H6" s="4">
-        <v>1557.8</v>
-      </c>
-      <c r="I6" s="2">
-        <v>2224.1</v>
-      </c>
-      <c r="J6" s="2">
-        <v>5.2808999999999999</v>
-      </c>
-      <c r="K6" s="2">
-        <v>6.5113000000000003</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="13"/>
-      <c r="B7" s="16"/>
-      <c r="C7" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="D7" s="4">
-        <v>4.1860999999999997</v>
-      </c>
-      <c r="E7" s="4">
-        <v>84.548000000000002</v>
-      </c>
-      <c r="F7" s="4">
-        <v>2.1124999999999998</v>
-      </c>
-      <c r="G7" s="4">
-        <v>4.7670000000000003</v>
-      </c>
-      <c r="H7" s="4">
-        <v>1574.1</v>
-      </c>
-      <c r="I7" s="4">
-        <v>2883.2</v>
-      </c>
-      <c r="J7" s="4">
-        <v>4.8395000000000001</v>
-      </c>
-      <c r="K7" s="4">
-        <v>4.5430999999999999</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" s="13"/>
-      <c r="B8" s="16"/>
-      <c r="C8" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="D8" s="2">
-        <v>27.867999999999999</v>
-      </c>
-      <c r="E8" s="2">
-        <v>89.338999999999999</v>
-      </c>
-      <c r="F8" s="2">
-        <v>0.59711999999999998</v>
-      </c>
-      <c r="G8" s="2">
-        <v>4.1981999999999999</v>
-      </c>
-      <c r="H8" s="2">
-        <v>1818</v>
-      </c>
-      <c r="I8" s="2">
-        <v>2645.2</v>
-      </c>
-      <c r="J8" s="2">
-        <v>5.1192000000000002</v>
-      </c>
-      <c r="K8" s="2">
-        <v>10.125</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" s="13"/>
-      <c r="B9" s="16"/>
-      <c r="C9" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="D9" s="2">
-        <v>28.599</v>
-      </c>
-      <c r="E9" s="2">
-        <v>78.057000000000002</v>
-      </c>
-      <c r="F9" s="2">
-        <v>0.84292</v>
-      </c>
-      <c r="G9" s="2">
-        <v>3.8371</v>
-      </c>
-      <c r="H9" s="2">
-        <v>2441.5</v>
-      </c>
-      <c r="I9" s="2">
-        <v>2969.6</v>
-      </c>
-      <c r="J9" s="2">
-        <v>4.9976000000000003</v>
-      </c>
-      <c r="K9" s="2">
-        <v>10.641999999999999</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" s="13"/>
-      <c r="B10" s="16"/>
-      <c r="C10" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="D10" s="2">
-        <v>29.978999999999999</v>
-      </c>
-      <c r="E10" s="2">
-        <v>119.58</v>
-      </c>
-      <c r="F10" s="2">
-        <v>0.55200000000000005</v>
-      </c>
-      <c r="G10" s="2">
-        <v>3.8504999999999998</v>
-      </c>
-      <c r="H10" s="2">
-        <v>2314.4</v>
-      </c>
-      <c r="I10" s="2">
-        <v>2808.8</v>
-      </c>
-      <c r="J10" s="2">
-        <v>5.0354000000000001</v>
-      </c>
-      <c r="K10" s="2">
-        <v>9.5434999999999999</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" s="13"/>
-      <c r="B11" s="16"/>
-      <c r="C11" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="D11" s="4">
-        <v>19.125</v>
-      </c>
-      <c r="E11" s="4">
-        <v>43.640999999999998</v>
-      </c>
-      <c r="F11" s="4">
-        <v>5.6147999999999998</v>
-      </c>
-      <c r="G11" s="4">
-        <v>4.1688000000000001</v>
-      </c>
-      <c r="H11" s="4">
-        <v>1616</v>
-      </c>
-      <c r="I11" s="4">
-        <v>1876.8</v>
-      </c>
-      <c r="J11" s="4">
-        <v>5.5594000000000001</v>
-      </c>
-      <c r="K11" s="4">
-        <v>6.8653000000000004</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" s="13"/>
-      <c r="B12" s="16"/>
-      <c r="C12" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="D12" s="4">
-        <v>22.012</v>
-      </c>
-      <c r="E12" s="4">
-        <v>38.872999999999998</v>
-      </c>
-      <c r="F12" s="4">
-        <v>2.2033</v>
-      </c>
-      <c r="G12" s="4">
-        <v>4.2450000000000001</v>
-      </c>
-      <c r="H12" s="4">
-        <v>1841.2</v>
-      </c>
-      <c r="I12" s="2">
-        <v>2377</v>
-      </c>
-      <c r="J12" s="2">
-        <v>5.2897999999999996</v>
-      </c>
-      <c r="K12" s="2">
-        <v>9.7712000000000003</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="14"/>
-      <c r="B13" s="17"/>
-      <c r="C13" s="7"/>
-      <c r="L13" s="11"/>
-    </row>
-    <row r="14" spans="1:12" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="12">
-        <v>800</v>
-      </c>
-      <c r="B14" s="15" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A15" s="13"/>
-      <c r="B15" s="16"/>
-      <c r="C15" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="D15" s="4">
-        <v>31.646999999999998</v>
-      </c>
-      <c r="E15" s="4">
-        <v>120.62</v>
-      </c>
-      <c r="F15" s="4">
-        <v>0.85485</v>
-      </c>
-      <c r="G15" s="4">
-        <v>3.7265999999999999</v>
-      </c>
-      <c r="H15" s="4">
-        <v>2297.8000000000002</v>
-      </c>
-      <c r="I15" s="4">
-        <v>2165.6999999999998</v>
-      </c>
-      <c r="J15" s="4">
-        <v>5.3247</v>
-      </c>
-      <c r="K15" s="4">
-        <v>7.7724000000000002</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A16" s="13"/>
-      <c r="B16" s="16"/>
-      <c r="C16" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="D16" s="2">
-        <v>33.296999999999997</v>
-      </c>
-      <c r="E16" s="2">
-        <v>522.85</v>
-      </c>
-      <c r="F16" s="2">
-        <v>0.11871</v>
-      </c>
-      <c r="G16" s="2">
-        <v>3.9767000000000001</v>
-      </c>
-      <c r="H16" s="2">
-        <v>1762.4</v>
-      </c>
-      <c r="I16" s="2">
-        <v>1913.8</v>
-      </c>
-      <c r="J16" s="2">
-        <v>5.6638000000000002</v>
-      </c>
-      <c r="K16" s="2">
-        <v>11.287000000000001</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A17" s="13"/>
-      <c r="B17" s="16"/>
-      <c r="C17" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="D17" s="2">
-        <v>10.788</v>
-      </c>
-      <c r="E17" s="2">
-        <v>53.85</v>
-      </c>
-      <c r="F17" s="2">
-        <v>7.1745999999999999</v>
-      </c>
-      <c r="G17" s="2">
-        <v>3.8603999999999998</v>
-      </c>
-      <c r="H17" s="2">
-        <v>2196.3000000000002</v>
-      </c>
-      <c r="I17" s="2">
-        <v>3182.9</v>
-      </c>
-      <c r="J17" s="2">
-        <v>4.6458000000000004</v>
-      </c>
-      <c r="K17" s="2">
-        <v>3.7222</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A18" s="13"/>
-      <c r="B18" s="16"/>
-      <c r="C18" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="D18" s="2">
-        <v>38.180999999999997</v>
-      </c>
-      <c r="E18" s="2">
-        <v>51.055</v>
-      </c>
-      <c r="F18" s="2">
-        <v>2.4819</v>
-      </c>
-      <c r="G18" s="2">
-        <v>3.2572000000000001</v>
-      </c>
-      <c r="H18" s="2">
-        <v>3154.4</v>
-      </c>
-      <c r="I18" s="2">
-        <v>2725.2</v>
-      </c>
-      <c r="J18" s="2">
-        <v>5.0167000000000002</v>
-      </c>
-      <c r="K18" s="2">
-        <v>8.33</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A19" s="13"/>
-      <c r="B19" s="16"/>
-      <c r="C19" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="D19" s="4">
-        <v>24.888999999999999</v>
-      </c>
-      <c r="E19" s="4">
-        <v>44.932000000000002</v>
-      </c>
-      <c r="F19" s="4">
-        <v>1.2076</v>
-      </c>
-      <c r="G19" s="4">
-        <v>4.5054999999999996</v>
-      </c>
-      <c r="H19" s="4">
-        <v>1527.9</v>
-      </c>
-      <c r="I19" s="4">
-        <v>2589.6999999999998</v>
-      </c>
-      <c r="J19" s="4">
-        <v>5.1066000000000003</v>
-      </c>
-      <c r="K19" s="4">
-        <v>8.6950000000000003</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A20" s="13"/>
-      <c r="B20" s="16"/>
-      <c r="C20" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="D20" s="2">
-        <v>23.303999999999998</v>
-      </c>
-      <c r="E20" s="2">
-        <v>276.66000000000003</v>
-      </c>
-      <c r="F20" s="2">
-        <v>0.32123000000000002</v>
-      </c>
-      <c r="G20" s="2">
-        <v>4.2591999999999999</v>
-      </c>
-      <c r="H20" s="2">
-        <v>1767.2</v>
-      </c>
-      <c r="I20" s="2">
-        <v>2168.5</v>
-      </c>
-      <c r="J20" s="2">
-        <v>5.3181000000000003</v>
-      </c>
-      <c r="K20" s="2">
-        <v>6.7618999999999998</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A21" s="13"/>
-      <c r="B21" s="16"/>
-      <c r="C21" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="D21" s="2">
-        <v>30.401</v>
-      </c>
-      <c r="E21" s="2">
-        <v>34.817</v>
-      </c>
-      <c r="F21" s="2">
-        <v>4.5983000000000001</v>
-      </c>
-      <c r="G21" s="2">
-        <v>3.5323000000000002</v>
-      </c>
-      <c r="H21" s="2">
-        <v>2583</v>
-      </c>
-      <c r="I21" s="2">
-        <v>2520.9</v>
-      </c>
-      <c r="J21" s="2">
-        <v>5.1558999999999999</v>
-      </c>
-      <c r="K21" s="2">
-        <v>8.5891000000000002</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A22" s="13"/>
-      <c r="B22" s="16"/>
-      <c r="C22" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="D22" s="4">
-        <v>5.0568999999999997</v>
-      </c>
-      <c r="E22" s="4">
-        <v>40.475999999999999</v>
-      </c>
-      <c r="F22" s="4">
-        <v>10.016999999999999</v>
-      </c>
-      <c r="G22" s="4">
-        <v>4.1585000000000001</v>
-      </c>
-      <c r="H22" s="4">
-        <v>1730.1</v>
-      </c>
-      <c r="I22" s="4">
-        <v>1998.1</v>
-      </c>
-      <c r="J22" s="4">
-        <v>5.5564</v>
-      </c>
-      <c r="K22" s="4">
-        <v>10.337</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A23" s="13"/>
-      <c r="B23" s="16"/>
-      <c r="C23" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="D23" s="2">
-        <v>31.809000000000001</v>
-      </c>
-      <c r="E23" s="2">
-        <v>43.194000000000003</v>
-      </c>
-      <c r="F23" s="2">
-        <v>2.2399</v>
-      </c>
-      <c r="G23" s="2">
-        <v>3.9613</v>
-      </c>
-      <c r="H23" s="2">
-        <v>1820.1</v>
-      </c>
-      <c r="I23" s="2">
-        <v>2245.4</v>
-      </c>
-      <c r="J23" s="2">
-        <v>5.3178999999999998</v>
-      </c>
-      <c r="K23" s="2">
-        <v>8.5096000000000007</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A24" s="13"/>
-      <c r="B24" s="16"/>
-      <c r="C24" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="D24" s="4">
-        <v>0.36498999999999998</v>
-      </c>
-      <c r="E24" s="4">
-        <v>45.374000000000002</v>
-      </c>
-      <c r="F24" s="4">
-        <v>15.686999999999999</v>
-      </c>
-      <c r="G24" s="4">
-        <v>3.6105</v>
-      </c>
-      <c r="H24" s="4">
-        <v>2878.3</v>
-      </c>
-      <c r="I24" s="2">
-        <v>3325.8</v>
-      </c>
-      <c r="J24" s="2">
-        <v>4.8470000000000004</v>
-      </c>
-      <c r="K24" s="2">
-        <v>12.327999999999999</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="14"/>
-      <c r="B25" s="17"/>
-      <c r="C25" s="7"/>
-      <c r="L25" s="11"/>
-    </row>
-    <row r="26" spans="1:12" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="12">
-        <v>900</v>
-      </c>
-      <c r="B26" s="15" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A27" s="13"/>
-      <c r="B27" s="16"/>
-      <c r="C27" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="D27" s="2">
-        <v>3.6261999999999999</v>
-      </c>
-      <c r="E27" s="2">
-        <v>13.804</v>
-      </c>
-      <c r="F27" s="2">
-        <v>6.9824999999999999</v>
-      </c>
-      <c r="G27" s="2">
-        <v>4.2416</v>
-      </c>
-      <c r="H27" s="2">
-        <v>1138.2</v>
-      </c>
-      <c r="I27" s="2">
-        <v>1986</v>
-      </c>
-      <c r="J27" s="2">
-        <v>4.4408000000000003</v>
-      </c>
-      <c r="K27" s="2">
-        <v>9.1929999999999996</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A28" s="13"/>
-      <c r="B28" s="16"/>
-      <c r="C28" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="D28" s="2">
-        <v>10.683</v>
-      </c>
-      <c r="E28" s="2">
-        <v>31.381</v>
-      </c>
-      <c r="F28" s="2">
-        <v>2.9727000000000001</v>
-      </c>
-      <c r="G28" s="2">
-        <v>3.7155</v>
-      </c>
-      <c r="H28" s="2">
-        <v>1422</v>
-      </c>
-      <c r="I28" s="2">
-        <v>1626.7</v>
-      </c>
-      <c r="J28" s="2">
-        <v>4.5519999999999996</v>
-      </c>
-      <c r="K28" s="2">
-        <v>6.2319000000000004</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A29" s="13"/>
-      <c r="B29" s="16"/>
-      <c r="C29" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="D29" s="2">
-        <v>10.340999999999999</v>
-      </c>
-      <c r="E29" s="2">
-        <v>24.475999999999999</v>
-      </c>
-      <c r="F29" s="2">
-        <v>2.3226</v>
-      </c>
-      <c r="G29" s="2">
-        <v>3.9651000000000001</v>
-      </c>
-      <c r="H29" s="2">
-        <v>1176.4000000000001</v>
-      </c>
-      <c r="I29" s="2">
-        <v>1743</v>
-      </c>
-      <c r="J29" s="2">
-        <v>4.5865</v>
-      </c>
-      <c r="K29" s="2">
-        <v>9.1586999999999996</v>
-      </c>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A30" s="13"/>
-      <c r="B30" s="16"/>
-      <c r="C30" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="D30" s="2">
-        <v>11.112</v>
-      </c>
-      <c r="E30" s="2">
-        <v>18.959</v>
-      </c>
-      <c r="F30" s="2">
-        <v>5.9504999999999999</v>
-      </c>
-      <c r="G30" s="2">
-        <v>3.6368</v>
-      </c>
-      <c r="H30" s="2">
-        <v>1471.6</v>
-      </c>
-      <c r="I30" s="2">
-        <v>2064.3000000000002</v>
-      </c>
-      <c r="J30" s="2">
-        <v>4.3163999999999998</v>
-      </c>
-      <c r="K30" s="2">
-        <v>7.2249999999999996</v>
-      </c>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A31" s="13"/>
-      <c r="B31" s="16"/>
-      <c r="C31" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="D31" s="2">
-        <v>8.0817999999999994</v>
-      </c>
-      <c r="E31" s="2">
-        <v>9.2744</v>
-      </c>
-      <c r="F31" s="2">
-        <v>7.9561999999999999</v>
-      </c>
-      <c r="G31" s="2">
-        <v>3.9839000000000002</v>
-      </c>
-      <c r="H31" s="2">
-        <v>1310.7</v>
-      </c>
-      <c r="I31" s="2">
-        <v>4972.3999999999996</v>
-      </c>
-      <c r="J31" s="2">
-        <v>3.6442999999999999</v>
-      </c>
-      <c r="K31" s="2">
-        <v>9.6707000000000001</v>
-      </c>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A32" s="13"/>
-      <c r="B32" s="16"/>
-      <c r="C32" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="D32" s="2">
-        <v>11.394</v>
-      </c>
-      <c r="E32" s="2">
-        <v>13.887</v>
-      </c>
-      <c r="F32" s="2">
-        <v>7.532</v>
-      </c>
-      <c r="G32" s="2">
-        <v>3.5691000000000002</v>
-      </c>
-      <c r="H32" s="2">
-        <v>1581.2</v>
-      </c>
-      <c r="I32" s="2">
-        <v>1959.8</v>
-      </c>
-      <c r="J32" s="2">
-        <v>4.4120999999999997</v>
-      </c>
-      <c r="K32" s="2">
-        <v>8.5846999999999998</v>
-      </c>
-    </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A33" s="13"/>
-      <c r="B33" s="16"/>
-      <c r="C33" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="D33" s="4">
-        <v>5.6656000000000004</v>
-      </c>
-      <c r="E33" s="4">
-        <v>7.6356999999999999</v>
-      </c>
-      <c r="F33" s="4">
-        <v>9.1336999999999993</v>
-      </c>
-      <c r="G33" s="4">
-        <v>4.3000999999999996</v>
-      </c>
-      <c r="H33" s="4">
-        <v>1055.4000000000001</v>
-      </c>
-      <c r="I33" s="4">
-        <v>3494.5</v>
-      </c>
-      <c r="J33" s="4">
-        <v>3.9628999999999999</v>
-      </c>
-      <c r="K33" s="4">
-        <v>11.622999999999999</v>
-      </c>
-    </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A34" s="13"/>
-      <c r="B34" s="16"/>
-      <c r="C34" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="D34" s="2">
-        <v>15.177</v>
-      </c>
-      <c r="E34" s="2">
-        <v>64.875</v>
-      </c>
-      <c r="F34" s="2">
-        <v>1.1737</v>
-      </c>
-      <c r="G34" s="2">
-        <v>3.2002999999999999</v>
-      </c>
-      <c r="H34" s="2">
-        <v>2165.3000000000002</v>
-      </c>
-      <c r="I34" s="2">
-        <v>2320.3000000000002</v>
-      </c>
-      <c r="J34" s="2">
-        <v>4.1947999999999999</v>
-      </c>
-      <c r="K34" s="2">
-        <v>6.7274000000000003</v>
-      </c>
-    </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A35" s="13"/>
-      <c r="B35" s="16"/>
-      <c r="C35" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="D35" s="4">
-        <v>8.0267999999999997</v>
-      </c>
-      <c r="E35" s="4">
-        <v>28.899000000000001</v>
-      </c>
-      <c r="F35" s="4">
-        <v>2.5811000000000002</v>
-      </c>
-      <c r="G35" s="4">
-        <v>4.0179999999999998</v>
-      </c>
-      <c r="H35" s="4">
-        <v>1213.4000000000001</v>
-      </c>
-      <c r="I35" s="2">
-        <v>1698.5</v>
-      </c>
-      <c r="J35" s="2">
-        <v>4.5711000000000004</v>
-      </c>
-      <c r="K35" s="2">
-        <v>7.3220999999999998</v>
-      </c>
-    </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A36" s="13"/>
-      <c r="B36" s="16"/>
-      <c r="C36" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="D36" s="4">
-        <v>8.0846</v>
-      </c>
-      <c r="E36" s="4">
-        <v>21.623000000000001</v>
-      </c>
-      <c r="F36" s="4">
-        <v>4.9984999999999999</v>
-      </c>
-      <c r="G36" s="4">
-        <v>3.8734000000000002</v>
-      </c>
-      <c r="H36" s="4">
-        <v>1330.8</v>
-      </c>
-      <c r="I36" s="4">
-        <v>2586.3000000000002</v>
-      </c>
-      <c r="J36" s="4">
-        <v>4.0925000000000002</v>
-      </c>
-      <c r="K36" s="4">
-        <v>6.8217999999999996</v>
-      </c>
-    </row>
-    <row r="37" spans="1:12" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="14"/>
-      <c r="B37" s="17"/>
-      <c r="C37" s="7"/>
-      <c r="L37" s="11"/>
-    </row>
-    <row r="38" spans="1:12" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="12">
-        <v>900</v>
-      </c>
-      <c r="B38" s="15" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A39" s="13"/>
-      <c r="B39" s="16"/>
-      <c r="C39" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="D39" s="4">
-        <v>8.7007999999999992</v>
-      </c>
-      <c r="E39" s="4">
-        <v>379.67</v>
-      </c>
-      <c r="F39" s="4">
-        <v>0.15739</v>
-      </c>
-      <c r="G39" s="4">
-        <v>4.2165999999999997</v>
-      </c>
-      <c r="H39" s="4">
-        <v>994.53</v>
-      </c>
-      <c r="I39" s="4">
-        <v>1533.4</v>
-      </c>
-      <c r="J39" s="4">
-        <v>4.6802000000000001</v>
-      </c>
-      <c r="K39" s="4">
-        <v>7.0461</v>
-      </c>
-    </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A40" s="13"/>
-      <c r="B40" s="16"/>
-      <c r="C40" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="D40" s="2">
-        <v>9.3439999999999994</v>
-      </c>
-      <c r="E40" s="2">
-        <v>45.972000000000001</v>
-      </c>
-      <c r="F40" s="2">
-        <v>2.5375000000000001</v>
-      </c>
-      <c r="G40" s="2">
-        <v>3.4094000000000002</v>
-      </c>
-      <c r="H40" s="2">
-        <v>1902</v>
-      </c>
-      <c r="I40" s="2">
-        <v>2101.5</v>
-      </c>
-      <c r="J40" s="2">
-        <v>4.3022</v>
-      </c>
-      <c r="K40" s="2">
-        <v>6.1081000000000003</v>
-      </c>
-    </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A41" s="13"/>
-      <c r="B41" s="16"/>
-      <c r="C41" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="D41" s="2">
-        <v>3.0011000000000001</v>
-      </c>
-      <c r="E41" s="2">
-        <v>18.974</v>
-      </c>
-      <c r="F41" s="2">
-        <v>32.389000000000003</v>
-      </c>
-      <c r="G41" s="2">
-        <v>3.2721</v>
-      </c>
-      <c r="H41" s="2">
-        <v>2021.2</v>
-      </c>
-      <c r="I41" s="2">
-        <v>2356.1999999999998</v>
-      </c>
-      <c r="J41" s="2">
-        <v>4.4100999999999999</v>
-      </c>
-      <c r="K41" s="2">
-        <v>17.539000000000001</v>
-      </c>
-    </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A42" s="13"/>
-      <c r="B42" s="16"/>
-      <c r="C42" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="D42" s="2">
-        <v>2.1263000000000001</v>
-      </c>
-      <c r="E42" s="2">
-        <v>19.571000000000002</v>
-      </c>
-      <c r="F42" s="2">
-        <v>18.852</v>
-      </c>
-      <c r="G42" s="2">
-        <v>3.3525</v>
-      </c>
-      <c r="H42" s="2">
-        <v>1999.6</v>
-      </c>
-      <c r="I42" s="2">
-        <v>2639.8</v>
-      </c>
-      <c r="J42" s="2">
-        <v>4.3577000000000004</v>
-      </c>
-      <c r="K42" s="2">
-        <v>21.824999999999999</v>
-      </c>
-    </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A43" s="13"/>
-      <c r="B43" s="16"/>
-      <c r="C43" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="D43" s="2">
-        <v>16.257000000000001</v>
-      </c>
-      <c r="E43" s="2">
-        <v>181.45</v>
-      </c>
-      <c r="F43" s="2">
-        <v>0.50260000000000005</v>
-      </c>
-      <c r="G43" s="2">
-        <v>3.0154000000000001</v>
-      </c>
-      <c r="H43" s="2">
-        <v>2606.1999999999998</v>
-      </c>
-      <c r="I43" s="2">
-        <v>2445.1</v>
-      </c>
-      <c r="J43" s="2">
-        <v>4.1307</v>
-      </c>
-      <c r="K43" s="2">
-        <v>5.6963999999999997</v>
-      </c>
-    </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A44" s="13"/>
-      <c r="B44" s="16"/>
-      <c r="C44" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="D44" s="2">
-        <v>9.5314999999999994</v>
-      </c>
-      <c r="E44" s="2">
-        <v>149.26</v>
-      </c>
-      <c r="F44" s="2">
-        <v>0.37325999999999998</v>
-      </c>
-      <c r="G44" s="2">
-        <v>3.9582000000000002</v>
-      </c>
-      <c r="H44" s="2">
-        <v>1254.5999999999999</v>
-      </c>
-      <c r="I44" s="2">
-        <v>2014.8</v>
-      </c>
-      <c r="J44" s="2">
-        <v>4.3853999999999997</v>
-      </c>
-      <c r="K44" s="2">
-        <v>8.0510999999999999</v>
-      </c>
-    </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A45" s="13"/>
-      <c r="B45" s="16"/>
-      <c r="C45" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="D45" s="2">
-        <v>6.4694000000000003</v>
-      </c>
-      <c r="E45" s="2">
-        <v>149.62</v>
-      </c>
-      <c r="F45" s="2">
-        <v>0.29610999999999998</v>
-      </c>
-      <c r="G45" s="2">
-        <v>4.1942000000000004</v>
-      </c>
-      <c r="H45" s="2">
-        <v>1123.8</v>
-      </c>
-      <c r="I45" s="2">
-        <v>2045.9</v>
-      </c>
-      <c r="J45" s="2">
-        <v>4.4272</v>
-      </c>
-      <c r="K45" s="2">
-        <v>9.5322999999999993</v>
-      </c>
-    </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A46" s="13"/>
-      <c r="B46" s="16"/>
-      <c r="C46" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="D46" s="2">
-        <v>12.617000000000001</v>
-      </c>
-      <c r="E46" s="2">
-        <v>119.8</v>
-      </c>
-      <c r="F46" s="2">
-        <v>0.37544</v>
-      </c>
-      <c r="G46" s="2">
-        <v>3.7416</v>
-      </c>
-      <c r="H46" s="2">
-        <v>1366.4</v>
-      </c>
-      <c r="I46" s="2">
-        <v>1894.5</v>
-      </c>
-      <c r="J46" s="2">
-        <v>4.5370999999999997</v>
-      </c>
-      <c r="K46" s="2">
-        <v>9.6135999999999999</v>
-      </c>
-    </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A47" s="13"/>
-      <c r="B47" s="16"/>
-      <c r="C47" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="D47" s="4">
-        <v>11.849</v>
-      </c>
-      <c r="E47" s="4">
-        <v>272.72000000000003</v>
-      </c>
-      <c r="F47" s="4">
-        <v>0.21346999999999999</v>
-      </c>
-      <c r="G47" s="4">
-        <v>3.8447</v>
-      </c>
-      <c r="H47" s="4">
-        <v>1238.3</v>
-      </c>
-      <c r="I47" s="4">
-        <v>1731</v>
-      </c>
-      <c r="J47" s="4">
-        <v>4.5635000000000003</v>
-      </c>
-      <c r="K47" s="4">
-        <v>7.4757999999999996</v>
-      </c>
-    </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A48" s="13"/>
-      <c r="B48" s="16"/>
-      <c r="C48" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="D48" s="4">
-        <v>7.9996999999999998</v>
-      </c>
-      <c r="E48" s="4">
-        <v>25.007999999999999</v>
-      </c>
-      <c r="F48" s="4">
-        <v>2.2597</v>
-      </c>
-      <c r="G48" s="4">
-        <v>4.1269999999999998</v>
-      </c>
-      <c r="H48" s="4">
-        <v>1102.2</v>
-      </c>
-      <c r="I48" s="2">
-        <v>1841.7</v>
-      </c>
-      <c r="J48" s="2">
-        <v>4.5534999999999997</v>
-      </c>
-      <c r="K48" s="2">
-        <v>10.206</v>
-      </c>
-    </row>
-    <row r="49" spans="1:12" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="14"/>
-      <c r="B49" s="17"/>
-      <c r="C49" s="7"/>
-      <c r="L49" s="11"/>
-    </row>
-    <row r="50" spans="1:12" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="12">
-        <v>1000</v>
-      </c>
-      <c r="B50" s="15" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A51" s="13"/>
-      <c r="B51" s="16"/>
-    </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A52" s="13"/>
-      <c r="B52" s="16"/>
-    </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A53" s="13"/>
-      <c r="B53" s="16"/>
-    </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A54" s="13"/>
-      <c r="B54" s="16"/>
-    </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A55" s="13"/>
-      <c r="B55" s="16"/>
-    </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A56" s="13"/>
-      <c r="B56" s="16"/>
-    </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A57" s="13"/>
-      <c r="B57" s="16"/>
-    </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A58" s="13"/>
-      <c r="B58" s="16"/>
-    </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A59" s="13"/>
-      <c r="B59" s="16"/>
-    </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A60" s="13"/>
-      <c r="B60" s="16"/>
-    </row>
-    <row r="61" spans="1:12" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="14"/>
-      <c r="B61" s="17"/>
-      <c r="C61" s="7"/>
-      <c r="L61" s="11"/>
-    </row>
-    <row r="62" spans="1:12" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="12">
-        <v>1000</v>
-      </c>
-      <c r="B62" s="15" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A63" s="13"/>
-      <c r="B63" s="16"/>
-    </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A64" s="13"/>
-      <c r="B64" s="16"/>
-    </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A65" s="13"/>
-      <c r="B65" s="16"/>
-    </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A66" s="13"/>
-      <c r="B66" s="16"/>
-    </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A67" s="13"/>
-      <c r="B67" s="16"/>
-    </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A68" s="13"/>
-      <c r="B68" s="16"/>
-    </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A69" s="13"/>
-      <c r="B69" s="16"/>
-    </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A70" s="13"/>
-      <c r="B70" s="16"/>
-    </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A71" s="13"/>
-      <c r="B71" s="16"/>
-    </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A72" s="13"/>
-      <c r="B72" s="16"/>
-    </row>
-    <row r="73" spans="1:12" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="14"/>
-      <c r="B73" s="17"/>
-      <c r="C73" s="7"/>
-      <c r="L73" s="11"/>
-    </row>
-  </sheetData>
-  <mergeCells count="12">
-    <mergeCell ref="A38:A49"/>
-    <mergeCell ref="B38:B49"/>
-    <mergeCell ref="A50:A61"/>
-    <mergeCell ref="B50:B61"/>
-    <mergeCell ref="A62:A73"/>
-    <mergeCell ref="B62:B73"/>
-    <mergeCell ref="A2:A13"/>
-    <mergeCell ref="B2:B13"/>
-    <mergeCell ref="A14:A25"/>
-    <mergeCell ref="B14:B25"/>
-    <mergeCell ref="A26:A37"/>
-    <mergeCell ref="B26:B37"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C18A26E-30CA-4E63-A18A-C9C101DAF33C}">
   <dimension ref="A1:O73"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M12" sqref="M12"/>
+      <selection pane="bottomLeft" activeCell="N27" sqref="D27:N27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5095,7 +5098,7 @@
       <c r="A3" s="13"/>
       <c r="B3" s="16"/>
       <c r="C3" s="8" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="D3" s="4">
         <v>17.216999999999999</v>
@@ -5113,22 +5116,22 @@
         <v>1783.5</v>
       </c>
       <c r="I3" s="2">
-        <v>1.4998</v>
+        <v>1.6216999999999999</v>
       </c>
       <c r="J3" s="2">
-        <v>0.64100999999999997</v>
+        <v>0.29459999999999997</v>
       </c>
       <c r="K3" s="2">
-        <v>5.4347000000000003</v>
+        <v>3.3557999999999999</v>
       </c>
       <c r="L3" s="2">
-        <v>1.7194</v>
+        <v>1.0135000000000001</v>
       </c>
       <c r="M3" s="2">
-        <v>0.30907000000000001</v>
+        <v>0.34161999999999998</v>
       </c>
       <c r="N3" s="1">
-        <v>3.3214999999999999</v>
+        <v>3.4578000000000002</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
@@ -5360,22 +5363,22 @@
         <v>2575.8000000000002</v>
       </c>
       <c r="I15" s="4">
-        <v>1.6236999999999999</v>
+        <v>1.0368999999999999</v>
       </c>
       <c r="J15" s="4">
-        <v>0.39095000000000002</v>
+        <v>0.33298</v>
       </c>
       <c r="K15" s="4">
-        <v>3.8603999999999998</v>
+        <v>3.661</v>
       </c>
       <c r="L15" s="4">
-        <v>3.4752999999999998</v>
+        <v>1.9359999999999999</v>
       </c>
       <c r="M15" s="4">
-        <v>0.11533</v>
+        <v>0.26541999999999999</v>
       </c>
       <c r="N15" s="3">
-        <v>2.5640000000000001</v>
+        <v>3.1442999999999999</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
@@ -6225,18 +6228,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A38:A49"/>
+    <mergeCell ref="B38:B49"/>
+    <mergeCell ref="A50:A61"/>
+    <mergeCell ref="B50:B61"/>
+    <mergeCell ref="A62:A73"/>
+    <mergeCell ref="B62:B73"/>
     <mergeCell ref="A2:A13"/>
     <mergeCell ref="B2:B13"/>
     <mergeCell ref="A14:A25"/>
     <mergeCell ref="B14:B25"/>
     <mergeCell ref="A26:A37"/>
     <mergeCell ref="B26:B37"/>
-    <mergeCell ref="A38:A49"/>
-    <mergeCell ref="B38:B49"/>
-    <mergeCell ref="A50:A61"/>
-    <mergeCell ref="B50:B61"/>
-    <mergeCell ref="A62:A73"/>
-    <mergeCell ref="B62:B73"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -6652,18 +6655,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A2:A13"/>
+    <mergeCell ref="B2:B13"/>
+    <mergeCell ref="A14:A25"/>
+    <mergeCell ref="B14:B25"/>
+    <mergeCell ref="A26:A37"/>
+    <mergeCell ref="B26:B37"/>
     <mergeCell ref="A38:A49"/>
     <mergeCell ref="B38:B49"/>
     <mergeCell ref="A50:A61"/>
     <mergeCell ref="B50:B61"/>
     <mergeCell ref="A62:A73"/>
     <mergeCell ref="B62:B73"/>
-    <mergeCell ref="A2:A13"/>
-    <mergeCell ref="B2:B13"/>
-    <mergeCell ref="A14:A25"/>
-    <mergeCell ref="B14:B25"/>
-    <mergeCell ref="A26:A37"/>
-    <mergeCell ref="B26:B37"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
Changes to recorder and changed params for evpwd
</commit_message>
<xml_diff>
--- a/scripts/__other__/__sem__.xlsx
+++ b/scripts/__other__/__sem__.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Janzen\Desktop\code\moga_neml\scripts\__other__\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D045F33-5097-403A-B3C8-92DE9E7EF2E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A79FADF-661B-4B20-9BE0-3AB555056CCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="15600" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="evp" sheetId="13" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="47">
   <si>
     <t>temp</t>
   </si>
@@ -178,6 +178,9 @@
   </si>
   <si>
     <t>6; 8</t>
+  </si>
+  <si>
+    <t>6; 7</t>
   </si>
 </sst>
 </file>
@@ -2069,7 +2072,7 @@
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D3" sqref="D3:K12"/>
+      <selection pane="bottomLeft" activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2516,7 +2519,7 @@
       <c r="A17" s="13"/>
       <c r="B17" s="16"/>
       <c r="C17" s="8" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D17" s="4">
         <v>11.45</v>
@@ -2534,13 +2537,13 @@
         <v>2221.6</v>
       </c>
       <c r="I17" s="2">
-        <v>3182.9</v>
+        <v>4188.8999999999996</v>
       </c>
       <c r="J17" s="2">
-        <v>4.6406999999999998</v>
+        <v>4.3604000000000003</v>
       </c>
       <c r="K17" s="2">
-        <v>3.7244999999999999</v>
+        <v>4.7172000000000001</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
@@ -3546,8 +3549,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF6E341A-51E3-4AF7-809B-A8594B1323BC}">
   <dimension ref="A1:L73"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
@@ -5025,9 +5028,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C18A26E-30CA-4E63-A18A-C9C101DAF33C}">
   <dimension ref="A1:O73"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N27" sqref="D27:N27"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C42" sqref="C42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5098,7 +5101,7 @@
       <c r="A3" s="13"/>
       <c r="B3" s="16"/>
       <c r="C3" s="8" t="s">
-        <v>29</v>
+        <v>46</v>
       </c>
       <c r="D3" s="4">
         <v>17.216999999999999</v>
@@ -5155,28 +5158,31 @@
       <c r="H4" s="4">
         <v>1621.6</v>
       </c>
-      <c r="I4" s="4">
-        <v>2.5101</v>
-      </c>
-      <c r="J4" s="4">
-        <v>0.51356000000000002</v>
-      </c>
-      <c r="K4" s="4">
-        <v>4.2454000000000001</v>
-      </c>
-      <c r="L4" s="4">
-        <v>1.9213</v>
-      </c>
-      <c r="M4" s="4">
-        <v>1.5276E-2</v>
-      </c>
-      <c r="N4" s="3">
-        <v>2.6046</v>
+      <c r="I4" s="2">
+        <v>1.8904000000000001</v>
+      </c>
+      <c r="J4" s="2">
+        <v>0.54329000000000005</v>
+      </c>
+      <c r="K4" s="2">
+        <v>4.6087999999999996</v>
+      </c>
+      <c r="L4" s="2">
+        <v>1.8685</v>
+      </c>
+      <c r="M4" s="2">
+        <v>9.3698000000000004E-2</v>
+      </c>
+      <c r="N4" s="2">
+        <v>2.7471999999999999</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="13"/>
       <c r="B5" s="16"/>
+      <c r="C5" s="8" t="s">
+        <v>46</v>
+      </c>
       <c r="D5" s="4">
         <v>9.3076000000000008</v>
       </c>
@@ -5191,6 +5197,24 @@
       </c>
       <c r="H5" s="4">
         <v>1775.9</v>
+      </c>
+      <c r="I5" s="2">
+        <v>12.116</v>
+      </c>
+      <c r="J5" s="2">
+        <v>0.72907</v>
+      </c>
+      <c r="K5" s="2">
+        <v>9.6295000000000002</v>
+      </c>
+      <c r="L5" s="2">
+        <v>2.1265000000000001</v>
+      </c>
+      <c r="M5" s="2">
+        <v>0.31591999999999998</v>
+      </c>
+      <c r="N5" s="2">
+        <v>3.2599</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
@@ -5402,28 +5426,31 @@
       <c r="H16" s="4">
         <v>1828.1</v>
       </c>
-      <c r="I16" s="4">
-        <v>2.0705</v>
-      </c>
-      <c r="J16" s="4">
-        <v>0.52429999999999999</v>
-      </c>
-      <c r="K16" s="4">
-        <v>4.4337</v>
-      </c>
-      <c r="L16" s="4">
-        <v>5.2408999999999999</v>
-      </c>
-      <c r="M16" s="4">
-        <v>3.4408000000000001E-2</v>
-      </c>
-      <c r="N16" s="3">
-        <v>2.3807999999999998</v>
+      <c r="I16" s="2">
+        <v>1.9733000000000001</v>
+      </c>
+      <c r="J16" s="2">
+        <v>0.27233000000000002</v>
+      </c>
+      <c r="K16" s="2">
+        <v>3.1234000000000002</v>
+      </c>
+      <c r="L16" s="2">
+        <v>2.0615999999999999</v>
+      </c>
+      <c r="M16" s="2">
+        <v>9.5870999999999994E-3</v>
+      </c>
+      <c r="N16" s="2">
+        <v>5.4309000000000003</v>
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" s="13"/>
       <c r="B17" s="16"/>
+      <c r="C17" s="8" t="s">
+        <v>45</v>
+      </c>
       <c r="D17" s="4">
         <v>11.45</v>
       </c>
@@ -5438,6 +5465,24 @@
       </c>
       <c r="H17" s="4">
         <v>2221.6</v>
+      </c>
+      <c r="I17" s="2">
+        <v>1.373</v>
+      </c>
+      <c r="J17" s="2">
+        <v>0.39922000000000002</v>
+      </c>
+      <c r="K17" s="2">
+        <v>3.891</v>
+      </c>
+      <c r="L17" s="2">
+        <v>3.8786999999999998</v>
+      </c>
+      <c r="M17" s="2">
+        <v>0.13688</v>
+      </c>
+      <c r="N17" s="2">
+        <v>2.6692999999999998</v>
       </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
@@ -5649,23 +5694,23 @@
       <c r="H28" s="4">
         <v>1433.5</v>
       </c>
-      <c r="I28" s="4">
-        <v>2.7648999999999999</v>
-      </c>
-      <c r="J28" s="4">
-        <v>0.68981999999999999</v>
-      </c>
-      <c r="K28" s="4">
-        <v>5.0537999999999998</v>
-      </c>
-      <c r="L28" s="4">
-        <v>6.1146000000000003</v>
-      </c>
-      <c r="M28" s="4">
-        <v>0.19602</v>
-      </c>
-      <c r="N28" s="3">
-        <v>2.4864000000000002</v>
+      <c r="I28" s="2">
+        <v>2.3410000000000002</v>
+      </c>
+      <c r="J28" s="2">
+        <v>0.39410000000000001</v>
+      </c>
+      <c r="K28" s="2">
+        <v>3.3374000000000001</v>
+      </c>
+      <c r="L28" s="2">
+        <v>5.6124999999999998</v>
+      </c>
+      <c r="M28" s="2">
+        <v>0.94169000000000003</v>
+      </c>
+      <c r="N28" s="2">
+        <v>3.4904999999999999</v>
       </c>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.25">
@@ -5917,30 +5962,30 @@
       <c r="H40" s="4">
         <v>1829.9</v>
       </c>
-      <c r="I40" s="4">
-        <v>1.4641</v>
-      </c>
-      <c r="J40" s="4">
-        <v>0.47352</v>
-      </c>
-      <c r="K40" s="4">
-        <v>3.8866999999999998</v>
-      </c>
-      <c r="L40" s="4">
-        <v>7.1471</v>
-      </c>
-      <c r="M40" s="4">
-        <v>5.6285000000000002E-2</v>
-      </c>
-      <c r="N40" s="3">
-        <v>2.2601</v>
+      <c r="I40" s="2">
+        <v>1.3602000000000001</v>
+      </c>
+      <c r="J40" s="2">
+        <v>0.34182000000000001</v>
+      </c>
+      <c r="K40" s="2">
+        <v>3.1635</v>
+      </c>
+      <c r="L40" s="2">
+        <v>12.426</v>
+      </c>
+      <c r="M40" s="2">
+        <v>0.21156</v>
+      </c>
+      <c r="N40" s="2">
+        <v>3.3578000000000001</v>
       </c>
     </row>
     <row r="41" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A41" s="13"/>
       <c r="B41" s="16"/>
       <c r="C41" s="8" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D41" s="4">
         <v>3.0461</v>

</xml_diff>

<commit_message>
Minor changes for displaying time; new evpwd params
</commit_message>
<xml_diff>
--- a/scripts/__other__/__sem__.xlsx
+++ b/scripts/__other__/__sem__.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Janzen\Desktop\code\moga_neml\scripts\__other__\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A79FADF-661B-4B20-9BE0-3AB555056CCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9071A706-61CE-47B9-A4C4-1EE5C0AC4A44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="15600" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="evp" sheetId="13" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="50">
   <si>
     <t>temp</t>
   </si>
@@ -181,6 +181,15 @@
   </si>
   <si>
     <t>6; 7</t>
+  </si>
+  <si>
+    <t>5; 9</t>
+  </si>
+  <si>
+    <t>5; 7</t>
+  </si>
+  <si>
+    <t>8; 6</t>
   </si>
 </sst>
 </file>
@@ -3550,8 +3559,8 @@
   <dimension ref="A1:L73"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G21" sqref="G21"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3998,31 +4007,31 @@
       <c r="A17" s="13"/>
       <c r="B17" s="16"/>
       <c r="C17" s="8" t="s">
-        <v>45</v>
+        <v>34</v>
       </c>
       <c r="D17" s="2">
-        <v>10.788</v>
+        <v>15.042</v>
       </c>
       <c r="E17" s="2">
-        <v>53.85</v>
+        <v>35.436999999999998</v>
       </c>
       <c r="F17" s="2">
-        <v>7.1745999999999999</v>
+        <v>8.4</v>
       </c>
       <c r="G17" s="2">
-        <v>3.8603999999999998</v>
+        <v>3.9586000000000001</v>
       </c>
       <c r="H17" s="2">
-        <v>2196.3000000000002</v>
+        <v>2283.5</v>
       </c>
       <c r="I17" s="2">
-        <v>3182.9</v>
+        <v>4184.6000000000004</v>
       </c>
       <c r="J17" s="2">
-        <v>4.6458000000000004</v>
+        <v>4.4257</v>
       </c>
       <c r="K17" s="2">
-        <v>3.7222</v>
+        <v>6.6603000000000003</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
@@ -5030,7 +5039,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C42" sqref="C42"/>
+      <selection pane="bottomLeft" activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5220,6 +5229,9 @@
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="13"/>
       <c r="B6" s="16"/>
+      <c r="C6" s="8" t="s">
+        <v>36</v>
+      </c>
       <c r="D6" s="4">
         <v>5.8951000000000002</v>
       </c>
@@ -5234,11 +5246,32 @@
       </c>
       <c r="H6" s="4">
         <v>1598.4</v>
+      </c>
+      <c r="I6" s="4">
+        <v>2.4487000000000001</v>
+      </c>
+      <c r="J6" s="4">
+        <v>0.36314000000000002</v>
+      </c>
+      <c r="K6" s="4">
+        <v>3.4647000000000001</v>
+      </c>
+      <c r="L6" s="4">
+        <v>9.3416999999999994</v>
+      </c>
+      <c r="M6" s="4">
+        <v>0.10058</v>
+      </c>
+      <c r="N6" s="3">
+        <v>3.1581999999999999</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="13"/>
       <c r="B7" s="16"/>
+      <c r="C7" s="8" t="s">
+        <v>48</v>
+      </c>
       <c r="D7" s="4">
         <v>4.1862000000000004</v>
       </c>
@@ -5253,6 +5286,24 @@
       </c>
       <c r="H7" s="4">
         <v>1574.3</v>
+      </c>
+      <c r="I7" s="4">
+        <v>2.0863</v>
+      </c>
+      <c r="J7" s="4">
+        <v>0.34093000000000001</v>
+      </c>
+      <c r="K7" s="4">
+        <v>3.3365999999999998</v>
+      </c>
+      <c r="L7" s="4">
+        <v>1.3308</v>
+      </c>
+      <c r="M7" s="4">
+        <v>1.7129999999999999E-2</v>
+      </c>
+      <c r="N7" s="3">
+        <v>4.0391000000000004</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
@@ -5488,6 +5539,9 @@
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" s="13"/>
       <c r="B18" s="16"/>
+      <c r="C18" s="8" t="s">
+        <v>30</v>
+      </c>
       <c r="D18" s="4">
         <v>37.741999999999997</v>
       </c>
@@ -5502,11 +5556,32 @@
       </c>
       <c r="H18" s="4">
         <v>3172</v>
+      </c>
+      <c r="I18" s="4">
+        <v>2.0438000000000001</v>
+      </c>
+      <c r="J18" s="4">
+        <v>0.32084000000000001</v>
+      </c>
+      <c r="K18" s="4">
+        <v>3.3363999999999998</v>
+      </c>
+      <c r="L18" s="4">
+        <v>8.5211000000000006</v>
+      </c>
+      <c r="M18" s="4">
+        <v>0.38894000000000001</v>
+      </c>
+      <c r="N18" s="3">
+        <v>2.7608999999999999</v>
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" s="13"/>
       <c r="B19" s="16"/>
+      <c r="C19" s="8" t="s">
+        <v>36</v>
+      </c>
       <c r="D19" s="4">
         <v>18.768000000000001</v>
       </c>
@@ -5521,6 +5596,24 @@
       </c>
       <c r="H19" s="4">
         <v>1677.4</v>
+      </c>
+      <c r="I19" s="4">
+        <v>1.9628000000000001</v>
+      </c>
+      <c r="J19" s="4">
+        <v>0.35322999999999999</v>
+      </c>
+      <c r="K19" s="4">
+        <v>3.5571000000000002</v>
+      </c>
+      <c r="L19" s="4">
+        <v>4.0984999999999996</v>
+      </c>
+      <c r="M19" s="4">
+        <v>5.9319999999999998E-2</v>
+      </c>
+      <c r="N19" s="3">
+        <v>2.5131999999999999</v>
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
@@ -5756,6 +5849,9 @@
     <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30" s="13"/>
       <c r="B30" s="16"/>
+      <c r="C30" s="8" t="s">
+        <v>29</v>
+      </c>
       <c r="D30" s="4">
         <v>11.208</v>
       </c>
@@ -5770,11 +5866,32 @@
       </c>
       <c r="H30" s="4">
         <v>1530.1</v>
+      </c>
+      <c r="I30" s="4">
+        <v>1.0164</v>
+      </c>
+      <c r="J30" s="4">
+        <v>0.51859999999999995</v>
+      </c>
+      <c r="K30" s="4">
+        <v>4.4584999999999999</v>
+      </c>
+      <c r="L30" s="4">
+        <v>3.1135000000000002</v>
+      </c>
+      <c r="M30" s="4">
+        <v>0.38601000000000002</v>
+      </c>
+      <c r="N30" s="3">
+        <v>3.3180999999999998</v>
       </c>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A31" s="13"/>
       <c r="B31" s="16"/>
+      <c r="C31" s="8" t="s">
+        <v>49</v>
+      </c>
       <c r="D31" s="4">
         <v>10.45</v>
       </c>
@@ -5789,6 +5906,24 @@
       </c>
       <c r="H31" s="4">
         <v>1787.3</v>
+      </c>
+      <c r="I31" s="4">
+        <v>1.0242</v>
+      </c>
+      <c r="J31" s="4">
+        <v>0.52897000000000005</v>
+      </c>
+      <c r="K31" s="4">
+        <v>4.5477999999999996</v>
+      </c>
+      <c r="L31" s="4">
+        <v>4.5894000000000004</v>
+      </c>
+      <c r="M31" s="4">
+        <v>0.44313000000000002</v>
+      </c>
+      <c r="N31" s="3">
+        <v>3.6385000000000001</v>
       </c>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.25">
@@ -6024,6 +6159,9 @@
     <row r="42" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A42" s="13"/>
       <c r="B42" s="16"/>
+      <c r="C42" s="8" t="s">
+        <v>47</v>
+      </c>
       <c r="D42" s="4">
         <v>4.6340000000000003</v>
       </c>
@@ -6038,11 +6176,32 @@
       </c>
       <c r="H42" s="4">
         <v>1999.7</v>
+      </c>
+      <c r="I42" s="4">
+        <v>2.2488000000000001</v>
+      </c>
+      <c r="J42" s="4">
+        <v>0.27339999999999998</v>
+      </c>
+      <c r="K42" s="4">
+        <v>2.6326000000000001</v>
+      </c>
+      <c r="L42" s="4">
+        <v>4.8822000000000001</v>
+      </c>
+      <c r="M42" s="4">
+        <v>0.17643</v>
+      </c>
+      <c r="N42" s="3">
+        <v>2.3942000000000001</v>
       </c>
     </row>
     <row r="43" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A43" s="13"/>
       <c r="B43" s="16"/>
+      <c r="C43" s="8" t="s">
+        <v>33</v>
+      </c>
       <c r="D43" s="4">
         <v>16.286999999999999</v>
       </c>
@@ -6057,6 +6216,24 @@
       </c>
       <c r="H43" s="4">
         <v>2606.1999999999998</v>
+      </c>
+      <c r="I43" s="4">
+        <v>7.6341000000000001</v>
+      </c>
+      <c r="J43" s="4">
+        <v>0.55245999999999995</v>
+      </c>
+      <c r="K43" s="4">
+        <v>7.7807000000000004</v>
+      </c>
+      <c r="L43" s="4">
+        <v>2.0291999999999999</v>
+      </c>
+      <c r="M43" s="4">
+        <v>0.31213000000000002</v>
+      </c>
+      <c r="N43" s="3">
+        <v>2.8618000000000001</v>
       </c>
     </row>
     <row r="44" spans="1:15" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Added new evpwd params
</commit_message>
<xml_diff>
--- a/scripts/__other__/__sem__.xlsx
+++ b/scripts/__other__/__sem__.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Janzen\Desktop\code\moga_neml\scripts\__other__\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3599D03D-12D5-433F-AA40-E7C9786B7B28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3100ACB5-0548-4CFD-8DC0-1B950F7D6EF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="15600" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="evp" sheetId="13" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="54">
   <si>
     <t>temp</t>
   </si>
@@ -186,9 +186,6 @@
     <t>5; 9</t>
   </si>
   <si>
-    <t>5; 7</t>
-  </si>
-  <si>
     <t>8; 6</t>
   </si>
   <si>
@@ -196,6 +193,15 @@
   </si>
   <si>
     <t>6; 9</t>
+  </si>
+  <si>
+    <t>7; 5</t>
+  </si>
+  <si>
+    <t>5; 6</t>
+  </si>
+  <si>
+    <t>4; 7</t>
   </si>
 </sst>
 </file>
@@ -324,7 +330,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -376,6 +382,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2063,18 +2072,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A38:A49"/>
+    <mergeCell ref="B38:B49"/>
+    <mergeCell ref="A50:A61"/>
+    <mergeCell ref="B50:B61"/>
+    <mergeCell ref="A62:A73"/>
+    <mergeCell ref="B62:B73"/>
     <mergeCell ref="A2:A13"/>
     <mergeCell ref="B2:B13"/>
     <mergeCell ref="A14:A25"/>
     <mergeCell ref="B14:B25"/>
     <mergeCell ref="A26:A37"/>
     <mergeCell ref="B26:B37"/>
-    <mergeCell ref="A38:A49"/>
-    <mergeCell ref="B38:B49"/>
-    <mergeCell ref="A50:A61"/>
-    <mergeCell ref="B50:B61"/>
-    <mergeCell ref="A62:A73"/>
-    <mergeCell ref="B62:B73"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -3542,18 +3551,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A38:A49"/>
+    <mergeCell ref="B38:B49"/>
+    <mergeCell ref="A50:A61"/>
+    <mergeCell ref="B50:B61"/>
+    <mergeCell ref="A62:A73"/>
+    <mergeCell ref="B62:B73"/>
     <mergeCell ref="A2:A13"/>
     <mergeCell ref="B2:B13"/>
     <mergeCell ref="A14:A25"/>
     <mergeCell ref="B14:B25"/>
     <mergeCell ref="A26:A37"/>
     <mergeCell ref="B26:B37"/>
-    <mergeCell ref="A38:A49"/>
-    <mergeCell ref="B38:B49"/>
-    <mergeCell ref="A50:A61"/>
-    <mergeCell ref="B50:B61"/>
-    <mergeCell ref="A62:A73"/>
-    <mergeCell ref="B62:B73"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -5021,18 +5030,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A2:A13"/>
+    <mergeCell ref="B2:B13"/>
+    <mergeCell ref="A14:A25"/>
+    <mergeCell ref="B14:B25"/>
+    <mergeCell ref="A26:A37"/>
+    <mergeCell ref="B26:B37"/>
     <mergeCell ref="A38:A49"/>
     <mergeCell ref="B38:B49"/>
     <mergeCell ref="A50:A61"/>
     <mergeCell ref="B50:B61"/>
     <mergeCell ref="A62:A73"/>
     <mergeCell ref="B62:B73"/>
-    <mergeCell ref="A2:A13"/>
-    <mergeCell ref="B2:B13"/>
-    <mergeCell ref="A14:A25"/>
-    <mergeCell ref="B14:B25"/>
-    <mergeCell ref="A26:A37"/>
-    <mergeCell ref="B26:B37"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -5044,8 +5053,8 @@
   <dimension ref="A1:O73"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G19" sqref="G19"/>
+      <pane ySplit="1" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C48" sqref="C48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5276,47 +5285,47 @@
       <c r="A7" s="13"/>
       <c r="B7" s="16"/>
       <c r="C7" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="D7" s="4">
+        <v>29</v>
+      </c>
+      <c r="D7" s="18">
         <v>4.1862000000000004</v>
       </c>
-      <c r="E7" s="4">
+      <c r="E7" s="18">
         <v>84.548000000000002</v>
       </c>
-      <c r="F7" s="4">
+      <c r="F7" s="18">
         <v>2.1122999999999998</v>
       </c>
-      <c r="G7" s="4">
+      <c r="G7" s="18">
         <v>4.7751999999999999</v>
       </c>
-      <c r="H7" s="4">
+      <c r="H7" s="18">
         <v>1574.3</v>
       </c>
-      <c r="I7" s="4">
-        <v>2.0863</v>
-      </c>
-      <c r="J7" s="4">
-        <v>0.34093000000000001</v>
-      </c>
-      <c r="K7" s="4">
-        <v>3.3365999999999998</v>
-      </c>
-      <c r="L7" s="4">
-        <v>1.3308</v>
-      </c>
-      <c r="M7" s="4">
-        <v>1.7129999999999999E-2</v>
-      </c>
-      <c r="N7" s="3">
-        <v>4.0391000000000004</v>
+      <c r="I7" s="18">
+        <v>1.6472</v>
+      </c>
+      <c r="J7" s="18">
+        <v>0.34209000000000001</v>
+      </c>
+      <c r="K7" s="18">
+        <v>3.5358000000000001</v>
+      </c>
+      <c r="L7" s="18">
+        <v>10.343</v>
+      </c>
+      <c r="M7" s="18">
+        <v>0.55237999999999998</v>
+      </c>
+      <c r="N7" s="18">
+        <v>2.4053</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="13"/>
       <c r="B8" s="16"/>
       <c r="C8" s="8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D8" s="4">
         <v>25.038</v>
@@ -5395,6 +5404,9 @@
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="13"/>
       <c r="B10" s="16"/>
+      <c r="C10" s="8" t="s">
+        <v>36</v>
+      </c>
       <c r="D10" s="4">
         <v>27.885000000000002</v>
       </c>
@@ -5409,11 +5421,32 @@
       </c>
       <c r="H10" s="4">
         <v>2390.5</v>
+      </c>
+      <c r="I10" s="4">
+        <v>1.1933</v>
+      </c>
+      <c r="J10" s="4">
+        <v>0.18759999999999999</v>
+      </c>
+      <c r="K10" s="4">
+        <v>2.4325999999999999</v>
+      </c>
+      <c r="L10" s="4">
+        <v>2.4598</v>
+      </c>
+      <c r="M10" s="4">
+        <v>0.27822999999999998</v>
+      </c>
+      <c r="N10" s="3">
+        <v>3.0878999999999999</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="13"/>
       <c r="B11" s="16"/>
+      <c r="C11" s="8" t="s">
+        <v>52</v>
+      </c>
       <c r="D11" s="4">
         <v>19.2</v>
       </c>
@@ -5428,6 +5461,24 @@
       </c>
       <c r="H11" s="4">
         <v>1614.6</v>
+      </c>
+      <c r="I11" s="4">
+        <v>2.2593000000000001</v>
+      </c>
+      <c r="J11" s="4">
+        <v>0.63022</v>
+      </c>
+      <c r="K11" s="4">
+        <v>4.9957000000000003</v>
+      </c>
+      <c r="L11" s="4">
+        <v>1.0884</v>
+      </c>
+      <c r="M11" s="4">
+        <v>5.1331000000000002E-2</v>
+      </c>
+      <c r="N11" s="3">
+        <v>3.407</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
@@ -5747,6 +5798,9 @@
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" s="13"/>
       <c r="B22" s="16"/>
+      <c r="C22" s="8" t="s">
+        <v>46</v>
+      </c>
       <c r="D22" s="4">
         <v>29.725999999999999</v>
       </c>
@@ -5761,11 +5815,32 @@
       </c>
       <c r="H22" s="4">
         <v>2101.3000000000002</v>
+      </c>
+      <c r="I22" s="4">
+        <v>1.5924</v>
+      </c>
+      <c r="J22" s="4">
+        <v>0.33024999999999999</v>
+      </c>
+      <c r="K22" s="4">
+        <v>3.5438999999999998</v>
+      </c>
+      <c r="L22" s="4">
+        <v>2.0625</v>
+      </c>
+      <c r="M22" s="4">
+        <v>1.2094000000000001E-2</v>
+      </c>
+      <c r="N22" s="3">
+        <v>2.7164000000000001</v>
       </c>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" s="13"/>
       <c r="B23" s="16"/>
+      <c r="C23" s="8" t="s">
+        <v>53</v>
+      </c>
       <c r="D23" s="4">
         <v>0.85682000000000003</v>
       </c>
@@ -5780,6 +5855,24 @@
       </c>
       <c r="H23" s="4">
         <v>1707</v>
+      </c>
+      <c r="I23" s="4">
+        <v>1.5074000000000001</v>
+      </c>
+      <c r="J23" s="4">
+        <v>0.46747</v>
+      </c>
+      <c r="K23" s="4">
+        <v>4.2224000000000004</v>
+      </c>
+      <c r="L23" s="4">
+        <v>7.0061</v>
+      </c>
+      <c r="M23" s="4">
+        <v>0.72074000000000005</v>
+      </c>
+      <c r="N23" s="3">
+        <v>4.0982000000000003</v>
       </c>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
@@ -5980,7 +6073,7 @@
       <c r="A31" s="13"/>
       <c r="B31" s="16"/>
       <c r="C31" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D31" s="4">
         <v>10.45</v>
@@ -6099,6 +6192,9 @@
     <row r="34" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A34" s="13"/>
       <c r="B34" s="16"/>
+      <c r="C34" s="8" t="s">
+        <v>51</v>
+      </c>
       <c r="D34" s="4">
         <v>15.185</v>
       </c>
@@ -6113,11 +6209,32 @@
       </c>
       <c r="H34" s="4">
         <v>2110.6</v>
+      </c>
+      <c r="I34" s="4">
+        <v>1.6442000000000001</v>
+      </c>
+      <c r="J34" s="4">
+        <v>0.55276000000000003</v>
+      </c>
+      <c r="K34" s="4">
+        <v>4.5461</v>
+      </c>
+      <c r="L34" s="4">
+        <v>8.8484999999999996</v>
+      </c>
+      <c r="M34" s="4">
+        <v>0.20913000000000001</v>
+      </c>
+      <c r="N34" s="3">
+        <v>2.6558000000000002</v>
       </c>
     </row>
     <row r="35" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A35" s="13"/>
       <c r="B35" s="16"/>
+      <c r="C35" s="8" t="s">
+        <v>46</v>
+      </c>
       <c r="D35" s="4">
         <v>8.0571999999999999</v>
       </c>
@@ -6132,6 +6249,24 @@
       </c>
       <c r="H35" s="4">
         <v>1210.4000000000001</v>
+      </c>
+      <c r="I35" s="4">
+        <v>3.2982</v>
+      </c>
+      <c r="J35" s="4">
+        <v>0.69935000000000003</v>
+      </c>
+      <c r="K35" s="4">
+        <v>5.0255000000000001</v>
+      </c>
+      <c r="L35" s="4">
+        <v>2.2077</v>
+      </c>
+      <c r="M35" s="4">
+        <v>0.21060999999999999</v>
+      </c>
+      <c r="N35" s="3">
+        <v>3.0865</v>
       </c>
     </row>
     <row r="36" spans="1:15" x14ac:dyDescent="0.25">
@@ -6372,7 +6507,7 @@
       <c r="A44" s="13"/>
       <c r="B44" s="16"/>
       <c r="C44" s="8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D44" s="4">
         <v>9.5312999999999999</v>
@@ -6451,6 +6586,9 @@
     <row r="46" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A46" s="13"/>
       <c r="B46" s="16"/>
+      <c r="C46" s="8" t="s">
+        <v>37</v>
+      </c>
       <c r="D46" s="4">
         <v>12.622</v>
       </c>
@@ -6465,11 +6603,32 @@
       </c>
       <c r="H46" s="4">
         <v>1371.6</v>
+      </c>
+      <c r="I46" s="4">
+        <v>2.1859999999999999</v>
+      </c>
+      <c r="J46" s="4">
+        <v>0.20261000000000001</v>
+      </c>
+      <c r="K46" s="4">
+        <v>2.2957999999999998</v>
+      </c>
+      <c r="L46" s="4">
+        <v>8.5665999999999993</v>
+      </c>
+      <c r="M46" s="4">
+        <v>0.39078000000000002</v>
+      </c>
+      <c r="N46" s="3">
+        <v>2.7238000000000002</v>
       </c>
     </row>
     <row r="47" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A47" s="13"/>
       <c r="B47" s="16"/>
+      <c r="C47" s="8" t="s">
+        <v>31</v>
+      </c>
       <c r="D47" s="4">
         <v>12.256</v>
       </c>
@@ -6484,6 +6643,24 @@
       </c>
       <c r="H47" s="4">
         <v>1242.3</v>
+      </c>
+      <c r="I47" s="4">
+        <v>1.8718999999999999</v>
+      </c>
+      <c r="J47" s="4">
+        <v>0.38352999999999998</v>
+      </c>
+      <c r="K47" s="4">
+        <v>3.4464999999999999</v>
+      </c>
+      <c r="L47" s="4">
+        <v>3.8252999999999999</v>
+      </c>
+      <c r="M47" s="4">
+        <v>0.19616</v>
+      </c>
+      <c r="N47" s="3">
+        <v>2.4363999999999999</v>
       </c>
     </row>
     <row r="48" spans="1:15" x14ac:dyDescent="0.25">
@@ -6624,18 +6801,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A38:A49"/>
+    <mergeCell ref="B38:B49"/>
+    <mergeCell ref="A50:A61"/>
+    <mergeCell ref="B50:B61"/>
+    <mergeCell ref="A62:A73"/>
+    <mergeCell ref="B62:B73"/>
     <mergeCell ref="A2:A13"/>
     <mergeCell ref="B2:B13"/>
     <mergeCell ref="A14:A25"/>
     <mergeCell ref="B14:B25"/>
     <mergeCell ref="A26:A37"/>
     <mergeCell ref="B26:B37"/>
-    <mergeCell ref="A38:A49"/>
-    <mergeCell ref="B38:B49"/>
-    <mergeCell ref="A50:A61"/>
-    <mergeCell ref="B50:B61"/>
-    <mergeCell ref="A62:A73"/>
-    <mergeCell ref="B62:B73"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -7051,18 +7228,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A2:A13"/>
+    <mergeCell ref="B2:B13"/>
+    <mergeCell ref="A14:A25"/>
+    <mergeCell ref="B14:B25"/>
+    <mergeCell ref="A26:A37"/>
+    <mergeCell ref="B26:B37"/>
     <mergeCell ref="A38:A49"/>
     <mergeCell ref="B38:B49"/>
     <mergeCell ref="A50:A61"/>
     <mergeCell ref="B50:B61"/>
     <mergeCell ref="A62:A73"/>
     <mergeCell ref="B62:B73"/>
-    <mergeCell ref="A2:A13"/>
-    <mergeCell ref="B2:B13"/>
-    <mergeCell ref="A14:A25"/>
-    <mergeCell ref="B14:B25"/>
-    <mergeCell ref="A26:A37"/>
-    <mergeCell ref="B26:B37"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
Removed stdev as an option for initialising parameters
</commit_message>
<xml_diff>
--- a/scripts/__other__/__sem__.xlsx
+++ b/scripts/__other__/__sem__.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Janzen\Desktop\code\moga_neml\scripts\__other__\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B479385-BE90-4486-B96A-47759687EF28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24B5579E-9A62-4298-8DC3-55ABDD90EBB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="52">
   <si>
     <t>temp</t>
   </si>
@@ -5043,9 +5043,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C18A26E-30CA-4E63-A18A-C9C101DAF33C}">
   <dimension ref="A1:O73"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O52" sqref="O52"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5116,7 +5116,7 @@
       <c r="A3" s="13"/>
       <c r="B3" s="16"/>
       <c r="C3" s="8" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="D3" s="4">
         <v>17.216999999999999</v>
@@ -5134,22 +5134,22 @@
         <v>1783.5</v>
       </c>
       <c r="I3" s="2">
-        <v>1.6216999999999999</v>
+        <v>1.0025999999999999</v>
       </c>
       <c r="J3" s="2">
-        <v>0.29459999999999997</v>
+        <v>0.41060999999999998</v>
       </c>
       <c r="K3" s="2">
-        <v>3.3557999999999999</v>
+        <v>4.2331000000000003</v>
       </c>
       <c r="L3" s="2">
-        <v>1.0135000000000001</v>
+        <v>2.2349000000000001</v>
       </c>
       <c r="M3" s="2">
-        <v>0.34161999999999998</v>
+        <v>0.29105999999999999</v>
       </c>
       <c r="N3" s="1">
-        <v>3.4578000000000002</v>
+        <v>3.1743000000000001</v>
       </c>
       <c r="O3" s="9" t="s">
         <v>51</v>
@@ -6472,6 +6472,9 @@
       <c r="N40" s="2">
         <v>3.3578000000000001</v>
       </c>
+      <c r="O40" s="9" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="41" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A41" s="13"/>
@@ -6552,6 +6555,9 @@
       <c r="N42" s="3">
         <v>2.3942000000000001</v>
       </c>
+      <c r="O42" s="9" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="43" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A43" s="13"/>
@@ -6592,6 +6598,9 @@
       <c r="N43" s="3">
         <v>2.8618000000000001</v>
       </c>
+      <c r="O43" s="9" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="44" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A44" s="13"/>
@@ -6632,6 +6641,9 @@
       <c r="N44" s="3">
         <v>2.3904000000000001</v>
       </c>
+      <c r="O44" s="9" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="45" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A45" s="13"/>
@@ -6711,6 +6723,9 @@
       </c>
       <c r="N46" s="3">
         <v>2.7238000000000002</v>
+      </c>
+      <c r="O46" s="9" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="47" spans="1:15" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Updated SEM results and added params for evpwd_i
</commit_message>
<xml_diff>
--- a/scripts/__other__/__sem__.xlsx
+++ b/scripts/__other__/__sem__.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Janzen\Desktop\code\moga_neml\scripts\__other__\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24B5579E-9A62-4298-8DC3-55ABDD90EBB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00861E26-399F-4627-A9C5-BDFF34BBD1C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="evp" sheetId="13" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="47">
   <si>
     <t>temp</t>
   </si>
@@ -180,22 +180,7 @@
     <t>6; 8</t>
   </si>
   <si>
-    <t>6; 7</t>
-  </si>
-  <si>
     <t>5; 9</t>
-  </si>
-  <si>
-    <t>8; 6</t>
-  </si>
-  <si>
-    <t>6; 6</t>
-  </si>
-  <si>
-    <t>6; 9</t>
-  </si>
-  <si>
-    <t>x</t>
   </si>
 </sst>
 </file>
@@ -659,9 +644,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4D7A15E-4182-42F6-82DA-99E9B04906BA}">
   <dimension ref="A1:Q73"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="T41" sqref="T41"/>
+      <selection pane="bottomLeft" activeCell="N8" sqref="N8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -749,7 +734,7 @@
         <v>22</v>
       </c>
       <c r="K3" s="8" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
@@ -810,6 +795,9 @@
       <c r="J5" s="8" t="s">
         <v>19</v>
       </c>
+      <c r="K5" s="8" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="13"/>
@@ -838,6 +826,9 @@
       <c r="J6" s="8" t="s">
         <v>20</v>
       </c>
+      <c r="K6" s="8" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="13"/>
@@ -866,6 +857,9 @@
       <c r="J7" s="8" t="s">
         <v>26</v>
       </c>
+      <c r="K7" s="8" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="13"/>
@@ -894,6 +888,9 @@
       <c r="J8" s="8" t="s">
         <v>19</v>
       </c>
+      <c r="K8" s="8" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="13"/>
@@ -922,6 +919,9 @@
       <c r="J9" s="8" t="s">
         <v>35</v>
       </c>
+      <c r="K9" s="8" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="13"/>
@@ -950,6 +950,9 @@
       <c r="J10" s="8" t="s">
         <v>34</v>
       </c>
+      <c r="K10" s="8" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="13"/>
@@ -978,6 +981,9 @@
       <c r="J11" s="8" t="s">
         <v>38</v>
       </c>
+      <c r="K11" s="8" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="13"/>
@@ -1005,6 +1011,9 @@
       </c>
       <c r="J12" s="8" t="s">
         <v>26</v>
+      </c>
+      <c r="K12" s="8" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="13" spans="1:12" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
@@ -1114,6 +1123,9 @@
       <c r="J17" s="8" t="s">
         <v>34</v>
       </c>
+      <c r="K17" s="8" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="13"/>
@@ -1142,6 +1154,9 @@
       <c r="J18" s="8" t="s">
         <v>19</v>
       </c>
+      <c r="K18" s="8" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="13"/>
@@ -1170,6 +1185,9 @@
       <c r="J19" s="8" t="s">
         <v>38</v>
       </c>
+      <c r="K19" s="8" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="13"/>
@@ -1198,6 +1216,9 @@
       <c r="J20" s="8" t="s">
         <v>20</v>
       </c>
+      <c r="K20" s="8" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="13"/>
@@ -1226,6 +1247,9 @@
       <c r="J21" s="8" t="s">
         <v>19</v>
       </c>
+      <c r="K21" s="8" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="13"/>
@@ -1254,6 +1278,9 @@
       <c r="J22" s="8" t="s">
         <v>38</v>
       </c>
+      <c r="K22" s="8" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="13"/>
@@ -1282,6 +1309,9 @@
       <c r="J23" s="8" t="s">
         <v>20</v>
       </c>
+      <c r="K23" s="8" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="13"/>
@@ -1309,6 +1339,9 @@
       </c>
       <c r="J24" s="8" t="s">
         <v>35</v>
+      </c>
+      <c r="K24" s="8" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="25" spans="1:12" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
@@ -1357,7 +1390,7 @@
         <v>23</v>
       </c>
       <c r="K27" s="8" t="s">
-        <v>22</v>
+        <v>35</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
@@ -1449,6 +1482,9 @@
       <c r="J30" s="8" t="s">
         <v>20</v>
       </c>
+      <c r="K30" s="8" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" s="13"/>
@@ -1477,6 +1513,9 @@
       <c r="J31" s="8" t="s">
         <v>19</v>
       </c>
+      <c r="K31" s="8" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" s="13"/>
@@ -1505,6 +1544,9 @@
       <c r="J32" s="8" t="s">
         <v>26</v>
       </c>
+      <c r="K32" s="8" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="33" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A33" s="13"/>
@@ -1533,6 +1575,9 @@
       <c r="J33" s="8" t="s">
         <v>26</v>
       </c>
+      <c r="K33" s="8" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="34" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A34" s="13"/>
@@ -1561,6 +1606,9 @@
       <c r="J34" s="8" t="s">
         <v>22</v>
       </c>
+      <c r="K34" s="8" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="35" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A35" s="13"/>
@@ -1589,6 +1637,9 @@
       <c r="J35" s="8" t="s">
         <v>25</v>
       </c>
+      <c r="K35" s="8" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="36" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A36" s="13"/>
@@ -1616,6 +1667,9 @@
       </c>
       <c r="J36" s="8" t="s">
         <v>26</v>
+      </c>
+      <c r="K36" s="8" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="37" spans="1:17" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
@@ -1700,7 +1754,7 @@
         <v>22</v>
       </c>
       <c r="K40" s="8" t="s">
-        <v>33</v>
+        <v>45</v>
       </c>
       <c r="M40" s="2"/>
       <c r="N40" s="2"/>
@@ -1736,7 +1790,7 @@
         <v>23</v>
       </c>
       <c r="K41" s="8" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="42" spans="1:17" x14ac:dyDescent="0.25">
@@ -1766,6 +1820,9 @@
       <c r="J42" s="8" t="s">
         <v>37</v>
       </c>
+      <c r="K42" s="8" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="43" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A43" s="13"/>
@@ -1794,6 +1851,9 @@
       <c r="J43" s="8" t="s">
         <v>23</v>
       </c>
+      <c r="K43" s="8" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="44" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A44" s="13"/>
@@ -1822,6 +1882,9 @@
       <c r="J44" s="8" t="s">
         <v>25</v>
       </c>
+      <c r="K44" s="8" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="45" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A45" s="13"/>
@@ -1850,6 +1913,9 @@
       <c r="J45" s="8" t="s">
         <v>23</v>
       </c>
+      <c r="K45" s="8" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="46" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A46" s="13"/>
@@ -1878,6 +1944,9 @@
       <c r="J46" s="8" t="s">
         <v>22</v>
       </c>
+      <c r="K46" s="8" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="47" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A47" s="13"/>
@@ -1906,6 +1975,9 @@
       <c r="J47" s="8" t="s">
         <v>35</v>
       </c>
+      <c r="K47" s="8" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="48" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A48" s="13"/>
@@ -1933,6 +2005,9 @@
       </c>
       <c r="J48" s="8" t="s">
         <v>22</v>
+      </c>
+      <c r="K48" s="8" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="49" spans="1:12" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
@@ -5043,9 +5118,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C18A26E-30CA-4E63-A18A-C9C101DAF33C}">
   <dimension ref="A1:O73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K15" sqref="K15"/>
+      <selection pane="bottomLeft" activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5151,9 +5226,6 @@
       <c r="N3" s="1">
         <v>3.1743000000000001</v>
       </c>
-      <c r="O3" s="9" t="s">
-        <v>51</v>
-      </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="13"/>
@@ -5194,15 +5266,12 @@
       <c r="N4" s="2">
         <v>2.7471999999999999</v>
       </c>
-      <c r="O4" s="9" t="s">
-        <v>51</v>
-      </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="13"/>
       <c r="B5" s="16"/>
       <c r="C5" s="8" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="D5" s="4">
         <v>9.3076000000000008</v>
@@ -5220,25 +5289,22 @@
         <v>1775.9</v>
       </c>
       <c r="I5" s="2">
-        <v>12.116</v>
+        <v>1.8393999999999999</v>
       </c>
       <c r="J5" s="2">
-        <v>0.72907</v>
+        <v>0.71550999999999998</v>
       </c>
       <c r="K5" s="2">
-        <v>9.6295000000000002</v>
+        <v>5.8657000000000004</v>
       </c>
       <c r="L5" s="2">
-        <v>2.1265000000000001</v>
+        <v>1.8920999999999999</v>
       </c>
       <c r="M5" s="2">
-        <v>0.31591999999999998</v>
+        <v>0.34444000000000002</v>
       </c>
       <c r="N5" s="2">
-        <v>3.2599</v>
-      </c>
-      <c r="O5" s="9" t="s">
-        <v>51</v>
+        <v>3.5432999999999999</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
@@ -5325,7 +5391,7 @@
       <c r="A8" s="13"/>
       <c r="B8" s="16"/>
       <c r="C8" s="8" t="s">
-        <v>49</v>
+        <v>29</v>
       </c>
       <c r="D8" s="4">
         <v>25.038</v>
@@ -5359,9 +5425,6 @@
       </c>
       <c r="N8" s="3">
         <v>2.9091</v>
-      </c>
-      <c r="O8" s="9" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
@@ -5658,15 +5721,12 @@
       <c r="N17" s="2">
         <v>2.6692999999999998</v>
       </c>
-      <c r="O17" s="9" t="s">
-        <v>51</v>
-      </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" s="13"/>
       <c r="B18" s="16"/>
       <c r="C18" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D18" s="4">
         <v>37.741999999999997</v>
@@ -5684,25 +5744,22 @@
         <v>3172</v>
       </c>
       <c r="I18" s="4">
-        <v>2.0438000000000001</v>
+        <v>1.0524</v>
       </c>
       <c r="J18" s="4">
-        <v>0.32084000000000001</v>
+        <v>0.68115000000000003</v>
       </c>
       <c r="K18" s="4">
-        <v>3.3363999999999998</v>
+        <v>6.5023999999999997</v>
       </c>
       <c r="L18" s="4">
-        <v>8.5211000000000006</v>
+        <v>1.6215999999999999</v>
       </c>
       <c r="M18" s="4">
-        <v>0.38894000000000001</v>
+        <v>0.19822000000000001</v>
       </c>
       <c r="N18" s="3">
-        <v>2.7608999999999999</v>
-      </c>
-      <c r="O18" s="9" t="s">
-        <v>51</v>
+        <v>2.7772999999999999</v>
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
@@ -5829,7 +5886,7 @@
       <c r="A22" s="13"/>
       <c r="B22" s="16"/>
       <c r="C22" s="8" t="s">
-        <v>46</v>
+        <v>29</v>
       </c>
       <c r="D22" s="4">
         <v>29.725999999999999</v>
@@ -5847,25 +5904,22 @@
         <v>2101.3000000000002</v>
       </c>
       <c r="I22" s="4">
-        <v>1.5924</v>
+        <v>1.617</v>
       </c>
       <c r="J22" s="4">
-        <v>0.33024999999999999</v>
+        <v>0.27362999999999998</v>
       </c>
       <c r="K22" s="4">
-        <v>3.5438999999999998</v>
+        <v>3.2206000000000001</v>
       </c>
       <c r="L22" s="4">
-        <v>2.0625</v>
+        <v>5.6994999999999996</v>
       </c>
       <c r="M22" s="4">
-        <v>1.2094000000000001E-2</v>
+        <v>0.96150999999999998</v>
       </c>
       <c r="N22" s="3">
-        <v>2.7164000000000001</v>
-      </c>
-      <c r="O22" s="9" t="s">
-        <v>51</v>
+        <v>3.9527000000000001</v>
       </c>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.25">
@@ -5946,9 +6000,6 @@
       </c>
       <c r="N24" s="3">
         <v>2.7280000000000002</v>
-      </c>
-      <c r="O24" s="9" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="25" spans="1:15" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
@@ -6130,7 +6181,7 @@
       <c r="A31" s="13"/>
       <c r="B31" s="16"/>
       <c r="C31" s="8" t="s">
-        <v>48</v>
+        <v>29</v>
       </c>
       <c r="D31" s="4">
         <v>10.45</v>
@@ -6148,25 +6199,22 @@
         <v>1787.3</v>
       </c>
       <c r="I31" s="4">
-        <v>1.0242</v>
+        <v>1.3337000000000001</v>
       </c>
       <c r="J31" s="4">
-        <v>0.52897000000000005</v>
+        <v>0.59784999999999999</v>
       </c>
       <c r="K31" s="4">
-        <v>4.5477999999999996</v>
+        <v>4.8552999999999997</v>
       </c>
       <c r="L31" s="4">
-        <v>4.5894000000000004</v>
+        <v>2.6320000000000001</v>
       </c>
       <c r="M31" s="4">
-        <v>0.44313000000000002</v>
+        <v>0.34475</v>
       </c>
       <c r="N31" s="3">
-        <v>3.6385000000000001</v>
-      </c>
-      <c r="O31" s="9" t="s">
-        <v>51</v>
+        <v>3.0926</v>
       </c>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.25">
@@ -6248,15 +6296,12 @@
       <c r="N33" s="3">
         <v>3.2061000000000002</v>
       </c>
-      <c r="O33" s="9" t="s">
-        <v>51</v>
-      </c>
     </row>
     <row r="34" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A34" s="13"/>
       <c r="B34" s="16"/>
       <c r="C34" s="8" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="D34" s="4">
         <v>15.185</v>
@@ -6274,32 +6319,29 @@
         <v>2110.6</v>
       </c>
       <c r="I34" s="4">
-        <v>1.2271000000000001</v>
+        <v>1.7833000000000001</v>
       </c>
       <c r="J34" s="4">
-        <v>0.55157999999999996</v>
+        <v>0.51853000000000005</v>
       </c>
       <c r="K34" s="4">
-        <v>4.4852999999999996</v>
+        <v>4.2645</v>
       </c>
       <c r="L34" s="4">
-        <v>3.7134</v>
+        <v>3.7526000000000002</v>
       </c>
       <c r="M34" s="4">
-        <v>0.31269000000000002</v>
+        <v>0.20075000000000001</v>
       </c>
       <c r="N34" s="3">
-        <v>2.7696000000000001</v>
-      </c>
-      <c r="O34" s="9" t="s">
-        <v>51</v>
+        <v>2.5205000000000002</v>
       </c>
     </row>
     <row r="35" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A35" s="13"/>
       <c r="B35" s="16"/>
       <c r="C35" s="8" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="D35" s="4">
         <v>8.0571999999999999</v>
@@ -6317,25 +6359,22 @@
         <v>1210.4000000000001</v>
       </c>
       <c r="I35" s="4">
-        <v>3.2982</v>
+        <v>1.2011000000000001</v>
       </c>
       <c r="J35" s="4">
-        <v>0.69935000000000003</v>
+        <v>0.49431999999999998</v>
       </c>
       <c r="K35" s="4">
-        <v>5.0255000000000001</v>
+        <v>4.3479000000000001</v>
       </c>
       <c r="L35" s="4">
-        <v>2.2077</v>
+        <v>2.7725</v>
       </c>
       <c r="M35" s="4">
-        <v>0.21060999999999999</v>
+        <v>0.29389999999999999</v>
       </c>
       <c r="N35" s="3">
-        <v>3.0865</v>
-      </c>
-      <c r="O35" s="9" t="s">
-        <v>51</v>
+        <v>2.7284999999999999</v>
       </c>
     </row>
     <row r="36" spans="1:15" x14ac:dyDescent="0.25">
@@ -6437,7 +6476,7 @@
       <c r="A40" s="13"/>
       <c r="B40" s="16"/>
       <c r="C40" s="8" t="s">
-        <v>33</v>
+        <v>45</v>
       </c>
       <c r="D40" s="4">
         <v>7.1036999999999999</v>
@@ -6471,9 +6510,6 @@
       </c>
       <c r="N40" s="2">
         <v>3.3578000000000001</v>
-      </c>
-      <c r="O40" s="9" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="41" spans="1:15" x14ac:dyDescent="0.25">
@@ -6520,7 +6556,7 @@
       <c r="A42" s="13"/>
       <c r="B42" s="16"/>
       <c r="C42" s="8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D42" s="4">
         <v>4.6340000000000003</v>
@@ -6554,9 +6590,6 @@
       </c>
       <c r="N42" s="3">
         <v>2.3942000000000001</v>
-      </c>
-      <c r="O42" s="9" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="43" spans="1:15" x14ac:dyDescent="0.25">
@@ -6598,15 +6631,12 @@
       <c r="N43" s="3">
         <v>2.8618000000000001</v>
       </c>
-      <c r="O43" s="9" t="s">
-        <v>51</v>
-      </c>
     </row>
     <row r="44" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A44" s="13"/>
       <c r="B44" s="16"/>
       <c r="C44" s="8" t="s">
-        <v>50</v>
+        <v>36</v>
       </c>
       <c r="D44" s="4">
         <v>9.5312999999999999</v>
@@ -6624,25 +6654,22 @@
         <v>1253.9000000000001</v>
       </c>
       <c r="I44" s="4">
-        <v>2.5960999999999999</v>
+        <v>2.3045</v>
       </c>
       <c r="J44" s="4">
-        <v>0.27945999999999999</v>
+        <v>0.34014</v>
       </c>
       <c r="K44" s="4">
-        <v>2.6425000000000001</v>
+        <v>3.0451000000000001</v>
       </c>
       <c r="L44" s="4">
-        <v>1.018</v>
+        <v>2.7208000000000001</v>
       </c>
       <c r="M44" s="4">
-        <v>0.10278</v>
+        <v>6.7532999999999996E-2</v>
       </c>
       <c r="N44" s="3">
-        <v>2.3904000000000001</v>
-      </c>
-      <c r="O44" s="9" t="s">
-        <v>51</v>
+        <v>2.4268999999999998</v>
       </c>
     </row>
     <row r="45" spans="1:15" x14ac:dyDescent="0.25">
@@ -6689,7 +6716,7 @@
       <c r="A46" s="13"/>
       <c r="B46" s="16"/>
       <c r="C46" s="8" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="D46" s="4">
         <v>12.622</v>
@@ -6707,25 +6734,22 @@
         <v>1371.6</v>
       </c>
       <c r="I46" s="4">
-        <v>2.1859999999999999</v>
+        <v>2.2448999999999999</v>
       </c>
       <c r="J46" s="4">
-        <v>0.20261000000000001</v>
+        <v>0.40698000000000001</v>
       </c>
       <c r="K46" s="4">
-        <v>2.2957999999999998</v>
+        <v>3.5036</v>
       </c>
       <c r="L46" s="4">
-        <v>8.5665999999999993</v>
+        <v>4.0568</v>
       </c>
       <c r="M46" s="4">
-        <v>0.39078000000000002</v>
+        <v>0.21132000000000001</v>
       </c>
       <c r="N46" s="3">
-        <v>2.7238000000000002</v>
-      </c>
-      <c r="O46" s="9" t="s">
-        <v>51</v>
+        <v>2.4597000000000002</v>
       </c>
     </row>
     <row r="47" spans="1:15" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Changed evpwdb_f model to reject bad params
</commit_message>
<xml_diff>
--- a/scripts/__other__/__sem__.xlsx
+++ b/scripts/__other__/__sem__.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Janzen\Desktop\code\moga_neml\scripts\__other__\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00861E26-399F-4627-A9C5-BDFF34BBD1C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3016A677-967C-42D1-8E00-6534D90ED773}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="evp" sheetId="13" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="373" uniqueCount="47">
   <si>
     <t>temp</t>
   </si>
@@ -644,9 +644,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4D7A15E-4182-42F6-82DA-99E9B04906BA}">
   <dimension ref="A1:Q73"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N8" sqref="N8"/>
+      <selection pane="bottomLeft" activeCell="D4" sqref="D4:H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2138,18 +2138,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A38:A49"/>
+    <mergeCell ref="B38:B49"/>
+    <mergeCell ref="A50:A61"/>
+    <mergeCell ref="B50:B61"/>
+    <mergeCell ref="A62:A73"/>
+    <mergeCell ref="B62:B73"/>
     <mergeCell ref="A2:A13"/>
     <mergeCell ref="B2:B13"/>
     <mergeCell ref="A14:A25"/>
     <mergeCell ref="B14:B25"/>
     <mergeCell ref="A26:A37"/>
     <mergeCell ref="B26:B37"/>
-    <mergeCell ref="A38:A49"/>
-    <mergeCell ref="B38:B49"/>
-    <mergeCell ref="A50:A61"/>
-    <mergeCell ref="B50:B61"/>
-    <mergeCell ref="A62:A73"/>
-    <mergeCell ref="B62:B73"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -3617,18 +3617,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A38:A49"/>
+    <mergeCell ref="B38:B49"/>
+    <mergeCell ref="A50:A61"/>
+    <mergeCell ref="B50:B61"/>
+    <mergeCell ref="A62:A73"/>
+    <mergeCell ref="B62:B73"/>
     <mergeCell ref="A2:A13"/>
     <mergeCell ref="B2:B13"/>
     <mergeCell ref="A14:A25"/>
     <mergeCell ref="B14:B25"/>
     <mergeCell ref="A26:A37"/>
     <mergeCell ref="B26:B37"/>
-    <mergeCell ref="A38:A49"/>
-    <mergeCell ref="B38:B49"/>
-    <mergeCell ref="A50:A61"/>
-    <mergeCell ref="B50:B61"/>
-    <mergeCell ref="A62:A73"/>
-    <mergeCell ref="B62:B73"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -5096,6 +5096,1861 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A2:A13"/>
+    <mergeCell ref="B2:B13"/>
+    <mergeCell ref="A14:A25"/>
+    <mergeCell ref="B14:B25"/>
+    <mergeCell ref="A26:A37"/>
+    <mergeCell ref="B26:B37"/>
+    <mergeCell ref="A38:A49"/>
+    <mergeCell ref="B38:B49"/>
+    <mergeCell ref="A50:A61"/>
+    <mergeCell ref="B50:B61"/>
+    <mergeCell ref="A62:A73"/>
+    <mergeCell ref="B62:B73"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C18A26E-30CA-4E63-A18A-C9C101DAF33C}">
+  <dimension ref="A1:O73"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L1" sqref="L1:L1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="4"/>
+    <col min="2" max="2" width="9.140625" style="3"/>
+    <col min="3" max="3" width="15.7109375" style="8" customWidth="1"/>
+    <col min="4" max="13" width="9.140625" style="4"/>
+    <col min="14" max="14" width="9.140625" style="3"/>
+    <col min="15" max="15" width="9.140625" style="9"/>
+    <col min="16" max="16384" width="9.140625" style="4"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="L1" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="M1" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="N1" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="O1" s="11"/>
+    </row>
+    <row r="2" spans="1:15" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="12">
+        <v>800</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3" s="13"/>
+      <c r="B3" s="16"/>
+      <c r="C3" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="D3" s="4">
+        <v>17.216999999999999</v>
+      </c>
+      <c r="E3" s="4">
+        <v>179.74</v>
+      </c>
+      <c r="F3" s="4">
+        <v>0.61753999999999998</v>
+      </c>
+      <c r="G3" s="4">
+        <v>4.4165999999999999</v>
+      </c>
+      <c r="H3" s="4">
+        <v>1783.5</v>
+      </c>
+      <c r="I3" s="2">
+        <v>1.0025999999999999</v>
+      </c>
+      <c r="J3" s="2">
+        <v>0.41060999999999998</v>
+      </c>
+      <c r="K3" s="2">
+        <v>4.2331000000000003</v>
+      </c>
+      <c r="L3" s="2">
+        <v>2.2349000000000001</v>
+      </c>
+      <c r="M3" s="2">
+        <v>0.29105999999999999</v>
+      </c>
+      <c r="N3" s="1">
+        <v>3.1743000000000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4" s="13"/>
+      <c r="B4" s="16"/>
+      <c r="C4" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="D4" s="4">
+        <v>5.6908000000000003</v>
+      </c>
+      <c r="E4" s="4">
+        <v>66.626999999999995</v>
+      </c>
+      <c r="F4" s="4">
+        <v>1.9851000000000001</v>
+      </c>
+      <c r="G4" s="4">
+        <v>4.7723000000000004</v>
+      </c>
+      <c r="H4" s="4">
+        <v>1621.6</v>
+      </c>
+      <c r="I4" s="2">
+        <v>1.8904000000000001</v>
+      </c>
+      <c r="J4" s="2">
+        <v>0.54329000000000005</v>
+      </c>
+      <c r="K4" s="2">
+        <v>4.6087999999999996</v>
+      </c>
+      <c r="L4" s="2">
+        <v>1.8685</v>
+      </c>
+      <c r="M4" s="2">
+        <v>9.3698000000000004E-2</v>
+      </c>
+      <c r="N4" s="2">
+        <v>2.7471999999999999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5" s="13"/>
+      <c r="B5" s="16"/>
+      <c r="C5" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="D5" s="4">
+        <v>9.3076000000000008</v>
+      </c>
+      <c r="E5" s="4">
+        <v>32.595999999999997</v>
+      </c>
+      <c r="F5" s="4">
+        <v>5.8113999999999999</v>
+      </c>
+      <c r="G5" s="4">
+        <v>4.5263</v>
+      </c>
+      <c r="H5" s="4">
+        <v>1775.9</v>
+      </c>
+      <c r="I5" s="2">
+        <v>1.8393999999999999</v>
+      </c>
+      <c r="J5" s="2">
+        <v>0.71550999999999998</v>
+      </c>
+      <c r="K5" s="2">
+        <v>5.8657000000000004</v>
+      </c>
+      <c r="L5" s="2">
+        <v>1.8920999999999999</v>
+      </c>
+      <c r="M5" s="2">
+        <v>0.34444000000000002</v>
+      </c>
+      <c r="N5" s="2">
+        <v>3.5432999999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6" s="13"/>
+      <c r="B6" s="16"/>
+      <c r="C6" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="D6" s="4">
+        <v>5.8951000000000002</v>
+      </c>
+      <c r="E6" s="4">
+        <v>36.244999999999997</v>
+      </c>
+      <c r="F6" s="4">
+        <v>5.3757000000000001</v>
+      </c>
+      <c r="G6" s="4">
+        <v>4.7310999999999996</v>
+      </c>
+      <c r="H6" s="4">
+        <v>1598.4</v>
+      </c>
+      <c r="I6" s="4">
+        <v>2.4487000000000001</v>
+      </c>
+      <c r="J6" s="4">
+        <v>0.36314000000000002</v>
+      </c>
+      <c r="K6" s="4">
+        <v>3.4647000000000001</v>
+      </c>
+      <c r="L6" s="4">
+        <v>9.3416999999999994</v>
+      </c>
+      <c r="M6" s="4">
+        <v>0.10058</v>
+      </c>
+      <c r="N6" s="3">
+        <v>3.1581999999999999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A7" s="13"/>
+      <c r="B7" s="16"/>
+      <c r="C7" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="D7" s="2">
+        <v>4.1862000000000004</v>
+      </c>
+      <c r="E7" s="2">
+        <v>84.548000000000002</v>
+      </c>
+      <c r="F7" s="2">
+        <v>2.1122999999999998</v>
+      </c>
+      <c r="G7" s="2">
+        <v>4.7751999999999999</v>
+      </c>
+      <c r="H7" s="2">
+        <v>1574.3</v>
+      </c>
+      <c r="I7" s="2">
+        <v>1.6472</v>
+      </c>
+      <c r="J7" s="2">
+        <v>0.34209000000000001</v>
+      </c>
+      <c r="K7" s="2">
+        <v>3.5358000000000001</v>
+      </c>
+      <c r="L7" s="2">
+        <v>10.343</v>
+      </c>
+      <c r="M7" s="2">
+        <v>0.55237999999999998</v>
+      </c>
+      <c r="N7" s="2">
+        <v>2.4053</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A8" s="13"/>
+      <c r="B8" s="16"/>
+      <c r="C8" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="D8" s="4">
+        <v>25.038</v>
+      </c>
+      <c r="E8" s="4">
+        <v>90.692999999999998</v>
+      </c>
+      <c r="F8" s="4">
+        <v>0.61002000000000001</v>
+      </c>
+      <c r="G8" s="4">
+        <v>4.1981999999999999</v>
+      </c>
+      <c r="H8" s="4">
+        <v>1944.6</v>
+      </c>
+      <c r="I8" s="4">
+        <v>1.3413999999999999</v>
+      </c>
+      <c r="J8" s="4">
+        <v>0.39294000000000001</v>
+      </c>
+      <c r="K8" s="4">
+        <v>3.9001000000000001</v>
+      </c>
+      <c r="L8" s="4">
+        <v>4.3860999999999999</v>
+      </c>
+      <c r="M8" s="4">
+        <v>0.24360999999999999</v>
+      </c>
+      <c r="N8" s="3">
+        <v>2.9091</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A9" s="13"/>
+      <c r="B9" s="16"/>
+      <c r="C9" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="D9" s="4">
+        <v>27.547000000000001</v>
+      </c>
+      <c r="E9" s="4">
+        <v>78.081000000000003</v>
+      </c>
+      <c r="F9" s="4">
+        <v>0.84272999999999998</v>
+      </c>
+      <c r="G9" s="4">
+        <v>3.8992</v>
+      </c>
+      <c r="H9" s="4">
+        <v>2454.8000000000002</v>
+      </c>
+      <c r="I9" s="4">
+        <v>1.8298000000000001</v>
+      </c>
+      <c r="J9" s="4">
+        <v>0.44322</v>
+      </c>
+      <c r="K9" s="4">
+        <v>4.1135000000000002</v>
+      </c>
+      <c r="L9" s="4">
+        <v>4.6660000000000004</v>
+      </c>
+      <c r="M9" s="4">
+        <v>7.2484999999999994E-2</v>
+      </c>
+      <c r="N9" s="3">
+        <v>2.4855999999999998</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A10" s="13"/>
+      <c r="B10" s="16"/>
+      <c r="C10" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="D10" s="4">
+        <v>27.885000000000002</v>
+      </c>
+      <c r="E10" s="4">
+        <v>124.89</v>
+      </c>
+      <c r="F10" s="4">
+        <v>0.65636000000000005</v>
+      </c>
+      <c r="G10" s="4">
+        <v>3.8874</v>
+      </c>
+      <c r="H10" s="4">
+        <v>2390.5</v>
+      </c>
+      <c r="I10" s="4">
+        <v>1.1933</v>
+      </c>
+      <c r="J10" s="4">
+        <v>0.18759999999999999</v>
+      </c>
+      <c r="K10" s="4">
+        <v>2.4325999999999999</v>
+      </c>
+      <c r="L10" s="4">
+        <v>2.4598</v>
+      </c>
+      <c r="M10" s="4">
+        <v>0.27822999999999998</v>
+      </c>
+      <c r="N10" s="3">
+        <v>3.0878999999999999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A11" s="13"/>
+      <c r="B11" s="16"/>
+      <c r="C11" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="D11" s="4">
+        <v>19.2</v>
+      </c>
+      <c r="E11" s="4">
+        <v>52.204000000000001</v>
+      </c>
+      <c r="F11" s="4">
+        <v>1.7579</v>
+      </c>
+      <c r="G11" s="4">
+        <v>4.5105000000000004</v>
+      </c>
+      <c r="H11" s="4">
+        <v>1614.6</v>
+      </c>
+      <c r="I11" s="4">
+        <v>1.0317000000000001</v>
+      </c>
+      <c r="J11" s="4">
+        <v>0.54349000000000003</v>
+      </c>
+      <c r="K11" s="4">
+        <v>5.2065000000000001</v>
+      </c>
+      <c r="L11" s="4">
+        <v>3.1556999999999999</v>
+      </c>
+      <c r="M11" s="4">
+        <v>0.27356999999999998</v>
+      </c>
+      <c r="N11" s="3">
+        <v>3.1248</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A12" s="13"/>
+      <c r="B12" s="16"/>
+      <c r="C12" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="D12" s="4">
+        <v>8.5922999999999998</v>
+      </c>
+      <c r="E12" s="4">
+        <v>38.904000000000003</v>
+      </c>
+      <c r="F12" s="4">
+        <v>5.4828999999999999</v>
+      </c>
+      <c r="G12" s="4">
+        <v>4.4794999999999998</v>
+      </c>
+      <c r="H12" s="4">
+        <v>1841</v>
+      </c>
+      <c r="I12" s="4">
+        <v>2.2498</v>
+      </c>
+      <c r="J12" s="4">
+        <v>0.39954000000000001</v>
+      </c>
+      <c r="K12" s="4">
+        <v>3.722</v>
+      </c>
+      <c r="L12" s="4">
+        <v>4.2567000000000004</v>
+      </c>
+      <c r="M12" s="4">
+        <v>0.19838</v>
+      </c>
+      <c r="N12" s="3">
+        <v>3.5486</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="14"/>
+      <c r="B13" s="17"/>
+      <c r="C13" s="7"/>
+      <c r="N13" s="6"/>
+      <c r="O13" s="11"/>
+    </row>
+    <row r="14" spans="1:15" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="12">
+        <v>800</v>
+      </c>
+      <c r="B14" s="15" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A15" s="13"/>
+      <c r="B15" s="16"/>
+      <c r="C15" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="D15" s="4">
+        <v>31.327000000000002</v>
+      </c>
+      <c r="E15" s="4">
+        <v>104.92</v>
+      </c>
+      <c r="F15" s="4">
+        <v>0.8548</v>
+      </c>
+      <c r="G15" s="4">
+        <v>3.7507999999999999</v>
+      </c>
+      <c r="H15" s="4">
+        <v>2575.8000000000002</v>
+      </c>
+      <c r="I15" s="4">
+        <v>1.0368999999999999</v>
+      </c>
+      <c r="J15" s="4">
+        <v>0.33298</v>
+      </c>
+      <c r="K15" s="4">
+        <v>3.661</v>
+      </c>
+      <c r="L15" s="4">
+        <v>1.9359999999999999</v>
+      </c>
+      <c r="M15" s="4">
+        <v>0.26541999999999999</v>
+      </c>
+      <c r="N15" s="3">
+        <v>3.1442999999999999</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A16" s="13"/>
+      <c r="B16" s="16"/>
+      <c r="C16" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="D16" s="4">
+        <v>22.393000000000001</v>
+      </c>
+      <c r="E16" s="4">
+        <v>462.57</v>
+      </c>
+      <c r="F16" s="4">
+        <v>0.13572999999999999</v>
+      </c>
+      <c r="G16" s="4">
+        <v>4.3140000000000001</v>
+      </c>
+      <c r="H16" s="4">
+        <v>1828.1</v>
+      </c>
+      <c r="I16" s="2">
+        <v>1.9733000000000001</v>
+      </c>
+      <c r="J16" s="2">
+        <v>0.27233000000000002</v>
+      </c>
+      <c r="K16" s="2">
+        <v>3.1234000000000002</v>
+      </c>
+      <c r="L16" s="2">
+        <v>2.0615999999999999</v>
+      </c>
+      <c r="M16" s="2">
+        <v>9.5870999999999994E-3</v>
+      </c>
+      <c r="N16" s="2">
+        <v>5.4309000000000003</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A17" s="13"/>
+      <c r="B17" s="16"/>
+      <c r="C17" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="D17" s="4">
+        <v>11.45</v>
+      </c>
+      <c r="E17" s="4">
+        <v>53.151000000000003</v>
+      </c>
+      <c r="F17" s="4">
+        <v>7.1665999999999999</v>
+      </c>
+      <c r="G17" s="4">
+        <v>3.9502000000000002</v>
+      </c>
+      <c r="H17" s="4">
+        <v>2221.6</v>
+      </c>
+      <c r="I17" s="2">
+        <v>1.373</v>
+      </c>
+      <c r="J17" s="2">
+        <v>0.39922000000000002</v>
+      </c>
+      <c r="K17" s="2">
+        <v>3.891</v>
+      </c>
+      <c r="L17" s="2">
+        <v>3.8786999999999998</v>
+      </c>
+      <c r="M17" s="2">
+        <v>0.13688</v>
+      </c>
+      <c r="N17" s="2">
+        <v>2.6692999999999998</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A18" s="13"/>
+      <c r="B18" s="16"/>
+      <c r="C18" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="D18" s="4">
+        <v>37.741999999999997</v>
+      </c>
+      <c r="E18" s="4">
+        <v>49.122999999999998</v>
+      </c>
+      <c r="F18" s="4">
+        <v>2.4996</v>
+      </c>
+      <c r="G18" s="4">
+        <v>3.4102000000000001</v>
+      </c>
+      <c r="H18" s="4">
+        <v>3172</v>
+      </c>
+      <c r="I18" s="4">
+        <v>1.0524</v>
+      </c>
+      <c r="J18" s="4">
+        <v>0.68115000000000003</v>
+      </c>
+      <c r="K18" s="4">
+        <v>6.5023999999999997</v>
+      </c>
+      <c r="L18" s="4">
+        <v>1.6215999999999999</v>
+      </c>
+      <c r="M18" s="4">
+        <v>0.19822000000000001</v>
+      </c>
+      <c r="N18" s="3">
+        <v>2.7772999999999999</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A19" s="13"/>
+      <c r="B19" s="16"/>
+      <c r="C19" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="D19" s="4">
+        <v>18.768000000000001</v>
+      </c>
+      <c r="E19" s="4">
+        <v>89.18</v>
+      </c>
+      <c r="F19" s="4">
+        <v>0.88068999999999997</v>
+      </c>
+      <c r="G19" s="4">
+        <v>4.5054999999999996</v>
+      </c>
+      <c r="H19" s="4">
+        <v>1677.4</v>
+      </c>
+      <c r="I19" s="4">
+        <v>1.9628000000000001</v>
+      </c>
+      <c r="J19" s="4">
+        <v>0.35322999999999999</v>
+      </c>
+      <c r="K19" s="4">
+        <v>3.5571000000000002</v>
+      </c>
+      <c r="L19" s="4">
+        <v>4.0984999999999996</v>
+      </c>
+      <c r="M19" s="4">
+        <v>5.9319999999999998E-2</v>
+      </c>
+      <c r="N19" s="3">
+        <v>2.5131999999999999</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A20" s="13"/>
+      <c r="B20" s="16"/>
+      <c r="C20" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="D20" s="4">
+        <v>23.303999999999998</v>
+      </c>
+      <c r="E20" s="4">
+        <v>306.58</v>
+      </c>
+      <c r="F20" s="4">
+        <v>0.32123000000000002</v>
+      </c>
+      <c r="G20" s="4">
+        <v>4.2591999999999999</v>
+      </c>
+      <c r="H20" s="4">
+        <v>1822.6</v>
+      </c>
+      <c r="I20" s="4">
+        <v>1.6464000000000001</v>
+      </c>
+      <c r="J20" s="4">
+        <v>0.23887</v>
+      </c>
+      <c r="K20" s="4">
+        <v>2.9979</v>
+      </c>
+      <c r="L20" s="4">
+        <v>4.1620999999999997</v>
+      </c>
+      <c r="M20" s="4">
+        <v>2.9884999999999998E-3</v>
+      </c>
+      <c r="N20" s="3">
+        <v>2.3424999999999998</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A21" s="13"/>
+      <c r="B21" s="16"/>
+      <c r="C21" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="D21" s="4">
+        <v>31.137</v>
+      </c>
+      <c r="E21" s="4">
+        <v>31.413</v>
+      </c>
+      <c r="F21" s="4">
+        <v>4.6002999999999998</v>
+      </c>
+      <c r="G21" s="4">
+        <v>3.6958000000000002</v>
+      </c>
+      <c r="H21" s="4">
+        <v>2583</v>
+      </c>
+      <c r="I21" s="4">
+        <v>1.2944</v>
+      </c>
+      <c r="J21" s="4">
+        <v>0.36685000000000001</v>
+      </c>
+      <c r="K21" s="4">
+        <v>3.8721000000000001</v>
+      </c>
+      <c r="L21" s="4">
+        <v>2.0034000000000001</v>
+      </c>
+      <c r="M21" s="4">
+        <v>0.2167</v>
+      </c>
+      <c r="N21" s="3">
+        <v>2.8479999999999999</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A22" s="13"/>
+      <c r="B22" s="16"/>
+      <c r="C22" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="D22" s="4">
+        <v>29.725999999999999</v>
+      </c>
+      <c r="E22" s="4">
+        <v>45.991</v>
+      </c>
+      <c r="F22" s="4">
+        <v>2.3174000000000001</v>
+      </c>
+      <c r="G22" s="4">
+        <v>3.9613</v>
+      </c>
+      <c r="H22" s="4">
+        <v>2101.3000000000002</v>
+      </c>
+      <c r="I22" s="4">
+        <v>1.617</v>
+      </c>
+      <c r="J22" s="4">
+        <v>0.27362999999999998</v>
+      </c>
+      <c r="K22" s="4">
+        <v>3.2206000000000001</v>
+      </c>
+      <c r="L22" s="4">
+        <v>5.6994999999999996</v>
+      </c>
+      <c r="M22" s="4">
+        <v>0.96150999999999998</v>
+      </c>
+      <c r="N22" s="3">
+        <v>3.9527000000000001</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A23" s="13"/>
+      <c r="B23" s="16"/>
+      <c r="C23" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="D23" s="4">
+        <v>0.85682000000000003</v>
+      </c>
+      <c r="E23" s="4">
+        <v>42.524000000000001</v>
+      </c>
+      <c r="F23" s="4">
+        <v>9.6282999999999994</v>
+      </c>
+      <c r="G23" s="4">
+        <v>4.5033000000000003</v>
+      </c>
+      <c r="H23" s="4">
+        <v>1707</v>
+      </c>
+      <c r="I23" s="4">
+        <v>1.2393000000000001</v>
+      </c>
+      <c r="J23" s="4">
+        <v>0.28849000000000002</v>
+      </c>
+      <c r="K23" s="4">
+        <v>3.4293</v>
+      </c>
+      <c r="L23" s="4">
+        <v>3.0653999999999999</v>
+      </c>
+      <c r="M23" s="4">
+        <v>0.11899999999999999</v>
+      </c>
+      <c r="N23" s="3">
+        <v>2.6208</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A24" s="13"/>
+      <c r="B24" s="16"/>
+      <c r="C24" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="D24" s="4">
+        <v>4.4611000000000001</v>
+      </c>
+      <c r="E24" s="4">
+        <v>35.628</v>
+      </c>
+      <c r="F24" s="4">
+        <v>31.021000000000001</v>
+      </c>
+      <c r="G24" s="4">
+        <v>3.6185999999999998</v>
+      </c>
+      <c r="H24" s="4">
+        <v>3016.2</v>
+      </c>
+      <c r="I24" s="4">
+        <v>9.5056999999999992</v>
+      </c>
+      <c r="J24" s="4">
+        <v>0.33045999999999998</v>
+      </c>
+      <c r="K24" s="4">
+        <v>3.327</v>
+      </c>
+      <c r="L24" s="4">
+        <v>4.6459000000000001</v>
+      </c>
+      <c r="M24" s="4">
+        <v>0.20498</v>
+      </c>
+      <c r="N24" s="3">
+        <v>2.7280000000000002</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="14"/>
+      <c r="B25" s="17"/>
+      <c r="C25" s="7"/>
+      <c r="N25" s="6"/>
+      <c r="O25" s="11"/>
+    </row>
+    <row r="26" spans="1:15" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="12">
+        <v>900</v>
+      </c>
+      <c r="B26" s="15" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A27" s="13"/>
+      <c r="B27" s="16"/>
+      <c r="C27" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="D27" s="4">
+        <v>4.8710000000000004</v>
+      </c>
+      <c r="E27" s="4">
+        <v>11.518000000000001</v>
+      </c>
+      <c r="F27" s="4">
+        <v>7.0281000000000002</v>
+      </c>
+      <c r="G27" s="4">
+        <v>4.2420999999999998</v>
+      </c>
+      <c r="H27" s="4">
+        <v>1138.3</v>
+      </c>
+      <c r="I27" s="4">
+        <v>1.2072000000000001</v>
+      </c>
+      <c r="J27" s="4">
+        <v>0.44550000000000001</v>
+      </c>
+      <c r="K27" s="4">
+        <v>3.8687</v>
+      </c>
+      <c r="L27" s="4">
+        <v>3.6877</v>
+      </c>
+      <c r="M27" s="4">
+        <v>0.25385000000000002</v>
+      </c>
+      <c r="N27" s="3">
+        <v>2.5308000000000002</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A28" s="13"/>
+      <c r="B28" s="16"/>
+      <c r="C28" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="D28" s="4">
+        <v>10.692</v>
+      </c>
+      <c r="E28" s="4">
+        <v>29.068000000000001</v>
+      </c>
+      <c r="F28" s="4">
+        <v>2.9830999999999999</v>
+      </c>
+      <c r="G28" s="4">
+        <v>3.7277999999999998</v>
+      </c>
+      <c r="H28" s="4">
+        <v>1433.5</v>
+      </c>
+      <c r="I28" s="2">
+        <v>2.3410000000000002</v>
+      </c>
+      <c r="J28" s="2">
+        <v>0.39410000000000001</v>
+      </c>
+      <c r="K28" s="2">
+        <v>3.3374000000000001</v>
+      </c>
+      <c r="L28" s="2">
+        <v>5.6124999999999998</v>
+      </c>
+      <c r="M28" s="2">
+        <v>0.94169000000000003</v>
+      </c>
+      <c r="N28" s="2">
+        <v>3.4904999999999999</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A29" s="13"/>
+      <c r="B29" s="16"/>
+      <c r="C29" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="D29" s="4">
+        <v>11.2</v>
+      </c>
+      <c r="E29" s="4">
+        <v>24.262</v>
+      </c>
+      <c r="F29" s="4">
+        <v>2.2614999999999998</v>
+      </c>
+      <c r="G29" s="4">
+        <v>3.9651000000000001</v>
+      </c>
+      <c r="H29" s="4">
+        <v>1163</v>
+      </c>
+      <c r="I29" s="4">
+        <v>1.7908999999999999</v>
+      </c>
+      <c r="J29" s="4">
+        <v>0.45981</v>
+      </c>
+      <c r="K29" s="4">
+        <v>3.9491000000000001</v>
+      </c>
+      <c r="L29" s="4">
+        <v>3.3142</v>
+      </c>
+      <c r="M29" s="4">
+        <v>0.20016999999999999</v>
+      </c>
+      <c r="N29" s="3">
+        <v>2.4437000000000002</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A30" s="13"/>
+      <c r="B30" s="16"/>
+      <c r="C30" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="D30" s="4">
+        <v>11.208</v>
+      </c>
+      <c r="E30" s="4">
+        <v>16.738</v>
+      </c>
+      <c r="F30" s="4">
+        <v>5.9587000000000003</v>
+      </c>
+      <c r="G30" s="4">
+        <v>3.6377000000000002</v>
+      </c>
+      <c r="H30" s="4">
+        <v>1530.1</v>
+      </c>
+      <c r="I30" s="4">
+        <v>1.0164</v>
+      </c>
+      <c r="J30" s="4">
+        <v>0.51859999999999995</v>
+      </c>
+      <c r="K30" s="4">
+        <v>4.4584999999999999</v>
+      </c>
+      <c r="L30" s="4">
+        <v>3.1135000000000002</v>
+      </c>
+      <c r="M30" s="4">
+        <v>0.38601000000000002</v>
+      </c>
+      <c r="N30" s="3">
+        <v>3.3180999999999998</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A31" s="13"/>
+      <c r="B31" s="16"/>
+      <c r="C31" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="D31" s="4">
+        <v>10.45</v>
+      </c>
+      <c r="E31" s="4">
+        <v>14.769</v>
+      </c>
+      <c r="F31" s="4">
+        <v>7.8792</v>
+      </c>
+      <c r="G31" s="4">
+        <v>3.54</v>
+      </c>
+      <c r="H31" s="4">
+        <v>1787.3</v>
+      </c>
+      <c r="I31" s="4">
+        <v>1.3337000000000001</v>
+      </c>
+      <c r="J31" s="4">
+        <v>0.59784999999999999</v>
+      </c>
+      <c r="K31" s="4">
+        <v>4.8552999999999997</v>
+      </c>
+      <c r="L31" s="4">
+        <v>2.6320000000000001</v>
+      </c>
+      <c r="M31" s="4">
+        <v>0.34475</v>
+      </c>
+      <c r="N31" s="3">
+        <v>3.0926</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A32" s="13"/>
+      <c r="B32" s="16"/>
+      <c r="C32" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D32" s="4">
+        <v>11.010999999999999</v>
+      </c>
+      <c r="E32" s="4">
+        <v>11.071</v>
+      </c>
+      <c r="F32" s="4">
+        <v>13.523</v>
+      </c>
+      <c r="G32" s="4">
+        <v>3.5672000000000001</v>
+      </c>
+      <c r="H32" s="4">
+        <v>1593.8</v>
+      </c>
+      <c r="I32" s="4">
+        <v>2.0019</v>
+      </c>
+      <c r="J32" s="4">
+        <v>0.50361</v>
+      </c>
+      <c r="K32" s="4">
+        <v>4.1786000000000003</v>
+      </c>
+      <c r="L32" s="4">
+        <v>4.2843</v>
+      </c>
+      <c r="M32" s="4">
+        <v>0.22523000000000001</v>
+      </c>
+      <c r="N32" s="3">
+        <v>2.6124999999999998</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A33" s="13"/>
+      <c r="B33" s="16"/>
+      <c r="C33" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="D33" s="4">
+        <v>5.6656000000000004</v>
+      </c>
+      <c r="E33" s="4">
+        <v>8.2222000000000008</v>
+      </c>
+      <c r="F33" s="4">
+        <v>14.47</v>
+      </c>
+      <c r="G33" s="4">
+        <v>4.3000999999999996</v>
+      </c>
+      <c r="H33" s="4">
+        <v>1000.8</v>
+      </c>
+      <c r="I33" s="4">
+        <v>1.3364</v>
+      </c>
+      <c r="J33" s="4">
+        <v>0.73826000000000003</v>
+      </c>
+      <c r="K33" s="4">
+        <v>6.1936999999999998</v>
+      </c>
+      <c r="L33" s="4">
+        <v>2.6962999999999999</v>
+      </c>
+      <c r="M33" s="4">
+        <v>0.35518</v>
+      </c>
+      <c r="N33" s="3">
+        <v>3.2061000000000002</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A34" s="13"/>
+      <c r="B34" s="16"/>
+      <c r="C34" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="D34" s="4">
+        <v>15.185</v>
+      </c>
+      <c r="E34" s="4">
+        <v>64.875</v>
+      </c>
+      <c r="F34" s="4">
+        <v>1.4525999999999999</v>
+      </c>
+      <c r="G34" s="4">
+        <v>3.2002999999999999</v>
+      </c>
+      <c r="H34" s="4">
+        <v>2110.6</v>
+      </c>
+      <c r="I34" s="4">
+        <v>1.7833000000000001</v>
+      </c>
+      <c r="J34" s="4">
+        <v>0.51853000000000005</v>
+      </c>
+      <c r="K34" s="4">
+        <v>4.2645</v>
+      </c>
+      <c r="L34" s="4">
+        <v>3.7526000000000002</v>
+      </c>
+      <c r="M34" s="4">
+        <v>0.20075000000000001</v>
+      </c>
+      <c r="N34" s="3">
+        <v>2.5205000000000002</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A35" s="13"/>
+      <c r="B35" s="16"/>
+      <c r="C35" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="D35" s="4">
+        <v>8.0571999999999999</v>
+      </c>
+      <c r="E35" s="4">
+        <v>29.803999999999998</v>
+      </c>
+      <c r="F35" s="4">
+        <v>2.5836000000000001</v>
+      </c>
+      <c r="G35" s="4">
+        <v>4.0204000000000004</v>
+      </c>
+      <c r="H35" s="4">
+        <v>1210.4000000000001</v>
+      </c>
+      <c r="I35" s="4">
+        <v>1.2011000000000001</v>
+      </c>
+      <c r="J35" s="4">
+        <v>0.49431999999999998</v>
+      </c>
+      <c r="K35" s="4">
+        <v>4.3479000000000001</v>
+      </c>
+      <c r="L35" s="4">
+        <v>2.7725</v>
+      </c>
+      <c r="M35" s="4">
+        <v>0.29389999999999999</v>
+      </c>
+      <c r="N35" s="3">
+        <v>2.7284999999999999</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A36" s="13"/>
+      <c r="B36" s="16"/>
+      <c r="C36" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="D36" s="4">
+        <v>7.5292000000000003</v>
+      </c>
+      <c r="E36" s="4">
+        <v>23.504999999999999</v>
+      </c>
+      <c r="F36" s="4">
+        <v>4.9898999999999996</v>
+      </c>
+      <c r="G36" s="4">
+        <v>3.8622999999999998</v>
+      </c>
+      <c r="H36" s="4">
+        <v>1369.1</v>
+      </c>
+      <c r="I36" s="4">
+        <v>1.9939</v>
+      </c>
+      <c r="J36" s="4">
+        <v>0.36113000000000001</v>
+      </c>
+      <c r="K36" s="4">
+        <v>3.2098</v>
+      </c>
+      <c r="L36" s="4">
+        <v>1.6549</v>
+      </c>
+      <c r="M36" s="4">
+        <v>0.25001000000000001</v>
+      </c>
+      <c r="N36" s="3">
+        <v>3.9885000000000002</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="14"/>
+      <c r="B37" s="17"/>
+      <c r="C37" s="7"/>
+      <c r="N37" s="6"/>
+      <c r="O37" s="11"/>
+    </row>
+    <row r="38" spans="1:15" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="12">
+        <v>900</v>
+      </c>
+      <c r="B38" s="15" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A39" s="13"/>
+      <c r="B39" s="16"/>
+      <c r="C39" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="D39" s="4">
+        <v>4.8238000000000003</v>
+      </c>
+      <c r="E39" s="4">
+        <v>378.86</v>
+      </c>
+      <c r="F39" s="4">
+        <v>0.14230000000000001</v>
+      </c>
+      <c r="G39" s="4">
+        <v>4.4020999999999999</v>
+      </c>
+      <c r="H39" s="4">
+        <v>1006.9</v>
+      </c>
+      <c r="I39" s="4">
+        <v>1.3282</v>
+      </c>
+      <c r="J39" s="4">
+        <v>0.54573000000000005</v>
+      </c>
+      <c r="K39" s="4">
+        <v>4.6946000000000003</v>
+      </c>
+      <c r="L39" s="4">
+        <v>3.1678999999999999</v>
+      </c>
+      <c r="M39" s="4">
+        <v>0.25372</v>
+      </c>
+      <c r="N39" s="3">
+        <v>2.5291999999999999</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A40" s="13"/>
+      <c r="B40" s="16"/>
+      <c r="C40" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="D40" s="4">
+        <v>7.1036999999999999</v>
+      </c>
+      <c r="E40" s="4">
+        <v>48.234999999999999</v>
+      </c>
+      <c r="F40" s="4">
+        <v>4.2972000000000001</v>
+      </c>
+      <c r="G40" s="4">
+        <v>3.4083999999999999</v>
+      </c>
+      <c r="H40" s="4">
+        <v>1829.9</v>
+      </c>
+      <c r="I40" s="2">
+        <v>1.3602000000000001</v>
+      </c>
+      <c r="J40" s="2">
+        <v>0.34182000000000001</v>
+      </c>
+      <c r="K40" s="2">
+        <v>3.1635</v>
+      </c>
+      <c r="L40" s="2">
+        <v>12.426</v>
+      </c>
+      <c r="M40" s="2">
+        <v>0.21156</v>
+      </c>
+      <c r="N40" s="2">
+        <v>3.3578000000000001</v>
+      </c>
+    </row>
+    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A41" s="13"/>
+      <c r="B41" s="16"/>
+      <c r="C41" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="D41" s="4">
+        <v>3.0461</v>
+      </c>
+      <c r="E41" s="4">
+        <v>19.608000000000001</v>
+      </c>
+      <c r="F41" s="4">
+        <v>32.420999999999999</v>
+      </c>
+      <c r="G41" s="4">
+        <v>3.2736000000000001</v>
+      </c>
+      <c r="H41" s="4">
+        <v>2022.3</v>
+      </c>
+      <c r="I41" s="2">
+        <v>1.9328000000000001</v>
+      </c>
+      <c r="J41" s="2">
+        <v>0.59299999999999997</v>
+      </c>
+      <c r="K41" s="2">
+        <v>4.7255000000000003</v>
+      </c>
+      <c r="L41" s="2">
+        <v>2.6515</v>
+      </c>
+      <c r="M41" s="2">
+        <v>0.25479000000000002</v>
+      </c>
+      <c r="N41" s="1">
+        <v>2.5724</v>
+      </c>
+    </row>
+    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A42" s="13"/>
+      <c r="B42" s="16"/>
+      <c r="C42" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="D42" s="4">
+        <v>4.6340000000000003</v>
+      </c>
+      <c r="E42" s="4">
+        <v>18.606999999999999</v>
+      </c>
+      <c r="F42" s="4">
+        <v>24.896000000000001</v>
+      </c>
+      <c r="G42" s="4">
+        <v>3.3435999999999999</v>
+      </c>
+      <c r="H42" s="4">
+        <v>1999.7</v>
+      </c>
+      <c r="I42" s="4">
+        <v>2.2488000000000001</v>
+      </c>
+      <c r="J42" s="4">
+        <v>0.27339999999999998</v>
+      </c>
+      <c r="K42" s="4">
+        <v>2.6326000000000001</v>
+      </c>
+      <c r="L42" s="4">
+        <v>4.8822000000000001</v>
+      </c>
+      <c r="M42" s="4">
+        <v>0.17643</v>
+      </c>
+      <c r="N42" s="3">
+        <v>2.3942000000000001</v>
+      </c>
+    </row>
+    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A43" s="13"/>
+      <c r="B43" s="16"/>
+      <c r="C43" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="D43" s="4">
+        <v>16.286999999999999</v>
+      </c>
+      <c r="E43" s="4">
+        <v>181.45</v>
+      </c>
+      <c r="F43" s="4">
+        <v>0.52517000000000003</v>
+      </c>
+      <c r="G43" s="4">
+        <v>3.0160999999999998</v>
+      </c>
+      <c r="H43" s="4">
+        <v>2606.1999999999998</v>
+      </c>
+      <c r="I43" s="4">
+        <v>7.6341000000000001</v>
+      </c>
+      <c r="J43" s="4">
+        <v>0.55245999999999995</v>
+      </c>
+      <c r="K43" s="4">
+        <v>7.7807000000000004</v>
+      </c>
+      <c r="L43" s="4">
+        <v>2.0291999999999999</v>
+      </c>
+      <c r="M43" s="4">
+        <v>0.31213000000000002</v>
+      </c>
+      <c r="N43" s="3">
+        <v>2.8618000000000001</v>
+      </c>
+    </row>
+    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A44" s="13"/>
+      <c r="B44" s="16"/>
+      <c r="C44" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="D44" s="4">
+        <v>9.5312999999999999</v>
+      </c>
+      <c r="E44" s="4">
+        <v>148.61000000000001</v>
+      </c>
+      <c r="F44" s="4">
+        <v>0.37484000000000001</v>
+      </c>
+      <c r="G44" s="4">
+        <v>3.9621</v>
+      </c>
+      <c r="H44" s="4">
+        <v>1253.9000000000001</v>
+      </c>
+      <c r="I44" s="4">
+        <v>2.3045</v>
+      </c>
+      <c r="J44" s="4">
+        <v>0.34014</v>
+      </c>
+      <c r="K44" s="4">
+        <v>3.0451000000000001</v>
+      </c>
+      <c r="L44" s="4">
+        <v>2.7208000000000001</v>
+      </c>
+      <c r="M44" s="4">
+        <v>6.7532999999999996E-2</v>
+      </c>
+      <c r="N44" s="3">
+        <v>2.4268999999999998</v>
+      </c>
+    </row>
+    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A45" s="13"/>
+      <c r="B45" s="16"/>
+      <c r="C45" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="D45" s="4">
+        <v>6.3647</v>
+      </c>
+      <c r="E45" s="4">
+        <v>149.54</v>
+      </c>
+      <c r="F45" s="4">
+        <v>0.43913000000000002</v>
+      </c>
+      <c r="G45" s="4">
+        <v>4.1839000000000004</v>
+      </c>
+      <c r="H45" s="4">
+        <v>1127.5999999999999</v>
+      </c>
+      <c r="I45" s="4">
+        <v>2.2016</v>
+      </c>
+      <c r="J45" s="4">
+        <v>0.28632000000000002</v>
+      </c>
+      <c r="K45" s="4">
+        <v>2.7416</v>
+      </c>
+      <c r="L45" s="4">
+        <v>1.1881999999999999</v>
+      </c>
+      <c r="M45" s="4">
+        <v>0.70389999999999997</v>
+      </c>
+      <c r="N45" s="3">
+        <v>8.2974999999999993E-2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A46" s="13"/>
+      <c r="B46" s="16"/>
+      <c r="C46" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="D46" s="4">
+        <v>12.622</v>
+      </c>
+      <c r="E46" s="4">
+        <v>15.441000000000001</v>
+      </c>
+      <c r="F46" s="4">
+        <v>4.5385999999999997</v>
+      </c>
+      <c r="G46" s="4">
+        <v>3.7305000000000001</v>
+      </c>
+      <c r="H46" s="4">
+        <v>1371.6</v>
+      </c>
+      <c r="I46" s="4">
+        <v>2.2448999999999999</v>
+      </c>
+      <c r="J46" s="4">
+        <v>0.40698000000000001</v>
+      </c>
+      <c r="K46" s="4">
+        <v>3.5036</v>
+      </c>
+      <c r="L46" s="4">
+        <v>4.0568</v>
+      </c>
+      <c r="M46" s="4">
+        <v>0.21132000000000001</v>
+      </c>
+      <c r="N46" s="3">
+        <v>2.4597000000000002</v>
+      </c>
+    </row>
+    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A47" s="13"/>
+      <c r="B47" s="16"/>
+      <c r="C47" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="D47" s="4">
+        <v>12.256</v>
+      </c>
+      <c r="E47" s="4">
+        <v>273.68</v>
+      </c>
+      <c r="F47" s="4">
+        <v>0.20866000000000001</v>
+      </c>
+      <c r="G47" s="4">
+        <v>3.8422000000000001</v>
+      </c>
+      <c r="H47" s="4">
+        <v>1242.3</v>
+      </c>
+      <c r="I47" s="4">
+        <v>1.8718999999999999</v>
+      </c>
+      <c r="J47" s="4">
+        <v>0.38352999999999998</v>
+      </c>
+      <c r="K47" s="4">
+        <v>3.4464999999999999</v>
+      </c>
+      <c r="L47" s="4">
+        <v>3.8252999999999999</v>
+      </c>
+      <c r="M47" s="4">
+        <v>0.19616</v>
+      </c>
+      <c r="N47" s="3">
+        <v>2.4363999999999999</v>
+      </c>
+    </row>
+    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A48" s="13"/>
+      <c r="B48" s="16"/>
+      <c r="C48" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="D48" s="4">
+        <v>7.0439999999999996</v>
+      </c>
+      <c r="E48" s="4">
+        <v>16.175000000000001</v>
+      </c>
+      <c r="F48" s="4">
+        <v>6.7949000000000002</v>
+      </c>
+      <c r="G48" s="4">
+        <v>4.1207000000000003</v>
+      </c>
+      <c r="H48" s="4">
+        <v>1090</v>
+      </c>
+      <c r="I48" s="4">
+        <v>2.2446999999999999</v>
+      </c>
+      <c r="J48" s="4">
+        <v>0.43214999999999998</v>
+      </c>
+      <c r="K48" s="4">
+        <v>3.6272000000000002</v>
+      </c>
+      <c r="L48" s="4">
+        <v>5.3937999999999997</v>
+      </c>
+      <c r="M48" s="4">
+        <v>0.16178999999999999</v>
+      </c>
+      <c r="N48" s="3">
+        <v>2.391</v>
+      </c>
+    </row>
+    <row r="49" spans="1:15" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="14"/>
+      <c r="B49" s="17"/>
+      <c r="C49" s="7"/>
+      <c r="N49" s="6"/>
+      <c r="O49" s="11"/>
+    </row>
+    <row r="50" spans="1:15" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="12">
+        <v>1000</v>
+      </c>
+      <c r="B50" s="15" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="51" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A51" s="13"/>
+      <c r="B51" s="16"/>
+    </row>
+    <row r="52" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A52" s="13"/>
+      <c r="B52" s="16"/>
+    </row>
+    <row r="53" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A53" s="13"/>
+      <c r="B53" s="16"/>
+    </row>
+    <row r="54" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A54" s="13"/>
+      <c r="B54" s="16"/>
+    </row>
+    <row r="55" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A55" s="13"/>
+      <c r="B55" s="16"/>
+    </row>
+    <row r="56" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A56" s="13"/>
+      <c r="B56" s="16"/>
+    </row>
+    <row r="57" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A57" s="13"/>
+      <c r="B57" s="16"/>
+    </row>
+    <row r="58" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A58" s="13"/>
+      <c r="B58" s="16"/>
+    </row>
+    <row r="59" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A59" s="13"/>
+      <c r="B59" s="16"/>
+    </row>
+    <row r="60" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A60" s="13"/>
+      <c r="B60" s="16"/>
+    </row>
+    <row r="61" spans="1:15" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="14"/>
+      <c r="B61" s="17"/>
+      <c r="C61" s="7"/>
+      <c r="N61" s="6"/>
+      <c r="O61" s="11"/>
+    </row>
+    <row r="62" spans="1:15" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="12">
+        <v>1000</v>
+      </c>
+      <c r="B62" s="15" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="63" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A63" s="13"/>
+      <c r="B63" s="16"/>
+    </row>
+    <row r="64" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A64" s="13"/>
+      <c r="B64" s="16"/>
+    </row>
+    <row r="65" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A65" s="13"/>
+      <c r="B65" s="16"/>
+    </row>
+    <row r="66" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A66" s="13"/>
+      <c r="B66" s="16"/>
+    </row>
+    <row r="67" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A67" s="13"/>
+      <c r="B67" s="16"/>
+    </row>
+    <row r="68" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A68" s="13"/>
+      <c r="B68" s="16"/>
+    </row>
+    <row r="69" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A69" s="13"/>
+      <c r="B69" s="16"/>
+    </row>
+    <row r="70" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A70" s="13"/>
+      <c r="B70" s="16"/>
+    </row>
+    <row r="71" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A71" s="13"/>
+      <c r="B71" s="16"/>
+    </row>
+    <row r="72" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A72" s="13"/>
+      <c r="B72" s="16"/>
+    </row>
+    <row r="73" spans="1:15" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A73" s="14"/>
+      <c r="B73" s="17"/>
+      <c r="C73" s="7"/>
+      <c r="N73" s="6"/>
+      <c r="O73" s="11"/>
+    </row>
+  </sheetData>
+  <mergeCells count="12">
     <mergeCell ref="A38:A49"/>
     <mergeCell ref="B38:B49"/>
     <mergeCell ref="A50:A61"/>
@@ -5114,13 +6969,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C18A26E-30CA-4E63-A18A-C9C101DAF33C}">
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F200E048-5FAF-4136-82F6-92204CC50E12}">
   <dimension ref="A1:O73"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C1" sqref="C1:C1048576"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="N51" sqref="N51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5142,7 +6997,7 @@
         <v>11</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D1" s="5" t="s">
         <v>1</v>
@@ -5190,402 +7045,48 @@
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="13"/>
       <c r="B3" s="16"/>
-      <c r="C3" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="D3" s="4">
-        <v>17.216999999999999</v>
-      </c>
-      <c r="E3" s="4">
-        <v>179.74</v>
-      </c>
-      <c r="F3" s="4">
-        <v>0.61753999999999998</v>
-      </c>
-      <c r="G3" s="4">
-        <v>4.4165999999999999</v>
-      </c>
-      <c r="H3" s="4">
-        <v>1783.5</v>
-      </c>
-      <c r="I3" s="2">
-        <v>1.0025999999999999</v>
-      </c>
-      <c r="J3" s="2">
-        <v>0.41060999999999998</v>
-      </c>
-      <c r="K3" s="2">
-        <v>4.2331000000000003</v>
-      </c>
-      <c r="L3" s="2">
-        <v>2.2349000000000001</v>
-      </c>
-      <c r="M3" s="2">
-        <v>0.29105999999999999</v>
-      </c>
-      <c r="N3" s="1">
-        <v>3.1743000000000001</v>
-      </c>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2"/>
+      <c r="N3" s="1"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="13"/>
       <c r="B4" s="16"/>
-      <c r="C4" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="D4" s="4">
-        <v>5.6908000000000003</v>
-      </c>
-      <c r="E4" s="4">
-        <v>66.626999999999995</v>
-      </c>
-      <c r="F4" s="4">
-        <v>1.9851000000000001</v>
-      </c>
-      <c r="G4" s="4">
-        <v>4.7723000000000004</v>
-      </c>
-      <c r="H4" s="4">
-        <v>1621.6</v>
-      </c>
-      <c r="I4" s="2">
-        <v>1.8904000000000001</v>
-      </c>
-      <c r="J4" s="2">
-        <v>0.54329000000000005</v>
-      </c>
-      <c r="K4" s="2">
-        <v>4.6087999999999996</v>
-      </c>
-      <c r="L4" s="2">
-        <v>1.8685</v>
-      </c>
-      <c r="M4" s="2">
-        <v>9.3698000000000004E-2</v>
-      </c>
-      <c r="N4" s="2">
-        <v>2.7471999999999999</v>
-      </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="13"/>
       <c r="B5" s="16"/>
-      <c r="C5" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="D5" s="4">
-        <v>9.3076000000000008</v>
-      </c>
-      <c r="E5" s="4">
-        <v>32.595999999999997</v>
-      </c>
-      <c r="F5" s="4">
-        <v>5.8113999999999999</v>
-      </c>
-      <c r="G5" s="4">
-        <v>4.5263</v>
-      </c>
-      <c r="H5" s="4">
-        <v>1775.9</v>
-      </c>
-      <c r="I5" s="2">
-        <v>1.8393999999999999</v>
-      </c>
-      <c r="J5" s="2">
-        <v>0.71550999999999998</v>
-      </c>
-      <c r="K5" s="2">
-        <v>5.8657000000000004</v>
-      </c>
-      <c r="L5" s="2">
-        <v>1.8920999999999999</v>
-      </c>
-      <c r="M5" s="2">
-        <v>0.34444000000000002</v>
-      </c>
-      <c r="N5" s="2">
-        <v>3.5432999999999999</v>
-      </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="13"/>
       <c r="B6" s="16"/>
-      <c r="C6" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="D6" s="4">
-        <v>5.8951000000000002</v>
-      </c>
-      <c r="E6" s="4">
-        <v>36.244999999999997</v>
-      </c>
-      <c r="F6" s="4">
-        <v>5.3757000000000001</v>
-      </c>
-      <c r="G6" s="4">
-        <v>4.7310999999999996</v>
-      </c>
-      <c r="H6" s="4">
-        <v>1598.4</v>
-      </c>
-      <c r="I6" s="4">
-        <v>2.4487000000000001</v>
-      </c>
-      <c r="J6" s="4">
-        <v>0.36314000000000002</v>
-      </c>
-      <c r="K6" s="4">
-        <v>3.4647000000000001</v>
-      </c>
-      <c r="L6" s="4">
-        <v>9.3416999999999994</v>
-      </c>
-      <c r="M6" s="4">
-        <v>0.10058</v>
-      </c>
-      <c r="N6" s="3">
-        <v>3.1581999999999999</v>
-      </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="13"/>
       <c r="B7" s="16"/>
-      <c r="C7" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="D7" s="2">
-        <v>4.1862000000000004</v>
-      </c>
-      <c r="E7" s="2">
-        <v>84.548000000000002</v>
-      </c>
-      <c r="F7" s="2">
-        <v>2.1122999999999998</v>
-      </c>
-      <c r="G7" s="2">
-        <v>4.7751999999999999</v>
-      </c>
-      <c r="H7" s="2">
-        <v>1574.3</v>
-      </c>
-      <c r="I7" s="2">
-        <v>1.6472</v>
-      </c>
-      <c r="J7" s="2">
-        <v>0.34209000000000001</v>
-      </c>
-      <c r="K7" s="2">
-        <v>3.5358000000000001</v>
-      </c>
-      <c r="L7" s="2">
-        <v>10.343</v>
-      </c>
-      <c r="M7" s="2">
-        <v>0.55237999999999998</v>
-      </c>
-      <c r="N7" s="2">
-        <v>2.4053</v>
-      </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="13"/>
       <c r="B8" s="16"/>
-      <c r="C8" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="D8" s="4">
-        <v>25.038</v>
-      </c>
-      <c r="E8" s="4">
-        <v>90.692999999999998</v>
-      </c>
-      <c r="F8" s="4">
-        <v>0.61002000000000001</v>
-      </c>
-      <c r="G8" s="4">
-        <v>4.1981999999999999</v>
-      </c>
-      <c r="H8" s="4">
-        <v>1944.6</v>
-      </c>
-      <c r="I8" s="4">
-        <v>1.3413999999999999</v>
-      </c>
-      <c r="J8" s="4">
-        <v>0.39294000000000001</v>
-      </c>
-      <c r="K8" s="4">
-        <v>3.9001000000000001</v>
-      </c>
-      <c r="L8" s="4">
-        <v>4.3860999999999999</v>
-      </c>
-      <c r="M8" s="4">
-        <v>0.24360999999999999</v>
-      </c>
-      <c r="N8" s="3">
-        <v>2.9091</v>
-      </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="13"/>
       <c r="B9" s="16"/>
-      <c r="C9" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="D9" s="4">
-        <v>27.547000000000001</v>
-      </c>
-      <c r="E9" s="4">
-        <v>78.081000000000003</v>
-      </c>
-      <c r="F9" s="4">
-        <v>0.84272999999999998</v>
-      </c>
-      <c r="G9" s="4">
-        <v>3.8992</v>
-      </c>
-      <c r="H9" s="4">
-        <v>2454.8000000000002</v>
-      </c>
-      <c r="I9" s="4">
-        <v>1.8298000000000001</v>
-      </c>
-      <c r="J9" s="4">
-        <v>0.44322</v>
-      </c>
-      <c r="K9" s="4">
-        <v>4.1135000000000002</v>
-      </c>
-      <c r="L9" s="4">
-        <v>4.6660000000000004</v>
-      </c>
-      <c r="M9" s="4">
-        <v>7.2484999999999994E-2</v>
-      </c>
-      <c r="N9" s="3">
-        <v>2.4855999999999998</v>
-      </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="13"/>
       <c r="B10" s="16"/>
-      <c r="C10" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="D10" s="4">
-        <v>27.885000000000002</v>
-      </c>
-      <c r="E10" s="4">
-        <v>124.89</v>
-      </c>
-      <c r="F10" s="4">
-        <v>0.65636000000000005</v>
-      </c>
-      <c r="G10" s="4">
-        <v>3.8874</v>
-      </c>
-      <c r="H10" s="4">
-        <v>2390.5</v>
-      </c>
-      <c r="I10" s="4">
-        <v>1.1933</v>
-      </c>
-      <c r="J10" s="4">
-        <v>0.18759999999999999</v>
-      </c>
-      <c r="K10" s="4">
-        <v>2.4325999999999999</v>
-      </c>
-      <c r="L10" s="4">
-        <v>2.4598</v>
-      </c>
-      <c r="M10" s="4">
-        <v>0.27822999999999998</v>
-      </c>
-      <c r="N10" s="3">
-        <v>3.0878999999999999</v>
-      </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="13"/>
       <c r="B11" s="16"/>
-      <c r="C11" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="D11" s="4">
-        <v>19.2</v>
-      </c>
-      <c r="E11" s="4">
-        <v>52.204000000000001</v>
-      </c>
-      <c r="F11" s="4">
-        <v>1.7579</v>
-      </c>
-      <c r="G11" s="4">
-        <v>4.5105000000000004</v>
-      </c>
-      <c r="H11" s="4">
-        <v>1614.6</v>
-      </c>
-      <c r="I11" s="4">
-        <v>1.0317000000000001</v>
-      </c>
-      <c r="J11" s="4">
-        <v>0.54349000000000003</v>
-      </c>
-      <c r="K11" s="4">
-        <v>5.2065000000000001</v>
-      </c>
-      <c r="L11" s="4">
-        <v>3.1556999999999999</v>
-      </c>
-      <c r="M11" s="4">
-        <v>0.27356999999999998</v>
-      </c>
-      <c r="N11" s="3">
-        <v>3.1248</v>
-      </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="13"/>
       <c r="B12" s="16"/>
-      <c r="C12" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="D12" s="4">
-        <v>8.5922999999999998</v>
-      </c>
-      <c r="E12" s="4">
-        <v>38.904000000000003</v>
-      </c>
-      <c r="F12" s="4">
-        <v>5.4828999999999999</v>
-      </c>
-      <c r="G12" s="4">
-        <v>4.4794999999999998</v>
-      </c>
-      <c r="H12" s="4">
-        <v>1841</v>
-      </c>
-      <c r="I12" s="4">
-        <v>2.2498</v>
-      </c>
-      <c r="J12" s="4">
-        <v>0.39954000000000001</v>
-      </c>
-      <c r="K12" s="4">
-        <v>3.722</v>
-      </c>
-      <c r="L12" s="4">
-        <v>4.2567000000000004</v>
-      </c>
-      <c r="M12" s="4">
-        <v>0.19838</v>
-      </c>
-      <c r="N12" s="3">
-        <v>3.5486</v>
-      </c>
     </row>
     <row r="13" spans="1:15" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="14"/>
@@ -5605,402 +7106,42 @@
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="13"/>
       <c r="B15" s="16"/>
-      <c r="C15" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="D15" s="4">
-        <v>31.327000000000002</v>
-      </c>
-      <c r="E15" s="4">
-        <v>104.92</v>
-      </c>
-      <c r="F15" s="4">
-        <v>0.8548</v>
-      </c>
-      <c r="G15" s="4">
-        <v>3.7507999999999999</v>
-      </c>
-      <c r="H15" s="4">
-        <v>2575.8000000000002</v>
-      </c>
-      <c r="I15" s="4">
-        <v>1.0368999999999999</v>
-      </c>
-      <c r="J15" s="4">
-        <v>0.33298</v>
-      </c>
-      <c r="K15" s="4">
-        <v>3.661</v>
-      </c>
-      <c r="L15" s="4">
-        <v>1.9359999999999999</v>
-      </c>
-      <c r="M15" s="4">
-        <v>0.26541999999999999</v>
-      </c>
-      <c r="N15" s="3">
-        <v>3.1442999999999999</v>
-      </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="13"/>
       <c r="B16" s="16"/>
-      <c r="C16" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="D16" s="4">
-        <v>22.393000000000001</v>
-      </c>
-      <c r="E16" s="4">
-        <v>462.57</v>
-      </c>
-      <c r="F16" s="4">
-        <v>0.13572999999999999</v>
-      </c>
-      <c r="G16" s="4">
-        <v>4.3140000000000001</v>
-      </c>
-      <c r="H16" s="4">
-        <v>1828.1</v>
-      </c>
-      <c r="I16" s="2">
-        <v>1.9733000000000001</v>
-      </c>
-      <c r="J16" s="2">
-        <v>0.27233000000000002</v>
-      </c>
-      <c r="K16" s="2">
-        <v>3.1234000000000002</v>
-      </c>
-      <c r="L16" s="2">
-        <v>2.0615999999999999</v>
-      </c>
-      <c r="M16" s="2">
-        <v>9.5870999999999994E-3</v>
-      </c>
-      <c r="N16" s="2">
-        <v>5.4309000000000003</v>
-      </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" s="13"/>
       <c r="B17" s="16"/>
-      <c r="C17" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="D17" s="4">
-        <v>11.45</v>
-      </c>
-      <c r="E17" s="4">
-        <v>53.151000000000003</v>
-      </c>
-      <c r="F17" s="4">
-        <v>7.1665999999999999</v>
-      </c>
-      <c r="G17" s="4">
-        <v>3.9502000000000002</v>
-      </c>
-      <c r="H17" s="4">
-        <v>2221.6</v>
-      </c>
-      <c r="I17" s="2">
-        <v>1.373</v>
-      </c>
-      <c r="J17" s="2">
-        <v>0.39922000000000002</v>
-      </c>
-      <c r="K17" s="2">
-        <v>3.891</v>
-      </c>
-      <c r="L17" s="2">
-        <v>3.8786999999999998</v>
-      </c>
-      <c r="M17" s="2">
-        <v>0.13688</v>
-      </c>
-      <c r="N17" s="2">
-        <v>2.6692999999999998</v>
-      </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" s="13"/>
       <c r="B18" s="16"/>
-      <c r="C18" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="D18" s="4">
-        <v>37.741999999999997</v>
-      </c>
-      <c r="E18" s="4">
-        <v>49.122999999999998</v>
-      </c>
-      <c r="F18" s="4">
-        <v>2.4996</v>
-      </c>
-      <c r="G18" s="4">
-        <v>3.4102000000000001</v>
-      </c>
-      <c r="H18" s="4">
-        <v>3172</v>
-      </c>
-      <c r="I18" s="4">
-        <v>1.0524</v>
-      </c>
-      <c r="J18" s="4">
-        <v>0.68115000000000003</v>
-      </c>
-      <c r="K18" s="4">
-        <v>6.5023999999999997</v>
-      </c>
-      <c r="L18" s="4">
-        <v>1.6215999999999999</v>
-      </c>
-      <c r="M18" s="4">
-        <v>0.19822000000000001</v>
-      </c>
-      <c r="N18" s="3">
-        <v>2.7772999999999999</v>
-      </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" s="13"/>
       <c r="B19" s="16"/>
-      <c r="C19" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="D19" s="4">
-        <v>18.768000000000001</v>
-      </c>
-      <c r="E19" s="4">
-        <v>89.18</v>
-      </c>
-      <c r="F19" s="4">
-        <v>0.88068999999999997</v>
-      </c>
-      <c r="G19" s="4">
-        <v>4.5054999999999996</v>
-      </c>
-      <c r="H19" s="4">
-        <v>1677.4</v>
-      </c>
-      <c r="I19" s="4">
-        <v>1.9628000000000001</v>
-      </c>
-      <c r="J19" s="4">
-        <v>0.35322999999999999</v>
-      </c>
-      <c r="K19" s="4">
-        <v>3.5571000000000002</v>
-      </c>
-      <c r="L19" s="4">
-        <v>4.0984999999999996</v>
-      </c>
-      <c r="M19" s="4">
-        <v>5.9319999999999998E-2</v>
-      </c>
-      <c r="N19" s="3">
-        <v>2.5131999999999999</v>
-      </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" s="13"/>
       <c r="B20" s="16"/>
-      <c r="C20" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="D20" s="4">
-        <v>23.303999999999998</v>
-      </c>
-      <c r="E20" s="4">
-        <v>306.58</v>
-      </c>
-      <c r="F20" s="4">
-        <v>0.32123000000000002</v>
-      </c>
-      <c r="G20" s="4">
-        <v>4.2591999999999999</v>
-      </c>
-      <c r="H20" s="4">
-        <v>1822.6</v>
-      </c>
-      <c r="I20" s="4">
-        <v>1.6464000000000001</v>
-      </c>
-      <c r="J20" s="4">
-        <v>0.23887</v>
-      </c>
-      <c r="K20" s="4">
-        <v>2.9979</v>
-      </c>
-      <c r="L20" s="4">
-        <v>4.1620999999999997</v>
-      </c>
-      <c r="M20" s="4">
-        <v>2.9884999999999998E-3</v>
-      </c>
-      <c r="N20" s="3">
-        <v>2.3424999999999998</v>
-      </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" s="13"/>
       <c r="B21" s="16"/>
-      <c r="C21" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="D21" s="4">
-        <v>31.137</v>
-      </c>
-      <c r="E21" s="4">
-        <v>31.413</v>
-      </c>
-      <c r="F21" s="4">
-        <v>4.6002999999999998</v>
-      </c>
-      <c r="G21" s="4">
-        <v>3.6958000000000002</v>
-      </c>
-      <c r="H21" s="4">
-        <v>2583</v>
-      </c>
-      <c r="I21" s="4">
-        <v>1.2944</v>
-      </c>
-      <c r="J21" s="4">
-        <v>0.36685000000000001</v>
-      </c>
-      <c r="K21" s="4">
-        <v>3.8721000000000001</v>
-      </c>
-      <c r="L21" s="4">
-        <v>2.0034000000000001</v>
-      </c>
-      <c r="M21" s="4">
-        <v>0.2167</v>
-      </c>
-      <c r="N21" s="3">
-        <v>2.8479999999999999</v>
-      </c>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" s="13"/>
       <c r="B22" s="16"/>
-      <c r="C22" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="D22" s="4">
-        <v>29.725999999999999</v>
-      </c>
-      <c r="E22" s="4">
-        <v>45.991</v>
-      </c>
-      <c r="F22" s="4">
-        <v>2.3174000000000001</v>
-      </c>
-      <c r="G22" s="4">
-        <v>3.9613</v>
-      </c>
-      <c r="H22" s="4">
-        <v>2101.3000000000002</v>
-      </c>
-      <c r="I22" s="4">
-        <v>1.617</v>
-      </c>
-      <c r="J22" s="4">
-        <v>0.27362999999999998</v>
-      </c>
-      <c r="K22" s="4">
-        <v>3.2206000000000001</v>
-      </c>
-      <c r="L22" s="4">
-        <v>5.6994999999999996</v>
-      </c>
-      <c r="M22" s="4">
-        <v>0.96150999999999998</v>
-      </c>
-      <c r="N22" s="3">
-        <v>3.9527000000000001</v>
-      </c>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" s="13"/>
       <c r="B23" s="16"/>
-      <c r="C23" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="D23" s="4">
-        <v>0.85682000000000003</v>
-      </c>
-      <c r="E23" s="4">
-        <v>42.524000000000001</v>
-      </c>
-      <c r="F23" s="4">
-        <v>9.6282999999999994</v>
-      </c>
-      <c r="G23" s="4">
-        <v>4.5033000000000003</v>
-      </c>
-      <c r="H23" s="4">
-        <v>1707</v>
-      </c>
-      <c r="I23" s="4">
-        <v>1.2393000000000001</v>
-      </c>
-      <c r="J23" s="4">
-        <v>0.28849000000000002</v>
-      </c>
-      <c r="K23" s="4">
-        <v>3.4293</v>
-      </c>
-      <c r="L23" s="4">
-        <v>3.0653999999999999</v>
-      </c>
-      <c r="M23" s="4">
-        <v>0.11899999999999999</v>
-      </c>
-      <c r="N23" s="3">
-        <v>2.6208</v>
-      </c>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" s="13"/>
       <c r="B24" s="16"/>
-      <c r="C24" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="D24" s="4">
-        <v>4.4611000000000001</v>
-      </c>
-      <c r="E24" s="4">
-        <v>35.628</v>
-      </c>
-      <c r="F24" s="4">
-        <v>31.021000000000001</v>
-      </c>
-      <c r="G24" s="4">
-        <v>3.6185999999999998</v>
-      </c>
-      <c r="H24" s="4">
-        <v>3016.2</v>
-      </c>
-      <c r="I24" s="4">
-        <v>9.5056999999999992</v>
-      </c>
-      <c r="J24" s="4">
-        <v>0.33045999999999998</v>
-      </c>
-      <c r="K24" s="4">
-        <v>3.327</v>
-      </c>
-      <c r="L24" s="4">
-        <v>4.6459000000000001</v>
-      </c>
-      <c r="M24" s="4">
-        <v>0.20498</v>
-      </c>
-      <c r="N24" s="3">
-        <v>2.7280000000000002</v>
-      </c>
     </row>
     <row r="25" spans="1:15" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="14"/>
@@ -6020,402 +7161,42 @@
     <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27" s="13"/>
       <c r="B27" s="16"/>
-      <c r="C27" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="D27" s="4">
-        <v>4.8710000000000004</v>
-      </c>
-      <c r="E27" s="4">
-        <v>11.518000000000001</v>
-      </c>
-      <c r="F27" s="4">
-        <v>7.0281000000000002</v>
-      </c>
-      <c r="G27" s="4">
-        <v>4.2420999999999998</v>
-      </c>
-      <c r="H27" s="4">
-        <v>1138.3</v>
-      </c>
-      <c r="I27" s="4">
-        <v>1.2072000000000001</v>
-      </c>
-      <c r="J27" s="4">
-        <v>0.44550000000000001</v>
-      </c>
-      <c r="K27" s="4">
-        <v>3.8687</v>
-      </c>
-      <c r="L27" s="4">
-        <v>3.6877</v>
-      </c>
-      <c r="M27" s="4">
-        <v>0.25385000000000002</v>
-      </c>
-      <c r="N27" s="3">
-        <v>2.5308000000000002</v>
-      </c>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28" s="13"/>
       <c r="B28" s="16"/>
-      <c r="C28" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="D28" s="4">
-        <v>10.692</v>
-      </c>
-      <c r="E28" s="4">
-        <v>29.068000000000001</v>
-      </c>
-      <c r="F28" s="4">
-        <v>2.9830999999999999</v>
-      </c>
-      <c r="G28" s="4">
-        <v>3.7277999999999998</v>
-      </c>
-      <c r="H28" s="4">
-        <v>1433.5</v>
-      </c>
-      <c r="I28" s="2">
-        <v>2.3410000000000002</v>
-      </c>
-      <c r="J28" s="2">
-        <v>0.39410000000000001</v>
-      </c>
-      <c r="K28" s="2">
-        <v>3.3374000000000001</v>
-      </c>
-      <c r="L28" s="2">
-        <v>5.6124999999999998</v>
-      </c>
-      <c r="M28" s="2">
-        <v>0.94169000000000003</v>
-      </c>
-      <c r="N28" s="2">
-        <v>3.4904999999999999</v>
-      </c>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29" s="13"/>
       <c r="B29" s="16"/>
-      <c r="C29" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="D29" s="4">
-        <v>11.2</v>
-      </c>
-      <c r="E29" s="4">
-        <v>24.262</v>
-      </c>
-      <c r="F29" s="4">
-        <v>2.2614999999999998</v>
-      </c>
-      <c r="G29" s="4">
-        <v>3.9651000000000001</v>
-      </c>
-      <c r="H29" s="4">
-        <v>1163</v>
-      </c>
-      <c r="I29" s="4">
-        <v>1.7908999999999999</v>
-      </c>
-      <c r="J29" s="4">
-        <v>0.45981</v>
-      </c>
-      <c r="K29" s="4">
-        <v>3.9491000000000001</v>
-      </c>
-      <c r="L29" s="4">
-        <v>3.3142</v>
-      </c>
-      <c r="M29" s="4">
-        <v>0.20016999999999999</v>
-      </c>
-      <c r="N29" s="3">
-        <v>2.4437000000000002</v>
-      </c>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30" s="13"/>
       <c r="B30" s="16"/>
-      <c r="C30" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="D30" s="4">
-        <v>11.208</v>
-      </c>
-      <c r="E30" s="4">
-        <v>16.738</v>
-      </c>
-      <c r="F30" s="4">
-        <v>5.9587000000000003</v>
-      </c>
-      <c r="G30" s="4">
-        <v>3.6377000000000002</v>
-      </c>
-      <c r="H30" s="4">
-        <v>1530.1</v>
-      </c>
-      <c r="I30" s="4">
-        <v>1.0164</v>
-      </c>
-      <c r="J30" s="4">
-        <v>0.51859999999999995</v>
-      </c>
-      <c r="K30" s="4">
-        <v>4.4584999999999999</v>
-      </c>
-      <c r="L30" s="4">
-        <v>3.1135000000000002</v>
-      </c>
-      <c r="M30" s="4">
-        <v>0.38601000000000002</v>
-      </c>
-      <c r="N30" s="3">
-        <v>3.3180999999999998</v>
-      </c>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A31" s="13"/>
       <c r="B31" s="16"/>
-      <c r="C31" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="D31" s="4">
-        <v>10.45</v>
-      </c>
-      <c r="E31" s="4">
-        <v>14.769</v>
-      </c>
-      <c r="F31" s="4">
-        <v>7.8792</v>
-      </c>
-      <c r="G31" s="4">
-        <v>3.54</v>
-      </c>
-      <c r="H31" s="4">
-        <v>1787.3</v>
-      </c>
-      <c r="I31" s="4">
-        <v>1.3337000000000001</v>
-      </c>
-      <c r="J31" s="4">
-        <v>0.59784999999999999</v>
-      </c>
-      <c r="K31" s="4">
-        <v>4.8552999999999997</v>
-      </c>
-      <c r="L31" s="4">
-        <v>2.6320000000000001</v>
-      </c>
-      <c r="M31" s="4">
-        <v>0.34475</v>
-      </c>
-      <c r="N31" s="3">
-        <v>3.0926</v>
-      </c>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A32" s="13"/>
       <c r="B32" s="16"/>
-      <c r="C32" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="D32" s="4">
-        <v>11.010999999999999</v>
-      </c>
-      <c r="E32" s="4">
-        <v>11.071</v>
-      </c>
-      <c r="F32" s="4">
-        <v>13.523</v>
-      </c>
-      <c r="G32" s="4">
-        <v>3.5672000000000001</v>
-      </c>
-      <c r="H32" s="4">
-        <v>1593.8</v>
-      </c>
-      <c r="I32" s="4">
-        <v>2.0019</v>
-      </c>
-      <c r="J32" s="4">
-        <v>0.50361</v>
-      </c>
-      <c r="K32" s="4">
-        <v>4.1786000000000003</v>
-      </c>
-      <c r="L32" s="4">
-        <v>4.2843</v>
-      </c>
-      <c r="M32" s="4">
-        <v>0.22523000000000001</v>
-      </c>
-      <c r="N32" s="3">
-        <v>2.6124999999999998</v>
-      </c>
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A33" s="13"/>
       <c r="B33" s="16"/>
-      <c r="C33" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="D33" s="4">
-        <v>5.6656000000000004</v>
-      </c>
-      <c r="E33" s="4">
-        <v>8.2222000000000008</v>
-      </c>
-      <c r="F33" s="4">
-        <v>14.47</v>
-      </c>
-      <c r="G33" s="4">
-        <v>4.3000999999999996</v>
-      </c>
-      <c r="H33" s="4">
-        <v>1000.8</v>
-      </c>
-      <c r="I33" s="4">
-        <v>1.3364</v>
-      </c>
-      <c r="J33" s="4">
-        <v>0.73826000000000003</v>
-      </c>
-      <c r="K33" s="4">
-        <v>6.1936999999999998</v>
-      </c>
-      <c r="L33" s="4">
-        <v>2.6962999999999999</v>
-      </c>
-      <c r="M33" s="4">
-        <v>0.35518</v>
-      </c>
-      <c r="N33" s="3">
-        <v>3.2061000000000002</v>
-      </c>
     </row>
     <row r="34" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A34" s="13"/>
       <c r="B34" s="16"/>
-      <c r="C34" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="D34" s="4">
-        <v>15.185</v>
-      </c>
-      <c r="E34" s="4">
-        <v>64.875</v>
-      </c>
-      <c r="F34" s="4">
-        <v>1.4525999999999999</v>
-      </c>
-      <c r="G34" s="4">
-        <v>3.2002999999999999</v>
-      </c>
-      <c r="H34" s="4">
-        <v>2110.6</v>
-      </c>
-      <c r="I34" s="4">
-        <v>1.7833000000000001</v>
-      </c>
-      <c r="J34" s="4">
-        <v>0.51853000000000005</v>
-      </c>
-      <c r="K34" s="4">
-        <v>4.2645</v>
-      </c>
-      <c r="L34" s="4">
-        <v>3.7526000000000002</v>
-      </c>
-      <c r="M34" s="4">
-        <v>0.20075000000000001</v>
-      </c>
-      <c r="N34" s="3">
-        <v>2.5205000000000002</v>
-      </c>
     </row>
     <row r="35" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A35" s="13"/>
       <c r="B35" s="16"/>
-      <c r="C35" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="D35" s="4">
-        <v>8.0571999999999999</v>
-      </c>
-      <c r="E35" s="4">
-        <v>29.803999999999998</v>
-      </c>
-      <c r="F35" s="4">
-        <v>2.5836000000000001</v>
-      </c>
-      <c r="G35" s="4">
-        <v>4.0204000000000004</v>
-      </c>
-      <c r="H35" s="4">
-        <v>1210.4000000000001</v>
-      </c>
-      <c r="I35" s="4">
-        <v>1.2011000000000001</v>
-      </c>
-      <c r="J35" s="4">
-        <v>0.49431999999999998</v>
-      </c>
-      <c r="K35" s="4">
-        <v>4.3479000000000001</v>
-      </c>
-      <c r="L35" s="4">
-        <v>2.7725</v>
-      </c>
-      <c r="M35" s="4">
-        <v>0.29389999999999999</v>
-      </c>
-      <c r="N35" s="3">
-        <v>2.7284999999999999</v>
-      </c>
     </row>
     <row r="36" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A36" s="13"/>
       <c r="B36" s="16"/>
-      <c r="C36" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="D36" s="4">
-        <v>7.5292000000000003</v>
-      </c>
-      <c r="E36" s="4">
-        <v>23.504999999999999</v>
-      </c>
-      <c r="F36" s="4">
-        <v>4.9898999999999996</v>
-      </c>
-      <c r="G36" s="4">
-        <v>3.8622999999999998</v>
-      </c>
-      <c r="H36" s="4">
-        <v>1369.1</v>
-      </c>
-      <c r="I36" s="4">
-        <v>1.9939</v>
-      </c>
-      <c r="J36" s="4">
-        <v>0.36113000000000001</v>
-      </c>
-      <c r="K36" s="4">
-        <v>3.2098</v>
-      </c>
-      <c r="L36" s="4">
-        <v>1.6549</v>
-      </c>
-      <c r="M36" s="4">
-        <v>0.25001000000000001</v>
-      </c>
-      <c r="N36" s="3">
-        <v>3.9885000000000002</v>
-      </c>
     </row>
     <row r="37" spans="1:15" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="14"/>
@@ -6435,402 +7216,84 @@
     <row r="39" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A39" s="13"/>
       <c r="B39" s="16"/>
-      <c r="C39" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="D39" s="4">
-        <v>4.8238000000000003</v>
-      </c>
-      <c r="E39" s="4">
-        <v>378.86</v>
-      </c>
-      <c r="F39" s="4">
-        <v>0.14230000000000001</v>
-      </c>
-      <c r="G39" s="4">
-        <v>4.4020999999999999</v>
-      </c>
-      <c r="H39" s="4">
-        <v>1006.9</v>
-      </c>
-      <c r="I39" s="4">
-        <v>1.3282</v>
-      </c>
-      <c r="J39" s="4">
-        <v>0.54573000000000005</v>
-      </c>
-      <c r="K39" s="4">
-        <v>4.6946000000000003</v>
-      </c>
-      <c r="L39" s="4">
-        <v>3.1678999999999999</v>
-      </c>
-      <c r="M39" s="4">
-        <v>0.25372</v>
-      </c>
-      <c r="N39" s="3">
-        <v>2.5291999999999999</v>
-      </c>
     </row>
     <row r="40" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A40" s="13"/>
       <c r="B40" s="16"/>
       <c r="C40" s="8" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="D40" s="4">
-        <v>7.1036999999999999</v>
+        <v>7.1031000000000004</v>
       </c>
       <c r="E40" s="4">
-        <v>48.234999999999999</v>
+        <v>56.988999999999997</v>
       </c>
       <c r="F40" s="4">
-        <v>4.2972000000000001</v>
+        <v>4.2892999999999999</v>
       </c>
       <c r="G40" s="4">
-        <v>3.4083999999999999</v>
+        <v>3.3986999999999998</v>
       </c>
       <c r="H40" s="4">
-        <v>1829.9</v>
-      </c>
-      <c r="I40" s="2">
-        <v>1.3602000000000001</v>
-      </c>
-      <c r="J40" s="2">
-        <v>0.34182000000000001</v>
-      </c>
-      <c r="K40" s="2">
-        <v>3.1635</v>
-      </c>
-      <c r="L40" s="2">
-        <v>12.426</v>
-      </c>
-      <c r="M40" s="2">
-        <v>0.21156</v>
-      </c>
-      <c r="N40" s="2">
-        <v>3.3578000000000001</v>
+        <v>1829.5</v>
+      </c>
+      <c r="I40" s="4">
+        <v>1.3612</v>
+      </c>
+      <c r="J40" s="4">
+        <v>0.34809000000000001</v>
+      </c>
+      <c r="K40" s="4">
+        <v>3.1223000000000001</v>
+      </c>
+      <c r="L40" s="4">
+        <v>12.302</v>
+      </c>
+      <c r="M40" s="4">
+        <v>0.21134</v>
+      </c>
+      <c r="N40" s="3">
+        <v>3.3576999999999999</v>
       </c>
     </row>
     <row r="41" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A41" s="13"/>
       <c r="B41" s="16"/>
-      <c r="C41" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="D41" s="4">
-        <v>3.0461</v>
-      </c>
-      <c r="E41" s="4">
-        <v>19.608000000000001</v>
-      </c>
-      <c r="F41" s="4">
-        <v>32.420999999999999</v>
-      </c>
-      <c r="G41" s="4">
-        <v>3.2736000000000001</v>
-      </c>
-      <c r="H41" s="4">
-        <v>2022.3</v>
-      </c>
-      <c r="I41" s="2">
-        <v>1.9328000000000001</v>
-      </c>
-      <c r="J41" s="2">
-        <v>0.59299999999999997</v>
-      </c>
-      <c r="K41" s="2">
-        <v>4.7255000000000003</v>
-      </c>
-      <c r="L41" s="2">
-        <v>2.6515</v>
-      </c>
-      <c r="M41" s="2">
-        <v>0.25479000000000002</v>
-      </c>
-      <c r="N41" s="1">
-        <v>2.5724</v>
-      </c>
+      <c r="I41" s="2"/>
+      <c r="J41" s="2"/>
+      <c r="K41" s="2"/>
+      <c r="L41" s="2"/>
+      <c r="M41" s="2"/>
+      <c r="N41" s="1"/>
     </row>
     <row r="42" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A42" s="13"/>
       <c r="B42" s="16"/>
-      <c r="C42" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="D42" s="4">
-        <v>4.6340000000000003</v>
-      </c>
-      <c r="E42" s="4">
-        <v>18.606999999999999</v>
-      </c>
-      <c r="F42" s="4">
-        <v>24.896000000000001</v>
-      </c>
-      <c r="G42" s="4">
-        <v>3.3435999999999999</v>
-      </c>
-      <c r="H42" s="4">
-        <v>1999.7</v>
-      </c>
-      <c r="I42" s="4">
-        <v>2.2488000000000001</v>
-      </c>
-      <c r="J42" s="4">
-        <v>0.27339999999999998</v>
-      </c>
-      <c r="K42" s="4">
-        <v>2.6326000000000001</v>
-      </c>
-      <c r="L42" s="4">
-        <v>4.8822000000000001</v>
-      </c>
-      <c r="M42" s="4">
-        <v>0.17643</v>
-      </c>
-      <c r="N42" s="3">
-        <v>2.3942000000000001</v>
-      </c>
     </row>
     <row r="43" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A43" s="13"/>
       <c r="B43" s="16"/>
-      <c r="C43" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="D43" s="4">
-        <v>16.286999999999999</v>
-      </c>
-      <c r="E43" s="4">
-        <v>181.45</v>
-      </c>
-      <c r="F43" s="4">
-        <v>0.52517000000000003</v>
-      </c>
-      <c r="G43" s="4">
-        <v>3.0160999999999998</v>
-      </c>
-      <c r="H43" s="4">
-        <v>2606.1999999999998</v>
-      </c>
-      <c r="I43" s="4">
-        <v>7.6341000000000001</v>
-      </c>
-      <c r="J43" s="4">
-        <v>0.55245999999999995</v>
-      </c>
-      <c r="K43" s="4">
-        <v>7.7807000000000004</v>
-      </c>
-      <c r="L43" s="4">
-        <v>2.0291999999999999</v>
-      </c>
-      <c r="M43" s="4">
-        <v>0.31213000000000002</v>
-      </c>
-      <c r="N43" s="3">
-        <v>2.8618000000000001</v>
-      </c>
     </row>
     <row r="44" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A44" s="13"/>
       <c r="B44" s="16"/>
-      <c r="C44" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="D44" s="4">
-        <v>9.5312999999999999</v>
-      </c>
-      <c r="E44" s="4">
-        <v>148.61000000000001</v>
-      </c>
-      <c r="F44" s="4">
-        <v>0.37484000000000001</v>
-      </c>
-      <c r="G44" s="4">
-        <v>3.9621</v>
-      </c>
-      <c r="H44" s="4">
-        <v>1253.9000000000001</v>
-      </c>
-      <c r="I44" s="4">
-        <v>2.3045</v>
-      </c>
-      <c r="J44" s="4">
-        <v>0.34014</v>
-      </c>
-      <c r="K44" s="4">
-        <v>3.0451000000000001</v>
-      </c>
-      <c r="L44" s="4">
-        <v>2.7208000000000001</v>
-      </c>
-      <c r="M44" s="4">
-        <v>6.7532999999999996E-2</v>
-      </c>
-      <c r="N44" s="3">
-        <v>2.4268999999999998</v>
-      </c>
     </row>
     <row r="45" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A45" s="13"/>
       <c r="B45" s="16"/>
-      <c r="C45" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="D45" s="4">
-        <v>6.3647</v>
-      </c>
-      <c r="E45" s="4">
-        <v>149.54</v>
-      </c>
-      <c r="F45" s="4">
-        <v>0.43913000000000002</v>
-      </c>
-      <c r="G45" s="4">
-        <v>4.1839000000000004</v>
-      </c>
-      <c r="H45" s="4">
-        <v>1127.5999999999999</v>
-      </c>
-      <c r="I45" s="4">
-        <v>2.2016</v>
-      </c>
-      <c r="J45" s="4">
-        <v>0.28632000000000002</v>
-      </c>
-      <c r="K45" s="4">
-        <v>2.7416</v>
-      </c>
-      <c r="L45" s="4">
-        <v>1.1881999999999999</v>
-      </c>
-      <c r="M45" s="4">
-        <v>0.70389999999999997</v>
-      </c>
-      <c r="N45" s="3">
-        <v>8.2974999999999993E-2</v>
-      </c>
     </row>
     <row r="46" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A46" s="13"/>
       <c r="B46" s="16"/>
-      <c r="C46" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="D46" s="4">
-        <v>12.622</v>
-      </c>
-      <c r="E46" s="4">
-        <v>15.441000000000001</v>
-      </c>
-      <c r="F46" s="4">
-        <v>4.5385999999999997</v>
-      </c>
-      <c r="G46" s="4">
-        <v>3.7305000000000001</v>
-      </c>
-      <c r="H46" s="4">
-        <v>1371.6</v>
-      </c>
-      <c r="I46" s="4">
-        <v>2.2448999999999999</v>
-      </c>
-      <c r="J46" s="4">
-        <v>0.40698000000000001</v>
-      </c>
-      <c r="K46" s="4">
-        <v>3.5036</v>
-      </c>
-      <c r="L46" s="4">
-        <v>4.0568</v>
-      </c>
-      <c r="M46" s="4">
-        <v>0.21132000000000001</v>
-      </c>
-      <c r="N46" s="3">
-        <v>2.4597000000000002</v>
-      </c>
     </row>
     <row r="47" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A47" s="13"/>
       <c r="B47" s="16"/>
-      <c r="C47" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="D47" s="4">
-        <v>12.256</v>
-      </c>
-      <c r="E47" s="4">
-        <v>273.68</v>
-      </c>
-      <c r="F47" s="4">
-        <v>0.20866000000000001</v>
-      </c>
-      <c r="G47" s="4">
-        <v>3.8422000000000001</v>
-      </c>
-      <c r="H47" s="4">
-        <v>1242.3</v>
-      </c>
-      <c r="I47" s="4">
-        <v>1.8718999999999999</v>
-      </c>
-      <c r="J47" s="4">
-        <v>0.38352999999999998</v>
-      </c>
-      <c r="K47" s="4">
-        <v>3.4464999999999999</v>
-      </c>
-      <c r="L47" s="4">
-        <v>3.8252999999999999</v>
-      </c>
-      <c r="M47" s="4">
-        <v>0.19616</v>
-      </c>
-      <c r="N47" s="3">
-        <v>2.4363999999999999</v>
-      </c>
     </row>
     <row r="48" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A48" s="13"/>
       <c r="B48" s="16"/>
-      <c r="C48" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="D48" s="4">
-        <v>7.0439999999999996</v>
-      </c>
-      <c r="E48" s="4">
-        <v>16.175000000000001</v>
-      </c>
-      <c r="F48" s="4">
-        <v>6.7949000000000002</v>
-      </c>
-      <c r="G48" s="4">
-        <v>4.1207000000000003</v>
-      </c>
-      <c r="H48" s="4">
-        <v>1090</v>
-      </c>
-      <c r="I48" s="4">
-        <v>2.2446999999999999</v>
-      </c>
-      <c r="J48" s="4">
-        <v>0.43214999999999998</v>
-      </c>
-      <c r="K48" s="4">
-        <v>3.6272000000000002</v>
-      </c>
-      <c r="L48" s="4">
-        <v>5.3937999999999997</v>
-      </c>
-      <c r="M48" s="4">
-        <v>0.16178999999999999</v>
-      </c>
-      <c r="N48" s="3">
-        <v>2.391</v>
-      </c>
     </row>
     <row r="49" spans="1:15" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="14"/>
@@ -6967,431 +7430,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F200E048-5FAF-4136-82F6-92204CC50E12}">
-  <dimension ref="A1:O73"/>
-  <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O1" sqref="O1:O1048576"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="9.140625" style="4"/>
-    <col min="2" max="2" width="9.140625" style="3"/>
-    <col min="3" max="3" width="15.7109375" style="8" customWidth="1"/>
-    <col min="4" max="13" width="9.140625" style="4"/>
-    <col min="14" max="14" width="9.140625" style="3"/>
-    <col min="15" max="15" width="9.140625" style="9"/>
-    <col min="16" max="16384" width="9.140625" style="4"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:15" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C1" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="H1" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="I1" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="J1" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="K1" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="L1" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="M1" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="N1" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="O1" s="11"/>
-    </row>
-    <row r="2" spans="1:15" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="12">
-        <v>800</v>
-      </c>
-      <c r="B2" s="15" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A3" s="13"/>
-      <c r="B3" s="16"/>
-      <c r="I3" s="2"/>
-      <c r="J3" s="2"/>
-      <c r="K3" s="2"/>
-      <c r="L3" s="2"/>
-      <c r="M3" s="2"/>
-      <c r="N3" s="1"/>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A4" s="13"/>
-      <c r="B4" s="16"/>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A5" s="13"/>
-      <c r="B5" s="16"/>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A6" s="13"/>
-      <c r="B6" s="16"/>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A7" s="13"/>
-      <c r="B7" s="16"/>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A8" s="13"/>
-      <c r="B8" s="16"/>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A9" s="13"/>
-      <c r="B9" s="16"/>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A10" s="13"/>
-      <c r="B10" s="16"/>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A11" s="13"/>
-      <c r="B11" s="16"/>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A12" s="13"/>
-      <c r="B12" s="16"/>
-    </row>
-    <row r="13" spans="1:15" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="14"/>
-      <c r="B13" s="17"/>
-      <c r="C13" s="7"/>
-      <c r="N13" s="6"/>
-      <c r="O13" s="11"/>
-    </row>
-    <row r="14" spans="1:15" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="12">
-        <v>800</v>
-      </c>
-      <c r="B14" s="15" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A15" s="13"/>
-      <c r="B15" s="16"/>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A16" s="13"/>
-      <c r="B16" s="16"/>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A17" s="13"/>
-      <c r="B17" s="16"/>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A18" s="13"/>
-      <c r="B18" s="16"/>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A19" s="13"/>
-      <c r="B19" s="16"/>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A20" s="13"/>
-      <c r="B20" s="16"/>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A21" s="13"/>
-      <c r="B21" s="16"/>
-    </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A22" s="13"/>
-      <c r="B22" s="16"/>
-    </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A23" s="13"/>
-      <c r="B23" s="16"/>
-    </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A24" s="13"/>
-      <c r="B24" s="16"/>
-    </row>
-    <row r="25" spans="1:15" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="14"/>
-      <c r="B25" s="17"/>
-      <c r="C25" s="7"/>
-      <c r="N25" s="6"/>
-      <c r="O25" s="11"/>
-    </row>
-    <row r="26" spans="1:15" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="12">
-        <v>900</v>
-      </c>
-      <c r="B26" s="15" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A27" s="13"/>
-      <c r="B27" s="16"/>
-    </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A28" s="13"/>
-      <c r="B28" s="16"/>
-    </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A29" s="13"/>
-      <c r="B29" s="16"/>
-    </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A30" s="13"/>
-      <c r="B30" s="16"/>
-    </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A31" s="13"/>
-      <c r="B31" s="16"/>
-    </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A32" s="13"/>
-      <c r="B32" s="16"/>
-    </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A33" s="13"/>
-      <c r="B33" s="16"/>
-    </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A34" s="13"/>
-      <c r="B34" s="16"/>
-    </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A35" s="13"/>
-      <c r="B35" s="16"/>
-    </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A36" s="13"/>
-      <c r="B36" s="16"/>
-    </row>
-    <row r="37" spans="1:15" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="14"/>
-      <c r="B37" s="17"/>
-      <c r="C37" s="7"/>
-      <c r="N37" s="6"/>
-      <c r="O37" s="11"/>
-    </row>
-    <row r="38" spans="1:15" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="12">
-        <v>900</v>
-      </c>
-      <c r="B38" s="15" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A39" s="13"/>
-      <c r="B39" s="16"/>
-    </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A40" s="13"/>
-      <c r="B40" s="16"/>
-    </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A41" s="13"/>
-      <c r="B41" s="16"/>
-      <c r="I41" s="2"/>
-      <c r="J41" s="2"/>
-      <c r="K41" s="2"/>
-      <c r="L41" s="2"/>
-      <c r="M41" s="2"/>
-      <c r="N41" s="1"/>
-    </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A42" s="13"/>
-      <c r="B42" s="16"/>
-    </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A43" s="13"/>
-      <c r="B43" s="16"/>
-    </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A44" s="13"/>
-      <c r="B44" s="16"/>
-    </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A45" s="13"/>
-      <c r="B45" s="16"/>
-    </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A46" s="13"/>
-      <c r="B46" s="16"/>
-    </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A47" s="13"/>
-      <c r="B47" s="16"/>
-    </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A48" s="13"/>
-      <c r="B48" s="16"/>
-    </row>
-    <row r="49" spans="1:15" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="14"/>
-      <c r="B49" s="17"/>
-      <c r="C49" s="7"/>
-      <c r="N49" s="6"/>
-      <c r="O49" s="11"/>
-    </row>
-    <row r="50" spans="1:15" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="12">
-        <v>1000</v>
-      </c>
-      <c r="B50" s="15" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="51" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A51" s="13"/>
-      <c r="B51" s="16"/>
-    </row>
-    <row r="52" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A52" s="13"/>
-      <c r="B52" s="16"/>
-    </row>
-    <row r="53" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A53" s="13"/>
-      <c r="B53" s="16"/>
-    </row>
-    <row r="54" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A54" s="13"/>
-      <c r="B54" s="16"/>
-    </row>
-    <row r="55" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A55" s="13"/>
-      <c r="B55" s="16"/>
-    </row>
-    <row r="56" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A56" s="13"/>
-      <c r="B56" s="16"/>
-    </row>
-    <row r="57" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A57" s="13"/>
-      <c r="B57" s="16"/>
-    </row>
-    <row r="58" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A58" s="13"/>
-      <c r="B58" s="16"/>
-    </row>
-    <row r="59" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A59" s="13"/>
-      <c r="B59" s="16"/>
-    </row>
-    <row r="60" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A60" s="13"/>
-      <c r="B60" s="16"/>
-    </row>
-    <row r="61" spans="1:15" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="14"/>
-      <c r="B61" s="17"/>
-      <c r="C61" s="7"/>
-      <c r="N61" s="6"/>
-      <c r="O61" s="11"/>
-    </row>
-    <row r="62" spans="1:15" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="12">
-        <v>1000</v>
-      </c>
-      <c r="B62" s="15" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="63" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A63" s="13"/>
-      <c r="B63" s="16"/>
-    </row>
-    <row r="64" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A64" s="13"/>
-      <c r="B64" s="16"/>
-    </row>
-    <row r="65" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A65" s="13"/>
-      <c r="B65" s="16"/>
-    </row>
-    <row r="66" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A66" s="13"/>
-      <c r="B66" s="16"/>
-    </row>
-    <row r="67" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A67" s="13"/>
-      <c r="B67" s="16"/>
-    </row>
-    <row r="68" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A68" s="13"/>
-      <c r="B68" s="16"/>
-    </row>
-    <row r="69" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A69" s="13"/>
-      <c r="B69" s="16"/>
-    </row>
-    <row r="70" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A70" s="13"/>
-      <c r="B70" s="16"/>
-    </row>
-    <row r="71" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A71" s="13"/>
-      <c r="B71" s="16"/>
-    </row>
-    <row r="72" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A72" s="13"/>
-      <c r="B72" s="16"/>
-    </row>
-    <row r="73" spans="1:15" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="14"/>
-      <c r="B73" s="17"/>
-      <c r="C73" s="7"/>
-      <c r="N73" s="6"/>
-      <c r="O73" s="11"/>
-    </row>
-  </sheetData>
-  <mergeCells count="12">
-    <mergeCell ref="A38:A49"/>
-    <mergeCell ref="B38:B49"/>
-    <mergeCell ref="A50:A61"/>
-    <mergeCell ref="B50:B61"/>
-    <mergeCell ref="A62:A73"/>
-    <mergeCell ref="B62:B73"/>
-    <mergeCell ref="A2:A13"/>
-    <mergeCell ref="B2:B13"/>
-    <mergeCell ref="A14:A25"/>
-    <mergeCell ref="B14:B25"/>
-    <mergeCell ref="A26:A37"/>
-    <mergeCell ref="B26:B37"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Removed some unnecessary helper plotting scripts and improved the critical work plotting script; also added another rejection criterion for the EVPWD model
</commit_message>
<xml_diff>
--- a/scripts/__other__/__sem__.xlsx
+++ b/scripts/__other__/__sem__.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27126"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Janzen\Desktop\code\moga_neml\scripts\__other__\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3016A677-967C-42D1-8E00-6534D90ED773}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C91F9074-ECDE-4F80-8772-7B28635C7D1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,6 +18,7 @@
     <sheet name="evp-cd_i" sheetId="17" r:id="rId3"/>
     <sheet name="evp-wd_f" sheetId="15" r:id="rId4"/>
     <sheet name="evp-wd_i" sheetId="18" r:id="rId5"/>
+    <sheet name="evp-wd_f (old)" sheetId="19" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="373" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="47">
   <si>
     <t>temp</t>
   </si>
@@ -2138,18 +2139,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A2:A13"/>
+    <mergeCell ref="B2:B13"/>
+    <mergeCell ref="A14:A25"/>
+    <mergeCell ref="B14:B25"/>
+    <mergeCell ref="A26:A37"/>
+    <mergeCell ref="B26:B37"/>
     <mergeCell ref="A38:A49"/>
     <mergeCell ref="B38:B49"/>
     <mergeCell ref="A50:A61"/>
     <mergeCell ref="B50:B61"/>
     <mergeCell ref="A62:A73"/>
     <mergeCell ref="B62:B73"/>
-    <mergeCell ref="A2:A13"/>
-    <mergeCell ref="B2:B13"/>
-    <mergeCell ref="A14:A25"/>
-    <mergeCell ref="B14:B25"/>
-    <mergeCell ref="A26:A37"/>
-    <mergeCell ref="B26:B37"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -3617,18 +3618,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A2:A13"/>
+    <mergeCell ref="B2:B13"/>
+    <mergeCell ref="A14:A25"/>
+    <mergeCell ref="B14:B25"/>
+    <mergeCell ref="A26:A37"/>
+    <mergeCell ref="B26:B37"/>
     <mergeCell ref="A38:A49"/>
     <mergeCell ref="B38:B49"/>
     <mergeCell ref="A50:A61"/>
     <mergeCell ref="B50:B61"/>
     <mergeCell ref="A62:A73"/>
     <mergeCell ref="B62:B73"/>
-    <mergeCell ref="A2:A13"/>
-    <mergeCell ref="B2:B13"/>
-    <mergeCell ref="A14:A25"/>
-    <mergeCell ref="B14:B25"/>
-    <mergeCell ref="A26:A37"/>
-    <mergeCell ref="B26:B37"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -5096,6 +5097,480 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A38:A49"/>
+    <mergeCell ref="B38:B49"/>
+    <mergeCell ref="A50:A61"/>
+    <mergeCell ref="B50:B61"/>
+    <mergeCell ref="A62:A73"/>
+    <mergeCell ref="B62:B73"/>
+    <mergeCell ref="A2:A13"/>
+    <mergeCell ref="B2:B13"/>
+    <mergeCell ref="A14:A25"/>
+    <mergeCell ref="B14:B25"/>
+    <mergeCell ref="A26:A37"/>
+    <mergeCell ref="B26:B37"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C18A26E-30CA-4E63-A18A-C9C101DAF33C}">
+  <dimension ref="A1:O73"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="N56" sqref="N56"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="4"/>
+    <col min="2" max="2" width="9.140625" style="3"/>
+    <col min="3" max="3" width="15.7109375" style="8" customWidth="1"/>
+    <col min="4" max="13" width="9.140625" style="4"/>
+    <col min="14" max="14" width="9.140625" style="3"/>
+    <col min="15" max="15" width="9.140625" style="9"/>
+    <col min="16" max="16384" width="9.140625" style="4"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="L1" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="M1" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="N1" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="O1" s="11"/>
+    </row>
+    <row r="2" spans="1:15" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="12">
+        <v>800</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3" s="13"/>
+      <c r="B3" s="16"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2"/>
+      <c r="N3" s="1"/>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4" s="13"/>
+      <c r="B4" s="16"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
+      <c r="L4" s="2"/>
+      <c r="M4" s="2"/>
+      <c r="N4" s="2"/>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5" s="13"/>
+      <c r="B5" s="16"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2"/>
+      <c r="L5" s="2"/>
+      <c r="M5" s="2"/>
+      <c r="N5" s="2"/>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6" s="13"/>
+      <c r="B6" s="16"/>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A7" s="13"/>
+      <c r="B7" s="16"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="2"/>
+      <c r="L7" s="2"/>
+      <c r="M7" s="2"/>
+      <c r="N7" s="2"/>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A8" s="13"/>
+      <c r="B8" s="16"/>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A9" s="13"/>
+      <c r="B9" s="16"/>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A10" s="13"/>
+      <c r="B10" s="16"/>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A11" s="13"/>
+      <c r="B11" s="16"/>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A12" s="13"/>
+      <c r="B12" s="16"/>
+    </row>
+    <row r="13" spans="1:15" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="14"/>
+      <c r="B13" s="17"/>
+      <c r="C13" s="7"/>
+      <c r="N13" s="6"/>
+      <c r="O13" s="11"/>
+    </row>
+    <row r="14" spans="1:15" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="12">
+        <v>800</v>
+      </c>
+      <c r="B14" s="15" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A15" s="13"/>
+      <c r="B15" s="16"/>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A16" s="13"/>
+      <c r="B16" s="16"/>
+      <c r="I16" s="2"/>
+      <c r="J16" s="2"/>
+      <c r="K16" s="2"/>
+      <c r="L16" s="2"/>
+      <c r="M16" s="2"/>
+      <c r="N16" s="2"/>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A17" s="13"/>
+      <c r="B17" s="16"/>
+      <c r="I17" s="2"/>
+      <c r="J17" s="2"/>
+      <c r="K17" s="2"/>
+      <c r="L17" s="2"/>
+      <c r="M17" s="2"/>
+      <c r="N17" s="2"/>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A18" s="13"/>
+      <c r="B18" s="16"/>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A19" s="13"/>
+      <c r="B19" s="16"/>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A20" s="13"/>
+      <c r="B20" s="16"/>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A21" s="13"/>
+      <c r="B21" s="16"/>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A22" s="13"/>
+      <c r="B22" s="16"/>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A23" s="13"/>
+      <c r="B23" s="16"/>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A24" s="13"/>
+      <c r="B24" s="16"/>
+    </row>
+    <row r="25" spans="1:15" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="14"/>
+      <c r="B25" s="17"/>
+      <c r="C25" s="7"/>
+      <c r="N25" s="6"/>
+      <c r="O25" s="11"/>
+    </row>
+    <row r="26" spans="1:15" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="12">
+        <v>900</v>
+      </c>
+      <c r="B26" s="15" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A27" s="13"/>
+      <c r="B27" s="16"/>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A28" s="13"/>
+      <c r="B28" s="16"/>
+      <c r="I28" s="2"/>
+      <c r="J28" s="2"/>
+      <c r="K28" s="2"/>
+      <c r="L28" s="2"/>
+      <c r="M28" s="2"/>
+      <c r="N28" s="2"/>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A29" s="13"/>
+      <c r="B29" s="16"/>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A30" s="13"/>
+      <c r="B30" s="16"/>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A31" s="13"/>
+      <c r="B31" s="16"/>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A32" s="13"/>
+      <c r="B32" s="16"/>
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A33" s="13"/>
+      <c r="B33" s="16"/>
+    </row>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A34" s="13"/>
+      <c r="B34" s="16"/>
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A35" s="13"/>
+      <c r="B35" s="16"/>
+    </row>
+    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A36" s="13"/>
+      <c r="B36" s="16"/>
+    </row>
+    <row r="37" spans="1:15" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="14"/>
+      <c r="B37" s="17"/>
+      <c r="C37" s="7"/>
+      <c r="N37" s="6"/>
+      <c r="O37" s="11"/>
+    </row>
+    <row r="38" spans="1:15" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="12">
+        <v>900</v>
+      </c>
+      <c r="B38" s="15" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A39" s="13"/>
+      <c r="B39" s="16"/>
+    </row>
+    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A40" s="13"/>
+      <c r="B40" s="16"/>
+      <c r="I40" s="2"/>
+      <c r="J40" s="2"/>
+      <c r="K40" s="2"/>
+      <c r="L40" s="2"/>
+      <c r="M40" s="2"/>
+      <c r="N40" s="2"/>
+    </row>
+    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A41" s="13"/>
+      <c r="B41" s="16"/>
+      <c r="I41" s="2"/>
+      <c r="J41" s="2"/>
+      <c r="K41" s="2"/>
+      <c r="L41" s="2"/>
+      <c r="M41" s="2"/>
+      <c r="N41" s="1"/>
+    </row>
+    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A42" s="13"/>
+      <c r="B42" s="16"/>
+    </row>
+    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A43" s="13"/>
+      <c r="B43" s="16"/>
+    </row>
+    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A44" s="13"/>
+      <c r="B44" s="16"/>
+    </row>
+    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A45" s="13"/>
+      <c r="B45" s="16"/>
+    </row>
+    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A46" s="13"/>
+      <c r="B46" s="16"/>
+    </row>
+    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A47" s="13"/>
+      <c r="B47" s="16"/>
+    </row>
+    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A48" s="13"/>
+      <c r="B48" s="16"/>
+    </row>
+    <row r="49" spans="1:15" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="14"/>
+      <c r="B49" s="17"/>
+      <c r="C49" s="7"/>
+      <c r="N49" s="6"/>
+      <c r="O49" s="11"/>
+    </row>
+    <row r="50" spans="1:15" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="12">
+        <v>1000</v>
+      </c>
+      <c r="B50" s="15" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="51" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A51" s="13"/>
+      <c r="B51" s="16"/>
+    </row>
+    <row r="52" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A52" s="13"/>
+      <c r="B52" s="16"/>
+    </row>
+    <row r="53" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A53" s="13"/>
+      <c r="B53" s="16"/>
+    </row>
+    <row r="54" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A54" s="13"/>
+      <c r="B54" s="16"/>
+    </row>
+    <row r="55" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A55" s="13"/>
+      <c r="B55" s="16"/>
+    </row>
+    <row r="56" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A56" s="13"/>
+      <c r="B56" s="16"/>
+    </row>
+    <row r="57" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A57" s="13"/>
+      <c r="B57" s="16"/>
+    </row>
+    <row r="58" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A58" s="13"/>
+      <c r="B58" s="16"/>
+    </row>
+    <row r="59" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A59" s="13"/>
+      <c r="B59" s="16"/>
+    </row>
+    <row r="60" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A60" s="13"/>
+      <c r="B60" s="16"/>
+    </row>
+    <row r="61" spans="1:15" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="14"/>
+      <c r="B61" s="17"/>
+      <c r="C61" s="7"/>
+      <c r="N61" s="6"/>
+      <c r="O61" s="11"/>
+    </row>
+    <row r="62" spans="1:15" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="12">
+        <v>1000</v>
+      </c>
+      <c r="B62" s="15" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="63" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A63" s="13"/>
+      <c r="B63" s="16"/>
+    </row>
+    <row r="64" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A64" s="13"/>
+      <c r="B64" s="16"/>
+    </row>
+    <row r="65" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A65" s="13"/>
+      <c r="B65" s="16"/>
+    </row>
+    <row r="66" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A66" s="13"/>
+      <c r="B66" s="16"/>
+    </row>
+    <row r="67" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A67" s="13"/>
+      <c r="B67" s="16"/>
+    </row>
+    <row r="68" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A68" s="13"/>
+      <c r="B68" s="16"/>
+    </row>
+    <row r="69" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A69" s="13"/>
+      <c r="B69" s="16"/>
+    </row>
+    <row r="70" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A70" s="13"/>
+      <c r="B70" s="16"/>
+    </row>
+    <row r="71" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A71" s="13"/>
+      <c r="B71" s="16"/>
+    </row>
+    <row r="72" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A72" s="13"/>
+      <c r="B72" s="16"/>
+    </row>
+    <row r="73" spans="1:15" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A73" s="14"/>
+      <c r="B73" s="17"/>
+      <c r="C73" s="7"/>
+      <c r="N73" s="6"/>
+      <c r="O73" s="11"/>
+    </row>
+  </sheetData>
+  <mergeCells count="12">
     <mergeCell ref="A2:A13"/>
     <mergeCell ref="B2:B13"/>
     <mergeCell ref="A14:A25"/>
@@ -5114,13 +5589,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C18A26E-30CA-4E63-A18A-C9C101DAF33C}">
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F200E048-5FAF-4136-82F6-92204CC50E12}">
   <dimension ref="A1:O73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L1" sqref="L1:L1048576"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H53" sqref="H53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5142,7 +5617,7 @@
         <v>11</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D1" s="5" t="s">
         <v>1</v>
@@ -5190,402 +5665,48 @@
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="13"/>
       <c r="B3" s="16"/>
-      <c r="C3" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="D3" s="4">
-        <v>17.216999999999999</v>
-      </c>
-      <c r="E3" s="4">
-        <v>179.74</v>
-      </c>
-      <c r="F3" s="4">
-        <v>0.61753999999999998</v>
-      </c>
-      <c r="G3" s="4">
-        <v>4.4165999999999999</v>
-      </c>
-      <c r="H3" s="4">
-        <v>1783.5</v>
-      </c>
-      <c r="I3" s="2">
-        <v>1.0025999999999999</v>
-      </c>
-      <c r="J3" s="2">
-        <v>0.41060999999999998</v>
-      </c>
-      <c r="K3" s="2">
-        <v>4.2331000000000003</v>
-      </c>
-      <c r="L3" s="2">
-        <v>2.2349000000000001</v>
-      </c>
-      <c r="M3" s="2">
-        <v>0.29105999999999999</v>
-      </c>
-      <c r="N3" s="1">
-        <v>3.1743000000000001</v>
-      </c>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2"/>
+      <c r="N3" s="1"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="13"/>
       <c r="B4" s="16"/>
-      <c r="C4" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="D4" s="4">
-        <v>5.6908000000000003</v>
-      </c>
-      <c r="E4" s="4">
-        <v>66.626999999999995</v>
-      </c>
-      <c r="F4" s="4">
-        <v>1.9851000000000001</v>
-      </c>
-      <c r="G4" s="4">
-        <v>4.7723000000000004</v>
-      </c>
-      <c r="H4" s="4">
-        <v>1621.6</v>
-      </c>
-      <c r="I4" s="2">
-        <v>1.8904000000000001</v>
-      </c>
-      <c r="J4" s="2">
-        <v>0.54329000000000005</v>
-      </c>
-      <c r="K4" s="2">
-        <v>4.6087999999999996</v>
-      </c>
-      <c r="L4" s="2">
-        <v>1.8685</v>
-      </c>
-      <c r="M4" s="2">
-        <v>9.3698000000000004E-2</v>
-      </c>
-      <c r="N4" s="2">
-        <v>2.7471999999999999</v>
-      </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="13"/>
       <c r="B5" s="16"/>
-      <c r="C5" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="D5" s="4">
-        <v>9.3076000000000008</v>
-      </c>
-      <c r="E5" s="4">
-        <v>32.595999999999997</v>
-      </c>
-      <c r="F5" s="4">
-        <v>5.8113999999999999</v>
-      </c>
-      <c r="G5" s="4">
-        <v>4.5263</v>
-      </c>
-      <c r="H5" s="4">
-        <v>1775.9</v>
-      </c>
-      <c r="I5" s="2">
-        <v>1.8393999999999999</v>
-      </c>
-      <c r="J5" s="2">
-        <v>0.71550999999999998</v>
-      </c>
-      <c r="K5" s="2">
-        <v>5.8657000000000004</v>
-      </c>
-      <c r="L5" s="2">
-        <v>1.8920999999999999</v>
-      </c>
-      <c r="M5" s="2">
-        <v>0.34444000000000002</v>
-      </c>
-      <c r="N5" s="2">
-        <v>3.5432999999999999</v>
-      </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="13"/>
       <c r="B6" s="16"/>
-      <c r="C6" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="D6" s="4">
-        <v>5.8951000000000002</v>
-      </c>
-      <c r="E6" s="4">
-        <v>36.244999999999997</v>
-      </c>
-      <c r="F6" s="4">
-        <v>5.3757000000000001</v>
-      </c>
-      <c r="G6" s="4">
-        <v>4.7310999999999996</v>
-      </c>
-      <c r="H6" s="4">
-        <v>1598.4</v>
-      </c>
-      <c r="I6" s="4">
-        <v>2.4487000000000001</v>
-      </c>
-      <c r="J6" s="4">
-        <v>0.36314000000000002</v>
-      </c>
-      <c r="K6" s="4">
-        <v>3.4647000000000001</v>
-      </c>
-      <c r="L6" s="4">
-        <v>9.3416999999999994</v>
-      </c>
-      <c r="M6" s="4">
-        <v>0.10058</v>
-      </c>
-      <c r="N6" s="3">
-        <v>3.1581999999999999</v>
-      </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="13"/>
       <c r="B7" s="16"/>
-      <c r="C7" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="D7" s="2">
-        <v>4.1862000000000004</v>
-      </c>
-      <c r="E7" s="2">
-        <v>84.548000000000002</v>
-      </c>
-      <c r="F7" s="2">
-        <v>2.1122999999999998</v>
-      </c>
-      <c r="G7" s="2">
-        <v>4.7751999999999999</v>
-      </c>
-      <c r="H7" s="2">
-        <v>1574.3</v>
-      </c>
-      <c r="I7" s="2">
-        <v>1.6472</v>
-      </c>
-      <c r="J7" s="2">
-        <v>0.34209000000000001</v>
-      </c>
-      <c r="K7" s="2">
-        <v>3.5358000000000001</v>
-      </c>
-      <c r="L7" s="2">
-        <v>10.343</v>
-      </c>
-      <c r="M7" s="2">
-        <v>0.55237999999999998</v>
-      </c>
-      <c r="N7" s="2">
-        <v>2.4053</v>
-      </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="13"/>
       <c r="B8" s="16"/>
-      <c r="C8" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="D8" s="4">
-        <v>25.038</v>
-      </c>
-      <c r="E8" s="4">
-        <v>90.692999999999998</v>
-      </c>
-      <c r="F8" s="4">
-        <v>0.61002000000000001</v>
-      </c>
-      <c r="G8" s="4">
-        <v>4.1981999999999999</v>
-      </c>
-      <c r="H8" s="4">
-        <v>1944.6</v>
-      </c>
-      <c r="I8" s="4">
-        <v>1.3413999999999999</v>
-      </c>
-      <c r="J8" s="4">
-        <v>0.39294000000000001</v>
-      </c>
-      <c r="K8" s="4">
-        <v>3.9001000000000001</v>
-      </c>
-      <c r="L8" s="4">
-        <v>4.3860999999999999</v>
-      </c>
-      <c r="M8" s="4">
-        <v>0.24360999999999999</v>
-      </c>
-      <c r="N8" s="3">
-        <v>2.9091</v>
-      </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="13"/>
       <c r="B9" s="16"/>
-      <c r="C9" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="D9" s="4">
-        <v>27.547000000000001</v>
-      </c>
-      <c r="E9" s="4">
-        <v>78.081000000000003</v>
-      </c>
-      <c r="F9" s="4">
-        <v>0.84272999999999998</v>
-      </c>
-      <c r="G9" s="4">
-        <v>3.8992</v>
-      </c>
-      <c r="H9" s="4">
-        <v>2454.8000000000002</v>
-      </c>
-      <c r="I9" s="4">
-        <v>1.8298000000000001</v>
-      </c>
-      <c r="J9" s="4">
-        <v>0.44322</v>
-      </c>
-      <c r="K9" s="4">
-        <v>4.1135000000000002</v>
-      </c>
-      <c r="L9" s="4">
-        <v>4.6660000000000004</v>
-      </c>
-      <c r="M9" s="4">
-        <v>7.2484999999999994E-2</v>
-      </c>
-      <c r="N9" s="3">
-        <v>2.4855999999999998</v>
-      </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="13"/>
       <c r="B10" s="16"/>
-      <c r="C10" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="D10" s="4">
-        <v>27.885000000000002</v>
-      </c>
-      <c r="E10" s="4">
-        <v>124.89</v>
-      </c>
-      <c r="F10" s="4">
-        <v>0.65636000000000005</v>
-      </c>
-      <c r="G10" s="4">
-        <v>3.8874</v>
-      </c>
-      <c r="H10" s="4">
-        <v>2390.5</v>
-      </c>
-      <c r="I10" s="4">
-        <v>1.1933</v>
-      </c>
-      <c r="J10" s="4">
-        <v>0.18759999999999999</v>
-      </c>
-      <c r="K10" s="4">
-        <v>2.4325999999999999</v>
-      </c>
-      <c r="L10" s="4">
-        <v>2.4598</v>
-      </c>
-      <c r="M10" s="4">
-        <v>0.27822999999999998</v>
-      </c>
-      <c r="N10" s="3">
-        <v>3.0878999999999999</v>
-      </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="13"/>
       <c r="B11" s="16"/>
-      <c r="C11" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="D11" s="4">
-        <v>19.2</v>
-      </c>
-      <c r="E11" s="4">
-        <v>52.204000000000001</v>
-      </c>
-      <c r="F11" s="4">
-        <v>1.7579</v>
-      </c>
-      <c r="G11" s="4">
-        <v>4.5105000000000004</v>
-      </c>
-      <c r="H11" s="4">
-        <v>1614.6</v>
-      </c>
-      <c r="I11" s="4">
-        <v>1.0317000000000001</v>
-      </c>
-      <c r="J11" s="4">
-        <v>0.54349000000000003</v>
-      </c>
-      <c r="K11" s="4">
-        <v>5.2065000000000001</v>
-      </c>
-      <c r="L11" s="4">
-        <v>3.1556999999999999</v>
-      </c>
-      <c r="M11" s="4">
-        <v>0.27356999999999998</v>
-      </c>
-      <c r="N11" s="3">
-        <v>3.1248</v>
-      </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="13"/>
       <c r="B12" s="16"/>
-      <c r="C12" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="D12" s="4">
-        <v>8.5922999999999998</v>
-      </c>
-      <c r="E12" s="4">
-        <v>38.904000000000003</v>
-      </c>
-      <c r="F12" s="4">
-        <v>5.4828999999999999</v>
-      </c>
-      <c r="G12" s="4">
-        <v>4.4794999999999998</v>
-      </c>
-      <c r="H12" s="4">
-        <v>1841</v>
-      </c>
-      <c r="I12" s="4">
-        <v>2.2498</v>
-      </c>
-      <c r="J12" s="4">
-        <v>0.39954000000000001</v>
-      </c>
-      <c r="K12" s="4">
-        <v>3.722</v>
-      </c>
-      <c r="L12" s="4">
-        <v>4.2567000000000004</v>
-      </c>
-      <c r="M12" s="4">
-        <v>0.19838</v>
-      </c>
-      <c r="N12" s="3">
-        <v>3.5486</v>
-      </c>
     </row>
     <row r="13" spans="1:15" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="14"/>
@@ -5605,402 +5726,42 @@
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="13"/>
       <c r="B15" s="16"/>
-      <c r="C15" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="D15" s="4">
-        <v>31.327000000000002</v>
-      </c>
-      <c r="E15" s="4">
-        <v>104.92</v>
-      </c>
-      <c r="F15" s="4">
-        <v>0.8548</v>
-      </c>
-      <c r="G15" s="4">
-        <v>3.7507999999999999</v>
-      </c>
-      <c r="H15" s="4">
-        <v>2575.8000000000002</v>
-      </c>
-      <c r="I15" s="4">
-        <v>1.0368999999999999</v>
-      </c>
-      <c r="J15" s="4">
-        <v>0.33298</v>
-      </c>
-      <c r="K15" s="4">
-        <v>3.661</v>
-      </c>
-      <c r="L15" s="4">
-        <v>1.9359999999999999</v>
-      </c>
-      <c r="M15" s="4">
-        <v>0.26541999999999999</v>
-      </c>
-      <c r="N15" s="3">
-        <v>3.1442999999999999</v>
-      </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="13"/>
       <c r="B16" s="16"/>
-      <c r="C16" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="D16" s="4">
-        <v>22.393000000000001</v>
-      </c>
-      <c r="E16" s="4">
-        <v>462.57</v>
-      </c>
-      <c r="F16" s="4">
-        <v>0.13572999999999999</v>
-      </c>
-      <c r="G16" s="4">
-        <v>4.3140000000000001</v>
-      </c>
-      <c r="H16" s="4">
-        <v>1828.1</v>
-      </c>
-      <c r="I16" s="2">
-        <v>1.9733000000000001</v>
-      </c>
-      <c r="J16" s="2">
-        <v>0.27233000000000002</v>
-      </c>
-      <c r="K16" s="2">
-        <v>3.1234000000000002</v>
-      </c>
-      <c r="L16" s="2">
-        <v>2.0615999999999999</v>
-      </c>
-      <c r="M16" s="2">
-        <v>9.5870999999999994E-3</v>
-      </c>
-      <c r="N16" s="2">
-        <v>5.4309000000000003</v>
-      </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" s="13"/>
       <c r="B17" s="16"/>
-      <c r="C17" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="D17" s="4">
-        <v>11.45</v>
-      </c>
-      <c r="E17" s="4">
-        <v>53.151000000000003</v>
-      </c>
-      <c r="F17" s="4">
-        <v>7.1665999999999999</v>
-      </c>
-      <c r="G17" s="4">
-        <v>3.9502000000000002</v>
-      </c>
-      <c r="H17" s="4">
-        <v>2221.6</v>
-      </c>
-      <c r="I17" s="2">
-        <v>1.373</v>
-      </c>
-      <c r="J17" s="2">
-        <v>0.39922000000000002</v>
-      </c>
-      <c r="K17" s="2">
-        <v>3.891</v>
-      </c>
-      <c r="L17" s="2">
-        <v>3.8786999999999998</v>
-      </c>
-      <c r="M17" s="2">
-        <v>0.13688</v>
-      </c>
-      <c r="N17" s="2">
-        <v>2.6692999999999998</v>
-      </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" s="13"/>
       <c r="B18" s="16"/>
-      <c r="C18" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="D18" s="4">
-        <v>37.741999999999997</v>
-      </c>
-      <c r="E18" s="4">
-        <v>49.122999999999998</v>
-      </c>
-      <c r="F18" s="4">
-        <v>2.4996</v>
-      </c>
-      <c r="G18" s="4">
-        <v>3.4102000000000001</v>
-      </c>
-      <c r="H18" s="4">
-        <v>3172</v>
-      </c>
-      <c r="I18" s="4">
-        <v>1.0524</v>
-      </c>
-      <c r="J18" s="4">
-        <v>0.68115000000000003</v>
-      </c>
-      <c r="K18" s="4">
-        <v>6.5023999999999997</v>
-      </c>
-      <c r="L18" s="4">
-        <v>1.6215999999999999</v>
-      </c>
-      <c r="M18" s="4">
-        <v>0.19822000000000001</v>
-      </c>
-      <c r="N18" s="3">
-        <v>2.7772999999999999</v>
-      </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" s="13"/>
       <c r="B19" s="16"/>
-      <c r="C19" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="D19" s="4">
-        <v>18.768000000000001</v>
-      </c>
-      <c r="E19" s="4">
-        <v>89.18</v>
-      </c>
-      <c r="F19" s="4">
-        <v>0.88068999999999997</v>
-      </c>
-      <c r="G19" s="4">
-        <v>4.5054999999999996</v>
-      </c>
-      <c r="H19" s="4">
-        <v>1677.4</v>
-      </c>
-      <c r="I19" s="4">
-        <v>1.9628000000000001</v>
-      </c>
-      <c r="J19" s="4">
-        <v>0.35322999999999999</v>
-      </c>
-      <c r="K19" s="4">
-        <v>3.5571000000000002</v>
-      </c>
-      <c r="L19" s="4">
-        <v>4.0984999999999996</v>
-      </c>
-      <c r="M19" s="4">
-        <v>5.9319999999999998E-2</v>
-      </c>
-      <c r="N19" s="3">
-        <v>2.5131999999999999</v>
-      </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" s="13"/>
       <c r="B20" s="16"/>
-      <c r="C20" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="D20" s="4">
-        <v>23.303999999999998</v>
-      </c>
-      <c r="E20" s="4">
-        <v>306.58</v>
-      </c>
-      <c r="F20" s="4">
-        <v>0.32123000000000002</v>
-      </c>
-      <c r="G20" s="4">
-        <v>4.2591999999999999</v>
-      </c>
-      <c r="H20" s="4">
-        <v>1822.6</v>
-      </c>
-      <c r="I20" s="4">
-        <v>1.6464000000000001</v>
-      </c>
-      <c r="J20" s="4">
-        <v>0.23887</v>
-      </c>
-      <c r="K20" s="4">
-        <v>2.9979</v>
-      </c>
-      <c r="L20" s="4">
-        <v>4.1620999999999997</v>
-      </c>
-      <c r="M20" s="4">
-        <v>2.9884999999999998E-3</v>
-      </c>
-      <c r="N20" s="3">
-        <v>2.3424999999999998</v>
-      </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" s="13"/>
       <c r="B21" s="16"/>
-      <c r="C21" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="D21" s="4">
-        <v>31.137</v>
-      </c>
-      <c r="E21" s="4">
-        <v>31.413</v>
-      </c>
-      <c r="F21" s="4">
-        <v>4.6002999999999998</v>
-      </c>
-      <c r="G21" s="4">
-        <v>3.6958000000000002</v>
-      </c>
-      <c r="H21" s="4">
-        <v>2583</v>
-      </c>
-      <c r="I21" s="4">
-        <v>1.2944</v>
-      </c>
-      <c r="J21" s="4">
-        <v>0.36685000000000001</v>
-      </c>
-      <c r="K21" s="4">
-        <v>3.8721000000000001</v>
-      </c>
-      <c r="L21" s="4">
-        <v>2.0034000000000001</v>
-      </c>
-      <c r="M21" s="4">
-        <v>0.2167</v>
-      </c>
-      <c r="N21" s="3">
-        <v>2.8479999999999999</v>
-      </c>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" s="13"/>
       <c r="B22" s="16"/>
-      <c r="C22" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="D22" s="4">
-        <v>29.725999999999999</v>
-      </c>
-      <c r="E22" s="4">
-        <v>45.991</v>
-      </c>
-      <c r="F22" s="4">
-        <v>2.3174000000000001</v>
-      </c>
-      <c r="G22" s="4">
-        <v>3.9613</v>
-      </c>
-      <c r="H22" s="4">
-        <v>2101.3000000000002</v>
-      </c>
-      <c r="I22" s="4">
-        <v>1.617</v>
-      </c>
-      <c r="J22" s="4">
-        <v>0.27362999999999998</v>
-      </c>
-      <c r="K22" s="4">
-        <v>3.2206000000000001</v>
-      </c>
-      <c r="L22" s="4">
-        <v>5.6994999999999996</v>
-      </c>
-      <c r="M22" s="4">
-        <v>0.96150999999999998</v>
-      </c>
-      <c r="N22" s="3">
-        <v>3.9527000000000001</v>
-      </c>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" s="13"/>
       <c r="B23" s="16"/>
-      <c r="C23" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="D23" s="4">
-        <v>0.85682000000000003</v>
-      </c>
-      <c r="E23" s="4">
-        <v>42.524000000000001</v>
-      </c>
-      <c r="F23" s="4">
-        <v>9.6282999999999994</v>
-      </c>
-      <c r="G23" s="4">
-        <v>4.5033000000000003</v>
-      </c>
-      <c r="H23" s="4">
-        <v>1707</v>
-      </c>
-      <c r="I23" s="4">
-        <v>1.2393000000000001</v>
-      </c>
-      <c r="J23" s="4">
-        <v>0.28849000000000002</v>
-      </c>
-      <c r="K23" s="4">
-        <v>3.4293</v>
-      </c>
-      <c r="L23" s="4">
-        <v>3.0653999999999999</v>
-      </c>
-      <c r="M23" s="4">
-        <v>0.11899999999999999</v>
-      </c>
-      <c r="N23" s="3">
-        <v>2.6208</v>
-      </c>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" s="13"/>
       <c r="B24" s="16"/>
-      <c r="C24" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="D24" s="4">
-        <v>4.4611000000000001</v>
-      </c>
-      <c r="E24" s="4">
-        <v>35.628</v>
-      </c>
-      <c r="F24" s="4">
-        <v>31.021000000000001</v>
-      </c>
-      <c r="G24" s="4">
-        <v>3.6185999999999998</v>
-      </c>
-      <c r="H24" s="4">
-        <v>3016.2</v>
-      </c>
-      <c r="I24" s="4">
-        <v>9.5056999999999992</v>
-      </c>
-      <c r="J24" s="4">
-        <v>0.33045999999999998</v>
-      </c>
-      <c r="K24" s="4">
-        <v>3.327</v>
-      </c>
-      <c r="L24" s="4">
-        <v>4.6459000000000001</v>
-      </c>
-      <c r="M24" s="4">
-        <v>0.20498</v>
-      </c>
-      <c r="N24" s="3">
-        <v>2.7280000000000002</v>
-      </c>
     </row>
     <row r="25" spans="1:15" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="14"/>
@@ -6020,402 +5781,42 @@
     <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27" s="13"/>
       <c r="B27" s="16"/>
-      <c r="C27" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="D27" s="4">
-        <v>4.8710000000000004</v>
-      </c>
-      <c r="E27" s="4">
-        <v>11.518000000000001</v>
-      </c>
-      <c r="F27" s="4">
-        <v>7.0281000000000002</v>
-      </c>
-      <c r="G27" s="4">
-        <v>4.2420999999999998</v>
-      </c>
-      <c r="H27" s="4">
-        <v>1138.3</v>
-      </c>
-      <c r="I27" s="4">
-        <v>1.2072000000000001</v>
-      </c>
-      <c r="J27" s="4">
-        <v>0.44550000000000001</v>
-      </c>
-      <c r="K27" s="4">
-        <v>3.8687</v>
-      </c>
-      <c r="L27" s="4">
-        <v>3.6877</v>
-      </c>
-      <c r="M27" s="4">
-        <v>0.25385000000000002</v>
-      </c>
-      <c r="N27" s="3">
-        <v>2.5308000000000002</v>
-      </c>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28" s="13"/>
       <c r="B28" s="16"/>
-      <c r="C28" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="D28" s="4">
-        <v>10.692</v>
-      </c>
-      <c r="E28" s="4">
-        <v>29.068000000000001</v>
-      </c>
-      <c r="F28" s="4">
-        <v>2.9830999999999999</v>
-      </c>
-      <c r="G28" s="4">
-        <v>3.7277999999999998</v>
-      </c>
-      <c r="H28" s="4">
-        <v>1433.5</v>
-      </c>
-      <c r="I28" s="2">
-        <v>2.3410000000000002</v>
-      </c>
-      <c r="J28" s="2">
-        <v>0.39410000000000001</v>
-      </c>
-      <c r="K28" s="2">
-        <v>3.3374000000000001</v>
-      </c>
-      <c r="L28" s="2">
-        <v>5.6124999999999998</v>
-      </c>
-      <c r="M28" s="2">
-        <v>0.94169000000000003</v>
-      </c>
-      <c r="N28" s="2">
-        <v>3.4904999999999999</v>
-      </c>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29" s="13"/>
       <c r="B29" s="16"/>
-      <c r="C29" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="D29" s="4">
-        <v>11.2</v>
-      </c>
-      <c r="E29" s="4">
-        <v>24.262</v>
-      </c>
-      <c r="F29" s="4">
-        <v>2.2614999999999998</v>
-      </c>
-      <c r="G29" s="4">
-        <v>3.9651000000000001</v>
-      </c>
-      <c r="H29" s="4">
-        <v>1163</v>
-      </c>
-      <c r="I29" s="4">
-        <v>1.7908999999999999</v>
-      </c>
-      <c r="J29" s="4">
-        <v>0.45981</v>
-      </c>
-      <c r="K29" s="4">
-        <v>3.9491000000000001</v>
-      </c>
-      <c r="L29" s="4">
-        <v>3.3142</v>
-      </c>
-      <c r="M29" s="4">
-        <v>0.20016999999999999</v>
-      </c>
-      <c r="N29" s="3">
-        <v>2.4437000000000002</v>
-      </c>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30" s="13"/>
       <c r="B30" s="16"/>
-      <c r="C30" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="D30" s="4">
-        <v>11.208</v>
-      </c>
-      <c r="E30" s="4">
-        <v>16.738</v>
-      </c>
-      <c r="F30" s="4">
-        <v>5.9587000000000003</v>
-      </c>
-      <c r="G30" s="4">
-        <v>3.6377000000000002</v>
-      </c>
-      <c r="H30" s="4">
-        <v>1530.1</v>
-      </c>
-      <c r="I30" s="4">
-        <v>1.0164</v>
-      </c>
-      <c r="J30" s="4">
-        <v>0.51859999999999995</v>
-      </c>
-      <c r="K30" s="4">
-        <v>4.4584999999999999</v>
-      </c>
-      <c r="L30" s="4">
-        <v>3.1135000000000002</v>
-      </c>
-      <c r="M30" s="4">
-        <v>0.38601000000000002</v>
-      </c>
-      <c r="N30" s="3">
-        <v>3.3180999999999998</v>
-      </c>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A31" s="13"/>
       <c r="B31" s="16"/>
-      <c r="C31" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="D31" s="4">
-        <v>10.45</v>
-      </c>
-      <c r="E31" s="4">
-        <v>14.769</v>
-      </c>
-      <c r="F31" s="4">
-        <v>7.8792</v>
-      </c>
-      <c r="G31" s="4">
-        <v>3.54</v>
-      </c>
-      <c r="H31" s="4">
-        <v>1787.3</v>
-      </c>
-      <c r="I31" s="4">
-        <v>1.3337000000000001</v>
-      </c>
-      <c r="J31" s="4">
-        <v>0.59784999999999999</v>
-      </c>
-      <c r="K31" s="4">
-        <v>4.8552999999999997</v>
-      </c>
-      <c r="L31" s="4">
-        <v>2.6320000000000001</v>
-      </c>
-      <c r="M31" s="4">
-        <v>0.34475</v>
-      </c>
-      <c r="N31" s="3">
-        <v>3.0926</v>
-      </c>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A32" s="13"/>
       <c r="B32" s="16"/>
-      <c r="C32" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="D32" s="4">
-        <v>11.010999999999999</v>
-      </c>
-      <c r="E32" s="4">
-        <v>11.071</v>
-      </c>
-      <c r="F32" s="4">
-        <v>13.523</v>
-      </c>
-      <c r="G32" s="4">
-        <v>3.5672000000000001</v>
-      </c>
-      <c r="H32" s="4">
-        <v>1593.8</v>
-      </c>
-      <c r="I32" s="4">
-        <v>2.0019</v>
-      </c>
-      <c r="J32" s="4">
-        <v>0.50361</v>
-      </c>
-      <c r="K32" s="4">
-        <v>4.1786000000000003</v>
-      </c>
-      <c r="L32" s="4">
-        <v>4.2843</v>
-      </c>
-      <c r="M32" s="4">
-        <v>0.22523000000000001</v>
-      </c>
-      <c r="N32" s="3">
-        <v>2.6124999999999998</v>
-      </c>
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A33" s="13"/>
       <c r="B33" s="16"/>
-      <c r="C33" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="D33" s="4">
-        <v>5.6656000000000004</v>
-      </c>
-      <c r="E33" s="4">
-        <v>8.2222000000000008</v>
-      </c>
-      <c r="F33" s="4">
-        <v>14.47</v>
-      </c>
-      <c r="G33" s="4">
-        <v>4.3000999999999996</v>
-      </c>
-      <c r="H33" s="4">
-        <v>1000.8</v>
-      </c>
-      <c r="I33" s="4">
-        <v>1.3364</v>
-      </c>
-      <c r="J33" s="4">
-        <v>0.73826000000000003</v>
-      </c>
-      <c r="K33" s="4">
-        <v>6.1936999999999998</v>
-      </c>
-      <c r="L33" s="4">
-        <v>2.6962999999999999</v>
-      </c>
-      <c r="M33" s="4">
-        <v>0.35518</v>
-      </c>
-      <c r="N33" s="3">
-        <v>3.2061000000000002</v>
-      </c>
     </row>
     <row r="34" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A34" s="13"/>
       <c r="B34" s="16"/>
-      <c r="C34" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="D34" s="4">
-        <v>15.185</v>
-      </c>
-      <c r="E34" s="4">
-        <v>64.875</v>
-      </c>
-      <c r="F34" s="4">
-        <v>1.4525999999999999</v>
-      </c>
-      <c r="G34" s="4">
-        <v>3.2002999999999999</v>
-      </c>
-      <c r="H34" s="4">
-        <v>2110.6</v>
-      </c>
-      <c r="I34" s="4">
-        <v>1.7833000000000001</v>
-      </c>
-      <c r="J34" s="4">
-        <v>0.51853000000000005</v>
-      </c>
-      <c r="K34" s="4">
-        <v>4.2645</v>
-      </c>
-      <c r="L34" s="4">
-        <v>3.7526000000000002</v>
-      </c>
-      <c r="M34" s="4">
-        <v>0.20075000000000001</v>
-      </c>
-      <c r="N34" s="3">
-        <v>2.5205000000000002</v>
-      </c>
     </row>
     <row r="35" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A35" s="13"/>
       <c r="B35" s="16"/>
-      <c r="C35" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="D35" s="4">
-        <v>8.0571999999999999</v>
-      </c>
-      <c r="E35" s="4">
-        <v>29.803999999999998</v>
-      </c>
-      <c r="F35" s="4">
-        <v>2.5836000000000001</v>
-      </c>
-      <c r="G35" s="4">
-        <v>4.0204000000000004</v>
-      </c>
-      <c r="H35" s="4">
-        <v>1210.4000000000001</v>
-      </c>
-      <c r="I35" s="4">
-        <v>1.2011000000000001</v>
-      </c>
-      <c r="J35" s="4">
-        <v>0.49431999999999998</v>
-      </c>
-      <c r="K35" s="4">
-        <v>4.3479000000000001</v>
-      </c>
-      <c r="L35" s="4">
-        <v>2.7725</v>
-      </c>
-      <c r="M35" s="4">
-        <v>0.29389999999999999</v>
-      </c>
-      <c r="N35" s="3">
-        <v>2.7284999999999999</v>
-      </c>
     </row>
     <row r="36" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A36" s="13"/>
       <c r="B36" s="16"/>
-      <c r="C36" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="D36" s="4">
-        <v>7.5292000000000003</v>
-      </c>
-      <c r="E36" s="4">
-        <v>23.504999999999999</v>
-      </c>
-      <c r="F36" s="4">
-        <v>4.9898999999999996</v>
-      </c>
-      <c r="G36" s="4">
-        <v>3.8622999999999998</v>
-      </c>
-      <c r="H36" s="4">
-        <v>1369.1</v>
-      </c>
-      <c r="I36" s="4">
-        <v>1.9939</v>
-      </c>
-      <c r="J36" s="4">
-        <v>0.36113000000000001</v>
-      </c>
-      <c r="K36" s="4">
-        <v>3.2098</v>
-      </c>
-      <c r="L36" s="4">
-        <v>1.6549</v>
-      </c>
-      <c r="M36" s="4">
-        <v>0.25001000000000001</v>
-      </c>
-      <c r="N36" s="3">
-        <v>3.9885000000000002</v>
-      </c>
     </row>
     <row r="37" spans="1:15" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="14"/>
@@ -6435,402 +5836,48 @@
     <row r="39" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A39" s="13"/>
       <c r="B39" s="16"/>
-      <c r="C39" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="D39" s="4">
-        <v>4.8238000000000003</v>
-      </c>
-      <c r="E39" s="4">
-        <v>378.86</v>
-      </c>
-      <c r="F39" s="4">
-        <v>0.14230000000000001</v>
-      </c>
-      <c r="G39" s="4">
-        <v>4.4020999999999999</v>
-      </c>
-      <c r="H39" s="4">
-        <v>1006.9</v>
-      </c>
-      <c r="I39" s="4">
-        <v>1.3282</v>
-      </c>
-      <c r="J39" s="4">
-        <v>0.54573000000000005</v>
-      </c>
-      <c r="K39" s="4">
-        <v>4.6946000000000003</v>
-      </c>
-      <c r="L39" s="4">
-        <v>3.1678999999999999</v>
-      </c>
-      <c r="M39" s="4">
-        <v>0.25372</v>
-      </c>
-      <c r="N39" s="3">
-        <v>2.5291999999999999</v>
-      </c>
     </row>
     <row r="40" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A40" s="13"/>
       <c r="B40" s="16"/>
-      <c r="C40" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="D40" s="4">
-        <v>7.1036999999999999</v>
-      </c>
-      <c r="E40" s="4">
-        <v>48.234999999999999</v>
-      </c>
-      <c r="F40" s="4">
-        <v>4.2972000000000001</v>
-      </c>
-      <c r="G40" s="4">
-        <v>3.4083999999999999</v>
-      </c>
-      <c r="H40" s="4">
-        <v>1829.9</v>
-      </c>
-      <c r="I40" s="2">
-        <v>1.3602000000000001</v>
-      </c>
-      <c r="J40" s="2">
-        <v>0.34182000000000001</v>
-      </c>
-      <c r="K40" s="2">
-        <v>3.1635</v>
-      </c>
-      <c r="L40" s="2">
-        <v>12.426</v>
-      </c>
-      <c r="M40" s="2">
-        <v>0.21156</v>
-      </c>
-      <c r="N40" s="2">
-        <v>3.3578000000000001</v>
-      </c>
     </row>
     <row r="41" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A41" s="13"/>
       <c r="B41" s="16"/>
-      <c r="C41" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="D41" s="4">
-        <v>3.0461</v>
-      </c>
-      <c r="E41" s="4">
-        <v>19.608000000000001</v>
-      </c>
-      <c r="F41" s="4">
-        <v>32.420999999999999</v>
-      </c>
-      <c r="G41" s="4">
-        <v>3.2736000000000001</v>
-      </c>
-      <c r="H41" s="4">
-        <v>2022.3</v>
-      </c>
-      <c r="I41" s="2">
-        <v>1.9328000000000001</v>
-      </c>
-      <c r="J41" s="2">
-        <v>0.59299999999999997</v>
-      </c>
-      <c r="K41" s="2">
-        <v>4.7255000000000003</v>
-      </c>
-      <c r="L41" s="2">
-        <v>2.6515</v>
-      </c>
-      <c r="M41" s="2">
-        <v>0.25479000000000002</v>
-      </c>
-      <c r="N41" s="1">
-        <v>2.5724</v>
-      </c>
+      <c r="I41" s="2"/>
+      <c r="J41" s="2"/>
+      <c r="K41" s="2"/>
+      <c r="L41" s="2"/>
+      <c r="M41" s="2"/>
+      <c r="N41" s="1"/>
     </row>
     <row r="42" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A42" s="13"/>
       <c r="B42" s="16"/>
-      <c r="C42" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="D42" s="4">
-        <v>4.6340000000000003</v>
-      </c>
-      <c r="E42" s="4">
-        <v>18.606999999999999</v>
-      </c>
-      <c r="F42" s="4">
-        <v>24.896000000000001</v>
-      </c>
-      <c r="G42" s="4">
-        <v>3.3435999999999999</v>
-      </c>
-      <c r="H42" s="4">
-        <v>1999.7</v>
-      </c>
-      <c r="I42" s="4">
-        <v>2.2488000000000001</v>
-      </c>
-      <c r="J42" s="4">
-        <v>0.27339999999999998</v>
-      </c>
-      <c r="K42" s="4">
-        <v>2.6326000000000001</v>
-      </c>
-      <c r="L42" s="4">
-        <v>4.8822000000000001</v>
-      </c>
-      <c r="M42" s="4">
-        <v>0.17643</v>
-      </c>
-      <c r="N42" s="3">
-        <v>2.3942000000000001</v>
-      </c>
     </row>
     <row r="43" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A43" s="13"/>
       <c r="B43" s="16"/>
-      <c r="C43" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="D43" s="4">
-        <v>16.286999999999999</v>
-      </c>
-      <c r="E43" s="4">
-        <v>181.45</v>
-      </c>
-      <c r="F43" s="4">
-        <v>0.52517000000000003</v>
-      </c>
-      <c r="G43" s="4">
-        <v>3.0160999999999998</v>
-      </c>
-      <c r="H43" s="4">
-        <v>2606.1999999999998</v>
-      </c>
-      <c r="I43" s="4">
-        <v>7.6341000000000001</v>
-      </c>
-      <c r="J43" s="4">
-        <v>0.55245999999999995</v>
-      </c>
-      <c r="K43" s="4">
-        <v>7.7807000000000004</v>
-      </c>
-      <c r="L43" s="4">
-        <v>2.0291999999999999</v>
-      </c>
-      <c r="M43" s="4">
-        <v>0.31213000000000002</v>
-      </c>
-      <c r="N43" s="3">
-        <v>2.8618000000000001</v>
-      </c>
     </row>
     <row r="44" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A44" s="13"/>
       <c r="B44" s="16"/>
-      <c r="C44" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="D44" s="4">
-        <v>9.5312999999999999</v>
-      </c>
-      <c r="E44" s="4">
-        <v>148.61000000000001</v>
-      </c>
-      <c r="F44" s="4">
-        <v>0.37484000000000001</v>
-      </c>
-      <c r="G44" s="4">
-        <v>3.9621</v>
-      </c>
-      <c r="H44" s="4">
-        <v>1253.9000000000001</v>
-      </c>
-      <c r="I44" s="4">
-        <v>2.3045</v>
-      </c>
-      <c r="J44" s="4">
-        <v>0.34014</v>
-      </c>
-      <c r="K44" s="4">
-        <v>3.0451000000000001</v>
-      </c>
-      <c r="L44" s="4">
-        <v>2.7208000000000001</v>
-      </c>
-      <c r="M44" s="4">
-        <v>6.7532999999999996E-2</v>
-      </c>
-      <c r="N44" s="3">
-        <v>2.4268999999999998</v>
-      </c>
     </row>
     <row r="45" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A45" s="13"/>
       <c r="B45" s="16"/>
-      <c r="C45" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="D45" s="4">
-        <v>6.3647</v>
-      </c>
-      <c r="E45" s="4">
-        <v>149.54</v>
-      </c>
-      <c r="F45" s="4">
-        <v>0.43913000000000002</v>
-      </c>
-      <c r="G45" s="4">
-        <v>4.1839000000000004</v>
-      </c>
-      <c r="H45" s="4">
-        <v>1127.5999999999999</v>
-      </c>
-      <c r="I45" s="4">
-        <v>2.2016</v>
-      </c>
-      <c r="J45" s="4">
-        <v>0.28632000000000002</v>
-      </c>
-      <c r="K45" s="4">
-        <v>2.7416</v>
-      </c>
-      <c r="L45" s="4">
-        <v>1.1881999999999999</v>
-      </c>
-      <c r="M45" s="4">
-        <v>0.70389999999999997</v>
-      </c>
-      <c r="N45" s="3">
-        <v>8.2974999999999993E-2</v>
-      </c>
     </row>
     <row r="46" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A46" s="13"/>
       <c r="B46" s="16"/>
-      <c r="C46" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="D46" s="4">
-        <v>12.622</v>
-      </c>
-      <c r="E46" s="4">
-        <v>15.441000000000001</v>
-      </c>
-      <c r="F46" s="4">
-        <v>4.5385999999999997</v>
-      </c>
-      <c r="G46" s="4">
-        <v>3.7305000000000001</v>
-      </c>
-      <c r="H46" s="4">
-        <v>1371.6</v>
-      </c>
-      <c r="I46" s="4">
-        <v>2.2448999999999999</v>
-      </c>
-      <c r="J46" s="4">
-        <v>0.40698000000000001</v>
-      </c>
-      <c r="K46" s="4">
-        <v>3.5036</v>
-      </c>
-      <c r="L46" s="4">
-        <v>4.0568</v>
-      </c>
-      <c r="M46" s="4">
-        <v>0.21132000000000001</v>
-      </c>
-      <c r="N46" s="3">
-        <v>2.4597000000000002</v>
-      </c>
     </row>
     <row r="47" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A47" s="13"/>
       <c r="B47" s="16"/>
-      <c r="C47" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="D47" s="4">
-        <v>12.256</v>
-      </c>
-      <c r="E47" s="4">
-        <v>273.68</v>
-      </c>
-      <c r="F47" s="4">
-        <v>0.20866000000000001</v>
-      </c>
-      <c r="G47" s="4">
-        <v>3.8422000000000001</v>
-      </c>
-      <c r="H47" s="4">
-        <v>1242.3</v>
-      </c>
-      <c r="I47" s="4">
-        <v>1.8718999999999999</v>
-      </c>
-      <c r="J47" s="4">
-        <v>0.38352999999999998</v>
-      </c>
-      <c r="K47" s="4">
-        <v>3.4464999999999999</v>
-      </c>
-      <c r="L47" s="4">
-        <v>3.8252999999999999</v>
-      </c>
-      <c r="M47" s="4">
-        <v>0.19616</v>
-      </c>
-      <c r="N47" s="3">
-        <v>2.4363999999999999</v>
-      </c>
     </row>
     <row r="48" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A48" s="13"/>
       <c r="B48" s="16"/>
-      <c r="C48" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="D48" s="4">
-        <v>7.0439999999999996</v>
-      </c>
-      <c r="E48" s="4">
-        <v>16.175000000000001</v>
-      </c>
-      <c r="F48" s="4">
-        <v>6.7949000000000002</v>
-      </c>
-      <c r="G48" s="4">
-        <v>4.1207000000000003</v>
-      </c>
-      <c r="H48" s="4">
-        <v>1090</v>
-      </c>
-      <c r="I48" s="4">
-        <v>2.2446999999999999</v>
-      </c>
-      <c r="J48" s="4">
-        <v>0.43214999999999998</v>
-      </c>
-      <c r="K48" s="4">
-        <v>3.6272000000000002</v>
-      </c>
-      <c r="L48" s="4">
-        <v>5.3937999999999997</v>
-      </c>
-      <c r="M48" s="4">
-        <v>0.16178999999999999</v>
-      </c>
-      <c r="N48" s="3">
-        <v>2.391</v>
-      </c>
     </row>
     <row r="49" spans="1:15" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="14"/>
@@ -6969,13 +6016,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F200E048-5FAF-4136-82F6-92204CC50E12}">
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1D987DC-5A74-4932-B56A-48A4420F0E95}">
   <dimension ref="A1:O73"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N51" sqref="N51"/>
+    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L1" sqref="L1:L1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6997,7 +6044,7 @@
         <v>11</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D1" s="5" t="s">
         <v>1</v>
@@ -7045,48 +6092,402 @@
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="13"/>
       <c r="B3" s="16"/>
-      <c r="I3" s="2"/>
-      <c r="J3" s="2"/>
-      <c r="K3" s="2"/>
-      <c r="L3" s="2"/>
-      <c r="M3" s="2"/>
-      <c r="N3" s="1"/>
+      <c r="C3" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="D3" s="4">
+        <v>17.216999999999999</v>
+      </c>
+      <c r="E3" s="4">
+        <v>179.74</v>
+      </c>
+      <c r="F3" s="4">
+        <v>0.61753999999999998</v>
+      </c>
+      <c r="G3" s="4">
+        <v>4.4165999999999999</v>
+      </c>
+      <c r="H3" s="4">
+        <v>1783.5</v>
+      </c>
+      <c r="I3" s="2">
+        <v>1.0025999999999999</v>
+      </c>
+      <c r="J3" s="2">
+        <v>0.41060999999999998</v>
+      </c>
+      <c r="K3" s="2">
+        <v>4.2331000000000003</v>
+      </c>
+      <c r="L3" s="2">
+        <v>2.2349000000000001</v>
+      </c>
+      <c r="M3" s="2">
+        <v>0.29105999999999999</v>
+      </c>
+      <c r="N3" s="1">
+        <v>3.1743000000000001</v>
+      </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="13"/>
       <c r="B4" s="16"/>
+      <c r="C4" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="D4" s="4">
+        <v>5.6908000000000003</v>
+      </c>
+      <c r="E4" s="4">
+        <v>66.626999999999995</v>
+      </c>
+      <c r="F4" s="4">
+        <v>1.9851000000000001</v>
+      </c>
+      <c r="G4" s="4">
+        <v>4.7723000000000004</v>
+      </c>
+      <c r="H4" s="4">
+        <v>1621.6</v>
+      </c>
+      <c r="I4" s="2">
+        <v>1.8904000000000001</v>
+      </c>
+      <c r="J4" s="2">
+        <v>0.54329000000000005</v>
+      </c>
+      <c r="K4" s="2">
+        <v>4.6087999999999996</v>
+      </c>
+      <c r="L4" s="2">
+        <v>1.8685</v>
+      </c>
+      <c r="M4" s="2">
+        <v>9.3698000000000004E-2</v>
+      </c>
+      <c r="N4" s="2">
+        <v>2.7471999999999999</v>
+      </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="13"/>
       <c r="B5" s="16"/>
+      <c r="C5" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="D5" s="4">
+        <v>9.3076000000000008</v>
+      </c>
+      <c r="E5" s="4">
+        <v>32.595999999999997</v>
+      </c>
+      <c r="F5" s="4">
+        <v>5.8113999999999999</v>
+      </c>
+      <c r="G5" s="4">
+        <v>4.5263</v>
+      </c>
+      <c r="H5" s="4">
+        <v>1775.9</v>
+      </c>
+      <c r="I5" s="2">
+        <v>1.8393999999999999</v>
+      </c>
+      <c r="J5" s="2">
+        <v>0.71550999999999998</v>
+      </c>
+      <c r="K5" s="2">
+        <v>5.8657000000000004</v>
+      </c>
+      <c r="L5" s="2">
+        <v>1.8920999999999999</v>
+      </c>
+      <c r="M5" s="2">
+        <v>0.34444000000000002</v>
+      </c>
+      <c r="N5" s="2">
+        <v>3.5432999999999999</v>
+      </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="13"/>
       <c r="B6" s="16"/>
+      <c r="C6" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="D6" s="4">
+        <v>5.8951000000000002</v>
+      </c>
+      <c r="E6" s="4">
+        <v>36.244999999999997</v>
+      </c>
+      <c r="F6" s="4">
+        <v>5.3757000000000001</v>
+      </c>
+      <c r="G6" s="4">
+        <v>4.7310999999999996</v>
+      </c>
+      <c r="H6" s="4">
+        <v>1598.4</v>
+      </c>
+      <c r="I6" s="4">
+        <v>2.4487000000000001</v>
+      </c>
+      <c r="J6" s="4">
+        <v>0.36314000000000002</v>
+      </c>
+      <c r="K6" s="4">
+        <v>3.4647000000000001</v>
+      </c>
+      <c r="L6" s="4">
+        <v>9.3416999999999994</v>
+      </c>
+      <c r="M6" s="4">
+        <v>0.10058</v>
+      </c>
+      <c r="N6" s="3">
+        <v>3.1581999999999999</v>
+      </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="13"/>
       <c r="B7" s="16"/>
+      <c r="C7" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="D7" s="2">
+        <v>4.1862000000000004</v>
+      </c>
+      <c r="E7" s="2">
+        <v>84.548000000000002</v>
+      </c>
+      <c r="F7" s="2">
+        <v>2.1122999999999998</v>
+      </c>
+      <c r="G7" s="2">
+        <v>4.7751999999999999</v>
+      </c>
+      <c r="H7" s="2">
+        <v>1574.3</v>
+      </c>
+      <c r="I7" s="2">
+        <v>1.6472</v>
+      </c>
+      <c r="J7" s="2">
+        <v>0.34209000000000001</v>
+      </c>
+      <c r="K7" s="2">
+        <v>3.5358000000000001</v>
+      </c>
+      <c r="L7" s="2">
+        <v>10.343</v>
+      </c>
+      <c r="M7" s="2">
+        <v>0.55237999999999998</v>
+      </c>
+      <c r="N7" s="2">
+        <v>2.4053</v>
+      </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="13"/>
       <c r="B8" s="16"/>
+      <c r="C8" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="D8" s="4">
+        <v>25.038</v>
+      </c>
+      <c r="E8" s="4">
+        <v>90.692999999999998</v>
+      </c>
+      <c r="F8" s="4">
+        <v>0.61002000000000001</v>
+      </c>
+      <c r="G8" s="4">
+        <v>4.1981999999999999</v>
+      </c>
+      <c r="H8" s="4">
+        <v>1944.6</v>
+      </c>
+      <c r="I8" s="4">
+        <v>1.3413999999999999</v>
+      </c>
+      <c r="J8" s="4">
+        <v>0.39294000000000001</v>
+      </c>
+      <c r="K8" s="4">
+        <v>3.9001000000000001</v>
+      </c>
+      <c r="L8" s="4">
+        <v>4.3860999999999999</v>
+      </c>
+      <c r="M8" s="4">
+        <v>0.24360999999999999</v>
+      </c>
+      <c r="N8" s="3">
+        <v>2.9091</v>
+      </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="13"/>
       <c r="B9" s="16"/>
+      <c r="C9" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="D9" s="4">
+        <v>27.547000000000001</v>
+      </c>
+      <c r="E9" s="4">
+        <v>78.081000000000003</v>
+      </c>
+      <c r="F9" s="4">
+        <v>0.84272999999999998</v>
+      </c>
+      <c r="G9" s="4">
+        <v>3.8992</v>
+      </c>
+      <c r="H9" s="4">
+        <v>2454.8000000000002</v>
+      </c>
+      <c r="I9" s="4">
+        <v>1.8298000000000001</v>
+      </c>
+      <c r="J9" s="4">
+        <v>0.44322</v>
+      </c>
+      <c r="K9" s="4">
+        <v>4.1135000000000002</v>
+      </c>
+      <c r="L9" s="4">
+        <v>4.6660000000000004</v>
+      </c>
+      <c r="M9" s="4">
+        <v>7.2484999999999994E-2</v>
+      </c>
+      <c r="N9" s="3">
+        <v>2.4855999999999998</v>
+      </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="13"/>
       <c r="B10" s="16"/>
+      <c r="C10" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="D10" s="4">
+        <v>27.885000000000002</v>
+      </c>
+      <c r="E10" s="4">
+        <v>124.89</v>
+      </c>
+      <c r="F10" s="4">
+        <v>0.65636000000000005</v>
+      </c>
+      <c r="G10" s="4">
+        <v>3.8874</v>
+      </c>
+      <c r="H10" s="4">
+        <v>2390.5</v>
+      </c>
+      <c r="I10" s="4">
+        <v>1.1933</v>
+      </c>
+      <c r="J10" s="4">
+        <v>0.18759999999999999</v>
+      </c>
+      <c r="K10" s="4">
+        <v>2.4325999999999999</v>
+      </c>
+      <c r="L10" s="4">
+        <v>2.4598</v>
+      </c>
+      <c r="M10" s="4">
+        <v>0.27822999999999998</v>
+      </c>
+      <c r="N10" s="3">
+        <v>3.0878999999999999</v>
+      </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="13"/>
       <c r="B11" s="16"/>
+      <c r="C11" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="D11" s="4">
+        <v>19.2</v>
+      </c>
+      <c r="E11" s="4">
+        <v>52.204000000000001</v>
+      </c>
+      <c r="F11" s="4">
+        <v>1.7579</v>
+      </c>
+      <c r="G11" s="4">
+        <v>4.5105000000000004</v>
+      </c>
+      <c r="H11" s="4">
+        <v>1614.6</v>
+      </c>
+      <c r="I11" s="4">
+        <v>1.0317000000000001</v>
+      </c>
+      <c r="J11" s="4">
+        <v>0.54349000000000003</v>
+      </c>
+      <c r="K11" s="4">
+        <v>5.2065000000000001</v>
+      </c>
+      <c r="L11" s="4">
+        <v>3.1556999999999999</v>
+      </c>
+      <c r="M11" s="4">
+        <v>0.27356999999999998</v>
+      </c>
+      <c r="N11" s="3">
+        <v>3.1248</v>
+      </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="13"/>
       <c r="B12" s="16"/>
+      <c r="C12" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="D12" s="4">
+        <v>8.5922999999999998</v>
+      </c>
+      <c r="E12" s="4">
+        <v>38.904000000000003</v>
+      </c>
+      <c r="F12" s="4">
+        <v>5.4828999999999999</v>
+      </c>
+      <c r="G12" s="4">
+        <v>4.4794999999999998</v>
+      </c>
+      <c r="H12" s="4">
+        <v>1841</v>
+      </c>
+      <c r="I12" s="4">
+        <v>2.2498</v>
+      </c>
+      <c r="J12" s="4">
+        <v>0.39954000000000001</v>
+      </c>
+      <c r="K12" s="4">
+        <v>3.722</v>
+      </c>
+      <c r="L12" s="4">
+        <v>4.2567000000000004</v>
+      </c>
+      <c r="M12" s="4">
+        <v>0.19838</v>
+      </c>
+      <c r="N12" s="3">
+        <v>3.5486</v>
+      </c>
     </row>
     <row r="13" spans="1:15" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="14"/>
@@ -7106,42 +6507,402 @@
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="13"/>
       <c r="B15" s="16"/>
+      <c r="C15" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="D15" s="4">
+        <v>31.327000000000002</v>
+      </c>
+      <c r="E15" s="4">
+        <v>104.92</v>
+      </c>
+      <c r="F15" s="4">
+        <v>0.8548</v>
+      </c>
+      <c r="G15" s="4">
+        <v>3.7507999999999999</v>
+      </c>
+      <c r="H15" s="4">
+        <v>2575.8000000000002</v>
+      </c>
+      <c r="I15" s="4">
+        <v>1.0368999999999999</v>
+      </c>
+      <c r="J15" s="4">
+        <v>0.33298</v>
+      </c>
+      <c r="K15" s="4">
+        <v>3.661</v>
+      </c>
+      <c r="L15" s="4">
+        <v>1.9359999999999999</v>
+      </c>
+      <c r="M15" s="4">
+        <v>0.26541999999999999</v>
+      </c>
+      <c r="N15" s="3">
+        <v>3.1442999999999999</v>
+      </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="13"/>
       <c r="B16" s="16"/>
+      <c r="C16" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="D16" s="4">
+        <v>22.393000000000001</v>
+      </c>
+      <c r="E16" s="4">
+        <v>462.57</v>
+      </c>
+      <c r="F16" s="4">
+        <v>0.13572999999999999</v>
+      </c>
+      <c r="G16" s="4">
+        <v>4.3140000000000001</v>
+      </c>
+      <c r="H16" s="4">
+        <v>1828.1</v>
+      </c>
+      <c r="I16" s="2">
+        <v>1.9733000000000001</v>
+      </c>
+      <c r="J16" s="2">
+        <v>0.27233000000000002</v>
+      </c>
+      <c r="K16" s="2">
+        <v>3.1234000000000002</v>
+      </c>
+      <c r="L16" s="2">
+        <v>2.0615999999999999</v>
+      </c>
+      <c r="M16" s="2">
+        <v>9.5870999999999994E-3</v>
+      </c>
+      <c r="N16" s="2">
+        <v>5.4309000000000003</v>
+      </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" s="13"/>
       <c r="B17" s="16"/>
+      <c r="C17" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="D17" s="4">
+        <v>11.45</v>
+      </c>
+      <c r="E17" s="4">
+        <v>53.151000000000003</v>
+      </c>
+      <c r="F17" s="4">
+        <v>7.1665999999999999</v>
+      </c>
+      <c r="G17" s="4">
+        <v>3.9502000000000002</v>
+      </c>
+      <c r="H17" s="4">
+        <v>2221.6</v>
+      </c>
+      <c r="I17" s="2">
+        <v>1.373</v>
+      </c>
+      <c r="J17" s="2">
+        <v>0.39922000000000002</v>
+      </c>
+      <c r="K17" s="2">
+        <v>3.891</v>
+      </c>
+      <c r="L17" s="2">
+        <v>3.8786999999999998</v>
+      </c>
+      <c r="M17" s="2">
+        <v>0.13688</v>
+      </c>
+      <c r="N17" s="2">
+        <v>2.6692999999999998</v>
+      </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" s="13"/>
       <c r="B18" s="16"/>
+      <c r="C18" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="D18" s="4">
+        <v>37.741999999999997</v>
+      </c>
+      <c r="E18" s="4">
+        <v>49.122999999999998</v>
+      </c>
+      <c r="F18" s="4">
+        <v>2.4996</v>
+      </c>
+      <c r="G18" s="4">
+        <v>3.4102000000000001</v>
+      </c>
+      <c r="H18" s="4">
+        <v>3172</v>
+      </c>
+      <c r="I18" s="4">
+        <v>1.0524</v>
+      </c>
+      <c r="J18" s="4">
+        <v>0.68115000000000003</v>
+      </c>
+      <c r="K18" s="4">
+        <v>6.5023999999999997</v>
+      </c>
+      <c r="L18" s="4">
+        <v>1.6215999999999999</v>
+      </c>
+      <c r="M18" s="4">
+        <v>0.19822000000000001</v>
+      </c>
+      <c r="N18" s="3">
+        <v>2.7772999999999999</v>
+      </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" s="13"/>
       <c r="B19" s="16"/>
+      <c r="C19" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="D19" s="4">
+        <v>18.768000000000001</v>
+      </c>
+      <c r="E19" s="4">
+        <v>89.18</v>
+      </c>
+      <c r="F19" s="4">
+        <v>0.88068999999999997</v>
+      </c>
+      <c r="G19" s="4">
+        <v>4.5054999999999996</v>
+      </c>
+      <c r="H19" s="4">
+        <v>1677.4</v>
+      </c>
+      <c r="I19" s="4">
+        <v>1.9628000000000001</v>
+      </c>
+      <c r="J19" s="4">
+        <v>0.35322999999999999</v>
+      </c>
+      <c r="K19" s="4">
+        <v>3.5571000000000002</v>
+      </c>
+      <c r="L19" s="4">
+        <v>4.0984999999999996</v>
+      </c>
+      <c r="M19" s="4">
+        <v>5.9319999999999998E-2</v>
+      </c>
+      <c r="N19" s="3">
+        <v>2.5131999999999999</v>
+      </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" s="13"/>
       <c r="B20" s="16"/>
+      <c r="C20" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="D20" s="4">
+        <v>23.303999999999998</v>
+      </c>
+      <c r="E20" s="4">
+        <v>306.58</v>
+      </c>
+      <c r="F20" s="4">
+        <v>0.32123000000000002</v>
+      </c>
+      <c r="G20" s="4">
+        <v>4.2591999999999999</v>
+      </c>
+      <c r="H20" s="4">
+        <v>1822.6</v>
+      </c>
+      <c r="I20" s="4">
+        <v>1.6464000000000001</v>
+      </c>
+      <c r="J20" s="4">
+        <v>0.23887</v>
+      </c>
+      <c r="K20" s="4">
+        <v>2.9979</v>
+      </c>
+      <c r="L20" s="4">
+        <v>4.1620999999999997</v>
+      </c>
+      <c r="M20" s="4">
+        <v>2.9884999999999998E-3</v>
+      </c>
+      <c r="N20" s="3">
+        <v>2.3424999999999998</v>
+      </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" s="13"/>
       <c r="B21" s="16"/>
+      <c r="C21" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="D21" s="4">
+        <v>31.137</v>
+      </c>
+      <c r="E21" s="4">
+        <v>31.413</v>
+      </c>
+      <c r="F21" s="4">
+        <v>4.6002999999999998</v>
+      </c>
+      <c r="G21" s="4">
+        <v>3.6958000000000002</v>
+      </c>
+      <c r="H21" s="4">
+        <v>2583</v>
+      </c>
+      <c r="I21" s="4">
+        <v>1.2944</v>
+      </c>
+      <c r="J21" s="4">
+        <v>0.36685000000000001</v>
+      </c>
+      <c r="K21" s="4">
+        <v>3.8721000000000001</v>
+      </c>
+      <c r="L21" s="4">
+        <v>2.0034000000000001</v>
+      </c>
+      <c r="M21" s="4">
+        <v>0.2167</v>
+      </c>
+      <c r="N21" s="3">
+        <v>2.8479999999999999</v>
+      </c>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" s="13"/>
       <c r="B22" s="16"/>
+      <c r="C22" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="D22" s="4">
+        <v>29.725999999999999</v>
+      </c>
+      <c r="E22" s="4">
+        <v>45.991</v>
+      </c>
+      <c r="F22" s="4">
+        <v>2.3174000000000001</v>
+      </c>
+      <c r="G22" s="4">
+        <v>3.9613</v>
+      </c>
+      <c r="H22" s="4">
+        <v>2101.3000000000002</v>
+      </c>
+      <c r="I22" s="4">
+        <v>1.617</v>
+      </c>
+      <c r="J22" s="4">
+        <v>0.27362999999999998</v>
+      </c>
+      <c r="K22" s="4">
+        <v>3.2206000000000001</v>
+      </c>
+      <c r="L22" s="4">
+        <v>5.6994999999999996</v>
+      </c>
+      <c r="M22" s="4">
+        <v>0.96150999999999998</v>
+      </c>
+      <c r="N22" s="3">
+        <v>3.9527000000000001</v>
+      </c>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" s="13"/>
       <c r="B23" s="16"/>
+      <c r="C23" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="D23" s="4">
+        <v>0.85682000000000003</v>
+      </c>
+      <c r="E23" s="4">
+        <v>42.524000000000001</v>
+      </c>
+      <c r="F23" s="4">
+        <v>9.6282999999999994</v>
+      </c>
+      <c r="G23" s="4">
+        <v>4.5033000000000003</v>
+      </c>
+      <c r="H23" s="4">
+        <v>1707</v>
+      </c>
+      <c r="I23" s="4">
+        <v>1.2393000000000001</v>
+      </c>
+      <c r="J23" s="4">
+        <v>0.28849000000000002</v>
+      </c>
+      <c r="K23" s="4">
+        <v>3.4293</v>
+      </c>
+      <c r="L23" s="4">
+        <v>3.0653999999999999</v>
+      </c>
+      <c r="M23" s="4">
+        <v>0.11899999999999999</v>
+      </c>
+      <c r="N23" s="3">
+        <v>2.6208</v>
+      </c>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" s="13"/>
       <c r="B24" s="16"/>
+      <c r="C24" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="D24" s="4">
+        <v>4.4611000000000001</v>
+      </c>
+      <c r="E24" s="4">
+        <v>35.628</v>
+      </c>
+      <c r="F24" s="4">
+        <v>31.021000000000001</v>
+      </c>
+      <c r="G24" s="4">
+        <v>3.6185999999999998</v>
+      </c>
+      <c r="H24" s="4">
+        <v>3016.2</v>
+      </c>
+      <c r="I24" s="4">
+        <v>9.5056999999999992</v>
+      </c>
+      <c r="J24" s="4">
+        <v>0.33045999999999998</v>
+      </c>
+      <c r="K24" s="4">
+        <v>3.327</v>
+      </c>
+      <c r="L24" s="4">
+        <v>4.6459000000000001</v>
+      </c>
+      <c r="M24" s="4">
+        <v>0.20498</v>
+      </c>
+      <c r="N24" s="3">
+        <v>2.7280000000000002</v>
+      </c>
     </row>
     <row r="25" spans="1:15" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="14"/>
@@ -7161,42 +6922,402 @@
     <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27" s="13"/>
       <c r="B27" s="16"/>
+      <c r="C27" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="D27" s="4">
+        <v>4.8710000000000004</v>
+      </c>
+      <c r="E27" s="4">
+        <v>11.518000000000001</v>
+      </c>
+      <c r="F27" s="4">
+        <v>7.0281000000000002</v>
+      </c>
+      <c r="G27" s="4">
+        <v>4.2420999999999998</v>
+      </c>
+      <c r="H27" s="4">
+        <v>1138.3</v>
+      </c>
+      <c r="I27" s="4">
+        <v>1.2072000000000001</v>
+      </c>
+      <c r="J27" s="4">
+        <v>0.44550000000000001</v>
+      </c>
+      <c r="K27" s="4">
+        <v>3.8687</v>
+      </c>
+      <c r="L27" s="4">
+        <v>3.6877</v>
+      </c>
+      <c r="M27" s="4">
+        <v>0.25385000000000002</v>
+      </c>
+      <c r="N27" s="3">
+        <v>2.5308000000000002</v>
+      </c>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28" s="13"/>
       <c r="B28" s="16"/>
+      <c r="C28" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="D28" s="4">
+        <v>10.692</v>
+      </c>
+      <c r="E28" s="4">
+        <v>29.068000000000001</v>
+      </c>
+      <c r="F28" s="4">
+        <v>2.9830999999999999</v>
+      </c>
+      <c r="G28" s="4">
+        <v>3.7277999999999998</v>
+      </c>
+      <c r="H28" s="4">
+        <v>1433.5</v>
+      </c>
+      <c r="I28" s="2">
+        <v>2.3410000000000002</v>
+      </c>
+      <c r="J28" s="2">
+        <v>0.39410000000000001</v>
+      </c>
+      <c r="K28" s="2">
+        <v>3.3374000000000001</v>
+      </c>
+      <c r="L28" s="2">
+        <v>5.6124999999999998</v>
+      </c>
+      <c r="M28" s="2">
+        <v>0.94169000000000003</v>
+      </c>
+      <c r="N28" s="2">
+        <v>3.4904999999999999</v>
+      </c>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29" s="13"/>
       <c r="B29" s="16"/>
+      <c r="C29" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="D29" s="4">
+        <v>11.2</v>
+      </c>
+      <c r="E29" s="4">
+        <v>24.262</v>
+      </c>
+      <c r="F29" s="4">
+        <v>2.2614999999999998</v>
+      </c>
+      <c r="G29" s="4">
+        <v>3.9651000000000001</v>
+      </c>
+      <c r="H29" s="4">
+        <v>1163</v>
+      </c>
+      <c r="I29" s="4">
+        <v>1.7908999999999999</v>
+      </c>
+      <c r="J29" s="4">
+        <v>0.45981</v>
+      </c>
+      <c r="K29" s="4">
+        <v>3.9491000000000001</v>
+      </c>
+      <c r="L29" s="4">
+        <v>3.3142</v>
+      </c>
+      <c r="M29" s="4">
+        <v>0.20016999999999999</v>
+      </c>
+      <c r="N29" s="3">
+        <v>2.4437000000000002</v>
+      </c>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30" s="13"/>
       <c r="B30" s="16"/>
+      <c r="C30" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="D30" s="4">
+        <v>11.208</v>
+      </c>
+      <c r="E30" s="4">
+        <v>16.738</v>
+      </c>
+      <c r="F30" s="4">
+        <v>5.9587000000000003</v>
+      </c>
+      <c r="G30" s="4">
+        <v>3.6377000000000002</v>
+      </c>
+      <c r="H30" s="4">
+        <v>1530.1</v>
+      </c>
+      <c r="I30" s="4">
+        <v>1.0164</v>
+      </c>
+      <c r="J30" s="4">
+        <v>0.51859999999999995</v>
+      </c>
+      <c r="K30" s="4">
+        <v>4.4584999999999999</v>
+      </c>
+      <c r="L30" s="4">
+        <v>3.1135000000000002</v>
+      </c>
+      <c r="M30" s="4">
+        <v>0.38601000000000002</v>
+      </c>
+      <c r="N30" s="3">
+        <v>3.3180999999999998</v>
+      </c>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A31" s="13"/>
       <c r="B31" s="16"/>
+      <c r="C31" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="D31" s="4">
+        <v>10.45</v>
+      </c>
+      <c r="E31" s="4">
+        <v>14.769</v>
+      </c>
+      <c r="F31" s="4">
+        <v>7.8792</v>
+      </c>
+      <c r="G31" s="4">
+        <v>3.54</v>
+      </c>
+      <c r="H31" s="4">
+        <v>1787.3</v>
+      </c>
+      <c r="I31" s="4">
+        <v>1.3337000000000001</v>
+      </c>
+      <c r="J31" s="4">
+        <v>0.59784999999999999</v>
+      </c>
+      <c r="K31" s="4">
+        <v>4.8552999999999997</v>
+      </c>
+      <c r="L31" s="4">
+        <v>2.6320000000000001</v>
+      </c>
+      <c r="M31" s="4">
+        <v>0.34475</v>
+      </c>
+      <c r="N31" s="3">
+        <v>3.0926</v>
+      </c>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A32" s="13"/>
       <c r="B32" s="16"/>
+      <c r="C32" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D32" s="4">
+        <v>11.010999999999999</v>
+      </c>
+      <c r="E32" s="4">
+        <v>11.071</v>
+      </c>
+      <c r="F32" s="4">
+        <v>13.523</v>
+      </c>
+      <c r="G32" s="4">
+        <v>3.5672000000000001</v>
+      </c>
+      <c r="H32" s="4">
+        <v>1593.8</v>
+      </c>
+      <c r="I32" s="4">
+        <v>2.0019</v>
+      </c>
+      <c r="J32" s="4">
+        <v>0.50361</v>
+      </c>
+      <c r="K32" s="4">
+        <v>4.1786000000000003</v>
+      </c>
+      <c r="L32" s="4">
+        <v>4.2843</v>
+      </c>
+      <c r="M32" s="4">
+        <v>0.22523000000000001</v>
+      </c>
+      <c r="N32" s="3">
+        <v>2.6124999999999998</v>
+      </c>
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A33" s="13"/>
       <c r="B33" s="16"/>
+      <c r="C33" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="D33" s="4">
+        <v>5.6656000000000004</v>
+      </c>
+      <c r="E33" s="4">
+        <v>8.2222000000000008</v>
+      </c>
+      <c r="F33" s="4">
+        <v>14.47</v>
+      </c>
+      <c r="G33" s="4">
+        <v>4.3000999999999996</v>
+      </c>
+      <c r="H33" s="4">
+        <v>1000.8</v>
+      </c>
+      <c r="I33" s="4">
+        <v>1.3364</v>
+      </c>
+      <c r="J33" s="4">
+        <v>0.73826000000000003</v>
+      </c>
+      <c r="K33" s="4">
+        <v>6.1936999999999998</v>
+      </c>
+      <c r="L33" s="4">
+        <v>2.6962999999999999</v>
+      </c>
+      <c r="M33" s="4">
+        <v>0.35518</v>
+      </c>
+      <c r="N33" s="3">
+        <v>3.2061000000000002</v>
+      </c>
     </row>
     <row r="34" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A34" s="13"/>
       <c r="B34" s="16"/>
+      <c r="C34" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="D34" s="4">
+        <v>15.185</v>
+      </c>
+      <c r="E34" s="4">
+        <v>64.875</v>
+      </c>
+      <c r="F34" s="4">
+        <v>1.4525999999999999</v>
+      </c>
+      <c r="G34" s="4">
+        <v>3.2002999999999999</v>
+      </c>
+      <c r="H34" s="4">
+        <v>2110.6</v>
+      </c>
+      <c r="I34" s="4">
+        <v>1.7833000000000001</v>
+      </c>
+      <c r="J34" s="4">
+        <v>0.51853000000000005</v>
+      </c>
+      <c r="K34" s="4">
+        <v>4.2645</v>
+      </c>
+      <c r="L34" s="4">
+        <v>3.7526000000000002</v>
+      </c>
+      <c r="M34" s="4">
+        <v>0.20075000000000001</v>
+      </c>
+      <c r="N34" s="3">
+        <v>2.5205000000000002</v>
+      </c>
     </row>
     <row r="35" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A35" s="13"/>
       <c r="B35" s="16"/>
+      <c r="C35" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="D35" s="4">
+        <v>8.0571999999999999</v>
+      </c>
+      <c r="E35" s="4">
+        <v>29.803999999999998</v>
+      </c>
+      <c r="F35" s="4">
+        <v>2.5836000000000001</v>
+      </c>
+      <c r="G35" s="4">
+        <v>4.0204000000000004</v>
+      </c>
+      <c r="H35" s="4">
+        <v>1210.4000000000001</v>
+      </c>
+      <c r="I35" s="4">
+        <v>1.2011000000000001</v>
+      </c>
+      <c r="J35" s="4">
+        <v>0.49431999999999998</v>
+      </c>
+      <c r="K35" s="4">
+        <v>4.3479000000000001</v>
+      </c>
+      <c r="L35" s="4">
+        <v>2.7725</v>
+      </c>
+      <c r="M35" s="4">
+        <v>0.29389999999999999</v>
+      </c>
+      <c r="N35" s="3">
+        <v>2.7284999999999999</v>
+      </c>
     </row>
     <row r="36" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A36" s="13"/>
       <c r="B36" s="16"/>
+      <c r="C36" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="D36" s="4">
+        <v>7.5292000000000003</v>
+      </c>
+      <c r="E36" s="4">
+        <v>23.504999999999999</v>
+      </c>
+      <c r="F36" s="4">
+        <v>4.9898999999999996</v>
+      </c>
+      <c r="G36" s="4">
+        <v>3.8622999999999998</v>
+      </c>
+      <c r="H36" s="4">
+        <v>1369.1</v>
+      </c>
+      <c r="I36" s="4">
+        <v>1.9939</v>
+      </c>
+      <c r="J36" s="4">
+        <v>0.36113000000000001</v>
+      </c>
+      <c r="K36" s="4">
+        <v>3.2098</v>
+      </c>
+      <c r="L36" s="4">
+        <v>1.6549</v>
+      </c>
+      <c r="M36" s="4">
+        <v>0.25001000000000001</v>
+      </c>
+      <c r="N36" s="3">
+        <v>3.9885000000000002</v>
+      </c>
     </row>
     <row r="37" spans="1:15" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="14"/>
@@ -7216,84 +7337,402 @@
     <row r="39" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A39" s="13"/>
       <c r="B39" s="16"/>
+      <c r="C39" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="D39" s="4">
+        <v>4.8238000000000003</v>
+      </c>
+      <c r="E39" s="4">
+        <v>378.86</v>
+      </c>
+      <c r="F39" s="4">
+        <v>0.14230000000000001</v>
+      </c>
+      <c r="G39" s="4">
+        <v>4.4020999999999999</v>
+      </c>
+      <c r="H39" s="4">
+        <v>1006.9</v>
+      </c>
+      <c r="I39" s="4">
+        <v>1.3282</v>
+      </c>
+      <c r="J39" s="4">
+        <v>0.54573000000000005</v>
+      </c>
+      <c r="K39" s="4">
+        <v>4.6946000000000003</v>
+      </c>
+      <c r="L39" s="4">
+        <v>3.1678999999999999</v>
+      </c>
+      <c r="M39" s="4">
+        <v>0.25372</v>
+      </c>
+      <c r="N39" s="3">
+        <v>2.5291999999999999</v>
+      </c>
     </row>
     <row r="40" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A40" s="13"/>
       <c r="B40" s="16"/>
       <c r="C40" s="8" t="s">
-        <v>32</v>
+        <v>45</v>
       </c>
       <c r="D40" s="4">
-        <v>7.1031000000000004</v>
+        <v>7.1036999999999999</v>
       </c>
       <c r="E40" s="4">
-        <v>56.988999999999997</v>
+        <v>48.234999999999999</v>
       </c>
       <c r="F40" s="4">
-        <v>4.2892999999999999</v>
+        <v>4.2972000000000001</v>
       </c>
       <c r="G40" s="4">
-        <v>3.3986999999999998</v>
+        <v>3.4083999999999999</v>
       </c>
       <c r="H40" s="4">
-        <v>1829.5</v>
-      </c>
-      <c r="I40" s="4">
-        <v>1.3612</v>
-      </c>
-      <c r="J40" s="4">
-        <v>0.34809000000000001</v>
-      </c>
-      <c r="K40" s="4">
-        <v>3.1223000000000001</v>
-      </c>
-      <c r="L40" s="4">
-        <v>12.302</v>
-      </c>
-      <c r="M40" s="4">
-        <v>0.21134</v>
-      </c>
-      <c r="N40" s="3">
-        <v>3.3576999999999999</v>
+        <v>1829.9</v>
+      </c>
+      <c r="I40" s="2">
+        <v>1.3602000000000001</v>
+      </c>
+      <c r="J40" s="2">
+        <v>0.34182000000000001</v>
+      </c>
+      <c r="K40" s="2">
+        <v>3.1635</v>
+      </c>
+      <c r="L40" s="2">
+        <v>12.426</v>
+      </c>
+      <c r="M40" s="2">
+        <v>0.21156</v>
+      </c>
+      <c r="N40" s="2">
+        <v>3.3578000000000001</v>
       </c>
     </row>
     <row r="41" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A41" s="13"/>
       <c r="B41" s="16"/>
-      <c r="I41" s="2"/>
-      <c r="J41" s="2"/>
-      <c r="K41" s="2"/>
-      <c r="L41" s="2"/>
-      <c r="M41" s="2"/>
-      <c r="N41" s="1"/>
+      <c r="C41" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="D41" s="4">
+        <v>3.0461</v>
+      </c>
+      <c r="E41" s="4">
+        <v>19.608000000000001</v>
+      </c>
+      <c r="F41" s="4">
+        <v>32.420999999999999</v>
+      </c>
+      <c r="G41" s="4">
+        <v>3.2736000000000001</v>
+      </c>
+      <c r="H41" s="4">
+        <v>2022.3</v>
+      </c>
+      <c r="I41" s="2">
+        <v>1.9328000000000001</v>
+      </c>
+      <c r="J41" s="2">
+        <v>0.59299999999999997</v>
+      </c>
+      <c r="K41" s="2">
+        <v>4.7255000000000003</v>
+      </c>
+      <c r="L41" s="2">
+        <v>2.6515</v>
+      </c>
+      <c r="M41" s="2">
+        <v>0.25479000000000002</v>
+      </c>
+      <c r="N41" s="1">
+        <v>2.5724</v>
+      </c>
     </row>
     <row r="42" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A42" s="13"/>
       <c r="B42" s="16"/>
+      <c r="C42" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="D42" s="4">
+        <v>4.6340000000000003</v>
+      </c>
+      <c r="E42" s="4">
+        <v>18.606999999999999</v>
+      </c>
+      <c r="F42" s="4">
+        <v>24.896000000000001</v>
+      </c>
+      <c r="G42" s="4">
+        <v>3.3435999999999999</v>
+      </c>
+      <c r="H42" s="4">
+        <v>1999.7</v>
+      </c>
+      <c r="I42" s="4">
+        <v>2.2488000000000001</v>
+      </c>
+      <c r="J42" s="4">
+        <v>0.27339999999999998</v>
+      </c>
+      <c r="K42" s="4">
+        <v>2.6326000000000001</v>
+      </c>
+      <c r="L42" s="4">
+        <v>4.8822000000000001</v>
+      </c>
+      <c r="M42" s="4">
+        <v>0.17643</v>
+      </c>
+      <c r="N42" s="3">
+        <v>2.3942000000000001</v>
+      </c>
     </row>
     <row r="43" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A43" s="13"/>
       <c r="B43" s="16"/>
+      <c r="C43" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="D43" s="4">
+        <v>16.286999999999999</v>
+      </c>
+      <c r="E43" s="4">
+        <v>181.45</v>
+      </c>
+      <c r="F43" s="4">
+        <v>0.52517000000000003</v>
+      </c>
+      <c r="G43" s="4">
+        <v>3.0160999999999998</v>
+      </c>
+      <c r="H43" s="4">
+        <v>2606.1999999999998</v>
+      </c>
+      <c r="I43" s="4">
+        <v>7.6341000000000001</v>
+      </c>
+      <c r="J43" s="4">
+        <v>0.55245999999999995</v>
+      </c>
+      <c r="K43" s="4">
+        <v>7.7807000000000004</v>
+      </c>
+      <c r="L43" s="4">
+        <v>2.0291999999999999</v>
+      </c>
+      <c r="M43" s="4">
+        <v>0.31213000000000002</v>
+      </c>
+      <c r="N43" s="3">
+        <v>2.8618000000000001</v>
+      </c>
     </row>
     <row r="44" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A44" s="13"/>
       <c r="B44" s="16"/>
+      <c r="C44" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="D44" s="4">
+        <v>9.5312999999999999</v>
+      </c>
+      <c r="E44" s="4">
+        <v>148.61000000000001</v>
+      </c>
+      <c r="F44" s="4">
+        <v>0.37484000000000001</v>
+      </c>
+      <c r="G44" s="4">
+        <v>3.9621</v>
+      </c>
+      <c r="H44" s="4">
+        <v>1253.9000000000001</v>
+      </c>
+      <c r="I44" s="4">
+        <v>2.3045</v>
+      </c>
+      <c r="J44" s="4">
+        <v>0.34014</v>
+      </c>
+      <c r="K44" s="4">
+        <v>3.0451000000000001</v>
+      </c>
+      <c r="L44" s="4">
+        <v>2.7208000000000001</v>
+      </c>
+      <c r="M44" s="4">
+        <v>6.7532999999999996E-2</v>
+      </c>
+      <c r="N44" s="3">
+        <v>2.4268999999999998</v>
+      </c>
     </row>
     <row r="45" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A45" s="13"/>
       <c r="B45" s="16"/>
+      <c r="C45" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="D45" s="4">
+        <v>6.3647</v>
+      </c>
+      <c r="E45" s="4">
+        <v>149.54</v>
+      </c>
+      <c r="F45" s="4">
+        <v>0.43913000000000002</v>
+      </c>
+      <c r="G45" s="4">
+        <v>4.1839000000000004</v>
+      </c>
+      <c r="H45" s="4">
+        <v>1127.5999999999999</v>
+      </c>
+      <c r="I45" s="4">
+        <v>2.2016</v>
+      </c>
+      <c r="J45" s="4">
+        <v>0.28632000000000002</v>
+      </c>
+      <c r="K45" s="4">
+        <v>2.7416</v>
+      </c>
+      <c r="L45" s="4">
+        <v>1.1881999999999999</v>
+      </c>
+      <c r="M45" s="4">
+        <v>0.70389999999999997</v>
+      </c>
+      <c r="N45" s="3">
+        <v>8.2974999999999993E-2</v>
+      </c>
     </row>
     <row r="46" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A46" s="13"/>
       <c r="B46" s="16"/>
+      <c r="C46" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="D46" s="4">
+        <v>12.622</v>
+      </c>
+      <c r="E46" s="4">
+        <v>15.441000000000001</v>
+      </c>
+      <c r="F46" s="4">
+        <v>4.5385999999999997</v>
+      </c>
+      <c r="G46" s="4">
+        <v>3.7305000000000001</v>
+      </c>
+      <c r="H46" s="4">
+        <v>1371.6</v>
+      </c>
+      <c r="I46" s="4">
+        <v>2.2448999999999999</v>
+      </c>
+      <c r="J46" s="4">
+        <v>0.40698000000000001</v>
+      </c>
+      <c r="K46" s="4">
+        <v>3.5036</v>
+      </c>
+      <c r="L46" s="4">
+        <v>4.0568</v>
+      </c>
+      <c r="M46" s="4">
+        <v>0.21132000000000001</v>
+      </c>
+      <c r="N46" s="3">
+        <v>2.4597000000000002</v>
+      </c>
     </row>
     <row r="47" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A47" s="13"/>
       <c r="B47" s="16"/>
+      <c r="C47" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="D47" s="4">
+        <v>12.256</v>
+      </c>
+      <c r="E47" s="4">
+        <v>273.68</v>
+      </c>
+      <c r="F47" s="4">
+        <v>0.20866000000000001</v>
+      </c>
+      <c r="G47" s="4">
+        <v>3.8422000000000001</v>
+      </c>
+      <c r="H47" s="4">
+        <v>1242.3</v>
+      </c>
+      <c r="I47" s="4">
+        <v>1.8718999999999999</v>
+      </c>
+      <c r="J47" s="4">
+        <v>0.38352999999999998</v>
+      </c>
+      <c r="K47" s="4">
+        <v>3.4464999999999999</v>
+      </c>
+      <c r="L47" s="4">
+        <v>3.8252999999999999</v>
+      </c>
+      <c r="M47" s="4">
+        <v>0.19616</v>
+      </c>
+      <c r="N47" s="3">
+        <v>2.4363999999999999</v>
+      </c>
     </row>
     <row r="48" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A48" s="13"/>
       <c r="B48" s="16"/>
+      <c r="C48" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="D48" s="4">
+        <v>7.0439999999999996</v>
+      </c>
+      <c r="E48" s="4">
+        <v>16.175000000000001</v>
+      </c>
+      <c r="F48" s="4">
+        <v>6.7949000000000002</v>
+      </c>
+      <c r="G48" s="4">
+        <v>4.1207000000000003</v>
+      </c>
+      <c r="H48" s="4">
+        <v>1090</v>
+      </c>
+      <c r="I48" s="4">
+        <v>2.2446999999999999</v>
+      </c>
+      <c r="J48" s="4">
+        <v>0.43214999999999998</v>
+      </c>
+      <c r="K48" s="4">
+        <v>3.6272000000000002</v>
+      </c>
+      <c r="L48" s="4">
+        <v>5.3937999999999997</v>
+      </c>
+      <c r="M48" s="4">
+        <v>0.16178999999999999</v>
+      </c>
+      <c r="N48" s="3">
+        <v>2.391</v>
+      </c>
     </row>
     <row r="49" spans="1:15" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="14"/>
@@ -7414,18 +7853,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A38:A49"/>
+    <mergeCell ref="B38:B49"/>
+    <mergeCell ref="A50:A61"/>
+    <mergeCell ref="B50:B61"/>
+    <mergeCell ref="A62:A73"/>
+    <mergeCell ref="B62:B73"/>
     <mergeCell ref="A2:A13"/>
     <mergeCell ref="B2:B13"/>
     <mergeCell ref="A14:A25"/>
     <mergeCell ref="B14:B25"/>
     <mergeCell ref="A26:A37"/>
     <mergeCell ref="B26:B37"/>
-    <mergeCell ref="A38:A49"/>
-    <mergeCell ref="B38:B49"/>
-    <mergeCell ref="A50:A61"/>
-    <mergeCell ref="B50:B61"/>
-    <mergeCell ref="A62:A73"/>
-    <mergeCell ref="B62:B73"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
changed to evpwd model and changed run scripts
</commit_message>
<xml_diff>
--- a/scripts/__other__/__sem__.xlsx
+++ b/scripts/__other__/__sem__.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Janzen\Desktop\code\moga_neml\scripts\__other__\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AC24A10-5533-4A0E-9EBE-FC11266CA989}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{303781E2-5759-4A5B-9253-DB6772B63AD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="evp" sheetId="13" r:id="rId1"/>
@@ -2142,18 +2142,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A38:A49"/>
+    <mergeCell ref="B38:B49"/>
+    <mergeCell ref="A50:A61"/>
+    <mergeCell ref="B50:B61"/>
+    <mergeCell ref="A62:A73"/>
+    <mergeCell ref="B62:B73"/>
     <mergeCell ref="A2:A13"/>
     <mergeCell ref="B2:B13"/>
     <mergeCell ref="A14:A25"/>
     <mergeCell ref="B14:B25"/>
     <mergeCell ref="A26:A37"/>
     <mergeCell ref="B26:B37"/>
-    <mergeCell ref="A38:A49"/>
-    <mergeCell ref="B38:B49"/>
-    <mergeCell ref="A50:A61"/>
-    <mergeCell ref="B50:B61"/>
-    <mergeCell ref="A62:A73"/>
-    <mergeCell ref="B62:B73"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -3621,18 +3621,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A38:A49"/>
+    <mergeCell ref="B38:B49"/>
+    <mergeCell ref="A50:A61"/>
+    <mergeCell ref="B50:B61"/>
+    <mergeCell ref="A62:A73"/>
+    <mergeCell ref="B62:B73"/>
     <mergeCell ref="A2:A13"/>
     <mergeCell ref="B2:B13"/>
     <mergeCell ref="A14:A25"/>
     <mergeCell ref="B14:B25"/>
     <mergeCell ref="A26:A37"/>
     <mergeCell ref="B26:B37"/>
-    <mergeCell ref="A38:A49"/>
-    <mergeCell ref="B38:B49"/>
-    <mergeCell ref="A50:A61"/>
-    <mergeCell ref="B50:B61"/>
-    <mergeCell ref="A62:A73"/>
-    <mergeCell ref="B62:B73"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -5100,18 +5100,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A2:A13"/>
+    <mergeCell ref="B2:B13"/>
+    <mergeCell ref="A14:A25"/>
+    <mergeCell ref="B14:B25"/>
+    <mergeCell ref="A26:A37"/>
+    <mergeCell ref="B26:B37"/>
     <mergeCell ref="A38:A49"/>
     <mergeCell ref="B38:B49"/>
     <mergeCell ref="A50:A61"/>
     <mergeCell ref="B50:B61"/>
     <mergeCell ref="A62:A73"/>
     <mergeCell ref="B62:B73"/>
-    <mergeCell ref="A2:A13"/>
-    <mergeCell ref="B2:B13"/>
-    <mergeCell ref="A14:A25"/>
-    <mergeCell ref="B14:B25"/>
-    <mergeCell ref="A26:A37"/>
-    <mergeCell ref="B26:B37"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -5122,8 +5122,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C18A26E-30CA-4E63-A18A-C9C101DAF33C}">
   <dimension ref="A1:O73"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>
@@ -5857,18 +5857,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A38:A49"/>
+    <mergeCell ref="B38:B49"/>
+    <mergeCell ref="A50:A61"/>
+    <mergeCell ref="B50:B61"/>
+    <mergeCell ref="A62:A73"/>
+    <mergeCell ref="B62:B73"/>
     <mergeCell ref="A2:A13"/>
     <mergeCell ref="B2:B13"/>
     <mergeCell ref="A14:A25"/>
     <mergeCell ref="B14:B25"/>
     <mergeCell ref="A26:A37"/>
     <mergeCell ref="B26:B37"/>
-    <mergeCell ref="A38:A49"/>
-    <mergeCell ref="B38:B49"/>
-    <mergeCell ref="A50:A61"/>
-    <mergeCell ref="B50:B61"/>
-    <mergeCell ref="A62:A73"/>
-    <mergeCell ref="B62:B73"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -6284,18 +6284,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A2:A13"/>
+    <mergeCell ref="B2:B13"/>
+    <mergeCell ref="A14:A25"/>
+    <mergeCell ref="B14:B25"/>
+    <mergeCell ref="A26:A37"/>
+    <mergeCell ref="B26:B37"/>
     <mergeCell ref="A38:A49"/>
     <mergeCell ref="B38:B49"/>
     <mergeCell ref="A50:A61"/>
     <mergeCell ref="B50:B61"/>
     <mergeCell ref="A62:A73"/>
     <mergeCell ref="B62:B73"/>
-    <mergeCell ref="A2:A13"/>
-    <mergeCell ref="B2:B13"/>
-    <mergeCell ref="A14:A25"/>
-    <mergeCell ref="B14:B25"/>
-    <mergeCell ref="A26:A37"/>
-    <mergeCell ref="B26:B37"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -6304,11 +6304,11 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1D987DC-5A74-4932-B56A-48A4420F0E95}">
-  <dimension ref="A1:O73"/>
+  <dimension ref="A1:Z73"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O3" sqref="O3"/>
+      <selection pane="bottomLeft" activeCell="Z5" sqref="P3:Z5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6322,7 +6322,7 @@
     <col min="16" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -6367,7 +6367,7 @@
       </c>
       <c r="O1" s="11"/>
     </row>
-    <row r="2" spans="1:15" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:26" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="12">
         <v>800</v>
       </c>
@@ -6375,7 +6375,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A3" s="13"/>
       <c r="B3" s="16"/>
       <c r="C3" s="8" t="s">
@@ -6414,8 +6414,14 @@
       <c r="N3" s="1">
         <v>3.1743000000000001</v>
       </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="U3" s="2"/>
+      <c r="V3" s="2"/>
+      <c r="W3" s="2"/>
+      <c r="X3" s="2"/>
+      <c r="Y3" s="2"/>
+      <c r="Z3" s="1"/>
+    </row>
+    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A4" s="13"/>
       <c r="B4" s="16"/>
       <c r="C4" s="8" t="s">
@@ -6454,8 +6460,10 @@
       <c r="N4" s="1">
         <v>2.7471999999999999</v>
       </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="U4" s="2"/>
+      <c r="X4" s="2"/>
+    </row>
+    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A5" s="13"/>
       <c r="B5" s="16"/>
       <c r="C5" s="8" t="s">
@@ -6495,7 +6503,7 @@
         <v>3.5432999999999999</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A6" s="13"/>
       <c r="B6" s="16"/>
       <c r="C6" s="8" t="s">
@@ -6535,7 +6543,7 @@
         <v>3.1581999999999999</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A7" s="13"/>
       <c r="B7" s="16"/>
       <c r="C7" s="8" t="s">
@@ -6575,7 +6583,7 @@
         <v>2.4053</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A8" s="13"/>
       <c r="B8" s="16"/>
       <c r="C8" s="8" t="s">
@@ -6615,7 +6623,7 @@
         <v>2.9091</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A9" s="13"/>
       <c r="B9" s="16"/>
       <c r="C9" s="8" t="s">
@@ -6655,7 +6663,7 @@
         <v>2.4855999999999998</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A10" s="13"/>
       <c r="B10" s="16"/>
       <c r="C10" s="8" t="s">
@@ -6695,7 +6703,7 @@
         <v>3.0878999999999999</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A11" s="13"/>
       <c r="B11" s="16"/>
       <c r="C11" s="8" t="s">
@@ -6735,7 +6743,7 @@
         <v>3.1248</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A12" s="13"/>
       <c r="B12" s="16"/>
       <c r="C12" s="8" t="s">
@@ -6775,14 +6783,14 @@
         <v>3.5486</v>
       </c>
     </row>
-    <row r="13" spans="1:15" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:26" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="14"/>
       <c r="B13" s="17"/>
       <c r="C13" s="7"/>
       <c r="N13" s="6"/>
       <c r="O13" s="11"/>
     </row>
-    <row r="14" spans="1:15" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:26" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="12">
         <v>800</v>
       </c>
@@ -6790,7 +6798,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A15" s="13"/>
       <c r="B15" s="16"/>
       <c r="C15" s="8" t="s">
@@ -6830,7 +6838,7 @@
         <v>3.1442999999999999</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A16" s="13"/>
       <c r="B16" s="16"/>
       <c r="C16" s="8" t="s">
@@ -8139,18 +8147,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A2:A13"/>
+    <mergeCell ref="B2:B13"/>
+    <mergeCell ref="A14:A25"/>
+    <mergeCell ref="B14:B25"/>
+    <mergeCell ref="A26:A37"/>
+    <mergeCell ref="B26:B37"/>
     <mergeCell ref="A38:A49"/>
     <mergeCell ref="B38:B49"/>
     <mergeCell ref="A50:A61"/>
     <mergeCell ref="B50:B61"/>
     <mergeCell ref="A62:A73"/>
     <mergeCell ref="B62:B73"/>
-    <mergeCell ref="A2:A13"/>
-    <mergeCell ref="B2:B13"/>
-    <mergeCell ref="A14:A25"/>
-    <mergeCell ref="B14:B25"/>
-    <mergeCell ref="A26:A37"/>
-    <mergeCell ref="B26:B37"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
Changed 1000C exp data
</commit_message>
<xml_diff>
--- a/scripts/__other__/__sem__.xlsx
+++ b/scripts/__other__/__sem__.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Janzen\Desktop\code\moga_neml\scripts\__other__\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{303781E2-5759-4A5B-9253-DB6772B63AD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46A0BBAC-FE17-4C96-974E-6A56E8757070}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="evp" sheetId="13" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="401" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="397" uniqueCount="47">
   <si>
     <t>temp</t>
   </si>
@@ -182,9 +182,6 @@
   </si>
   <si>
     <t>5; 9</t>
-  </si>
-  <si>
-    <t>6; 7</t>
   </si>
 </sst>
 </file>
@@ -648,9 +645,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4D7A15E-4182-42F6-82DA-99E9B04906BA}">
   <dimension ref="A1:Q73"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D4" sqref="D4:H4"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F55" sqref="F55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2035,14 +2032,68 @@
     <row r="51" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A51" s="13"/>
       <c r="B51" s="16"/>
+      <c r="C51" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D51" s="4">
+        <v>1.9315</v>
+      </c>
+      <c r="E51" s="4">
+        <v>481.1</v>
+      </c>
+      <c r="F51" s="4">
+        <v>2.1642000000000002E-2</v>
+      </c>
+      <c r="G51" s="4">
+        <v>4.1571999999999996</v>
+      </c>
+      <c r="H51" s="3">
+        <v>723.11</v>
+      </c>
     </row>
     <row r="52" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A52" s="13"/>
       <c r="B52" s="16"/>
+      <c r="C52" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="D52" s="4">
+        <v>3.746</v>
+      </c>
+      <c r="E52" s="4">
+        <v>8.6539999999999999</v>
+      </c>
+      <c r="F52" s="4">
+        <v>4.2439</v>
+      </c>
+      <c r="G52" s="4">
+        <v>3.9319999999999999</v>
+      </c>
+      <c r="H52" s="3">
+        <v>749.09</v>
+      </c>
     </row>
     <row r="53" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A53" s="13"/>
       <c r="B53" s="16"/>
+      <c r="C53" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="D53" s="4">
+        <v>4.6150000000000002E-3</v>
+      </c>
+      <c r="E53" s="4">
+        <v>6.1843000000000004</v>
+      </c>
+      <c r="F53" s="4">
+        <v>2.2823000000000002</v>
+      </c>
+      <c r="G53" s="4">
+        <v>4.8326000000000002</v>
+      </c>
+      <c r="H53" s="3">
+        <v>460.27</v>
+      </c>
     </row>
     <row r="54" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A54" s="13"/>
@@ -2093,6 +2144,24 @@
     <row r="63" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A63" s="13"/>
       <c r="B63" s="16"/>
+      <c r="C63" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D63" s="4">
+        <v>0.26123000000000002</v>
+      </c>
+      <c r="E63" s="4">
+        <v>35.054000000000002</v>
+      </c>
+      <c r="F63" s="4">
+        <v>0.42681000000000002</v>
+      </c>
+      <c r="G63" s="4">
+        <v>4.7435999999999998</v>
+      </c>
+      <c r="H63" s="3">
+        <v>490.7</v>
+      </c>
     </row>
     <row r="64" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A64" s="13"/>
@@ -5124,7 +5193,7 @@
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C41" sqref="C41"/>
+      <selection pane="bottomLeft" activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5195,7 +5264,7 @@
       <c r="A3" s="13"/>
       <c r="B3" s="16"/>
       <c r="C3" s="8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D3" s="4">
         <v>17.216999999999999</v>
@@ -5213,103 +5282,43 @@
         <v>1783.5</v>
       </c>
       <c r="I3" s="2">
-        <v>1.5566</v>
+        <v>2.0167000000000002</v>
       </c>
       <c r="J3" s="2">
-        <v>0.29131000000000001</v>
+        <v>27.012</v>
       </c>
       <c r="K3" s="2">
-        <v>3.3172999999999999</v>
+        <v>187.86</v>
       </c>
       <c r="L3" s="2">
-        <v>1.5367999999999999</v>
+        <v>9.6981000000000002</v>
       </c>
       <c r="M3" s="2">
-        <v>0.48293999999999998</v>
+        <v>87.406999999999996</v>
       </c>
       <c r="N3" s="1">
-        <v>2.7461000000000002</v>
+        <v>320.89</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="13"/>
       <c r="B4" s="16"/>
-      <c r="C4" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="D4" s="4">
-        <v>5.6908000000000003</v>
-      </c>
-      <c r="E4" s="4">
-        <v>66.626999999999995</v>
-      </c>
-      <c r="F4" s="4">
-        <v>1.9851000000000001</v>
-      </c>
-      <c r="G4" s="4">
-        <v>4.7723000000000004</v>
-      </c>
-      <c r="H4" s="4">
-        <v>1621.6</v>
-      </c>
-      <c r="I4" s="2">
-        <v>1.9604999999999999</v>
-      </c>
-      <c r="J4" s="2">
-        <v>0.30275000000000002</v>
-      </c>
-      <c r="K4" s="2">
-        <v>3.2364999999999999</v>
-      </c>
-      <c r="L4" s="2">
-        <v>12.154999999999999</v>
-      </c>
-      <c r="M4" s="2">
-        <v>0.52964999999999995</v>
-      </c>
-      <c r="N4" s="2">
-        <v>2.9596</v>
-      </c>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
+      <c r="L4" s="2"/>
+      <c r="M4" s="2"/>
+      <c r="N4" s="2"/>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="13"/>
       <c r="B5" s="16"/>
-      <c r="C5" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="D5" s="4">
-        <v>9.3076000000000008</v>
-      </c>
-      <c r="E5" s="4">
-        <v>32.595999999999997</v>
-      </c>
-      <c r="F5" s="4">
-        <v>5.8113999999999999</v>
-      </c>
-      <c r="G5" s="4">
-        <v>4.5263</v>
-      </c>
-      <c r="H5" s="4">
-        <v>1775.9</v>
-      </c>
-      <c r="I5" s="2">
-        <v>2.0874999999999999</v>
-      </c>
-      <c r="J5" s="2">
-        <v>0.46390999999999999</v>
-      </c>
-      <c r="K5" s="2">
-        <v>4.1624999999999996</v>
-      </c>
-      <c r="L5" s="2">
-        <v>2.0491000000000001</v>
-      </c>
-      <c r="M5" s="2">
-        <v>0.90242</v>
-      </c>
-      <c r="N5" s="2">
-        <v>3.3069999999999999</v>
-      </c>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2"/>
+      <c r="L5" s="2"/>
+      <c r="M5" s="2"/>
+      <c r="N5" s="2"/>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="13"/>
@@ -5318,42 +5327,17 @@
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="13"/>
       <c r="B7" s="16"/>
-      <c r="C7" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="D7" s="2">
-        <v>4.1862000000000004</v>
-      </c>
-      <c r="E7" s="2">
-        <v>84.548000000000002</v>
-      </c>
-      <c r="F7" s="2">
-        <v>2.1122999999999998</v>
-      </c>
-      <c r="G7" s="2">
-        <v>4.7751999999999999</v>
-      </c>
-      <c r="H7" s="2">
-        <v>1574.3</v>
-      </c>
-      <c r="I7" s="2">
-        <v>1.6472</v>
-      </c>
-      <c r="J7" s="2">
-        <v>0.34209000000000001</v>
-      </c>
-      <c r="K7" s="2">
-        <v>3.5358000000000001</v>
-      </c>
-      <c r="L7" s="2">
-        <v>10.343</v>
-      </c>
-      <c r="M7" s="2">
-        <v>0.55237999999999998</v>
-      </c>
-      <c r="N7" s="2">
-        <v>2.4053</v>
-      </c>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="2"/>
+      <c r="L7" s="2"/>
+      <c r="M7" s="2"/>
+      <c r="N7" s="2"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="13"/>
@@ -5407,82 +5391,16 @@
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" s="13"/>
       <c r="B17" s="16"/>
-      <c r="C17" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="D17" s="4">
-        <v>11.45</v>
-      </c>
-      <c r="E17" s="4">
-        <v>53.151000000000003</v>
-      </c>
-      <c r="F17" s="4">
-        <v>7.1665999999999999</v>
-      </c>
-      <c r="G17" s="4">
-        <v>3.9502000000000002</v>
-      </c>
-      <c r="H17" s="4">
-        <v>2221.6</v>
-      </c>
-      <c r="I17" s="2">
-        <v>1.2526999999999999</v>
-      </c>
-      <c r="J17" s="2">
-        <v>0.29722999999999999</v>
-      </c>
-      <c r="K17" s="2">
-        <v>3.3908999999999998</v>
-      </c>
-      <c r="L17" s="2">
-        <v>7.8418999999999999</v>
-      </c>
-      <c r="M17" s="2">
-        <v>0.71702999999999995</v>
-      </c>
-      <c r="N17" s="2">
-        <v>2.2921999999999998</v>
-      </c>
+      <c r="I17" s="2"/>
+      <c r="J17" s="2"/>
+      <c r="K17" s="2"/>
+      <c r="L17" s="2"/>
+      <c r="M17" s="2"/>
+      <c r="N17" s="2"/>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" s="13"/>
       <c r="B18" s="16"/>
-      <c r="C18" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="D18" s="4">
-        <v>37.741999999999997</v>
-      </c>
-      <c r="E18" s="4">
-        <v>49.122999999999998</v>
-      </c>
-      <c r="F18" s="4">
-        <v>2.4996</v>
-      </c>
-      <c r="G18" s="4">
-        <v>3.4102000000000001</v>
-      </c>
-      <c r="H18" s="4">
-        <v>3172</v>
-      </c>
-      <c r="I18" s="4">
-        <v>1.4922</v>
-      </c>
-      <c r="J18" s="4">
-        <v>0.29803000000000002</v>
-      </c>
-      <c r="K18" s="4">
-        <v>3.3704999999999998</v>
-      </c>
-      <c r="L18" s="4">
-        <v>10.712</v>
-      </c>
-      <c r="M18" s="4">
-        <v>0.71250000000000002</v>
-      </c>
-      <c r="N18" s="3">
-        <v>2.3138999999999998</v>
-      </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" s="13"/>
@@ -5526,42 +5444,6 @@
     <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27" s="13"/>
       <c r="B27" s="16"/>
-      <c r="C27" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="D27" s="4">
-        <v>4.8710000000000004</v>
-      </c>
-      <c r="E27" s="4">
-        <v>11.518000000000001</v>
-      </c>
-      <c r="F27" s="4">
-        <v>7.0281000000000002</v>
-      </c>
-      <c r="G27" s="4">
-        <v>4.2420999999999998</v>
-      </c>
-      <c r="H27" s="4">
-        <v>1138.3</v>
-      </c>
-      <c r="I27" s="4">
-        <v>2.7233999999999998</v>
-      </c>
-      <c r="J27" s="4">
-        <v>0.55910000000000004</v>
-      </c>
-      <c r="K27" s="4">
-        <v>4.2544000000000004</v>
-      </c>
-      <c r="L27" s="4">
-        <v>9.1884999999999994</v>
-      </c>
-      <c r="M27" s="4">
-        <v>0.57372999999999996</v>
-      </c>
-      <c r="N27" s="3">
-        <v>0.43879000000000001</v>
-      </c>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28" s="13"/>
@@ -5627,42 +5509,12 @@
     <row r="40" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A40" s="13"/>
       <c r="B40" s="16"/>
-      <c r="C40" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="D40" s="4">
-        <v>7.1036999999999999</v>
-      </c>
-      <c r="E40" s="4">
-        <v>48.234999999999999</v>
-      </c>
-      <c r="F40" s="4">
-        <v>4.2972000000000001</v>
-      </c>
-      <c r="G40" s="4">
-        <v>3.4083999999999999</v>
-      </c>
-      <c r="H40" s="4">
-        <v>1829.9</v>
-      </c>
-      <c r="I40" s="2">
-        <v>1.6407</v>
-      </c>
-      <c r="J40" s="2">
-        <v>0.32468000000000002</v>
-      </c>
-      <c r="K40" s="2">
-        <v>2.9868000000000001</v>
-      </c>
-      <c r="L40" s="2">
-        <v>19.919</v>
-      </c>
-      <c r="M40" s="2">
-        <v>0.79890000000000005</v>
-      </c>
-      <c r="N40" s="2">
-        <v>0.20008999999999999</v>
-      </c>
+      <c r="I40" s="2"/>
+      <c r="J40" s="2"/>
+      <c r="K40" s="2"/>
+      <c r="L40" s="2"/>
+      <c r="M40" s="2"/>
+      <c r="N40" s="2"/>
     </row>
     <row r="41" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A41" s="13"/>
@@ -5689,42 +5541,6 @@
     <row r="45" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A45" s="13"/>
       <c r="B45" s="16"/>
-      <c r="C45" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="D45" s="4">
-        <v>6.3647</v>
-      </c>
-      <c r="E45" s="4">
-        <v>149.54</v>
-      </c>
-      <c r="F45" s="4">
-        <v>0.43913000000000002</v>
-      </c>
-      <c r="G45" s="4">
-        <v>4.1839000000000004</v>
-      </c>
-      <c r="H45" s="4">
-        <v>1127.5999999999999</v>
-      </c>
-      <c r="I45" s="4">
-        <v>2.2016</v>
-      </c>
-      <c r="J45" s="4">
-        <v>0.28632000000000002</v>
-      </c>
-      <c r="K45" s="4">
-        <v>2.7416</v>
-      </c>
-      <c r="L45" s="4">
-        <v>1.1881999999999999</v>
-      </c>
-      <c r="M45" s="4">
-        <v>0.70389999999999997</v>
-      </c>
-      <c r="N45" s="3">
-        <v>8.2974999999999993E-2</v>
-      </c>
     </row>
     <row r="46" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A46" s="13"/>
@@ -6306,7 +6122,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1D987DC-5A74-4932-B56A-48A4420F0E95}">
   <dimension ref="A1:Z73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView topLeftCell="H1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="Z5" sqref="P3:Z5"/>
     </sheetView>

</xml_diff>

<commit_message>
Changes throughout; fixed issue with 1000C evpcd_f
</commit_message>
<xml_diff>
--- a/scripts/__other__/__sem__.xlsx
+++ b/scripts/__other__/__sem__.xlsx
@@ -8,18 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Janzen\Desktop\code\moga_neml\scripts\__other__\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{844ABD68-CFAB-490E-A3A5-4A32549E3139}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4278C4F-BE90-4993-8B8E-A58FF350AACA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="15600" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="evp" sheetId="13" r:id="rId1"/>
     <sheet name="evp-cd_f" sheetId="14" r:id="rId2"/>
     <sheet name="evp-cd_i" sheetId="17" r:id="rId3"/>
-    <sheet name="evp-wd_f" sheetId="15" r:id="rId4"/>
+    <sheet name="evp-wd_f" sheetId="20" r:id="rId4"/>
     <sheet name="evp-wd_i" sheetId="18" r:id="rId5"/>
     <sheet name="evp-wd_f_1" sheetId="19" r:id="rId6"/>
-    <sheet name="evp-wd_f_2" sheetId="20" r:id="rId7"/>
+    <sheet name="evp-wd_f_2" sheetId="15" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="446" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="472" uniqueCount="54">
   <si>
     <t>temp</t>
   </si>
@@ -190,6 +190,21 @@
   <si>
     <t>6; 9</t>
   </si>
+  <si>
+    <t>7; 5</t>
+  </si>
+  <si>
+    <t>6; 6</t>
+  </si>
+  <si>
+    <t>4; 7</t>
+  </si>
+  <si>
+    <t>5; 7</t>
+  </si>
+  <si>
+    <t>5; 6</t>
+  </si>
 </sst>
 </file>
 
@@ -323,7 +338,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -374,6 +389,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -656,11 +674,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4D7A15E-4182-42F6-82DA-99E9B04906BA}">
-  <dimension ref="A1:Q73"/>
+  <dimension ref="A1:Q75"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A48" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D75" sqref="D75"/>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A58" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D75" sqref="D75:H75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2509,6 +2527,36 @@
       <c r="J73" s="7"/>
       <c r="K73" s="7"/>
       <c r="L73" s="7"/>
+    </row>
+    <row r="74" spans="1:12" s="18" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B74" s="3"/>
+      <c r="C74" s="8"/>
+      <c r="I74" s="8"/>
+      <c r="J74" s="8"/>
+      <c r="K74" s="8"/>
+      <c r="L74" s="8"/>
+    </row>
+    <row r="75" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D75" s="4">
+        <f>MAX(D2:D72)</f>
+        <v>37.741999999999997</v>
+      </c>
+      <c r="E75" s="4">
+        <f t="shared" ref="E75:H75" si="0">MAX(E2:E72)</f>
+        <v>481.1</v>
+      </c>
+      <c r="F75" s="4">
+        <f t="shared" si="0"/>
+        <v>32.420999999999999</v>
+      </c>
+      <c r="G75" s="4">
+        <f t="shared" si="0"/>
+        <v>4.8326000000000002</v>
+      </c>
+      <c r="H75" s="4">
+        <f t="shared" si="0"/>
+        <v>3172</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="12">
@@ -2533,11 +2581,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE483CC8-AF2C-4D5A-AEE5-EF7DF4EC0883}">
-  <dimension ref="A1:L73"/>
+  <dimension ref="A1:T75"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C53" sqref="C53"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A39" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D51" sqref="D51:K72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3876,13 +3924,13 @@
         <v>8.0541</v>
       </c>
     </row>
-    <row r="49" spans="1:12" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:20" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="14"/>
       <c r="B49" s="17"/>
       <c r="C49" s="7"/>
       <c r="L49" s="11"/>
     </row>
-    <row r="50" spans="1:12" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:20" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="12">
         <v>1000</v>
       </c>
@@ -3890,134 +3938,323 @@
         <v>6</v>
       </c>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A51" s="13"/>
       <c r="B51" s="16"/>
       <c r="C51" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="D51" s="4">
+        <v>47</v>
+      </c>
+      <c r="M51" s="4">
         <v>1.9315</v>
       </c>
-      <c r="E51" s="4">
+      <c r="N51" s="4">
         <v>481.1</v>
       </c>
-      <c r="F51" s="4">
+      <c r="O51" s="4">
         <v>2.1642000000000002E-2</v>
       </c>
-      <c r="G51" s="4">
+      <c r="P51" s="4">
         <v>4.1571999999999996</v>
       </c>
-      <c r="H51" s="4">
+      <c r="Q51" s="4">
         <v>723.11</v>
       </c>
-      <c r="I51" s="4">
+      <c r="R51" s="4">
         <v>5015.3</v>
       </c>
-      <c r="J51" s="4">
+      <c r="S51" s="4">
         <v>3.1227999999999998</v>
       </c>
-      <c r="K51" s="4">
+      <c r="T51" s="4">
         <v>9.1630000000000003</v>
       </c>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A52" s="13"/>
       <c r="B52" s="16"/>
       <c r="C52" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="D52" s="4">
+      <c r="M52" s="4">
         <v>3.746</v>
       </c>
-      <c r="E52" s="4">
+      <c r="N52" s="4">
         <v>8.6539999999999999</v>
       </c>
-      <c r="F52" s="4">
+      <c r="O52" s="4">
         <v>4.2439</v>
       </c>
-      <c r="G52" s="4">
+      <c r="P52" s="4">
         <v>3.9319999999999999</v>
       </c>
-      <c r="H52" s="4">
+      <c r="Q52" s="4">
         <v>749.09</v>
       </c>
-      <c r="I52" s="4">
+      <c r="R52" s="4">
         <v>9246.1</v>
       </c>
-      <c r="J52" s="4">
+      <c r="S52" s="4">
         <v>2.7896000000000001</v>
       </c>
-      <c r="K52" s="4">
+      <c r="T52" s="4">
         <v>5.7472000000000003</v>
       </c>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A53" s="13"/>
       <c r="B53" s="16"/>
       <c r="C53" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="D53" s="4">
+      <c r="M53" s="4">
         <v>0.98812</v>
       </c>
-      <c r="E53" s="4">
+      <c r="N53" s="4">
         <v>26.957999999999998</v>
       </c>
-      <c r="F53" s="4">
+      <c r="O53" s="4">
         <v>0.64437999999999995</v>
       </c>
-      <c r="G53" s="4">
+      <c r="P53" s="4">
         <v>4.4935999999999998</v>
       </c>
-      <c r="H53" s="4">
+      <c r="Q53" s="4">
         <v>567.97</v>
       </c>
-      <c r="I53" s="4">
+      <c r="R53" s="4">
         <v>2395</v>
       </c>
-      <c r="J53" s="4">
+      <c r="S53" s="4">
         <v>3.552</v>
       </c>
-      <c r="K53" s="4">
+      <c r="T53" s="4">
         <v>6.7481999999999998</v>
       </c>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A54" s="13"/>
       <c r="B54" s="16"/>
-    </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C54" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="M54" s="4">
+        <v>0.34142</v>
+      </c>
+      <c r="N54" s="4">
+        <v>0.1263</v>
+      </c>
+      <c r="O54" s="4">
+        <v>3.5680000000000001</v>
+      </c>
+      <c r="P54" s="4">
+        <v>4.6580000000000004</v>
+      </c>
+      <c r="Q54" s="4">
+        <v>537.80999999999995</v>
+      </c>
+      <c r="R54" s="4">
+        <v>5130.7</v>
+      </c>
+      <c r="S54" s="4">
+        <v>3.1514000000000002</v>
+      </c>
+      <c r="T54" s="4">
+        <v>9.5030999999999999</v>
+      </c>
+    </row>
+    <row r="55" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A55" s="13"/>
       <c r="B55" s="16"/>
-    </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C55" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="M55" s="4">
+        <v>0.90237000000000001</v>
+      </c>
+      <c r="N55" s="4">
+        <v>5.2742000000000004</v>
+      </c>
+      <c r="O55" s="4">
+        <v>1.5201</v>
+      </c>
+      <c r="P55" s="4">
+        <v>4.5481999999999996</v>
+      </c>
+      <c r="Q55" s="4">
+        <v>558.20000000000005</v>
+      </c>
+      <c r="R55" s="4">
+        <v>6762.3</v>
+      </c>
+      <c r="S55" s="4">
+        <v>2.9710000000000001</v>
+      </c>
+      <c r="T55" s="4">
+        <v>7.3547000000000002</v>
+      </c>
+    </row>
+    <row r="56" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A56" s="13"/>
       <c r="B56" s="16"/>
-    </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C56" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="M56" s="4">
+        <v>2.2723</v>
+      </c>
+      <c r="N56" s="4">
+        <v>17.684000000000001</v>
+      </c>
+      <c r="O56" s="4">
+        <v>0.52432000000000001</v>
+      </c>
+      <c r="P56" s="4">
+        <v>4.1894999999999998</v>
+      </c>
+      <c r="Q56" s="4">
+        <v>695.87</v>
+      </c>
+      <c r="R56" s="4">
+        <v>4416.3999999999996</v>
+      </c>
+      <c r="S56" s="4">
+        <v>3.1836000000000002</v>
+      </c>
+      <c r="T56" s="4">
+        <v>7.1730999999999998</v>
+      </c>
+    </row>
+    <row r="57" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A57" s="13"/>
       <c r="B57" s="16"/>
-    </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C57" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="M57" s="4">
+        <v>1.7845</v>
+      </c>
+      <c r="N57" s="4">
+        <v>0.26406000000000002</v>
+      </c>
+      <c r="O57" s="4">
+        <v>25.678000000000001</v>
+      </c>
+      <c r="P57" s="4">
+        <v>4.2798999999999996</v>
+      </c>
+      <c r="Q57" s="4">
+        <v>669.49</v>
+      </c>
+      <c r="R57" s="4">
+        <v>9702.4</v>
+      </c>
+      <c r="S57" s="4">
+        <v>2.8408000000000002</v>
+      </c>
+      <c r="T57" s="4">
+        <v>8.8193999999999999</v>
+      </c>
+    </row>
+    <row r="58" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A58" s="13"/>
       <c r="B58" s="16"/>
-    </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C58" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="M58" s="4">
+        <v>1.2223999999999999</v>
+      </c>
+      <c r="N58" s="4">
+        <v>3.6264999999999999E-2</v>
+      </c>
+      <c r="O58" s="4">
+        <v>6.5932000000000004</v>
+      </c>
+      <c r="P58" s="4">
+        <v>4.3323</v>
+      </c>
+      <c r="Q58" s="4">
+        <v>673.71</v>
+      </c>
+      <c r="R58" s="4">
+        <v>8825.2000000000007</v>
+      </c>
+      <c r="S58" s="4">
+        <v>2.8908999999999998</v>
+      </c>
+      <c r="T58" s="4">
+        <v>9.6677999999999997</v>
+      </c>
+    </row>
+    <row r="59" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A59" s="13"/>
       <c r="B59" s="16"/>
-    </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C59" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="M59" s="4">
+        <v>1.5227999999999999</v>
+      </c>
+      <c r="N59" s="4">
+        <v>4.8478000000000003</v>
+      </c>
+      <c r="O59" s="4">
+        <v>3.7315</v>
+      </c>
+      <c r="P59" s="4">
+        <v>4.4061000000000003</v>
+      </c>
+      <c r="Q59" s="4">
+        <v>590.03</v>
+      </c>
+      <c r="R59" s="4">
+        <v>4508.3</v>
+      </c>
+      <c r="S59" s="4">
+        <v>3.1535000000000002</v>
+      </c>
+      <c r="T59" s="4">
+        <v>6.3638000000000003</v>
+      </c>
+    </row>
+    <row r="60" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A60" s="13"/>
       <c r="B60" s="16"/>
-    </row>
-    <row r="61" spans="1:12" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C60" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="M60" s="4">
+        <v>3.0295000000000001</v>
+      </c>
+      <c r="N60" s="4">
+        <v>12.903</v>
+      </c>
+      <c r="O60" s="4">
+        <v>2.3944000000000001</v>
+      </c>
+      <c r="P60" s="4">
+        <v>4.0586000000000002</v>
+      </c>
+      <c r="Q60" s="4">
+        <v>713.26</v>
+      </c>
+      <c r="R60" s="4">
+        <v>3970.7</v>
+      </c>
+      <c r="S60" s="4">
+        <v>3.1777000000000002</v>
+      </c>
+      <c r="T60" s="4">
+        <v>4.9123999999999999</v>
+      </c>
+    </row>
+    <row r="61" spans="1:20" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="14"/>
       <c r="B61" s="17"/>
       <c r="C61" s="7"/>
       <c r="L61" s="11"/>
     </row>
-    <row r="62" spans="1:12" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:20" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="12">
         <v>1000</v>
       </c>
@@ -4025,51 +4262,360 @@
         <v>7</v>
       </c>
     </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A63" s="13"/>
       <c r="B63" s="16"/>
-    </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C63" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="M63" s="4">
+        <v>4.6150000000000002E-3</v>
+      </c>
+      <c r="N63" s="4">
+        <v>6.1843000000000004</v>
+      </c>
+      <c r="O63" s="4">
+        <v>2.2823000000000002</v>
+      </c>
+      <c r="P63" s="4">
+        <v>4.8326000000000002</v>
+      </c>
+      <c r="Q63" s="4">
+        <v>460.27</v>
+      </c>
+      <c r="R63" s="4">
+        <v>3478.8</v>
+      </c>
+      <c r="S63" s="4">
+        <v>3.3414000000000001</v>
+      </c>
+      <c r="T63" s="4">
+        <v>7.4029999999999996</v>
+      </c>
+    </row>
+    <row r="64" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A64" s="13"/>
       <c r="B64" s="16"/>
-    </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C64" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="M64" s="4">
+        <v>3.9207000000000001</v>
+      </c>
+      <c r="N64" s="4">
+        <v>130.97</v>
+      </c>
+      <c r="O64" s="4">
+        <v>0.16188</v>
+      </c>
+      <c r="P64" s="4">
+        <v>3.9466000000000001</v>
+      </c>
+      <c r="Q64" s="4">
+        <v>752.32</v>
+      </c>
+      <c r="R64" s="4">
+        <v>2965</v>
+      </c>
+      <c r="S64" s="4">
+        <v>3.3761000000000001</v>
+      </c>
+      <c r="T64" s="4">
+        <v>5.2625999999999999</v>
+      </c>
+    </row>
+    <row r="65" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A65" s="13"/>
       <c r="B65" s="16"/>
-    </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C65" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="M65" s="4">
+        <v>1.2675000000000001E-2</v>
+      </c>
+      <c r="N65" s="4">
+        <v>18.527999999999999</v>
+      </c>
+      <c r="O65" s="4">
+        <v>0.99367000000000005</v>
+      </c>
+      <c r="P65" s="4">
+        <v>4.8133999999999997</v>
+      </c>
+      <c r="Q65" s="4">
+        <v>471.18</v>
+      </c>
+      <c r="R65" s="4">
+        <v>2229.9</v>
+      </c>
+      <c r="S65" s="4">
+        <v>3.5893000000000002</v>
+      </c>
+      <c r="T65" s="4">
+        <v>5.6052</v>
+      </c>
+    </row>
+    <row r="66" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A66" s="13"/>
       <c r="B66" s="16"/>
-    </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C66" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="M66" s="4">
+        <v>0.26123000000000002</v>
+      </c>
+      <c r="N66" s="4">
+        <v>35.054000000000002</v>
+      </c>
+      <c r="O66" s="4">
+        <v>0.42681000000000002</v>
+      </c>
+      <c r="P66" s="4">
+        <v>4.7435999999999998</v>
+      </c>
+      <c r="Q66" s="4">
+        <v>490.7</v>
+      </c>
+      <c r="R66" s="4">
+        <v>2850.7</v>
+      </c>
+      <c r="S66" s="4">
+        <v>3.4043000000000001</v>
+      </c>
+      <c r="T66" s="4">
+        <v>5.3243</v>
+      </c>
+    </row>
+    <row r="67" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A67" s="13"/>
       <c r="B67" s="16"/>
-    </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C67" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="M67" s="4">
+        <v>1.4714</v>
+      </c>
+      <c r="N67" s="4">
+        <v>3.11</v>
+      </c>
+      <c r="O67" s="4">
+        <v>5.9009</v>
+      </c>
+      <c r="P67" s="4">
+        <v>4.4241000000000001</v>
+      </c>
+      <c r="Q67" s="4">
+        <v>584.77</v>
+      </c>
+      <c r="R67" s="4">
+        <v>3948.5</v>
+      </c>
+      <c r="S67" s="4">
+        <v>3.2559</v>
+      </c>
+      <c r="T67" s="4">
+        <v>7.3000999999999996</v>
+      </c>
+    </row>
+    <row r="68" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A68" s="13"/>
       <c r="B68" s="16"/>
-    </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C68" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="M68" s="4">
+        <v>4.1444999999999999</v>
+      </c>
+      <c r="N68" s="4">
+        <v>21.946000000000002</v>
+      </c>
+      <c r="O68" s="4">
+        <v>1.2583</v>
+      </c>
+      <c r="P68" s="4">
+        <v>3.9466999999999999</v>
+      </c>
+      <c r="Q68" s="4">
+        <v>726.26</v>
+      </c>
+      <c r="R68" s="4">
+        <v>3639.1</v>
+      </c>
+      <c r="S68" s="4">
+        <v>3.2450999999999999</v>
+      </c>
+      <c r="T68" s="4">
+        <v>4.9524999999999997</v>
+      </c>
+    </row>
+    <row r="69" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A69" s="13"/>
       <c r="B69" s="16"/>
-    </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C69" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="M69" s="4">
+        <v>3.2084999999999999</v>
+      </c>
+      <c r="N69" s="4">
+        <v>17.286999999999999</v>
+      </c>
+      <c r="O69" s="4">
+        <v>1.3622000000000001</v>
+      </c>
+      <c r="P69" s="4">
+        <v>4.0769000000000002</v>
+      </c>
+      <c r="Q69" s="4">
+        <v>697.16</v>
+      </c>
+      <c r="R69" s="4">
+        <v>3927.3</v>
+      </c>
+      <c r="S69" s="4">
+        <v>3.2118000000000002</v>
+      </c>
+      <c r="T69" s="4">
+        <v>4.7915999999999999</v>
+      </c>
+    </row>
+    <row r="70" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A70" s="13"/>
       <c r="B70" s="16"/>
-    </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C70" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="M70" s="4">
+        <v>4.3445999999999998</v>
+      </c>
+      <c r="N70" s="4">
+        <v>10.148</v>
+      </c>
+      <c r="O70" s="4">
+        <v>2.2065999999999999</v>
+      </c>
+      <c r="P70" s="4">
+        <v>3.8805999999999998</v>
+      </c>
+      <c r="Q70" s="4">
+        <v>776.41</v>
+      </c>
+      <c r="R70" s="4">
+        <v>4502.1000000000004</v>
+      </c>
+      <c r="S70" s="4">
+        <v>3.1688000000000001</v>
+      </c>
+      <c r="T70" s="4">
+        <v>6.5437000000000003</v>
+      </c>
+    </row>
+    <row r="71" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A71" s="13"/>
       <c r="B71" s="16"/>
-    </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C71" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="M71" s="4">
+        <v>3.3748</v>
+      </c>
+      <c r="N71" s="4">
+        <v>51.076000000000001</v>
+      </c>
+      <c r="O71" s="4">
+        <v>0.45746999999999999</v>
+      </c>
+      <c r="P71" s="4">
+        <v>4.0575000000000001</v>
+      </c>
+      <c r="Q71" s="4">
+        <v>700.49</v>
+      </c>
+      <c r="R71" s="4">
+        <v>2863</v>
+      </c>
+      <c r="S71" s="4">
+        <v>3.4026999999999998</v>
+      </c>
+      <c r="T71" s="4">
+        <v>5.3670999999999998</v>
+      </c>
+    </row>
+    <row r="72" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A72" s="13"/>
       <c r="B72" s="16"/>
-    </row>
-    <row r="73" spans="1:12" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C72" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="M72" s="4">
+        <v>4.2664999999999997</v>
+      </c>
+      <c r="N72" s="4">
+        <v>246.76</v>
+      </c>
+      <c r="O72" s="4">
+        <v>8.4953000000000001E-2</v>
+      </c>
+      <c r="P72" s="4">
+        <v>3.9445000000000001</v>
+      </c>
+      <c r="Q72" s="4">
+        <v>738.14</v>
+      </c>
+      <c r="R72" s="4">
+        <v>2087.1999999999998</v>
+      </c>
+      <c r="S72" s="4">
+        <v>3.6288</v>
+      </c>
+      <c r="T72" s="4">
+        <v>5.3070000000000004</v>
+      </c>
+    </row>
+    <row r="73" spans="1:20" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="14"/>
       <c r="B73" s="17"/>
       <c r="C73" s="7"/>
       <c r="L73" s="11"/>
+    </row>
+    <row r="74" spans="1:20" s="18" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B74" s="3"/>
+      <c r="C74" s="8"/>
+      <c r="L74" s="9"/>
+    </row>
+    <row r="75" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="D75" s="4">
+        <f>MAX(D1:D71)</f>
+        <v>37.741999999999997</v>
+      </c>
+      <c r="E75" s="4">
+        <f t="shared" ref="E75:K75" si="0">MAX(E1:E71)</f>
+        <v>462.57</v>
+      </c>
+      <c r="F75" s="4">
+        <f t="shared" si="0"/>
+        <v>32.420999999999999</v>
+      </c>
+      <c r="G75" s="4">
+        <f t="shared" si="0"/>
+        <v>4.7751999999999999</v>
+      </c>
+      <c r="H75" s="4">
+        <f t="shared" si="0"/>
+        <v>3172</v>
+      </c>
+      <c r="I75" s="4">
+        <f t="shared" si="0"/>
+        <v>4771.8999999999996</v>
+      </c>
+      <c r="J75" s="4">
+        <f t="shared" si="0"/>
+        <v>5.5552000000000001</v>
+      </c>
+      <c r="K75" s="4">
+        <f t="shared" si="0"/>
+        <v>21.834</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="12">
@@ -4093,11 +4639,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF6E341A-51E3-4AF7-809B-A8594B1323BC}">
-  <dimension ref="A1:L73"/>
+  <dimension ref="A1:L75"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C18" sqref="C18"/>
+    <sheetView topLeftCell="C1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M77" sqref="M77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5549,6 +6095,45 @@
       <c r="B73" s="17"/>
       <c r="C73" s="7"/>
       <c r="L73" s="11"/>
+    </row>
+    <row r="74" spans="1:12" s="18" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B74" s="3"/>
+      <c r="C74" s="8"/>
+      <c r="L74" s="9"/>
+    </row>
+    <row r="75" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D75" s="4">
+        <f>MAX(D1:D71)</f>
+        <v>38.180999999999997</v>
+      </c>
+      <c r="E75" s="4">
+        <f t="shared" ref="E75:K75" si="0">MAX(E1:E71)</f>
+        <v>522.85</v>
+      </c>
+      <c r="F75" s="4">
+        <f t="shared" si="0"/>
+        <v>32.389000000000003</v>
+      </c>
+      <c r="G75" s="4">
+        <f t="shared" si="0"/>
+        <v>4.7670000000000003</v>
+      </c>
+      <c r="H75" s="4">
+        <f t="shared" si="0"/>
+        <v>3154.4</v>
+      </c>
+      <c r="I75" s="4">
+        <f t="shared" si="0"/>
+        <v>4972.3999999999996</v>
+      </c>
+      <c r="J75" s="4">
+        <f t="shared" si="0"/>
+        <v>5.6638000000000002</v>
+      </c>
+      <c r="K75" s="4">
+        <f t="shared" si="0"/>
+        <v>21.824999999999999</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="12">
@@ -5571,12 +6156,12 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C18A26E-30CA-4E63-A18A-C9C101DAF33C}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{666CFF77-8976-439D-A33C-D7841D6EB88F}">
   <dimension ref="A1:O73"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E23" sqref="E23"/>
+      <pane ySplit="1" topLeftCell="A31" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C44" sqref="C44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5646,51 +6231,202 @@
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="13"/>
       <c r="B3" s="16"/>
-      <c r="I3" s="2"/>
-      <c r="J3" s="2"/>
-      <c r="K3" s="2"/>
-      <c r="L3" s="2"/>
-      <c r="M3" s="2"/>
-      <c r="N3" s="1"/>
+      <c r="C3" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="D3" s="4">
+        <v>17.216999999999999</v>
+      </c>
+      <c r="E3" s="4">
+        <v>179.74</v>
+      </c>
+      <c r="F3" s="4">
+        <v>0.61753999999999998</v>
+      </c>
+      <c r="G3" s="4">
+        <v>4.4165999999999999</v>
+      </c>
+      <c r="H3" s="4">
+        <v>1783.5</v>
+      </c>
+      <c r="I3" s="2">
+        <v>2.0167000000000002</v>
+      </c>
+      <c r="J3" s="2">
+        <v>27.012</v>
+      </c>
+      <c r="K3" s="2">
+        <v>187.86</v>
+      </c>
+      <c r="L3" s="2">
+        <v>9.6981000000000002</v>
+      </c>
+      <c r="M3" s="2">
+        <v>87.406999999999996</v>
+      </c>
+      <c r="N3" s="1">
+        <v>320.89</v>
+      </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="13"/>
       <c r="B4" s="16"/>
-      <c r="I4" s="2"/>
-      <c r="J4" s="2"/>
-      <c r="K4" s="2"/>
-      <c r="L4" s="2"/>
-      <c r="M4" s="2"/>
-      <c r="N4" s="2"/>
+      <c r="C4" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="D4" s="4">
+        <v>5.6908000000000003</v>
+      </c>
+      <c r="E4" s="4">
+        <v>66.626999999999995</v>
+      </c>
+      <c r="F4" s="4">
+        <v>1.9851000000000001</v>
+      </c>
+      <c r="G4" s="4">
+        <v>4.7723000000000004</v>
+      </c>
+      <c r="H4" s="4">
+        <v>1621.6</v>
+      </c>
+      <c r="I4" s="2">
+        <v>2.5163000000000002</v>
+      </c>
+      <c r="J4" s="2">
+        <v>27.937999999999999</v>
+      </c>
+      <c r="K4" s="2">
+        <v>187.97</v>
+      </c>
+      <c r="L4" s="2">
+        <v>9.4260999999999999</v>
+      </c>
+      <c r="M4" s="2">
+        <v>377.11</v>
+      </c>
+      <c r="N4" s="2">
+        <v>883.39</v>
+      </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="13"/>
       <c r="B5" s="16"/>
-      <c r="I5" s="2"/>
-      <c r="J5" s="2"/>
-      <c r="K5" s="2"/>
-      <c r="L5" s="2"/>
-      <c r="M5" s="2"/>
-      <c r="N5" s="2"/>
+      <c r="C5" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="D5" s="4">
+        <v>9.3076000000000008</v>
+      </c>
+      <c r="E5" s="4">
+        <v>32.595999999999997</v>
+      </c>
+      <c r="F5" s="4">
+        <v>5.8113999999999999</v>
+      </c>
+      <c r="G5" s="4">
+        <v>4.5263</v>
+      </c>
+      <c r="H5" s="4">
+        <v>1775.9</v>
+      </c>
+      <c r="I5" s="2">
+        <v>2.0687000000000002</v>
+      </c>
+      <c r="J5" s="2">
+        <v>33.454999999999998</v>
+      </c>
+      <c r="K5" s="2">
+        <v>225.37</v>
+      </c>
+      <c r="L5" s="2">
+        <v>3.5903999999999998</v>
+      </c>
+      <c r="M5" s="2">
+        <v>103.26</v>
+      </c>
+      <c r="N5" s="2">
+        <v>462.92</v>
+      </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="13"/>
       <c r="B6" s="16"/>
+      <c r="C6" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="D6" s="4">
+        <v>5.8951000000000002</v>
+      </c>
+      <c r="E6" s="4">
+        <v>36.244999999999997</v>
+      </c>
+      <c r="F6" s="4">
+        <v>5.3757000000000001</v>
+      </c>
+      <c r="G6" s="4">
+        <v>4.7310999999999996</v>
+      </c>
+      <c r="H6" s="4">
+        <v>1598.4</v>
+      </c>
+      <c r="I6" s="4">
+        <v>1.9289000000000001</v>
+      </c>
+      <c r="J6" s="4">
+        <v>39.776000000000003</v>
+      </c>
+      <c r="K6" s="4">
+        <v>261.52999999999997</v>
+      </c>
+      <c r="L6" s="4">
+        <v>2.7751000000000001</v>
+      </c>
+      <c r="M6" s="4">
+        <v>469.99</v>
+      </c>
+      <c r="N6" s="3">
+        <v>958.51</v>
+      </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="13"/>
       <c r="B7" s="16"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
-      <c r="I7" s="2"/>
-      <c r="J7" s="2"/>
-      <c r="K7" s="2"/>
-      <c r="L7" s="2"/>
-      <c r="M7" s="2"/>
-      <c r="N7" s="2"/>
+      <c r="C7" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="D7" s="2">
+        <v>4.1862000000000004</v>
+      </c>
+      <c r="E7" s="2">
+        <v>84.548000000000002</v>
+      </c>
+      <c r="F7" s="2">
+        <v>2.1122999999999998</v>
+      </c>
+      <c r="G7" s="2">
+        <v>4.7751999999999999</v>
+      </c>
+      <c r="H7" s="2">
+        <v>1574.3</v>
+      </c>
+      <c r="I7" s="2">
+        <v>2.0095999999999998</v>
+      </c>
+      <c r="J7" s="2">
+        <v>28.899000000000001</v>
+      </c>
+      <c r="K7" s="2">
+        <v>198.44</v>
+      </c>
+      <c r="L7" s="2">
+        <v>3.7132000000000001</v>
+      </c>
+      <c r="M7" s="2">
+        <v>286.14</v>
+      </c>
+      <c r="N7" s="2">
+        <v>732.59</v>
+      </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="13"/>
@@ -5730,34 +6466,202 @@
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="13"/>
       <c r="B15" s="16"/>
+      <c r="C15" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="D15" s="4">
+        <v>31.327000000000002</v>
+      </c>
+      <c r="E15" s="4">
+        <v>104.92</v>
+      </c>
+      <c r="F15" s="4">
+        <v>0.8548</v>
+      </c>
+      <c r="G15" s="4">
+        <v>3.7507999999999999</v>
+      </c>
+      <c r="H15" s="4">
+        <v>2575.8000000000002</v>
+      </c>
+      <c r="I15" s="4">
+        <v>1.9380999999999999</v>
+      </c>
+      <c r="J15" s="4">
+        <v>36.652999999999999</v>
+      </c>
+      <c r="K15" s="4">
+        <v>239.99</v>
+      </c>
+      <c r="L15" s="4">
+        <v>2.3007</v>
+      </c>
+      <c r="M15" s="4">
+        <v>266.47000000000003</v>
+      </c>
+      <c r="N15" s="3">
+        <v>843.59</v>
+      </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="13"/>
       <c r="B16" s="16"/>
-      <c r="I16" s="2"/>
-      <c r="J16" s="2"/>
-      <c r="K16" s="2"/>
-      <c r="L16" s="2"/>
-      <c r="M16" s="2"/>
-      <c r="N16" s="2"/>
+      <c r="C16" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="D16" s="4">
+        <v>22.393000000000001</v>
+      </c>
+      <c r="E16" s="4">
+        <v>462.57</v>
+      </c>
+      <c r="F16" s="4">
+        <v>0.13572999999999999</v>
+      </c>
+      <c r="G16" s="4">
+        <v>4.3140000000000001</v>
+      </c>
+      <c r="H16" s="4">
+        <v>1828.1</v>
+      </c>
+      <c r="I16" s="2">
+        <v>1.9944999999999999</v>
+      </c>
+      <c r="J16" s="2">
+        <v>39.430999999999997</v>
+      </c>
+      <c r="K16" s="2">
+        <v>259.74</v>
+      </c>
+      <c r="L16" s="2">
+        <v>1.7996000000000001</v>
+      </c>
+      <c r="M16" s="2">
+        <v>316.17</v>
+      </c>
+      <c r="N16" s="2">
+        <v>991.58</v>
+      </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" s="13"/>
       <c r="B17" s="16"/>
-      <c r="I17" s="2"/>
-      <c r="J17" s="2"/>
-      <c r="K17" s="2"/>
-      <c r="L17" s="2"/>
-      <c r="M17" s="2"/>
-      <c r="N17" s="2"/>
+      <c r="C17" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="D17" s="4">
+        <v>11.45</v>
+      </c>
+      <c r="E17" s="4">
+        <v>53.151000000000003</v>
+      </c>
+      <c r="F17" s="4">
+        <v>7.1665999999999999</v>
+      </c>
+      <c r="G17" s="4">
+        <v>3.9502000000000002</v>
+      </c>
+      <c r="H17" s="4">
+        <v>2221.6</v>
+      </c>
+      <c r="I17" s="2">
+        <v>1.3278000000000001</v>
+      </c>
+      <c r="J17" s="2">
+        <v>35.21</v>
+      </c>
+      <c r="K17" s="2">
+        <v>248.59</v>
+      </c>
+      <c r="L17" s="2">
+        <v>2.6511999999999998</v>
+      </c>
+      <c r="M17" s="2">
+        <v>281.86</v>
+      </c>
+      <c r="N17" s="2">
+        <v>728.27</v>
+      </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" s="13"/>
       <c r="B18" s="16"/>
+      <c r="C18" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="D18" s="4">
+        <v>37.741999999999997</v>
+      </c>
+      <c r="E18" s="4">
+        <v>49.122999999999998</v>
+      </c>
+      <c r="F18" s="4">
+        <v>2.4996</v>
+      </c>
+      <c r="G18" s="4">
+        <v>3.4102000000000001</v>
+      </c>
+      <c r="H18" s="4">
+        <v>3172</v>
+      </c>
+      <c r="I18" s="4">
+        <v>1.6356999999999999</v>
+      </c>
+      <c r="J18" s="4">
+        <v>38.524000000000001</v>
+      </c>
+      <c r="K18" s="4">
+        <v>262.60000000000002</v>
+      </c>
+      <c r="L18" s="4">
+        <v>2.7321</v>
+      </c>
+      <c r="M18" s="4">
+        <v>435.37</v>
+      </c>
+      <c r="N18" s="3">
+        <v>930.53</v>
+      </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" s="13"/>
       <c r="B19" s="16"/>
+      <c r="C19" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="D19" s="4">
+        <v>18.768000000000001</v>
+      </c>
+      <c r="E19" s="4">
+        <v>89.18</v>
+      </c>
+      <c r="F19" s="4">
+        <v>0.88068999999999997</v>
+      </c>
+      <c r="G19" s="4">
+        <v>4.5054999999999996</v>
+      </c>
+      <c r="H19" s="4">
+        <v>1677.4</v>
+      </c>
+      <c r="I19" s="4">
+        <v>1.871</v>
+      </c>
+      <c r="J19" s="4">
+        <v>38.057000000000002</v>
+      </c>
+      <c r="K19" s="4">
+        <v>252.43</v>
+      </c>
+      <c r="L19" s="4">
+        <v>2.2942</v>
+      </c>
+      <c r="M19" s="4">
+        <v>196.55</v>
+      </c>
+      <c r="N19" s="3">
+        <v>665.69</v>
+      </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" s="13"/>
@@ -5797,28 +6701,202 @@
     <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27" s="13"/>
       <c r="B27" s="16"/>
+      <c r="C27" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="D27" s="4">
+        <v>4.8710000000000004</v>
+      </c>
+      <c r="E27" s="4">
+        <v>11.518000000000001</v>
+      </c>
+      <c r="F27" s="4">
+        <v>7.0281000000000002</v>
+      </c>
+      <c r="G27" s="4">
+        <v>4.2420999999999998</v>
+      </c>
+      <c r="H27" s="4">
+        <v>1138.3</v>
+      </c>
+      <c r="I27" s="4">
+        <v>6.7659000000000002</v>
+      </c>
+      <c r="J27" s="4">
+        <v>31.863</v>
+      </c>
+      <c r="K27" s="4">
+        <v>194.21</v>
+      </c>
+      <c r="L27" s="4">
+        <v>15.672000000000001</v>
+      </c>
+      <c r="M27" s="4">
+        <v>969.61</v>
+      </c>
+      <c r="N27" s="3">
+        <v>979.36</v>
+      </c>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28" s="13"/>
       <c r="B28" s="16"/>
-      <c r="I28" s="2"/>
-      <c r="J28" s="2"/>
-      <c r="K28" s="2"/>
-      <c r="L28" s="2"/>
-      <c r="M28" s="2"/>
-      <c r="N28" s="2"/>
+      <c r="C28" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="D28" s="4">
+        <v>10.692</v>
+      </c>
+      <c r="E28" s="4">
+        <v>29.068000000000001</v>
+      </c>
+      <c r="F28" s="4">
+        <v>2.9830999999999999</v>
+      </c>
+      <c r="G28" s="4">
+        <v>3.7277999999999998</v>
+      </c>
+      <c r="H28" s="4">
+        <v>1433.5</v>
+      </c>
+      <c r="I28" s="2">
+        <v>2.5966999999999998</v>
+      </c>
+      <c r="J28" s="2">
+        <v>44.024999999999999</v>
+      </c>
+      <c r="K28" s="2">
+        <v>259.35000000000002</v>
+      </c>
+      <c r="L28" s="2">
+        <v>6.7335000000000003</v>
+      </c>
+      <c r="M28" s="2">
+        <v>364.63</v>
+      </c>
+      <c r="N28" s="2">
+        <v>719.77</v>
+      </c>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29" s="13"/>
       <c r="B29" s="16"/>
+      <c r="C29" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="D29" s="4">
+        <v>11.2</v>
+      </c>
+      <c r="E29" s="4">
+        <v>24.262</v>
+      </c>
+      <c r="F29" s="4">
+        <v>2.2614999999999998</v>
+      </c>
+      <c r="G29" s="4">
+        <v>3.9651000000000001</v>
+      </c>
+      <c r="H29" s="4">
+        <v>1163</v>
+      </c>
+      <c r="I29" s="4">
+        <v>2.5491999999999999</v>
+      </c>
+      <c r="J29" s="4">
+        <v>10</v>
+      </c>
+      <c r="K29" s="4">
+        <v>69.98</v>
+      </c>
+      <c r="L29" s="4">
+        <v>3.6154999999999999</v>
+      </c>
+      <c r="M29" s="4">
+        <v>333</v>
+      </c>
+      <c r="N29" s="3">
+        <v>755.26</v>
+      </c>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30" s="13"/>
       <c r="B30" s="16"/>
+      <c r="C30" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="D30" s="4">
+        <v>11.208</v>
+      </c>
+      <c r="E30" s="4">
+        <v>16.738</v>
+      </c>
+      <c r="F30" s="4">
+        <v>5.9587000000000003</v>
+      </c>
+      <c r="G30" s="4">
+        <v>3.6377000000000002</v>
+      </c>
+      <c r="H30" s="4">
+        <v>1530.1</v>
+      </c>
+      <c r="I30" s="4">
+        <v>6.9241000000000001</v>
+      </c>
+      <c r="J30" s="4">
+        <v>33.365000000000002</v>
+      </c>
+      <c r="K30" s="4">
+        <v>203.86</v>
+      </c>
+      <c r="L30" s="4">
+        <v>8.8675999999999995</v>
+      </c>
+      <c r="M30" s="4">
+        <v>246.12</v>
+      </c>
+      <c r="N30" s="3">
+        <v>642.74</v>
+      </c>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A31" s="13"/>
       <c r="B31" s="16"/>
+      <c r="C31" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="D31" s="4">
+        <v>10.45</v>
+      </c>
+      <c r="E31" s="4">
+        <v>14.769</v>
+      </c>
+      <c r="F31" s="4">
+        <v>7.8792</v>
+      </c>
+      <c r="G31" s="4">
+        <v>3.54</v>
+      </c>
+      <c r="H31" s="4">
+        <v>1787.3</v>
+      </c>
+      <c r="I31" s="4">
+        <v>6.9993999999999996</v>
+      </c>
+      <c r="J31" s="4">
+        <v>43.887999999999998</v>
+      </c>
+      <c r="K31" s="4">
+        <v>263.95999999999998</v>
+      </c>
+      <c r="L31" s="4">
+        <v>1.4023000000000001</v>
+      </c>
+      <c r="M31" s="4">
+        <v>217.5</v>
+      </c>
+      <c r="N31" s="3">
+        <v>775.78</v>
+      </c>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A32" s="13"/>
@@ -5858,34 +6936,202 @@
     <row r="39" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A39" s="13"/>
       <c r="B39" s="16"/>
+      <c r="C39" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="D39" s="4">
+        <v>4.8238000000000003</v>
+      </c>
+      <c r="E39" s="4">
+        <v>378.86</v>
+      </c>
+      <c r="F39" s="4">
+        <v>0.14230000000000001</v>
+      </c>
+      <c r="G39" s="4">
+        <v>4.4020999999999999</v>
+      </c>
+      <c r="H39" s="4">
+        <v>1006.9</v>
+      </c>
+      <c r="I39" s="4">
+        <v>2.7604000000000002</v>
+      </c>
+      <c r="J39" s="4">
+        <v>41.008000000000003</v>
+      </c>
+      <c r="K39" s="4">
+        <v>249.79</v>
+      </c>
+      <c r="L39" s="4">
+        <v>17.965</v>
+      </c>
+      <c r="M39" s="4">
+        <v>911.14</v>
+      </c>
+      <c r="N39" s="3">
+        <v>909.57</v>
+      </c>
     </row>
     <row r="40" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A40" s="13"/>
       <c r="B40" s="16"/>
-      <c r="I40" s="2"/>
-      <c r="J40" s="2"/>
-      <c r="K40" s="2"/>
-      <c r="L40" s="2"/>
-      <c r="M40" s="2"/>
-      <c r="N40" s="2"/>
+      <c r="C40" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="D40" s="4">
+        <v>7.1036999999999999</v>
+      </c>
+      <c r="E40" s="4">
+        <v>48.234999999999999</v>
+      </c>
+      <c r="F40" s="4">
+        <v>4.2972000000000001</v>
+      </c>
+      <c r="G40" s="4">
+        <v>3.4083999999999999</v>
+      </c>
+      <c r="H40" s="4">
+        <v>1829.9</v>
+      </c>
+      <c r="I40" s="2">
+        <v>1.9162999999999999</v>
+      </c>
+      <c r="J40" s="2">
+        <v>41.036000000000001</v>
+      </c>
+      <c r="K40" s="2">
+        <v>249.3</v>
+      </c>
+      <c r="L40" s="2">
+        <v>15.911</v>
+      </c>
+      <c r="M40" s="2">
+        <v>957.14</v>
+      </c>
+      <c r="N40" s="2">
+        <v>996</v>
+      </c>
     </row>
     <row r="41" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A41" s="13"/>
       <c r="B41" s="16"/>
-      <c r="I41" s="2"/>
-      <c r="J41" s="2"/>
-      <c r="K41" s="2"/>
-      <c r="L41" s="2"/>
-      <c r="M41" s="2"/>
-      <c r="N41" s="1"/>
+      <c r="C41" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="D41" s="4">
+        <v>3.0461</v>
+      </c>
+      <c r="E41" s="4">
+        <v>19.608000000000001</v>
+      </c>
+      <c r="F41" s="4">
+        <v>32.420999999999999</v>
+      </c>
+      <c r="G41" s="4">
+        <v>3.2736000000000001</v>
+      </c>
+      <c r="H41" s="4">
+        <v>2022.3</v>
+      </c>
+      <c r="I41" s="2">
+        <v>3.0718000000000001</v>
+      </c>
+      <c r="J41" s="2">
+        <v>31.423999999999999</v>
+      </c>
+      <c r="K41" s="2">
+        <v>192.41</v>
+      </c>
+      <c r="L41" s="2">
+        <v>7.1369999999999996</v>
+      </c>
+      <c r="M41" s="2">
+        <v>396.35</v>
+      </c>
+      <c r="N41" s="1">
+        <v>852.1</v>
+      </c>
     </row>
     <row r="42" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A42" s="13"/>
       <c r="B42" s="16"/>
+      <c r="C42" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="D42" s="4">
+        <v>4.6340000000000003</v>
+      </c>
+      <c r="E42" s="4">
+        <v>18.606999999999999</v>
+      </c>
+      <c r="F42" s="4">
+        <v>24.896000000000001</v>
+      </c>
+      <c r="G42" s="4">
+        <v>3.3435999999999999</v>
+      </c>
+      <c r="H42" s="4">
+        <v>1999.7</v>
+      </c>
+      <c r="I42" s="4">
+        <v>2.6438999999999999</v>
+      </c>
+      <c r="J42" s="4">
+        <v>10.422000000000001</v>
+      </c>
+      <c r="K42" s="4">
+        <v>72.31</v>
+      </c>
+      <c r="L42" s="4">
+        <v>16.370999999999999</v>
+      </c>
+      <c r="M42" s="4">
+        <v>260.37</v>
+      </c>
+      <c r="N42" s="3">
+        <v>628.53</v>
+      </c>
     </row>
     <row r="43" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A43" s="13"/>
       <c r="B43" s="16"/>
+      <c r="C43" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="D43" s="4">
+        <v>16.286999999999999</v>
+      </c>
+      <c r="E43" s="4">
+        <v>181.45</v>
+      </c>
+      <c r="F43" s="4">
+        <v>0.52517000000000003</v>
+      </c>
+      <c r="G43" s="4">
+        <v>3.0160999999999998</v>
+      </c>
+      <c r="H43" s="4">
+        <v>2606.1999999999998</v>
+      </c>
+      <c r="I43" s="4">
+        <v>2.7530999999999999</v>
+      </c>
+      <c r="J43" s="4">
+        <v>34.774000000000001</v>
+      </c>
+      <c r="K43" s="4">
+        <v>209.16</v>
+      </c>
+      <c r="L43" s="4">
+        <v>14.412000000000001</v>
+      </c>
+      <c r="M43" s="4">
+        <v>500.58</v>
+      </c>
+      <c r="N43" s="3">
+        <v>812.65</v>
+      </c>
     </row>
     <row r="44" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A44" s="13"/>
@@ -6026,18 +7272,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A38:A49"/>
+    <mergeCell ref="B38:B49"/>
+    <mergeCell ref="A50:A61"/>
+    <mergeCell ref="B50:B61"/>
+    <mergeCell ref="A62:A73"/>
+    <mergeCell ref="B62:B73"/>
     <mergeCell ref="A2:A13"/>
     <mergeCell ref="B2:B13"/>
     <mergeCell ref="A14:A25"/>
     <mergeCell ref="B14:B25"/>
     <mergeCell ref="A26:A37"/>
     <mergeCell ref="B26:B37"/>
-    <mergeCell ref="A38:A49"/>
-    <mergeCell ref="B38:B49"/>
-    <mergeCell ref="A50:A61"/>
-    <mergeCell ref="B50:B61"/>
-    <mergeCell ref="A62:A73"/>
-    <mergeCell ref="B62:B73"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -8335,12 +9581,12 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{666CFF77-8976-439D-A33C-D7841D6EB88F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C18A26E-30CA-4E63-A18A-C9C101DAF33C}">
   <dimension ref="A1:O73"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O35" sqref="O35"/>
+      <selection pane="bottomLeft" activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8410,202 +9656,51 @@
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="13"/>
       <c r="B3" s="16"/>
-      <c r="C3" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="D3" s="4">
-        <v>17.216999999999999</v>
-      </c>
-      <c r="E3" s="4">
-        <v>179.74</v>
-      </c>
-      <c r="F3" s="4">
-        <v>0.61753999999999998</v>
-      </c>
-      <c r="G3" s="4">
-        <v>4.4165999999999999</v>
-      </c>
-      <c r="H3" s="4">
-        <v>1783.5</v>
-      </c>
-      <c r="I3" s="2">
-        <v>2.0167000000000002</v>
-      </c>
-      <c r="J3" s="2">
-        <v>27.012</v>
-      </c>
-      <c r="K3" s="2">
-        <v>187.86</v>
-      </c>
-      <c r="L3" s="2">
-        <v>9.6981000000000002</v>
-      </c>
-      <c r="M3" s="2">
-        <v>87.406999999999996</v>
-      </c>
-      <c r="N3" s="1">
-        <v>320.89</v>
-      </c>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2"/>
+      <c r="N3" s="1"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="13"/>
       <c r="B4" s="16"/>
-      <c r="C4" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="D4" s="4">
-        <v>5.6908000000000003</v>
-      </c>
-      <c r="E4" s="4">
-        <v>66.626999999999995</v>
-      </c>
-      <c r="F4" s="4">
-        <v>1.9851000000000001</v>
-      </c>
-      <c r="G4" s="4">
-        <v>4.7723000000000004</v>
-      </c>
-      <c r="H4" s="4">
-        <v>1621.6</v>
-      </c>
-      <c r="I4" s="2">
-        <v>2.5163000000000002</v>
-      </c>
-      <c r="J4" s="2">
-        <v>27.937999999999999</v>
-      </c>
-      <c r="K4" s="2">
-        <v>187.97</v>
-      </c>
-      <c r="L4" s="2">
-        <v>9.4260999999999999</v>
-      </c>
-      <c r="M4" s="2">
-        <v>377.11</v>
-      </c>
-      <c r="N4" s="2">
-        <v>883.39</v>
-      </c>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
+      <c r="L4" s="2"/>
+      <c r="M4" s="2"/>
+      <c r="N4" s="2"/>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="13"/>
       <c r="B5" s="16"/>
-      <c r="C5" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="D5" s="4">
-        <v>9.3076000000000008</v>
-      </c>
-      <c r="E5" s="4">
-        <v>32.595999999999997</v>
-      </c>
-      <c r="F5" s="4">
-        <v>5.8113999999999999</v>
-      </c>
-      <c r="G5" s="4">
-        <v>4.5263</v>
-      </c>
-      <c r="H5" s="4">
-        <v>1775.9</v>
-      </c>
-      <c r="I5" s="2">
-        <v>2.0687000000000002</v>
-      </c>
-      <c r="J5" s="2">
-        <v>33.454999999999998</v>
-      </c>
-      <c r="K5" s="2">
-        <v>225.37</v>
-      </c>
-      <c r="L5" s="2">
-        <v>3.5903999999999998</v>
-      </c>
-      <c r="M5" s="2">
-        <v>103.26</v>
-      </c>
-      <c r="N5" s="2">
-        <v>462.92</v>
-      </c>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2"/>
+      <c r="L5" s="2"/>
+      <c r="M5" s="2"/>
+      <c r="N5" s="2"/>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="13"/>
       <c r="B6" s="16"/>
-      <c r="C6" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="D6" s="4">
-        <v>5.8951000000000002</v>
-      </c>
-      <c r="E6" s="4">
-        <v>36.244999999999997</v>
-      </c>
-      <c r="F6" s="4">
-        <v>5.3757000000000001</v>
-      </c>
-      <c r="G6" s="4">
-        <v>4.7310999999999996</v>
-      </c>
-      <c r="H6" s="4">
-        <v>1598.4</v>
-      </c>
-      <c r="I6" s="4">
-        <v>1.9289000000000001</v>
-      </c>
-      <c r="J6" s="4">
-        <v>39.776000000000003</v>
-      </c>
-      <c r="K6" s="4">
-        <v>261.52999999999997</v>
-      </c>
-      <c r="L6" s="4">
-        <v>2.7751000000000001</v>
-      </c>
-      <c r="M6" s="4">
-        <v>469.99</v>
-      </c>
-      <c r="N6" s="3">
-        <v>958.51</v>
-      </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="13"/>
       <c r="B7" s="16"/>
-      <c r="C7" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="D7" s="2">
-        <v>4.1862000000000004</v>
-      </c>
-      <c r="E7" s="2">
-        <v>84.548000000000002</v>
-      </c>
-      <c r="F7" s="2">
-        <v>2.1122999999999998</v>
-      </c>
-      <c r="G7" s="2">
-        <v>4.7751999999999999</v>
-      </c>
-      <c r="H7" s="2">
-        <v>1574.3</v>
-      </c>
-      <c r="I7" s="2">
-        <v>2.0095999999999998</v>
-      </c>
-      <c r="J7" s="2">
-        <v>28.899000000000001</v>
-      </c>
-      <c r="K7" s="2">
-        <v>198.44</v>
-      </c>
-      <c r="L7" s="2">
-        <v>3.7132000000000001</v>
-      </c>
-      <c r="M7" s="2">
-        <v>286.14</v>
-      </c>
-      <c r="N7" s="2">
-        <v>732.59</v>
-      </c>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="2"/>
+      <c r="L7" s="2"/>
+      <c r="M7" s="2"/>
+      <c r="N7" s="2"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="13"/>
@@ -8645,202 +9740,34 @@
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="13"/>
       <c r="B15" s="16"/>
-      <c r="C15" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="D15" s="4">
-        <v>31.327000000000002</v>
-      </c>
-      <c r="E15" s="4">
-        <v>104.92</v>
-      </c>
-      <c r="F15" s="4">
-        <v>0.8548</v>
-      </c>
-      <c r="G15" s="4">
-        <v>3.7507999999999999</v>
-      </c>
-      <c r="H15" s="4">
-        <v>2575.8000000000002</v>
-      </c>
-      <c r="I15" s="4">
-        <v>1.9380999999999999</v>
-      </c>
-      <c r="J15" s="4">
-        <v>36.652999999999999</v>
-      </c>
-      <c r="K15" s="4">
-        <v>239.99</v>
-      </c>
-      <c r="L15" s="4">
-        <v>2.3007</v>
-      </c>
-      <c r="M15" s="4">
-        <v>266.47000000000003</v>
-      </c>
-      <c r="N15" s="3">
-        <v>843.59</v>
-      </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="13"/>
       <c r="B16" s="16"/>
-      <c r="C16" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="D16" s="4">
-        <v>22.393000000000001</v>
-      </c>
-      <c r="E16" s="4">
-        <v>462.57</v>
-      </c>
-      <c r="F16" s="4">
-        <v>0.13572999999999999</v>
-      </c>
-      <c r="G16" s="4">
-        <v>4.3140000000000001</v>
-      </c>
-      <c r="H16" s="4">
-        <v>1828.1</v>
-      </c>
-      <c r="I16" s="2">
-        <v>1.9944999999999999</v>
-      </c>
-      <c r="J16" s="2">
-        <v>39.430999999999997</v>
-      </c>
-      <c r="K16" s="2">
-        <v>259.74</v>
-      </c>
-      <c r="L16" s="2">
-        <v>1.7996000000000001</v>
-      </c>
-      <c r="M16" s="2">
-        <v>316.17</v>
-      </c>
-      <c r="N16" s="2">
-        <v>991.58</v>
-      </c>
+      <c r="I16" s="2"/>
+      <c r="J16" s="2"/>
+      <c r="K16" s="2"/>
+      <c r="L16" s="2"/>
+      <c r="M16" s="2"/>
+      <c r="N16" s="2"/>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" s="13"/>
       <c r="B17" s="16"/>
-      <c r="C17" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="D17" s="4">
-        <v>11.45</v>
-      </c>
-      <c r="E17" s="4">
-        <v>53.151000000000003</v>
-      </c>
-      <c r="F17" s="4">
-        <v>7.1665999999999999</v>
-      </c>
-      <c r="G17" s="4">
-        <v>3.9502000000000002</v>
-      </c>
-      <c r="H17" s="4">
-        <v>2221.6</v>
-      </c>
-      <c r="I17" s="2">
-        <v>1.3278000000000001</v>
-      </c>
-      <c r="J17" s="2">
-        <v>35.21</v>
-      </c>
-      <c r="K17" s="2">
-        <v>248.59</v>
-      </c>
-      <c r="L17" s="2">
-        <v>2.6511999999999998</v>
-      </c>
-      <c r="M17" s="2">
-        <v>281.86</v>
-      </c>
-      <c r="N17" s="2">
-        <v>728.27</v>
-      </c>
+      <c r="I17" s="2"/>
+      <c r="J17" s="2"/>
+      <c r="K17" s="2"/>
+      <c r="L17" s="2"/>
+      <c r="M17" s="2"/>
+      <c r="N17" s="2"/>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" s="13"/>
       <c r="B18" s="16"/>
-      <c r="C18" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="D18" s="4">
-        <v>37.741999999999997</v>
-      </c>
-      <c r="E18" s="4">
-        <v>49.122999999999998</v>
-      </c>
-      <c r="F18" s="4">
-        <v>2.4996</v>
-      </c>
-      <c r="G18" s="4">
-        <v>3.4102000000000001</v>
-      </c>
-      <c r="H18" s="4">
-        <v>3172</v>
-      </c>
-      <c r="I18" s="4">
-        <v>1.6356999999999999</v>
-      </c>
-      <c r="J18" s="4">
-        <v>38.524000000000001</v>
-      </c>
-      <c r="K18" s="4">
-        <v>262.60000000000002</v>
-      </c>
-      <c r="L18" s="4">
-        <v>2.7321</v>
-      </c>
-      <c r="M18" s="4">
-        <v>435.37</v>
-      </c>
-      <c r="N18" s="3">
-        <v>930.53</v>
-      </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" s="13"/>
       <c r="B19" s="16"/>
-      <c r="C19" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="D19" s="4">
-        <v>18.768000000000001</v>
-      </c>
-      <c r="E19" s="4">
-        <v>89.18</v>
-      </c>
-      <c r="F19" s="4">
-        <v>0.88068999999999997</v>
-      </c>
-      <c r="G19" s="4">
-        <v>4.5054999999999996</v>
-      </c>
-      <c r="H19" s="4">
-        <v>1677.4</v>
-      </c>
-      <c r="I19" s="4">
-        <v>1.871</v>
-      </c>
-      <c r="J19" s="4">
-        <v>38.057000000000002</v>
-      </c>
-      <c r="K19" s="4">
-        <v>252.43</v>
-      </c>
-      <c r="L19" s="4">
-        <v>2.2942</v>
-      </c>
-      <c r="M19" s="4">
-        <v>196.55</v>
-      </c>
-      <c r="N19" s="3">
-        <v>665.69</v>
-      </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" s="13"/>
@@ -8880,42 +9807,6 @@
     <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27" s="13"/>
       <c r="B27" s="16"/>
-      <c r="C27" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="D27" s="4">
-        <v>4.8710000000000004</v>
-      </c>
-      <c r="E27" s="4">
-        <v>11.518000000000001</v>
-      </c>
-      <c r="F27" s="4">
-        <v>7.0281000000000002</v>
-      </c>
-      <c r="G27" s="4">
-        <v>4.2420999999999998</v>
-      </c>
-      <c r="H27" s="4">
-        <v>1138.3</v>
-      </c>
-      <c r="I27" s="4">
-        <v>6.7659000000000002</v>
-      </c>
-      <c r="J27" s="4">
-        <v>31.863</v>
-      </c>
-      <c r="K27" s="4">
-        <v>194.21</v>
-      </c>
-      <c r="L27" s="4">
-        <v>15.672000000000001</v>
-      </c>
-      <c r="M27" s="4">
-        <v>969.61</v>
-      </c>
-      <c r="N27" s="3">
-        <v>979.36</v>
-      </c>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28" s="13"/>
@@ -9145,18 +10036,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A2:A13"/>
+    <mergeCell ref="B2:B13"/>
+    <mergeCell ref="A14:A25"/>
+    <mergeCell ref="B14:B25"/>
+    <mergeCell ref="A26:A37"/>
+    <mergeCell ref="B26:B37"/>
     <mergeCell ref="A38:A49"/>
     <mergeCell ref="B38:B49"/>
     <mergeCell ref="A50:A61"/>
     <mergeCell ref="B50:B61"/>
     <mergeCell ref="A62:A73"/>
     <mergeCell ref="B62:B73"/>
-    <mergeCell ref="A2:A13"/>
-    <mergeCell ref="B2:B13"/>
-    <mergeCell ref="A14:A25"/>
-    <mergeCell ref="B14:B25"/>
-    <mergeCell ref="A26:A37"/>
-    <mergeCell ref="B26:B37"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
Added params for evpcd for 1000C and minor changes throughout scripts; also updated sem results
</commit_message>
<xml_diff>
--- a/scripts/__other__/__sem__.xlsx
+++ b/scripts/__other__/__sem__.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Janzen\Desktop\code\moga_neml\scripts\__other__\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4278C4F-BE90-4993-8B8E-A58FF350AACA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34CA155D-6BB9-40B1-BCC4-AF66CE904EBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="472" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="472" uniqueCount="53">
   <si>
     <t>temp</t>
   </si>
@@ -191,9 +191,6 @@
     <t>6; 9</t>
   </si>
   <si>
-    <t>7; 5</t>
-  </si>
-  <si>
     <t>6; 6</t>
   </si>
   <si>
@@ -210,7 +207,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -224,16 +221,316 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="10">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -334,11 +631,159 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="17" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -391,12 +836,50 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="42">
+    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -677,8 +1160,8 @@
   <dimension ref="A1:Q75"/>
   <sheetViews>
     <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A58" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D75" sqref="D75:H75"/>
+      <pane ySplit="1" topLeftCell="A51" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D63" sqref="D63:D72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2528,13 +3011,8 @@
       <c r="K73" s="7"/>
       <c r="L73" s="7"/>
     </row>
-    <row r="74" spans="1:12" s="18" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B74" s="3"/>
-      <c r="C74" s="8"/>
-      <c r="I74" s="8"/>
-      <c r="J74" s="8"/>
-      <c r="K74" s="8"/>
-      <c r="L74" s="8"/>
+    <row r="74" spans="1:12" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H74" s="4"/>
     </row>
     <row r="75" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D75" s="4">
@@ -2581,19 +3059,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE483CC8-AF2C-4D5A-AEE5-EF7DF4EC0883}">
-  <dimension ref="A1:T75"/>
+  <dimension ref="A1:L75"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A39" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D51" sqref="D51:K72"/>
+      <pane ySplit="1" topLeftCell="A42" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C72" sqref="C72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="4"/>
     <col min="2" max="2" width="9.140625" style="3"/>
-    <col min="3" max="3" width="15.7109375" style="8" customWidth="1"/>
-    <col min="4" max="11" width="9.140625" style="4"/>
+    <col min="3" max="3" width="15.7109375" style="9" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" style="9"/>
+    <col min="5" max="11" width="9.140625" style="4"/>
     <col min="12" max="12" width="9.140625" style="9"/>
     <col min="13" max="16384" width="9.140625" style="4"/>
   </cols>
@@ -2605,10 +3084,10 @@
       <c r="B1" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="11" t="s">
         <v>1</v>
       </c>
       <c r="E1" s="5" t="s">
@@ -2645,10 +3124,10 @@
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="13"/>
       <c r="B3" s="16"/>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="D3" s="4">
+      <c r="D3" s="9">
         <v>17.216999999999999</v>
       </c>
       <c r="E3" s="4">
@@ -2676,10 +3155,10 @@
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="13"/>
       <c r="B4" s="16"/>
-      <c r="C4" s="8" t="s">
+      <c r="C4" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="D4" s="4">
+      <c r="D4" s="9">
         <v>5.6908000000000003</v>
       </c>
       <c r="E4" s="4">
@@ -2707,10 +3186,10 @@
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="13"/>
       <c r="B5" s="16"/>
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="D5" s="4">
+      <c r="D5" s="9">
         <v>9.3076000000000008</v>
       </c>
       <c r="E5" s="4">
@@ -2738,10 +3217,10 @@
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="13"/>
       <c r="B6" s="16"/>
-      <c r="C6" s="8" t="s">
+      <c r="C6" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="D6" s="4">
+      <c r="D6" s="9">
         <v>5.8951000000000002</v>
       </c>
       <c r="E6" s="4">
@@ -2769,10 +3248,10 @@
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="13"/>
       <c r="B7" s="16"/>
-      <c r="C7" s="8" t="s">
+      <c r="C7" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="D7" s="4">
+      <c r="D7" s="9">
         <v>4.1862000000000004</v>
       </c>
       <c r="E7" s="4">
@@ -2800,10 +3279,10 @@
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="13"/>
       <c r="B8" s="16"/>
-      <c r="C8" s="8" t="s">
+      <c r="C8" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="D8" s="4">
+      <c r="D8" s="9">
         <v>25.038</v>
       </c>
       <c r="E8" s="4">
@@ -2831,10 +3310,10 @@
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="13"/>
       <c r="B9" s="16"/>
-      <c r="C9" s="8" t="s">
+      <c r="C9" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="D9" s="4">
+      <c r="D9" s="9">
         <v>27.547000000000001</v>
       </c>
       <c r="E9" s="4">
@@ -2862,10 +3341,10 @@
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="13"/>
       <c r="B10" s="16"/>
-      <c r="C10" s="8" t="s">
+      <c r="C10" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="D10" s="4">
+      <c r="D10" s="9">
         <v>27.885000000000002</v>
       </c>
       <c r="E10" s="4">
@@ -2893,10 +3372,10 @@
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="13"/>
       <c r="B11" s="16"/>
-      <c r="C11" s="8" t="s">
+      <c r="C11" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="D11" s="4">
+      <c r="D11" s="9">
         <v>19.2</v>
       </c>
       <c r="E11" s="4">
@@ -2924,10 +3403,10 @@
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="13"/>
       <c r="B12" s="16"/>
-      <c r="C12" s="8" t="s">
+      <c r="C12" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="D12" s="4">
+      <c r="D12" s="9">
         <v>8.5922999999999998</v>
       </c>
       <c r="E12" s="4">
@@ -2955,7 +3434,8 @@
     <row r="13" spans="1:12" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="14"/>
       <c r="B13" s="17"/>
-      <c r="C13" s="7"/>
+      <c r="C13" s="11"/>
+      <c r="D13" s="11"/>
       <c r="L13" s="11"/>
     </row>
     <row r="14" spans="1:12" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
@@ -2969,10 +3449,10 @@
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="13"/>
       <c r="B15" s="16"/>
-      <c r="C15" s="8" t="s">
+      <c r="C15" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="D15" s="4">
+      <c r="D15" s="9">
         <v>31.327000000000002</v>
       </c>
       <c r="E15" s="4">
@@ -3000,10 +3480,10 @@
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="13"/>
       <c r="B16" s="16"/>
-      <c r="C16" s="8" t="s">
+      <c r="C16" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="D16" s="2">
+      <c r="D16" s="10">
         <v>22.393000000000001</v>
       </c>
       <c r="E16" s="2">
@@ -3031,10 +3511,10 @@
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="13"/>
       <c r="B17" s="16"/>
-      <c r="C17" s="8" t="s">
+      <c r="C17" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="D17" s="4">
+      <c r="D17" s="9">
         <v>11.45</v>
       </c>
       <c r="E17" s="4">
@@ -3062,10 +3542,10 @@
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="13"/>
       <c r="B18" s="16"/>
-      <c r="C18" s="8" t="s">
+      <c r="C18" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="D18" s="4">
+      <c r="D18" s="9">
         <v>37.741999999999997</v>
       </c>
       <c r="E18" s="4">
@@ -3093,10 +3573,10 @@
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="13"/>
       <c r="B19" s="16"/>
-      <c r="C19" s="8" t="s">
+      <c r="C19" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="D19" s="4">
+      <c r="D19" s="9">
         <v>18.768000000000001</v>
       </c>
       <c r="E19" s="4">
@@ -3124,10 +3604,10 @@
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="13"/>
       <c r="B20" s="16"/>
-      <c r="C20" s="8" t="s">
+      <c r="C20" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="D20" s="4">
+      <c r="D20" s="9">
         <v>23.303999999999998</v>
       </c>
       <c r="E20" s="4">
@@ -3155,10 +3635,10 @@
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="13"/>
       <c r="B21" s="16"/>
-      <c r="C21" s="8" t="s">
+      <c r="C21" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="D21" s="4">
+      <c r="D21" s="9">
         <v>31.137</v>
       </c>
       <c r="E21" s="4">
@@ -3186,10 +3666,10 @@
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="13"/>
       <c r="B22" s="16"/>
-      <c r="C22" s="8" t="s">
+      <c r="C22" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="D22" s="4">
+      <c r="D22" s="9">
         <v>29.725999999999999</v>
       </c>
       <c r="E22" s="4">
@@ -3217,10 +3697,10 @@
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="13"/>
       <c r="B23" s="16"/>
-      <c r="C23" s="8" t="s">
+      <c r="C23" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="D23" s="4">
+      <c r="D23" s="9">
         <v>0.85682000000000003</v>
       </c>
       <c r="E23" s="4">
@@ -3248,10 +3728,10 @@
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="13"/>
       <c r="B24" s="16"/>
-      <c r="C24" s="8" t="s">
+      <c r="C24" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="D24" s="4">
+      <c r="D24" s="9">
         <v>4.4611000000000001</v>
       </c>
       <c r="E24" s="4">
@@ -3279,7 +3759,8 @@
     <row r="25" spans="1:12" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="14"/>
       <c r="B25" s="17"/>
-      <c r="C25" s="7"/>
+      <c r="C25" s="11"/>
+      <c r="D25" s="11"/>
       <c r="L25" s="11"/>
     </row>
     <row r="26" spans="1:12" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
@@ -3293,10 +3774,10 @@
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="13"/>
       <c r="B27" s="16"/>
-      <c r="C27" s="8" t="s">
+      <c r="C27" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="D27" s="4">
+      <c r="D27" s="9">
         <v>4.8710000000000004</v>
       </c>
       <c r="E27" s="4">
@@ -3324,10 +3805,10 @@
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="13"/>
       <c r="B28" s="16"/>
-      <c r="C28" s="8" t="s">
+      <c r="C28" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="D28" s="4">
+      <c r="D28" s="9">
         <v>10.692</v>
       </c>
       <c r="E28" s="4">
@@ -3355,10 +3836,10 @@
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" s="13"/>
       <c r="B29" s="16"/>
-      <c r="C29" s="8" t="s">
+      <c r="C29" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="D29" s="4">
+      <c r="D29" s="9">
         <v>11.2</v>
       </c>
       <c r="E29" s="4">
@@ -3386,10 +3867,10 @@
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" s="13"/>
       <c r="B30" s="16"/>
-      <c r="C30" s="8" t="s">
+      <c r="C30" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="D30" s="4">
+      <c r="D30" s="9">
         <v>11.208</v>
       </c>
       <c r="E30" s="4">
@@ -3417,10 +3898,10 @@
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" s="13"/>
       <c r="B31" s="16"/>
-      <c r="C31" s="8" t="s">
+      <c r="C31" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="D31" s="4">
+      <c r="D31" s="9">
         <v>10.45</v>
       </c>
       <c r="E31" s="4">
@@ -3448,10 +3929,10 @@
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" s="13"/>
       <c r="B32" s="16"/>
-      <c r="C32" s="8" t="s">
+      <c r="C32" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="D32" s="4">
+      <c r="D32" s="9">
         <v>11.010999999999999</v>
       </c>
       <c r="E32" s="4">
@@ -3479,10 +3960,10 @@
     <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" s="13"/>
       <c r="B33" s="16"/>
-      <c r="C33" s="8" t="s">
+      <c r="C33" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="D33" s="4">
+      <c r="D33" s="9">
         <v>5.6656000000000004</v>
       </c>
       <c r="E33" s="4">
@@ -3510,10 +3991,10 @@
     <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" s="13"/>
       <c r="B34" s="16"/>
-      <c r="C34" s="8" t="s">
+      <c r="C34" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="D34" s="4">
+      <c r="D34" s="9">
         <v>15.185</v>
       </c>
       <c r="E34" s="4">
@@ -3541,10 +4022,10 @@
     <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" s="13"/>
       <c r="B35" s="16"/>
-      <c r="C35" s="8" t="s">
+      <c r="C35" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="D35" s="4">
+      <c r="D35" s="9">
         <v>8.0571999999999999</v>
       </c>
       <c r="E35" s="4">
@@ -3572,10 +4053,10 @@
     <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" s="13"/>
       <c r="B36" s="16"/>
-      <c r="C36" s="8" t="s">
+      <c r="C36" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="D36" s="4">
+      <c r="D36" s="9">
         <v>7.5292000000000003</v>
       </c>
       <c r="E36" s="4">
@@ -3603,7 +4084,8 @@
     <row r="37" spans="1:12" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="14"/>
       <c r="B37" s="17"/>
-      <c r="C37" s="7"/>
+      <c r="C37" s="11"/>
+      <c r="D37" s="11"/>
       <c r="L37" s="11"/>
     </row>
     <row r="38" spans="1:12" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
@@ -3617,10 +4099,10 @@
     <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" s="13"/>
       <c r="B39" s="16"/>
-      <c r="C39" s="8" t="s">
+      <c r="C39" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="D39" s="4">
+      <c r="D39" s="9">
         <v>4.8238000000000003</v>
       </c>
       <c r="E39" s="4">
@@ -3648,10 +4130,10 @@
     <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40" s="13"/>
       <c r="B40" s="16"/>
-      <c r="C40" s="8" t="s">
+      <c r="C40" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="D40" s="4">
+      <c r="D40" s="9">
         <v>7.1036999999999999</v>
       </c>
       <c r="E40" s="4">
@@ -3679,10 +4161,10 @@
     <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41" s="13"/>
       <c r="B41" s="16"/>
-      <c r="C41" s="8" t="s">
+      <c r="C41" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="D41" s="4">
+      <c r="D41" s="9">
         <v>3.0461</v>
       </c>
       <c r="E41" s="4">
@@ -3710,10 +4192,10 @@
     <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42" s="13"/>
       <c r="B42" s="16"/>
-      <c r="C42" s="8" t="s">
+      <c r="C42" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="D42" s="4">
+      <c r="D42" s="9">
         <v>4.6340000000000003</v>
       </c>
       <c r="E42" s="4">
@@ -3741,10 +4223,10 @@
     <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43" s="13"/>
       <c r="B43" s="16"/>
-      <c r="C43" s="8" t="s">
+      <c r="C43" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="D43" s="4">
+      <c r="D43" s="9">
         <v>16.286999999999999</v>
       </c>
       <c r="E43" s="4">
@@ -3772,10 +4254,10 @@
     <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44" s="13"/>
       <c r="B44" s="16"/>
-      <c r="C44" s="8" t="s">
+      <c r="C44" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="D44" s="4">
+      <c r="D44" s="9">
         <v>9.5312999999999999</v>
       </c>
       <c r="E44" s="4">
@@ -3803,10 +4285,10 @@
     <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A45" s="13"/>
       <c r="B45" s="16"/>
-      <c r="C45" s="8" t="s">
+      <c r="C45" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="D45" s="4">
+      <c r="D45" s="9">
         <v>6.3647</v>
       </c>
       <c r="E45" s="4">
@@ -3834,10 +4316,10 @@
     <row r="46" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A46" s="13"/>
       <c r="B46" s="16"/>
-      <c r="C46" s="8" t="s">
+      <c r="C46" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="D46" s="4">
+      <c r="D46" s="9">
         <v>12.622</v>
       </c>
       <c r="E46" s="4">
@@ -3865,10 +4347,10 @@
     <row r="47" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A47" s="13"/>
       <c r="B47" s="16"/>
-      <c r="C47" s="8" t="s">
+      <c r="C47" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="D47" s="4">
+      <c r="D47" s="9">
         <v>12.256</v>
       </c>
       <c r="E47" s="4">
@@ -3896,10 +4378,10 @@
     <row r="48" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A48" s="13"/>
       <c r="B48" s="16"/>
-      <c r="C48" s="8" t="s">
+      <c r="C48" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="D48" s="4">
+      <c r="D48" s="9">
         <v>7.0439999999999996</v>
       </c>
       <c r="E48" s="4">
@@ -3924,13 +4406,14 @@
         <v>8.0541</v>
       </c>
     </row>
-    <row r="49" spans="1:20" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:12" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="14"/>
       <c r="B49" s="17"/>
-      <c r="C49" s="7"/>
+      <c r="C49" s="11"/>
+      <c r="D49" s="11"/>
       <c r="L49" s="11"/>
     </row>
-    <row r="50" spans="1:20" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:12" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="12">
         <v>1000</v>
       </c>
@@ -3938,323 +4421,324 @@
         <v>6</v>
       </c>
     </row>
-    <row r="51" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A51" s="13"/>
       <c r="B51" s="16"/>
-      <c r="C51" s="8" t="s">
+      <c r="C51" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="M51" s="4">
+      <c r="D51" s="9">
         <v>1.9315</v>
       </c>
-      <c r="N51" s="4">
+      <c r="E51" s="4">
         <v>481.1</v>
       </c>
-      <c r="O51" s="4">
+      <c r="F51" s="4">
         <v>2.1642000000000002E-2</v>
       </c>
-      <c r="P51" s="4">
+      <c r="G51" s="4">
         <v>4.1571999999999996</v>
       </c>
-      <c r="Q51" s="4">
+      <c r="H51" s="4">
         <v>723.11</v>
       </c>
-      <c r="R51" s="4">
-        <v>5015.3</v>
-      </c>
-      <c r="S51" s="4">
-        <v>3.1227999999999998</v>
-      </c>
-      <c r="T51" s="4">
-        <v>9.1630000000000003</v>
-      </c>
-    </row>
-    <row r="52" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="I51" s="4">
+        <v>3740</v>
+      </c>
+      <c r="J51" s="4">
+        <v>3.2786</v>
+      </c>
+      <c r="K51" s="4">
+        <v>7.5526</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A52" s="13"/>
       <c r="B52" s="16"/>
-      <c r="C52" s="8" t="s">
+      <c r="C52" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="M52" s="4">
+      <c r="D52" s="9">
         <v>3.746</v>
       </c>
-      <c r="N52" s="4">
+      <c r="E52" s="4">
         <v>8.6539999999999999</v>
       </c>
-      <c r="O52" s="4">
+      <c r="F52" s="4">
         <v>4.2439</v>
       </c>
-      <c r="P52" s="4">
+      <c r="G52" s="4">
         <v>3.9319999999999999</v>
       </c>
-      <c r="Q52" s="4">
+      <c r="H52" s="4">
         <v>749.09</v>
       </c>
-      <c r="R52" s="4">
-        <v>9246.1</v>
-      </c>
-      <c r="S52" s="4">
-        <v>2.7896000000000001</v>
-      </c>
-      <c r="T52" s="4">
-        <v>5.7472000000000003</v>
-      </c>
-    </row>
-    <row r="53" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="I52" s="4">
+        <v>9410</v>
+      </c>
+      <c r="J52" s="4">
+        <v>2.7616999999999998</v>
+      </c>
+      <c r="K52" s="4">
+        <v>5.2934000000000001</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A53" s="13"/>
       <c r="B53" s="16"/>
-      <c r="C53" s="8" t="s">
+      <c r="C53" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="M53" s="4">
+      <c r="D53" s="9">
         <v>0.98812</v>
       </c>
-      <c r="N53" s="4">
+      <c r="E53" s="4">
         <v>26.957999999999998</v>
       </c>
-      <c r="O53" s="4">
+      <c r="F53" s="4">
         <v>0.64437999999999995</v>
       </c>
-      <c r="P53" s="4">
+      <c r="G53" s="4">
         <v>4.4935999999999998</v>
       </c>
-      <c r="Q53" s="4">
+      <c r="H53" s="4">
         <v>567.97</v>
       </c>
-      <c r="R53" s="4">
-        <v>2395</v>
-      </c>
-      <c r="S53" s="4">
-        <v>3.552</v>
-      </c>
-      <c r="T53" s="4">
-        <v>6.7481999999999998</v>
-      </c>
-    </row>
-    <row r="54" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="I53" s="4">
+        <v>1468.2</v>
+      </c>
+      <c r="J53" s="4">
+        <v>3.8721999999999999</v>
+      </c>
+      <c r="K53" s="4">
+        <v>6.1177999999999999</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A54" s="13"/>
       <c r="B54" s="16"/>
-      <c r="C54" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="M54" s="4">
+      <c r="C54" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="D54" s="9">
         <v>0.34142</v>
       </c>
-      <c r="N54" s="4">
+      <c r="E54" s="4">
         <v>0.1263</v>
       </c>
-      <c r="O54" s="4">
+      <c r="F54" s="4">
         <v>3.5680000000000001</v>
       </c>
-      <c r="P54" s="4">
+      <c r="G54" s="4">
         <v>4.6580000000000004</v>
       </c>
-      <c r="Q54" s="4">
+      <c r="H54" s="4">
         <v>537.80999999999995</v>
       </c>
-      <c r="R54" s="4">
-        <v>5130.7</v>
-      </c>
-      <c r="S54" s="4">
-        <v>3.1514000000000002</v>
-      </c>
-      <c r="T54" s="4">
-        <v>9.5030999999999999</v>
-      </c>
-    </row>
-    <row r="55" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="I54" s="4">
+        <v>9589.7999999999993</v>
+      </c>
+      <c r="J54" s="4">
+        <v>2.8538999999999999</v>
+      </c>
+      <c r="K54" s="4">
+        <v>9.4672999999999998</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A55" s="13"/>
       <c r="B55" s="16"/>
-      <c r="C55" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="M55" s="4">
+      <c r="C55" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="D55" s="9">
         <v>0.90237000000000001</v>
       </c>
-      <c r="N55" s="4">
+      <c r="E55" s="4">
         <v>5.2742000000000004</v>
       </c>
-      <c r="O55" s="4">
+      <c r="F55" s="4">
         <v>1.5201</v>
       </c>
-      <c r="P55" s="4">
+      <c r="G55" s="4">
         <v>4.5481999999999996</v>
       </c>
-      <c r="Q55" s="4">
+      <c r="H55" s="4">
         <v>558.20000000000005</v>
       </c>
-      <c r="R55" s="4">
-        <v>6762.3</v>
-      </c>
-      <c r="S55" s="4">
-        <v>2.9710000000000001</v>
-      </c>
-      <c r="T55" s="4">
-        <v>7.3547000000000002</v>
-      </c>
-    </row>
-    <row r="56" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="I55" s="4">
+        <v>5918.3</v>
+      </c>
+      <c r="J55" s="4">
+        <v>3.0358000000000001</v>
+      </c>
+      <c r="K55" s="4">
+        <v>7.2259000000000002</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A56" s="13"/>
       <c r="B56" s="16"/>
-      <c r="C56" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="M56" s="4">
+      <c r="C56" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="D56" s="9">
         <v>2.2723</v>
       </c>
-      <c r="N56" s="4">
+      <c r="E56" s="4">
         <v>17.684000000000001</v>
       </c>
-      <c r="O56" s="4">
+      <c r="F56" s="4">
         <v>0.52432000000000001</v>
       </c>
-      <c r="P56" s="4">
+      <c r="G56" s="4">
         <v>4.1894999999999998</v>
       </c>
-      <c r="Q56" s="4">
+      <c r="H56" s="4">
         <v>695.87</v>
       </c>
-      <c r="R56" s="4">
-        <v>4416.3999999999996</v>
-      </c>
-      <c r="S56" s="4">
-        <v>3.1836000000000002</v>
-      </c>
-      <c r="T56" s="4">
-        <v>7.1730999999999998</v>
-      </c>
-    </row>
-    <row r="57" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="I56" s="4">
+        <v>4582.3</v>
+      </c>
+      <c r="J56" s="4">
+        <v>3.1497999999999999</v>
+      </c>
+      <c r="K56" s="4">
+        <v>7.1169000000000002</v>
+      </c>
+    </row>
+    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A57" s="13"/>
       <c r="B57" s="16"/>
-      <c r="C57" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="M57" s="4">
+      <c r="C57" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="D57" s="9">
         <v>1.7845</v>
       </c>
-      <c r="N57" s="4">
+      <c r="E57" s="4">
         <v>0.26406000000000002</v>
       </c>
-      <c r="O57" s="4">
+      <c r="F57" s="4">
         <v>25.678000000000001</v>
       </c>
-      <c r="P57" s="4">
+      <c r="G57" s="4">
         <v>4.2798999999999996</v>
       </c>
-      <c r="Q57" s="4">
+      <c r="H57" s="4">
         <v>669.49</v>
       </c>
-      <c r="R57" s="4">
-        <v>9702.4</v>
-      </c>
-      <c r="S57" s="4">
-        <v>2.8408000000000002</v>
-      </c>
-      <c r="T57" s="4">
-        <v>8.8193999999999999</v>
-      </c>
-    </row>
-    <row r="58" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="I57" s="4">
+        <v>9813.7000000000007</v>
+      </c>
+      <c r="J57" s="4">
+        <v>2.8523000000000001</v>
+      </c>
+      <c r="K57" s="4">
+        <v>10.242000000000001</v>
+      </c>
+    </row>
+    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A58" s="13"/>
       <c r="B58" s="16"/>
-      <c r="C58" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="M58" s="4">
+      <c r="C58" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="D58" s="9">
         <v>1.2223999999999999</v>
       </c>
-      <c r="N58" s="4">
+      <c r="E58" s="4">
         <v>3.6264999999999999E-2</v>
       </c>
-      <c r="O58" s="4">
+      <c r="F58" s="4">
         <v>6.5932000000000004</v>
       </c>
-      <c r="P58" s="4">
+      <c r="G58" s="4">
         <v>4.3323</v>
       </c>
-      <c r="Q58" s="4">
+      <c r="H58" s="4">
         <v>673.71</v>
       </c>
-      <c r="R58" s="4">
-        <v>8825.2000000000007</v>
-      </c>
-      <c r="S58" s="4">
-        <v>2.8908999999999998</v>
-      </c>
-      <c r="T58" s="4">
-        <v>9.6677999999999997</v>
-      </c>
-    </row>
-    <row r="59" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="I58" s="4">
+        <v>9449.6</v>
+      </c>
+      <c r="J58" s="4">
+        <v>2.8868999999999998</v>
+      </c>
+      <c r="K58" s="4">
+        <v>11.574999999999999</v>
+      </c>
+    </row>
+    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A59" s="13"/>
       <c r="B59" s="16"/>
-      <c r="C59" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="M59" s="4">
+      <c r="C59" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="D59" s="9">
         <v>1.5227999999999999</v>
       </c>
-      <c r="N59" s="4">
+      <c r="E59" s="4">
         <v>4.8478000000000003</v>
       </c>
-      <c r="O59" s="4">
+      <c r="F59" s="4">
         <v>3.7315</v>
       </c>
-      <c r="P59" s="4">
+      <c r="G59" s="4">
         <v>4.4061000000000003</v>
       </c>
-      <c r="Q59" s="4">
+      <c r="H59" s="4">
         <v>590.03</v>
       </c>
-      <c r="R59" s="4">
-        <v>4508.3</v>
-      </c>
-      <c r="S59" s="4">
-        <v>3.1535000000000002</v>
-      </c>
-      <c r="T59" s="4">
-        <v>6.3638000000000003</v>
-      </c>
-    </row>
-    <row r="60" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="I59" s="4">
+        <v>9411</v>
+      </c>
+      <c r="J59" s="4">
+        <v>2.8043999999999998</v>
+      </c>
+      <c r="K59" s="4">
+        <v>6.3834999999999997</v>
+      </c>
+    </row>
+    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A60" s="13"/>
       <c r="B60" s="16"/>
-      <c r="C60" s="8" t="s">
+      <c r="C60" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="M60" s="4">
+      <c r="D60" s="9">
         <v>3.0295000000000001</v>
       </c>
-      <c r="N60" s="4">
+      <c r="E60" s="4">
         <v>12.903</v>
       </c>
-      <c r="O60" s="4">
+      <c r="F60" s="4">
         <v>2.3944000000000001</v>
       </c>
-      <c r="P60" s="4">
+      <c r="G60" s="4">
         <v>4.0586000000000002</v>
       </c>
-      <c r="Q60" s="4">
+      <c r="H60" s="4">
         <v>713.26</v>
       </c>
-      <c r="R60" s="4">
-        <v>3970.7</v>
-      </c>
-      <c r="S60" s="4">
-        <v>3.1777000000000002</v>
-      </c>
-      <c r="T60" s="4">
-        <v>4.9123999999999999</v>
-      </c>
-    </row>
-    <row r="61" spans="1:20" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I60" s="4">
+        <v>1346.8</v>
+      </c>
+      <c r="J60" s="4">
+        <v>3.9352</v>
+      </c>
+      <c r="K60" s="4">
+        <v>5.4934000000000003</v>
+      </c>
+    </row>
+    <row r="61" spans="1:12" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="14"/>
       <c r="B61" s="17"/>
-      <c r="C61" s="7"/>
+      <c r="C61" s="11"/>
+      <c r="D61" s="11"/>
       <c r="L61" s="11"/>
     </row>
-    <row r="62" spans="1:20" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:12" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="12">
         <v>1000</v>
       </c>
@@ -4262,335 +4746,332 @@
         <v>7</v>
       </c>
     </row>
-    <row r="63" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A63" s="13"/>
       <c r="B63" s="16"/>
-      <c r="C63" s="8" t="s">
+      <c r="C63" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="M63" s="4">
+      <c r="D63" s="9">
         <v>4.6150000000000002E-3</v>
       </c>
-      <c r="N63" s="4">
+      <c r="E63" s="4">
         <v>6.1843000000000004</v>
       </c>
-      <c r="O63" s="4">
+      <c r="F63" s="4">
         <v>2.2823000000000002</v>
       </c>
-      <c r="P63" s="4">
+      <c r="G63" s="4">
         <v>4.8326000000000002</v>
       </c>
-      <c r="Q63" s="4">
+      <c r="H63" s="4">
         <v>460.27</v>
       </c>
-      <c r="R63" s="4">
-        <v>3478.8</v>
-      </c>
-      <c r="S63" s="4">
-        <v>3.3414000000000001</v>
-      </c>
-      <c r="T63" s="4">
-        <v>7.4029999999999996</v>
-      </c>
-    </row>
-    <row r="64" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="I63" s="4">
+        <v>2357.9</v>
+      </c>
+      <c r="J63" s="4">
+        <v>3.5989</v>
+      </c>
+      <c r="K63" s="4">
+        <v>6.8388</v>
+      </c>
+    </row>
+    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A64" s="13"/>
       <c r="B64" s="16"/>
-      <c r="C64" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="M64" s="4">
+      <c r="C64" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D64" s="9">
         <v>3.9207000000000001</v>
       </c>
-      <c r="N64" s="4">
+      <c r="E64" s="4">
         <v>130.97</v>
       </c>
-      <c r="O64" s="4">
+      <c r="F64" s="4">
         <v>0.16188</v>
       </c>
-      <c r="P64" s="4">
+      <c r="G64" s="4">
         <v>3.9466000000000001</v>
       </c>
-      <c r="Q64" s="4">
+      <c r="H64" s="4">
         <v>752.32</v>
       </c>
-      <c r="R64" s="4">
-        <v>2965</v>
-      </c>
-      <c r="S64" s="4">
-        <v>3.3761000000000001</v>
-      </c>
-      <c r="T64" s="4">
-        <v>5.2625999999999999</v>
-      </c>
-    </row>
-    <row r="65" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="I64" s="4">
+        <v>2450.1</v>
+      </c>
+      <c r="J64" s="4">
+        <v>3.5356000000000001</v>
+      </c>
+      <c r="K64" s="4">
+        <v>6.1744000000000003</v>
+      </c>
+    </row>
+    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A65" s="13"/>
       <c r="B65" s="16"/>
-      <c r="C65" s="8" t="s">
+      <c r="C65" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="M65" s="4">
+      <c r="D65" s="9">
         <v>1.2675000000000001E-2</v>
       </c>
-      <c r="N65" s="4">
+      <c r="E65" s="4">
         <v>18.527999999999999</v>
       </c>
-      <c r="O65" s="4">
+      <c r="F65" s="4">
         <v>0.99367000000000005</v>
       </c>
-      <c r="P65" s="4">
+      <c r="G65" s="4">
         <v>4.8133999999999997</v>
       </c>
-      <c r="Q65" s="4">
+      <c r="H65" s="4">
         <v>471.18</v>
       </c>
-      <c r="R65" s="4">
-        <v>2229.9</v>
-      </c>
-      <c r="S65" s="4">
-        <v>3.5893000000000002</v>
-      </c>
-      <c r="T65" s="4">
-        <v>5.6052</v>
-      </c>
-    </row>
-    <row r="66" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="I65" s="4">
+        <v>2932.6</v>
+      </c>
+      <c r="J65" s="4">
+        <v>3.3719999999999999</v>
+      </c>
+      <c r="K65" s="4">
+        <v>5.7801999999999998</v>
+      </c>
+    </row>
+    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A66" s="13"/>
       <c r="B66" s="16"/>
-      <c r="C66" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="M66" s="4">
+      <c r="C66" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="D66" s="9">
         <v>0.26123000000000002</v>
       </c>
-      <c r="N66" s="4">
+      <c r="E66" s="4">
         <v>35.054000000000002</v>
       </c>
-      <c r="O66" s="4">
+      <c r="F66" s="4">
         <v>0.42681000000000002</v>
       </c>
-      <c r="P66" s="4">
+      <c r="G66" s="4">
         <v>4.7435999999999998</v>
       </c>
-      <c r="Q66" s="4">
+      <c r="H66" s="4">
         <v>490.7</v>
       </c>
-      <c r="R66" s="4">
-        <v>2850.7</v>
-      </c>
-      <c r="S66" s="4">
-        <v>3.4043000000000001</v>
-      </c>
-      <c r="T66" s="4">
-        <v>5.3243</v>
-      </c>
-    </row>
-    <row r="67" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="I66" s="4">
+        <v>2942.6</v>
+      </c>
+      <c r="J66" s="4">
+        <v>3.3807</v>
+      </c>
+      <c r="K66" s="4">
+        <v>5.9217000000000004</v>
+      </c>
+    </row>
+    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A67" s="13"/>
       <c r="B67" s="16"/>
-      <c r="C67" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="M67" s="4">
+      <c r="C67" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="D67" s="9">
         <v>1.4714</v>
       </c>
-      <c r="N67" s="4">
+      <c r="E67" s="4">
         <v>3.11</v>
       </c>
-      <c r="O67" s="4">
+      <c r="F67" s="4">
         <v>5.9009</v>
       </c>
-      <c r="P67" s="4">
+      <c r="G67" s="4">
         <v>4.4241000000000001</v>
       </c>
-      <c r="Q67" s="4">
+      <c r="H67" s="4">
         <v>584.77</v>
       </c>
-      <c r="R67" s="4">
-        <v>3948.5</v>
-      </c>
-      <c r="S67" s="4">
-        <v>3.2559</v>
-      </c>
-      <c r="T67" s="4">
-        <v>7.3000999999999996</v>
-      </c>
-    </row>
-    <row r="68" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="I67" s="4">
+        <v>1053.2</v>
+      </c>
+      <c r="J67" s="4">
+        <v>4.2660999999999998</v>
+      </c>
+      <c r="K67" s="4">
+        <v>7.1360000000000001</v>
+      </c>
+    </row>
+    <row r="68" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A68" s="13"/>
       <c r="B68" s="16"/>
-      <c r="C68" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="M68" s="4">
+      <c r="C68" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="D68" s="9">
         <v>4.1444999999999999</v>
       </c>
-      <c r="N68" s="4">
+      <c r="E68" s="4">
         <v>21.946000000000002</v>
       </c>
-      <c r="O68" s="4">
+      <c r="F68" s="4">
         <v>1.2583</v>
       </c>
-      <c r="P68" s="4">
+      <c r="G68" s="4">
         <v>3.9466999999999999</v>
       </c>
-      <c r="Q68" s="4">
+      <c r="H68" s="4">
         <v>726.26</v>
       </c>
-      <c r="R68" s="4">
-        <v>3639.1</v>
-      </c>
-      <c r="S68" s="4">
-        <v>3.2450999999999999</v>
-      </c>
-      <c r="T68" s="4">
-        <v>4.9524999999999997</v>
-      </c>
-    </row>
-    <row r="69" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="I68" s="4">
+        <v>1609</v>
+      </c>
+      <c r="J68" s="4">
+        <v>3.8399000000000001</v>
+      </c>
+      <c r="K68" s="4">
+        <v>5.3898000000000001</v>
+      </c>
+    </row>
+    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A69" s="13"/>
       <c r="B69" s="16"/>
-      <c r="C69" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="M69" s="4">
+      <c r="C69" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="D69" s="9">
         <v>3.2084999999999999</v>
       </c>
-      <c r="N69" s="4">
+      <c r="E69" s="4">
         <v>17.286999999999999</v>
       </c>
-      <c r="O69" s="4">
+      <c r="F69" s="4">
         <v>1.3622000000000001</v>
       </c>
-      <c r="P69" s="4">
+      <c r="G69" s="4">
         <v>4.0769000000000002</v>
       </c>
-      <c r="Q69" s="4">
+      <c r="H69" s="4">
         <v>697.16</v>
       </c>
-      <c r="R69" s="4">
-        <v>3927.3</v>
-      </c>
-      <c r="S69" s="4">
-        <v>3.2118000000000002</v>
-      </c>
-      <c r="T69" s="4">
-        <v>4.7915999999999999</v>
-      </c>
-    </row>
-    <row r="70" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="I69" s="4">
+        <v>3844.1</v>
+      </c>
+      <c r="J69" s="4">
+        <v>3.2155999999999998</v>
+      </c>
+      <c r="K69" s="4">
+        <v>5.6135000000000002</v>
+      </c>
+    </row>
+    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A70" s="13"/>
       <c r="B70" s="16"/>
-      <c r="C70" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="M70" s="4">
+      <c r="C70" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="D70" s="9">
         <v>4.3445999999999998</v>
       </c>
-      <c r="N70" s="4">
+      <c r="E70" s="4">
         <v>10.148</v>
       </c>
-      <c r="O70" s="4">
+      <c r="F70" s="4">
         <v>2.2065999999999999</v>
       </c>
-      <c r="P70" s="4">
+      <c r="G70" s="4">
         <v>3.8805999999999998</v>
       </c>
-      <c r="Q70" s="4">
+      <c r="H70" s="4">
         <v>776.41</v>
       </c>
-      <c r="R70" s="4">
-        <v>4502.1000000000004</v>
-      </c>
-      <c r="S70" s="4">
-        <v>3.1688000000000001</v>
-      </c>
-      <c r="T70" s="4">
-        <v>6.5437000000000003</v>
-      </c>
-    </row>
-    <row r="71" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="I70" s="4">
+        <v>2358.5</v>
+      </c>
+      <c r="J70" s="4">
+        <v>3.5762999999999998</v>
+      </c>
+      <c r="K70" s="4">
+        <v>7.0132000000000003</v>
+      </c>
+    </row>
+    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A71" s="13"/>
       <c r="B71" s="16"/>
-      <c r="C71" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="M71" s="4">
+      <c r="C71" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="D71" s="9">
         <v>3.3748</v>
       </c>
-      <c r="N71" s="4">
+      <c r="E71" s="4">
         <v>51.076000000000001</v>
       </c>
-      <c r="O71" s="4">
+      <c r="F71" s="4">
         <v>0.45746999999999999</v>
       </c>
-      <c r="P71" s="4">
+      <c r="G71" s="4">
         <v>4.0575000000000001</v>
       </c>
-      <c r="Q71" s="4">
+      <c r="H71" s="4">
         <v>700.49</v>
       </c>
-      <c r="R71" s="4">
-        <v>2863</v>
-      </c>
-      <c r="S71" s="4">
-        <v>3.4026999999999998</v>
-      </c>
-      <c r="T71" s="4">
-        <v>5.3670999999999998</v>
-      </c>
-    </row>
-    <row r="72" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="I71" s="4">
+        <v>1035.7</v>
+      </c>
+      <c r="J71" s="4">
+        <v>4.2337999999999996</v>
+      </c>
+      <c r="K71" s="4">
+        <v>6.0335999999999999</v>
+      </c>
+    </row>
+    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A72" s="13"/>
       <c r="B72" s="16"/>
-      <c r="C72" s="8" t="s">
+      <c r="C72" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="M72" s="4">
+      <c r="D72" s="9">
         <v>4.2664999999999997</v>
       </c>
-      <c r="N72" s="4">
+      <c r="E72" s="4">
         <v>246.76</v>
       </c>
-      <c r="O72" s="4">
+      <c r="F72" s="4">
         <v>8.4953000000000001E-2</v>
       </c>
-      <c r="P72" s="4">
+      <c r="G72" s="4">
         <v>3.9445000000000001</v>
       </c>
-      <c r="Q72" s="4">
+      <c r="H72" s="4">
         <v>738.14</v>
       </c>
-      <c r="R72" s="4">
-        <v>2087.1999999999998</v>
-      </c>
-      <c r="S72" s="4">
-        <v>3.6288</v>
-      </c>
-      <c r="T72" s="4">
-        <v>5.3070000000000004</v>
-      </c>
-    </row>
-    <row r="73" spans="1:20" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I72" s="4">
+        <v>2675.8</v>
+      </c>
+      <c r="J72" s="4">
+        <v>3.4394999999999998</v>
+      </c>
+      <c r="K72" s="4">
+        <v>5.8158000000000003</v>
+      </c>
+    </row>
+    <row r="73" spans="1:12" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="14"/>
       <c r="B73" s="17"/>
-      <c r="C73" s="7"/>
+      <c r="C73" s="11"/>
+      <c r="D73" s="11"/>
       <c r="L73" s="11"/>
     </row>
-    <row r="74" spans="1:20" s="18" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B74" s="3"/>
-      <c r="C74" s="8"/>
-      <c r="L74" s="9"/>
-    </row>
-    <row r="75" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="D75" s="4">
+    <row r="74" spans="1:12" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="75" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D75" s="9">
         <f>MAX(D1:D71)</f>
         <v>37.741999999999997</v>
       </c>
       <c r="E75" s="4">
         <f t="shared" ref="E75:K75" si="0">MAX(E1:E71)</f>
-        <v>462.57</v>
+        <v>481.1</v>
       </c>
       <c r="F75" s="4">
         <f t="shared" si="0"/>
@@ -4598,7 +5079,7 @@
       </c>
       <c r="G75" s="4">
         <f t="shared" si="0"/>
-        <v>4.7751999999999999</v>
+        <v>4.8326000000000002</v>
       </c>
       <c r="H75" s="4">
         <f t="shared" si="0"/>
@@ -4606,7 +5087,7 @@
       </c>
       <c r="I75" s="4">
         <f t="shared" si="0"/>
-        <v>4771.8999999999996</v>
+        <v>9813.7000000000007</v>
       </c>
       <c r="J75" s="4">
         <f t="shared" si="0"/>
@@ -6096,11 +6577,7 @@
       <c r="C73" s="7"/>
       <c r="L73" s="11"/>
     </row>
-    <row r="74" spans="1:12" s="18" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B74" s="3"/>
-      <c r="C74" s="8"/>
-      <c r="L74" s="9"/>
-    </row>
+    <row r="74" spans="1:12" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="75" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D75" s="4">
         <f>MAX(D1:D71)</f>
@@ -6822,7 +7299,7 @@
       <c r="A30" s="13"/>
       <c r="B30" s="16"/>
       <c r="C30" s="8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D30" s="4">
         <v>11.208</v>
@@ -6977,7 +7454,7 @@
       <c r="A40" s="13"/>
       <c r="B40" s="16"/>
       <c r="C40" s="8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D40" s="4">
         <v>7.1036999999999999</v>
@@ -7017,7 +7494,7 @@
       <c r="A41" s="13"/>
       <c r="B41" s="16"/>
       <c r="C41" s="8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D41" s="4">
         <v>3.0461</v>
@@ -7057,7 +7534,7 @@
       <c r="A42" s="13"/>
       <c r="B42" s="16"/>
       <c r="C42" s="8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D42" s="4">
         <v>4.6340000000000003</v>
@@ -7097,7 +7574,7 @@
       <c r="A43" s="13"/>
       <c r="B43" s="16"/>
       <c r="C43" s="8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D43" s="4">
         <v>16.286999999999999</v>

</xml_diff>

<commit_message>
Added some testing scripts; many artefacts to be removed
</commit_message>
<xml_diff>
--- a/scripts/__other__/__sem__.xlsx
+++ b/scripts/__other__/__sem__.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Janzen\Desktop\code\moga_neml\scripts\__other__\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34CA155D-6BB9-40B1-BCC4-AF66CE904EBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C7FE0E5-13DA-4EB3-88E7-48F53D0EE399}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="evp" sheetId="13" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="472" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="532" uniqueCount="53">
   <si>
     <t>temp</t>
   </si>
@@ -1159,9 +1159,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4D7A15E-4182-42F6-82DA-99E9B04906BA}">
   <dimension ref="A1:Q75"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A51" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D63" sqref="D63:D72"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A42" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D62" sqref="D62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1171,7 +1171,8 @@
     <col min="3" max="3" width="15.7109375" style="8" customWidth="1"/>
     <col min="4" max="7" width="9.140625" style="4"/>
     <col min="8" max="8" width="9.140625" style="3"/>
-    <col min="9" max="12" width="15.7109375" style="8" customWidth="1"/>
+    <col min="9" max="9" width="15.7109375" style="9" customWidth="1"/>
+    <col min="10" max="12" width="15.7109375" style="8" customWidth="1"/>
     <col min="13" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
@@ -1200,7 +1201,7 @@
       <c r="H1" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="7" t="s">
+      <c r="I1" s="11" t="s">
         <v>39</v>
       </c>
       <c r="J1" s="7" t="s">
@@ -1242,7 +1243,7 @@
       <c r="H3" s="3">
         <v>1783.5</v>
       </c>
-      <c r="I3" s="8" t="s">
+      <c r="I3" s="9" t="s">
         <v>34</v>
       </c>
       <c r="J3" s="8" t="s">
@@ -1273,7 +1274,7 @@
       <c r="H4" s="1">
         <v>1621.6</v>
       </c>
-      <c r="I4" s="8" t="s">
+      <c r="I4" s="9" t="s">
         <v>29</v>
       </c>
       <c r="J4" s="8" t="s">
@@ -1304,7 +1305,7 @@
       <c r="H5" s="1">
         <v>1775.9</v>
       </c>
-      <c r="I5" s="8" t="s">
+      <c r="I5" s="9" t="s">
         <v>31</v>
       </c>
       <c r="J5" s="8" t="s">
@@ -1335,7 +1336,7 @@
       <c r="H6" s="1">
         <v>1598.4</v>
       </c>
-      <c r="I6" s="8" t="s">
+      <c r="I6" s="9" t="s">
         <v>38</v>
       </c>
       <c r="J6" s="8" t="s">
@@ -1366,7 +1367,7 @@
       <c r="H7" s="1">
         <v>1574.3</v>
       </c>
-      <c r="I7" s="8" t="s">
+      <c r="I7" s="9" t="s">
         <v>38</v>
       </c>
       <c r="J7" s="8" t="s">
@@ -1397,7 +1398,7 @@
       <c r="H8" s="1">
         <v>1944.6</v>
       </c>
-      <c r="I8" s="8" t="s">
+      <c r="I8" s="9" t="s">
         <v>19</v>
       </c>
       <c r="J8" s="8" t="s">
@@ -1428,7 +1429,7 @@
       <c r="H9" s="1">
         <v>2454.8000000000002</v>
       </c>
-      <c r="I9" s="8" t="s">
+      <c r="I9" s="9" t="s">
         <v>23</v>
       </c>
       <c r="J9" s="8" t="s">
@@ -1459,7 +1460,7 @@
       <c r="H10" s="1">
         <v>2390.5</v>
       </c>
-      <c r="I10" s="8" t="s">
+      <c r="I10" s="9" t="s">
         <v>29</v>
       </c>
       <c r="J10" s="8" t="s">
@@ -1490,7 +1491,7 @@
       <c r="H11" s="1">
         <v>1614.6</v>
       </c>
-      <c r="I11" s="8" t="s">
+      <c r="I11" s="9" t="s">
         <v>38</v>
       </c>
       <c r="J11" s="8" t="s">
@@ -1521,7 +1522,7 @@
       <c r="H12" s="3">
         <v>1841</v>
       </c>
-      <c r="I12" s="8" t="s">
+      <c r="I12" s="9" t="s">
         <v>26</v>
       </c>
       <c r="J12" s="8" t="s">
@@ -1536,7 +1537,7 @@
       <c r="B13" s="17"/>
       <c r="C13" s="7"/>
       <c r="H13" s="6"/>
-      <c r="I13" s="7"/>
+      <c r="I13" s="11"/>
       <c r="J13" s="7"/>
       <c r="K13" s="7"/>
       <c r="L13" s="7"/>
@@ -1570,7 +1571,7 @@
       <c r="H15" s="3">
         <v>2575.8000000000002</v>
       </c>
-      <c r="I15" s="8" t="s">
+      <c r="I15" s="9" t="s">
         <v>20</v>
       </c>
       <c r="J15" s="8" t="s">
@@ -1601,7 +1602,7 @@
       <c r="H16" s="1">
         <v>1828.1</v>
       </c>
-      <c r="I16" s="8" t="s">
+      <c r="I16" s="9" t="s">
         <v>34</v>
       </c>
       <c r="J16" s="8" t="s">
@@ -1632,7 +1633,7 @@
       <c r="H17" s="3">
         <v>2221.6</v>
       </c>
-      <c r="I17" s="8" t="s">
+      <c r="I17" s="9" t="s">
         <v>34</v>
       </c>
       <c r="J17" s="8" t="s">
@@ -1663,7 +1664,7 @@
       <c r="H18" s="3">
         <v>3172</v>
       </c>
-      <c r="I18" s="8" t="s">
+      <c r="I18" s="9" t="s">
         <v>24</v>
       </c>
       <c r="J18" s="8" t="s">
@@ -1694,7 +1695,7 @@
       <c r="H19" s="1">
         <v>1677.4</v>
       </c>
-      <c r="I19" s="8" t="s">
+      <c r="I19" s="9" t="s">
         <v>29</v>
       </c>
       <c r="J19" s="8" t="s">
@@ -1725,7 +1726,7 @@
       <c r="H20" s="1">
         <v>1822.6</v>
       </c>
-      <c r="I20" s="8" t="s">
+      <c r="I20" s="9" t="s">
         <v>38</v>
       </c>
       <c r="J20" s="8" t="s">
@@ -1756,7 +1757,7 @@
       <c r="H21" s="1">
         <v>2583</v>
       </c>
-      <c r="I21" s="8" t="s">
+      <c r="I21" s="9" t="s">
         <v>34</v>
       </c>
       <c r="J21" s="8" t="s">
@@ -1787,7 +1788,7 @@
       <c r="H22" s="1">
         <v>2101.3000000000002</v>
       </c>
-      <c r="I22" s="8" t="s">
+      <c r="I22" s="9" t="s">
         <v>32</v>
       </c>
       <c r="J22" s="8" t="s">
@@ -1818,7 +1819,7 @@
       <c r="H23" s="1">
         <v>1707</v>
       </c>
-      <c r="I23" s="8" t="s">
+      <c r="I23" s="9" t="s">
         <v>29</v>
       </c>
       <c r="J23" s="8" t="s">
@@ -1849,7 +1850,7 @@
       <c r="H24" s="3">
         <v>3016.2</v>
       </c>
-      <c r="I24" s="8" t="s">
+      <c r="I24" s="9" t="s">
         <v>35</v>
       </c>
       <c r="J24" s="8" t="s">
@@ -1864,7 +1865,7 @@
       <c r="B25" s="17"/>
       <c r="C25" s="7"/>
       <c r="H25" s="6"/>
-      <c r="I25" s="7"/>
+      <c r="I25" s="11"/>
       <c r="J25" s="7"/>
       <c r="K25" s="7"/>
       <c r="L25" s="7"/>
@@ -1898,7 +1899,7 @@
       <c r="H27" s="3">
         <v>1138.3</v>
       </c>
-      <c r="I27" s="8" t="s">
+      <c r="I27" s="9" t="s">
         <v>22</v>
       </c>
       <c r="J27" s="8" t="s">
@@ -1929,7 +1930,7 @@
       <c r="H28" s="1">
         <v>1433.5</v>
       </c>
-      <c r="I28" s="8" t="s">
+      <c r="I28" s="9" t="s">
         <v>26</v>
       </c>
       <c r="J28" s="8" t="s">
@@ -1960,7 +1961,7 @@
       <c r="H29" s="1">
         <v>1163</v>
       </c>
-      <c r="I29" s="8" t="s">
+      <c r="I29" s="9" t="s">
         <v>35</v>
       </c>
       <c r="J29" s="8" t="s">
@@ -1991,7 +1992,7 @@
       <c r="H30" s="3">
         <v>1530.1</v>
       </c>
-      <c r="I30" s="8" t="s">
+      <c r="I30" s="9" t="s">
         <v>20</v>
       </c>
       <c r="J30" s="8" t="s">
@@ -2022,7 +2023,7 @@
       <c r="H31" s="1">
         <v>1787.3</v>
       </c>
-      <c r="I31" s="8" t="s">
+      <c r="I31" s="9" t="s">
         <v>38</v>
       </c>
       <c r="J31" s="8" t="s">
@@ -2053,7 +2054,7 @@
       <c r="H32" s="1">
         <v>1593.8</v>
       </c>
-      <c r="I32" s="8" t="s">
+      <c r="I32" s="9" t="s">
         <v>26</v>
       </c>
       <c r="J32" s="8" t="s">
@@ -2084,7 +2085,7 @@
       <c r="H33" s="1">
         <v>1000.8</v>
       </c>
-      <c r="I33" s="8" t="s">
+      <c r="I33" s="9" t="s">
         <v>20</v>
       </c>
       <c r="J33" s="8" t="s">
@@ -2115,7 +2116,7 @@
       <c r="H34" s="1">
         <v>2110.6</v>
       </c>
-      <c r="I34" s="8" t="s">
+      <c r="I34" s="9" t="s">
         <v>31</v>
       </c>
       <c r="J34" s="8" t="s">
@@ -2146,7 +2147,7 @@
       <c r="H35" s="1">
         <v>1210.4000000000001</v>
       </c>
-      <c r="I35" s="8" t="s">
+      <c r="I35" s="9" t="s">
         <v>34</v>
       </c>
       <c r="J35" s="8" t="s">
@@ -2177,7 +2178,7 @@
       <c r="H36" s="1">
         <v>1369.1</v>
       </c>
-      <c r="I36" s="8" t="s">
+      <c r="I36" s="9" t="s">
         <v>34</v>
       </c>
       <c r="J36" s="8" t="s">
@@ -2192,7 +2193,7 @@
       <c r="B37" s="17"/>
       <c r="C37" s="7"/>
       <c r="H37" s="6"/>
-      <c r="I37" s="7"/>
+      <c r="I37" s="11"/>
       <c r="J37" s="7"/>
       <c r="K37" s="7"/>
       <c r="L37" s="7"/>
@@ -2226,7 +2227,7 @@
       <c r="H39" s="3">
         <v>1006.9</v>
       </c>
-      <c r="I39" s="8" t="s">
+      <c r="I39" s="9" t="s">
         <v>31</v>
       </c>
       <c r="J39" s="8" t="s">
@@ -2262,7 +2263,7 @@
       <c r="H40" s="3">
         <v>1829.9</v>
       </c>
-      <c r="I40" s="8" t="s">
+      <c r="I40" s="9" t="s">
         <v>36</v>
       </c>
       <c r="J40" s="8" t="s">
@@ -2298,7 +2299,7 @@
       <c r="H41" s="3">
         <v>2022.3</v>
       </c>
-      <c r="I41" s="8" t="s">
+      <c r="I41" s="9" t="s">
         <v>24</v>
       </c>
       <c r="J41" s="8" t="s">
@@ -2329,7 +2330,7 @@
       <c r="H42" s="1">
         <v>1999.7</v>
       </c>
-      <c r="I42" s="8" t="s">
+      <c r="I42" s="9" t="s">
         <v>44</v>
       </c>
       <c r="J42" s="8" t="s">
@@ -2360,7 +2361,7 @@
       <c r="H43" s="1">
         <v>2606.1999999999998</v>
       </c>
-      <c r="I43" s="8" t="s">
+      <c r="I43" s="9" t="s">
         <v>31</v>
       </c>
       <c r="J43" s="8" t="s">
@@ -2391,7 +2392,7 @@
       <c r="H44" s="1">
         <v>1253.9000000000001</v>
       </c>
-      <c r="I44" s="8" t="s">
+      <c r="I44" s="9" t="s">
         <v>25</v>
       </c>
       <c r="J44" s="8" t="s">
@@ -2422,7 +2423,7 @@
       <c r="H45" s="1">
         <v>1127.5999999999999</v>
       </c>
-      <c r="I45" s="8" t="s">
+      <c r="I45" s="9" t="s">
         <v>23</v>
       </c>
       <c r="J45" s="8" t="s">
@@ -2453,7 +2454,7 @@
       <c r="H46" s="1">
         <v>1371.6</v>
       </c>
-      <c r="I46" s="8" t="s">
+      <c r="I46" s="9" t="s">
         <v>31</v>
       </c>
       <c r="J46" s="8" t="s">
@@ -2484,7 +2485,7 @@
       <c r="H47" s="3">
         <v>1242.3</v>
       </c>
-      <c r="I47" s="8" t="s">
+      <c r="I47" s="9" t="s">
         <v>34</v>
       </c>
       <c r="J47" s="8" t="s">
@@ -2515,7 +2516,7 @@
       <c r="H48" s="1">
         <v>1090</v>
       </c>
-      <c r="I48" s="8" t="s">
+      <c r="I48" s="9" t="s">
         <v>34</v>
       </c>
       <c r="J48" s="8" t="s">
@@ -2530,7 +2531,7 @@
       <c r="B49" s="17"/>
       <c r="C49" s="7"/>
       <c r="H49" s="6"/>
-      <c r="I49" s="7"/>
+      <c r="I49" s="11"/>
       <c r="J49" s="7"/>
       <c r="K49" s="7"/>
       <c r="L49" s="7"/>
@@ -2564,6 +2565,12 @@
       <c r="H51" s="3">
         <v>723.11</v>
       </c>
+      <c r="I51" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="J51" s="8" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="52" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A52" s="13"/>
@@ -2586,6 +2593,12 @@
       <c r="H52" s="3">
         <v>749.09</v>
       </c>
+      <c r="I52" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="J52" s="8" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="53" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A53" s="13"/>
@@ -2608,6 +2621,12 @@
       <c r="H53" s="3">
         <v>567.97</v>
       </c>
+      <c r="I53" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="J53" s="8" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="54" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A54" s="13"/>
@@ -2630,6 +2649,12 @@
       <c r="H54" s="3">
         <v>537.80999999999995</v>
       </c>
+      <c r="I54" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="J54" s="8" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="55" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A55" s="13"/>
@@ -2652,6 +2677,12 @@
       <c r="H55" s="3">
         <v>558.20000000000005</v>
       </c>
+      <c r="I55" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="J55" s="8" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="56" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A56" s="13"/>
@@ -2674,6 +2705,12 @@
       <c r="H56" s="3">
         <v>695.87</v>
       </c>
+      <c r="I56" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="J56" s="8" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="57" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A57" s="13"/>
@@ -2696,6 +2733,12 @@
       <c r="H57" s="3">
         <v>669.49</v>
       </c>
+      <c r="I57" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="J57" s="8" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="58" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A58" s="13"/>
@@ -2718,6 +2761,12 @@
       <c r="H58" s="3">
         <v>673.71</v>
       </c>
+      <c r="I58" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="J58" s="8" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="59" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A59" s="13"/>
@@ -2740,6 +2789,12 @@
       <c r="H59" s="3">
         <v>590.03</v>
       </c>
+      <c r="I59" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="J59" s="8" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="60" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A60" s="13"/>
@@ -2762,13 +2817,19 @@
       <c r="H60" s="3">
         <v>713.26</v>
       </c>
+      <c r="I60" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="J60" s="8" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="61" spans="1:12" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="14"/>
       <c r="B61" s="17"/>
       <c r="C61" s="7"/>
       <c r="H61" s="6"/>
-      <c r="I61" s="7"/>
+      <c r="I61" s="11"/>
       <c r="J61" s="7"/>
       <c r="K61" s="7"/>
       <c r="L61" s="7"/>
@@ -2802,6 +2863,12 @@
       <c r="H63" s="3">
         <v>460.27</v>
       </c>
+      <c r="I63" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="J63" s="8" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="64" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A64" s="13"/>
@@ -2824,6 +2891,12 @@
       <c r="H64" s="3">
         <v>752.32</v>
       </c>
+      <c r="I64" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="J64" s="8" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="65" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A65" s="13"/>
@@ -2846,6 +2919,12 @@
       <c r="H65" s="3">
         <v>471.18</v>
       </c>
+      <c r="I65" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="J65" s="8" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="66" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A66" s="13"/>
@@ -2868,6 +2947,12 @@
       <c r="H66" s="3">
         <v>490.7</v>
       </c>
+      <c r="I66" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="J66" s="8" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="67" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A67" s="13"/>
@@ -2890,6 +2975,12 @@
       <c r="H67" s="3">
         <v>584.77</v>
       </c>
+      <c r="I67" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="J67" s="8" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="68" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A68" s="13"/>
@@ -2912,6 +3003,12 @@
       <c r="H68" s="3">
         <v>726.26</v>
       </c>
+      <c r="I68" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="J68" s="8" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="69" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A69" s="13"/>
@@ -2934,6 +3031,12 @@
       <c r="H69" s="3">
         <v>697.16</v>
       </c>
+      <c r="I69" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="J69" s="8" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="70" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A70" s="13"/>
@@ -2956,6 +3059,12 @@
       <c r="H70" s="3">
         <v>776.41</v>
       </c>
+      <c r="I70" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="J70" s="8" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="71" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A71" s="13"/>
@@ -2978,6 +3087,12 @@
       <c r="H71" s="3">
         <v>700.49</v>
       </c>
+      <c r="I71" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="J71" s="8" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="72" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A72" s="13"/>
@@ -3000,13 +3115,19 @@
       <c r="H72" s="3">
         <v>738.14</v>
       </c>
+      <c r="I72" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="J72" s="8" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="73" spans="1:12" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="14"/>
       <c r="B73" s="17"/>
       <c r="C73" s="7"/>
       <c r="H73" s="6"/>
-      <c r="I73" s="7"/>
+      <c r="I73" s="11"/>
       <c r="J73" s="7"/>
       <c r="K73" s="7"/>
       <c r="L73" s="7"/>
@@ -3061,9 +3182,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE483CC8-AF2C-4D5A-AEE5-EF7DF4EC0883}">
   <dimension ref="A1:L75"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A42" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C72" sqref="C72"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A49" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D63" sqref="D63:K72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4425,7 +4546,7 @@
       <c r="A51" s="13"/>
       <c r="B51" s="16"/>
       <c r="C51" s="4" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D51" s="9">
         <v>1.9315</v>
@@ -4487,7 +4608,7 @@
       <c r="A53" s="13"/>
       <c r="B53" s="16"/>
       <c r="C53" s="9" t="s">
-        <v>36</v>
+        <v>47</v>
       </c>
       <c r="D53" s="9">
         <v>0.98812</v>
@@ -5122,9 +5243,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF6E341A-51E3-4AF7-809B-A8594B1323BC}">
   <dimension ref="A1:L75"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M77" sqref="M77"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A51" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="P59" sqref="P59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6480,42 +6601,312 @@
     <row r="51" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A51" s="13"/>
       <c r="B51" s="16"/>
+      <c r="C51" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="D51" s="4">
+        <v>1.9302999999999999</v>
+      </c>
+      <c r="E51" s="4">
+        <v>413.72</v>
+      </c>
+      <c r="F51" s="4">
+        <v>2.4257999999999998E-2</v>
+      </c>
+      <c r="G51" s="4">
+        <v>4.1744000000000003</v>
+      </c>
+      <c r="H51" s="4">
+        <v>720.53</v>
+      </c>
+      <c r="I51" s="4">
+        <v>3740</v>
+      </c>
+      <c r="J51" s="4">
+        <v>3.2875000000000001</v>
+      </c>
+      <c r="K51" s="4">
+        <v>7.5471000000000004</v>
+      </c>
     </row>
     <row r="52" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A52" s="13"/>
       <c r="B52" s="16"/>
+      <c r="C52" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="D52" s="4">
+        <v>3.7450000000000001</v>
+      </c>
+      <c r="E52" s="4">
+        <v>5.5084999999999997</v>
+      </c>
+      <c r="F52" s="4">
+        <v>10.981999999999999</v>
+      </c>
+      <c r="G52" s="4">
+        <v>3.9323000000000001</v>
+      </c>
+      <c r="H52" s="4">
+        <v>723.41</v>
+      </c>
+      <c r="I52" s="4">
+        <v>9445.2999999999993</v>
+      </c>
+      <c r="J52" s="4">
+        <v>2.7645</v>
+      </c>
+      <c r="K52" s="4">
+        <v>5.3007</v>
+      </c>
     </row>
     <row r="53" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A53" s="13"/>
       <c r="B53" s="16"/>
+      <c r="C53" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="D53" s="4">
+        <v>1.0051000000000001</v>
+      </c>
+      <c r="E53" s="4">
+        <v>41.567999999999998</v>
+      </c>
+      <c r="F53" s="4">
+        <v>0.50309999999999999</v>
+      </c>
+      <c r="G53" s="4">
+        <v>4.4626000000000001</v>
+      </c>
+      <c r="H53" s="4">
+        <v>582.32000000000005</v>
+      </c>
+      <c r="I53" s="4">
+        <v>2413</v>
+      </c>
+      <c r="J53" s="4">
+        <v>3.508</v>
+      </c>
+      <c r="K53" s="4">
+        <v>6.1177999999999999</v>
+      </c>
     </row>
     <row r="54" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A54" s="13"/>
       <c r="B54" s="16"/>
+      <c r="C54" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="D54" s="4">
+        <v>0.34182000000000001</v>
+      </c>
+      <c r="E54" s="4">
+        <v>3.0001000000000002</v>
+      </c>
+      <c r="F54" s="4">
+        <v>2.6158000000000001</v>
+      </c>
+      <c r="G54" s="4">
+        <v>4.5224000000000002</v>
+      </c>
+      <c r="H54" s="4">
+        <v>605.76</v>
+      </c>
+      <c r="I54" s="4">
+        <v>9686.9</v>
+      </c>
+      <c r="J54" s="4">
+        <v>2.8176999999999999</v>
+      </c>
+      <c r="K54" s="4">
+        <v>7.5712000000000002</v>
+      </c>
     </row>
     <row r="55" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A55" s="13"/>
       <c r="B55" s="16"/>
+      <c r="C55" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="D55" s="4">
+        <v>0.74811000000000005</v>
+      </c>
+      <c r="E55" s="4">
+        <v>4.8129999999999997</v>
+      </c>
+      <c r="F55" s="4">
+        <v>1.5203</v>
+      </c>
+      <c r="G55" s="4">
+        <v>4.5427</v>
+      </c>
+      <c r="H55" s="4">
+        <v>578.84</v>
+      </c>
+      <c r="I55" s="4">
+        <v>5902.3</v>
+      </c>
+      <c r="J55" s="4">
+        <v>3.0358000000000001</v>
+      </c>
+      <c r="K55" s="4">
+        <v>7.2228000000000003</v>
+      </c>
     </row>
     <row r="56" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A56" s="13"/>
       <c r="B56" s="16"/>
+      <c r="C56" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="D56" s="4">
+        <v>2.2985000000000002</v>
+      </c>
+      <c r="E56" s="4">
+        <v>17.765000000000001</v>
+      </c>
+      <c r="F56" s="4">
+        <v>0.53407000000000004</v>
+      </c>
+      <c r="G56" s="4">
+        <v>4.1894999999999998</v>
+      </c>
+      <c r="H56" s="4">
+        <v>695.87</v>
+      </c>
+      <c r="I56" s="4">
+        <v>4582.3999999999996</v>
+      </c>
+      <c r="J56" s="4">
+        <v>3.1497999999999999</v>
+      </c>
+      <c r="K56" s="4">
+        <v>6.8537999999999997</v>
+      </c>
     </row>
     <row r="57" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A57" s="13"/>
       <c r="B57" s="16"/>
+      <c r="C57" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="D57" s="4">
+        <v>1.7064999999999999</v>
+      </c>
+      <c r="E57" s="4">
+        <v>2.9634999999999998</v>
+      </c>
+      <c r="F57" s="4">
+        <v>8.5671999999999997</v>
+      </c>
+      <c r="G57" s="4">
+        <v>4.2396000000000003</v>
+      </c>
+      <c r="H57" s="4">
+        <v>648.58000000000004</v>
+      </c>
+      <c r="I57" s="4">
+        <v>9968.2000000000007</v>
+      </c>
+      <c r="J57" s="4">
+        <v>2.8411</v>
+      </c>
+      <c r="K57" s="4">
+        <v>9.9029000000000007</v>
+      </c>
     </row>
     <row r="58" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A58" s="13"/>
       <c r="B58" s="16"/>
+      <c r="C58" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="D58" s="4">
+        <v>1.2569999999999999</v>
+      </c>
+      <c r="E58" s="4">
+        <v>4.6817000000000002</v>
+      </c>
+      <c r="F58" s="4">
+        <v>6.5932000000000004</v>
+      </c>
+      <c r="G58" s="4">
+        <v>4.2586000000000004</v>
+      </c>
+      <c r="H58" s="4">
+        <v>671.09</v>
+      </c>
+      <c r="I58" s="4">
+        <v>9375.2000000000007</v>
+      </c>
+      <c r="J58" s="4">
+        <v>2.7982999999999998</v>
+      </c>
+      <c r="K58" s="4">
+        <v>6.5297000000000001</v>
+      </c>
     </row>
     <row r="59" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A59" s="13"/>
       <c r="B59" s="16"/>
+      <c r="C59" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="D59" s="4">
+        <v>0.54088000000000003</v>
+      </c>
+      <c r="E59" s="4">
+        <v>3.4417</v>
+      </c>
+      <c r="F59" s="4">
+        <v>3.8666</v>
+      </c>
+      <c r="G59" s="4">
+        <v>4.4062000000000001</v>
+      </c>
+      <c r="H59" s="4">
+        <v>640.30999999999995</v>
+      </c>
+      <c r="I59" s="4">
+        <v>9914.9</v>
+      </c>
+      <c r="J59" s="4">
+        <v>2.8043999999999998</v>
+      </c>
+      <c r="K59" s="4">
+        <v>7.6501999999999999</v>
+      </c>
     </row>
     <row r="60" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A60" s="13"/>
       <c r="B60" s="16"/>
+      <c r="C60" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="D60" s="4">
+        <v>2.9771999999999998</v>
+      </c>
+      <c r="E60" s="4">
+        <v>13.58</v>
+      </c>
+      <c r="F60" s="4">
+        <v>2.2099000000000002</v>
+      </c>
+      <c r="G60" s="4">
+        <v>4.0601000000000003</v>
+      </c>
+      <c r="H60" s="4">
+        <v>697.13</v>
+      </c>
+      <c r="I60" s="4">
+        <v>2654.7</v>
+      </c>
+      <c r="J60" s="4">
+        <v>3.4464999999999999</v>
+      </c>
+      <c r="K60" s="4">
+        <v>5.4966999999999997</v>
+      </c>
     </row>
     <row r="61" spans="1:12" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="14"/>
@@ -6534,42 +6925,312 @@
     <row r="63" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A63" s="13"/>
       <c r="B63" s="16"/>
+      <c r="C63" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="D63" s="4">
+        <v>4.6173000000000004E-3</v>
+      </c>
+      <c r="E63" s="4">
+        <v>6.8475999999999999</v>
+      </c>
+      <c r="F63" s="4">
+        <v>2.2387000000000001</v>
+      </c>
+      <c r="G63" s="4">
+        <v>4.8326000000000002</v>
+      </c>
+      <c r="H63" s="4">
+        <v>460.38</v>
+      </c>
+      <c r="I63" s="4">
+        <v>2357.9</v>
+      </c>
+      <c r="J63" s="4">
+        <v>3.5989</v>
+      </c>
+      <c r="K63" s="4">
+        <v>6.8921999999999999</v>
+      </c>
     </row>
     <row r="64" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A64" s="13"/>
       <c r="B64" s="16"/>
+      <c r="C64" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="D64" s="4">
+        <v>3.1901000000000002</v>
+      </c>
+      <c r="E64" s="4">
+        <v>126.5</v>
+      </c>
+      <c r="F64" s="4">
+        <v>0.16925000000000001</v>
+      </c>
+      <c r="G64" s="4">
+        <v>3.8923999999999999</v>
+      </c>
+      <c r="H64" s="4">
+        <v>802.2</v>
+      </c>
+      <c r="I64" s="4">
+        <v>2253.9</v>
+      </c>
+      <c r="J64" s="4">
+        <v>3.6876000000000002</v>
+      </c>
+      <c r="K64" s="4">
+        <v>11.145</v>
+      </c>
     </row>
     <row r="65" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A65" s="13"/>
       <c r="B65" s="16"/>
+      <c r="C65" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="D65" s="4">
+        <v>0.31556000000000001</v>
+      </c>
+      <c r="E65" s="4">
+        <v>4.9177</v>
+      </c>
+      <c r="F65" s="4">
+        <v>4.2816000000000001</v>
+      </c>
+      <c r="G65" s="4">
+        <v>4.8133999999999997</v>
+      </c>
+      <c r="H65" s="4">
+        <v>468.63</v>
+      </c>
+      <c r="I65" s="4">
+        <v>3308.8</v>
+      </c>
+      <c r="J65" s="4">
+        <v>3.3386999999999998</v>
+      </c>
+      <c r="K65" s="4">
+        <v>5.7804000000000002</v>
+      </c>
     </row>
     <row r="66" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A66" s="13"/>
       <c r="B66" s="16"/>
+      <c r="C66" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="D66" s="4">
+        <v>0.26189000000000001</v>
+      </c>
+      <c r="E66" s="4">
+        <v>37.661999999999999</v>
+      </c>
+      <c r="F66" s="4">
+        <v>0.20133999999999999</v>
+      </c>
+      <c r="G66" s="4">
+        <v>4.8079000000000001</v>
+      </c>
+      <c r="H66" s="4">
+        <v>478.84</v>
+      </c>
+      <c r="I66" s="4">
+        <v>2939.9</v>
+      </c>
+      <c r="J66" s="4">
+        <v>3.4262000000000001</v>
+      </c>
+      <c r="K66" s="4">
+        <v>5.9608999999999996</v>
+      </c>
     </row>
     <row r="67" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A67" s="13"/>
       <c r="B67" s="16"/>
+      <c r="C67" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="D67" s="4">
+        <v>1.5331999999999999</v>
+      </c>
+      <c r="E67" s="4">
+        <v>6.9652000000000003</v>
+      </c>
+      <c r="F67" s="4">
+        <v>4.9490999999999996</v>
+      </c>
+      <c r="G67" s="4">
+        <v>4.3071999999999999</v>
+      </c>
+      <c r="H67" s="4">
+        <v>551.01</v>
+      </c>
+      <c r="I67" s="4">
+        <v>1467.1</v>
+      </c>
+      <c r="J67" s="4">
+        <v>4.0639000000000003</v>
+      </c>
+      <c r="K67" s="4">
+        <v>13.561</v>
+      </c>
     </row>
     <row r="68" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A68" s="13"/>
       <c r="B68" s="16"/>
+      <c r="C68" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="D68" s="4">
+        <v>0.18711</v>
+      </c>
+      <c r="E68" s="4">
+        <v>42.057000000000002</v>
+      </c>
+      <c r="F68" s="4">
+        <v>1.22</v>
+      </c>
+      <c r="G68" s="4">
+        <v>3.9495</v>
+      </c>
+      <c r="H68" s="4">
+        <v>803.58</v>
+      </c>
+      <c r="I68" s="4">
+        <v>1759.6</v>
+      </c>
+      <c r="J68" s="4">
+        <v>3.8088000000000002</v>
+      </c>
+      <c r="K68" s="4">
+        <v>6.9718</v>
+      </c>
     </row>
     <row r="69" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A69" s="13"/>
       <c r="B69" s="16"/>
+      <c r="C69" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="D69" s="4">
+        <v>3.4416000000000002</v>
+      </c>
+      <c r="E69" s="4">
+        <v>6.2590000000000003</v>
+      </c>
+      <c r="F69" s="4">
+        <v>1.3140000000000001</v>
+      </c>
+      <c r="G69" s="4">
+        <v>4.0781999999999998</v>
+      </c>
+      <c r="H69" s="4">
+        <v>707.11</v>
+      </c>
+      <c r="I69" s="4">
+        <v>4504.6000000000004</v>
+      </c>
+      <c r="J69" s="4">
+        <v>3.2162000000000002</v>
+      </c>
+      <c r="K69" s="4">
+        <v>8.2904</v>
+      </c>
     </row>
     <row r="70" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A70" s="13"/>
       <c r="B70" s="16"/>
+      <c r="C70" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="D70" s="4">
+        <v>4.5324999999999998</v>
+      </c>
+      <c r="E70" s="4">
+        <v>14.166</v>
+      </c>
+      <c r="F70" s="4">
+        <v>2.2204999999999999</v>
+      </c>
+      <c r="G70" s="4">
+        <v>3.8813</v>
+      </c>
+      <c r="H70" s="4">
+        <v>731.02</v>
+      </c>
+      <c r="I70" s="4">
+        <v>2379.1</v>
+      </c>
+      <c r="J70" s="4">
+        <v>3.5503999999999998</v>
+      </c>
+      <c r="K70" s="4">
+        <v>6.0315000000000003</v>
+      </c>
     </row>
     <row r="71" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A71" s="13"/>
       <c r="B71" s="16"/>
+      <c r="C71" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="D71" s="4">
+        <v>3.3203</v>
+      </c>
+      <c r="E71" s="4">
+        <v>95.748000000000005</v>
+      </c>
+      <c r="F71" s="4">
+        <v>0.45551999999999998</v>
+      </c>
+      <c r="G71" s="4">
+        <v>4.0633999999999997</v>
+      </c>
+      <c r="H71" s="4">
+        <v>574.87</v>
+      </c>
+      <c r="I71" s="4">
+        <v>1034.8</v>
+      </c>
+      <c r="J71" s="4">
+        <v>4.2290999999999999</v>
+      </c>
+      <c r="K71" s="4">
+        <v>6.0321999999999996</v>
+      </c>
     </row>
     <row r="72" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A72" s="13"/>
       <c r="B72" s="16"/>
+      <c r="C72" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="D72" s="4">
+        <v>4.0854999999999997</v>
+      </c>
+      <c r="E72" s="4">
+        <v>246.68</v>
+      </c>
+      <c r="F72" s="4">
+        <v>8.4526000000000004E-2</v>
+      </c>
+      <c r="G72" s="4">
+        <v>3.9321000000000002</v>
+      </c>
+      <c r="H72" s="4">
+        <v>776.2</v>
+      </c>
+      <c r="I72" s="4">
+        <v>2681.7</v>
+      </c>
+      <c r="J72" s="4">
+        <v>3.4426000000000001</v>
+      </c>
+      <c r="K72" s="4">
+        <v>5.5305</v>
+      </c>
     </row>
     <row r="73" spans="1:12" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="14"/>
@@ -6593,7 +7254,7 @@
       </c>
       <c r="G75" s="4">
         <f t="shared" si="0"/>
-        <v>4.7670000000000003</v>
+        <v>4.8326000000000002</v>
       </c>
       <c r="H75" s="4">
         <f t="shared" si="0"/>
@@ -6601,7 +7262,7 @@
       </c>
       <c r="I75" s="4">
         <f t="shared" si="0"/>
-        <v>4972.3999999999996</v>
+        <v>9968.2000000000007</v>
       </c>
       <c r="J75" s="4">
         <f t="shared" si="0"/>
@@ -6637,7 +7298,7 @@
   <dimension ref="A1:O73"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A31" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C44" sqref="C44"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Added exponential tail for EVP-WD
</commit_message>
<xml_diff>
--- a/scripts/__other__/__sem__.xlsx
+++ b/scripts/__other__/__sem__.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Janzen\Desktop\code\moga_neml\scripts\__other__\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C7FE0E5-13DA-4EB3-88E7-48F53D0EE399}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6F6846D-F035-4EB7-9CC5-4AA38CC10090}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="evp" sheetId="13" r:id="rId1"/>
@@ -3159,18 +3159,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A38:A49"/>
+    <mergeCell ref="B38:B49"/>
+    <mergeCell ref="A50:A61"/>
+    <mergeCell ref="B50:B61"/>
+    <mergeCell ref="A62:A73"/>
+    <mergeCell ref="B62:B73"/>
     <mergeCell ref="A2:A13"/>
     <mergeCell ref="B2:B13"/>
     <mergeCell ref="A14:A25"/>
     <mergeCell ref="B14:B25"/>
     <mergeCell ref="A26:A37"/>
     <mergeCell ref="B26:B37"/>
-    <mergeCell ref="A38:A49"/>
-    <mergeCell ref="B38:B49"/>
-    <mergeCell ref="A50:A61"/>
-    <mergeCell ref="B50:B61"/>
-    <mergeCell ref="A62:A73"/>
-    <mergeCell ref="B62:B73"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5221,6 +5221,2060 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A38:A49"/>
+    <mergeCell ref="B38:B49"/>
+    <mergeCell ref="A50:A61"/>
+    <mergeCell ref="B50:B61"/>
+    <mergeCell ref="A62:A73"/>
+    <mergeCell ref="B62:B73"/>
+    <mergeCell ref="A2:A13"/>
+    <mergeCell ref="B2:B13"/>
+    <mergeCell ref="A14:A25"/>
+    <mergeCell ref="B14:B25"/>
+    <mergeCell ref="A26:A37"/>
+    <mergeCell ref="B26:B37"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF6E341A-51E3-4AF7-809B-A8594B1323BC}">
+  <dimension ref="A1:L75"/>
+  <sheetViews>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A51" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="P59" sqref="P59"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="4"/>
+    <col min="2" max="2" width="9.140625" style="3"/>
+    <col min="3" max="3" width="15.7109375" style="8" customWidth="1"/>
+    <col min="4" max="11" width="9.140625" style="4"/>
+    <col min="12" max="12" width="9.140625" style="9"/>
+    <col min="13" max="16384" width="9.140625" style="4"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="11"/>
+    </row>
+    <row r="2" spans="1:12" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="12">
+        <v>800</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" s="13"/>
+      <c r="B3" s="16"/>
+      <c r="C3" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" s="4">
+        <v>16.994</v>
+      </c>
+      <c r="E3" s="4">
+        <v>187.83</v>
+      </c>
+      <c r="F3" s="4">
+        <v>0.26103999999999999</v>
+      </c>
+      <c r="G3" s="4">
+        <v>4.5019999999999998</v>
+      </c>
+      <c r="H3" s="4">
+        <v>1784.8</v>
+      </c>
+      <c r="I3" s="2">
+        <v>3263.5</v>
+      </c>
+      <c r="J3" s="2">
+        <v>4.9230999999999998</v>
+      </c>
+      <c r="K3" s="2">
+        <v>13.172000000000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" s="13"/>
+      <c r="B4" s="16"/>
+      <c r="C4" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D4" s="4">
+        <v>22.454000000000001</v>
+      </c>
+      <c r="E4" s="4">
+        <v>66.77</v>
+      </c>
+      <c r="F4" s="4">
+        <v>0.92681000000000002</v>
+      </c>
+      <c r="G4" s="4">
+        <v>4.4191000000000003</v>
+      </c>
+      <c r="H4" s="4">
+        <v>1610.1</v>
+      </c>
+      <c r="I4" s="2">
+        <v>2142</v>
+      </c>
+      <c r="J4" s="2">
+        <v>5.4843999999999999</v>
+      </c>
+      <c r="K4" s="2">
+        <v>11.449</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" s="13"/>
+      <c r="B5" s="16"/>
+      <c r="C5" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" s="4">
+        <v>9.1647999999999996</v>
+      </c>
+      <c r="E5" s="4">
+        <v>36.326000000000001</v>
+      </c>
+      <c r="F5" s="4">
+        <v>12.337</v>
+      </c>
+      <c r="G5" s="4">
+        <v>4.2247000000000003</v>
+      </c>
+      <c r="H5" s="4">
+        <v>1776.1</v>
+      </c>
+      <c r="I5" s="2">
+        <v>2731</v>
+      </c>
+      <c r="J5" s="2">
+        <v>5.0411000000000001</v>
+      </c>
+      <c r="K5" s="2">
+        <v>8.3102999999999998</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" s="13"/>
+      <c r="B6" s="16"/>
+      <c r="C6" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" s="4">
+        <v>5.8951000000000002</v>
+      </c>
+      <c r="E6" s="4">
+        <v>36.906999999999996</v>
+      </c>
+      <c r="F6" s="4">
+        <v>5.3551000000000002</v>
+      </c>
+      <c r="G6" s="4">
+        <v>4.7310999999999996</v>
+      </c>
+      <c r="H6" s="4">
+        <v>1557.8</v>
+      </c>
+      <c r="I6" s="2">
+        <v>2224.1</v>
+      </c>
+      <c r="J6" s="2">
+        <v>5.2808999999999999</v>
+      </c>
+      <c r="K6" s="2">
+        <v>6.5113000000000003</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" s="13"/>
+      <c r="B7" s="16"/>
+      <c r="C7" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D7" s="4">
+        <v>4.1860999999999997</v>
+      </c>
+      <c r="E7" s="4">
+        <v>84.548000000000002</v>
+      </c>
+      <c r="F7" s="4">
+        <v>2.1124999999999998</v>
+      </c>
+      <c r="G7" s="4">
+        <v>4.7670000000000003</v>
+      </c>
+      <c r="H7" s="4">
+        <v>1574.1</v>
+      </c>
+      <c r="I7" s="4">
+        <v>2883.2</v>
+      </c>
+      <c r="J7" s="4">
+        <v>4.8395000000000001</v>
+      </c>
+      <c r="K7" s="4">
+        <v>4.5430999999999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" s="13"/>
+      <c r="B8" s="16"/>
+      <c r="C8" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" s="2">
+        <v>27.867999999999999</v>
+      </c>
+      <c r="E8" s="2">
+        <v>89.338999999999999</v>
+      </c>
+      <c r="F8" s="2">
+        <v>0.59711999999999998</v>
+      </c>
+      <c r="G8" s="2">
+        <v>4.1981999999999999</v>
+      </c>
+      <c r="H8" s="2">
+        <v>1818</v>
+      </c>
+      <c r="I8" s="2">
+        <v>2645.2</v>
+      </c>
+      <c r="J8" s="2">
+        <v>5.1192000000000002</v>
+      </c>
+      <c r="K8" s="2">
+        <v>10.125</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" s="13"/>
+      <c r="B9" s="16"/>
+      <c r="C9" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="D9" s="2">
+        <v>28.599</v>
+      </c>
+      <c r="E9" s="2">
+        <v>78.057000000000002</v>
+      </c>
+      <c r="F9" s="2">
+        <v>0.84292</v>
+      </c>
+      <c r="G9" s="2">
+        <v>3.8371</v>
+      </c>
+      <c r="H9" s="2">
+        <v>2441.5</v>
+      </c>
+      <c r="I9" s="2">
+        <v>2969.6</v>
+      </c>
+      <c r="J9" s="2">
+        <v>4.9976000000000003</v>
+      </c>
+      <c r="K9" s="2">
+        <v>10.641999999999999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" s="13"/>
+      <c r="B10" s="16"/>
+      <c r="C10" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="D10" s="2">
+        <v>29.978999999999999</v>
+      </c>
+      <c r="E10" s="2">
+        <v>119.58</v>
+      </c>
+      <c r="F10" s="2">
+        <v>0.55200000000000005</v>
+      </c>
+      <c r="G10" s="2">
+        <v>3.8504999999999998</v>
+      </c>
+      <c r="H10" s="2">
+        <v>2314.4</v>
+      </c>
+      <c r="I10" s="2">
+        <v>2808.8</v>
+      </c>
+      <c r="J10" s="2">
+        <v>5.0354000000000001</v>
+      </c>
+      <c r="K10" s="2">
+        <v>9.5434999999999999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" s="13"/>
+      <c r="B11" s="16"/>
+      <c r="C11" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="D11" s="4">
+        <v>19.125</v>
+      </c>
+      <c r="E11" s="4">
+        <v>43.640999999999998</v>
+      </c>
+      <c r="F11" s="4">
+        <v>5.6147999999999998</v>
+      </c>
+      <c r="G11" s="4">
+        <v>4.1688000000000001</v>
+      </c>
+      <c r="H11" s="4">
+        <v>1616</v>
+      </c>
+      <c r="I11" s="4">
+        <v>1876.8</v>
+      </c>
+      <c r="J11" s="4">
+        <v>5.5594000000000001</v>
+      </c>
+      <c r="K11" s="4">
+        <v>6.8653000000000004</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" s="13"/>
+      <c r="B12" s="16"/>
+      <c r="C12" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D12" s="4">
+        <v>22.012</v>
+      </c>
+      <c r="E12" s="4">
+        <v>38.872999999999998</v>
+      </c>
+      <c r="F12" s="4">
+        <v>2.2033</v>
+      </c>
+      <c r="G12" s="4">
+        <v>4.2450000000000001</v>
+      </c>
+      <c r="H12" s="4">
+        <v>1841.2</v>
+      </c>
+      <c r="I12" s="2">
+        <v>2377</v>
+      </c>
+      <c r="J12" s="2">
+        <v>5.2897999999999996</v>
+      </c>
+      <c r="K12" s="2">
+        <v>9.7712000000000003</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="14"/>
+      <c r="B13" s="17"/>
+      <c r="C13" s="7"/>
+      <c r="L13" s="11"/>
+    </row>
+    <row r="14" spans="1:12" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="12">
+        <v>800</v>
+      </c>
+      <c r="B14" s="15" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15" s="13"/>
+      <c r="B15" s="16"/>
+      <c r="C15" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D15" s="4">
+        <v>31.646999999999998</v>
+      </c>
+      <c r="E15" s="4">
+        <v>120.62</v>
+      </c>
+      <c r="F15" s="4">
+        <v>0.85485</v>
+      </c>
+      <c r="G15" s="4">
+        <v>3.7265999999999999</v>
+      </c>
+      <c r="H15" s="4">
+        <v>2297.8000000000002</v>
+      </c>
+      <c r="I15" s="4">
+        <v>2165.6999999999998</v>
+      </c>
+      <c r="J15" s="4">
+        <v>5.3247</v>
+      </c>
+      <c r="K15" s="4">
+        <v>7.7724000000000002</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A16" s="13"/>
+      <c r="B16" s="16"/>
+      <c r="C16" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D16" s="2">
+        <v>33.296999999999997</v>
+      </c>
+      <c r="E16" s="2">
+        <v>522.85</v>
+      </c>
+      <c r="F16" s="2">
+        <v>0.11871</v>
+      </c>
+      <c r="G16" s="2">
+        <v>3.9767000000000001</v>
+      </c>
+      <c r="H16" s="2">
+        <v>1762.4</v>
+      </c>
+      <c r="I16" s="2">
+        <v>1913.8</v>
+      </c>
+      <c r="J16" s="2">
+        <v>5.6638000000000002</v>
+      </c>
+      <c r="K16" s="2">
+        <v>11.287000000000001</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A17" s="13"/>
+      <c r="B17" s="16"/>
+      <c r="C17" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="D17" s="2">
+        <v>15.042</v>
+      </c>
+      <c r="E17" s="2">
+        <v>35.436999999999998</v>
+      </c>
+      <c r="F17" s="2">
+        <v>8.4</v>
+      </c>
+      <c r="G17" s="2">
+        <v>3.9586000000000001</v>
+      </c>
+      <c r="H17" s="2">
+        <v>2283.5</v>
+      </c>
+      <c r="I17" s="2">
+        <v>4184.6000000000004</v>
+      </c>
+      <c r="J17" s="2">
+        <v>4.4257</v>
+      </c>
+      <c r="K17" s="2">
+        <v>6.6603000000000003</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A18" s="13"/>
+      <c r="B18" s="16"/>
+      <c r="C18" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D18" s="2">
+        <v>38.180999999999997</v>
+      </c>
+      <c r="E18" s="2">
+        <v>51.055</v>
+      </c>
+      <c r="F18" s="2">
+        <v>2.4819</v>
+      </c>
+      <c r="G18" s="2">
+        <v>3.2572000000000001</v>
+      </c>
+      <c r="H18" s="2">
+        <v>3154.4</v>
+      </c>
+      <c r="I18" s="2">
+        <v>2725.2</v>
+      </c>
+      <c r="J18" s="2">
+        <v>5.0167000000000002</v>
+      </c>
+      <c r="K18" s="2">
+        <v>8.33</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A19" s="13"/>
+      <c r="B19" s="16"/>
+      <c r="C19" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="D19" s="4">
+        <v>24.888999999999999</v>
+      </c>
+      <c r="E19" s="4">
+        <v>44.932000000000002</v>
+      </c>
+      <c r="F19" s="4">
+        <v>1.2076</v>
+      </c>
+      <c r="G19" s="4">
+        <v>4.5054999999999996</v>
+      </c>
+      <c r="H19" s="4">
+        <v>1527.9</v>
+      </c>
+      <c r="I19" s="4">
+        <v>2589.6999999999998</v>
+      </c>
+      <c r="J19" s="4">
+        <v>5.1066000000000003</v>
+      </c>
+      <c r="K19" s="4">
+        <v>8.6950000000000003</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A20" s="13"/>
+      <c r="B20" s="16"/>
+      <c r="C20" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D20" s="2">
+        <v>23.303999999999998</v>
+      </c>
+      <c r="E20" s="2">
+        <v>276.66000000000003</v>
+      </c>
+      <c r="F20" s="2">
+        <v>0.32123000000000002</v>
+      </c>
+      <c r="G20" s="2">
+        <v>4.2591999999999999</v>
+      </c>
+      <c r="H20" s="2">
+        <v>1767.2</v>
+      </c>
+      <c r="I20" s="2">
+        <v>2168.5</v>
+      </c>
+      <c r="J20" s="2">
+        <v>5.3181000000000003</v>
+      </c>
+      <c r="K20" s="2">
+        <v>6.7618999999999998</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A21" s="13"/>
+      <c r="B21" s="16"/>
+      <c r="C21" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D21" s="2">
+        <v>30.401</v>
+      </c>
+      <c r="E21" s="2">
+        <v>34.817</v>
+      </c>
+      <c r="F21" s="2">
+        <v>4.5983000000000001</v>
+      </c>
+      <c r="G21" s="2">
+        <v>3.5323000000000002</v>
+      </c>
+      <c r="H21" s="2">
+        <v>2583</v>
+      </c>
+      <c r="I21" s="2">
+        <v>2520.9</v>
+      </c>
+      <c r="J21" s="2">
+        <v>5.1558999999999999</v>
+      </c>
+      <c r="K21" s="2">
+        <v>8.5891000000000002</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A22" s="13"/>
+      <c r="B22" s="16"/>
+      <c r="C22" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="D22" s="4">
+        <v>5.0568999999999997</v>
+      </c>
+      <c r="E22" s="4">
+        <v>40.475999999999999</v>
+      </c>
+      <c r="F22" s="4">
+        <v>10.016999999999999</v>
+      </c>
+      <c r="G22" s="4">
+        <v>4.1585000000000001</v>
+      </c>
+      <c r="H22" s="4">
+        <v>1730.1</v>
+      </c>
+      <c r="I22" s="4">
+        <v>1998.1</v>
+      </c>
+      <c r="J22" s="4">
+        <v>5.5564</v>
+      </c>
+      <c r="K22" s="4">
+        <v>10.337</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A23" s="13"/>
+      <c r="B23" s="16"/>
+      <c r="C23" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D23" s="2">
+        <v>31.809000000000001</v>
+      </c>
+      <c r="E23" s="2">
+        <v>43.194000000000003</v>
+      </c>
+      <c r="F23" s="2">
+        <v>2.2399</v>
+      </c>
+      <c r="G23" s="2">
+        <v>3.9613</v>
+      </c>
+      <c r="H23" s="2">
+        <v>1820.1</v>
+      </c>
+      <c r="I23" s="2">
+        <v>2245.4</v>
+      </c>
+      <c r="J23" s="2">
+        <v>5.3178999999999998</v>
+      </c>
+      <c r="K23" s="2">
+        <v>8.5096000000000007</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A24" s="13"/>
+      <c r="B24" s="16"/>
+      <c r="C24" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="D24" s="4">
+        <v>0.36498999999999998</v>
+      </c>
+      <c r="E24" s="4">
+        <v>45.374000000000002</v>
+      </c>
+      <c r="F24" s="4">
+        <v>15.686999999999999</v>
+      </c>
+      <c r="G24" s="4">
+        <v>3.6105</v>
+      </c>
+      <c r="H24" s="4">
+        <v>2878.3</v>
+      </c>
+      <c r="I24" s="2">
+        <v>3325.8</v>
+      </c>
+      <c r="J24" s="2">
+        <v>4.8470000000000004</v>
+      </c>
+      <c r="K24" s="2">
+        <v>12.327999999999999</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="14"/>
+      <c r="B25" s="17"/>
+      <c r="C25" s="7"/>
+      <c r="L25" s="11"/>
+    </row>
+    <row r="26" spans="1:12" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="12">
+        <v>900</v>
+      </c>
+      <c r="B26" s="15" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A27" s="13"/>
+      <c r="B27" s="16"/>
+      <c r="C27" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D27" s="2">
+        <v>3.6261999999999999</v>
+      </c>
+      <c r="E27" s="2">
+        <v>13.804</v>
+      </c>
+      <c r="F27" s="2">
+        <v>6.9824999999999999</v>
+      </c>
+      <c r="G27" s="2">
+        <v>4.2416</v>
+      </c>
+      <c r="H27" s="2">
+        <v>1138.2</v>
+      </c>
+      <c r="I27" s="2">
+        <v>1986</v>
+      </c>
+      <c r="J27" s="2">
+        <v>4.4408000000000003</v>
+      </c>
+      <c r="K27" s="2">
+        <v>9.1929999999999996</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A28" s="13"/>
+      <c r="B28" s="16"/>
+      <c r="C28" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="D28" s="2">
+        <v>10.683</v>
+      </c>
+      <c r="E28" s="2">
+        <v>31.381</v>
+      </c>
+      <c r="F28" s="2">
+        <v>2.9727000000000001</v>
+      </c>
+      <c r="G28" s="2">
+        <v>3.7155</v>
+      </c>
+      <c r="H28" s="2">
+        <v>1422</v>
+      </c>
+      <c r="I28" s="2">
+        <v>1626.7</v>
+      </c>
+      <c r="J28" s="2">
+        <v>4.5519999999999996</v>
+      </c>
+      <c r="K28" s="2">
+        <v>6.2319000000000004</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A29" s="13"/>
+      <c r="B29" s="16"/>
+      <c r="C29" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="D29" s="2">
+        <v>10.340999999999999</v>
+      </c>
+      <c r="E29" s="2">
+        <v>24.475999999999999</v>
+      </c>
+      <c r="F29" s="2">
+        <v>2.3226</v>
+      </c>
+      <c r="G29" s="2">
+        <v>3.9651000000000001</v>
+      </c>
+      <c r="H29" s="2">
+        <v>1176.4000000000001</v>
+      </c>
+      <c r="I29" s="2">
+        <v>1743</v>
+      </c>
+      <c r="J29" s="2">
+        <v>4.5865</v>
+      </c>
+      <c r="K29" s="2">
+        <v>9.1586999999999996</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A30" s="13"/>
+      <c r="B30" s="16"/>
+      <c r="C30" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D30" s="2">
+        <v>11.112</v>
+      </c>
+      <c r="E30" s="2">
+        <v>18.959</v>
+      </c>
+      <c r="F30" s="2">
+        <v>5.9504999999999999</v>
+      </c>
+      <c r="G30" s="2">
+        <v>3.6368</v>
+      </c>
+      <c r="H30" s="2">
+        <v>1471.6</v>
+      </c>
+      <c r="I30" s="2">
+        <v>2064.3000000000002</v>
+      </c>
+      <c r="J30" s="2">
+        <v>4.3163999999999998</v>
+      </c>
+      <c r="K30" s="2">
+        <v>7.2249999999999996</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A31" s="13"/>
+      <c r="B31" s="16"/>
+      <c r="C31" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D31" s="2">
+        <v>8.0817999999999994</v>
+      </c>
+      <c r="E31" s="2">
+        <v>9.2744</v>
+      </c>
+      <c r="F31" s="2">
+        <v>7.9561999999999999</v>
+      </c>
+      <c r="G31" s="2">
+        <v>3.9839000000000002</v>
+      </c>
+      <c r="H31" s="2">
+        <v>1310.7</v>
+      </c>
+      <c r="I31" s="2">
+        <v>4972.3999999999996</v>
+      </c>
+      <c r="J31" s="2">
+        <v>3.6442999999999999</v>
+      </c>
+      <c r="K31" s="2">
+        <v>9.6707000000000001</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A32" s="13"/>
+      <c r="B32" s="16"/>
+      <c r="C32" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D32" s="2">
+        <v>11.394</v>
+      </c>
+      <c r="E32" s="2">
+        <v>13.887</v>
+      </c>
+      <c r="F32" s="2">
+        <v>7.532</v>
+      </c>
+      <c r="G32" s="2">
+        <v>3.5691000000000002</v>
+      </c>
+      <c r="H32" s="2">
+        <v>1581.2</v>
+      </c>
+      <c r="I32" s="2">
+        <v>1959.8</v>
+      </c>
+      <c r="J32" s="2">
+        <v>4.4120999999999997</v>
+      </c>
+      <c r="K32" s="2">
+        <v>8.5846999999999998</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A33" s="13"/>
+      <c r="B33" s="16"/>
+      <c r="C33" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D33" s="4">
+        <v>5.6656000000000004</v>
+      </c>
+      <c r="E33" s="4">
+        <v>7.6356999999999999</v>
+      </c>
+      <c r="F33" s="4">
+        <v>9.1336999999999993</v>
+      </c>
+      <c r="G33" s="4">
+        <v>4.3000999999999996</v>
+      </c>
+      <c r="H33" s="4">
+        <v>1055.4000000000001</v>
+      </c>
+      <c r="I33" s="4">
+        <v>3494.5</v>
+      </c>
+      <c r="J33" s="4">
+        <v>3.9628999999999999</v>
+      </c>
+      <c r="K33" s="4">
+        <v>11.622999999999999</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A34" s="13"/>
+      <c r="B34" s="16"/>
+      <c r="C34" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D34" s="2">
+        <v>15.177</v>
+      </c>
+      <c r="E34" s="2">
+        <v>64.875</v>
+      </c>
+      <c r="F34" s="2">
+        <v>1.1737</v>
+      </c>
+      <c r="G34" s="2">
+        <v>3.2002999999999999</v>
+      </c>
+      <c r="H34" s="2">
+        <v>2165.3000000000002</v>
+      </c>
+      <c r="I34" s="2">
+        <v>2320.3000000000002</v>
+      </c>
+      <c r="J34" s="2">
+        <v>4.1947999999999999</v>
+      </c>
+      <c r="K34" s="2">
+        <v>6.7274000000000003</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A35" s="13"/>
+      <c r="B35" s="16"/>
+      <c r="C35" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="D35" s="4">
+        <v>8.0267999999999997</v>
+      </c>
+      <c r="E35" s="4">
+        <v>28.899000000000001</v>
+      </c>
+      <c r="F35" s="4">
+        <v>2.5811000000000002</v>
+      </c>
+      <c r="G35" s="4">
+        <v>4.0179999999999998</v>
+      </c>
+      <c r="H35" s="4">
+        <v>1213.4000000000001</v>
+      </c>
+      <c r="I35" s="2">
+        <v>1698.5</v>
+      </c>
+      <c r="J35" s="2">
+        <v>4.5711000000000004</v>
+      </c>
+      <c r="K35" s="2">
+        <v>7.3220999999999998</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A36" s="13"/>
+      <c r="B36" s="16"/>
+      <c r="C36" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D36" s="4">
+        <v>8.0846</v>
+      </c>
+      <c r="E36" s="4">
+        <v>21.623000000000001</v>
+      </c>
+      <c r="F36" s="4">
+        <v>4.9984999999999999</v>
+      </c>
+      <c r="G36" s="4">
+        <v>3.8734000000000002</v>
+      </c>
+      <c r="H36" s="4">
+        <v>1330.8</v>
+      </c>
+      <c r="I36" s="4">
+        <v>2586.3000000000002</v>
+      </c>
+      <c r="J36" s="4">
+        <v>4.0925000000000002</v>
+      </c>
+      <c r="K36" s="4">
+        <v>6.8217999999999996</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="14"/>
+      <c r="B37" s="17"/>
+      <c r="C37" s="7"/>
+      <c r="L37" s="11"/>
+    </row>
+    <row r="38" spans="1:12" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="12">
+        <v>900</v>
+      </c>
+      <c r="B38" s="15" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A39" s="13"/>
+      <c r="B39" s="16"/>
+      <c r="C39" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D39" s="4">
+        <v>8.7007999999999992</v>
+      </c>
+      <c r="E39" s="4">
+        <v>379.67</v>
+      </c>
+      <c r="F39" s="4">
+        <v>0.15739</v>
+      </c>
+      <c r="G39" s="4">
+        <v>4.2165999999999997</v>
+      </c>
+      <c r="H39" s="4">
+        <v>994.53</v>
+      </c>
+      <c r="I39" s="4">
+        <v>1533.4</v>
+      </c>
+      <c r="J39" s="4">
+        <v>4.6802000000000001</v>
+      </c>
+      <c r="K39" s="4">
+        <v>7.0461</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A40" s="13"/>
+      <c r="B40" s="16"/>
+      <c r="C40" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D40" s="2">
+        <v>9.3439999999999994</v>
+      </c>
+      <c r="E40" s="2">
+        <v>45.972000000000001</v>
+      </c>
+      <c r="F40" s="2">
+        <v>2.5375000000000001</v>
+      </c>
+      <c r="G40" s="2">
+        <v>3.4094000000000002</v>
+      </c>
+      <c r="H40" s="2">
+        <v>1902</v>
+      </c>
+      <c r="I40" s="2">
+        <v>2101.5</v>
+      </c>
+      <c r="J40" s="2">
+        <v>4.3022</v>
+      </c>
+      <c r="K40" s="2">
+        <v>6.1081000000000003</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A41" s="13"/>
+      <c r="B41" s="16"/>
+      <c r="C41" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D41" s="2">
+        <v>3.0011000000000001</v>
+      </c>
+      <c r="E41" s="2">
+        <v>18.974</v>
+      </c>
+      <c r="F41" s="2">
+        <v>32.389000000000003</v>
+      </c>
+      <c r="G41" s="2">
+        <v>3.2721</v>
+      </c>
+      <c r="H41" s="2">
+        <v>2021.2</v>
+      </c>
+      <c r="I41" s="2">
+        <v>2356.1999999999998</v>
+      </c>
+      <c r="J41" s="2">
+        <v>4.4100999999999999</v>
+      </c>
+      <c r="K41" s="2">
+        <v>17.539000000000001</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A42" s="13"/>
+      <c r="B42" s="16"/>
+      <c r="C42" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="D42" s="2">
+        <v>2.1263000000000001</v>
+      </c>
+      <c r="E42" s="2">
+        <v>19.571000000000002</v>
+      </c>
+      <c r="F42" s="2">
+        <v>18.852</v>
+      </c>
+      <c r="G42" s="2">
+        <v>3.3525</v>
+      </c>
+      <c r="H42" s="2">
+        <v>1999.6</v>
+      </c>
+      <c r="I42" s="2">
+        <v>2639.8</v>
+      </c>
+      <c r="J42" s="2">
+        <v>4.3577000000000004</v>
+      </c>
+      <c r="K42" s="2">
+        <v>21.824999999999999</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A43" s="13"/>
+      <c r="B43" s="16"/>
+      <c r="C43" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D43" s="2">
+        <v>16.257000000000001</v>
+      </c>
+      <c r="E43" s="2">
+        <v>181.45</v>
+      </c>
+      <c r="F43" s="2">
+        <v>0.50260000000000005</v>
+      </c>
+      <c r="G43" s="2">
+        <v>3.0154000000000001</v>
+      </c>
+      <c r="H43" s="2">
+        <v>2606.1999999999998</v>
+      </c>
+      <c r="I43" s="2">
+        <v>2445.1</v>
+      </c>
+      <c r="J43" s="2">
+        <v>4.1307</v>
+      </c>
+      <c r="K43" s="2">
+        <v>5.6963999999999997</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A44" s="13"/>
+      <c r="B44" s="16"/>
+      <c r="C44" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="D44" s="2">
+        <v>9.5314999999999994</v>
+      </c>
+      <c r="E44" s="2">
+        <v>149.26</v>
+      </c>
+      <c r="F44" s="2">
+        <v>0.37325999999999998</v>
+      </c>
+      <c r="G44" s="2">
+        <v>3.9582000000000002</v>
+      </c>
+      <c r="H44" s="2">
+        <v>1254.5999999999999</v>
+      </c>
+      <c r="I44" s="2">
+        <v>2014.8</v>
+      </c>
+      <c r="J44" s="2">
+        <v>4.3853999999999997</v>
+      </c>
+      <c r="K44" s="2">
+        <v>8.0510999999999999</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A45" s="13"/>
+      <c r="B45" s="16"/>
+      <c r="C45" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D45" s="2">
+        <v>6.4694000000000003</v>
+      </c>
+      <c r="E45" s="2">
+        <v>149.62</v>
+      </c>
+      <c r="F45" s="2">
+        <v>0.29610999999999998</v>
+      </c>
+      <c r="G45" s="2">
+        <v>4.1942000000000004</v>
+      </c>
+      <c r="H45" s="2">
+        <v>1123.8</v>
+      </c>
+      <c r="I45" s="2">
+        <v>2045.9</v>
+      </c>
+      <c r="J45" s="2">
+        <v>4.4272</v>
+      </c>
+      <c r="K45" s="2">
+        <v>9.5322999999999993</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A46" s="13"/>
+      <c r="B46" s="16"/>
+      <c r="C46" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D46" s="2">
+        <v>12.617000000000001</v>
+      </c>
+      <c r="E46" s="2">
+        <v>119.8</v>
+      </c>
+      <c r="F46" s="2">
+        <v>0.37544</v>
+      </c>
+      <c r="G46" s="2">
+        <v>3.7416</v>
+      </c>
+      <c r="H46" s="2">
+        <v>1366.4</v>
+      </c>
+      <c r="I46" s="2">
+        <v>1894.5</v>
+      </c>
+      <c r="J46" s="2">
+        <v>4.5370999999999997</v>
+      </c>
+      <c r="K46" s="2">
+        <v>9.6135999999999999</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A47" s="13"/>
+      <c r="B47" s="16"/>
+      <c r="C47" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="D47" s="4">
+        <v>11.849</v>
+      </c>
+      <c r="E47" s="4">
+        <v>272.72000000000003</v>
+      </c>
+      <c r="F47" s="4">
+        <v>0.21346999999999999</v>
+      </c>
+      <c r="G47" s="4">
+        <v>3.8447</v>
+      </c>
+      <c r="H47" s="4">
+        <v>1238.3</v>
+      </c>
+      <c r="I47" s="4">
+        <v>1731</v>
+      </c>
+      <c r="J47" s="4">
+        <v>4.5635000000000003</v>
+      </c>
+      <c r="K47" s="4">
+        <v>7.4757999999999996</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A48" s="13"/>
+      <c r="B48" s="16"/>
+      <c r="C48" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D48" s="4">
+        <v>7.9996999999999998</v>
+      </c>
+      <c r="E48" s="4">
+        <v>25.007999999999999</v>
+      </c>
+      <c r="F48" s="4">
+        <v>2.2597</v>
+      </c>
+      <c r="G48" s="4">
+        <v>4.1269999999999998</v>
+      </c>
+      <c r="H48" s="4">
+        <v>1102.2</v>
+      </c>
+      <c r="I48" s="2">
+        <v>1841.7</v>
+      </c>
+      <c r="J48" s="2">
+        <v>4.5534999999999997</v>
+      </c>
+      <c r="K48" s="2">
+        <v>10.206</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="14"/>
+      <c r="B49" s="17"/>
+      <c r="C49" s="7"/>
+      <c r="L49" s="11"/>
+    </row>
+    <row r="50" spans="1:12" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="12">
+        <v>1000</v>
+      </c>
+      <c r="B50" s="15" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A51" s="13"/>
+      <c r="B51" s="16"/>
+      <c r="C51" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="D51" s="4">
+        <v>1.9302999999999999</v>
+      </c>
+      <c r="E51" s="4">
+        <v>413.72</v>
+      </c>
+      <c r="F51" s="4">
+        <v>2.4257999999999998E-2</v>
+      </c>
+      <c r="G51" s="4">
+        <v>4.1744000000000003</v>
+      </c>
+      <c r="H51" s="4">
+        <v>720.53</v>
+      </c>
+      <c r="I51" s="4">
+        <v>3740</v>
+      </c>
+      <c r="J51" s="4">
+        <v>3.2875000000000001</v>
+      </c>
+      <c r="K51" s="4">
+        <v>7.5471000000000004</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A52" s="13"/>
+      <c r="B52" s="16"/>
+      <c r="C52" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="D52" s="4">
+        <v>3.7450000000000001</v>
+      </c>
+      <c r="E52" s="4">
+        <v>5.5084999999999997</v>
+      </c>
+      <c r="F52" s="4">
+        <v>10.981999999999999</v>
+      </c>
+      <c r="G52" s="4">
+        <v>3.9323000000000001</v>
+      </c>
+      <c r="H52" s="4">
+        <v>723.41</v>
+      </c>
+      <c r="I52" s="4">
+        <v>9445.2999999999993</v>
+      </c>
+      <c r="J52" s="4">
+        <v>2.7645</v>
+      </c>
+      <c r="K52" s="4">
+        <v>5.3007</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A53" s="13"/>
+      <c r="B53" s="16"/>
+      <c r="C53" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="D53" s="4">
+        <v>1.0051000000000001</v>
+      </c>
+      <c r="E53" s="4">
+        <v>41.567999999999998</v>
+      </c>
+      <c r="F53" s="4">
+        <v>0.50309999999999999</v>
+      </c>
+      <c r="G53" s="4">
+        <v>4.4626000000000001</v>
+      </c>
+      <c r="H53" s="4">
+        <v>582.32000000000005</v>
+      </c>
+      <c r="I53" s="4">
+        <v>2413</v>
+      </c>
+      <c r="J53" s="4">
+        <v>3.508</v>
+      </c>
+      <c r="K53" s="4">
+        <v>6.1177999999999999</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A54" s="13"/>
+      <c r="B54" s="16"/>
+      <c r="C54" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="D54" s="4">
+        <v>0.34182000000000001</v>
+      </c>
+      <c r="E54" s="4">
+        <v>3.0001000000000002</v>
+      </c>
+      <c r="F54" s="4">
+        <v>2.6158000000000001</v>
+      </c>
+      <c r="G54" s="4">
+        <v>4.5224000000000002</v>
+      </c>
+      <c r="H54" s="4">
+        <v>605.76</v>
+      </c>
+      <c r="I54" s="4">
+        <v>9686.9</v>
+      </c>
+      <c r="J54" s="4">
+        <v>2.8176999999999999</v>
+      </c>
+      <c r="K54" s="4">
+        <v>7.5712000000000002</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A55" s="13"/>
+      <c r="B55" s="16"/>
+      <c r="C55" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="D55" s="4">
+        <v>0.74811000000000005</v>
+      </c>
+      <c r="E55" s="4">
+        <v>4.8129999999999997</v>
+      </c>
+      <c r="F55" s="4">
+        <v>1.5203</v>
+      </c>
+      <c r="G55" s="4">
+        <v>4.5427</v>
+      </c>
+      <c r="H55" s="4">
+        <v>578.84</v>
+      </c>
+      <c r="I55" s="4">
+        <v>5902.3</v>
+      </c>
+      <c r="J55" s="4">
+        <v>3.0358000000000001</v>
+      </c>
+      <c r="K55" s="4">
+        <v>7.2228000000000003</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A56" s="13"/>
+      <c r="B56" s="16"/>
+      <c r="C56" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="D56" s="4">
+        <v>2.2985000000000002</v>
+      </c>
+      <c r="E56" s="4">
+        <v>17.765000000000001</v>
+      </c>
+      <c r="F56" s="4">
+        <v>0.53407000000000004</v>
+      </c>
+      <c r="G56" s="4">
+        <v>4.1894999999999998</v>
+      </c>
+      <c r="H56" s="4">
+        <v>695.87</v>
+      </c>
+      <c r="I56" s="4">
+        <v>4582.3999999999996</v>
+      </c>
+      <c r="J56" s="4">
+        <v>3.1497999999999999</v>
+      </c>
+      <c r="K56" s="4">
+        <v>6.8537999999999997</v>
+      </c>
+    </row>
+    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A57" s="13"/>
+      <c r="B57" s="16"/>
+      <c r="C57" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="D57" s="4">
+        <v>1.7064999999999999</v>
+      </c>
+      <c r="E57" s="4">
+        <v>2.9634999999999998</v>
+      </c>
+      <c r="F57" s="4">
+        <v>8.5671999999999997</v>
+      </c>
+      <c r="G57" s="4">
+        <v>4.2396000000000003</v>
+      </c>
+      <c r="H57" s="4">
+        <v>648.58000000000004</v>
+      </c>
+      <c r="I57" s="4">
+        <v>9968.2000000000007</v>
+      </c>
+      <c r="J57" s="4">
+        <v>2.8411</v>
+      </c>
+      <c r="K57" s="4">
+        <v>9.9029000000000007</v>
+      </c>
+    </row>
+    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A58" s="13"/>
+      <c r="B58" s="16"/>
+      <c r="C58" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="D58" s="4">
+        <v>1.2569999999999999</v>
+      </c>
+      <c r="E58" s="4">
+        <v>4.6817000000000002</v>
+      </c>
+      <c r="F58" s="4">
+        <v>6.5932000000000004</v>
+      </c>
+      <c r="G58" s="4">
+        <v>4.2586000000000004</v>
+      </c>
+      <c r="H58" s="4">
+        <v>671.09</v>
+      </c>
+      <c r="I58" s="4">
+        <v>9375.2000000000007</v>
+      </c>
+      <c r="J58" s="4">
+        <v>2.7982999999999998</v>
+      </c>
+      <c r="K58" s="4">
+        <v>6.5297000000000001</v>
+      </c>
+    </row>
+    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A59" s="13"/>
+      <c r="B59" s="16"/>
+      <c r="C59" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="D59" s="4">
+        <v>0.54088000000000003</v>
+      </c>
+      <c r="E59" s="4">
+        <v>3.4417</v>
+      </c>
+      <c r="F59" s="4">
+        <v>3.8666</v>
+      </c>
+      <c r="G59" s="4">
+        <v>4.4062000000000001</v>
+      </c>
+      <c r="H59" s="4">
+        <v>640.30999999999995</v>
+      </c>
+      <c r="I59" s="4">
+        <v>9914.9</v>
+      </c>
+      <c r="J59" s="4">
+        <v>2.8043999999999998</v>
+      </c>
+      <c r="K59" s="4">
+        <v>7.6501999999999999</v>
+      </c>
+    </row>
+    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A60" s="13"/>
+      <c r="B60" s="16"/>
+      <c r="C60" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="D60" s="4">
+        <v>2.9771999999999998</v>
+      </c>
+      <c r="E60" s="4">
+        <v>13.58</v>
+      </c>
+      <c r="F60" s="4">
+        <v>2.2099000000000002</v>
+      </c>
+      <c r="G60" s="4">
+        <v>4.0601000000000003</v>
+      </c>
+      <c r="H60" s="4">
+        <v>697.13</v>
+      </c>
+      <c r="I60" s="4">
+        <v>2654.7</v>
+      </c>
+      <c r="J60" s="4">
+        <v>3.4464999999999999</v>
+      </c>
+      <c r="K60" s="4">
+        <v>5.4966999999999997</v>
+      </c>
+    </row>
+    <row r="61" spans="1:12" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="14"/>
+      <c r="B61" s="17"/>
+      <c r="C61" s="7"/>
+      <c r="L61" s="11"/>
+    </row>
+    <row r="62" spans="1:12" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="12">
+        <v>1000</v>
+      </c>
+      <c r="B62" s="15" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A63" s="13"/>
+      <c r="B63" s="16"/>
+      <c r="C63" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="D63" s="4">
+        <v>4.6173000000000004E-3</v>
+      </c>
+      <c r="E63" s="4">
+        <v>6.8475999999999999</v>
+      </c>
+      <c r="F63" s="4">
+        <v>2.2387000000000001</v>
+      </c>
+      <c r="G63" s="4">
+        <v>4.8326000000000002</v>
+      </c>
+      <c r="H63" s="4">
+        <v>460.38</v>
+      </c>
+      <c r="I63" s="4">
+        <v>2357.9</v>
+      </c>
+      <c r="J63" s="4">
+        <v>3.5989</v>
+      </c>
+      <c r="K63" s="4">
+        <v>6.8921999999999999</v>
+      </c>
+    </row>
+    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A64" s="13"/>
+      <c r="B64" s="16"/>
+      <c r="C64" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="D64" s="4">
+        <v>3.1901000000000002</v>
+      </c>
+      <c r="E64" s="4">
+        <v>126.5</v>
+      </c>
+      <c r="F64" s="4">
+        <v>0.16925000000000001</v>
+      </c>
+      <c r="G64" s="4">
+        <v>3.8923999999999999</v>
+      </c>
+      <c r="H64" s="4">
+        <v>802.2</v>
+      </c>
+      <c r="I64" s="4">
+        <v>2253.9</v>
+      </c>
+      <c r="J64" s="4">
+        <v>3.6876000000000002</v>
+      </c>
+      <c r="K64" s="4">
+        <v>11.145</v>
+      </c>
+    </row>
+    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A65" s="13"/>
+      <c r="B65" s="16"/>
+      <c r="C65" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="D65" s="4">
+        <v>0.31556000000000001</v>
+      </c>
+      <c r="E65" s="4">
+        <v>4.9177</v>
+      </c>
+      <c r="F65" s="4">
+        <v>4.2816000000000001</v>
+      </c>
+      <c r="G65" s="4">
+        <v>4.8133999999999997</v>
+      </c>
+      <c r="H65" s="4">
+        <v>468.63</v>
+      </c>
+      <c r="I65" s="4">
+        <v>3308.8</v>
+      </c>
+      <c r="J65" s="4">
+        <v>3.3386999999999998</v>
+      </c>
+      <c r="K65" s="4">
+        <v>5.7804000000000002</v>
+      </c>
+    </row>
+    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A66" s="13"/>
+      <c r="B66" s="16"/>
+      <c r="C66" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="D66" s="4">
+        <v>0.26189000000000001</v>
+      </c>
+      <c r="E66" s="4">
+        <v>37.661999999999999</v>
+      </c>
+      <c r="F66" s="4">
+        <v>0.20133999999999999</v>
+      </c>
+      <c r="G66" s="4">
+        <v>4.8079000000000001</v>
+      </c>
+      <c r="H66" s="4">
+        <v>478.84</v>
+      </c>
+      <c r="I66" s="4">
+        <v>2939.9</v>
+      </c>
+      <c r="J66" s="4">
+        <v>3.4262000000000001</v>
+      </c>
+      <c r="K66" s="4">
+        <v>5.9608999999999996</v>
+      </c>
+    </row>
+    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A67" s="13"/>
+      <c r="B67" s="16"/>
+      <c r="C67" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="D67" s="4">
+        <v>1.5331999999999999</v>
+      </c>
+      <c r="E67" s="4">
+        <v>6.9652000000000003</v>
+      </c>
+      <c r="F67" s="4">
+        <v>4.9490999999999996</v>
+      </c>
+      <c r="G67" s="4">
+        <v>4.3071999999999999</v>
+      </c>
+      <c r="H67" s="4">
+        <v>551.01</v>
+      </c>
+      <c r="I67" s="4">
+        <v>1467.1</v>
+      </c>
+      <c r="J67" s="4">
+        <v>4.0639000000000003</v>
+      </c>
+      <c r="K67" s="4">
+        <v>13.561</v>
+      </c>
+    </row>
+    <row r="68" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A68" s="13"/>
+      <c r="B68" s="16"/>
+      <c r="C68" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="D68" s="4">
+        <v>0.18711</v>
+      </c>
+      <c r="E68" s="4">
+        <v>42.057000000000002</v>
+      </c>
+      <c r="F68" s="4">
+        <v>1.22</v>
+      </c>
+      <c r="G68" s="4">
+        <v>3.9495</v>
+      </c>
+      <c r="H68" s="4">
+        <v>803.58</v>
+      </c>
+      <c r="I68" s="4">
+        <v>1759.6</v>
+      </c>
+      <c r="J68" s="4">
+        <v>3.8088000000000002</v>
+      </c>
+      <c r="K68" s="4">
+        <v>6.9718</v>
+      </c>
+    </row>
+    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A69" s="13"/>
+      <c r="B69" s="16"/>
+      <c r="C69" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="D69" s="4">
+        <v>3.4416000000000002</v>
+      </c>
+      <c r="E69" s="4">
+        <v>6.2590000000000003</v>
+      </c>
+      <c r="F69" s="4">
+        <v>1.3140000000000001</v>
+      </c>
+      <c r="G69" s="4">
+        <v>4.0781999999999998</v>
+      </c>
+      <c r="H69" s="4">
+        <v>707.11</v>
+      </c>
+      <c r="I69" s="4">
+        <v>4504.6000000000004</v>
+      </c>
+      <c r="J69" s="4">
+        <v>3.2162000000000002</v>
+      </c>
+      <c r="K69" s="4">
+        <v>8.2904</v>
+      </c>
+    </row>
+    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A70" s="13"/>
+      <c r="B70" s="16"/>
+      <c r="C70" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="D70" s="4">
+        <v>4.5324999999999998</v>
+      </c>
+      <c r="E70" s="4">
+        <v>14.166</v>
+      </c>
+      <c r="F70" s="4">
+        <v>2.2204999999999999</v>
+      </c>
+      <c r="G70" s="4">
+        <v>3.8813</v>
+      </c>
+      <c r="H70" s="4">
+        <v>731.02</v>
+      </c>
+      <c r="I70" s="4">
+        <v>2379.1</v>
+      </c>
+      <c r="J70" s="4">
+        <v>3.5503999999999998</v>
+      </c>
+      <c r="K70" s="4">
+        <v>6.0315000000000003</v>
+      </c>
+    </row>
+    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A71" s="13"/>
+      <c r="B71" s="16"/>
+      <c r="C71" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="D71" s="4">
+        <v>3.3203</v>
+      </c>
+      <c r="E71" s="4">
+        <v>95.748000000000005</v>
+      </c>
+      <c r="F71" s="4">
+        <v>0.45551999999999998</v>
+      </c>
+      <c r="G71" s="4">
+        <v>4.0633999999999997</v>
+      </c>
+      <c r="H71" s="4">
+        <v>574.87</v>
+      </c>
+      <c r="I71" s="4">
+        <v>1034.8</v>
+      </c>
+      <c r="J71" s="4">
+        <v>4.2290999999999999</v>
+      </c>
+      <c r="K71" s="4">
+        <v>6.0321999999999996</v>
+      </c>
+    </row>
+    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A72" s="13"/>
+      <c r="B72" s="16"/>
+      <c r="C72" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="D72" s="4">
+        <v>4.0854999999999997</v>
+      </c>
+      <c r="E72" s="4">
+        <v>246.68</v>
+      </c>
+      <c r="F72" s="4">
+        <v>8.4526000000000004E-2</v>
+      </c>
+      <c r="G72" s="4">
+        <v>3.9321000000000002</v>
+      </c>
+      <c r="H72" s="4">
+        <v>776.2</v>
+      </c>
+      <c r="I72" s="4">
+        <v>2681.7</v>
+      </c>
+      <c r="J72" s="4">
+        <v>3.4426000000000001</v>
+      </c>
+      <c r="K72" s="4">
+        <v>5.5305</v>
+      </c>
+    </row>
+    <row r="73" spans="1:12" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A73" s="14"/>
+      <c r="B73" s="17"/>
+      <c r="C73" s="7"/>
+      <c r="L73" s="11"/>
+    </row>
+    <row r="74" spans="1:12" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="75" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D75" s="4">
+        <f>MAX(D1:D71)</f>
+        <v>38.180999999999997</v>
+      </c>
+      <c r="E75" s="4">
+        <f t="shared" ref="E75:K75" si="0">MAX(E1:E71)</f>
+        <v>522.85</v>
+      </c>
+      <c r="F75" s="4">
+        <f t="shared" si="0"/>
+        <v>32.389000000000003</v>
+      </c>
+      <c r="G75" s="4">
+        <f t="shared" si="0"/>
+        <v>4.8326000000000002</v>
+      </c>
+      <c r="H75" s="4">
+        <f t="shared" si="0"/>
+        <v>3154.4</v>
+      </c>
+      <c r="I75" s="4">
+        <f t="shared" si="0"/>
+        <v>9968.2000000000007</v>
+      </c>
+      <c r="J75" s="4">
+        <f t="shared" si="0"/>
+        <v>5.6638000000000002</v>
+      </c>
+      <c r="K75" s="4">
+        <f t="shared" si="0"/>
+        <v>21.824999999999999</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="12">
     <mergeCell ref="A2:A13"/>
     <mergeCell ref="B2:B13"/>
     <mergeCell ref="A14:A25"/>
@@ -5239,2067 +7293,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF6E341A-51E3-4AF7-809B-A8594B1323BC}">
-  <dimension ref="A1:L75"/>
-  <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A51" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P59" sqref="P59"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="9.140625" style="4"/>
-    <col min="2" max="2" width="9.140625" style="3"/>
-    <col min="3" max="3" width="15.7109375" style="8" customWidth="1"/>
-    <col min="4" max="11" width="9.140625" style="4"/>
-    <col min="12" max="12" width="9.140625" style="9"/>
-    <col min="13" max="16384" width="9.140625" style="4"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C1" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="H1" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="I1" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="11"/>
-    </row>
-    <row r="2" spans="1:12" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="12">
-        <v>800</v>
-      </c>
-      <c r="B2" s="15" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="13"/>
-      <c r="B3" s="16"/>
-      <c r="C3" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="D3" s="4">
-        <v>16.994</v>
-      </c>
-      <c r="E3" s="4">
-        <v>187.83</v>
-      </c>
-      <c r="F3" s="4">
-        <v>0.26103999999999999</v>
-      </c>
-      <c r="G3" s="4">
-        <v>4.5019999999999998</v>
-      </c>
-      <c r="H3" s="4">
-        <v>1784.8</v>
-      </c>
-      <c r="I3" s="2">
-        <v>3263.5</v>
-      </c>
-      <c r="J3" s="2">
-        <v>4.9230999999999998</v>
-      </c>
-      <c r="K3" s="2">
-        <v>13.172000000000001</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="13"/>
-      <c r="B4" s="16"/>
-      <c r="C4" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="D4" s="4">
-        <v>22.454000000000001</v>
-      </c>
-      <c r="E4" s="4">
-        <v>66.77</v>
-      </c>
-      <c r="F4" s="4">
-        <v>0.92681000000000002</v>
-      </c>
-      <c r="G4" s="4">
-        <v>4.4191000000000003</v>
-      </c>
-      <c r="H4" s="4">
-        <v>1610.1</v>
-      </c>
-      <c r="I4" s="2">
-        <v>2142</v>
-      </c>
-      <c r="J4" s="2">
-        <v>5.4843999999999999</v>
-      </c>
-      <c r="K4" s="2">
-        <v>11.449</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" s="13"/>
-      <c r="B5" s="16"/>
-      <c r="C5" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="D5" s="4">
-        <v>9.1647999999999996</v>
-      </c>
-      <c r="E5" s="4">
-        <v>36.326000000000001</v>
-      </c>
-      <c r="F5" s="4">
-        <v>12.337</v>
-      </c>
-      <c r="G5" s="4">
-        <v>4.2247000000000003</v>
-      </c>
-      <c r="H5" s="4">
-        <v>1776.1</v>
-      </c>
-      <c r="I5" s="2">
-        <v>2731</v>
-      </c>
-      <c r="J5" s="2">
-        <v>5.0411000000000001</v>
-      </c>
-      <c r="K5" s="2">
-        <v>8.3102999999999998</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="13"/>
-      <c r="B6" s="16"/>
-      <c r="C6" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="D6" s="4">
-        <v>5.8951000000000002</v>
-      </c>
-      <c r="E6" s="4">
-        <v>36.906999999999996</v>
-      </c>
-      <c r="F6" s="4">
-        <v>5.3551000000000002</v>
-      </c>
-      <c r="G6" s="4">
-        <v>4.7310999999999996</v>
-      </c>
-      <c r="H6" s="4">
-        <v>1557.8</v>
-      </c>
-      <c r="I6" s="2">
-        <v>2224.1</v>
-      </c>
-      <c r="J6" s="2">
-        <v>5.2808999999999999</v>
-      </c>
-      <c r="K6" s="2">
-        <v>6.5113000000000003</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="13"/>
-      <c r="B7" s="16"/>
-      <c r="C7" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="D7" s="4">
-        <v>4.1860999999999997</v>
-      </c>
-      <c r="E7" s="4">
-        <v>84.548000000000002</v>
-      </c>
-      <c r="F7" s="4">
-        <v>2.1124999999999998</v>
-      </c>
-      <c r="G7" s="4">
-        <v>4.7670000000000003</v>
-      </c>
-      <c r="H7" s="4">
-        <v>1574.1</v>
-      </c>
-      <c r="I7" s="4">
-        <v>2883.2</v>
-      </c>
-      <c r="J7" s="4">
-        <v>4.8395000000000001</v>
-      </c>
-      <c r="K7" s="4">
-        <v>4.5430999999999999</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" s="13"/>
-      <c r="B8" s="16"/>
-      <c r="C8" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="D8" s="2">
-        <v>27.867999999999999</v>
-      </c>
-      <c r="E8" s="2">
-        <v>89.338999999999999</v>
-      </c>
-      <c r="F8" s="2">
-        <v>0.59711999999999998</v>
-      </c>
-      <c r="G8" s="2">
-        <v>4.1981999999999999</v>
-      </c>
-      <c r="H8" s="2">
-        <v>1818</v>
-      </c>
-      <c r="I8" s="2">
-        <v>2645.2</v>
-      </c>
-      <c r="J8" s="2">
-        <v>5.1192000000000002</v>
-      </c>
-      <c r="K8" s="2">
-        <v>10.125</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" s="13"/>
-      <c r="B9" s="16"/>
-      <c r="C9" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="D9" s="2">
-        <v>28.599</v>
-      </c>
-      <c r="E9" s="2">
-        <v>78.057000000000002</v>
-      </c>
-      <c r="F9" s="2">
-        <v>0.84292</v>
-      </c>
-      <c r="G9" s="2">
-        <v>3.8371</v>
-      </c>
-      <c r="H9" s="2">
-        <v>2441.5</v>
-      </c>
-      <c r="I9" s="2">
-        <v>2969.6</v>
-      </c>
-      <c r="J9" s="2">
-        <v>4.9976000000000003</v>
-      </c>
-      <c r="K9" s="2">
-        <v>10.641999999999999</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" s="13"/>
-      <c r="B10" s="16"/>
-      <c r="C10" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="D10" s="2">
-        <v>29.978999999999999</v>
-      </c>
-      <c r="E10" s="2">
-        <v>119.58</v>
-      </c>
-      <c r="F10" s="2">
-        <v>0.55200000000000005</v>
-      </c>
-      <c r="G10" s="2">
-        <v>3.8504999999999998</v>
-      </c>
-      <c r="H10" s="2">
-        <v>2314.4</v>
-      </c>
-      <c r="I10" s="2">
-        <v>2808.8</v>
-      </c>
-      <c r="J10" s="2">
-        <v>5.0354000000000001</v>
-      </c>
-      <c r="K10" s="2">
-        <v>9.5434999999999999</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" s="13"/>
-      <c r="B11" s="16"/>
-      <c r="C11" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="D11" s="4">
-        <v>19.125</v>
-      </c>
-      <c r="E11" s="4">
-        <v>43.640999999999998</v>
-      </c>
-      <c r="F11" s="4">
-        <v>5.6147999999999998</v>
-      </c>
-      <c r="G11" s="4">
-        <v>4.1688000000000001</v>
-      </c>
-      <c r="H11" s="4">
-        <v>1616</v>
-      </c>
-      <c r="I11" s="4">
-        <v>1876.8</v>
-      </c>
-      <c r="J11" s="4">
-        <v>5.5594000000000001</v>
-      </c>
-      <c r="K11" s="4">
-        <v>6.8653000000000004</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" s="13"/>
-      <c r="B12" s="16"/>
-      <c r="C12" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="D12" s="4">
-        <v>22.012</v>
-      </c>
-      <c r="E12" s="4">
-        <v>38.872999999999998</v>
-      </c>
-      <c r="F12" s="4">
-        <v>2.2033</v>
-      </c>
-      <c r="G12" s="4">
-        <v>4.2450000000000001</v>
-      </c>
-      <c r="H12" s="4">
-        <v>1841.2</v>
-      </c>
-      <c r="I12" s="2">
-        <v>2377</v>
-      </c>
-      <c r="J12" s="2">
-        <v>5.2897999999999996</v>
-      </c>
-      <c r="K12" s="2">
-        <v>9.7712000000000003</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="14"/>
-      <c r="B13" s="17"/>
-      <c r="C13" s="7"/>
-      <c r="L13" s="11"/>
-    </row>
-    <row r="14" spans="1:12" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="12">
-        <v>800</v>
-      </c>
-      <c r="B14" s="15" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A15" s="13"/>
-      <c r="B15" s="16"/>
-      <c r="C15" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="D15" s="4">
-        <v>31.646999999999998</v>
-      </c>
-      <c r="E15" s="4">
-        <v>120.62</v>
-      </c>
-      <c r="F15" s="4">
-        <v>0.85485</v>
-      </c>
-      <c r="G15" s="4">
-        <v>3.7265999999999999</v>
-      </c>
-      <c r="H15" s="4">
-        <v>2297.8000000000002</v>
-      </c>
-      <c r="I15" s="4">
-        <v>2165.6999999999998</v>
-      </c>
-      <c r="J15" s="4">
-        <v>5.3247</v>
-      </c>
-      <c r="K15" s="4">
-        <v>7.7724000000000002</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A16" s="13"/>
-      <c r="B16" s="16"/>
-      <c r="C16" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="D16" s="2">
-        <v>33.296999999999997</v>
-      </c>
-      <c r="E16" s="2">
-        <v>522.85</v>
-      </c>
-      <c r="F16" s="2">
-        <v>0.11871</v>
-      </c>
-      <c r="G16" s="2">
-        <v>3.9767000000000001</v>
-      </c>
-      <c r="H16" s="2">
-        <v>1762.4</v>
-      </c>
-      <c r="I16" s="2">
-        <v>1913.8</v>
-      </c>
-      <c r="J16" s="2">
-        <v>5.6638000000000002</v>
-      </c>
-      <c r="K16" s="2">
-        <v>11.287000000000001</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A17" s="13"/>
-      <c r="B17" s="16"/>
-      <c r="C17" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="D17" s="2">
-        <v>15.042</v>
-      </c>
-      <c r="E17" s="2">
-        <v>35.436999999999998</v>
-      </c>
-      <c r="F17" s="2">
-        <v>8.4</v>
-      </c>
-      <c r="G17" s="2">
-        <v>3.9586000000000001</v>
-      </c>
-      <c r="H17" s="2">
-        <v>2283.5</v>
-      </c>
-      <c r="I17" s="2">
-        <v>4184.6000000000004</v>
-      </c>
-      <c r="J17" s="2">
-        <v>4.4257</v>
-      </c>
-      <c r="K17" s="2">
-        <v>6.6603000000000003</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A18" s="13"/>
-      <c r="B18" s="16"/>
-      <c r="C18" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="D18" s="2">
-        <v>38.180999999999997</v>
-      </c>
-      <c r="E18" s="2">
-        <v>51.055</v>
-      </c>
-      <c r="F18" s="2">
-        <v>2.4819</v>
-      </c>
-      <c r="G18" s="2">
-        <v>3.2572000000000001</v>
-      </c>
-      <c r="H18" s="2">
-        <v>3154.4</v>
-      </c>
-      <c r="I18" s="2">
-        <v>2725.2</v>
-      </c>
-      <c r="J18" s="2">
-        <v>5.0167000000000002</v>
-      </c>
-      <c r="K18" s="2">
-        <v>8.33</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A19" s="13"/>
-      <c r="B19" s="16"/>
-      <c r="C19" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="D19" s="4">
-        <v>24.888999999999999</v>
-      </c>
-      <c r="E19" s="4">
-        <v>44.932000000000002</v>
-      </c>
-      <c r="F19" s="4">
-        <v>1.2076</v>
-      </c>
-      <c r="G19" s="4">
-        <v>4.5054999999999996</v>
-      </c>
-      <c r="H19" s="4">
-        <v>1527.9</v>
-      </c>
-      <c r="I19" s="4">
-        <v>2589.6999999999998</v>
-      </c>
-      <c r="J19" s="4">
-        <v>5.1066000000000003</v>
-      </c>
-      <c r="K19" s="4">
-        <v>8.6950000000000003</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A20" s="13"/>
-      <c r="B20" s="16"/>
-      <c r="C20" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="D20" s="2">
-        <v>23.303999999999998</v>
-      </c>
-      <c r="E20" s="2">
-        <v>276.66000000000003</v>
-      </c>
-      <c r="F20" s="2">
-        <v>0.32123000000000002</v>
-      </c>
-      <c r="G20" s="2">
-        <v>4.2591999999999999</v>
-      </c>
-      <c r="H20" s="2">
-        <v>1767.2</v>
-      </c>
-      <c r="I20" s="2">
-        <v>2168.5</v>
-      </c>
-      <c r="J20" s="2">
-        <v>5.3181000000000003</v>
-      </c>
-      <c r="K20" s="2">
-        <v>6.7618999999999998</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A21" s="13"/>
-      <c r="B21" s="16"/>
-      <c r="C21" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="D21" s="2">
-        <v>30.401</v>
-      </c>
-      <c r="E21" s="2">
-        <v>34.817</v>
-      </c>
-      <c r="F21" s="2">
-        <v>4.5983000000000001</v>
-      </c>
-      <c r="G21" s="2">
-        <v>3.5323000000000002</v>
-      </c>
-      <c r="H21" s="2">
-        <v>2583</v>
-      </c>
-      <c r="I21" s="2">
-        <v>2520.9</v>
-      </c>
-      <c r="J21" s="2">
-        <v>5.1558999999999999</v>
-      </c>
-      <c r="K21" s="2">
-        <v>8.5891000000000002</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A22" s="13"/>
-      <c r="B22" s="16"/>
-      <c r="C22" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="D22" s="4">
-        <v>5.0568999999999997</v>
-      </c>
-      <c r="E22" s="4">
-        <v>40.475999999999999</v>
-      </c>
-      <c r="F22" s="4">
-        <v>10.016999999999999</v>
-      </c>
-      <c r="G22" s="4">
-        <v>4.1585000000000001</v>
-      </c>
-      <c r="H22" s="4">
-        <v>1730.1</v>
-      </c>
-      <c r="I22" s="4">
-        <v>1998.1</v>
-      </c>
-      <c r="J22" s="4">
-        <v>5.5564</v>
-      </c>
-      <c r="K22" s="4">
-        <v>10.337</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A23" s="13"/>
-      <c r="B23" s="16"/>
-      <c r="C23" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="D23" s="2">
-        <v>31.809000000000001</v>
-      </c>
-      <c r="E23" s="2">
-        <v>43.194000000000003</v>
-      </c>
-      <c r="F23" s="2">
-        <v>2.2399</v>
-      </c>
-      <c r="G23" s="2">
-        <v>3.9613</v>
-      </c>
-      <c r="H23" s="2">
-        <v>1820.1</v>
-      </c>
-      <c r="I23" s="2">
-        <v>2245.4</v>
-      </c>
-      <c r="J23" s="2">
-        <v>5.3178999999999998</v>
-      </c>
-      <c r="K23" s="2">
-        <v>8.5096000000000007</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A24" s="13"/>
-      <c r="B24" s="16"/>
-      <c r="C24" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="D24" s="4">
-        <v>0.36498999999999998</v>
-      </c>
-      <c r="E24" s="4">
-        <v>45.374000000000002</v>
-      </c>
-      <c r="F24" s="4">
-        <v>15.686999999999999</v>
-      </c>
-      <c r="G24" s="4">
-        <v>3.6105</v>
-      </c>
-      <c r="H24" s="4">
-        <v>2878.3</v>
-      </c>
-      <c r="I24" s="2">
-        <v>3325.8</v>
-      </c>
-      <c r="J24" s="2">
-        <v>4.8470000000000004</v>
-      </c>
-      <c r="K24" s="2">
-        <v>12.327999999999999</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="14"/>
-      <c r="B25" s="17"/>
-      <c r="C25" s="7"/>
-      <c r="L25" s="11"/>
-    </row>
-    <row r="26" spans="1:12" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="12">
-        <v>900</v>
-      </c>
-      <c r="B26" s="15" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A27" s="13"/>
-      <c r="B27" s="16"/>
-      <c r="C27" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="D27" s="2">
-        <v>3.6261999999999999</v>
-      </c>
-      <c r="E27" s="2">
-        <v>13.804</v>
-      </c>
-      <c r="F27" s="2">
-        <v>6.9824999999999999</v>
-      </c>
-      <c r="G27" s="2">
-        <v>4.2416</v>
-      </c>
-      <c r="H27" s="2">
-        <v>1138.2</v>
-      </c>
-      <c r="I27" s="2">
-        <v>1986</v>
-      </c>
-      <c r="J27" s="2">
-        <v>4.4408000000000003</v>
-      </c>
-      <c r="K27" s="2">
-        <v>9.1929999999999996</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A28" s="13"/>
-      <c r="B28" s="16"/>
-      <c r="C28" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="D28" s="2">
-        <v>10.683</v>
-      </c>
-      <c r="E28" s="2">
-        <v>31.381</v>
-      </c>
-      <c r="F28" s="2">
-        <v>2.9727000000000001</v>
-      </c>
-      <c r="G28" s="2">
-        <v>3.7155</v>
-      </c>
-      <c r="H28" s="2">
-        <v>1422</v>
-      </c>
-      <c r="I28" s="2">
-        <v>1626.7</v>
-      </c>
-      <c r="J28" s="2">
-        <v>4.5519999999999996</v>
-      </c>
-      <c r="K28" s="2">
-        <v>6.2319000000000004</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A29" s="13"/>
-      <c r="B29" s="16"/>
-      <c r="C29" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="D29" s="2">
-        <v>10.340999999999999</v>
-      </c>
-      <c r="E29" s="2">
-        <v>24.475999999999999</v>
-      </c>
-      <c r="F29" s="2">
-        <v>2.3226</v>
-      </c>
-      <c r="G29" s="2">
-        <v>3.9651000000000001</v>
-      </c>
-      <c r="H29" s="2">
-        <v>1176.4000000000001</v>
-      </c>
-      <c r="I29" s="2">
-        <v>1743</v>
-      </c>
-      <c r="J29" s="2">
-        <v>4.5865</v>
-      </c>
-      <c r="K29" s="2">
-        <v>9.1586999999999996</v>
-      </c>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A30" s="13"/>
-      <c r="B30" s="16"/>
-      <c r="C30" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="D30" s="2">
-        <v>11.112</v>
-      </c>
-      <c r="E30" s="2">
-        <v>18.959</v>
-      </c>
-      <c r="F30" s="2">
-        <v>5.9504999999999999</v>
-      </c>
-      <c r="G30" s="2">
-        <v>3.6368</v>
-      </c>
-      <c r="H30" s="2">
-        <v>1471.6</v>
-      </c>
-      <c r="I30" s="2">
-        <v>2064.3000000000002</v>
-      </c>
-      <c r="J30" s="2">
-        <v>4.3163999999999998</v>
-      </c>
-      <c r="K30" s="2">
-        <v>7.2249999999999996</v>
-      </c>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A31" s="13"/>
-      <c r="B31" s="16"/>
-      <c r="C31" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="D31" s="2">
-        <v>8.0817999999999994</v>
-      </c>
-      <c r="E31" s="2">
-        <v>9.2744</v>
-      </c>
-      <c r="F31" s="2">
-        <v>7.9561999999999999</v>
-      </c>
-      <c r="G31" s="2">
-        <v>3.9839000000000002</v>
-      </c>
-      <c r="H31" s="2">
-        <v>1310.7</v>
-      </c>
-      <c r="I31" s="2">
-        <v>4972.3999999999996</v>
-      </c>
-      <c r="J31" s="2">
-        <v>3.6442999999999999</v>
-      </c>
-      <c r="K31" s="2">
-        <v>9.6707000000000001</v>
-      </c>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A32" s="13"/>
-      <c r="B32" s="16"/>
-      <c r="C32" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="D32" s="2">
-        <v>11.394</v>
-      </c>
-      <c r="E32" s="2">
-        <v>13.887</v>
-      </c>
-      <c r="F32" s="2">
-        <v>7.532</v>
-      </c>
-      <c r="G32" s="2">
-        <v>3.5691000000000002</v>
-      </c>
-      <c r="H32" s="2">
-        <v>1581.2</v>
-      </c>
-      <c r="I32" s="2">
-        <v>1959.8</v>
-      </c>
-      <c r="J32" s="2">
-        <v>4.4120999999999997</v>
-      </c>
-      <c r="K32" s="2">
-        <v>8.5846999999999998</v>
-      </c>
-    </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A33" s="13"/>
-      <c r="B33" s="16"/>
-      <c r="C33" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="D33" s="4">
-        <v>5.6656000000000004</v>
-      </c>
-      <c r="E33" s="4">
-        <v>7.6356999999999999</v>
-      </c>
-      <c r="F33" s="4">
-        <v>9.1336999999999993</v>
-      </c>
-      <c r="G33" s="4">
-        <v>4.3000999999999996</v>
-      </c>
-      <c r="H33" s="4">
-        <v>1055.4000000000001</v>
-      </c>
-      <c r="I33" s="4">
-        <v>3494.5</v>
-      </c>
-      <c r="J33" s="4">
-        <v>3.9628999999999999</v>
-      </c>
-      <c r="K33" s="4">
-        <v>11.622999999999999</v>
-      </c>
-    </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A34" s="13"/>
-      <c r="B34" s="16"/>
-      <c r="C34" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="D34" s="2">
-        <v>15.177</v>
-      </c>
-      <c r="E34" s="2">
-        <v>64.875</v>
-      </c>
-      <c r="F34" s="2">
-        <v>1.1737</v>
-      </c>
-      <c r="G34" s="2">
-        <v>3.2002999999999999</v>
-      </c>
-      <c r="H34" s="2">
-        <v>2165.3000000000002</v>
-      </c>
-      <c r="I34" s="2">
-        <v>2320.3000000000002</v>
-      </c>
-      <c r="J34" s="2">
-        <v>4.1947999999999999</v>
-      </c>
-      <c r="K34" s="2">
-        <v>6.7274000000000003</v>
-      </c>
-    </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A35" s="13"/>
-      <c r="B35" s="16"/>
-      <c r="C35" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="D35" s="4">
-        <v>8.0267999999999997</v>
-      </c>
-      <c r="E35" s="4">
-        <v>28.899000000000001</v>
-      </c>
-      <c r="F35" s="4">
-        <v>2.5811000000000002</v>
-      </c>
-      <c r="G35" s="4">
-        <v>4.0179999999999998</v>
-      </c>
-      <c r="H35" s="4">
-        <v>1213.4000000000001</v>
-      </c>
-      <c r="I35" s="2">
-        <v>1698.5</v>
-      </c>
-      <c r="J35" s="2">
-        <v>4.5711000000000004</v>
-      </c>
-      <c r="K35" s="2">
-        <v>7.3220999999999998</v>
-      </c>
-    </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A36" s="13"/>
-      <c r="B36" s="16"/>
-      <c r="C36" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="D36" s="4">
-        <v>8.0846</v>
-      </c>
-      <c r="E36" s="4">
-        <v>21.623000000000001</v>
-      </c>
-      <c r="F36" s="4">
-        <v>4.9984999999999999</v>
-      </c>
-      <c r="G36" s="4">
-        <v>3.8734000000000002</v>
-      </c>
-      <c r="H36" s="4">
-        <v>1330.8</v>
-      </c>
-      <c r="I36" s="4">
-        <v>2586.3000000000002</v>
-      </c>
-      <c r="J36" s="4">
-        <v>4.0925000000000002</v>
-      </c>
-      <c r="K36" s="4">
-        <v>6.8217999999999996</v>
-      </c>
-    </row>
-    <row r="37" spans="1:12" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="14"/>
-      <c r="B37" s="17"/>
-      <c r="C37" s="7"/>
-      <c r="L37" s="11"/>
-    </row>
-    <row r="38" spans="1:12" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="12">
-        <v>900</v>
-      </c>
-      <c r="B38" s="15" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A39" s="13"/>
-      <c r="B39" s="16"/>
-      <c r="C39" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="D39" s="4">
-        <v>8.7007999999999992</v>
-      </c>
-      <c r="E39" s="4">
-        <v>379.67</v>
-      </c>
-      <c r="F39" s="4">
-        <v>0.15739</v>
-      </c>
-      <c r="G39" s="4">
-        <v>4.2165999999999997</v>
-      </c>
-      <c r="H39" s="4">
-        <v>994.53</v>
-      </c>
-      <c r="I39" s="4">
-        <v>1533.4</v>
-      </c>
-      <c r="J39" s="4">
-        <v>4.6802000000000001</v>
-      </c>
-      <c r="K39" s="4">
-        <v>7.0461</v>
-      </c>
-    </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A40" s="13"/>
-      <c r="B40" s="16"/>
-      <c r="C40" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="D40" s="2">
-        <v>9.3439999999999994</v>
-      </c>
-      <c r="E40" s="2">
-        <v>45.972000000000001</v>
-      </c>
-      <c r="F40" s="2">
-        <v>2.5375000000000001</v>
-      </c>
-      <c r="G40" s="2">
-        <v>3.4094000000000002</v>
-      </c>
-      <c r="H40" s="2">
-        <v>1902</v>
-      </c>
-      <c r="I40" s="2">
-        <v>2101.5</v>
-      </c>
-      <c r="J40" s="2">
-        <v>4.3022</v>
-      </c>
-      <c r="K40" s="2">
-        <v>6.1081000000000003</v>
-      </c>
-    </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A41" s="13"/>
-      <c r="B41" s="16"/>
-      <c r="C41" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="D41" s="2">
-        <v>3.0011000000000001</v>
-      </c>
-      <c r="E41" s="2">
-        <v>18.974</v>
-      </c>
-      <c r="F41" s="2">
-        <v>32.389000000000003</v>
-      </c>
-      <c r="G41" s="2">
-        <v>3.2721</v>
-      </c>
-      <c r="H41" s="2">
-        <v>2021.2</v>
-      </c>
-      <c r="I41" s="2">
-        <v>2356.1999999999998</v>
-      </c>
-      <c r="J41" s="2">
-        <v>4.4100999999999999</v>
-      </c>
-      <c r="K41" s="2">
-        <v>17.539000000000001</v>
-      </c>
-    </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A42" s="13"/>
-      <c r="B42" s="16"/>
-      <c r="C42" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="D42" s="2">
-        <v>2.1263000000000001</v>
-      </c>
-      <c r="E42" s="2">
-        <v>19.571000000000002</v>
-      </c>
-      <c r="F42" s="2">
-        <v>18.852</v>
-      </c>
-      <c r="G42" s="2">
-        <v>3.3525</v>
-      </c>
-      <c r="H42" s="2">
-        <v>1999.6</v>
-      </c>
-      <c r="I42" s="2">
-        <v>2639.8</v>
-      </c>
-      <c r="J42" s="2">
-        <v>4.3577000000000004</v>
-      </c>
-      <c r="K42" s="2">
-        <v>21.824999999999999</v>
-      </c>
-    </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A43" s="13"/>
-      <c r="B43" s="16"/>
-      <c r="C43" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="D43" s="2">
-        <v>16.257000000000001</v>
-      </c>
-      <c r="E43" s="2">
-        <v>181.45</v>
-      </c>
-      <c r="F43" s="2">
-        <v>0.50260000000000005</v>
-      </c>
-      <c r="G43" s="2">
-        <v>3.0154000000000001</v>
-      </c>
-      <c r="H43" s="2">
-        <v>2606.1999999999998</v>
-      </c>
-      <c r="I43" s="2">
-        <v>2445.1</v>
-      </c>
-      <c r="J43" s="2">
-        <v>4.1307</v>
-      </c>
-      <c r="K43" s="2">
-        <v>5.6963999999999997</v>
-      </c>
-    </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A44" s="13"/>
-      <c r="B44" s="16"/>
-      <c r="C44" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="D44" s="2">
-        <v>9.5314999999999994</v>
-      </c>
-      <c r="E44" s="2">
-        <v>149.26</v>
-      </c>
-      <c r="F44" s="2">
-        <v>0.37325999999999998</v>
-      </c>
-      <c r="G44" s="2">
-        <v>3.9582000000000002</v>
-      </c>
-      <c r="H44" s="2">
-        <v>1254.5999999999999</v>
-      </c>
-      <c r="I44" s="2">
-        <v>2014.8</v>
-      </c>
-      <c r="J44" s="2">
-        <v>4.3853999999999997</v>
-      </c>
-      <c r="K44" s="2">
-        <v>8.0510999999999999</v>
-      </c>
-    </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A45" s="13"/>
-      <c r="B45" s="16"/>
-      <c r="C45" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="D45" s="2">
-        <v>6.4694000000000003</v>
-      </c>
-      <c r="E45" s="2">
-        <v>149.62</v>
-      </c>
-      <c r="F45" s="2">
-        <v>0.29610999999999998</v>
-      </c>
-      <c r="G45" s="2">
-        <v>4.1942000000000004</v>
-      </c>
-      <c r="H45" s="2">
-        <v>1123.8</v>
-      </c>
-      <c r="I45" s="2">
-        <v>2045.9</v>
-      </c>
-      <c r="J45" s="2">
-        <v>4.4272</v>
-      </c>
-      <c r="K45" s="2">
-        <v>9.5322999999999993</v>
-      </c>
-    </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A46" s="13"/>
-      <c r="B46" s="16"/>
-      <c r="C46" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="D46" s="2">
-        <v>12.617000000000001</v>
-      </c>
-      <c r="E46" s="2">
-        <v>119.8</v>
-      </c>
-      <c r="F46" s="2">
-        <v>0.37544</v>
-      </c>
-      <c r="G46" s="2">
-        <v>3.7416</v>
-      </c>
-      <c r="H46" s="2">
-        <v>1366.4</v>
-      </c>
-      <c r="I46" s="2">
-        <v>1894.5</v>
-      </c>
-      <c r="J46" s="2">
-        <v>4.5370999999999997</v>
-      </c>
-      <c r="K46" s="2">
-        <v>9.6135999999999999</v>
-      </c>
-    </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A47" s="13"/>
-      <c r="B47" s="16"/>
-      <c r="C47" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="D47" s="4">
-        <v>11.849</v>
-      </c>
-      <c r="E47" s="4">
-        <v>272.72000000000003</v>
-      </c>
-      <c r="F47" s="4">
-        <v>0.21346999999999999</v>
-      </c>
-      <c r="G47" s="4">
-        <v>3.8447</v>
-      </c>
-      <c r="H47" s="4">
-        <v>1238.3</v>
-      </c>
-      <c r="I47" s="4">
-        <v>1731</v>
-      </c>
-      <c r="J47" s="4">
-        <v>4.5635000000000003</v>
-      </c>
-      <c r="K47" s="4">
-        <v>7.4757999999999996</v>
-      </c>
-    </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A48" s="13"/>
-      <c r="B48" s="16"/>
-      <c r="C48" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="D48" s="4">
-        <v>7.9996999999999998</v>
-      </c>
-      <c r="E48" s="4">
-        <v>25.007999999999999</v>
-      </c>
-      <c r="F48" s="4">
-        <v>2.2597</v>
-      </c>
-      <c r="G48" s="4">
-        <v>4.1269999999999998</v>
-      </c>
-      <c r="H48" s="4">
-        <v>1102.2</v>
-      </c>
-      <c r="I48" s="2">
-        <v>1841.7</v>
-      </c>
-      <c r="J48" s="2">
-        <v>4.5534999999999997</v>
-      </c>
-      <c r="K48" s="2">
-        <v>10.206</v>
-      </c>
-    </row>
-    <row r="49" spans="1:12" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="14"/>
-      <c r="B49" s="17"/>
-      <c r="C49" s="7"/>
-      <c r="L49" s="11"/>
-    </row>
-    <row r="50" spans="1:12" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="12">
-        <v>1000</v>
-      </c>
-      <c r="B50" s="15" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A51" s="13"/>
-      <c r="B51" s="16"/>
-      <c r="C51" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="D51" s="4">
-        <v>1.9302999999999999</v>
-      </c>
-      <c r="E51" s="4">
-        <v>413.72</v>
-      </c>
-      <c r="F51" s="4">
-        <v>2.4257999999999998E-2</v>
-      </c>
-      <c r="G51" s="4">
-        <v>4.1744000000000003</v>
-      </c>
-      <c r="H51" s="4">
-        <v>720.53</v>
-      </c>
-      <c r="I51" s="4">
-        <v>3740</v>
-      </c>
-      <c r="J51" s="4">
-        <v>3.2875000000000001</v>
-      </c>
-      <c r="K51" s="4">
-        <v>7.5471000000000004</v>
-      </c>
-    </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A52" s="13"/>
-      <c r="B52" s="16"/>
-      <c r="C52" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="D52" s="4">
-        <v>3.7450000000000001</v>
-      </c>
-      <c r="E52" s="4">
-        <v>5.5084999999999997</v>
-      </c>
-      <c r="F52" s="4">
-        <v>10.981999999999999</v>
-      </c>
-      <c r="G52" s="4">
-        <v>3.9323000000000001</v>
-      </c>
-      <c r="H52" s="4">
-        <v>723.41</v>
-      </c>
-      <c r="I52" s="4">
-        <v>9445.2999999999993</v>
-      </c>
-      <c r="J52" s="4">
-        <v>2.7645</v>
-      </c>
-      <c r="K52" s="4">
-        <v>5.3007</v>
-      </c>
-    </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A53" s="13"/>
-      <c r="B53" s="16"/>
-      <c r="C53" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="D53" s="4">
-        <v>1.0051000000000001</v>
-      </c>
-      <c r="E53" s="4">
-        <v>41.567999999999998</v>
-      </c>
-      <c r="F53" s="4">
-        <v>0.50309999999999999</v>
-      </c>
-      <c r="G53" s="4">
-        <v>4.4626000000000001</v>
-      </c>
-      <c r="H53" s="4">
-        <v>582.32000000000005</v>
-      </c>
-      <c r="I53" s="4">
-        <v>2413</v>
-      </c>
-      <c r="J53" s="4">
-        <v>3.508</v>
-      </c>
-      <c r="K53" s="4">
-        <v>6.1177999999999999</v>
-      </c>
-    </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A54" s="13"/>
-      <c r="B54" s="16"/>
-      <c r="C54" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="D54" s="4">
-        <v>0.34182000000000001</v>
-      </c>
-      <c r="E54" s="4">
-        <v>3.0001000000000002</v>
-      </c>
-      <c r="F54" s="4">
-        <v>2.6158000000000001</v>
-      </c>
-      <c r="G54" s="4">
-        <v>4.5224000000000002</v>
-      </c>
-      <c r="H54" s="4">
-        <v>605.76</v>
-      </c>
-      <c r="I54" s="4">
-        <v>9686.9</v>
-      </c>
-      <c r="J54" s="4">
-        <v>2.8176999999999999</v>
-      </c>
-      <c r="K54" s="4">
-        <v>7.5712000000000002</v>
-      </c>
-    </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A55" s="13"/>
-      <c r="B55" s="16"/>
-      <c r="C55" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="D55" s="4">
-        <v>0.74811000000000005</v>
-      </c>
-      <c r="E55" s="4">
-        <v>4.8129999999999997</v>
-      </c>
-      <c r="F55" s="4">
-        <v>1.5203</v>
-      </c>
-      <c r="G55" s="4">
-        <v>4.5427</v>
-      </c>
-      <c r="H55" s="4">
-        <v>578.84</v>
-      </c>
-      <c r="I55" s="4">
-        <v>5902.3</v>
-      </c>
-      <c r="J55" s="4">
-        <v>3.0358000000000001</v>
-      </c>
-      <c r="K55" s="4">
-        <v>7.2228000000000003</v>
-      </c>
-    </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A56" s="13"/>
-      <c r="B56" s="16"/>
-      <c r="C56" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="D56" s="4">
-        <v>2.2985000000000002</v>
-      </c>
-      <c r="E56" s="4">
-        <v>17.765000000000001</v>
-      </c>
-      <c r="F56" s="4">
-        <v>0.53407000000000004</v>
-      </c>
-      <c r="G56" s="4">
-        <v>4.1894999999999998</v>
-      </c>
-      <c r="H56" s="4">
-        <v>695.87</v>
-      </c>
-      <c r="I56" s="4">
-        <v>4582.3999999999996</v>
-      </c>
-      <c r="J56" s="4">
-        <v>3.1497999999999999</v>
-      </c>
-      <c r="K56" s="4">
-        <v>6.8537999999999997</v>
-      </c>
-    </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A57" s="13"/>
-      <c r="B57" s="16"/>
-      <c r="C57" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="D57" s="4">
-        <v>1.7064999999999999</v>
-      </c>
-      <c r="E57" s="4">
-        <v>2.9634999999999998</v>
-      </c>
-      <c r="F57" s="4">
-        <v>8.5671999999999997</v>
-      </c>
-      <c r="G57" s="4">
-        <v>4.2396000000000003</v>
-      </c>
-      <c r="H57" s="4">
-        <v>648.58000000000004</v>
-      </c>
-      <c r="I57" s="4">
-        <v>9968.2000000000007</v>
-      </c>
-      <c r="J57" s="4">
-        <v>2.8411</v>
-      </c>
-      <c r="K57" s="4">
-        <v>9.9029000000000007</v>
-      </c>
-    </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A58" s="13"/>
-      <c r="B58" s="16"/>
-      <c r="C58" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="D58" s="4">
-        <v>1.2569999999999999</v>
-      </c>
-      <c r="E58" s="4">
-        <v>4.6817000000000002</v>
-      </c>
-      <c r="F58" s="4">
-        <v>6.5932000000000004</v>
-      </c>
-      <c r="G58" s="4">
-        <v>4.2586000000000004</v>
-      </c>
-      <c r="H58" s="4">
-        <v>671.09</v>
-      </c>
-      <c r="I58" s="4">
-        <v>9375.2000000000007</v>
-      </c>
-      <c r="J58" s="4">
-        <v>2.7982999999999998</v>
-      </c>
-      <c r="K58" s="4">
-        <v>6.5297000000000001</v>
-      </c>
-    </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A59" s="13"/>
-      <c r="B59" s="16"/>
-      <c r="C59" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="D59" s="4">
-        <v>0.54088000000000003</v>
-      </c>
-      <c r="E59" s="4">
-        <v>3.4417</v>
-      </c>
-      <c r="F59" s="4">
-        <v>3.8666</v>
-      </c>
-      <c r="G59" s="4">
-        <v>4.4062000000000001</v>
-      </c>
-      <c r="H59" s="4">
-        <v>640.30999999999995</v>
-      </c>
-      <c r="I59" s="4">
-        <v>9914.9</v>
-      </c>
-      <c r="J59" s="4">
-        <v>2.8043999999999998</v>
-      </c>
-      <c r="K59" s="4">
-        <v>7.6501999999999999</v>
-      </c>
-    </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A60" s="13"/>
-      <c r="B60" s="16"/>
-      <c r="C60" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="D60" s="4">
-        <v>2.9771999999999998</v>
-      </c>
-      <c r="E60" s="4">
-        <v>13.58</v>
-      </c>
-      <c r="F60" s="4">
-        <v>2.2099000000000002</v>
-      </c>
-      <c r="G60" s="4">
-        <v>4.0601000000000003</v>
-      </c>
-      <c r="H60" s="4">
-        <v>697.13</v>
-      </c>
-      <c r="I60" s="4">
-        <v>2654.7</v>
-      </c>
-      <c r="J60" s="4">
-        <v>3.4464999999999999</v>
-      </c>
-      <c r="K60" s="4">
-        <v>5.4966999999999997</v>
-      </c>
-    </row>
-    <row r="61" spans="1:12" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="14"/>
-      <c r="B61" s="17"/>
-      <c r="C61" s="7"/>
-      <c r="L61" s="11"/>
-    </row>
-    <row r="62" spans="1:12" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="12">
-        <v>1000</v>
-      </c>
-      <c r="B62" s="15" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A63" s="13"/>
-      <c r="B63" s="16"/>
-      <c r="C63" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="D63" s="4">
-        <v>4.6173000000000004E-3</v>
-      </c>
-      <c r="E63" s="4">
-        <v>6.8475999999999999</v>
-      </c>
-      <c r="F63" s="4">
-        <v>2.2387000000000001</v>
-      </c>
-      <c r="G63" s="4">
-        <v>4.8326000000000002</v>
-      </c>
-      <c r="H63" s="4">
-        <v>460.38</v>
-      </c>
-      <c r="I63" s="4">
-        <v>2357.9</v>
-      </c>
-      <c r="J63" s="4">
-        <v>3.5989</v>
-      </c>
-      <c r="K63" s="4">
-        <v>6.8921999999999999</v>
-      </c>
-    </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A64" s="13"/>
-      <c r="B64" s="16"/>
-      <c r="C64" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="D64" s="4">
-        <v>3.1901000000000002</v>
-      </c>
-      <c r="E64" s="4">
-        <v>126.5</v>
-      </c>
-      <c r="F64" s="4">
-        <v>0.16925000000000001</v>
-      </c>
-      <c r="G64" s="4">
-        <v>3.8923999999999999</v>
-      </c>
-      <c r="H64" s="4">
-        <v>802.2</v>
-      </c>
-      <c r="I64" s="4">
-        <v>2253.9</v>
-      </c>
-      <c r="J64" s="4">
-        <v>3.6876000000000002</v>
-      </c>
-      <c r="K64" s="4">
-        <v>11.145</v>
-      </c>
-    </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A65" s="13"/>
-      <c r="B65" s="16"/>
-      <c r="C65" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="D65" s="4">
-        <v>0.31556000000000001</v>
-      </c>
-      <c r="E65" s="4">
-        <v>4.9177</v>
-      </c>
-      <c r="F65" s="4">
-        <v>4.2816000000000001</v>
-      </c>
-      <c r="G65" s="4">
-        <v>4.8133999999999997</v>
-      </c>
-      <c r="H65" s="4">
-        <v>468.63</v>
-      </c>
-      <c r="I65" s="4">
-        <v>3308.8</v>
-      </c>
-      <c r="J65" s="4">
-        <v>3.3386999999999998</v>
-      </c>
-      <c r="K65" s="4">
-        <v>5.7804000000000002</v>
-      </c>
-    </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A66" s="13"/>
-      <c r="B66" s="16"/>
-      <c r="C66" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="D66" s="4">
-        <v>0.26189000000000001</v>
-      </c>
-      <c r="E66" s="4">
-        <v>37.661999999999999</v>
-      </c>
-      <c r="F66" s="4">
-        <v>0.20133999999999999</v>
-      </c>
-      <c r="G66" s="4">
-        <v>4.8079000000000001</v>
-      </c>
-      <c r="H66" s="4">
-        <v>478.84</v>
-      </c>
-      <c r="I66" s="4">
-        <v>2939.9</v>
-      </c>
-      <c r="J66" s="4">
-        <v>3.4262000000000001</v>
-      </c>
-      <c r="K66" s="4">
-        <v>5.9608999999999996</v>
-      </c>
-    </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A67" s="13"/>
-      <c r="B67" s="16"/>
-      <c r="C67" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="D67" s="4">
-        <v>1.5331999999999999</v>
-      </c>
-      <c r="E67" s="4">
-        <v>6.9652000000000003</v>
-      </c>
-      <c r="F67" s="4">
-        <v>4.9490999999999996</v>
-      </c>
-      <c r="G67" s="4">
-        <v>4.3071999999999999</v>
-      </c>
-      <c r="H67" s="4">
-        <v>551.01</v>
-      </c>
-      <c r="I67" s="4">
-        <v>1467.1</v>
-      </c>
-      <c r="J67" s="4">
-        <v>4.0639000000000003</v>
-      </c>
-      <c r="K67" s="4">
-        <v>13.561</v>
-      </c>
-    </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A68" s="13"/>
-      <c r="B68" s="16"/>
-      <c r="C68" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="D68" s="4">
-        <v>0.18711</v>
-      </c>
-      <c r="E68" s="4">
-        <v>42.057000000000002</v>
-      </c>
-      <c r="F68" s="4">
-        <v>1.22</v>
-      </c>
-      <c r="G68" s="4">
-        <v>3.9495</v>
-      </c>
-      <c r="H68" s="4">
-        <v>803.58</v>
-      </c>
-      <c r="I68" s="4">
-        <v>1759.6</v>
-      </c>
-      <c r="J68" s="4">
-        <v>3.8088000000000002</v>
-      </c>
-      <c r="K68" s="4">
-        <v>6.9718</v>
-      </c>
-    </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A69" s="13"/>
-      <c r="B69" s="16"/>
-      <c r="C69" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="D69" s="4">
-        <v>3.4416000000000002</v>
-      </c>
-      <c r="E69" s="4">
-        <v>6.2590000000000003</v>
-      </c>
-      <c r="F69" s="4">
-        <v>1.3140000000000001</v>
-      </c>
-      <c r="G69" s="4">
-        <v>4.0781999999999998</v>
-      </c>
-      <c r="H69" s="4">
-        <v>707.11</v>
-      </c>
-      <c r="I69" s="4">
-        <v>4504.6000000000004</v>
-      </c>
-      <c r="J69" s="4">
-        <v>3.2162000000000002</v>
-      </c>
-      <c r="K69" s="4">
-        <v>8.2904</v>
-      </c>
-    </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A70" s="13"/>
-      <c r="B70" s="16"/>
-      <c r="C70" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="D70" s="4">
-        <v>4.5324999999999998</v>
-      </c>
-      <c r="E70" s="4">
-        <v>14.166</v>
-      </c>
-      <c r="F70" s="4">
-        <v>2.2204999999999999</v>
-      </c>
-      <c r="G70" s="4">
-        <v>3.8813</v>
-      </c>
-      <c r="H70" s="4">
-        <v>731.02</v>
-      </c>
-      <c r="I70" s="4">
-        <v>2379.1</v>
-      </c>
-      <c r="J70" s="4">
-        <v>3.5503999999999998</v>
-      </c>
-      <c r="K70" s="4">
-        <v>6.0315000000000003</v>
-      </c>
-    </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A71" s="13"/>
-      <c r="B71" s="16"/>
-      <c r="C71" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="D71" s="4">
-        <v>3.3203</v>
-      </c>
-      <c r="E71" s="4">
-        <v>95.748000000000005</v>
-      </c>
-      <c r="F71" s="4">
-        <v>0.45551999999999998</v>
-      </c>
-      <c r="G71" s="4">
-        <v>4.0633999999999997</v>
-      </c>
-      <c r="H71" s="4">
-        <v>574.87</v>
-      </c>
-      <c r="I71" s="4">
-        <v>1034.8</v>
-      </c>
-      <c r="J71" s="4">
-        <v>4.2290999999999999</v>
-      </c>
-      <c r="K71" s="4">
-        <v>6.0321999999999996</v>
-      </c>
-    </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A72" s="13"/>
-      <c r="B72" s="16"/>
-      <c r="C72" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="D72" s="4">
-        <v>4.0854999999999997</v>
-      </c>
-      <c r="E72" s="4">
-        <v>246.68</v>
-      </c>
-      <c r="F72" s="4">
-        <v>8.4526000000000004E-2</v>
-      </c>
-      <c r="G72" s="4">
-        <v>3.9321000000000002</v>
-      </c>
-      <c r="H72" s="4">
-        <v>776.2</v>
-      </c>
-      <c r="I72" s="4">
-        <v>2681.7</v>
-      </c>
-      <c r="J72" s="4">
-        <v>3.4426000000000001</v>
-      </c>
-      <c r="K72" s="4">
-        <v>5.5305</v>
-      </c>
-    </row>
-    <row r="73" spans="1:12" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="14"/>
-      <c r="B73" s="17"/>
-      <c r="C73" s="7"/>
-      <c r="L73" s="11"/>
-    </row>
-    <row r="74" spans="1:12" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D75" s="4">
-        <f>MAX(D1:D71)</f>
-        <v>38.180999999999997</v>
-      </c>
-      <c r="E75" s="4">
-        <f t="shared" ref="E75:K75" si="0">MAX(E1:E71)</f>
-        <v>522.85</v>
-      </c>
-      <c r="F75" s="4">
-        <f t="shared" si="0"/>
-        <v>32.389000000000003</v>
-      </c>
-      <c r="G75" s="4">
-        <f t="shared" si="0"/>
-        <v>4.8326000000000002</v>
-      </c>
-      <c r="H75" s="4">
-        <f t="shared" si="0"/>
-        <v>3154.4</v>
-      </c>
-      <c r="I75" s="4">
-        <f t="shared" si="0"/>
-        <v>9968.2000000000007</v>
-      </c>
-      <c r="J75" s="4">
-        <f t="shared" si="0"/>
-        <v>5.6638000000000002</v>
-      </c>
-      <c r="K75" s="4">
-        <f t="shared" si="0"/>
-        <v>21.824999999999999</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="12">
-    <mergeCell ref="A38:A49"/>
-    <mergeCell ref="B38:B49"/>
-    <mergeCell ref="A50:A61"/>
-    <mergeCell ref="B50:B61"/>
-    <mergeCell ref="A62:A73"/>
-    <mergeCell ref="B62:B73"/>
-    <mergeCell ref="A2:A13"/>
-    <mergeCell ref="B2:B13"/>
-    <mergeCell ref="A14:A25"/>
-    <mergeCell ref="B14:B25"/>
-    <mergeCell ref="A26:A37"/>
-    <mergeCell ref="B26:B37"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{666CFF77-8976-439D-A33C-D7841D6EB88F}">
   <dimension ref="A1:O73"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C44" sqref="C44"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="Z34" sqref="P30:Z34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8410,18 +8410,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A2:A13"/>
+    <mergeCell ref="B2:B13"/>
+    <mergeCell ref="A14:A25"/>
+    <mergeCell ref="B14:B25"/>
+    <mergeCell ref="A26:A37"/>
+    <mergeCell ref="B26:B37"/>
     <mergeCell ref="A38:A49"/>
     <mergeCell ref="B38:B49"/>
     <mergeCell ref="A50:A61"/>
     <mergeCell ref="B50:B61"/>
     <mergeCell ref="A62:A73"/>
     <mergeCell ref="B62:B73"/>
-    <mergeCell ref="A2:A13"/>
-    <mergeCell ref="B2:B13"/>
-    <mergeCell ref="A14:A25"/>
-    <mergeCell ref="B14:B25"/>
-    <mergeCell ref="A26:A37"/>
-    <mergeCell ref="B26:B37"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -8433,8 +8433,8 @@
   <dimension ref="A1:O73"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H53" sqref="H53"/>
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F41" sqref="A26:F49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8837,18 +8837,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A2:A13"/>
+    <mergeCell ref="B2:B13"/>
+    <mergeCell ref="A14:A25"/>
+    <mergeCell ref="B14:B25"/>
+    <mergeCell ref="A26:A37"/>
+    <mergeCell ref="B26:B37"/>
     <mergeCell ref="A38:A49"/>
     <mergeCell ref="B38:B49"/>
     <mergeCell ref="A50:A61"/>
     <mergeCell ref="B50:B61"/>
     <mergeCell ref="A62:A73"/>
     <mergeCell ref="B62:B73"/>
-    <mergeCell ref="A2:A13"/>
-    <mergeCell ref="B2:B13"/>
-    <mergeCell ref="A14:A25"/>
-    <mergeCell ref="B14:B25"/>
-    <mergeCell ref="A26:A37"/>
-    <mergeCell ref="B26:B37"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -8859,9 +8859,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1D987DC-5A74-4932-B56A-48A4420F0E95}">
   <dimension ref="A1:Z73"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Z5" sqref="P3:Z5"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G53" sqref="G53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9431,7 +9431,7 @@
         <v>5.4309000000000003</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" s="13"/>
       <c r="B17" s="16"/>
       <c r="C17" s="8" t="s">
@@ -9471,7 +9471,7 @@
         <v>2.6692999999999998</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" s="13"/>
       <c r="B18" s="16"/>
       <c r="C18" s="8" t="s">
@@ -9511,7 +9511,7 @@
         <v>2.7772999999999999</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19" s="13"/>
       <c r="B19" s="16"/>
       <c r="C19" s="8" t="s">
@@ -9551,7 +9551,7 @@
         <v>2.5131999999999999</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20" s="13"/>
       <c r="B20" s="16"/>
       <c r="C20" s="8" t="s">
@@ -9591,7 +9591,7 @@
         <v>2.3424999999999998</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21" s="13"/>
       <c r="B21" s="16"/>
       <c r="C21" s="8" t="s">
@@ -9631,7 +9631,7 @@
         <v>2.8479999999999999</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A22" s="13"/>
       <c r="B22" s="16"/>
       <c r="C22" s="8" t="s">
@@ -9671,7 +9671,7 @@
         <v>3.9527000000000001</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A23" s="13"/>
       <c r="B23" s="16"/>
       <c r="C23" s="8" t="s">
@@ -9711,7 +9711,7 @@
         <v>2.6208</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A24" s="13"/>
       <c r="B24" s="16"/>
       <c r="C24" s="8" t="s">
@@ -9751,14 +9751,14 @@
         <v>2.7280000000000002</v>
       </c>
     </row>
-    <row r="25" spans="1:15" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:17" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="14"/>
       <c r="B25" s="17"/>
       <c r="C25" s="7"/>
       <c r="N25" s="6"/>
       <c r="O25" s="11"/>
     </row>
-    <row r="26" spans="1:15" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:17" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="12">
         <v>900</v>
       </c>
@@ -9766,7 +9766,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A27" s="13"/>
       <c r="B27" s="16"/>
       <c r="C27" s="8" t="s">
@@ -9806,7 +9806,7 @@
         <v>2.5308000000000002</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A28" s="13"/>
       <c r="B28" s="16"/>
       <c r="C28" s="8" t="s">
@@ -9845,8 +9845,9 @@
       <c r="N28" s="1">
         <v>3.4904999999999999</v>
       </c>
-    </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q28" s="9"/>
+    </row>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A29" s="13"/>
       <c r="B29" s="16"/>
       <c r="C29" s="8" t="s">
@@ -9886,7 +9887,7 @@
         <v>2.4437000000000002</v>
       </c>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A30" s="13"/>
       <c r="B30" s="16"/>
       <c r="C30" s="8" t="s">
@@ -9926,7 +9927,7 @@
         <v>3.3180999999999998</v>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A31" s="13"/>
       <c r="B31" s="16"/>
       <c r="C31" s="8" t="s">
@@ -9966,7 +9967,7 @@
         <v>3.0926</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A32" s="13"/>
       <c r="B32" s="16"/>
       <c r="C32" s="8" t="s">
@@ -10700,18 +10701,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A2:A13"/>
+    <mergeCell ref="B2:B13"/>
+    <mergeCell ref="A14:A25"/>
+    <mergeCell ref="B14:B25"/>
+    <mergeCell ref="A26:A37"/>
+    <mergeCell ref="B26:B37"/>
     <mergeCell ref="A38:A49"/>
     <mergeCell ref="B38:B49"/>
     <mergeCell ref="A50:A61"/>
     <mergeCell ref="B50:B61"/>
     <mergeCell ref="A62:A73"/>
     <mergeCell ref="B62:B73"/>
-    <mergeCell ref="A2:A13"/>
-    <mergeCell ref="B2:B13"/>
-    <mergeCell ref="A14:A25"/>
-    <mergeCell ref="B14:B25"/>
-    <mergeCell ref="A26:A37"/>
-    <mergeCell ref="B26:B37"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -11174,18 +11175,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A38:A49"/>
+    <mergeCell ref="B38:B49"/>
+    <mergeCell ref="A50:A61"/>
+    <mergeCell ref="B50:B61"/>
+    <mergeCell ref="A62:A73"/>
+    <mergeCell ref="B62:B73"/>
     <mergeCell ref="A2:A13"/>
     <mergeCell ref="B2:B13"/>
     <mergeCell ref="A14:A25"/>
     <mergeCell ref="B14:B25"/>
     <mergeCell ref="A26:A37"/>
     <mergeCell ref="B26:B37"/>
-    <mergeCell ref="A38:A49"/>
-    <mergeCell ref="B38:B49"/>
-    <mergeCell ref="A50:A61"/>
-    <mergeCell ref="B50:B61"/>
-    <mergeCell ref="A62:A73"/>
-    <mergeCell ref="B62:B73"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
Added new results; minor changes to model
</commit_message>
<xml_diff>
--- a/scripts/__other__/__sem__.xlsx
+++ b/scripts/__other__/__sem__.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Janzen\Desktop\code\moga_neml\scripts\__other__\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48165A81-6C03-4340-BD6F-CF3500050DE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2387290B-5866-4931-A162-452FCE8E5678}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="436" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="452" uniqueCount="50">
   <si>
     <t>temp</t>
   </si>
@@ -187,6 +187,9 @@
   </si>
   <si>
     <t>6; 6</t>
+  </si>
+  <si>
+    <t>5; 7</t>
   </si>
 </sst>
 </file>
@@ -7284,8 +7287,8 @@
   <dimension ref="A1:O73"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D6" sqref="D6:N6"/>
+      <pane ySplit="1" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C44" sqref="C44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7515,6 +7518,9 @@
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="13"/>
       <c r="B7" s="16"/>
+      <c r="C7" s="8" t="s">
+        <v>47</v>
+      </c>
       <c r="D7" s="2">
         <v>4.1862000000000004</v>
       </c>
@@ -7530,12 +7536,24 @@
       <c r="H7" s="2">
         <v>1574.3</v>
       </c>
-      <c r="I7" s="2"/>
-      <c r="J7" s="2"/>
-      <c r="K7" s="2"/>
-      <c r="L7" s="2"/>
-      <c r="M7" s="2"/>
-      <c r="N7" s="2"/>
+      <c r="I7" s="2">
+        <v>58.988999999999997</v>
+      </c>
+      <c r="J7" s="2">
+        <v>353.89</v>
+      </c>
+      <c r="K7" s="2">
+        <v>203.49</v>
+      </c>
+      <c r="L7" s="2">
+        <v>837.33</v>
+      </c>
+      <c r="M7" s="2">
+        <v>2.0440999999999998</v>
+      </c>
+      <c r="N7" s="2">
+        <v>1.5337000000000001</v>
+      </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="13"/>
@@ -7650,34 +7668,202 @@
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="13"/>
       <c r="B15" s="16"/>
+      <c r="C15" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="D15" s="4">
+        <v>31.327000000000002</v>
+      </c>
+      <c r="E15" s="4">
+        <v>104.92</v>
+      </c>
+      <c r="F15" s="4">
+        <v>0.8548</v>
+      </c>
+      <c r="G15" s="4">
+        <v>3.7507999999999999</v>
+      </c>
+      <c r="H15" s="4">
+        <v>2575.8000000000002</v>
+      </c>
+      <c r="I15" s="4">
+        <v>54.389000000000003</v>
+      </c>
+      <c r="J15" s="4">
+        <v>332.02</v>
+      </c>
+      <c r="K15" s="4">
+        <v>305.08</v>
+      </c>
+      <c r="L15" s="4">
+        <v>649.63</v>
+      </c>
+      <c r="M15" s="4">
+        <v>1.9968999999999999</v>
+      </c>
+      <c r="N15" s="3">
+        <v>6.8034999999999997</v>
+      </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="13"/>
       <c r="B16" s="16"/>
-      <c r="I16" s="2"/>
-      <c r="J16" s="2"/>
-      <c r="K16" s="2"/>
-      <c r="L16" s="2"/>
-      <c r="M16" s="2"/>
-      <c r="N16" s="2"/>
+      <c r="C16" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D16" s="4">
+        <v>22.393000000000001</v>
+      </c>
+      <c r="E16" s="4">
+        <v>462.57</v>
+      </c>
+      <c r="F16" s="4">
+        <v>0.13572999999999999</v>
+      </c>
+      <c r="G16" s="4">
+        <v>4.3140000000000001</v>
+      </c>
+      <c r="H16" s="4">
+        <v>1828.1</v>
+      </c>
+      <c r="I16" s="2">
+        <v>39.270000000000003</v>
+      </c>
+      <c r="J16" s="2">
+        <v>260.64999999999998</v>
+      </c>
+      <c r="K16" s="2">
+        <v>413.34</v>
+      </c>
+      <c r="L16" s="2">
+        <v>811.22</v>
+      </c>
+      <c r="M16" s="2">
+        <v>1.9452</v>
+      </c>
+      <c r="N16" s="2">
+        <v>6.8817000000000004</v>
+      </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" s="13"/>
       <c r="B17" s="16"/>
-      <c r="I17" s="2"/>
-      <c r="J17" s="2"/>
-      <c r="K17" s="2"/>
-      <c r="L17" s="2"/>
-      <c r="M17" s="2"/>
-      <c r="N17" s="2"/>
+      <c r="C17" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D17" s="4">
+        <v>11.45</v>
+      </c>
+      <c r="E17" s="4">
+        <v>53.151000000000003</v>
+      </c>
+      <c r="F17" s="4">
+        <v>7.1665999999999999</v>
+      </c>
+      <c r="G17" s="4">
+        <v>3.9502000000000002</v>
+      </c>
+      <c r="H17" s="4">
+        <v>2221.6</v>
+      </c>
+      <c r="I17" s="2">
+        <v>30.864000000000001</v>
+      </c>
+      <c r="J17" s="2">
+        <v>224.62</v>
+      </c>
+      <c r="K17" s="2">
+        <v>344.66</v>
+      </c>
+      <c r="L17" s="2">
+        <v>727.88</v>
+      </c>
+      <c r="M17" s="2">
+        <v>1.3496999999999999</v>
+      </c>
+      <c r="N17" s="2">
+        <v>5.9263000000000003</v>
+      </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" s="13"/>
       <c r="B18" s="16"/>
+      <c r="C18" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="D18" s="4">
+        <v>37.741999999999997</v>
+      </c>
+      <c r="E18" s="4">
+        <v>49.122999999999998</v>
+      </c>
+      <c r="F18" s="4">
+        <v>2.4996</v>
+      </c>
+      <c r="G18" s="4">
+        <v>3.4102000000000001</v>
+      </c>
+      <c r="H18" s="4">
+        <v>3172</v>
+      </c>
+      <c r="I18" s="4">
+        <v>47.05</v>
+      </c>
+      <c r="J18" s="4">
+        <v>308.45999999999998</v>
+      </c>
+      <c r="K18" s="4">
+        <v>233.67</v>
+      </c>
+      <c r="L18" s="4">
+        <v>544.38</v>
+      </c>
+      <c r="M18" s="4">
+        <v>1.665</v>
+      </c>
+      <c r="N18" s="3">
+        <v>14.12</v>
+      </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" s="13"/>
       <c r="B19" s="16"/>
+      <c r="C19" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="D19" s="4">
+        <v>18.768000000000001</v>
+      </c>
+      <c r="E19" s="4">
+        <v>89.18</v>
+      </c>
+      <c r="F19" s="4">
+        <v>0.88068999999999997</v>
+      </c>
+      <c r="G19" s="4">
+        <v>4.5054999999999996</v>
+      </c>
+      <c r="H19" s="4">
+        <v>1677.4</v>
+      </c>
+      <c r="I19" s="4">
+        <v>50.14</v>
+      </c>
+      <c r="J19" s="4">
+        <v>314.23</v>
+      </c>
+      <c r="K19" s="4">
+        <v>237.66</v>
+      </c>
+      <c r="L19" s="4">
+        <v>763.31</v>
+      </c>
+      <c r="M19" s="4">
+        <v>2.0076999999999998</v>
+      </c>
+      <c r="N19" s="3">
+        <v>2.4095</v>
+      </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" s="13"/>
@@ -7717,28 +7903,202 @@
     <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27" s="13"/>
       <c r="B27" s="16"/>
+      <c r="C27" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="D27" s="4">
+        <v>4.8710000000000004</v>
+      </c>
+      <c r="E27" s="4">
+        <v>11.518000000000001</v>
+      </c>
+      <c r="F27" s="4">
+        <v>7.0281000000000002</v>
+      </c>
+      <c r="G27" s="4">
+        <v>4.2420999999999998</v>
+      </c>
+      <c r="H27" s="4">
+        <v>1138.3</v>
+      </c>
+      <c r="I27" s="4">
+        <v>70.744</v>
+      </c>
+      <c r="J27" s="4">
+        <v>372.25</v>
+      </c>
+      <c r="K27" s="4">
+        <v>129.19999999999999</v>
+      </c>
+      <c r="L27" s="4">
+        <v>799.23</v>
+      </c>
+      <c r="M27" s="4">
+        <v>1.5445</v>
+      </c>
+      <c r="N27" s="3">
+        <v>1.9850000000000001</v>
+      </c>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28" s="13"/>
       <c r="B28" s="16"/>
-      <c r="I28" s="2"/>
-      <c r="J28" s="2"/>
-      <c r="K28" s="2"/>
-      <c r="L28" s="2"/>
-      <c r="M28" s="2"/>
-      <c r="N28" s="2"/>
+      <c r="C28" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="D28" s="4">
+        <v>10.692</v>
+      </c>
+      <c r="E28" s="4">
+        <v>29.068000000000001</v>
+      </c>
+      <c r="F28" s="4">
+        <v>2.9830999999999999</v>
+      </c>
+      <c r="G28" s="4">
+        <v>3.7277999999999998</v>
+      </c>
+      <c r="H28" s="4">
+        <v>1433.5</v>
+      </c>
+      <c r="I28" s="2">
+        <v>46.429000000000002</v>
+      </c>
+      <c r="J28" s="2">
+        <v>238.5</v>
+      </c>
+      <c r="K28" s="2">
+        <v>687.68</v>
+      </c>
+      <c r="L28" s="2">
+        <v>627.48</v>
+      </c>
+      <c r="M28" s="2">
+        <v>2.7423000000000002</v>
+      </c>
+      <c r="N28" s="2">
+        <v>6.5118</v>
+      </c>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29" s="13"/>
       <c r="B29" s="16"/>
+      <c r="C29" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="D29" s="4">
+        <v>11.2</v>
+      </c>
+      <c r="E29" s="4">
+        <v>24.262</v>
+      </c>
+      <c r="F29" s="4">
+        <v>2.2614999999999998</v>
+      </c>
+      <c r="G29" s="4">
+        <v>3.9651000000000001</v>
+      </c>
+      <c r="H29" s="4">
+        <v>1163</v>
+      </c>
+      <c r="I29" s="4">
+        <v>115.27</v>
+      </c>
+      <c r="J29" s="4">
+        <v>524.64</v>
+      </c>
+      <c r="K29" s="4">
+        <v>490</v>
+      </c>
+      <c r="L29" s="4">
+        <v>846.07</v>
+      </c>
+      <c r="M29" s="4">
+        <v>2.387</v>
+      </c>
+      <c r="N29" s="3">
+        <v>15.609</v>
+      </c>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30" s="13"/>
       <c r="B30" s="16"/>
+      <c r="C30" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="D30" s="4">
+        <v>11.208</v>
+      </c>
+      <c r="E30" s="4">
+        <v>16.738</v>
+      </c>
+      <c r="F30" s="4">
+        <v>5.9587000000000003</v>
+      </c>
+      <c r="G30" s="4">
+        <v>3.6377000000000002</v>
+      </c>
+      <c r="H30" s="4">
+        <v>1530.1</v>
+      </c>
+      <c r="I30" s="4">
+        <v>35.195999999999998</v>
+      </c>
+      <c r="J30" s="4">
+        <v>206.85</v>
+      </c>
+      <c r="K30" s="4">
+        <v>120.11</v>
+      </c>
+      <c r="L30" s="4">
+        <v>774.72</v>
+      </c>
+      <c r="M30" s="4">
+        <v>1.494</v>
+      </c>
+      <c r="N30" s="3">
+        <v>2.7056</v>
+      </c>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A31" s="13"/>
       <c r="B31" s="16"/>
+      <c r="C31" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="D31" s="4">
+        <v>10.45</v>
+      </c>
+      <c r="E31" s="4">
+        <v>14.769</v>
+      </c>
+      <c r="F31" s="4">
+        <v>7.8792</v>
+      </c>
+      <c r="G31" s="4">
+        <v>3.54</v>
+      </c>
+      <c r="H31" s="4">
+        <v>1787.3</v>
+      </c>
+      <c r="I31" s="4">
+        <v>106.76</v>
+      </c>
+      <c r="J31" s="4">
+        <v>463.71</v>
+      </c>
+      <c r="K31" s="4">
+        <v>840.87</v>
+      </c>
+      <c r="L31" s="4">
+        <v>946.44</v>
+      </c>
+      <c r="M31" s="4">
+        <v>2.4241000000000001</v>
+      </c>
+      <c r="N31" s="3">
+        <v>11.114000000000001</v>
+      </c>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A32" s="13"/>
@@ -7778,34 +8138,202 @@
     <row r="39" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A39" s="13"/>
       <c r="B39" s="16"/>
+      <c r="C39" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="D39" s="4">
+        <v>4.8238000000000003</v>
+      </c>
+      <c r="E39" s="4">
+        <v>378.86</v>
+      </c>
+      <c r="F39" s="4">
+        <v>0.14230000000000001</v>
+      </c>
+      <c r="G39" s="4">
+        <v>4.4020999999999999</v>
+      </c>
+      <c r="H39" s="4">
+        <v>1006.9</v>
+      </c>
+      <c r="I39" s="4">
+        <v>44.823</v>
+      </c>
+      <c r="J39" s="4">
+        <v>247.59</v>
+      </c>
+      <c r="K39" s="4">
+        <v>621.83000000000004</v>
+      </c>
+      <c r="L39" s="4">
+        <v>914.87</v>
+      </c>
+      <c r="M39" s="4">
+        <v>2.4657</v>
+      </c>
+      <c r="N39" s="3">
+        <v>6.7609000000000004</v>
+      </c>
     </row>
     <row r="40" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A40" s="13"/>
       <c r="B40" s="16"/>
-      <c r="I40" s="2"/>
-      <c r="J40" s="2"/>
-      <c r="K40" s="2"/>
-      <c r="L40" s="2"/>
-      <c r="M40" s="2"/>
-      <c r="N40" s="2"/>
+      <c r="C40" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="D40" s="4">
+        <v>7.1036999999999999</v>
+      </c>
+      <c r="E40" s="4">
+        <v>48.234999999999999</v>
+      </c>
+      <c r="F40" s="4">
+        <v>4.2972000000000001</v>
+      </c>
+      <c r="G40" s="4">
+        <v>3.4083999999999999</v>
+      </c>
+      <c r="H40" s="4">
+        <v>1829.9</v>
+      </c>
+      <c r="I40" s="2">
+        <v>148.52000000000001</v>
+      </c>
+      <c r="J40" s="2">
+        <v>657.13</v>
+      </c>
+      <c r="K40" s="2">
+        <v>264.14999999999998</v>
+      </c>
+      <c r="L40" s="2">
+        <v>989.31</v>
+      </c>
+      <c r="M40" s="2">
+        <v>1.6649</v>
+      </c>
+      <c r="N40" s="2">
+        <v>1.0629</v>
+      </c>
     </row>
     <row r="41" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A41" s="13"/>
       <c r="B41" s="16"/>
-      <c r="I41" s="2"/>
-      <c r="J41" s="2"/>
-      <c r="K41" s="2"/>
-      <c r="L41" s="2"/>
-      <c r="M41" s="2"/>
-      <c r="N41" s="1"/>
+      <c r="C41" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="D41" s="4">
+        <v>3.0461</v>
+      </c>
+      <c r="E41" s="4">
+        <v>19.608000000000001</v>
+      </c>
+      <c r="F41" s="4">
+        <v>32.420999999999999</v>
+      </c>
+      <c r="G41" s="4">
+        <v>3.2736000000000001</v>
+      </c>
+      <c r="H41" s="4">
+        <v>2022.3</v>
+      </c>
+      <c r="I41" s="2">
+        <v>48.951999999999998</v>
+      </c>
+      <c r="J41" s="2">
+        <v>279.77999999999997</v>
+      </c>
+      <c r="K41" s="2">
+        <v>171.94</v>
+      </c>
+      <c r="L41" s="2">
+        <v>971.33</v>
+      </c>
+      <c r="M41" s="2">
+        <v>2.0947</v>
+      </c>
+      <c r="N41" s="1">
+        <v>5.125</v>
+      </c>
     </row>
     <row r="42" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A42" s="13"/>
       <c r="B42" s="16"/>
+      <c r="C42" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="D42" s="4">
+        <v>4.6340000000000003</v>
+      </c>
+      <c r="E42" s="4">
+        <v>18.606999999999999</v>
+      </c>
+      <c r="F42" s="4">
+        <v>24.896000000000001</v>
+      </c>
+      <c r="G42" s="4">
+        <v>3.3435999999999999</v>
+      </c>
+      <c r="H42" s="4">
+        <v>1999.7</v>
+      </c>
+      <c r="I42" s="4">
+        <v>25.863</v>
+      </c>
+      <c r="J42" s="4">
+        <v>156.41</v>
+      </c>
+      <c r="K42" s="4">
+        <v>502.72</v>
+      </c>
+      <c r="L42" s="4">
+        <v>948.08</v>
+      </c>
+      <c r="M42" s="4">
+        <v>2.2551999999999999</v>
+      </c>
+      <c r="N42" s="3">
+        <v>18.103000000000002</v>
+      </c>
     </row>
     <row r="43" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A43" s="13"/>
       <c r="B43" s="16"/>
+      <c r="C43" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="D43" s="4">
+        <v>16.286999999999999</v>
+      </c>
+      <c r="E43" s="4">
+        <v>181.45</v>
+      </c>
+      <c r="F43" s="4">
+        <v>0.52517000000000003</v>
+      </c>
+      <c r="G43" s="4">
+        <v>3.0160999999999998</v>
+      </c>
+      <c r="H43" s="4">
+        <v>2606.1999999999998</v>
+      </c>
+      <c r="I43" s="4">
+        <v>29.887</v>
+      </c>
+      <c r="J43" s="4">
+        <v>171.78</v>
+      </c>
+      <c r="K43" s="4">
+        <v>434.24</v>
+      </c>
+      <c r="L43" s="4">
+        <v>894.26</v>
+      </c>
+      <c r="M43" s="4">
+        <v>2.1920000000000002</v>
+      </c>
+      <c r="N43" s="3">
+        <v>2.8378000000000001</v>
+      </c>
     </row>
     <row r="44" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A44" s="13"/>

</xml_diff>

<commit_message>
Minor changes throughout repo
</commit_message>
<xml_diff>
--- a/scripts/__other__/__sem__.xlsx
+++ b/scripts/__other__/__sem__.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Janzen\Desktop\code\moga_neml\scripts\__other__\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unsw-my.sharepoint.com/personal/z5208868_ad_unsw_edu_au/Documents/Desktop/code/moga_neml/scripts/__other__/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4867B082-3585-4B5A-8192-6FFC53AB41B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="5" documentId="13_ncr:1_{4867B082-3585-4B5A-8192-6FFC53AB41B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F5741C39-42CB-4156-AF9B-8DB26B2E0108}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="evp" sheetId="13" r:id="rId1"/>
@@ -18,7 +18,6 @@
     <sheet name="evp-cd_i" sheetId="17" r:id="rId3"/>
     <sheet name="evp-wd_f" sheetId="20" r:id="rId4"/>
     <sheet name="evp-wd_i" sheetId="18" r:id="rId5"/>
-    <sheet name="evp-wd_i_2" sheetId="22" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="47">
   <si>
     <t>temp</t>
   </si>
@@ -1120,23 +1119,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4D7A15E-4182-42F6-82DA-99E9B04906BA}">
   <dimension ref="A1:K37"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J31" sqref="J31"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C27" sqref="C27:G36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="4"/>
-    <col min="2" max="2" width="15.7109375" style="8" customWidth="1"/>
-    <col min="3" max="6" width="9.140625" style="4"/>
-    <col min="7" max="7" width="9.140625" style="3"/>
-    <col min="8" max="8" width="15.7109375" style="9" customWidth="1"/>
-    <col min="9" max="11" width="15.7109375" style="8" customWidth="1"/>
-    <col min="12" max="16384" width="9.140625" style="4"/>
+    <col min="1" max="1" width="9.1796875" style="4"/>
+    <col min="2" max="2" width="15.7265625" style="8" customWidth="1"/>
+    <col min="3" max="6" width="9.1796875" style="4"/>
+    <col min="7" max="7" width="9.1796875" style="3"/>
+    <col min="8" max="8" width="15.7265625" style="9" customWidth="1"/>
+    <col min="9" max="11" width="15.7265625" style="8" customWidth="1"/>
+    <col min="12" max="16384" width="9.1796875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -1171,12 +1170,12 @@
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" ht="5.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="12">
         <v>800</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" s="13"/>
       <c r="B3" s="8" t="s">
         <v>15</v>
@@ -1206,7 +1205,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" s="13"/>
       <c r="B4" s="8" t="s">
         <v>15</v>
@@ -1236,7 +1235,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5" s="13"/>
       <c r="B5" s="8" t="s">
         <v>17</v>
@@ -1266,7 +1265,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" s="13"/>
       <c r="B6" s="8" t="s">
         <v>19</v>
@@ -1296,7 +1295,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7" s="13"/>
       <c r="B7" s="8" t="s">
         <v>15</v>
@@ -1326,7 +1325,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8" s="13"/>
       <c r="B8" s="8" t="s">
         <v>20</v>
@@ -1356,7 +1355,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9" s="13"/>
       <c r="B9" s="8" t="s">
         <v>16</v>
@@ -1386,7 +1385,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A10" s="13"/>
       <c r="B10" s="8" t="s">
         <v>16</v>
@@ -1416,7 +1415,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A11" s="13"/>
       <c r="B11" s="8" t="s">
         <v>21</v>
@@ -1446,7 +1445,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A12" s="13"/>
       <c r="B12" s="8" t="s">
         <v>21</v>
@@ -1476,7 +1475,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="13" spans="1:11" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" s="5" customFormat="1" ht="5.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="14"/>
       <c r="B13" s="7"/>
       <c r="G13" s="6"/>
@@ -1485,12 +1484,12 @@
       <c r="J13" s="7"/>
       <c r="K13" s="7"/>
     </row>
-    <row r="14" spans="1:11" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" ht="5.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="12">
         <v>900</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A15" s="13"/>
       <c r="B15" s="8" t="s">
         <v>15</v>
@@ -1520,7 +1519,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A16" s="13"/>
       <c r="B16" s="8" t="s">
         <v>15</v>
@@ -1550,7 +1549,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A17" s="13"/>
       <c r="B17" s="8" t="s">
         <v>15</v>
@@ -1580,7 +1579,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A18" s="13"/>
       <c r="B18" s="8" t="s">
         <v>17</v>
@@ -1610,7 +1609,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A19" s="13"/>
       <c r="B19" s="8" t="s">
         <v>18</v>
@@ -1640,7 +1639,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A20" s="13"/>
       <c r="B20" s="8" t="s">
         <v>18</v>
@@ -1670,7 +1669,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A21" s="13"/>
       <c r="B21" s="8" t="s">
         <v>24</v>
@@ -1700,7 +1699,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A22" s="13"/>
       <c r="B22" s="8" t="s">
         <v>28</v>
@@ -1730,7 +1729,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A23" s="13"/>
       <c r="B23" s="8" t="s">
         <v>15</v>
@@ -1760,7 +1759,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A24" s="13"/>
       <c r="B24" s="8" t="s">
         <v>16</v>
@@ -1790,7 +1789,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:11" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" s="5" customFormat="1" ht="5.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="14"/>
       <c r="B25" s="7"/>
       <c r="G25" s="6"/>
@@ -1799,12 +1798,12 @@
       <c r="J25" s="7"/>
       <c r="K25" s="7"/>
     </row>
-    <row r="26" spans="1:11" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" ht="5.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="12">
         <v>1000</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A27" s="13"/>
       <c r="B27" s="8" t="s">
         <v>23</v>
@@ -1831,7 +1830,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A28" s="13"/>
       <c r="B28" s="8" t="s">
         <v>28</v>
@@ -1858,7 +1857,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A29" s="13"/>
       <c r="B29" s="8" t="s">
         <v>23</v>
@@ -1885,7 +1884,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A30" s="13"/>
       <c r="B30" s="8" t="s">
         <v>30</v>
@@ -1912,7 +1911,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A31" s="13"/>
       <c r="B31" s="8" t="s">
         <v>22</v>
@@ -1939,7 +1938,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A32" s="13"/>
       <c r="B32" s="8" t="s">
         <v>28</v>
@@ -1966,7 +1965,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A33" s="13"/>
       <c r="B33" s="8" t="s">
         <v>28</v>
@@ -1993,7 +1992,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A34" s="13"/>
       <c r="B34" s="8" t="s">
         <v>28</v>
@@ -2020,7 +2019,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A35" s="13"/>
       <c r="B35" s="8" t="s">
         <v>28</v>
@@ -2047,7 +2046,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A36" s="13"/>
       <c r="B36" s="8" t="s">
         <v>27</v>
@@ -2074,7 +2073,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="37" spans="1:11" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" s="5" customFormat="1" ht="5.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A37" s="14"/>
       <c r="B37" s="7"/>
       <c r="G37" s="6"/>
@@ -2100,21 +2099,21 @@
   <dimension ref="A1:K37"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C15" sqref="C15:J24"/>
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C15" sqref="C15:J23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="4"/>
-    <col min="2" max="2" width="15.7109375" style="9" customWidth="1"/>
-    <col min="3" max="3" width="9.140625" style="9"/>
-    <col min="4" max="10" width="9.140625" style="4"/>
-    <col min="11" max="11" width="9.140625" style="9"/>
-    <col min="12" max="16384" width="9.140625" style="4"/>
+    <col min="1" max="1" width="9.1796875" style="4"/>
+    <col min="2" max="2" width="15.7265625" style="9" customWidth="1"/>
+    <col min="3" max="3" width="9.1796875" style="9"/>
+    <col min="4" max="10" width="9.1796875" style="4"/>
+    <col min="11" max="11" width="9.1796875" style="9"/>
+    <col min="12" max="16384" width="9.1796875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -2147,12 +2146,12 @@
       </c>
       <c r="K1" s="11"/>
     </row>
-    <row r="2" spans="1:11" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" ht="5.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="12">
         <v>800</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" s="13"/>
       <c r="B3" s="9" t="s">
         <v>28</v>
@@ -2182,7 +2181,7 @@
         <v>6.6364000000000001</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" s="13"/>
       <c r="B4" s="9" t="s">
         <v>24</v>
@@ -2212,7 +2211,7 @@
         <v>6.6859999999999999</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5" s="13"/>
       <c r="B5" s="9" t="s">
         <v>30</v>
@@ -2242,7 +2241,7 @@
         <v>8.4002999999999997</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" s="13"/>
       <c r="B6" s="9" t="s">
         <v>17</v>
@@ -2272,7 +2271,7 @@
         <v>6.5503999999999998</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7" s="13"/>
       <c r="B7" s="9" t="s">
         <v>28</v>
@@ -2302,7 +2301,7 @@
         <v>6.9638999999999998</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8" s="13"/>
       <c r="B8" s="9" t="s">
         <v>28</v>
@@ -2332,7 +2331,7 @@
         <v>4.7172000000000001</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9" s="13"/>
       <c r="B9" s="9" t="s">
         <v>24</v>
@@ -2362,7 +2361,7 @@
         <v>8.5634999999999994</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A10" s="13"/>
       <c r="B10" s="9" t="s">
         <v>30</v>
@@ -2392,7 +2391,7 @@
         <v>6.8597999999999999</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A11" s="13"/>
       <c r="B11" s="9" t="s">
         <v>28</v>
@@ -2422,7 +2421,7 @@
         <v>8.7353000000000005</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A12" s="13"/>
       <c r="B12" s="9" t="s">
         <v>27</v>
@@ -2452,18 +2451,18 @@
         <v>8.5096000000000007</v>
       </c>
     </row>
-    <row r="13" spans="1:11" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" s="5" customFormat="1" ht="5.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="14"/>
       <c r="B13" s="11"/>
       <c r="C13" s="11"/>
       <c r="K13" s="11"/>
     </row>
-    <row r="14" spans="1:11" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" ht="5.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="12">
         <v>900</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A15" s="13"/>
       <c r="B15" s="9" t="s">
         <v>19</v>
@@ -2493,7 +2492,7 @@
         <v>9.6201000000000008</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A16" s="13"/>
       <c r="B16" s="9" t="s">
         <v>17</v>
@@ -2523,7 +2522,7 @@
         <v>7.4964000000000004</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A17" s="13"/>
       <c r="B17" s="9" t="s">
         <v>22</v>
@@ -2553,7 +2552,7 @@
         <v>8.5838000000000001</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A18" s="13"/>
       <c r="B18" s="9" t="s">
         <v>17</v>
@@ -2583,7 +2582,7 @@
         <v>11.773</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A19" s="13"/>
       <c r="B19" s="9" t="s">
         <v>28</v>
@@ -2613,7 +2612,7 @@
         <v>6.8212000000000002</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A20" s="13"/>
       <c r="B20" s="9" t="s">
         <v>26</v>
@@ -2643,7 +2642,7 @@
         <v>6.5256999999999996</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A21" s="13"/>
       <c r="B21" s="9" t="s">
         <v>29</v>
@@ -2673,7 +2672,7 @@
         <v>3.5083000000000002</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A22" s="13"/>
       <c r="B22" s="9" t="s">
         <v>26</v>
@@ -2703,7 +2702,7 @@
         <v>5.8582999999999998</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A23" s="13"/>
       <c r="B23" s="9" t="s">
         <v>20</v>
@@ -2733,7 +2732,7 @@
         <v>6.9904999999999999</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A24" s="13"/>
       <c r="B24" s="9" t="s">
         <v>28</v>
@@ -2763,18 +2762,18 @@
         <v>8.0541</v>
       </c>
     </row>
-    <row r="25" spans="1:11" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" s="5" customFormat="1" ht="5.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="14"/>
       <c r="B25" s="11"/>
       <c r="C25" s="11"/>
       <c r="K25" s="11"/>
     </row>
-    <row r="26" spans="1:11" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" ht="5.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="12">
         <v>1000</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A27" s="13"/>
       <c r="B27" s="9" t="s">
         <v>38</v>
@@ -2804,7 +2803,7 @@
         <v>6.8388</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A28" s="13"/>
       <c r="B28" s="9" t="s">
         <v>25</v>
@@ -2834,7 +2833,7 @@
         <v>6.1744000000000003</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A29" s="13"/>
       <c r="B29" s="9" t="s">
         <v>38</v>
@@ -2864,7 +2863,7 @@
         <v>5.7801999999999998</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A30" s="13"/>
       <c r="B30" s="9" t="s">
         <v>38</v>
@@ -2894,7 +2893,7 @@
         <v>5.9217000000000004</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A31" s="13"/>
       <c r="B31" s="9" t="s">
         <v>37</v>
@@ -2924,7 +2923,7 @@
         <v>7.1360000000000001</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A32" s="13"/>
       <c r="B32" s="9" t="s">
         <v>38</v>
@@ -2954,7 +2953,7 @@
         <v>5.3898000000000001</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A33" s="13"/>
       <c r="B33" s="9" t="s">
         <v>37</v>
@@ -2984,7 +2983,7 @@
         <v>5.6135000000000002</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A34" s="13"/>
       <c r="B34" s="9" t="s">
         <v>37</v>
@@ -3014,7 +3013,7 @@
         <v>7.0132000000000003</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A35" s="13"/>
       <c r="B35" s="9" t="s">
         <v>37</v>
@@ -3044,7 +3043,7 @@
         <v>6.0335999999999999</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A36" s="13"/>
       <c r="B36" s="9" t="s">
         <v>37</v>
@@ -3074,7 +3073,7 @@
         <v>5.8158000000000003</v>
       </c>
     </row>
-    <row r="37" spans="1:11" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" s="5" customFormat="1" ht="5.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A37" s="14"/>
       <c r="B37" s="11"/>
       <c r="C37" s="11"/>
@@ -3095,21 +3094,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF6E341A-51E3-4AF7-809B-A8594B1323BC}">
   <dimension ref="A1:K53"/>
   <sheetViews>
-    <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C41" sqref="C41"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E41" sqref="E41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="4"/>
-    <col min="2" max="2" width="15.7109375" style="8" customWidth="1"/>
-    <col min="3" max="10" width="9.140625" style="4"/>
-    <col min="11" max="11" width="9.140625" style="9"/>
-    <col min="12" max="16384" width="9.140625" style="4"/>
+    <col min="1" max="1" width="9.1796875" style="4"/>
+    <col min="2" max="2" width="15.7265625" style="8" customWidth="1"/>
+    <col min="3" max="10" width="9.1796875" style="4"/>
+    <col min="11" max="11" width="9.1796875" style="9"/>
+    <col min="12" max="16384" width="9.1796875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -3142,12 +3141,12 @@
       </c>
       <c r="K1" s="11"/>
     </row>
-    <row r="2" spans="1:11" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" ht="5.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="12">
         <v>800</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" s="13"/>
       <c r="B3" s="8" t="s">
         <v>19</v>
@@ -3177,7 +3176,7 @@
         <v>13.172000000000001</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" s="13"/>
       <c r="B4" s="8" t="s">
         <v>22</v>
@@ -3207,7 +3206,7 @@
         <v>11.449</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5" s="13"/>
       <c r="B5" s="8" t="s">
         <v>30</v>
@@ -3237,7 +3236,7 @@
         <v>6.8653000000000004</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" s="13"/>
       <c r="B6" s="8" t="s">
         <v>22</v>
@@ -3267,7 +3266,7 @@
         <v>7.7724000000000002</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7" s="13"/>
       <c r="B7" s="8" t="s">
         <v>22</v>
@@ -3297,7 +3296,7 @@
         <v>11.287000000000001</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8" s="13"/>
       <c r="B8" s="8" t="s">
         <v>28</v>
@@ -3327,7 +3326,7 @@
         <v>6.6603000000000003</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9" s="13"/>
       <c r="B9" s="8" t="s">
         <v>30</v>
@@ -3357,7 +3356,7 @@
         <v>8.6950000000000003</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A10" s="13"/>
       <c r="B10" s="8" t="s">
         <v>17</v>
@@ -3387,7 +3386,7 @@
         <v>6.7618999999999998</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A11" s="13"/>
       <c r="B11" s="8" t="s">
         <v>16</v>
@@ -3417,7 +3416,7 @@
         <v>8.5891000000000002</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A12" s="13"/>
       <c r="B12" s="8" t="s">
         <v>30</v>
@@ -3447,17 +3446,17 @@
         <v>10.337</v>
       </c>
     </row>
-    <row r="13" spans="1:11" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" s="5" customFormat="1" ht="5.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="14"/>
       <c r="B13" s="7"/>
       <c r="K13" s="11"/>
     </row>
-    <row r="14" spans="1:11" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" ht="5.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="12">
         <v>900</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A15" s="13"/>
       <c r="B15" s="8" t="s">
         <v>20</v>
@@ -3487,7 +3486,7 @@
         <v>9.1929999999999996</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A16" s="13"/>
       <c r="B16" s="8" t="s">
         <v>17</v>
@@ -3517,7 +3516,7 @@
         <v>7.2249999999999996</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A17" s="13"/>
       <c r="B17" s="8" t="s">
         <v>22</v>
@@ -3547,7 +3546,7 @@
         <v>8.5846999999999998</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A18" s="13"/>
       <c r="B18" s="8" t="s">
         <v>22</v>
@@ -3577,7 +3576,7 @@
         <v>11.622999999999999</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A19" s="13"/>
       <c r="B19" s="8" t="s">
         <v>22</v>
@@ -3607,7 +3606,7 @@
         <v>6.8217999999999996</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A20" s="13"/>
       <c r="B20" s="8" t="s">
         <v>19</v>
@@ -3637,7 +3636,7 @@
         <v>7.0461</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A21" s="13"/>
       <c r="B21" s="8" t="s">
         <v>19</v>
@@ -3667,7 +3666,7 @@
         <v>6.1081000000000003</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A22" s="13"/>
       <c r="B22" s="8" t="s">
         <v>20</v>
@@ -3697,7 +3696,7 @@
         <v>5.6963999999999997</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A23" s="13"/>
       <c r="B23" s="8" t="s">
         <v>20</v>
@@ -3727,7 +3726,7 @@
         <v>9.5322999999999993</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A24" s="13"/>
       <c r="B24" s="8" t="s">
         <v>19</v>
@@ -3757,17 +3756,17 @@
         <v>10.206</v>
       </c>
     </row>
-    <row r="25" spans="1:11" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" s="5" customFormat="1" ht="5.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="14"/>
       <c r="B25" s="7"/>
       <c r="K25" s="11"/>
     </row>
-    <row r="26" spans="1:11" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" ht="5.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="12">
         <v>1000</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A27" s="13"/>
       <c r="B27" s="8" t="s">
         <v>38</v>
@@ -3797,7 +3796,7 @@
         <v>6.8921999999999999</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A28" s="13"/>
       <c r="B28" s="8" t="s">
         <v>37</v>
@@ -3827,7 +3826,7 @@
         <v>11.145</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A29" s="13"/>
       <c r="B29" s="8" t="s">
         <v>25</v>
@@ -3857,7 +3856,7 @@
         <v>5.7804000000000002</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A30" s="13"/>
       <c r="B30" s="8" t="s">
         <v>25</v>
@@ -3887,7 +3886,7 @@
         <v>5.9608999999999996</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A31" s="13"/>
       <c r="B31" s="8" t="s">
         <v>38</v>
@@ -3917,7 +3916,7 @@
         <v>13.561</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A32" s="13"/>
       <c r="B32" s="8" t="s">
         <v>36</v>
@@ -3947,7 +3946,7 @@
         <v>6.9718</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A33" s="13"/>
       <c r="B33" s="8" t="s">
         <v>37</v>
@@ -3977,7 +3976,7 @@
         <v>8.2904</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A34" s="13"/>
       <c r="B34" s="8" t="s">
         <v>37</v>
@@ -4007,7 +4006,7 @@
         <v>6.0315000000000003</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A35" s="13"/>
       <c r="B35" s="8" t="s">
         <v>37</v>
@@ -4037,7 +4036,7 @@
         <v>6.0321999999999996</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A36" s="13"/>
       <c r="B36" s="8" t="s">
         <v>29</v>
@@ -4067,13 +4066,13 @@
         <v>5.5305</v>
       </c>
     </row>
-    <row r="37" spans="1:11" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" s="5" customFormat="1" ht="5.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A37" s="14"/>
       <c r="B37" s="7"/>
       <c r="K37" s="11"/>
     </row>
-    <row r="38" spans="1:11" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" ht="5.15" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A39" s="4">
         <v>800</v>
       </c>
@@ -4113,7 +4112,7 @@
         <v>9.1589000000000009</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B40" s="8" t="s">
         <v>42</v>
       </c>
@@ -4150,7 +4149,7 @@
         <v>8.6420500000000011</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B41" s="8" t="s">
         <v>43</v>
       </c>
@@ -4187,13 +4186,13 @@
         <v>2.2846766914477032</v>
       </c>
     </row>
-    <row r="42" spans="1:11" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:11" s="5" customFormat="1" ht="5.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A42" s="6"/>
       <c r="B42" s="7"/>
       <c r="K42" s="11"/>
     </row>
-    <row r="43" spans="1:11" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:11" ht="5.15" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A44" s="4">
         <v>900</v>
       </c>
@@ -4233,7 +4232,7 @@
         <v>8.20364</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B45" s="8" t="s">
         <v>42</v>
       </c>
@@ -4270,7 +4269,7 @@
         <v>7.9048499999999997</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B46" s="8" t="s">
         <v>43</v>
       </c>
@@ -4307,13 +4306,13 @@
         <v>1.9286006125340347</v>
       </c>
     </row>
-    <row r="47" spans="1:11" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:11" s="5" customFormat="1" ht="5.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A47" s="6"/>
       <c r="B47" s="7"/>
       <c r="K47" s="11"/>
     </row>
-    <row r="48" spans="1:11" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:11" ht="5.15" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A49" s="4">
         <v>1000</v>
       </c>
@@ -4353,7 +4352,7 @@
         <v>7.6195900000000005</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B50" s="8" t="s">
         <v>42</v>
       </c>
@@ -4390,7 +4389,7 @@
         <v>6.4621999999999993</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B51" s="8" t="s">
         <v>43</v>
       </c>
@@ -4427,12 +4426,12 @@
         <v>2.6805386869267696</v>
       </c>
     </row>
-    <row r="52" spans="1:11" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:11" s="5" customFormat="1" ht="5.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A52" s="6"/>
       <c r="B52" s="7"/>
       <c r="K52" s="11"/>
     </row>
-    <row r="53" spans="1:11" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="53" spans="1:11" ht="5.15" customHeight="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="A2:A13"/>
@@ -4448,22 +4447,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{666CFF77-8976-439D-A33C-D7841D6EB88F}">
   <dimension ref="A1:N38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G44" sqref="G44"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L44" sqref="L44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="4"/>
-    <col min="2" max="2" width="15.7109375" style="8" customWidth="1"/>
-    <col min="3" max="12" width="9.140625" style="4"/>
-    <col min="13" max="13" width="9.140625" style="3"/>
-    <col min="14" max="14" width="9.140625" style="9"/>
-    <col min="15" max="16384" width="9.140625" style="4"/>
+    <col min="1" max="1" width="9.1796875" style="4"/>
+    <col min="2" max="2" width="15.7265625" style="8" customWidth="1"/>
+    <col min="3" max="12" width="9.1796875" style="4"/>
+    <col min="13" max="13" width="9.1796875" style="3"/>
+    <col min="14" max="14" width="9.1796875" style="9"/>
+    <col min="15" max="16384" width="9.1796875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -4505,12 +4504,12 @@
       </c>
       <c r="N1" s="11"/>
     </row>
-    <row r="2" spans="1:14" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" ht="5.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="12">
         <v>800</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A3" s="13"/>
       <c r="B3" s="8" t="s">
         <v>28</v>
@@ -4549,7 +4548,7 @@
         <v>2.1873999999999998</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A4" s="13"/>
       <c r="B4" s="8" t="s">
         <v>27</v>
@@ -4588,7 +4587,7 @@
         <v>11.349</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A5" s="13"/>
       <c r="B5" s="8" t="s">
         <v>27</v>
@@ -4627,7 +4626,7 @@
         <v>9.9943000000000008</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A6" s="13"/>
       <c r="B6" s="8" t="s">
         <v>28</v>
@@ -4666,7 +4665,7 @@
         <v>6.8034999999999997</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A7" s="13"/>
       <c r="B7" s="8" t="s">
         <v>22</v>
@@ -4705,7 +4704,7 @@
         <v>6.8817000000000004</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A8" s="13"/>
       <c r="B8" s="8" t="s">
         <v>22</v>
@@ -4744,7 +4743,7 @@
         <v>5.9263000000000003</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A9" s="13"/>
       <c r="B9" s="8" t="s">
         <v>24</v>
@@ -4783,7 +4782,7 @@
         <v>2.4095</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A10" s="13"/>
       <c r="B10" s="8" t="s">
         <v>22</v>
@@ -4822,7 +4821,7 @@
         <v>11.785</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A11" s="13"/>
       <c r="B11" s="8" t="s">
         <v>19</v>
@@ -4861,7 +4860,7 @@
         <v>18.082999999999998</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A12" s="13"/>
       <c r="B12" s="8" t="s">
         <v>28</v>
@@ -4900,18 +4899,18 @@
         <v>19.93</v>
       </c>
     </row>
-    <row r="13" spans="1:14" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" s="5" customFormat="1" ht="5.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="14"/>
       <c r="B13" s="7"/>
       <c r="M13" s="6"/>
       <c r="N13" s="11"/>
     </row>
-    <row r="14" spans="1:14" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" ht="5.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="12">
         <v>900</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A15" s="13"/>
       <c r="B15" s="8" t="s">
         <v>29</v>
@@ -4950,7 +4949,7 @@
         <v>1.9850000000000001</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A16" s="13"/>
       <c r="B16" s="8" t="s">
         <v>30</v>
@@ -4989,7 +4988,7 @@
         <v>2.7056</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A17" s="13"/>
       <c r="B17" s="8" t="s">
         <v>29</v>
@@ -5028,7 +5027,7 @@
         <v>2.3519000000000001</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A18" s="13"/>
       <c r="B18" s="8" t="s">
         <v>39</v>
@@ -5067,7 +5066,7 @@
         <v>2.8494999999999999</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A19" s="13"/>
       <c r="B19" s="8" t="s">
         <v>30</v>
@@ -5106,7 +5105,7 @@
         <v>7.9154</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A20" s="13"/>
       <c r="B20" s="8" t="s">
         <v>27</v>
@@ -5145,7 +5144,7 @@
         <v>6.7609000000000004</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A21" s="13"/>
       <c r="B21" s="8" t="s">
         <v>29</v>
@@ -5184,7 +5183,7 @@
         <v>1.0629</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A22" s="13"/>
       <c r="B22" s="8" t="s">
         <v>36</v>
@@ -5223,7 +5222,7 @@
         <v>2.8378000000000001</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A23" s="13"/>
       <c r="B23" s="8" t="s">
         <v>40</v>
@@ -5262,7 +5261,7 @@
         <v>10.67</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A24" s="13"/>
       <c r="B24" s="8" t="s">
         <v>22</v>
@@ -5301,18 +5300,18 @@
         <v>16.872</v>
       </c>
     </row>
-    <row r="25" spans="1:14" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:14" s="5" customFormat="1" ht="5.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="14"/>
       <c r="B25" s="7"/>
       <c r="M25" s="6"/>
       <c r="N25" s="11"/>
     </row>
-    <row r="26" spans="1:14" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:14" ht="5.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="12">
         <v>1000</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A27" s="13"/>
       <c r="B27" s="8" t="s">
         <v>39</v>
@@ -5351,7 +5350,7 @@
         <v>2.2120000000000002</v>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A28" s="13"/>
       <c r="B28" s="8" t="s">
         <v>46</v>
@@ -5390,7 +5389,7 @@
         <v>1.806</v>
       </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A29" s="13"/>
       <c r="B29" s="8" t="s">
         <v>38</v>
@@ -5429,7 +5428,7 @@
         <v>3.8136000000000001</v>
       </c>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A30" s="13"/>
       <c r="B30" s="8" t="s">
         <v>36</v>
@@ -5468,7 +5467,7 @@
         <v>9.5122999999999998</v>
       </c>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A31" s="13"/>
       <c r="B31" s="8" t="s">
         <v>46</v>
@@ -5507,7 +5506,7 @@
         <v>1.9576</v>
       </c>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A32" s="13"/>
       <c r="B32" s="8" t="s">
         <v>37</v>
@@ -5546,7 +5545,7 @@
         <v>13.461</v>
       </c>
     </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A33" s="13"/>
       <c r="B33" s="8" t="s">
         <v>37</v>
@@ -5585,7 +5584,7 @@
         <v>5.8274999999999997</v>
       </c>
     </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A34" s="13"/>
       <c r="B34" s="8" t="s">
         <v>46</v>
@@ -5624,7 +5623,7 @@
         <v>1.7726</v>
       </c>
     </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A35" s="13"/>
       <c r="B35" s="8" t="s">
         <v>37</v>
@@ -5663,7 +5662,7 @@
         <v>11.635</v>
       </c>
     </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A36" s="13"/>
       <c r="B36" s="8" t="s">
         <v>45</v>
@@ -5702,13 +5701,13 @@
         <v>10.334</v>
       </c>
     </row>
-    <row r="37" spans="1:14" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:14" s="5" customFormat="1" ht="5.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A37" s="14"/>
       <c r="B37" s="7"/>
       <c r="M37" s="6"/>
       <c r="N37" s="11"/>
     </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:14" x14ac:dyDescent="0.35">
       <c r="C38" s="4">
         <f>MAX(C3:C36)</f>
         <v>31.327000000000002</v>
@@ -5769,22 +5768,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F200E048-5FAF-4136-82F6-92204CC50E12}">
   <dimension ref="A1:N37"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J32" sqref="J32"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C15" sqref="C15:M24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="4"/>
-    <col min="2" max="2" width="15.7109375" style="8" customWidth="1"/>
-    <col min="3" max="12" width="9.140625" style="4"/>
-    <col min="13" max="13" width="9.140625" style="3"/>
-    <col min="14" max="14" width="9.140625" style="9"/>
-    <col min="15" max="16384" width="9.140625" style="4"/>
+    <col min="1" max="1" width="9.1796875" style="4"/>
+    <col min="2" max="2" width="15.7265625" style="8" customWidth="1"/>
+    <col min="3" max="12" width="9.1796875" style="4"/>
+    <col min="13" max="13" width="9.1796875" style="3"/>
+    <col min="14" max="14" width="9.1796875" style="9"/>
+    <col min="15" max="16384" width="9.1796875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -5826,12 +5825,12 @@
       </c>
       <c r="N1" s="11"/>
     </row>
-    <row r="2" spans="1:14" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" ht="5.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="12">
         <v>800</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A3" s="13"/>
       <c r="B3" s="8" t="s">
         <v>28</v>
@@ -5870,7 +5869,7 @@
         <v>2.1873999999999998</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A4" s="13"/>
       <c r="B4" s="8" t="s">
         <v>28</v>
@@ -5909,7 +5908,7 @@
         <v>11.411</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A5" s="13"/>
       <c r="B5" s="8" t="s">
         <v>22</v>
@@ -5948,7 +5947,7 @@
         <v>9.9943000000000008</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A6" s="13"/>
       <c r="B6" s="8" t="s">
         <v>19</v>
@@ -5987,7 +5986,7 @@
         <v>6.8034999999999997</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A7" s="13"/>
       <c r="B7" s="8" t="s">
         <v>44</v>
@@ -6026,7 +6025,7 @@
         <v>7.7561999999999998</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A8" s="13"/>
       <c r="B8" s="8" t="s">
         <v>44</v>
@@ -6065,7 +6064,7 @@
         <v>5.8611000000000004</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A9" s="13"/>
       <c r="B9" s="8" t="s">
         <v>22</v>
@@ -6104,7 +6103,7 @@
         <v>2.7730999999999999</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A10" s="13"/>
       <c r="B10" s="8" t="s">
         <v>22</v>
@@ -6143,7 +6142,7 @@
         <v>11.782</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A11" s="13"/>
       <c r="B11" s="8" t="s">
         <v>28</v>
@@ -6182,7 +6181,7 @@
         <v>18.094999999999999</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A12" s="13"/>
       <c r="B12" s="8" t="s">
         <v>28</v>
@@ -6221,18 +6220,18 @@
         <v>19.864000000000001</v>
       </c>
     </row>
-    <row r="13" spans="1:14" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" s="5" customFormat="1" ht="5.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="14"/>
       <c r="B13" s="7"/>
       <c r="M13" s="6"/>
       <c r="N13" s="11"/>
     </row>
-    <row r="14" spans="1:14" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" ht="5.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="12">
         <v>900</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A15" s="13"/>
       <c r="B15" s="8" t="s">
         <v>24</v>
@@ -6271,7 +6270,7 @@
         <v>1.9850000000000001</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A16" s="13"/>
       <c r="B16" s="8" t="s">
         <v>30</v>
@@ -6310,7 +6309,7 @@
         <v>2.5579000000000001</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A17" s="13"/>
       <c r="B17" s="8" t="s">
         <v>24</v>
@@ -6349,7 +6348,7 @@
         <v>2.3565999999999998</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A18" s="13"/>
       <c r="B18" s="8" t="s">
         <v>39</v>
@@ -6388,7 +6387,7 @@
         <v>2.8494999999999999</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A19" s="13"/>
       <c r="B19" s="8" t="s">
         <v>44</v>
@@ -6427,7 +6426,7 @@
         <v>7.9977</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A20" s="13"/>
       <c r="B20" s="8" t="s">
         <v>22</v>
@@ -6466,7 +6465,7 @@
         <v>7.0609000000000002</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A21" s="13"/>
       <c r="B21" s="8" t="s">
         <v>29</v>
@@ -6505,7 +6504,7 @@
         <v>1.0863</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A22" s="13"/>
       <c r="B22" s="8" t="s">
         <v>26</v>
@@ -6544,7 +6543,7 @@
         <v>2.8517999999999999</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A23" s="13"/>
       <c r="B23" s="8" t="s">
         <v>44</v>
@@ -6583,7 +6582,7 @@
         <v>10.568</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A24" s="13"/>
       <c r="B24" s="8" t="s">
         <v>22</v>
@@ -6622,249 +6621,48 @@
         <v>15.843999999999999</v>
       </c>
     </row>
-    <row r="25" spans="1:14" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:14" s="5" customFormat="1" ht="5.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="14"/>
       <c r="B25" s="7"/>
       <c r="M25" s="6"/>
       <c r="N25" s="11"/>
     </row>
-    <row r="26" spans="1:14" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:14" ht="5.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="12">
         <v>1000</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A27" s="13"/>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A28" s="13"/>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A29" s="13"/>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A30" s="13"/>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A31" s="13"/>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A32" s="13"/>
     </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A33" s="13"/>
     </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A34" s="13"/>
     </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A35" s="13"/>
     </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A36" s="13"/>
     </row>
-    <row r="37" spans="1:14" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="14"/>
-      <c r="B37" s="7"/>
-      <c r="M37" s="6"/>
-      <c r="N37" s="11"/>
-    </row>
-  </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="A2:A13"/>
-    <mergeCell ref="A14:A25"/>
-    <mergeCell ref="A26:A37"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE086293-56DA-4DD0-A6F8-91C9D98E51F8}">
-  <dimension ref="A1:N37"/>
-  <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F51" sqref="F51"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="9.140625" style="4"/>
-    <col min="2" max="2" width="15.7109375" style="8" customWidth="1"/>
-    <col min="3" max="12" width="9.140625" style="4"/>
-    <col min="13" max="13" width="9.140625" style="3"/>
-    <col min="14" max="14" width="9.140625" style="9"/>
-    <col min="15" max="16384" width="9.140625" style="4"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="I1" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="J1" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="K1" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="L1" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="M1" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" s="11"/>
-    </row>
-    <row r="2" spans="1:14" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="12">
-        <v>800</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A3" s="13"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
-      <c r="J3" s="2"/>
-      <c r="K3" s="2"/>
-      <c r="L3" s="2"/>
-      <c r="M3" s="1"/>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A4" s="13"/>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A5" s="13"/>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6" s="13"/>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A7" s="13"/>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A8" s="13"/>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A9" s="13"/>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A10" s="13"/>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A11" s="13"/>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A12" s="13"/>
-    </row>
-    <row r="13" spans="1:14" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="14"/>
-      <c r="B13" s="7"/>
-      <c r="M13" s="6"/>
-      <c r="N13" s="11"/>
-    </row>
-    <row r="14" spans="1:14" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="12">
-        <v>900</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A15" s="13"/>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A16" s="13"/>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A17" s="13"/>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A18" s="13"/>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A19" s="13"/>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A20" s="13"/>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A21" s="13"/>
-    </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A22" s="13"/>
-    </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A23" s="13"/>
-    </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A24" s="13"/>
-    </row>
-    <row r="25" spans="1:14" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="14"/>
-      <c r="B25" s="7"/>
-      <c r="M25" s="6"/>
-      <c r="N25" s="11"/>
-    </row>
-    <row r="26" spans="1:14" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="12">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A27" s="13"/>
-    </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A28" s="13"/>
-    </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A29" s="13"/>
-    </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A30" s="13"/>
-    </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A31" s="13"/>
-    </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A32" s="13"/>
-    </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A33" s="13"/>
-    </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A34" s="13"/>
-    </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A35" s="13"/>
-    </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A36" s="13"/>
-    </row>
-    <row r="37" spans="1:14" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:14" s="5" customFormat="1" ht="5.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A37" s="14"/>
       <c r="B37" s="7"/>
       <c r="M37" s="6"/>

</xml_diff>

<commit_message>
minor changes to script
</commit_message>
<xml_diff>
--- a/scripts/__other__/__sem__.xlsx
+++ b/scripts/__other__/__sem__.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Janzen\Desktop\code\moga_neml\scripts\__other__\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3EDBBAA-825F-4794-ADA2-AD34D6A770CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCB17739-7BE1-4ED8-ACDF-CBEB6EA87718}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="evp" sheetId="13" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="44">
   <si>
     <t>temp</t>
   </si>
@@ -163,6 +163,15 @@
   </si>
   <si>
     <t>6; 9</t>
+  </si>
+  <si>
+    <t>mean</t>
+  </si>
+  <si>
+    <t>median</t>
+  </si>
+  <si>
+    <t>stdev</t>
   </si>
 </sst>
 </file>
@@ -734,7 +743,7 @@
     <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -776,6 +785,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1103,7 +1115,7 @@
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J37" sqref="J37"/>
+      <selection pane="bottomLeft" activeCell="C15" sqref="C15:G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3074,11 +3086,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF6E341A-51E3-4AF7-809B-A8594B1323BC}">
-  <dimension ref="A1:K37"/>
+  <dimension ref="A1:K53"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E28" sqref="E28"/>
+    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4052,6 +4064,379 @@
       <c r="A37" s="14"/>
       <c r="B37" s="7"/>
       <c r="K37" s="11"/>
+    </row>
+    <row r="38" spans="1:11" s="15" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B38" s="8"/>
+      <c r="K38" s="9"/>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A39" s="4">
+        <v>800</v>
+      </c>
+      <c r="B39" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="C39" s="4">
+        <f>AVERAGE(C3:C12)</f>
+        <v>22.220990000000004</v>
+      </c>
+      <c r="D39" s="4">
+        <f t="shared" ref="D39:I39" si="0">AVERAGE(D3:D12)</f>
+        <v>137.4033</v>
+      </c>
+      <c r="E39" s="4">
+        <f t="shared" si="0"/>
+        <v>3.2320340000000001</v>
+      </c>
+      <c r="F39" s="4">
+        <f t="shared" si="0"/>
+        <v>4.12073</v>
+      </c>
+      <c r="G39" s="4">
+        <f t="shared" si="0"/>
+        <v>1896.28</v>
+      </c>
+      <c r="H39" s="4">
+        <f t="shared" si="0"/>
+        <v>2482.3599999999997</v>
+      </c>
+      <c r="I39" s="4">
+        <f t="shared" si="0"/>
+        <v>5.2518100000000008</v>
+      </c>
+      <c r="J39" s="4">
+        <f>AVERAGE(J3:J12)</f>
+        <v>9.1589000000000009</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B40" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="C40" s="4">
+        <f>MEDIAN(C3:C12)</f>
+        <v>22.878999999999998</v>
+      </c>
+      <c r="D40" s="4">
+        <f t="shared" ref="D40:J40" si="1">MEDIAN(D3:D12)</f>
+        <v>55.850999999999999</v>
+      </c>
+      <c r="E40" s="4">
+        <f t="shared" si="1"/>
+        <v>1.067205</v>
+      </c>
+      <c r="F40" s="4">
+        <f t="shared" si="1"/>
+        <v>4.1636500000000005</v>
+      </c>
+      <c r="G40" s="4">
+        <f t="shared" si="1"/>
+        <v>1764.8000000000002</v>
+      </c>
+      <c r="H40" s="4">
+        <f t="shared" si="1"/>
+        <v>2167.1</v>
+      </c>
+      <c r="I40" s="4">
+        <f t="shared" si="1"/>
+        <v>5.3214000000000006</v>
+      </c>
+      <c r="J40" s="4">
+        <f t="shared" si="1"/>
+        <v>8.6420500000000011</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B41" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="C41" s="4">
+        <f>STDEV(C3:C12)</f>
+        <v>8.6270644473527298</v>
+      </c>
+      <c r="D41" s="4">
+        <f t="shared" ref="D41:J41" si="2">STDEV(D3:D12)</f>
+        <v>157.56249847462649</v>
+      </c>
+      <c r="E41" s="4">
+        <f t="shared" si="2"/>
+        <v>3.686968927868949</v>
+      </c>
+      <c r="F41" s="4">
+        <f t="shared" si="2"/>
+        <v>0.32557125197276099</v>
+      </c>
+      <c r="G41" s="4">
+        <f t="shared" si="2"/>
+        <v>358.00850020945353</v>
+      </c>
+      <c r="H41" s="4">
+        <f t="shared" si="2"/>
+        <v>727.24026627304477</v>
+      </c>
+      <c r="I41" s="4">
+        <f t="shared" si="2"/>
+        <v>0.37144171503301388</v>
+      </c>
+      <c r="J41" s="4">
+        <f t="shared" si="2"/>
+        <v>2.2846766914477032</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="6"/>
+      <c r="B42" s="7"/>
+      <c r="K42" s="11"/>
+    </row>
+    <row r="43" spans="1:11" s="15" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B43" s="8"/>
+      <c r="K43" s="9"/>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A44" s="4">
+        <v>900</v>
+      </c>
+      <c r="B44" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="C44" s="4">
+        <f>AVERAGE(C15:C24)</f>
+        <v>8.8653300000000019</v>
+      </c>
+      <c r="D44" s="4">
+        <f t="shared" ref="D44:J44" si="3">AVERAGE(D15:D24)</f>
+        <v>85.762870000000007</v>
+      </c>
+      <c r="E44" s="4">
+        <f t="shared" si="3"/>
+        <v>4.03505</v>
+      </c>
+      <c r="F44" s="4">
+        <f t="shared" si="3"/>
+        <v>3.8583600000000002</v>
+      </c>
+      <c r="G44" s="4">
+        <f t="shared" si="3"/>
+        <v>1430.5930000000001</v>
+      </c>
+      <c r="H44" s="4">
+        <f t="shared" si="3"/>
+        <v>2205.8500000000004</v>
+      </c>
+      <c r="I44" s="4">
+        <f t="shared" si="3"/>
+        <v>4.3318500000000002</v>
+      </c>
+      <c r="J44" s="4">
+        <f t="shared" si="3"/>
+        <v>8.20364</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B45" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="C45" s="4">
+        <f>MEDIAN(C15:C24)</f>
+        <v>8.3926999999999996</v>
+      </c>
+      <c r="D45" s="4">
+        <f t="shared" ref="D45:J45" si="4">MEDIAN(D15:D24)</f>
+        <v>23.3155</v>
+      </c>
+      <c r="E45" s="4">
+        <f t="shared" si="4"/>
+        <v>3.7679999999999998</v>
+      </c>
+      <c r="F45" s="4">
+        <f t="shared" si="4"/>
+        <v>4.0001999999999995</v>
+      </c>
+      <c r="G45" s="4">
+        <f t="shared" si="4"/>
+        <v>1234.5</v>
+      </c>
+      <c r="H45" s="4">
+        <f t="shared" si="4"/>
+        <v>2055.1000000000004</v>
+      </c>
+      <c r="I45" s="4">
+        <f t="shared" si="4"/>
+        <v>4.3642500000000002</v>
+      </c>
+      <c r="J45" s="4">
+        <f t="shared" si="4"/>
+        <v>7.9048499999999997</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B46" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="C46" s="4">
+        <f>STDEV(C15:C24)</f>
+        <v>3.5137945453281358</v>
+      </c>
+      <c r="D46" s="4">
+        <f t="shared" ref="D46:J46" si="5">STDEV(D15:D24)</f>
+        <v>120.14545945603741</v>
+      </c>
+      <c r="E46" s="4">
+        <f t="shared" si="5"/>
+        <v>3.3065286137041734</v>
+      </c>
+      <c r="F46" s="4">
+        <f t="shared" si="5"/>
+        <v>0.43466871216287523</v>
+      </c>
+      <c r="G46" s="4">
+        <f t="shared" si="5"/>
+        <v>500.77466261006259</v>
+      </c>
+      <c r="H46" s="4">
+        <f t="shared" si="5"/>
+        <v>538.80317628775742</v>
+      </c>
+      <c r="I46" s="4">
+        <f t="shared" si="5"/>
+        <v>0.21930949845164277</v>
+      </c>
+      <c r="J46" s="4">
+        <f t="shared" si="5"/>
+        <v>1.9286006125340347</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="6"/>
+      <c r="B47" s="7"/>
+      <c r="K47" s="11"/>
+    </row>
+    <row r="48" spans="1:11" s="15" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B48" s="8"/>
+      <c r="K48" s="9"/>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A49" s="4">
+        <v>1000</v>
+      </c>
+      <c r="B49" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="C49" s="4">
+        <f>AVERAGE(C27:C36)</f>
+        <v>2.08723773</v>
+      </c>
+      <c r="D49" s="4">
+        <f t="shared" ref="D49:J49" si="6">AVERAGE(D27:D36)</f>
+        <v>58.780250000000002</v>
+      </c>
+      <c r="E49" s="4">
+        <f t="shared" si="6"/>
+        <v>1.7134536</v>
+      </c>
+      <c r="F49" s="4">
+        <f t="shared" si="6"/>
+        <v>4.2557999999999998</v>
+      </c>
+      <c r="G49" s="4">
+        <f t="shared" si="6"/>
+        <v>635.38400000000001</v>
+      </c>
+      <c r="H49" s="4">
+        <f t="shared" si="6"/>
+        <v>2468.7400000000002</v>
+      </c>
+      <c r="I49" s="4">
+        <f t="shared" si="6"/>
+        <v>3.6362399999999999</v>
+      </c>
+      <c r="J49" s="4">
+        <f t="shared" si="6"/>
+        <v>7.6195900000000005</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B50" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="C50" s="4">
+        <f>MEDIAN(C27:C36)</f>
+        <v>2.36165</v>
+      </c>
+      <c r="D50" s="4">
+        <f t="shared" ref="D50:J50" si="7">MEDIAN(D27:D36)</f>
+        <v>25.914000000000001</v>
+      </c>
+      <c r="E50" s="4">
+        <f t="shared" si="7"/>
+        <v>1.2669999999999999</v>
+      </c>
+      <c r="F50" s="4">
+        <f t="shared" si="7"/>
+        <v>4.0708000000000002</v>
+      </c>
+      <c r="G50" s="4">
+        <f t="shared" si="7"/>
+        <v>640.99</v>
+      </c>
+      <c r="H50" s="4">
+        <f t="shared" si="7"/>
+        <v>2368.5</v>
+      </c>
+      <c r="I50" s="4">
+        <f t="shared" si="7"/>
+        <v>3.5746500000000001</v>
+      </c>
+      <c r="J50" s="4">
+        <f t="shared" si="7"/>
+        <v>6.4621999999999993</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B51" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="C51" s="4">
+        <f>STDEV(C27:C36)</f>
+        <v>1.8033577306391468</v>
+      </c>
+      <c r="D51" s="4">
+        <f t="shared" ref="D51:J51" si="8">STDEV(D27:D36)</f>
+        <v>78.185271093349527</v>
+      </c>
+      <c r="E51" s="4">
+        <f t="shared" si="8"/>
+        <v>1.7290870227327868</v>
+      </c>
+      <c r="F51" s="4">
+        <f t="shared" si="8"/>
+        <v>0.40695933184751742</v>
+      </c>
+      <c r="G51" s="4">
+        <f t="shared" si="8"/>
+        <v>142.96764134275682</v>
+      </c>
+      <c r="H51" s="4">
+        <f t="shared" si="8"/>
+        <v>985.82135320982172</v>
+      </c>
+      <c r="I51" s="4">
+        <f t="shared" si="8"/>
+        <v>0.32009209508098346</v>
+      </c>
+      <c r="J51" s="4">
+        <f t="shared" si="8"/>
+        <v>2.6805386869267696</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="6"/>
+      <c r="B52" s="7"/>
+      <c r="K52" s="11"/>
+    </row>
+    <row r="53" spans="1:11" s="15" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B53" s="8"/>
+      <c r="K53" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -4068,8 +4453,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{666CFF77-8976-439D-A33C-D7841D6EB88F}">
   <dimension ref="A1:N38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="K42" sqref="K42"/>
     </sheetView>
   </sheetViews>
@@ -5186,8 +5571,8 @@
   <dimension ref="A1:N37"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D10" sqref="D10"/>
+      <pane ySplit="1" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A38" sqref="A38:XFD54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
added params for evpwd_i 1000C
</commit_message>
<xml_diff>
--- a/scripts/__other__/__sem__.xlsx
+++ b/scripts/__other__/__sem__.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Janzen\Desktop\code\moga_neml\scripts\__other__\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCB17739-7BE1-4ED8-ACDF-CBEB6EA87718}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4867B082-3585-4B5A-8192-6FFC53AB41B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="evp" sheetId="13" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="evp-cd_i" sheetId="17" r:id="rId3"/>
     <sheet name="evp-wd_f" sheetId="20" r:id="rId4"/>
     <sheet name="evp-wd_i" sheetId="18" r:id="rId5"/>
+    <sheet name="evp-wd_i_2" sheetId="22" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="47">
   <si>
     <t>temp</t>
   </si>
@@ -172,6 +173,15 @@
   </si>
   <si>
     <t>stdev</t>
+  </si>
+  <si>
+    <t>9; 9</t>
+  </si>
+  <si>
+    <t>5; 7</t>
+  </si>
+  <si>
+    <t>4; 7</t>
   </si>
 </sst>
 </file>
@@ -743,7 +753,7 @@
     <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -785,9 +795,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1115,7 +1122,7 @@
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C15" sqref="C15:G24"/>
+      <selection pane="bottomLeft" activeCell="J31" sqref="J31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2093,8 +2100,8 @@
   <dimension ref="A1:K37"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C27" sqref="C27:J36"/>
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C15" sqref="C15:J24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3088,8 +3095,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF6E341A-51E3-4AF7-809B-A8594B1323BC}">
   <dimension ref="A1:K53"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
+    <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>
@@ -4065,10 +4072,7 @@
       <c r="B37" s="7"/>
       <c r="K37" s="11"/>
     </row>
-    <row r="38" spans="1:11" s="15" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B38" s="8"/>
-      <c r="K38" s="9"/>
-    </row>
+    <row r="38" spans="1:11" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" s="4">
         <v>800</v>
@@ -4188,10 +4192,7 @@
       <c r="B42" s="7"/>
       <c r="K42" s="11"/>
     </row>
-    <row r="43" spans="1:11" s="15" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B43" s="8"/>
-      <c r="K43" s="9"/>
-    </row>
+    <row r="43" spans="1:11" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" s="4">
         <v>900</v>
@@ -4311,10 +4312,7 @@
       <c r="B47" s="7"/>
       <c r="K47" s="11"/>
     </row>
-    <row r="48" spans="1:11" s="15" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B48" s="8"/>
-      <c r="K48" s="9"/>
-    </row>
+    <row r="48" spans="1:11" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" s="4">
         <v>1000</v>
@@ -4434,10 +4432,7 @@
       <c r="B52" s="7"/>
       <c r="K52" s="11"/>
     </row>
-    <row r="53" spans="1:11" s="15" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B53" s="8"/>
-      <c r="K53" s="9"/>
-    </row>
+    <row r="53" spans="1:11" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="A2:A13"/>
@@ -4453,9 +4448,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{666CFF77-8976-439D-A33C-D7841D6EB88F}">
   <dimension ref="A1:N38"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K42" sqref="K42"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G44" sqref="G44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5319,6 +5314,9 @@
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" s="13"/>
+      <c r="B27" s="8" t="s">
+        <v>39</v>
+      </c>
       <c r="C27" s="4">
         <v>4.6150000000000002E-3</v>
       </c>
@@ -5334,9 +5332,30 @@
       <c r="G27" s="4">
         <v>460.27</v>
       </c>
+      <c r="H27" s="4">
+        <v>95.944999999999993</v>
+      </c>
+      <c r="I27" s="4">
+        <v>455.06</v>
+      </c>
+      <c r="J27" s="4">
+        <v>144.66999999999999</v>
+      </c>
+      <c r="K27" s="4">
+        <v>804.12</v>
+      </c>
+      <c r="L27" s="4">
+        <v>1.1256999999999999</v>
+      </c>
+      <c r="M27" s="3">
+        <v>2.2120000000000002</v>
+      </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" s="13"/>
+      <c r="B28" s="8" t="s">
+        <v>46</v>
+      </c>
       <c r="C28" s="4">
         <v>3.9207000000000001</v>
       </c>
@@ -5352,15 +5371,30 @@
       <c r="G28" s="4">
         <v>752.32</v>
       </c>
-      <c r="H28" s="2"/>
-      <c r="I28" s="2"/>
-      <c r="J28" s="2"/>
-      <c r="K28" s="2"/>
-      <c r="L28" s="2"/>
-      <c r="M28" s="2"/>
+      <c r="H28" s="2">
+        <v>41.393999999999998</v>
+      </c>
+      <c r="I28" s="2">
+        <v>219.89</v>
+      </c>
+      <c r="J28" s="2">
+        <v>47.171999999999997</v>
+      </c>
+      <c r="K28" s="2">
+        <v>291.43</v>
+      </c>
+      <c r="L28" s="2">
+        <v>4.5823999999999998</v>
+      </c>
+      <c r="M28" s="2">
+        <v>1.806</v>
+      </c>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29" s="13"/>
+      <c r="B29" s="8" t="s">
+        <v>38</v>
+      </c>
       <c r="C29" s="4">
         <v>1.2675000000000001E-2</v>
       </c>
@@ -5376,9 +5410,30 @@
       <c r="G29" s="4">
         <v>471.18</v>
       </c>
+      <c r="H29" s="4">
+        <v>64.659000000000006</v>
+      </c>
+      <c r="I29" s="4">
+        <v>330.07</v>
+      </c>
+      <c r="J29" s="4">
+        <v>176.31</v>
+      </c>
+      <c r="K29" s="4">
+        <v>409.25</v>
+      </c>
+      <c r="L29" s="4">
+        <v>1.6171</v>
+      </c>
+      <c r="M29" s="3">
+        <v>3.8136000000000001</v>
+      </c>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30" s="13"/>
+      <c r="B30" s="8" t="s">
+        <v>36</v>
+      </c>
       <c r="C30" s="4">
         <v>0.26123000000000002</v>
       </c>
@@ -5394,9 +5449,30 @@
       <c r="G30" s="4">
         <v>490.7</v>
       </c>
+      <c r="H30" s="4">
+        <v>6.8769999999999998</v>
+      </c>
+      <c r="I30" s="4">
+        <v>51.307000000000002</v>
+      </c>
+      <c r="J30" s="4">
+        <v>271.39999999999998</v>
+      </c>
+      <c r="K30" s="4">
+        <v>601.54999999999995</v>
+      </c>
+      <c r="L30" s="4">
+        <v>1.5584</v>
+      </c>
+      <c r="M30" s="3">
+        <v>9.5122999999999998</v>
+      </c>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31" s="13"/>
+      <c r="B31" s="8" t="s">
+        <v>46</v>
+      </c>
       <c r="C31" s="4">
         <v>1.4714</v>
       </c>
@@ -5412,9 +5488,30 @@
       <c r="G31" s="4">
         <v>584.77</v>
       </c>
+      <c r="H31" s="4">
+        <v>172.19</v>
+      </c>
+      <c r="I31" s="4">
+        <v>693.66</v>
+      </c>
+      <c r="J31" s="4">
+        <v>175.36</v>
+      </c>
+      <c r="K31" s="4">
+        <v>903.63</v>
+      </c>
+      <c r="L31" s="4">
+        <v>3.9590999999999998</v>
+      </c>
+      <c r="M31" s="3">
+        <v>1.9576</v>
+      </c>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32" s="13"/>
+      <c r="B32" s="8" t="s">
+        <v>37</v>
+      </c>
       <c r="C32" s="4">
         <v>4.1444999999999999</v>
       </c>
@@ -5430,9 +5527,30 @@
       <c r="G32" s="4">
         <v>726.26</v>
       </c>
+      <c r="H32" s="4">
+        <v>111.62</v>
+      </c>
+      <c r="I32" s="4">
+        <v>502.2</v>
+      </c>
+      <c r="J32" s="4">
+        <v>509.49</v>
+      </c>
+      <c r="K32" s="4">
+        <v>969.18</v>
+      </c>
+      <c r="L32" s="4">
+        <v>1.5902000000000001</v>
+      </c>
+      <c r="M32" s="3">
+        <v>13.461</v>
+      </c>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A33" s="13"/>
+      <c r="B33" s="8" t="s">
+        <v>37</v>
+      </c>
       <c r="C33" s="4">
         <v>3.2084999999999999</v>
       </c>
@@ -5448,9 +5566,30 @@
       <c r="G33" s="4">
         <v>697.16</v>
       </c>
+      <c r="H33" s="4">
+        <v>136.85</v>
+      </c>
+      <c r="I33" s="4">
+        <v>584.70000000000005</v>
+      </c>
+      <c r="J33" s="4">
+        <v>669.43</v>
+      </c>
+      <c r="K33" s="4">
+        <v>983.14</v>
+      </c>
+      <c r="L33" s="4">
+        <v>1.6515</v>
+      </c>
+      <c r="M33" s="3">
+        <v>5.8274999999999997</v>
+      </c>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A34" s="13"/>
+      <c r="B34" s="8" t="s">
+        <v>46</v>
+      </c>
       <c r="C34" s="4">
         <v>4.3445999999999998</v>
       </c>
@@ -5466,9 +5605,30 @@
       <c r="G34" s="4">
         <v>776.41</v>
       </c>
+      <c r="H34" s="4">
+        <v>178.93</v>
+      </c>
+      <c r="I34" s="4">
+        <v>713.6</v>
+      </c>
+      <c r="J34" s="4">
+        <v>182.86</v>
+      </c>
+      <c r="K34" s="4">
+        <v>794.32</v>
+      </c>
+      <c r="L34" s="4">
+        <v>7.1326000000000001</v>
+      </c>
+      <c r="M34" s="3">
+        <v>1.7726</v>
+      </c>
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A35" s="13"/>
+      <c r="B35" s="8" t="s">
+        <v>37</v>
+      </c>
       <c r="C35" s="4">
         <v>3.3748</v>
       </c>
@@ -5484,9 +5644,30 @@
       <c r="G35" s="4">
         <v>700.49</v>
       </c>
+      <c r="H35" s="4">
+        <v>137.86000000000001</v>
+      </c>
+      <c r="I35" s="4">
+        <v>593.98</v>
+      </c>
+      <c r="J35" s="4">
+        <v>777.75</v>
+      </c>
+      <c r="K35" s="4">
+        <v>978.49</v>
+      </c>
+      <c r="L35" s="4">
+        <v>1.4765999999999999</v>
+      </c>
+      <c r="M35" s="3">
+        <v>11.635</v>
+      </c>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A36" s="13"/>
+      <c r="B36" s="8" t="s">
+        <v>45</v>
+      </c>
       <c r="C36" s="4">
         <v>4.2664999999999997</v>
       </c>
@@ -5501,6 +5682,24 @@
       </c>
       <c r="G36" s="4">
         <v>738.14</v>
+      </c>
+      <c r="H36" s="4">
+        <v>69.611999999999995</v>
+      </c>
+      <c r="I36" s="4">
+        <v>348.59</v>
+      </c>
+      <c r="J36" s="4">
+        <v>651.24</v>
+      </c>
+      <c r="K36" s="4">
+        <v>742.61</v>
+      </c>
+      <c r="L36" s="4">
+        <v>1.5462</v>
+      </c>
+      <c r="M36" s="3">
+        <v>10.334</v>
       </c>
     </row>
     <row r="37" spans="1:14" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
@@ -5532,15 +5731,15 @@
       </c>
       <c r="H38" s="4">
         <f t="shared" si="0"/>
-        <v>148.52000000000001</v>
+        <v>178.93</v>
       </c>
       <c r="I38" s="4">
         <f t="shared" si="0"/>
-        <v>657.13</v>
+        <v>713.6</v>
       </c>
       <c r="J38" s="4">
         <f t="shared" si="0"/>
-        <v>621.83000000000004</v>
+        <v>777.75</v>
       </c>
       <c r="K38" s="4">
         <f t="shared" si="0"/>
@@ -5570,9 +5769,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F200E048-5FAF-4136-82F6-92204CC50E12}">
   <dimension ref="A1:N37"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A38" sqref="A38:XFD54"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J32" sqref="J32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5634,6 +5833,921 @@
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="13"/>
+      <c r="B3" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3" s="4">
+        <v>16.78</v>
+      </c>
+      <c r="D3" s="4">
+        <v>98.972999999999999</v>
+      </c>
+      <c r="E3" s="4">
+        <v>0.60185999999999995</v>
+      </c>
+      <c r="F3" s="4">
+        <v>4.4156000000000004</v>
+      </c>
+      <c r="G3" s="4">
+        <v>1780.3</v>
+      </c>
+      <c r="H3" s="2">
+        <v>92.941999999999993</v>
+      </c>
+      <c r="I3" s="2">
+        <v>466.64</v>
+      </c>
+      <c r="J3" s="2">
+        <v>124.21</v>
+      </c>
+      <c r="K3" s="2">
+        <v>627.17999999999995</v>
+      </c>
+      <c r="L3" s="2">
+        <v>5.7007000000000003</v>
+      </c>
+      <c r="M3" s="1">
+        <v>2.1873999999999998</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4" s="13"/>
+      <c r="B4" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4" s="4">
+        <v>5.6924999999999999</v>
+      </c>
+      <c r="D4" s="4">
+        <v>67.099999999999994</v>
+      </c>
+      <c r="E4" s="4">
+        <v>1.8542000000000001</v>
+      </c>
+      <c r="F4" s="4">
+        <v>4.7721</v>
+      </c>
+      <c r="G4" s="4">
+        <v>1621.6</v>
+      </c>
+      <c r="H4" s="4">
+        <v>72.41</v>
+      </c>
+      <c r="I4" s="4">
+        <v>404.77</v>
+      </c>
+      <c r="J4" s="4">
+        <v>243.19</v>
+      </c>
+      <c r="K4" s="4">
+        <v>619.92999999999995</v>
+      </c>
+      <c r="L4" s="4">
+        <v>2.4798</v>
+      </c>
+      <c r="M4" s="3">
+        <v>11.411</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5" s="13"/>
+      <c r="B5" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" s="4">
+        <v>19.2</v>
+      </c>
+      <c r="D5" s="4">
+        <v>52.604999999999997</v>
+      </c>
+      <c r="E5" s="4">
+        <v>1.542</v>
+      </c>
+      <c r="F5" s="4">
+        <v>4.5105000000000004</v>
+      </c>
+      <c r="G5" s="4">
+        <v>1614.6</v>
+      </c>
+      <c r="H5" s="4">
+        <v>42.527999999999999</v>
+      </c>
+      <c r="I5" s="4">
+        <v>267.95</v>
+      </c>
+      <c r="J5" s="4">
+        <v>334.54</v>
+      </c>
+      <c r="K5" s="4">
+        <v>705.42</v>
+      </c>
+      <c r="L5" s="4">
+        <v>2.4140999999999999</v>
+      </c>
+      <c r="M5" s="3">
+        <v>9.9943000000000008</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6" s="13"/>
+      <c r="B6" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" s="4">
+        <v>31.327000000000002</v>
+      </c>
+      <c r="D6" s="4">
+        <v>105.29</v>
+      </c>
+      <c r="E6" s="4">
+        <v>0.85489999999999999</v>
+      </c>
+      <c r="F6" s="4">
+        <v>3.7256</v>
+      </c>
+      <c r="G6" s="4">
+        <v>2576.6999999999998</v>
+      </c>
+      <c r="H6" s="4">
+        <v>54.271000000000001</v>
+      </c>
+      <c r="I6" s="4">
+        <v>333.56</v>
+      </c>
+      <c r="J6" s="4">
+        <v>307.45</v>
+      </c>
+      <c r="K6" s="4">
+        <v>694.47</v>
+      </c>
+      <c r="L6" s="4">
+        <v>1.9991000000000001</v>
+      </c>
+      <c r="M6" s="3">
+        <v>6.8034999999999997</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A7" s="13"/>
+      <c r="B7" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="C7" s="4">
+        <v>22.154</v>
+      </c>
+      <c r="D7" s="4">
+        <v>462.34</v>
+      </c>
+      <c r="E7" s="4">
+        <v>0.17408000000000001</v>
+      </c>
+      <c r="F7" s="4">
+        <v>4.3140000000000001</v>
+      </c>
+      <c r="G7" s="4">
+        <v>1828.1</v>
+      </c>
+      <c r="H7" s="4">
+        <v>40.1</v>
+      </c>
+      <c r="I7" s="4">
+        <v>260.64999999999998</v>
+      </c>
+      <c r="J7" s="4">
+        <v>408.44</v>
+      </c>
+      <c r="K7" s="4">
+        <v>853.65</v>
+      </c>
+      <c r="L7" s="4">
+        <v>1.9240999999999999</v>
+      </c>
+      <c r="M7" s="3">
+        <v>7.7561999999999998</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A8" s="13"/>
+      <c r="B8" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="C8" s="4">
+        <v>12.372</v>
+      </c>
+      <c r="D8" s="4">
+        <v>53.15</v>
+      </c>
+      <c r="E8" s="4">
+        <v>7.1665999999999999</v>
+      </c>
+      <c r="F8" s="4">
+        <v>3.9502000000000002</v>
+      </c>
+      <c r="G8" s="4">
+        <v>2220.5</v>
+      </c>
+      <c r="H8" s="4">
+        <v>30.95</v>
+      </c>
+      <c r="I8" s="4">
+        <v>224.67</v>
+      </c>
+      <c r="J8" s="4">
+        <v>344.66</v>
+      </c>
+      <c r="K8" s="4">
+        <v>727.88</v>
+      </c>
+      <c r="L8" s="4">
+        <v>1.3354999999999999</v>
+      </c>
+      <c r="M8" s="3">
+        <v>5.8611000000000004</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A9" s="13"/>
+      <c r="B9" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" s="4">
+        <v>19.024999999999999</v>
+      </c>
+      <c r="D9" s="4">
+        <v>97.213999999999999</v>
+      </c>
+      <c r="E9" s="4">
+        <v>0.88068999999999997</v>
+      </c>
+      <c r="F9" s="4">
+        <v>4.5054999999999996</v>
+      </c>
+      <c r="G9" s="4">
+        <v>1667.4</v>
+      </c>
+      <c r="H9" s="4">
+        <v>50.238</v>
+      </c>
+      <c r="I9" s="4">
+        <v>313.98</v>
+      </c>
+      <c r="J9" s="4">
+        <v>237.66</v>
+      </c>
+      <c r="K9" s="4">
+        <v>764.67</v>
+      </c>
+      <c r="L9" s="4">
+        <v>2.0070999999999999</v>
+      </c>
+      <c r="M9" s="3">
+        <v>2.7730999999999999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A10" s="13"/>
+      <c r="B10" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" s="4">
+        <v>25.12</v>
+      </c>
+      <c r="D10" s="4">
+        <v>307.10000000000002</v>
+      </c>
+      <c r="E10" s="4">
+        <v>0.32185000000000002</v>
+      </c>
+      <c r="F10" s="4">
+        <v>4.2606999999999999</v>
+      </c>
+      <c r="G10" s="4">
+        <v>1819.8</v>
+      </c>
+      <c r="H10" s="4">
+        <v>23.271999999999998</v>
+      </c>
+      <c r="I10" s="4">
+        <v>175.2</v>
+      </c>
+      <c r="J10" s="4">
+        <v>324.36</v>
+      </c>
+      <c r="K10" s="4">
+        <v>665.04</v>
+      </c>
+      <c r="L10" s="4">
+        <v>1.609</v>
+      </c>
+      <c r="M10" s="3">
+        <v>11.782</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A11" s="13"/>
+      <c r="B11" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="C11" s="4">
+        <v>31.123000000000001</v>
+      </c>
+      <c r="D11" s="4">
+        <v>35.65</v>
+      </c>
+      <c r="E11" s="4">
+        <v>4.5808999999999997</v>
+      </c>
+      <c r="F11" s="4">
+        <v>3.6960999999999999</v>
+      </c>
+      <c r="G11" s="4">
+        <v>2581.8000000000002</v>
+      </c>
+      <c r="H11" s="4">
+        <v>33.787999999999997</v>
+      </c>
+      <c r="I11" s="4">
+        <v>237.43</v>
+      </c>
+      <c r="J11" s="4">
+        <v>566.67999999999995</v>
+      </c>
+      <c r="K11" s="4">
+        <v>982.88</v>
+      </c>
+      <c r="L11" s="4">
+        <v>1.6294</v>
+      </c>
+      <c r="M11" s="3">
+        <v>18.094999999999999</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A12" s="13"/>
+      <c r="B12" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="C12" s="4">
+        <v>29.73</v>
+      </c>
+      <c r="D12" s="4">
+        <v>43.859000000000002</v>
+      </c>
+      <c r="E12" s="4">
+        <v>3.2743000000000002</v>
+      </c>
+      <c r="F12" s="4">
+        <v>3.9613</v>
+      </c>
+      <c r="G12" s="4">
+        <v>2101.3000000000002</v>
+      </c>
+      <c r="H12" s="4">
+        <v>32.4</v>
+      </c>
+      <c r="I12" s="4">
+        <v>228.95</v>
+      </c>
+      <c r="J12" s="4">
+        <v>430.57</v>
+      </c>
+      <c r="K12" s="4">
+        <v>764.96</v>
+      </c>
+      <c r="L12" s="4">
+        <v>1.5793999999999999</v>
+      </c>
+      <c r="M12" s="3">
+        <v>19.864000000000001</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="14"/>
+      <c r="B13" s="7"/>
+      <c r="M13" s="6"/>
+      <c r="N13" s="11"/>
+    </row>
+    <row r="14" spans="1:14" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="12">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A15" s="13"/>
+      <c r="B15" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C15" s="4">
+        <v>5.1227</v>
+      </c>
+      <c r="D15" s="4">
+        <v>14.129</v>
+      </c>
+      <c r="E15" s="4">
+        <v>9.6059999999999999</v>
+      </c>
+      <c r="F15" s="4">
+        <v>4.2420999999999998</v>
+      </c>
+      <c r="G15" s="4">
+        <v>1089.0999999999999</v>
+      </c>
+      <c r="H15" s="4">
+        <v>56.116999999999997</v>
+      </c>
+      <c r="I15" s="4">
+        <v>308.89</v>
+      </c>
+      <c r="J15" s="4">
+        <v>129.29</v>
+      </c>
+      <c r="K15" s="4">
+        <v>799.25</v>
+      </c>
+      <c r="L15" s="4">
+        <v>1.5668</v>
+      </c>
+      <c r="M15" s="3">
+        <v>1.9850000000000001</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A16" s="13"/>
+      <c r="B16" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="C16" s="4">
+        <v>11.192</v>
+      </c>
+      <c r="D16" s="4">
+        <v>16.738</v>
+      </c>
+      <c r="E16" s="4">
+        <v>5.9587000000000003</v>
+      </c>
+      <c r="F16" s="4">
+        <v>3.6368999999999998</v>
+      </c>
+      <c r="G16" s="4">
+        <v>1530.1</v>
+      </c>
+      <c r="H16" s="4">
+        <v>35.195999999999998</v>
+      </c>
+      <c r="I16" s="4">
+        <v>206.85</v>
+      </c>
+      <c r="J16" s="4">
+        <v>119.96</v>
+      </c>
+      <c r="K16" s="4">
+        <v>774.72</v>
+      </c>
+      <c r="L16" s="4">
+        <v>1.5092000000000001</v>
+      </c>
+      <c r="M16" s="3">
+        <v>2.5579000000000001</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A17" s="13"/>
+      <c r="B17" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C17" s="4">
+        <v>9.6829000000000001</v>
+      </c>
+      <c r="D17" s="4">
+        <v>13.118</v>
+      </c>
+      <c r="E17" s="4">
+        <v>13.621</v>
+      </c>
+      <c r="F17" s="4">
+        <v>3.5053999999999998</v>
+      </c>
+      <c r="G17" s="4">
+        <v>1604.4</v>
+      </c>
+      <c r="H17" s="4">
+        <v>19.213000000000001</v>
+      </c>
+      <c r="I17" s="4">
+        <v>129</v>
+      </c>
+      <c r="J17" s="4">
+        <v>110.83</v>
+      </c>
+      <c r="K17" s="4">
+        <v>868.84</v>
+      </c>
+      <c r="L17" s="4">
+        <v>1.0492999999999999</v>
+      </c>
+      <c r="M17" s="3">
+        <v>2.3565999999999998</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A18" s="13"/>
+      <c r="B18" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="C18" s="4">
+        <v>5.6656000000000004</v>
+      </c>
+      <c r="D18" s="4">
+        <v>8.2222000000000008</v>
+      </c>
+      <c r="E18" s="4">
+        <v>14.47</v>
+      </c>
+      <c r="F18" s="4">
+        <v>4.3000999999999996</v>
+      </c>
+      <c r="G18" s="4">
+        <v>1006.2</v>
+      </c>
+      <c r="H18" s="4">
+        <v>144.26</v>
+      </c>
+      <c r="I18" s="4">
+        <v>644.21</v>
+      </c>
+      <c r="J18" s="4">
+        <v>178.5</v>
+      </c>
+      <c r="K18" s="4">
+        <v>935.23</v>
+      </c>
+      <c r="L18" s="4">
+        <v>10.004</v>
+      </c>
+      <c r="M18" s="3">
+        <v>2.8494999999999999</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A19" s="13"/>
+      <c r="B19" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="C19" s="4">
+        <v>7.5308999999999999</v>
+      </c>
+      <c r="D19" s="4">
+        <v>23.5</v>
+      </c>
+      <c r="E19" s="4">
+        <v>5.1997999999999998</v>
+      </c>
+      <c r="F19" s="4">
+        <v>3.8620000000000001</v>
+      </c>
+      <c r="G19" s="4">
+        <v>1374.9</v>
+      </c>
+      <c r="H19" s="4">
+        <v>24.858000000000001</v>
+      </c>
+      <c r="I19" s="4">
+        <v>154.83000000000001</v>
+      </c>
+      <c r="J19" s="4">
+        <v>511.79</v>
+      </c>
+      <c r="K19" s="4">
+        <v>997.24</v>
+      </c>
+      <c r="L19" s="4">
+        <v>2.0041000000000002</v>
+      </c>
+      <c r="M19" s="3">
+        <v>7.9977</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A20" s="13"/>
+      <c r="B20" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C20" s="4">
+        <v>4.8239000000000001</v>
+      </c>
+      <c r="D20" s="4">
+        <v>389.25</v>
+      </c>
+      <c r="E20" s="4">
+        <v>0.18435000000000001</v>
+      </c>
+      <c r="F20" s="4">
+        <v>4.4132999999999996</v>
+      </c>
+      <c r="G20" s="4">
+        <v>941.87</v>
+      </c>
+      <c r="H20" s="4">
+        <v>44.973999999999997</v>
+      </c>
+      <c r="I20" s="4">
+        <v>248.15</v>
+      </c>
+      <c r="J20" s="4">
+        <v>621.83000000000004</v>
+      </c>
+      <c r="K20" s="4">
+        <v>913.9</v>
+      </c>
+      <c r="L20" s="4">
+        <v>2.4338000000000002</v>
+      </c>
+      <c r="M20" s="3">
+        <v>7.0609000000000002</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A21" s="13"/>
+      <c r="B21" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C21" s="4">
+        <v>9.7277000000000005</v>
+      </c>
+      <c r="D21" s="4">
+        <v>49.011000000000003</v>
+      </c>
+      <c r="E21" s="4">
+        <v>4.1806000000000001</v>
+      </c>
+      <c r="F21" s="4">
+        <v>3.4098999999999999</v>
+      </c>
+      <c r="G21" s="4">
+        <v>1834.3</v>
+      </c>
+      <c r="H21" s="4">
+        <v>151.05000000000001</v>
+      </c>
+      <c r="I21" s="4">
+        <v>657.1</v>
+      </c>
+      <c r="J21" s="4">
+        <v>262.5</v>
+      </c>
+      <c r="K21" s="4">
+        <v>989.31</v>
+      </c>
+      <c r="L21" s="4">
+        <v>1.6647000000000001</v>
+      </c>
+      <c r="M21" s="3">
+        <v>1.0863</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A22" s="13"/>
+      <c r="B22" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="C22" s="4">
+        <v>16.262</v>
+      </c>
+      <c r="D22" s="4">
+        <v>181.79</v>
+      </c>
+      <c r="E22" s="4">
+        <v>0.52517000000000003</v>
+      </c>
+      <c r="F22" s="4">
+        <v>3.0160999999999998</v>
+      </c>
+      <c r="G22" s="4">
+        <v>2376.6</v>
+      </c>
+      <c r="H22" s="4">
+        <v>29.326000000000001</v>
+      </c>
+      <c r="I22" s="4">
+        <v>172.8</v>
+      </c>
+      <c r="J22" s="4">
+        <v>434.17</v>
+      </c>
+      <c r="K22" s="4">
+        <v>894.26</v>
+      </c>
+      <c r="L22" s="4">
+        <v>2.1920000000000002</v>
+      </c>
+      <c r="M22" s="3">
+        <v>2.8517999999999999</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A23" s="13"/>
+      <c r="B23" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="C23" s="4">
+        <v>6.3647</v>
+      </c>
+      <c r="D23" s="4">
+        <v>183.42</v>
+      </c>
+      <c r="E23" s="4">
+        <v>0.44712000000000002</v>
+      </c>
+      <c r="F23" s="4">
+        <v>4.1839000000000004</v>
+      </c>
+      <c r="G23" s="4">
+        <v>1075.3</v>
+      </c>
+      <c r="H23" s="4">
+        <v>27.326000000000001</v>
+      </c>
+      <c r="I23" s="4">
+        <v>165.15</v>
+      </c>
+      <c r="J23" s="4">
+        <v>422.54</v>
+      </c>
+      <c r="K23" s="4">
+        <v>849.67</v>
+      </c>
+      <c r="L23" s="4">
+        <v>2.2181000000000002</v>
+      </c>
+      <c r="M23" s="3">
+        <v>10.568</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A24" s="13"/>
+      <c r="B24" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C24" s="4">
+        <v>6.5395000000000003</v>
+      </c>
+      <c r="D24" s="4">
+        <v>16.731999999999999</v>
+      </c>
+      <c r="E24" s="4">
+        <v>6.8581000000000003</v>
+      </c>
+      <c r="F24" s="4">
+        <v>4.1207000000000003</v>
+      </c>
+      <c r="G24" s="4">
+        <v>1096.5</v>
+      </c>
+      <c r="H24" s="4">
+        <v>119.77</v>
+      </c>
+      <c r="I24" s="4">
+        <v>547.38</v>
+      </c>
+      <c r="J24" s="4">
+        <v>572.29999999999995</v>
+      </c>
+      <c r="K24" s="4">
+        <v>678.83</v>
+      </c>
+      <c r="L24" s="4">
+        <v>2.3506</v>
+      </c>
+      <c r="M24" s="3">
+        <v>15.843999999999999</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="14"/>
+      <c r="B25" s="7"/>
+      <c r="M25" s="6"/>
+      <c r="N25" s="11"/>
+    </row>
+    <row r="26" spans="1:14" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="12">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A27" s="13"/>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A28" s="13"/>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A29" s="13"/>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A30" s="13"/>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A31" s="13"/>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A32" s="13"/>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A33" s="13"/>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A34" s="13"/>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A35" s="13"/>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A36" s="13"/>
+    </row>
+    <row r="37" spans="1:14" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="14"/>
+      <c r="B37" s="7"/>
+      <c r="M37" s="6"/>
+      <c r="N37" s="11"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A2:A13"/>
+    <mergeCell ref="A14:A25"/>
+    <mergeCell ref="A26:A37"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE086293-56DA-4DD0-A6F8-91C9D98E51F8}">
+  <dimension ref="A1:N37"/>
+  <sheetViews>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F51" sqref="F51"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="4"/>
+    <col min="2" max="2" width="15.7109375" style="8" customWidth="1"/>
+    <col min="3" max="12" width="9.140625" style="4"/>
+    <col min="13" max="13" width="9.140625" style="3"/>
+    <col min="14" max="14" width="9.140625" style="9"/>
+    <col min="15" max="16384" width="9.140625" style="4"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="L1" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="11"/>
+    </row>
+    <row r="2" spans="1:14" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="12">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3" s="13"/>
       <c r="H3" s="2"/>
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>

</xml_diff>

<commit_message>
minor evp-wd_i script changes
</commit_message>
<xml_diff>
--- a/scripts/__other__/__sem__.xlsx
+++ b/scripts/__other__/__sem__.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unsw-my.sharepoint.com/personal/z5208868_ad_unsw_edu_au/Documents/Desktop/code/moga_neml/scripts/__other__/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Janzen\Desktop\code\moga_neml\scripts\__other__\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="5" documentId="13_ncr:1_{4867B082-3585-4B5A-8192-6FFC53AB41B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F5741C39-42CB-4156-AF9B-8DB26B2E0108}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE4C4108-BC03-4ED9-A869-8BFD88BC9790}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="15600" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="evp" sheetId="13" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="49">
   <si>
     <t>temp</t>
   </si>
@@ -181,6 +181,12 @@
   </si>
   <si>
     <t>4; 7</t>
+  </si>
+  <si>
+    <t>5; 8</t>
+  </si>
+  <si>
+    <t>7; 10</t>
   </si>
 </sst>
 </file>
@@ -1124,18 +1130,18 @@
       <selection pane="bottomLeft" activeCell="C27" sqref="C27:G36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.1796875" style="4"/>
-    <col min="2" max="2" width="15.7265625" style="8" customWidth="1"/>
-    <col min="3" max="6" width="9.1796875" style="4"/>
-    <col min="7" max="7" width="9.1796875" style="3"/>
-    <col min="8" max="8" width="15.7265625" style="9" customWidth="1"/>
-    <col min="9" max="11" width="15.7265625" style="8" customWidth="1"/>
-    <col min="12" max="16384" width="9.1796875" style="4"/>
+    <col min="1" max="1" width="9.140625" style="4"/>
+    <col min="2" max="2" width="15.7109375" style="8" customWidth="1"/>
+    <col min="3" max="6" width="9.140625" style="4"/>
+    <col min="7" max="7" width="9.140625" style="3"/>
+    <col min="8" max="8" width="15.7109375" style="9" customWidth="1"/>
+    <col min="9" max="11" width="15.7109375" style="8" customWidth="1"/>
+    <col min="12" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -1170,12 +1176,12 @@
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="5.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="12">
         <v>800</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="13"/>
       <c r="B3" s="8" t="s">
         <v>15</v>
@@ -1205,7 +1211,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="13"/>
       <c r="B4" s="8" t="s">
         <v>15</v>
@@ -1235,7 +1241,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="13"/>
       <c r="B5" s="8" t="s">
         <v>17</v>
@@ -1265,7 +1271,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="13"/>
       <c r="B6" s="8" t="s">
         <v>19</v>
@@ -1295,7 +1301,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="13"/>
       <c r="B7" s="8" t="s">
         <v>15</v>
@@ -1325,7 +1331,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="13"/>
       <c r="B8" s="8" t="s">
         <v>20</v>
@@ -1355,7 +1361,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="13"/>
       <c r="B9" s="8" t="s">
         <v>16</v>
@@ -1385,7 +1391,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="13"/>
       <c r="B10" s="8" t="s">
         <v>16</v>
@@ -1415,7 +1421,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="13"/>
       <c r="B11" s="8" t="s">
         <v>21</v>
@@ -1445,7 +1451,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="13"/>
       <c r="B12" s="8" t="s">
         <v>21</v>
@@ -1475,7 +1481,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="13" spans="1:11" s="5" customFormat="1" ht="5.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:11" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="14"/>
       <c r="B13" s="7"/>
       <c r="G13" s="6"/>
@@ -1484,12 +1490,12 @@
       <c r="J13" s="7"/>
       <c r="K13" s="7"/>
     </row>
-    <row r="14" spans="1:11" ht="5.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:11" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="12">
         <v>900</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="13"/>
       <c r="B15" s="8" t="s">
         <v>15</v>
@@ -1519,7 +1525,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="13"/>
       <c r="B16" s="8" t="s">
         <v>15</v>
@@ -1549,7 +1555,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="13"/>
       <c r="B17" s="8" t="s">
         <v>15</v>
@@ -1579,7 +1585,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="13"/>
       <c r="B18" s="8" t="s">
         <v>17</v>
@@ -1609,7 +1615,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="13"/>
       <c r="B19" s="8" t="s">
         <v>18</v>
@@ -1639,7 +1645,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="13"/>
       <c r="B20" s="8" t="s">
         <v>18</v>
@@ -1669,7 +1675,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="13"/>
       <c r="B21" s="8" t="s">
         <v>24</v>
@@ -1699,7 +1705,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="13"/>
       <c r="B22" s="8" t="s">
         <v>28</v>
@@ -1729,7 +1735,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="13"/>
       <c r="B23" s="8" t="s">
         <v>15</v>
@@ -1759,7 +1765,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="13"/>
       <c r="B24" s="8" t="s">
         <v>16</v>
@@ -1789,7 +1795,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:11" s="5" customFormat="1" ht="5.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:11" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="14"/>
       <c r="B25" s="7"/>
       <c r="G25" s="6"/>
@@ -1798,12 +1804,12 @@
       <c r="J25" s="7"/>
       <c r="K25" s="7"/>
     </row>
-    <row r="26" spans="1:11" ht="5.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:11" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="12">
         <v>1000</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="13"/>
       <c r="B27" s="8" t="s">
         <v>23</v>
@@ -1830,7 +1836,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="13"/>
       <c r="B28" s="8" t="s">
         <v>28</v>
@@ -1857,7 +1863,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="13"/>
       <c r="B29" s="8" t="s">
         <v>23</v>
@@ -1884,7 +1890,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="13"/>
       <c r="B30" s="8" t="s">
         <v>30</v>
@@ -1911,7 +1917,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="13"/>
       <c r="B31" s="8" t="s">
         <v>22</v>
@@ -1938,7 +1944,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="13"/>
       <c r="B32" s="8" t="s">
         <v>28</v>
@@ -1965,7 +1971,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" s="13"/>
       <c r="B33" s="8" t="s">
         <v>28</v>
@@ -1992,7 +1998,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" s="13"/>
       <c r="B34" s="8" t="s">
         <v>28</v>
@@ -2019,7 +2025,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" s="13"/>
       <c r="B35" s="8" t="s">
         <v>28</v>
@@ -2046,7 +2052,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" s="13"/>
       <c r="B36" s="8" t="s">
         <v>27</v>
@@ -2073,7 +2079,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="37" spans="1:11" s="5" customFormat="1" ht="5.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:11" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="14"/>
       <c r="B37" s="7"/>
       <c r="G37" s="6"/>
@@ -2103,17 +2109,17 @@
       <selection pane="bottomLeft" activeCell="C15" sqref="C15:J23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.1796875" style="4"/>
-    <col min="2" max="2" width="15.7265625" style="9" customWidth="1"/>
-    <col min="3" max="3" width="9.1796875" style="9"/>
-    <col min="4" max="10" width="9.1796875" style="4"/>
-    <col min="11" max="11" width="9.1796875" style="9"/>
-    <col min="12" max="16384" width="9.1796875" style="4"/>
+    <col min="1" max="1" width="9.140625" style="4"/>
+    <col min="2" max="2" width="15.7109375" style="9" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" style="9"/>
+    <col min="4" max="10" width="9.140625" style="4"/>
+    <col min="11" max="11" width="9.140625" style="9"/>
+    <col min="12" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -2146,12 +2152,12 @@
       </c>
       <c r="K1" s="11"/>
     </row>
-    <row r="2" spans="1:11" ht="5.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="12">
         <v>800</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="13"/>
       <c r="B3" s="9" t="s">
         <v>28</v>
@@ -2181,7 +2187,7 @@
         <v>6.6364000000000001</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="13"/>
       <c r="B4" s="9" t="s">
         <v>24</v>
@@ -2211,7 +2217,7 @@
         <v>6.6859999999999999</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="13"/>
       <c r="B5" s="9" t="s">
         <v>30</v>
@@ -2241,7 +2247,7 @@
         <v>8.4002999999999997</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="13"/>
       <c r="B6" s="9" t="s">
         <v>17</v>
@@ -2271,7 +2277,7 @@
         <v>6.5503999999999998</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="13"/>
       <c r="B7" s="9" t="s">
         <v>28</v>
@@ -2301,7 +2307,7 @@
         <v>6.9638999999999998</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="13"/>
       <c r="B8" s="9" t="s">
         <v>28</v>
@@ -2331,7 +2337,7 @@
         <v>4.7172000000000001</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="13"/>
       <c r="B9" s="9" t="s">
         <v>24</v>
@@ -2361,7 +2367,7 @@
         <v>8.5634999999999994</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="13"/>
       <c r="B10" s="9" t="s">
         <v>30</v>
@@ -2391,7 +2397,7 @@
         <v>6.8597999999999999</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="13"/>
       <c r="B11" s="9" t="s">
         <v>28</v>
@@ -2421,7 +2427,7 @@
         <v>8.7353000000000005</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="13"/>
       <c r="B12" s="9" t="s">
         <v>27</v>
@@ -2451,18 +2457,18 @@
         <v>8.5096000000000007</v>
       </c>
     </row>
-    <row r="13" spans="1:11" s="5" customFormat="1" ht="5.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:11" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="14"/>
       <c r="B13" s="11"/>
       <c r="C13" s="11"/>
       <c r="K13" s="11"/>
     </row>
-    <row r="14" spans="1:11" ht="5.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:11" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="12">
         <v>900</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="13"/>
       <c r="B15" s="9" t="s">
         <v>19</v>
@@ -2492,7 +2498,7 @@
         <v>9.6201000000000008</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="13"/>
       <c r="B16" s="9" t="s">
         <v>17</v>
@@ -2522,7 +2528,7 @@
         <v>7.4964000000000004</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="13"/>
       <c r="B17" s="9" t="s">
         <v>22</v>
@@ -2552,7 +2558,7 @@
         <v>8.5838000000000001</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="13"/>
       <c r="B18" s="9" t="s">
         <v>17</v>
@@ -2582,7 +2588,7 @@
         <v>11.773</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="13"/>
       <c r="B19" s="9" t="s">
         <v>28</v>
@@ -2612,7 +2618,7 @@
         <v>6.8212000000000002</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="13"/>
       <c r="B20" s="9" t="s">
         <v>26</v>
@@ -2642,7 +2648,7 @@
         <v>6.5256999999999996</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="13"/>
       <c r="B21" s="9" t="s">
         <v>29</v>
@@ -2672,7 +2678,7 @@
         <v>3.5083000000000002</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="13"/>
       <c r="B22" s="9" t="s">
         <v>26</v>
@@ -2702,7 +2708,7 @@
         <v>5.8582999999999998</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="13"/>
       <c r="B23" s="9" t="s">
         <v>20</v>
@@ -2732,7 +2738,7 @@
         <v>6.9904999999999999</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="13"/>
       <c r="B24" s="9" t="s">
         <v>28</v>
@@ -2762,18 +2768,18 @@
         <v>8.0541</v>
       </c>
     </row>
-    <row r="25" spans="1:11" s="5" customFormat="1" ht="5.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:11" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="14"/>
       <c r="B25" s="11"/>
       <c r="C25" s="11"/>
       <c r="K25" s="11"/>
     </row>
-    <row r="26" spans="1:11" ht="5.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:11" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="12">
         <v>1000</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="13"/>
       <c r="B27" s="9" t="s">
         <v>38</v>
@@ -2803,7 +2809,7 @@
         <v>6.8388</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="13"/>
       <c r="B28" s="9" t="s">
         <v>25</v>
@@ -2833,7 +2839,7 @@
         <v>6.1744000000000003</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="13"/>
       <c r="B29" s="9" t="s">
         <v>38</v>
@@ -2863,7 +2869,7 @@
         <v>5.7801999999999998</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="13"/>
       <c r="B30" s="9" t="s">
         <v>38</v>
@@ -2893,7 +2899,7 @@
         <v>5.9217000000000004</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="13"/>
       <c r="B31" s="9" t="s">
         <v>37</v>
@@ -2923,7 +2929,7 @@
         <v>7.1360000000000001</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="13"/>
       <c r="B32" s="9" t="s">
         <v>38</v>
@@ -2953,7 +2959,7 @@
         <v>5.3898000000000001</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" s="13"/>
       <c r="B33" s="9" t="s">
         <v>37</v>
@@ -2983,7 +2989,7 @@
         <v>5.6135000000000002</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" s="13"/>
       <c r="B34" s="9" t="s">
         <v>37</v>
@@ -3013,7 +3019,7 @@
         <v>7.0132000000000003</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" s="13"/>
       <c r="B35" s="9" t="s">
         <v>37</v>
@@ -3043,7 +3049,7 @@
         <v>6.0335999999999999</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" s="13"/>
       <c r="B36" s="9" t="s">
         <v>37</v>
@@ -3073,7 +3079,7 @@
         <v>5.8158000000000003</v>
       </c>
     </row>
-    <row r="37" spans="1:11" s="5" customFormat="1" ht="5.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:11" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="14"/>
       <c r="B37" s="11"/>
       <c r="C37" s="11"/>
@@ -3094,21 +3100,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF6E341A-51E3-4AF7-809B-A8594B1323BC}">
   <dimension ref="A1:K53"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="E41" sqref="E41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.1796875" style="4"/>
-    <col min="2" max="2" width="15.7265625" style="8" customWidth="1"/>
-    <col min="3" max="10" width="9.1796875" style="4"/>
-    <col min="11" max="11" width="9.1796875" style="9"/>
-    <col min="12" max="16384" width="9.1796875" style="4"/>
+    <col min="1" max="1" width="9.140625" style="4"/>
+    <col min="2" max="2" width="15.7109375" style="8" customWidth="1"/>
+    <col min="3" max="10" width="9.140625" style="4"/>
+    <col min="11" max="11" width="9.140625" style="9"/>
+    <col min="12" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -3141,12 +3147,12 @@
       </c>
       <c r="K1" s="11"/>
     </row>
-    <row r="2" spans="1:11" ht="5.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="12">
         <v>800</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="13"/>
       <c r="B3" s="8" t="s">
         <v>19</v>
@@ -3176,7 +3182,7 @@
         <v>13.172000000000001</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="13"/>
       <c r="B4" s="8" t="s">
         <v>22</v>
@@ -3206,7 +3212,7 @@
         <v>11.449</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="13"/>
       <c r="B5" s="8" t="s">
         <v>30</v>
@@ -3236,7 +3242,7 @@
         <v>6.8653000000000004</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="13"/>
       <c r="B6" s="8" t="s">
         <v>22</v>
@@ -3266,7 +3272,7 @@
         <v>7.7724000000000002</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="13"/>
       <c r="B7" s="8" t="s">
         <v>22</v>
@@ -3296,7 +3302,7 @@
         <v>11.287000000000001</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="13"/>
       <c r="B8" s="8" t="s">
         <v>28</v>
@@ -3326,7 +3332,7 @@
         <v>6.6603000000000003</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="13"/>
       <c r="B9" s="8" t="s">
         <v>30</v>
@@ -3356,7 +3362,7 @@
         <v>8.6950000000000003</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="13"/>
       <c r="B10" s="8" t="s">
         <v>17</v>
@@ -3386,7 +3392,7 @@
         <v>6.7618999999999998</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="13"/>
       <c r="B11" s="8" t="s">
         <v>16</v>
@@ -3416,7 +3422,7 @@
         <v>8.5891000000000002</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="13"/>
       <c r="B12" s="8" t="s">
         <v>30</v>
@@ -3446,17 +3452,17 @@
         <v>10.337</v>
       </c>
     </row>
-    <row r="13" spans="1:11" s="5" customFormat="1" ht="5.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:11" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="14"/>
       <c r="B13" s="7"/>
       <c r="K13" s="11"/>
     </row>
-    <row r="14" spans="1:11" ht="5.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:11" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="12">
         <v>900</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="13"/>
       <c r="B15" s="8" t="s">
         <v>20</v>
@@ -3486,7 +3492,7 @@
         <v>9.1929999999999996</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="13"/>
       <c r="B16" s="8" t="s">
         <v>17</v>
@@ -3516,7 +3522,7 @@
         <v>7.2249999999999996</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="13"/>
       <c r="B17" s="8" t="s">
         <v>22</v>
@@ -3546,7 +3552,7 @@
         <v>8.5846999999999998</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="13"/>
       <c r="B18" s="8" t="s">
         <v>22</v>
@@ -3576,7 +3582,7 @@
         <v>11.622999999999999</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="13"/>
       <c r="B19" s="8" t="s">
         <v>22</v>
@@ -3606,7 +3612,7 @@
         <v>6.8217999999999996</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="13"/>
       <c r="B20" s="8" t="s">
         <v>19</v>
@@ -3636,7 +3642,7 @@
         <v>7.0461</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="13"/>
       <c r="B21" s="8" t="s">
         <v>19</v>
@@ -3666,7 +3672,7 @@
         <v>6.1081000000000003</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="13"/>
       <c r="B22" s="8" t="s">
         <v>20</v>
@@ -3696,7 +3702,7 @@
         <v>5.6963999999999997</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="13"/>
       <c r="B23" s="8" t="s">
         <v>20</v>
@@ -3726,7 +3732,7 @@
         <v>9.5322999999999993</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="13"/>
       <c r="B24" s="8" t="s">
         <v>19</v>
@@ -3756,17 +3762,17 @@
         <v>10.206</v>
       </c>
     </row>
-    <row r="25" spans="1:11" s="5" customFormat="1" ht="5.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:11" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="14"/>
       <c r="B25" s="7"/>
       <c r="K25" s="11"/>
     </row>
-    <row r="26" spans="1:11" ht="5.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:11" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="12">
         <v>1000</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="13"/>
       <c r="B27" s="8" t="s">
         <v>38</v>
@@ -3796,7 +3802,7 @@
         <v>6.8921999999999999</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="13"/>
       <c r="B28" s="8" t="s">
         <v>37</v>
@@ -3826,7 +3832,7 @@
         <v>11.145</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="13"/>
       <c r="B29" s="8" t="s">
         <v>25</v>
@@ -3856,7 +3862,7 @@
         <v>5.7804000000000002</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="13"/>
       <c r="B30" s="8" t="s">
         <v>25</v>
@@ -3886,7 +3892,7 @@
         <v>5.9608999999999996</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="13"/>
       <c r="B31" s="8" t="s">
         <v>38</v>
@@ -3916,7 +3922,7 @@
         <v>13.561</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="13"/>
       <c r="B32" s="8" t="s">
         <v>36</v>
@@ -3946,7 +3952,7 @@
         <v>6.9718</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" s="13"/>
       <c r="B33" s="8" t="s">
         <v>37</v>
@@ -3976,7 +3982,7 @@
         <v>8.2904</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" s="13"/>
       <c r="B34" s="8" t="s">
         <v>37</v>
@@ -4006,7 +4012,7 @@
         <v>6.0315000000000003</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" s="13"/>
       <c r="B35" s="8" t="s">
         <v>37</v>
@@ -4036,7 +4042,7 @@
         <v>6.0321999999999996</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" s="13"/>
       <c r="B36" s="8" t="s">
         <v>29</v>
@@ -4066,13 +4072,13 @@
         <v>5.5305</v>
       </c>
     </row>
-    <row r="37" spans="1:11" s="5" customFormat="1" ht="5.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:11" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="14"/>
       <c r="B37" s="7"/>
       <c r="K37" s="11"/>
     </row>
-    <row r="38" spans="1:11" ht="5.15" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:11" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" s="4">
         <v>800</v>
       </c>
@@ -4112,7 +4118,7 @@
         <v>9.1589000000000009</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B40" s="8" t="s">
         <v>42</v>
       </c>
@@ -4149,7 +4155,7 @@
         <v>8.6420500000000011</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B41" s="8" t="s">
         <v>43</v>
       </c>
@@ -4186,13 +4192,13 @@
         <v>2.2846766914477032</v>
       </c>
     </row>
-    <row r="42" spans="1:11" s="5" customFormat="1" ht="5.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:11" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="6"/>
       <c r="B42" s="7"/>
       <c r="K42" s="11"/>
     </row>
-    <row r="43" spans="1:11" ht="5.15" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:11" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" s="4">
         <v>900</v>
       </c>
@@ -4232,7 +4238,7 @@
         <v>8.20364</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B45" s="8" t="s">
         <v>42</v>
       </c>
@@ -4269,7 +4275,7 @@
         <v>7.9048499999999997</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B46" s="8" t="s">
         <v>43</v>
       </c>
@@ -4306,13 +4312,13 @@
         <v>1.9286006125340347</v>
       </c>
     </row>
-    <row r="47" spans="1:11" s="5" customFormat="1" ht="5.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:11" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="6"/>
       <c r="B47" s="7"/>
       <c r="K47" s="11"/>
     </row>
-    <row r="48" spans="1:11" ht="5.15" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:11" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" s="4">
         <v>1000</v>
       </c>
@@ -4352,7 +4358,7 @@
         <v>7.6195900000000005</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B50" s="8" t="s">
         <v>42</v>
       </c>
@@ -4389,7 +4395,7 @@
         <v>6.4621999999999993</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B51" s="8" t="s">
         <v>43</v>
       </c>
@@ -4426,12 +4432,12 @@
         <v>2.6805386869267696</v>
       </c>
     </row>
-    <row r="52" spans="1:11" s="5" customFormat="1" ht="5.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:11" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="6"/>
       <c r="B52" s="7"/>
       <c r="K52" s="11"/>
     </row>
-    <row r="53" spans="1:11" ht="5.15" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="53" spans="1:11" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="A2:A13"/>
@@ -4452,17 +4458,17 @@
       <selection pane="bottomLeft" activeCell="L44" sqref="L44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.1796875" style="4"/>
-    <col min="2" max="2" width="15.7265625" style="8" customWidth="1"/>
-    <col min="3" max="12" width="9.1796875" style="4"/>
-    <col min="13" max="13" width="9.1796875" style="3"/>
-    <col min="14" max="14" width="9.1796875" style="9"/>
-    <col min="15" max="16384" width="9.1796875" style="4"/>
+    <col min="1" max="1" width="9.140625" style="4"/>
+    <col min="2" max="2" width="15.7109375" style="8" customWidth="1"/>
+    <col min="3" max="12" width="9.140625" style="4"/>
+    <col min="13" max="13" width="9.140625" style="3"/>
+    <col min="14" max="14" width="9.140625" style="9"/>
+    <col min="15" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -4504,12 +4510,12 @@
       </c>
       <c r="N1" s="11"/>
     </row>
-    <row r="2" spans="1:14" ht="5.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:14" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="12">
         <v>800</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="13"/>
       <c r="B3" s="8" t="s">
         <v>28</v>
@@ -4548,7 +4554,7 @@
         <v>2.1873999999999998</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="13"/>
       <c r="B4" s="8" t="s">
         <v>27</v>
@@ -4587,7 +4593,7 @@
         <v>11.349</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="13"/>
       <c r="B5" s="8" t="s">
         <v>27</v>
@@ -4626,7 +4632,7 @@
         <v>9.9943000000000008</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="13"/>
       <c r="B6" s="8" t="s">
         <v>28</v>
@@ -4665,7 +4671,7 @@
         <v>6.8034999999999997</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="13"/>
       <c r="B7" s="8" t="s">
         <v>22</v>
@@ -4704,7 +4710,7 @@
         <v>6.8817000000000004</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="13"/>
       <c r="B8" s="8" t="s">
         <v>22</v>
@@ -4743,7 +4749,7 @@
         <v>5.9263000000000003</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="13"/>
       <c r="B9" s="8" t="s">
         <v>24</v>
@@ -4782,7 +4788,7 @@
         <v>2.4095</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="13"/>
       <c r="B10" s="8" t="s">
         <v>22</v>
@@ -4821,7 +4827,7 @@
         <v>11.785</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="13"/>
       <c r="B11" s="8" t="s">
         <v>19</v>
@@ -4860,7 +4866,7 @@
         <v>18.082999999999998</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="13"/>
       <c r="B12" s="8" t="s">
         <v>28</v>
@@ -4899,18 +4905,18 @@
         <v>19.93</v>
       </c>
     </row>
-    <row r="13" spans="1:14" s="5" customFormat="1" ht="5.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:14" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="14"/>
       <c r="B13" s="7"/>
       <c r="M13" s="6"/>
       <c r="N13" s="11"/>
     </row>
-    <row r="14" spans="1:14" ht="5.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:14" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="12">
         <v>900</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="13"/>
       <c r="B15" s="8" t="s">
         <v>29</v>
@@ -4949,7 +4955,7 @@
         <v>1.9850000000000001</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="13"/>
       <c r="B16" s="8" t="s">
         <v>30</v>
@@ -4988,7 +4994,7 @@
         <v>2.7056</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" s="13"/>
       <c r="B17" s="8" t="s">
         <v>29</v>
@@ -5027,7 +5033,7 @@
         <v>2.3519000000000001</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" s="13"/>
       <c r="B18" s="8" t="s">
         <v>39</v>
@@ -5066,7 +5072,7 @@
         <v>2.8494999999999999</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" s="13"/>
       <c r="B19" s="8" t="s">
         <v>30</v>
@@ -5105,7 +5111,7 @@
         <v>7.9154</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" s="13"/>
       <c r="B20" s="8" t="s">
         <v>27</v>
@@ -5144,7 +5150,7 @@
         <v>6.7609000000000004</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" s="13"/>
       <c r="B21" s="8" t="s">
         <v>29</v>
@@ -5183,7 +5189,7 @@
         <v>1.0629</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" s="13"/>
       <c r="B22" s="8" t="s">
         <v>36</v>
@@ -5222,7 +5228,7 @@
         <v>2.8378000000000001</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" s="13"/>
       <c r="B23" s="8" t="s">
         <v>40</v>
@@ -5261,7 +5267,7 @@
         <v>10.67</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" s="13"/>
       <c r="B24" s="8" t="s">
         <v>22</v>
@@ -5300,18 +5306,18 @@
         <v>16.872</v>
       </c>
     </row>
-    <row r="25" spans="1:14" s="5" customFormat="1" ht="5.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:14" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="14"/>
       <c r="B25" s="7"/>
       <c r="M25" s="6"/>
       <c r="N25" s="11"/>
     </row>
-    <row r="26" spans="1:14" ht="5.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:14" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="12">
         <v>1000</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" s="13"/>
       <c r="B27" s="8" t="s">
         <v>39</v>
@@ -5350,7 +5356,7 @@
         <v>2.2120000000000002</v>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" s="13"/>
       <c r="B28" s="8" t="s">
         <v>46</v>
@@ -5389,7 +5395,7 @@
         <v>1.806</v>
       </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29" s="13"/>
       <c r="B29" s="8" t="s">
         <v>38</v>
@@ -5428,7 +5434,7 @@
         <v>3.8136000000000001</v>
       </c>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30" s="13"/>
       <c r="B30" s="8" t="s">
         <v>36</v>
@@ -5467,7 +5473,7 @@
         <v>9.5122999999999998</v>
       </c>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31" s="13"/>
       <c r="B31" s="8" t="s">
         <v>46</v>
@@ -5506,7 +5512,7 @@
         <v>1.9576</v>
       </c>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32" s="13"/>
       <c r="B32" s="8" t="s">
         <v>37</v>
@@ -5545,7 +5551,7 @@
         <v>13.461</v>
       </c>
     </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A33" s="13"/>
       <c r="B33" s="8" t="s">
         <v>37</v>
@@ -5584,7 +5590,7 @@
         <v>5.8274999999999997</v>
       </c>
     </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A34" s="13"/>
       <c r="B34" s="8" t="s">
         <v>46</v>
@@ -5623,7 +5629,7 @@
         <v>1.7726</v>
       </c>
     </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A35" s="13"/>
       <c r="B35" s="8" t="s">
         <v>37</v>
@@ -5662,7 +5668,7 @@
         <v>11.635</v>
       </c>
     </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A36" s="13"/>
       <c r="B36" s="8" t="s">
         <v>45</v>
@@ -5701,13 +5707,13 @@
         <v>10.334</v>
       </c>
     </row>
-    <row r="37" spans="1:14" s="5" customFormat="1" ht="5.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:14" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="14"/>
       <c r="B37" s="7"/>
       <c r="M37" s="6"/>
       <c r="N37" s="11"/>
     </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C38" s="4">
         <f>MAX(C3:C36)</f>
         <v>31.327000000000002</v>
@@ -5768,22 +5774,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F200E048-5FAF-4136-82F6-92204CC50E12}">
   <dimension ref="A1:N37"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C15" sqref="C15:M24"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.1796875" style="4"/>
-    <col min="2" max="2" width="15.7265625" style="8" customWidth="1"/>
-    <col min="3" max="12" width="9.1796875" style="4"/>
-    <col min="13" max="13" width="9.1796875" style="3"/>
-    <col min="14" max="14" width="9.1796875" style="9"/>
-    <col min="15" max="16384" width="9.1796875" style="4"/>
+    <col min="1" max="1" width="9.140625" style="4"/>
+    <col min="2" max="2" width="15.7109375" style="8" customWidth="1"/>
+    <col min="3" max="12" width="9.140625" style="4"/>
+    <col min="13" max="13" width="9.140625" style="3"/>
+    <col min="14" max="14" width="9.140625" style="9"/>
+    <col min="15" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -5825,12 +5831,12 @@
       </c>
       <c r="N1" s="11"/>
     </row>
-    <row r="2" spans="1:14" ht="5.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:14" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="12">
         <v>800</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="13"/>
       <c r="B3" s="8" t="s">
         <v>28</v>
@@ -5869,7 +5875,7 @@
         <v>2.1873999999999998</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="13"/>
       <c r="B4" s="8" t="s">
         <v>28</v>
@@ -5908,10 +5914,10 @@
         <v>11.411</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="13"/>
       <c r="B5" s="8" t="s">
-        <v>22</v>
+        <v>44</v>
       </c>
       <c r="C5" s="4">
         <v>19.2</v>
@@ -5947,7 +5953,7 @@
         <v>9.9943000000000008</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="13"/>
       <c r="B6" s="8" t="s">
         <v>19</v>
@@ -5986,7 +5992,7 @@
         <v>6.8034999999999997</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="13"/>
       <c r="B7" s="8" t="s">
         <v>44</v>
@@ -6025,46 +6031,46 @@
         <v>7.7561999999999998</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="13"/>
       <c r="B8" s="8" t="s">
         <v>44</v>
       </c>
       <c r="C8" s="4">
-        <v>12.372</v>
+        <v>11.45</v>
       </c>
       <c r="D8" s="4">
-        <v>53.15</v>
+        <v>53.134999999999998</v>
       </c>
       <c r="E8" s="4">
-        <v>7.1665999999999999</v>
+        <v>7.1795</v>
       </c>
       <c r="F8" s="4">
         <v>3.9502000000000002</v>
       </c>
       <c r="G8" s="4">
-        <v>2220.5</v>
+        <v>2205.4</v>
       </c>
       <c r="H8" s="4">
-        <v>30.95</v>
+        <v>30.864000000000001</v>
       </c>
       <c r="I8" s="4">
-        <v>224.67</v>
+        <v>224.62</v>
       </c>
       <c r="J8" s="4">
-        <v>344.66</v>
+        <v>340.9</v>
       </c>
       <c r="K8" s="4">
-        <v>727.88</v>
+        <v>729.26</v>
       </c>
       <c r="L8" s="4">
-        <v>1.3354999999999999</v>
+        <v>1.3505</v>
       </c>
       <c r="M8" s="3">
-        <v>5.8611000000000004</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
+        <v>6.6858000000000004</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="13"/>
       <c r="B9" s="8" t="s">
         <v>22</v>
@@ -6103,174 +6109,174 @@
         <v>2.7730999999999999</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="13"/>
       <c r="B10" s="8" t="s">
-        <v>22</v>
+        <v>44</v>
       </c>
       <c r="C10" s="4">
-        <v>25.12</v>
+        <v>24</v>
       </c>
       <c r="D10" s="4">
-        <v>307.10000000000002</v>
+        <v>301.54000000000002</v>
       </c>
       <c r="E10" s="4">
-        <v>0.32185000000000002</v>
+        <v>0.32007999999999998</v>
       </c>
       <c r="F10" s="4">
-        <v>4.2606999999999999</v>
+        <v>4.2862999999999998</v>
       </c>
       <c r="G10" s="4">
-        <v>1819.8</v>
+        <v>1836.9</v>
       </c>
       <c r="H10" s="4">
-        <v>23.271999999999998</v>
+        <v>23.713999999999999</v>
       </c>
       <c r="I10" s="4">
-        <v>175.2</v>
+        <v>176.69</v>
       </c>
       <c r="J10" s="4">
-        <v>324.36</v>
+        <v>323.39999999999998</v>
       </c>
       <c r="K10" s="4">
-        <v>665.04</v>
+        <v>686.91</v>
       </c>
       <c r="L10" s="4">
-        <v>1.609</v>
+        <v>1.6048</v>
       </c>
       <c r="M10" s="3">
-        <v>11.782</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
+        <v>13.085000000000001</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="13"/>
       <c r="B11" s="8" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="C11" s="4">
-        <v>31.123000000000001</v>
+        <v>27.852</v>
       </c>
       <c r="D11" s="4">
-        <v>35.65</v>
+        <v>31.390999999999998</v>
       </c>
       <c r="E11" s="4">
-        <v>4.5808999999999997</v>
+        <v>9.8369999999999997</v>
       </c>
       <c r="F11" s="4">
-        <v>3.6960999999999999</v>
+        <v>3.6958000000000002</v>
       </c>
       <c r="G11" s="4">
-        <v>2581.8000000000002</v>
+        <v>2458</v>
       </c>
       <c r="H11" s="4">
-        <v>33.787999999999997</v>
+        <v>31.946999999999999</v>
       </c>
       <c r="I11" s="4">
-        <v>237.43</v>
+        <v>224.92</v>
       </c>
       <c r="J11" s="4">
-        <v>566.67999999999995</v>
+        <v>521.29</v>
       </c>
       <c r="K11" s="4">
-        <v>982.88</v>
+        <v>982.66</v>
       </c>
       <c r="L11" s="4">
-        <v>1.6294</v>
+        <v>1.5924</v>
       </c>
       <c r="M11" s="3">
-        <v>18.094999999999999</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
+        <v>18.309000000000001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="13"/>
       <c r="B12" s="8" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="C12" s="4">
-        <v>29.73</v>
+        <v>31.91</v>
       </c>
       <c r="D12" s="4">
-        <v>43.859000000000002</v>
+        <v>46.601999999999997</v>
       </c>
       <c r="E12" s="4">
-        <v>3.2743000000000002</v>
+        <v>2.3174000000000001</v>
       </c>
       <c r="F12" s="4">
-        <v>3.9613</v>
+        <v>3.9685000000000001</v>
       </c>
       <c r="G12" s="4">
-        <v>2101.3000000000002</v>
+        <v>2091.1999999999998</v>
       </c>
       <c r="H12" s="4">
-        <v>32.4</v>
+        <v>32.887</v>
       </c>
       <c r="I12" s="4">
-        <v>228.95</v>
+        <v>230.31</v>
       </c>
       <c r="J12" s="4">
-        <v>430.57</v>
+        <v>430.83</v>
       </c>
       <c r="K12" s="4">
-        <v>764.96</v>
+        <v>854.33</v>
       </c>
       <c r="L12" s="4">
-        <v>1.5793999999999999</v>
+        <v>1.6352</v>
       </c>
       <c r="M12" s="3">
-        <v>19.864000000000001</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" s="5" customFormat="1" ht="5.15" customHeight="1" x14ac:dyDescent="0.35">
+        <v>19.951000000000001</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="14"/>
       <c r="B13" s="7"/>
       <c r="M13" s="6"/>
       <c r="N13" s="11"/>
     </row>
-    <row r="14" spans="1:14" ht="5.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:14" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="12">
         <v>900</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="13"/>
       <c r="B15" s="8" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="C15" s="4">
-        <v>5.1227</v>
+        <v>5.7150999999999996</v>
       </c>
       <c r="D15" s="4">
-        <v>14.129</v>
+        <v>13.737</v>
       </c>
       <c r="E15" s="4">
-        <v>9.6059999999999999</v>
+        <v>7.0170000000000003</v>
       </c>
       <c r="F15" s="4">
         <v>4.2420999999999998</v>
       </c>
       <c r="G15" s="4">
-        <v>1089.0999999999999</v>
+        <v>1138.4000000000001</v>
       </c>
       <c r="H15" s="4">
-        <v>56.116999999999997</v>
+        <v>70.744</v>
       </c>
       <c r="I15" s="4">
-        <v>308.89</v>
+        <v>372.33</v>
       </c>
       <c r="J15" s="4">
-        <v>129.29</v>
+        <v>129.13999999999999</v>
       </c>
       <c r="K15" s="4">
-        <v>799.25</v>
+        <v>800.2</v>
       </c>
       <c r="L15" s="4">
-        <v>1.5668</v>
+        <v>1.5445</v>
       </c>
       <c r="M15" s="3">
-        <v>1.9850000000000001</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
+        <v>1.9831000000000001</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="13"/>
       <c r="B16" s="8" t="s">
         <v>30</v>
@@ -6309,7 +6315,7 @@
         <v>2.5579000000000001</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" s="13"/>
       <c r="B17" s="8" t="s">
         <v>24</v>
@@ -6348,7 +6354,7 @@
         <v>2.3565999999999998</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" s="13"/>
       <c r="B18" s="8" t="s">
         <v>39</v>
@@ -6387,7 +6393,7 @@
         <v>2.8494999999999999</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" s="13"/>
       <c r="B19" s="8" t="s">
         <v>44</v>
@@ -6426,7 +6432,7 @@
         <v>7.9977</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" s="13"/>
       <c r="B20" s="8" t="s">
         <v>22</v>
@@ -6465,46 +6471,46 @@
         <v>7.0609000000000002</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" s="13"/>
       <c r="B21" s="8" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C21" s="4">
-        <v>9.7277000000000005</v>
+        <v>5.4767000000000001</v>
       </c>
       <c r="D21" s="4">
-        <v>49.011000000000003</v>
+        <v>43.262</v>
       </c>
       <c r="E21" s="4">
-        <v>4.1806000000000001</v>
+        <v>6.1147999999999998</v>
       </c>
       <c r="F21" s="4">
-        <v>3.4098999999999999</v>
+        <v>3.4083999999999999</v>
       </c>
       <c r="G21" s="4">
-        <v>1834.3</v>
+        <v>1788.2</v>
       </c>
       <c r="H21" s="4">
-        <v>151.05000000000001</v>
+        <v>150.13999999999999</v>
       </c>
       <c r="I21" s="4">
-        <v>657.1</v>
+        <v>656.75</v>
       </c>
       <c r="J21" s="4">
-        <v>262.5</v>
+        <v>266.01</v>
       </c>
       <c r="K21" s="4">
-        <v>989.31</v>
+        <v>957.42</v>
       </c>
       <c r="L21" s="4">
-        <v>1.6647000000000001</v>
+        <v>1.6911</v>
       </c>
       <c r="M21" s="3">
-        <v>1.0863</v>
-      </c>
-    </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.35">
+        <v>1.0717000000000001</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" s="13"/>
       <c r="B22" s="8" t="s">
         <v>26</v>
@@ -6543,7 +6549,7 @@
         <v>2.8517999999999999</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" s="13"/>
       <c r="B23" s="8" t="s">
         <v>44</v>
@@ -6582,7 +6588,7 @@
         <v>10.568</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" s="13"/>
       <c r="B24" s="8" t="s">
         <v>22</v>
@@ -6621,48 +6627,408 @@
         <v>15.843999999999999</v>
       </c>
     </row>
-    <row r="25" spans="1:14" s="5" customFormat="1" ht="5.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:14" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="14"/>
       <c r="B25" s="7"/>
       <c r="M25" s="6"/>
       <c r="N25" s="11"/>
     </row>
-    <row r="26" spans="1:14" ht="5.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:14" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="12">
         <v>1000</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" s="13"/>
-    </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="B27" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C27" s="4">
+        <v>0.41121000000000002</v>
+      </c>
+      <c r="D27" s="4">
+        <v>8.3185000000000002</v>
+      </c>
+      <c r="E27" s="4">
+        <v>1.5488</v>
+      </c>
+      <c r="F27" s="4">
+        <v>4.8285999999999998</v>
+      </c>
+      <c r="G27" s="4">
+        <v>468.32</v>
+      </c>
+      <c r="H27" s="4">
+        <v>91.108999999999995</v>
+      </c>
+      <c r="I27" s="4">
+        <v>420.27</v>
+      </c>
+      <c r="J27" s="4">
+        <v>145.97</v>
+      </c>
+      <c r="K27" s="4">
+        <v>814.06</v>
+      </c>
+      <c r="L27" s="4">
+        <v>1.1305000000000001</v>
+      </c>
+      <c r="M27" s="3">
+        <v>2.2793000000000001</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" s="13"/>
-    </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="B28" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="C28" s="4">
+        <v>4.2740999999999998</v>
+      </c>
+      <c r="D28" s="4">
+        <v>163.31</v>
+      </c>
+      <c r="E28" s="4">
+        <v>0.37485000000000002</v>
+      </c>
+      <c r="F28" s="4">
+        <v>3.8721000000000001</v>
+      </c>
+      <c r="G28" s="4">
+        <v>766.51</v>
+      </c>
+      <c r="H28" s="4">
+        <v>41.393999999999998</v>
+      </c>
+      <c r="I28" s="4">
+        <v>218.54</v>
+      </c>
+      <c r="J28" s="4">
+        <v>47.517000000000003</v>
+      </c>
+      <c r="K28" s="4">
+        <v>291.43</v>
+      </c>
+      <c r="L28" s="4">
+        <v>4.5815000000000001</v>
+      </c>
+      <c r="M28" s="3">
+        <v>1.2543</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29" s="13"/>
-    </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="B29" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C29" s="4">
+        <v>1.2678E-2</v>
+      </c>
+      <c r="D29" s="4">
+        <v>46.238999999999997</v>
+      </c>
+      <c r="E29" s="4">
+        <v>1.2403</v>
+      </c>
+      <c r="F29" s="4">
+        <v>4.7068000000000003</v>
+      </c>
+      <c r="G29" s="4">
+        <v>484.03</v>
+      </c>
+      <c r="H29" s="4">
+        <v>70.912999999999997</v>
+      </c>
+      <c r="I29" s="4">
+        <v>331.34</v>
+      </c>
+      <c r="J29" s="4">
+        <v>176.66</v>
+      </c>
+      <c r="K29" s="4">
+        <v>409.91</v>
+      </c>
+      <c r="L29" s="4">
+        <v>1.605</v>
+      </c>
+      <c r="M29" s="3">
+        <v>3.8136000000000001</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30" s="13"/>
-    </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="B30" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="C30" s="4">
+        <v>3.6912E-2</v>
+      </c>
+      <c r="D30" s="4">
+        <v>49.597999999999999</v>
+      </c>
+      <c r="E30" s="4">
+        <v>0.89181999999999995</v>
+      </c>
+      <c r="F30" s="4">
+        <v>4.7435999999999998</v>
+      </c>
+      <c r="G30" s="4">
+        <v>485.16</v>
+      </c>
+      <c r="H30" s="4">
+        <v>7.2737999999999996</v>
+      </c>
+      <c r="I30" s="4">
+        <v>50.912999999999997</v>
+      </c>
+      <c r="J30" s="4">
+        <v>269.77</v>
+      </c>
+      <c r="K30" s="4">
+        <v>601.74</v>
+      </c>
+      <c r="L30" s="4">
+        <v>1.5640000000000001</v>
+      </c>
+      <c r="M30" s="3">
+        <v>8.7390000000000008</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31" s="13"/>
-    </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="B31" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C31" s="4">
+        <v>0.70825000000000005</v>
+      </c>
+      <c r="D31" s="4">
+        <v>8.4600000000000009</v>
+      </c>
+      <c r="E31" s="4">
+        <v>5.8882000000000003</v>
+      </c>
+      <c r="F31" s="4">
+        <v>4.4476000000000004</v>
+      </c>
+      <c r="G31" s="4">
+        <v>580.37</v>
+      </c>
+      <c r="H31" s="4">
+        <v>179.7</v>
+      </c>
+      <c r="I31" s="4">
+        <v>686.62</v>
+      </c>
+      <c r="J31" s="4">
+        <v>184.92</v>
+      </c>
+      <c r="K31" s="4">
+        <v>898.32</v>
+      </c>
+      <c r="L31" s="4">
+        <v>3.9584999999999999</v>
+      </c>
+      <c r="M31" s="3">
+        <v>1.5712999999999999</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32" s="13"/>
-    </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="B32" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C32" s="4">
+        <v>0.35996</v>
+      </c>
+      <c r="D32" s="4">
+        <v>30.971</v>
+      </c>
+      <c r="E32" s="4">
+        <v>4.9036999999999997</v>
+      </c>
+      <c r="F32" s="4">
+        <v>3.95</v>
+      </c>
+      <c r="G32" s="4">
+        <v>685.6</v>
+      </c>
+      <c r="H32" s="4">
+        <v>118.29</v>
+      </c>
+      <c r="I32" s="4">
+        <v>499.25</v>
+      </c>
+      <c r="J32" s="4">
+        <v>428.38</v>
+      </c>
+      <c r="K32" s="4">
+        <v>969.45</v>
+      </c>
+      <c r="L32" s="4">
+        <v>1.1971000000000001</v>
+      </c>
+      <c r="M32" s="3">
+        <v>13.733000000000001</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A33" s="13"/>
-    </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="B33" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C33" s="4">
+        <v>0.48125000000000001</v>
+      </c>
+      <c r="D33" s="4">
+        <v>40.947000000000003</v>
+      </c>
+      <c r="E33" s="4">
+        <v>4.9225000000000003</v>
+      </c>
+      <c r="F33" s="4">
+        <v>4.0867000000000004</v>
+      </c>
+      <c r="G33" s="4">
+        <v>658</v>
+      </c>
+      <c r="H33" s="4">
+        <v>136.71</v>
+      </c>
+      <c r="I33" s="4">
+        <v>543.66</v>
+      </c>
+      <c r="J33" s="4">
+        <v>663.82</v>
+      </c>
+      <c r="K33" s="4">
+        <v>983.11</v>
+      </c>
+      <c r="L33" s="4">
+        <v>0.88280000000000003</v>
+      </c>
+      <c r="M33" s="3">
+        <v>5.8177000000000003</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A34" s="13"/>
-    </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="B34" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C34" s="4">
+        <v>4.1412000000000004</v>
+      </c>
+      <c r="D34" s="4">
+        <v>50.155000000000001</v>
+      </c>
+      <c r="E34" s="4">
+        <v>3.0377999999999998</v>
+      </c>
+      <c r="F34" s="4">
+        <v>3.8809</v>
+      </c>
+      <c r="G34" s="4">
+        <v>705.19</v>
+      </c>
+      <c r="H34" s="4">
+        <v>178.99</v>
+      </c>
+      <c r="I34" s="4">
+        <v>671.24</v>
+      </c>
+      <c r="J34" s="4">
+        <v>181.75</v>
+      </c>
+      <c r="K34" s="4">
+        <v>794.11</v>
+      </c>
+      <c r="L34" s="4">
+        <v>7.1307</v>
+      </c>
+      <c r="M34" s="3">
+        <v>0.83784000000000003</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A35" s="13"/>
-    </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="B35" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C35" s="4">
+        <v>2.1604999999999999</v>
+      </c>
+      <c r="D35" s="4">
+        <v>63.978000000000002</v>
+      </c>
+      <c r="E35" s="4">
+        <v>0.84965000000000002</v>
+      </c>
+      <c r="F35" s="4">
+        <v>3.9678</v>
+      </c>
+      <c r="G35" s="4">
+        <v>701.83</v>
+      </c>
+      <c r="H35" s="4">
+        <v>145.06</v>
+      </c>
+      <c r="I35" s="4">
+        <v>551.14</v>
+      </c>
+      <c r="J35" s="4">
+        <v>772.16</v>
+      </c>
+      <c r="K35" s="4">
+        <v>978.5</v>
+      </c>
+      <c r="L35" s="4">
+        <v>2.1997</v>
+      </c>
+      <c r="M35" s="3">
+        <v>11.635</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A36" s="13"/>
-    </row>
-    <row r="37" spans="1:14" s="5" customFormat="1" ht="5.15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B36" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C36" s="4">
+        <v>1.6011</v>
+      </c>
+      <c r="D36" s="4">
+        <v>196.8</v>
+      </c>
+      <c r="E36" s="4">
+        <v>0.53120999999999996</v>
+      </c>
+      <c r="F36" s="4">
+        <v>3.9438</v>
+      </c>
+      <c r="G36" s="4">
+        <v>706.71</v>
+      </c>
+      <c r="H36" s="4">
+        <v>115.92</v>
+      </c>
+      <c r="I36" s="4">
+        <v>468.23</v>
+      </c>
+      <c r="J36" s="4">
+        <v>654.29</v>
+      </c>
+      <c r="K36" s="4">
+        <v>742.61</v>
+      </c>
+      <c r="L36" s="4">
+        <v>1.5462</v>
+      </c>
+      <c r="M36" s="3">
+        <v>10.334</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="14"/>
       <c r="B37" s="7"/>
       <c r="M37" s="6"/>

</xml_diff>

<commit_message>
New performance summariser script
</commit_message>
<xml_diff>
--- a/scripts/__other__/__sem__.xlsx
+++ b/scripts/__other__/__sem__.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Janzen\Desktop\code\moga_neml\scripts\__other__\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unsw-my.sharepoint.com/personal/z5208868_ad_unsw_edu_au/Documents/Desktop/code/moga_neml/scripts/__other__/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0B9E5AD-86F1-4C60-9AF5-25B8263F1449}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="15600" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="evp" sheetId="13" r:id="rId1"/>
@@ -1158,18 +1158,18 @@
       <selection pane="bottomLeft" activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="4"/>
-    <col min="2" max="2" width="15.7109375" style="8" customWidth="1"/>
-    <col min="3" max="6" width="9.140625" style="4"/>
-    <col min="7" max="7" width="9.140625" style="3"/>
-    <col min="8" max="8" width="15.7109375" style="9" customWidth="1"/>
-    <col min="9" max="11" width="15.7109375" style="8" customWidth="1"/>
-    <col min="12" max="16384" width="9.140625" style="4"/>
+    <col min="1" max="1" width="9.1796875" style="4"/>
+    <col min="2" max="2" width="15.7265625" style="8" customWidth="1"/>
+    <col min="3" max="6" width="9.1796875" style="4"/>
+    <col min="7" max="7" width="9.1796875" style="3"/>
+    <col min="8" max="8" width="15.7265625" style="9" customWidth="1"/>
+    <col min="9" max="11" width="15.7265625" style="8" customWidth="1"/>
+    <col min="12" max="16384" width="9.1796875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -1204,12 +1204,12 @@
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" ht="5.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="14">
         <v>800</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" s="15"/>
       <c r="B3" s="8" t="s">
         <v>15</v>
@@ -1239,7 +1239,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" s="15"/>
       <c r="B4" s="8" t="s">
         <v>15</v>
@@ -1269,7 +1269,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5" s="15"/>
       <c r="B5" s="8" t="s">
         <v>17</v>
@@ -1299,7 +1299,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" s="15"/>
       <c r="B6" s="8" t="s">
         <v>19</v>
@@ -1329,7 +1329,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7" s="15"/>
       <c r="B7" s="8" t="s">
         <v>15</v>
@@ -1359,7 +1359,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8" s="15"/>
       <c r="B8" s="8" t="s">
         <v>20</v>
@@ -1389,7 +1389,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9" s="15"/>
       <c r="B9" s="8" t="s">
         <v>16</v>
@@ -1419,7 +1419,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A10" s="15"/>
       <c r="B10" s="8" t="s">
         <v>16</v>
@@ -1449,7 +1449,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A11" s="15"/>
       <c r="B11" s="8" t="s">
         <v>21</v>
@@ -1479,7 +1479,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A12" s="15"/>
       <c r="B12" s="8" t="s">
         <v>21</v>
@@ -1509,7 +1509,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="13" spans="1:11" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" s="5" customFormat="1" ht="5.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="16"/>
       <c r="B13" s="7"/>
       <c r="G13" s="6"/>
@@ -1518,12 +1518,12 @@
       <c r="J13" s="7"/>
       <c r="K13" s="7"/>
     </row>
-    <row r="14" spans="1:11" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" ht="5.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="14">
         <v>900</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A15" s="15"/>
       <c r="B15" s="8" t="s">
         <v>15</v>
@@ -1553,7 +1553,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A16" s="15"/>
       <c r="B16" s="8" t="s">
         <v>15</v>
@@ -1583,7 +1583,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A17" s="15"/>
       <c r="B17" s="8" t="s">
         <v>15</v>
@@ -1613,7 +1613,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A18" s="15"/>
       <c r="B18" s="8" t="s">
         <v>17</v>
@@ -1643,7 +1643,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A19" s="15"/>
       <c r="B19" s="8" t="s">
         <v>18</v>
@@ -1673,7 +1673,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A20" s="15"/>
       <c r="B20" s="8" t="s">
         <v>18</v>
@@ -1703,7 +1703,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A21" s="15"/>
       <c r="B21" s="8" t="s">
         <v>24</v>
@@ -1733,7 +1733,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A22" s="15"/>
       <c r="B22" s="8" t="s">
         <v>28</v>
@@ -1763,7 +1763,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A23" s="15"/>
       <c r="B23" s="8" t="s">
         <v>15</v>
@@ -1793,7 +1793,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A24" s="15"/>
       <c r="B24" s="8" t="s">
         <v>16</v>
@@ -1823,7 +1823,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:11" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" s="5" customFormat="1" ht="5.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="16"/>
       <c r="B25" s="7"/>
       <c r="G25" s="6"/>
@@ -1832,12 +1832,12 @@
       <c r="J25" s="7"/>
       <c r="K25" s="7"/>
     </row>
-    <row r="26" spans="1:11" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" ht="5.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="14">
         <v>1000</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A27" s="15"/>
       <c r="B27" s="8" t="s">
         <v>23</v>
@@ -1864,7 +1864,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A28" s="15"/>
       <c r="B28" s="8" t="s">
         <v>28</v>
@@ -1891,7 +1891,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A29" s="15"/>
       <c r="B29" s="8" t="s">
         <v>23</v>
@@ -1918,7 +1918,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A30" s="15"/>
       <c r="B30" s="8" t="s">
         <v>30</v>
@@ -1945,7 +1945,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A31" s="15"/>
       <c r="B31" s="8" t="s">
         <v>22</v>
@@ -1972,7 +1972,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A32" s="15"/>
       <c r="B32" s="8" t="s">
         <v>28</v>
@@ -1999,7 +1999,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A33" s="15"/>
       <c r="B33" s="8" t="s">
         <v>28</v>
@@ -2026,7 +2026,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A34" s="15"/>
       <c r="B34" s="8" t="s">
         <v>28</v>
@@ -2053,7 +2053,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A35" s="15"/>
       <c r="B35" s="8" t="s">
         <v>28</v>
@@ -2080,7 +2080,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A36" s="15"/>
       <c r="B36" s="8" t="s">
         <v>27</v>
@@ -2107,7 +2107,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="37" spans="1:11" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" s="5" customFormat="1" ht="5.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A37" s="16"/>
       <c r="B37" s="7"/>
       <c r="G37" s="6"/>
@@ -2137,17 +2137,17 @@
       <selection pane="bottomLeft" activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="4"/>
-    <col min="2" max="2" width="15.7109375" style="9" customWidth="1"/>
-    <col min="3" max="3" width="9.140625" style="9"/>
-    <col min="4" max="10" width="9.140625" style="4"/>
-    <col min="11" max="11" width="9.140625" style="9"/>
-    <col min="12" max="16384" width="9.140625" style="4"/>
+    <col min="1" max="1" width="9.1796875" style="4"/>
+    <col min="2" max="2" width="15.7265625" style="9" customWidth="1"/>
+    <col min="3" max="3" width="9.1796875" style="9"/>
+    <col min="4" max="10" width="9.1796875" style="4"/>
+    <col min="11" max="11" width="9.1796875" style="9"/>
+    <col min="12" max="16384" width="9.1796875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -2180,12 +2180,12 @@
       </c>
       <c r="K1" s="11"/>
     </row>
-    <row r="2" spans="1:11" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" ht="5.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="14">
         <v>800</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" s="15"/>
       <c r="B3" s="9" t="s">
         <v>28</v>
@@ -2215,7 +2215,7 @@
         <v>6.6364000000000001</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" s="15"/>
       <c r="B4" s="9" t="s">
         <v>24</v>
@@ -2245,7 +2245,7 @@
         <v>6.6859999999999999</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5" s="15"/>
       <c r="B5" s="9" t="s">
         <v>30</v>
@@ -2275,7 +2275,7 @@
         <v>8.4002999999999997</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" s="15"/>
       <c r="B6" s="9" t="s">
         <v>17</v>
@@ -2305,7 +2305,7 @@
         <v>6.5503999999999998</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7" s="15"/>
       <c r="B7" s="9" t="s">
         <v>28</v>
@@ -2335,7 +2335,7 @@
         <v>6.9638999999999998</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8" s="15"/>
       <c r="B8" s="9" t="s">
         <v>28</v>
@@ -2365,7 +2365,7 @@
         <v>4.7172000000000001</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9" s="15"/>
       <c r="B9" s="9" t="s">
         <v>24</v>
@@ -2395,7 +2395,7 @@
         <v>8.5634999999999994</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A10" s="15"/>
       <c r="B10" s="9" t="s">
         <v>30</v>
@@ -2425,7 +2425,7 @@
         <v>6.8597999999999999</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A11" s="15"/>
       <c r="B11" s="9" t="s">
         <v>28</v>
@@ -2455,7 +2455,7 @@
         <v>8.7353000000000005</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A12" s="15"/>
       <c r="B12" s="9" t="s">
         <v>27</v>
@@ -2485,18 +2485,18 @@
         <v>8.5096000000000007</v>
       </c>
     </row>
-    <row r="13" spans="1:11" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" s="5" customFormat="1" ht="5.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="16"/>
       <c r="B13" s="11"/>
       <c r="C13" s="11"/>
       <c r="K13" s="11"/>
     </row>
-    <row r="14" spans="1:11" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" ht="5.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="14">
         <v>900</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A15" s="15"/>
       <c r="B15" s="9" t="s">
         <v>19</v>
@@ -2526,7 +2526,7 @@
         <v>9.6201000000000008</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A16" s="15"/>
       <c r="B16" s="9" t="s">
         <v>17</v>
@@ -2556,7 +2556,7 @@
         <v>7.4964000000000004</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A17" s="15"/>
       <c r="B17" s="9" t="s">
         <v>22</v>
@@ -2586,7 +2586,7 @@
         <v>8.5838000000000001</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A18" s="15"/>
       <c r="B18" s="9" t="s">
         <v>17</v>
@@ -2616,7 +2616,7 @@
         <v>11.773</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A19" s="15"/>
       <c r="B19" s="9" t="s">
         <v>28</v>
@@ -2646,7 +2646,7 @@
         <v>6.8212000000000002</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A20" s="15"/>
       <c r="B20" s="9" t="s">
         <v>26</v>
@@ -2676,7 +2676,7 @@
         <v>6.5256999999999996</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A21" s="15"/>
       <c r="B21" s="9" t="s">
         <v>29</v>
@@ -2706,7 +2706,7 @@
         <v>3.5083000000000002</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A22" s="15"/>
       <c r="B22" s="9" t="s">
         <v>26</v>
@@ -2736,7 +2736,7 @@
         <v>5.8582999999999998</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A23" s="15"/>
       <c r="B23" s="9" t="s">
         <v>20</v>
@@ -2766,7 +2766,7 @@
         <v>6.9904999999999999</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A24" s="15"/>
       <c r="B24" s="9" t="s">
         <v>28</v>
@@ -2796,18 +2796,18 @@
         <v>8.0541</v>
       </c>
     </row>
-    <row r="25" spans="1:11" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" s="5" customFormat="1" ht="5.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="16"/>
       <c r="B25" s="11"/>
       <c r="C25" s="11"/>
       <c r="K25" s="11"/>
     </row>
-    <row r="26" spans="1:11" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" ht="5.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="14">
         <v>1000</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A27" s="15"/>
       <c r="B27" s="9" t="s">
         <v>38</v>
@@ -2837,7 +2837,7 @@
         <v>6.8388</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A28" s="15"/>
       <c r="B28" s="9" t="s">
         <v>25</v>
@@ -2867,7 +2867,7 @@
         <v>6.1744000000000003</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A29" s="15"/>
       <c r="B29" s="9" t="s">
         <v>38</v>
@@ -2897,7 +2897,7 @@
         <v>5.7801999999999998</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A30" s="15"/>
       <c r="B30" s="9" t="s">
         <v>38</v>
@@ -2927,7 +2927,7 @@
         <v>5.9217000000000004</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A31" s="15"/>
       <c r="B31" s="9" t="s">
         <v>37</v>
@@ -2957,7 +2957,7 @@
         <v>7.1360000000000001</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A32" s="15"/>
       <c r="B32" s="9" t="s">
         <v>38</v>
@@ -2987,7 +2987,7 @@
         <v>5.3898000000000001</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A33" s="15"/>
       <c r="B33" s="9" t="s">
         <v>37</v>
@@ -3017,7 +3017,7 @@
         <v>5.6135000000000002</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A34" s="15"/>
       <c r="B34" s="9" t="s">
         <v>37</v>
@@ -3047,7 +3047,7 @@
         <v>7.0132000000000003</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A35" s="15"/>
       <c r="B35" s="9" t="s">
         <v>37</v>
@@ -3077,7 +3077,7 @@
         <v>6.0335999999999999</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A36" s="15"/>
       <c r="B36" s="9" t="s">
         <v>37</v>
@@ -3107,7 +3107,7 @@
         <v>5.8158000000000003</v>
       </c>
     </row>
-    <row r="37" spans="1:11" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" s="5" customFormat="1" ht="5.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A37" s="16"/>
       <c r="B37" s="11"/>
       <c r="C37" s="11"/>
@@ -3129,20 +3129,20 @@
   <dimension ref="A1:K53"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F29" sqref="F29"/>
+      <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K22" sqref="K22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="4"/>
-    <col min="2" max="2" width="15.7109375" style="8" customWidth="1"/>
-    <col min="3" max="10" width="9.140625" style="4"/>
-    <col min="11" max="11" width="9.140625" style="9"/>
-    <col min="12" max="16384" width="9.140625" style="4"/>
+    <col min="1" max="1" width="9.1796875" style="4"/>
+    <col min="2" max="2" width="15.7265625" style="8" customWidth="1"/>
+    <col min="3" max="10" width="9.1796875" style="4"/>
+    <col min="11" max="11" width="9.1796875" style="9"/>
+    <col min="12" max="16384" width="9.1796875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -3175,12 +3175,12 @@
       </c>
       <c r="K1" s="11"/>
     </row>
-    <row r="2" spans="1:11" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" ht="5.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="14">
         <v>800</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" s="15"/>
       <c r="B3" s="8" t="s">
         <v>19</v>
@@ -3210,7 +3210,7 @@
         <v>13.172000000000001</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" s="15"/>
       <c r="B4" s="8" t="s">
         <v>22</v>
@@ -3240,7 +3240,7 @@
         <v>11.449</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5" s="15"/>
       <c r="B5" s="8" t="s">
         <v>30</v>
@@ -3270,7 +3270,7 @@
         <v>6.8653000000000004</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" s="15"/>
       <c r="B6" s="8" t="s">
         <v>22</v>
@@ -3300,7 +3300,7 @@
         <v>7.7724000000000002</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7" s="15"/>
       <c r="B7" s="8" t="s">
         <v>22</v>
@@ -3330,7 +3330,7 @@
         <v>11.287000000000001</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8" s="15"/>
       <c r="B8" s="8" t="s">
         <v>28</v>
@@ -3360,7 +3360,7 @@
         <v>6.6603000000000003</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9" s="15"/>
       <c r="B9" s="8" t="s">
         <v>30</v>
@@ -3390,7 +3390,7 @@
         <v>8.6950000000000003</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A10" s="15"/>
       <c r="B10" s="8" t="s">
         <v>17</v>
@@ -3423,7 +3423,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A11" s="15"/>
       <c r="B11" s="8" t="s">
         <v>16</v>
@@ -3453,7 +3453,7 @@
         <v>8.5891000000000002</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A12" s="15"/>
       <c r="B12" s="8" t="s">
         <v>30</v>
@@ -3483,17 +3483,17 @@
         <v>10.337</v>
       </c>
     </row>
-    <row r="13" spans="1:11" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" s="5" customFormat="1" ht="5.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="16"/>
       <c r="B13" s="7"/>
       <c r="K13" s="11"/>
     </row>
-    <row r="14" spans="1:11" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" ht="5.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="14">
         <v>900</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A15" s="15"/>
       <c r="B15" s="8" t="s">
         <v>20</v>
@@ -3526,7 +3526,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A16" s="15"/>
       <c r="B16" s="8" t="s">
         <v>17</v>
@@ -3556,7 +3556,7 @@
         <v>7.2249999999999996</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A17" s="15"/>
       <c r="B17" s="8" t="s">
         <v>22</v>
@@ -3586,7 +3586,7 @@
         <v>8.5846999999999998</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A18" s="15"/>
       <c r="B18" s="8" t="s">
         <v>22</v>
@@ -3616,7 +3616,7 @@
         <v>11.622999999999999</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A19" s="15"/>
       <c r="B19" s="8" t="s">
         <v>22</v>
@@ -3646,7 +3646,7 @@
         <v>6.8217999999999996</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A20" s="15"/>
       <c r="B20" s="8" t="s">
         <v>19</v>
@@ -3676,7 +3676,7 @@
         <v>7.0461</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A21" s="15"/>
       <c r="B21" s="8" t="s">
         <v>19</v>
@@ -3706,7 +3706,7 @@
         <v>6.1081000000000003</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A22" s="15"/>
       <c r="B22" s="8" t="s">
         <v>20</v>
@@ -3736,7 +3736,7 @@
         <v>5.6963999999999997</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A23" s="15"/>
       <c r="B23" s="8" t="s">
         <v>20</v>
@@ -3766,7 +3766,7 @@
         <v>9.5322999999999993</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A24" s="15"/>
       <c r="B24" s="8" t="s">
         <v>19</v>
@@ -3796,17 +3796,17 @@
         <v>10.206</v>
       </c>
     </row>
-    <row r="25" spans="1:11" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" s="5" customFormat="1" ht="5.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="16"/>
       <c r="B25" s="7"/>
       <c r="K25" s="11"/>
     </row>
-    <row r="26" spans="1:11" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" ht="5.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="14">
         <v>1000</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A27" s="15"/>
       <c r="B27" s="8" t="s">
         <v>38</v>
@@ -3836,7 +3836,7 @@
         <v>6.8921999999999999</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A28" s="15"/>
       <c r="B28" s="8" t="s">
         <v>37</v>
@@ -3866,7 +3866,7 @@
         <v>11.145</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A29" s="15"/>
       <c r="B29" s="8" t="s">
         <v>25</v>
@@ -3899,7 +3899,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A30" s="15"/>
       <c r="B30" s="8" t="s">
         <v>25</v>
@@ -3929,7 +3929,7 @@
         <v>5.9608999999999996</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A31" s="15"/>
       <c r="B31" s="8" t="s">
         <v>38</v>
@@ -3959,7 +3959,7 @@
         <v>13.561</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A32" s="15"/>
       <c r="B32" s="8" t="s">
         <v>36</v>
@@ -3989,7 +3989,7 @@
         <v>6.9718</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A33" s="15"/>
       <c r="B33" s="8" t="s">
         <v>37</v>
@@ -4019,7 +4019,7 @@
         <v>8.2904</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A34" s="15"/>
       <c r="B34" s="8" t="s">
         <v>37</v>
@@ -4049,7 +4049,7 @@
         <v>6.0315000000000003</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A35" s="15"/>
       <c r="B35" s="8" t="s">
         <v>37</v>
@@ -4079,7 +4079,7 @@
         <v>6.0321999999999996</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A36" s="15"/>
       <c r="B36" s="8" t="s">
         <v>29</v>
@@ -4109,13 +4109,13 @@
         <v>5.5305</v>
       </c>
     </row>
-    <row r="37" spans="1:11" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" s="5" customFormat="1" ht="5.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A37" s="16"/>
       <c r="B37" s="7"/>
       <c r="K37" s="11"/>
     </row>
-    <row r="38" spans="1:11" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" ht="5.15" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A39" s="4">
         <v>800</v>
       </c>
@@ -4155,7 +4155,7 @@
         <v>9.1589000000000009</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B40" s="8" t="s">
         <v>42</v>
       </c>
@@ -4192,7 +4192,7 @@
         <v>8.6420500000000011</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B41" s="8" t="s">
         <v>43</v>
       </c>
@@ -4229,13 +4229,13 @@
         <v>2.2846766914477032</v>
       </c>
     </row>
-    <row r="42" spans="1:11" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:11" s="5" customFormat="1" ht="5.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A42" s="6"/>
       <c r="B42" s="7"/>
       <c r="K42" s="11"/>
     </row>
-    <row r="43" spans="1:11" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:11" ht="5.15" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A44" s="4">
         <v>900</v>
       </c>
@@ -4275,7 +4275,7 @@
         <v>8.20364</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B45" s="8" t="s">
         <v>42</v>
       </c>
@@ -4312,7 +4312,7 @@
         <v>7.9048499999999997</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B46" s="8" t="s">
         <v>43</v>
       </c>
@@ -4349,13 +4349,13 @@
         <v>1.9286006125340347</v>
       </c>
     </row>
-    <row r="47" spans="1:11" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:11" s="5" customFormat="1" ht="5.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A47" s="6"/>
       <c r="B47" s="7"/>
       <c r="K47" s="11"/>
     </row>
-    <row r="48" spans="1:11" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:11" ht="5.15" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A49" s="4">
         <v>1000</v>
       </c>
@@ -4395,7 +4395,7 @@
         <v>7.6195900000000005</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B50" s="8" t="s">
         <v>42</v>
       </c>
@@ -4432,7 +4432,7 @@
         <v>6.4621999999999993</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B51" s="8" t="s">
         <v>43</v>
       </c>
@@ -4469,12 +4469,12 @@
         <v>2.6805386869267696</v>
       </c>
     </row>
-    <row r="52" spans="1:11" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:11" s="5" customFormat="1" ht="5.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A52" s="6"/>
       <c r="B52" s="7"/>
       <c r="K52" s="11"/>
     </row>
-    <row r="53" spans="1:11" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="53" spans="1:11" ht="5.15" customHeight="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="A2:A13"/>
@@ -4495,17 +4495,17 @@
       <selection pane="bottomLeft" activeCell="H38" sqref="H38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="4"/>
-    <col min="2" max="2" width="15.7109375" style="8" customWidth="1"/>
-    <col min="3" max="12" width="9.140625" style="4"/>
-    <col min="13" max="13" width="9.140625" style="3"/>
-    <col min="14" max="14" width="9.140625" style="9"/>
-    <col min="15" max="16384" width="9.140625" style="4"/>
+    <col min="1" max="1" width="9.1796875" style="4"/>
+    <col min="2" max="2" width="15.7265625" style="8" customWidth="1"/>
+    <col min="3" max="12" width="9.1796875" style="4"/>
+    <col min="13" max="13" width="9.1796875" style="3"/>
+    <col min="14" max="14" width="9.1796875" style="9"/>
+    <col min="15" max="16384" width="9.1796875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -4547,12 +4547,12 @@
       </c>
       <c r="N1" s="11"/>
     </row>
-    <row r="2" spans="1:14" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" ht="5.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="14">
         <v>800</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A3" s="15"/>
       <c r="B3" s="8" t="s">
         <v>26</v>
@@ -4594,7 +4594,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A4" s="15"/>
       <c r="B4" s="8" t="s">
         <v>27</v>
@@ -4636,7 +4636,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A5" s="15"/>
       <c r="B5" s="8" t="s">
         <v>27</v>
@@ -4675,7 +4675,7 @@
         <v>9.9943000000000008</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A6" s="15"/>
       <c r="B6" s="8" t="s">
         <v>28</v>
@@ -4714,7 +4714,7 @@
         <v>6.8034999999999997</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A7" s="15"/>
       <c r="B7" s="8" t="s">
         <v>22</v>
@@ -4753,7 +4753,7 @@
         <v>6.8817000000000004</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A8" s="15"/>
       <c r="B8" s="8" t="s">
         <v>22</v>
@@ -4792,7 +4792,7 @@
         <v>5.9263000000000003</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A9" s="15"/>
       <c r="B9" s="8" t="s">
         <v>19</v>
@@ -4834,7 +4834,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A10" s="15"/>
       <c r="B10" s="8" t="s">
         <v>22</v>
@@ -4873,7 +4873,7 @@
         <v>11.785</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A11" s="15"/>
       <c r="B11" s="8" t="s">
         <v>19</v>
@@ -4912,7 +4912,7 @@
         <v>18.082999999999998</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A12" s="15"/>
       <c r="B12" s="8" t="s">
         <v>28</v>
@@ -4951,13 +4951,13 @@
         <v>19.93</v>
       </c>
     </row>
-    <row r="13" spans="1:14" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" s="5" customFormat="1" ht="5.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="16"/>
       <c r="B13" s="7"/>
       <c r="M13" s="6"/>
       <c r="N13" s="11"/>
     </row>
-    <row r="14" spans="1:14" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" ht="5.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="14">
         <v>900</v>
       </c>
@@ -4974,7 +4974,7 @@
       <c r="L14"/>
       <c r="M14"/>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A15" s="15"/>
       <c r="B15" s="8" t="s">
         <v>26</v>
@@ -5016,7 +5016,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A16" s="15"/>
       <c r="B16" s="8" t="s">
         <v>26</v>
@@ -5058,7 +5058,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A17" s="15"/>
       <c r="B17" s="8" t="s">
         <v>26</v>
@@ -5100,7 +5100,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A18" s="15"/>
       <c r="B18" s="8" t="s">
         <v>27</v>
@@ -5142,7 +5142,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A19" s="15"/>
       <c r="B19" s="8" t="s">
         <v>30</v>
@@ -5181,7 +5181,7 @@
         <v>7.9154</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A20" s="15"/>
       <c r="B20" s="8" t="s">
         <v>27</v>
@@ -5223,7 +5223,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A21" s="15"/>
       <c r="B21" s="8" t="s">
         <v>26</v>
@@ -5265,7 +5265,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A22" s="15"/>
       <c r="B22" s="8" t="s">
         <v>36</v>
@@ -5304,7 +5304,7 @@
         <v>2.8378000000000001</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A23" s="15"/>
       <c r="B23" s="8" t="s">
         <v>40</v>
@@ -5343,7 +5343,7 @@
         <v>10.67</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A24" s="15"/>
       <c r="B24" s="8" t="s">
         <v>21</v>
@@ -5385,13 +5385,13 @@
         <v>48</v>
       </c>
     </row>
-    <row r="25" spans="1:14" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:14" s="5" customFormat="1" ht="5.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="16"/>
       <c r="B25" s="7"/>
       <c r="M25" s="6"/>
       <c r="N25" s="11"/>
     </row>
-    <row r="26" spans="1:14" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:14" ht="5.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="14">
         <v>1000</v>
       </c>
@@ -5408,7 +5408,7 @@
       <c r="L26"/>
       <c r="M26"/>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A27" s="15"/>
       <c r="B27" s="8" t="s">
         <v>36</v>
@@ -5450,7 +5450,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A28" s="15"/>
       <c r="B28" s="8" t="s">
         <v>27</v>
@@ -5492,7 +5492,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A29" s="15"/>
       <c r="B29" s="8" t="s">
         <v>27</v>
@@ -5534,7 +5534,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A30" s="15"/>
       <c r="B30" s="8" t="s">
         <v>27</v>
@@ -5576,7 +5576,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A31" s="15"/>
       <c r="B31" s="8" t="s">
         <v>46</v>
@@ -5618,7 +5618,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A32" s="15"/>
       <c r="B32" s="8" t="s">
         <v>40</v>
@@ -5660,7 +5660,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A33" s="15"/>
       <c r="B33" s="8" t="s">
         <v>27</v>
@@ -5702,7 +5702,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A34" s="15"/>
       <c r="B34" s="8" t="s">
         <v>26</v>
@@ -5744,7 +5744,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A35" s="15"/>
       <c r="B35" s="8" t="s">
         <v>26</v>
@@ -5786,7 +5786,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A36" s="15"/>
       <c r="B36" s="8" t="s">
         <v>26</v>
@@ -5828,13 +5828,13 @@
         <v>48</v>
       </c>
     </row>
-    <row r="37" spans="1:14" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:14" s="5" customFormat="1" ht="5.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A37" s="16"/>
       <c r="B37" s="7"/>
       <c r="M37" s="6"/>
       <c r="N37" s="11"/>
     </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:14" x14ac:dyDescent="0.35">
       <c r="C38" s="4">
         <f>MAX(C3:C36)</f>
         <v>31.327000000000002</v>
@@ -5881,91 +5881,91 @@
       </c>
       <c r="N38" s="4"/>
     </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:14" x14ac:dyDescent="0.35">
       <c r="N39" s="4"/>
     </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:14" x14ac:dyDescent="0.35">
       <c r="N40" s="4"/>
     </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:14" x14ac:dyDescent="0.35">
       <c r="N41" s="4"/>
     </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:14" x14ac:dyDescent="0.35">
       <c r="N42" s="4"/>
     </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:14" x14ac:dyDescent="0.35">
       <c r="N43" s="4"/>
     </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:14" x14ac:dyDescent="0.35">
       <c r="N44" s="4"/>
     </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:14" x14ac:dyDescent="0.35">
       <c r="N45" s="4"/>
     </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:14" x14ac:dyDescent="0.35">
       <c r="N46" s="4"/>
     </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:14" x14ac:dyDescent="0.35">
       <c r="N47" s="4"/>
     </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:14" x14ac:dyDescent="0.35">
       <c r="N48" s="4"/>
     </row>
-    <row r="49" spans="14:14" x14ac:dyDescent="0.25">
+    <row r="49" spans="14:14" x14ac:dyDescent="0.35">
       <c r="N49" s="4"/>
     </row>
-    <row r="50" spans="14:14" x14ac:dyDescent="0.25">
+    <row r="50" spans="14:14" x14ac:dyDescent="0.35">
       <c r="N50" s="4"/>
     </row>
-    <row r="51" spans="14:14" x14ac:dyDescent="0.25">
+    <row r="51" spans="14:14" x14ac:dyDescent="0.35">
       <c r="N51" s="4"/>
     </row>
-    <row r="52" spans="14:14" x14ac:dyDescent="0.25">
+    <row r="52" spans="14:14" x14ac:dyDescent="0.35">
       <c r="N52" s="4"/>
     </row>
-    <row r="53" spans="14:14" x14ac:dyDescent="0.25">
+    <row r="53" spans="14:14" x14ac:dyDescent="0.35">
       <c r="N53" s="4"/>
     </row>
-    <row r="54" spans="14:14" x14ac:dyDescent="0.25">
+    <row r="54" spans="14:14" x14ac:dyDescent="0.35">
       <c r="N54" s="4"/>
     </row>
-    <row r="55" spans="14:14" x14ac:dyDescent="0.25">
+    <row r="55" spans="14:14" x14ac:dyDescent="0.35">
       <c r="N55" s="4"/>
     </row>
-    <row r="56" spans="14:14" x14ac:dyDescent="0.25">
+    <row r="56" spans="14:14" x14ac:dyDescent="0.35">
       <c r="N56" s="4"/>
     </row>
-    <row r="57" spans="14:14" x14ac:dyDescent="0.25">
+    <row r="57" spans="14:14" x14ac:dyDescent="0.35">
       <c r="N57" s="4"/>
     </row>
-    <row r="58" spans="14:14" x14ac:dyDescent="0.25">
+    <row r="58" spans="14:14" x14ac:dyDescent="0.35">
       <c r="N58" s="4"/>
     </row>
-    <row r="59" spans="14:14" x14ac:dyDescent="0.25">
+    <row r="59" spans="14:14" x14ac:dyDescent="0.35">
       <c r="N59" s="4"/>
     </row>
-    <row r="60" spans="14:14" x14ac:dyDescent="0.25">
+    <row r="60" spans="14:14" x14ac:dyDescent="0.35">
       <c r="N60" s="4"/>
     </row>
-    <row r="61" spans="14:14" x14ac:dyDescent="0.25">
+    <row r="61" spans="14:14" x14ac:dyDescent="0.35">
       <c r="N61" s="4"/>
     </row>
-    <row r="62" spans="14:14" x14ac:dyDescent="0.25">
+    <row r="62" spans="14:14" x14ac:dyDescent="0.35">
       <c r="N62" s="4"/>
     </row>
-    <row r="63" spans="14:14" x14ac:dyDescent="0.25">
+    <row r="63" spans="14:14" x14ac:dyDescent="0.35">
       <c r="N63" s="4"/>
     </row>
-    <row r="64" spans="14:14" x14ac:dyDescent="0.25">
+    <row r="64" spans="14:14" x14ac:dyDescent="0.35">
       <c r="N64" s="4"/>
     </row>
-    <row r="65" spans="14:14" x14ac:dyDescent="0.25">
+    <row r="65" spans="14:14" x14ac:dyDescent="0.35">
       <c r="N65" s="4"/>
     </row>
-    <row r="66" spans="14:14" x14ac:dyDescent="0.25">
+    <row r="66" spans="14:14" x14ac:dyDescent="0.35">
       <c r="N66" s="4"/>
     </row>
-    <row r="67" spans="14:14" x14ac:dyDescent="0.25">
+    <row r="67" spans="14:14" x14ac:dyDescent="0.35">
       <c r="N67" s="4"/>
     </row>
   </sheetData>
@@ -5989,17 +5989,17 @@
       <selection pane="bottomLeft" activeCell="N1" sqref="N1:N1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="4"/>
-    <col min="2" max="2" width="15.7109375" style="8" customWidth="1"/>
-    <col min="3" max="12" width="9.140625" style="4"/>
-    <col min="13" max="13" width="9.140625" style="3"/>
-    <col min="14" max="14" width="9.140625" style="9"/>
-    <col min="15" max="16384" width="9.140625" style="4"/>
+    <col min="1" max="1" width="9.1796875" style="4"/>
+    <col min="2" max="2" width="15.7265625" style="8" customWidth="1"/>
+    <col min="3" max="12" width="9.1796875" style="4"/>
+    <col min="13" max="13" width="9.1796875" style="3"/>
+    <col min="14" max="14" width="9.1796875" style="9"/>
+    <col min="15" max="16384" width="9.1796875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -6041,12 +6041,12 @@
       </c>
       <c r="N1" s="11"/>
     </row>
-    <row r="2" spans="1:14" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" ht="5.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="14">
         <v>800</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A3" s="15"/>
       <c r="B3" s="8" t="s">
         <v>28</v>
@@ -6088,7 +6088,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A4" s="15"/>
       <c r="B4" s="8" t="s">
         <v>28</v>
@@ -6130,7 +6130,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A5" s="15"/>
       <c r="B5" s="8" t="s">
         <v>44</v>
@@ -6169,7 +6169,7 @@
         <v>9.9943000000000008</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A6" s="15"/>
       <c r="B6" s="8" t="s">
         <v>19</v>
@@ -6208,7 +6208,7 @@
         <v>6.8034999999999997</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A7" s="15"/>
       <c r="B7" s="8" t="s">
         <v>44</v>
@@ -6247,7 +6247,7 @@
         <v>7.7561999999999998</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A8" s="15"/>
       <c r="B8" s="8" t="s">
         <v>44</v>
@@ -6286,7 +6286,7 @@
         <v>6.6858000000000004</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A9" s="15"/>
       <c r="B9" s="8" t="s">
         <v>22</v>
@@ -6328,7 +6328,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A10" s="15"/>
       <c r="B10" s="8" t="s">
         <v>44</v>
@@ -6367,7 +6367,7 @@
         <v>13.085000000000001</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A11" s="15"/>
       <c r="B11" s="8" t="s">
         <v>19</v>
@@ -6406,7 +6406,7 @@
         <v>18.309000000000001</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A12" s="15"/>
       <c r="B12" s="8" t="s">
         <v>44</v>
@@ -6445,18 +6445,18 @@
         <v>19.667000000000002</v>
       </c>
     </row>
-    <row r="13" spans="1:14" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" s="5" customFormat="1" ht="5.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="16"/>
       <c r="B13" s="7"/>
       <c r="M13" s="6"/>
       <c r="N13" s="11"/>
     </row>
-    <row r="14" spans="1:14" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" ht="5.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="14">
         <v>900</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A15" s="15"/>
       <c r="B15" s="8" t="s">
         <v>28</v>
@@ -6498,7 +6498,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A16" s="15"/>
       <c r="B16" s="8" t="s">
         <v>30</v>
@@ -6540,7 +6540,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A17" s="15"/>
       <c r="B17" s="8" t="s">
         <v>24</v>
@@ -6582,7 +6582,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A18" s="15"/>
       <c r="B18" s="8" t="s">
         <v>39</v>
@@ -6624,7 +6624,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A19" s="15"/>
       <c r="B19" s="8" t="s">
         <v>44</v>
@@ -6663,7 +6663,7 @@
         <v>7.9977</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A20" s="15"/>
       <c r="B20" s="8" t="s">
         <v>22</v>
@@ -6705,7 +6705,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A21" s="15"/>
       <c r="B21" s="8" t="s">
         <v>27</v>
@@ -6747,7 +6747,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A22" s="15"/>
       <c r="B22" s="8" t="s">
         <v>26</v>
@@ -6786,7 +6786,7 @@
         <v>2.8517999999999999</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A23" s="15"/>
       <c r="B23" s="8" t="s">
         <v>44</v>
@@ -6825,7 +6825,7 @@
         <v>10.568</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A24" s="15"/>
       <c r="B24" s="8" t="s">
         <v>22</v>
@@ -6867,18 +6867,18 @@
         <v>47</v>
       </c>
     </row>
-    <row r="25" spans="1:14" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:14" s="5" customFormat="1" ht="5.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="16"/>
       <c r="B25" s="7"/>
       <c r="M25" s="6"/>
       <c r="N25" s="11"/>
     </row>
-    <row r="26" spans="1:14" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:14" ht="5.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="14">
         <v>1000</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A27" s="15"/>
       <c r="B27" s="8" t="s">
         <v>24</v>
@@ -6917,7 +6917,7 @@
         <v>2.2793000000000001</v>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A28" s="15"/>
       <c r="B28" s="8" t="s">
         <v>45</v>
@@ -6956,7 +6956,7 @@
         <v>1.2543</v>
       </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A29" s="15"/>
       <c r="B29" s="8" t="s">
         <v>27</v>
@@ -6995,7 +6995,7 @@
         <v>3.8136000000000001</v>
       </c>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A30" s="15"/>
       <c r="B30" s="8" t="s">
         <v>46</v>
@@ -7034,7 +7034,7 @@
         <v>8.7390000000000008</v>
       </c>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A31" s="15"/>
       <c r="B31" s="8" t="s">
         <v>27</v>
@@ -7073,7 +7073,7 @@
         <v>1.5712999999999999</v>
       </c>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A32" s="15"/>
       <c r="B32" s="8" t="s">
         <v>36</v>
@@ -7112,7 +7112,7 @@
         <v>13.733000000000001</v>
       </c>
     </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A33" s="15"/>
       <c r="B33" s="8" t="s">
         <v>36</v>
@@ -7151,7 +7151,7 @@
         <v>5.8177000000000003</v>
       </c>
     </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A34" s="15"/>
       <c r="B34" s="8" t="s">
         <v>27</v>
@@ -7190,7 +7190,7 @@
         <v>0.83784000000000003</v>
       </c>
     </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A35" s="15"/>
       <c r="B35" s="8" t="s">
         <v>29</v>
@@ -7229,7 +7229,7 @@
         <v>11.606</v>
       </c>
     </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A36" s="15"/>
       <c r="B36" s="8" t="s">
         <v>29</v>
@@ -7269,15 +7269,15 @@
       </c>
       <c r="N36" s="4"/>
     </row>
-    <row r="37" spans="1:14" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:14" s="5" customFormat="1" ht="5.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A37" s="16"/>
       <c r="B37" s="7"/>
       <c r="M37" s="6"/>
     </row>
-    <row r="38" spans="1:14" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:14" ht="5.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="N38" s="4"/>
     </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A39" s="4">
         <v>800</v>
       </c>
@@ -7330,7 +7330,7 @@
       </c>
       <c r="N39" s="4"/>
     </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B40" s="8" t="s">
         <v>42</v>
       </c>
@@ -7380,7 +7380,7 @@
       </c>
       <c r="N40" s="4"/>
     </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B41" s="8" t="s">
         <v>43</v>
       </c>
@@ -7430,15 +7430,15 @@
       </c>
       <c r="N41" s="4"/>
     </row>
-    <row r="42" spans="1:14" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:14" s="5" customFormat="1" ht="5.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A42" s="6"/>
       <c r="B42" s="7"/>
       <c r="M42" s="6"/>
     </row>
-    <row r="43" spans="1:14" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:14" ht="5.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="N43" s="4"/>
     </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A44" s="4">
         <v>900</v>
       </c>
@@ -7491,7 +7491,7 @@
       </c>
       <c r="N44" s="4"/>
     </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B45" s="8" t="s">
         <v>42</v>
       </c>
@@ -7541,7 +7541,7 @@
       </c>
       <c r="N45" s="4"/>
     </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B46" s="8" t="s">
         <v>43</v>
       </c>
@@ -7591,15 +7591,15 @@
       </c>
       <c r="N46" s="4"/>
     </row>
-    <row r="47" spans="1:14" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:14" s="5" customFormat="1" ht="5.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A47" s="6"/>
       <c r="B47" s="7"/>
       <c r="M47" s="6"/>
     </row>
-    <row r="48" spans="1:14" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:14" ht="5.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="N48" s="4"/>
     </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A49" s="4">
         <v>1000</v>
       </c>
@@ -7652,7 +7652,7 @@
       </c>
       <c r="N49" s="4"/>
     </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B50" s="8" t="s">
         <v>42</v>
       </c>
@@ -7702,7 +7702,7 @@
       </c>
       <c r="N50" s="4"/>
     </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B51" s="8" t="s">
         <v>43</v>
       </c>
@@ -7752,18 +7752,18 @@
       </c>
       <c r="N51" s="4"/>
     </row>
-    <row r="52" spans="1:14" s="5" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:14" s="5" customFormat="1" ht="5.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A52" s="6"/>
       <c r="B52" s="7"/>
       <c r="M52" s="6"/>
     </row>
-    <row r="53" spans="1:14" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:14" ht="5.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="N53" s="4"/>
     </row>
-    <row r="54" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:14" x14ac:dyDescent="0.35">
       <c r="N54" s="4"/>
     </row>
-    <row r="55" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:14" x14ac:dyDescent="0.35">
       <c r="N55" s="4"/>
     </row>
   </sheetData>

</xml_diff>